<commit_message>
Price Update: Fri Dec 19 05:36:58 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,16 +454,21 @@
           <t>URL</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Price Change</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-18 20:22</t>
+          <t>2025-12-19 05:25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -471,29 +476,656 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/8DkcqwJ</t>
+          <t>https://amzn.in/d/0D9RJyQ</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2025-12-19 05:25</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>499</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8DkcqwJ</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:26</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>929</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/9Vmpx9L</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:26</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>929</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/iUJnAAG</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:27</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>569</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8Xctx1i</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:28</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>929</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/isCQv09</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:28</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>499</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/4mstrat</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:29</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>929</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8D9SlMj</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:29</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>299</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/axvUrmf</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:29</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/1yTk7TG</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:30</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>499</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/aNPi1U2</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:30</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8MCAq5Z</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:30</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>299</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/bqE35ja</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:31</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/0V4kPll</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:32</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>929</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/7mqmyMs</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:32</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>299</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/bGuw5EZ</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:33</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2997</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/5fRuGGr</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:33</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>569</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/amDxu6e</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:34</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/fCdbdzb</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:34</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>299</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/i9MHRbf</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:34</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>499</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/d8JD7Ef</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:35</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>569</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/eQdsGNY</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:35</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>569</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/fETFYB9</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:36</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>299</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/fGRPZHm</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:36</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>929</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/27dBhA1</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-12-18 20:22</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>499</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8DkcqwJ</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>2025-12-18 20:24</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C28" t="n">
         <v>569</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Price Update: Fri Dec 19 05:57:49 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,45 +463,45 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-19 05:25</t>
+          <t>2025-12-19 05:45</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>499</v>
+        <v>929</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/0D9RJyQ</t>
+          <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-19 05:25</t>
+          <t>2025-12-19 05:46</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>499</v>
+        <v>1299</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/8DkcqwJ</t>
+          <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -513,107 +513,107 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-19 05:26</t>
+          <t>2025-12-19 05:46</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>929</v>
+        <v>299</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/9Vmpx9L</t>
+          <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-19 05:26</t>
+          <t>2025-12-19 05:47</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>929</v>
+        <v>299</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/iUJnAAG</t>
+          <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-19 05:27</t>
+          <t>2025-12-19 05:48</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>569</v>
+        <v>499</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/8Xctx1i</t>
+          <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-19 05:28</t>
+          <t>2025-12-19 05:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>929</v>
+        <v>1299</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/isCQv09</t>
+          <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-19 05:28</t>
+          <t>2025-12-19 05:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -631,114 +631,114 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-19 05:29</t>
+          <t>2025-12-19 05:49</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/8D9SlMj</t>
+          <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-19 05:29</t>
+          <t>2025-12-19 05:49</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>299</v>
+        <v>499</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/axvUrmf</t>
+          <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-19 05:29</t>
+          <t>2025-12-19 05:49</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1299</v>
+        <v>499</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/1yTk7TG</t>
+          <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-19 05:30</t>
+          <t>2025-12-19 05:50</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>499</v>
+        <v>929</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/aNPi1U2</t>
+          <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-19 05:30</t>
+          <t>2025-12-19 05:51</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -763,12 +763,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-19 05:30</t>
+          <t>2025-12-19 05:51</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -776,124 +776,124 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/bqE35ja</t>
+          <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-19 05:31</t>
+          <t>2025-12-19 05:52</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1299</v>
+        <v>929</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/0V4kPll</t>
+          <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-19 05:32</t>
+          <t>2025-12-19 05:52</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>929</v>
+        <v>299</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/7mqmyMs</t>
+          <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-19 05:32</t>
+          <t>2025-12-19 05:52</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>299</v>
+        <v>1299</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/bGuw5EZ</t>
+          <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-19 05:33</t>
+          <t>2025-12-19 05:53</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2997</v>
+        <v>499</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/5fRuGGr</t>
+          <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-19 05:33</t>
+          <t>2025-12-19 05:53</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -901,157 +901,157 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/amDxu6e</t>
+          <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-19 05:34</t>
+          <t>2025-12-19 05:54</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1299</v>
+        <v>929</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/fCdbdzb</t>
+          <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-19 05:34</t>
+          <t>2025-12-19 05:54</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>299</v>
+        <v>569</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/i9MHRbf</t>
+          <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-19 05:34</t>
+          <t>2025-12-19 05:55</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>499</v>
+        <v>569</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/d8JD7Ef</t>
+          <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-19 05:35</t>
+          <t>2025-12-19 05:56</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>569</v>
+        <v>929</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/eQdsGNY</t>
+          <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-19 05:35</t>
+          <t>2025-12-19 05:56</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>569</v>
+        <v>299</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/fETFYB9</t>
+          <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-19 05:36</t>
+          <t>2025-12-19 05:25</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>299</v>
+        <v>499</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/fGRPZHm</t>
+          <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1063,69 +1063,644 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-19 05:36</t>
+          <t>2025-12-19 05:25</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>929</v>
+        <v>499</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/27dBhA1</t>
+          <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>New Record</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-18 20:22</t>
+          <t>2025-12-19 05:26</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>499</v>
+        <v>929</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://amzn.in/d/8DkcqwJ</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>https://amzn.in/d/9Vmpx9L</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>2025-12-19 05:26</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>929</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/iUJnAAG</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:27</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>569</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8Xctx1i</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:28</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>929</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/isCQv09</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:28</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>499</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/4mstrat</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:29</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>929</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8D9SlMj</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:29</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>299</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/axvUrmf</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:29</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/1yTk7TG</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:30</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>499</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/aNPi1U2</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:30</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>569</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8MCAq5Z</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:30</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>299</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/bqE35ja</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:31</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/0V4kPll</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:32</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>929</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/7mqmyMs</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:32</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>299</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/bGuw5EZ</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:33</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>2997</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/5fRuGGr</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:33</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>569</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/amDxu6e</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:34</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/fCdbdzb</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:34</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>299</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/i9MHRbf</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:34</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>499</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/d8JD7Ef</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:35</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>569</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/eQdsGNY</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:35</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>569</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/fETFYB9</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:36</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>299</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/fGRPZHm</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-12-19 05:36</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>929</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/27dBhA1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>New Record</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-12-18 20:22</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>499</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>https://amzn.in/d/8DkcqwJ</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>2025-12-18 20:24</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="C51" t="n">
         <v>569</v>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Price Update: Fri Dec 19 06:22:43 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,1271 +436,1756 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>SKU Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2025-12-19 06:11</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Price Change</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
         <is>
           <t>2025-12-19 05:45</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>929</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>1299</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="E4" t="n">
         <v>299</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
         <is>
           <t>2025-12-19 05:47</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="E5" t="n">
         <v>299</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="E6" t="n">
         <v>499</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="E7" t="n">
         <v>1299</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="E8" t="n">
         <v>499</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="E9" t="n">
         <v>2997</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="E10" t="n">
         <v>499</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="E11" t="n">
         <v>499</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
         <is>
           <t>2025-12-19 05:50</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="E12" t="n">
         <v>929</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="E13" t="n">
         <v>569</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="E14" t="n">
         <v>299</v>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="E15" t="n">
         <v>929</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="E16" t="n">
         <v>299</v>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="E17" t="n">
         <v>1299</v>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="E18" t="n">
         <v>499</v>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="E19" t="n">
         <v>569</v>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="E20" t="n">
         <v>929</v>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="E21" t="n">
         <v>569</v>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
         <is>
           <t>2025-12-19 05:55</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="E22" t="n">
         <v>569</v>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="E23" t="n">
         <v>929</v>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="E24" t="n">
         <v>299</v>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="E25" t="n">
         <v>499</v>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="E26" t="n">
         <v>499</v>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="E27" t="n">
         <v>929</v>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="E28" t="n">
         <v>929</v>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
         <is>
           <t>2025-12-19 05:27</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="E29" t="n">
         <v>569</v>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="E30" t="n">
         <v>929</v>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="E31" t="n">
         <v>499</v>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="E32" t="n">
         <v>929</v>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="E33" t="n">
         <v>299</v>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="E34" t="n">
         <v>1299</v>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C35" t="n">
+      <c r="E35" t="n">
         <v>499</v>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="E36" t="n">
         <v>569</v>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="C37" t="n">
+      <c r="E37" t="n">
         <v>299</v>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
         <is>
           <t>2025-12-19 05:31</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C38" t="n">
+      <c r="E38" t="n">
         <v>1299</v>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="E39" t="n">
         <v>929</v>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>https://amzn.in/d/7mqmyMs</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="C40" t="n">
+      <c r="E40" t="n">
         <v>299</v>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C41" t="n">
+      <c r="E41" t="n">
         <v>2997</v>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C42" t="n">
+      <c r="E42" t="n">
         <v>569</v>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="G42" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="E43" t="n">
         <v>1299</v>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="E44" t="n">
         <v>299</v>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C45" t="n">
+      <c r="E45" t="n">
         <v>499</v>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="G45" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C46" t="n">
+      <c r="E46" t="n">
         <v>569</v>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>https://amzn.in/d/eQdsGNY</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="E47" t="n">
         <v>569</v>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="C48" t="n">
+      <c r="E48" t="n">
         <v>299</v>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C49" t="n">
+      <c r="E49" t="n">
         <v>929</v>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="G49" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
         <is>
           <t>2025-12-18 20:22</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="C50" t="n">
+      <c r="E50" t="n">
         <v>499</v>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
         <is>
           <t>2025-12-18 20:24</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="C51" t="n">
+      <c r="E51" t="n">
         <v>569</v>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>499</v>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>299</v>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>299</v>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>569</v>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>569</v>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>929</v>
+      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>499</v>
+      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>569</v>
+      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>299</v>
+      </c>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>499</v>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>299</v>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>2997</v>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>499</v>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>499</v>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>929</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>929</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>299</v>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>929</v>
+      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>569</v>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>929</v>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>569</v>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>929</v>
+      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Price Update: Fri Dec 19 07:54:39 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,30 +441,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-19 07:42</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-19 06:11</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Price Change</t>
         </is>
@@ -473,25 +478,26 @@
     <row r="2">
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
         <is>
           <t>2025-12-19 05:45</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>929</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -500,25 +506,26 @@
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>1299</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -527,25 +534,26 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>299</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -554,25 +562,26 @@
     <row r="5">
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
         <is>
           <t>2025-12-19 05:47</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>299</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -581,25 +590,26 @@
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>499</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -608,25 +618,26 @@
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>1299</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -635,25 +646,26 @@
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>499</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -662,25 +674,26 @@
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>2997</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -689,25 +702,26 @@
     <row r="10">
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>499</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -716,25 +730,26 @@
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>499</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -743,25 +758,26 @@
     <row r="12">
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
         <is>
           <t>2025-12-19 05:50</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>929</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -770,25 +786,26 @@
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>569</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -797,25 +814,26 @@
     <row r="14">
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>299</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -824,25 +842,26 @@
     <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>929</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -851,25 +870,26 @@
     <row r="16">
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>299</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -878,25 +898,26 @@
     <row r="17">
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>1299</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -905,25 +926,26 @@
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>499</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -932,25 +954,26 @@
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr">
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>569</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -959,25 +982,26 @@
     <row r="20">
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>929</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -986,25 +1010,26 @@
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>569</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1013,25 +1038,26 @@
     <row r="22">
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr">
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
         <is>
           <t>2025-12-19 05:55</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>569</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1040,25 +1066,26 @@
     <row r="23">
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>929</v>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1067,25 +1094,26 @@
     <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>299</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1094,25 +1122,26 @@
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>499</v>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1121,25 +1150,26 @@
     <row r="26">
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr">
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>499</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1148,25 +1178,26 @@
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr">
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>929</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1175,25 +1206,26 @@
     <row r="28">
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>929</v>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1202,25 +1234,26 @@
     <row r="29">
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr">
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
         <is>
           <t>2025-12-19 05:27</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>569</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1229,25 +1262,26 @@
     <row r="30">
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr">
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>929</v>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1256,25 +1290,26 @@
     <row r="31">
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr">
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>499</v>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1283,25 +1318,26 @@
     <row r="32">
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr">
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>929</v>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1310,25 +1346,26 @@
     <row r="33">
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr">
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>299</v>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1337,25 +1374,26 @@
     <row r="34">
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr">
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>1299</v>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1364,25 +1402,26 @@
     <row r="35">
       <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr">
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>499</v>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1391,25 +1430,26 @@
     <row r="36">
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr">
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>569</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1418,25 +1458,26 @@
     <row r="37">
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr">
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>299</v>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1445,25 +1486,26 @@
     <row r="38">
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr">
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
         <is>
           <t>2025-12-19 05:31</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>1299</v>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1472,25 +1514,26 @@
     <row r="39">
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr">
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>929</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>https://amzn.in/d/7mqmyMs</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1499,25 +1542,26 @@
     <row r="40">
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr">
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>299</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1526,25 +1570,26 @@
     <row r="41">
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr">
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>2997</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1553,25 +1598,26 @@
     <row r="42">
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr">
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>569</v>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="G42" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1580,25 +1626,26 @@
     <row r="43">
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr">
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>1299</v>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1607,25 +1654,26 @@
     <row r="44">
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr">
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>299</v>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1634,25 +1682,26 @@
     <row r="45">
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr">
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>499</v>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="G45" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1661,25 +1710,26 @@
     <row r="46">
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr">
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>569</v>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>https://amzn.in/d/eQdsGNY</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1688,25 +1738,26 @@
     <row r="47">
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr">
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>569</v>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1715,25 +1766,26 @@
     <row r="48">
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr">
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
         <v>299</v>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1742,25 +1794,26 @@
     <row r="49">
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr">
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>929</v>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="G49" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="H49" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1769,48 +1822,50 @@
     <row r="50">
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr">
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
         <is>
           <t>2025-12-18 20:22</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>499</v>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="G50" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr">
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
         <is>
           <t>2025-12-18 20:24</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>569</v>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="G51" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1821,11 +1876,14 @@
       <c r="B52" t="n">
         <v>499</v>
       </c>
-      <c r="C52" t="inlineStr"/>
+      <c r="C52" t="n">
+        <v>499</v>
+      </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1836,11 +1894,14 @@
       <c r="B53" t="n">
         <v>299</v>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="C53" t="n">
+        <v>299</v>
+      </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1851,11 +1912,14 @@
       <c r="B54" t="n">
         <v>299</v>
       </c>
-      <c r="C54" t="inlineStr"/>
+      <c r="C54" t="n">
+        <v>299</v>
+      </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1866,11 +1930,14 @@
       <c r="B55" t="n">
         <v>569</v>
       </c>
-      <c r="C55" t="inlineStr"/>
+      <c r="C55" t="n">
+        <v>569</v>
+      </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1881,11 +1948,14 @@
       <c r="B56" t="n">
         <v>569</v>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" t="n">
+        <v>569</v>
+      </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1896,11 +1966,14 @@
       <c r="B57" t="n">
         <v>1299</v>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="n">
+        <v>1299</v>
+      </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1911,11 +1984,14 @@
       <c r="B58" t="n">
         <v>1299</v>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" t="n">
+        <v>1299</v>
+      </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1926,11 +2002,14 @@
       <c r="B59" t="n">
         <v>1299</v>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>1299</v>
+      </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1941,11 +2020,14 @@
       <c r="B60" t="n">
         <v>929</v>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="C60" t="n">
+        <v>929</v>
+      </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1956,11 +2038,14 @@
       <c r="B61" t="n">
         <v>499</v>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="C61" t="n">
+        <v>499</v>
+      </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1971,11 +2056,14 @@
       <c r="B62" t="n">
         <v>569</v>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>569</v>
+      </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1986,11 +2074,14 @@
       <c r="B63" t="n">
         <v>299</v>
       </c>
-      <c r="C63" t="inlineStr"/>
+      <c r="C63" t="n">
+        <v>299</v>
+      </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2001,11 +2092,14 @@
       <c r="B64" t="n">
         <v>499</v>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" t="n">
+        <v>499</v>
+      </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2016,11 +2110,14 @@
       <c r="B65" t="n">
         <v>299</v>
       </c>
-      <c r="C65" t="inlineStr"/>
+      <c r="C65" t="n">
+        <v>299</v>
+      </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2031,11 +2128,14 @@
       <c r="B66" t="n">
         <v>2997</v>
       </c>
-      <c r="C66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>2997</v>
+      </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2046,11 +2146,14 @@
       <c r="B67" t="n">
         <v>499</v>
       </c>
-      <c r="C67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>499</v>
+      </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2061,11 +2164,14 @@
       <c r="B68" t="n">
         <v>499</v>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>499</v>
+      </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2076,11 +2182,14 @@
       <c r="B69" t="n">
         <v>929</v>
       </c>
-      <c r="C69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>929</v>
+      </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2091,11 +2200,14 @@
       <c r="B70" t="n">
         <v>929</v>
       </c>
-      <c r="C70" t="inlineStr"/>
+      <c r="C70" t="n">
+        <v>929</v>
+      </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2103,14 +2215,15 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B71" t="n">
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="n">
         <v>299</v>
       </c>
-      <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2121,11 +2234,14 @@
       <c r="B72" t="n">
         <v>929</v>
       </c>
-      <c r="C72" t="inlineStr"/>
+      <c r="C72" t="n">
+        <v>929</v>
+      </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2136,11 +2252,14 @@
       <c r="B73" t="n">
         <v>569</v>
       </c>
-      <c r="C73" t="inlineStr"/>
+      <c r="C73" t="n">
+        <v>569</v>
+      </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2151,11 +2270,14 @@
       <c r="B74" t="n">
         <v>929</v>
       </c>
-      <c r="C74" t="inlineStr"/>
+      <c r="C74" t="n">
+        <v>929</v>
+      </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2166,11 +2288,14 @@
       <c r="B75" t="n">
         <v>569</v>
       </c>
-      <c r="C75" t="inlineStr"/>
+      <c r="C75" t="n">
+        <v>569</v>
+      </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2181,11 +2306,14 @@
       <c r="B76" t="n">
         <v>929</v>
       </c>
-      <c r="C76" t="inlineStr"/>
+      <c r="C76" t="n">
+        <v>929</v>
+      </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Price Update: Fri Dec 19 09:07:03 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,35 +441,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-19 08:56</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-19 07:42</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 06:11</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Price Change</t>
         </is>
@@ -479,25 +484,26 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
         <is>
           <t>2025-12-19 05:45</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>929</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="n">
+        <v>929</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -507,25 +513,26 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>1299</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -535,25 +542,26 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>299</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -563,25 +571,26 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>2025-12-19 05:47</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>299</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -591,25 +600,26 @@
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>499</v>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" t="n">
+        <v>499</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -619,25 +629,26 @@
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>1299</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -647,25 +658,26 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>499</v>
-      </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" t="n">
+        <v>499</v>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -675,25 +687,26 @@
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>2997</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -703,25 +716,26 @@
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>499</v>
-      </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" t="n">
+        <v>499</v>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -731,25 +745,26 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>499</v>
-      </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" t="n">
+        <v>499</v>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -759,25 +774,26 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
         <is>
           <t>2025-12-19 05:50</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>929</v>
-      </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" t="n">
+        <v>929</v>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -787,25 +803,26 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>569</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -815,25 +832,26 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>299</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -843,25 +861,26 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>929</v>
-      </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" t="n">
+        <v>929</v>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -871,25 +890,26 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>299</v>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -899,25 +919,26 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>1299</v>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -927,25 +948,26 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F18" t="n">
-        <v>499</v>
-      </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" t="n">
+        <v>499</v>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -955,25 +977,26 @@
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>569</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -983,25 +1006,26 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F20" t="n">
-        <v>929</v>
-      </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" t="n">
+        <v>929</v>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1011,25 +1035,26 @@
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>569</v>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1039,25 +1064,26 @@
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr">
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
         <is>
           <t>2025-12-19 05:55</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>569</v>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1067,25 +1093,26 @@
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F23" t="n">
-        <v>929</v>
-      </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" t="n">
+        <v>929</v>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1095,25 +1122,26 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>299</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1123,25 +1151,26 @@
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr">
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F25" t="n">
-        <v>499</v>
-      </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" t="n">
+        <v>499</v>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1151,25 +1180,26 @@
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr">
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F26" t="n">
-        <v>499</v>
-      </c>
-      <c r="G26" t="inlineStr">
+      <c r="G26" t="n">
+        <v>499</v>
+      </c>
+      <c r="H26" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1179,25 +1209,26 @@
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F27" t="n">
-        <v>929</v>
-      </c>
-      <c r="G27" t="inlineStr">
+      <c r="G27" t="n">
+        <v>929</v>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1207,25 +1238,26 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr">
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F28" t="n">
-        <v>929</v>
-      </c>
-      <c r="G28" t="inlineStr">
+      <c r="G28" t="n">
+        <v>929</v>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1235,25 +1267,26 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr">
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
         <is>
           <t>2025-12-19 05:27</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>569</v>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1263,25 +1296,26 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr">
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F30" t="n">
-        <v>929</v>
-      </c>
-      <c r="G30" t="inlineStr">
+      <c r="G30" t="n">
+        <v>929</v>
+      </c>
+      <c r="H30" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1291,25 +1325,26 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr">
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F31" t="n">
-        <v>499</v>
-      </c>
-      <c r="G31" t="inlineStr">
+      <c r="G31" t="n">
+        <v>499</v>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1319,25 +1354,26 @@
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr">
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F32" t="n">
-        <v>929</v>
-      </c>
-      <c r="G32" t="inlineStr">
+      <c r="G32" t="n">
+        <v>929</v>
+      </c>
+      <c r="H32" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1347,25 +1383,26 @@
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr">
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>299</v>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1375,25 +1412,26 @@
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr">
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>1299</v>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1403,25 +1441,26 @@
       <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr">
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F35" t="n">
-        <v>499</v>
-      </c>
-      <c r="G35" t="inlineStr">
+      <c r="G35" t="n">
+        <v>499</v>
+      </c>
+      <c r="H35" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1431,25 +1470,26 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr">
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>569</v>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1459,25 +1499,26 @@
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr">
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>299</v>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1487,25 +1528,26 @@
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr">
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
         <is>
           <t>2025-12-19 05:31</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>1299</v>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1515,25 +1557,26 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr">
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F39" t="n">
-        <v>929</v>
-      </c>
-      <c r="G39" t="inlineStr">
+      <c r="G39" t="n">
+        <v>929</v>
+      </c>
+      <c r="H39" t="inlineStr">
         <is>
           <t>https://amzn.in/d/7mqmyMs</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1543,25 +1586,26 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr">
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>299</v>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1571,25 +1615,26 @@
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr">
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>2997</v>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1599,25 +1644,26 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr">
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>569</v>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
+      <c r="I42" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1627,25 +1673,26 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr">
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>1299</v>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="I43" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1655,25 +1702,26 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr">
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>299</v>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="I44" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1683,25 +1731,26 @@
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr">
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F45" t="n">
-        <v>499</v>
-      </c>
-      <c r="G45" t="inlineStr">
+      <c r="G45" t="n">
+        <v>499</v>
+      </c>
+      <c r="H45" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
+      <c r="I45" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1711,25 +1760,26 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr">
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>569</v>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>https://amzn.in/d/eQdsGNY</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="I46" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1739,25 +1789,26 @@
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr">
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>569</v>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
+      <c r="I47" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1767,25 +1818,26 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr">
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>299</v>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="I48" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1795,25 +1847,26 @@
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr">
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F49" t="n">
-        <v>929</v>
-      </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" t="n">
+        <v>929</v>
+      </c>
+      <c r="H49" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="I49" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1823,49 +1876,51 @@
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr">
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
         <is>
           <t>2025-12-18 20:22</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="F50" t="n">
-        <v>499</v>
-      </c>
-      <c r="G50" t="inlineStr">
+      <c r="G50" t="n">
+        <v>499</v>
+      </c>
+      <c r="H50" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr">
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
         <is>
           <t>2025-12-18 20:24</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>569</v>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="H51" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1879,11 +1934,14 @@
       <c r="C52" t="n">
         <v>499</v>
       </c>
-      <c r="D52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>499</v>
+      </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1897,11 +1955,14 @@
       <c r="C53" t="n">
         <v>299</v>
       </c>
-      <c r="D53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>299</v>
+      </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1915,11 +1976,14 @@
       <c r="C54" t="n">
         <v>299</v>
       </c>
-      <c r="D54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>299</v>
+      </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1933,11 +1997,14 @@
       <c r="C55" t="n">
         <v>569</v>
       </c>
-      <c r="D55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>569</v>
+      </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1951,11 +2018,14 @@
       <c r="C56" t="n">
         <v>569</v>
       </c>
-      <c r="D56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>569</v>
+      </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1969,11 +2039,14 @@
       <c r="C57" t="n">
         <v>1299</v>
       </c>
-      <c r="D57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>1299</v>
+      </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1987,11 +2060,14 @@
       <c r="C58" t="n">
         <v>1299</v>
       </c>
-      <c r="D58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>1299</v>
+      </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2005,11 +2081,14 @@
       <c r="C59" t="n">
         <v>1299</v>
       </c>
-      <c r="D59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>1299</v>
+      </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2023,11 +2102,14 @@
       <c r="C60" t="n">
         <v>929</v>
       </c>
-      <c r="D60" t="inlineStr"/>
+      <c r="D60" t="n">
+        <v>929</v>
+      </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2041,11 +2123,14 @@
       <c r="C61" t="n">
         <v>499</v>
       </c>
-      <c r="D61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>499</v>
+      </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2059,11 +2144,14 @@
       <c r="C62" t="n">
         <v>569</v>
       </c>
-      <c r="D62" t="inlineStr"/>
+      <c r="D62" t="n">
+        <v>569</v>
+      </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2077,11 +2165,14 @@
       <c r="C63" t="n">
         <v>299</v>
       </c>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="n">
+        <v>299</v>
+      </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2095,11 +2186,14 @@
       <c r="C64" t="n">
         <v>499</v>
       </c>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>499</v>
+      </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2113,11 +2207,14 @@
       <c r="C65" t="n">
         <v>299</v>
       </c>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>299</v>
+      </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2125,17 +2222,18 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B66" t="n">
-        <v>2997</v>
-      </c>
+      <c r="B66" t="inlineStr"/>
       <c r="C66" t="n">
         <v>2997</v>
       </c>
-      <c r="D66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>2997</v>
+      </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2149,11 +2247,14 @@
       <c r="C67" t="n">
         <v>499</v>
       </c>
-      <c r="D67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>499</v>
+      </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2167,11 +2268,14 @@
       <c r="C68" t="n">
         <v>499</v>
       </c>
-      <c r="D68" t="inlineStr"/>
+      <c r="D68" t="n">
+        <v>499</v>
+      </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2185,11 +2289,14 @@
       <c r="C69" t="n">
         <v>929</v>
       </c>
-      <c r="D69" t="inlineStr"/>
+      <c r="D69" t="n">
+        <v>929</v>
+      </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2203,11 +2310,14 @@
       <c r="C70" t="n">
         <v>929</v>
       </c>
-      <c r="D70" t="inlineStr"/>
+      <c r="D70" t="n">
+        <v>929</v>
+      </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2215,15 +2325,18 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr"/>
-      <c r="C71" t="n">
+      <c r="B71" t="n">
         <v>299</v>
       </c>
-      <c r="D71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>299</v>
+      </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2237,11 +2350,14 @@
       <c r="C72" t="n">
         <v>929</v>
       </c>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="n">
+        <v>929</v>
+      </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2255,11 +2371,14 @@
       <c r="C73" t="n">
         <v>569</v>
       </c>
-      <c r="D73" t="inlineStr"/>
+      <c r="D73" t="n">
+        <v>569</v>
+      </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2273,11 +2392,14 @@
       <c r="C74" t="n">
         <v>929</v>
       </c>
-      <c r="D74" t="inlineStr"/>
+      <c r="D74" t="n">
+        <v>929</v>
+      </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2291,11 +2413,14 @@
       <c r="C75" t="n">
         <v>569</v>
       </c>
-      <c r="D75" t="inlineStr"/>
+      <c r="D75" t="n">
+        <v>569</v>
+      </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2309,11 +2434,14 @@
       <c r="C76" t="n">
         <v>929</v>
       </c>
-      <c r="D76" t="inlineStr"/>
+      <c r="D76" t="n">
+        <v>929</v>
+      </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Price Update: Fri Dec 19 13:57:29 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,40 +441,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-19 13:45</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-19 08:56</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 07:42</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 06:11</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Price Change</t>
         </is>
@@ -485,25 +490,26 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>2025-12-19 05:45</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>929</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" t="n">
+        <v>929</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -514,25 +520,26 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>1299</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -543,25 +550,26 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>299</v>
-      </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" t="n">
+        <v>299</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -572,25 +580,26 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
         <is>
           <t>2025-12-19 05:47</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>299</v>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" t="n">
+        <v>299</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -601,25 +610,26 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>499</v>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" t="n">
+        <v>499</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -630,25 +640,26 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>1299</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -659,25 +670,26 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>499</v>
-      </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" t="n">
+        <v>499</v>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -688,25 +700,26 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>2997</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -717,25 +730,26 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G10" t="n">
-        <v>499</v>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" t="n">
+        <v>499</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -746,25 +760,26 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G11" t="n">
-        <v>499</v>
-      </c>
-      <c r="H11" t="inlineStr">
+      <c r="H11" t="n">
+        <v>499</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -775,25 +790,26 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
         <is>
           <t>2025-12-19 05:50</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G12" t="n">
-        <v>929</v>
-      </c>
-      <c r="H12" t="inlineStr">
+      <c r="H12" t="n">
+        <v>929</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -804,25 +820,26 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G13" t="n">
-        <v>569</v>
-      </c>
-      <c r="H13" t="inlineStr">
+      <c r="H13" t="n">
+        <v>569</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -833,25 +850,26 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>299</v>
-      </c>
-      <c r="H14" t="inlineStr">
+      <c r="H14" t="n">
+        <v>299</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -862,25 +880,26 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G15" t="n">
-        <v>929</v>
-      </c>
-      <c r="H15" t="inlineStr">
+      <c r="H15" t="n">
+        <v>929</v>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -891,25 +910,26 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="G16" t="n">
-        <v>299</v>
-      </c>
-      <c r="H16" t="inlineStr">
+      <c r="H16" t="n">
+        <v>299</v>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -920,25 +940,26 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>1299</v>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -949,25 +970,26 @@
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr">
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G18" t="n">
-        <v>499</v>
-      </c>
-      <c r="H18" t="inlineStr">
+      <c r="H18" t="n">
+        <v>499</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -978,25 +1000,26 @@
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr">
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G19" t="n">
-        <v>569</v>
-      </c>
-      <c r="H19" t="inlineStr">
+      <c r="H19" t="n">
+        <v>569</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1007,25 +1030,26 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G20" t="n">
-        <v>929</v>
-      </c>
-      <c r="H20" t="inlineStr">
+      <c r="H20" t="n">
+        <v>929</v>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1036,25 +1060,26 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G21" t="n">
-        <v>569</v>
-      </c>
-      <c r="H21" t="inlineStr">
+      <c r="H21" t="n">
+        <v>569</v>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1065,25 +1090,26 @@
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr">
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
         <is>
           <t>2025-12-19 05:55</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G22" t="n">
-        <v>569</v>
-      </c>
-      <c r="H22" t="inlineStr">
+      <c r="H22" t="n">
+        <v>569</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1094,25 +1120,26 @@
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G23" t="n">
-        <v>929</v>
-      </c>
-      <c r="H23" t="inlineStr">
+      <c r="H23" t="n">
+        <v>929</v>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1123,25 +1150,26 @@
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="G24" t="n">
-        <v>299</v>
-      </c>
-      <c r="H24" t="inlineStr">
+      <c r="H24" t="n">
+        <v>299</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1152,25 +1180,26 @@
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G25" t="n">
-        <v>499</v>
-      </c>
-      <c r="H25" t="inlineStr">
+      <c r="H25" t="n">
+        <v>499</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1181,25 +1210,26 @@
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr">
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G26" t="n">
-        <v>499</v>
-      </c>
-      <c r="H26" t="inlineStr">
+      <c r="H26" t="n">
+        <v>499</v>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1210,25 +1240,26 @@
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr">
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G27" t="n">
-        <v>929</v>
-      </c>
-      <c r="H27" t="inlineStr">
+      <c r="H27" t="n">
+        <v>929</v>
+      </c>
+      <c r="I27" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1239,25 +1270,26 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr">
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G28" t="n">
-        <v>929</v>
-      </c>
-      <c r="H28" t="inlineStr">
+      <c r="H28" t="n">
+        <v>929</v>
+      </c>
+      <c r="I28" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1268,25 +1300,26 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr">
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
         <is>
           <t>2025-12-19 05:27</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G29" t="n">
-        <v>569</v>
-      </c>
-      <c r="H29" t="inlineStr">
+      <c r="H29" t="n">
+        <v>569</v>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1297,25 +1330,26 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr">
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G30" t="n">
-        <v>929</v>
-      </c>
-      <c r="H30" t="inlineStr">
+      <c r="H30" t="n">
+        <v>929</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1326,25 +1360,26 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr">
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G31" t="n">
-        <v>499</v>
-      </c>
-      <c r="H31" t="inlineStr">
+      <c r="H31" t="n">
+        <v>499</v>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
+      <c r="J31" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1355,25 +1390,26 @@
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr">
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G32" t="n">
-        <v>929</v>
-      </c>
-      <c r="H32" t="inlineStr">
+      <c r="H32" t="n">
+        <v>929</v>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1384,25 +1420,26 @@
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr">
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="G33" t="n">
-        <v>299</v>
-      </c>
-      <c r="H33" t="inlineStr">
+      <c r="H33" t="n">
+        <v>299</v>
+      </c>
+      <c r="I33" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="J33" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1413,25 +1450,26 @@
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr">
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>1299</v>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1442,25 +1480,26 @@
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr">
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G35" t="n">
-        <v>499</v>
-      </c>
-      <c r="H35" t="inlineStr">
+      <c r="H35" t="n">
+        <v>499</v>
+      </c>
+      <c r="I35" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="J35" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1471,25 +1510,26 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr">
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G36" t="n">
-        <v>569</v>
-      </c>
-      <c r="H36" t="inlineStr">
+      <c r="H36" t="n">
+        <v>569</v>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="J36" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1500,25 +1540,26 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr">
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="G37" t="n">
-        <v>299</v>
-      </c>
-      <c r="H37" t="inlineStr">
+      <c r="H37" t="n">
+        <v>299</v>
+      </c>
+      <c r="I37" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
+      <c r="J37" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1529,25 +1570,26 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr">
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
         <is>
           <t>2025-12-19 05:31</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>1299</v>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
+      <c r="J38" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1558,25 +1600,26 @@
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr">
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G39" t="n">
-        <v>929</v>
-      </c>
-      <c r="H39" t="inlineStr">
+      <c r="H39" t="n">
+        <v>929</v>
+      </c>
+      <c r="I39" t="inlineStr">
         <is>
           <t>https://amzn.in/d/7mqmyMs</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr">
+      <c r="J39" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1587,25 +1630,26 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr">
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="G40" t="n">
-        <v>299</v>
-      </c>
-      <c r="H40" t="inlineStr">
+      <c r="H40" t="n">
+        <v>299</v>
+      </c>
+      <c r="I40" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="J40" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1616,25 +1660,26 @@
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr">
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>2997</v>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="J41" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1645,25 +1690,26 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr">
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="G42" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G42" t="n">
-        <v>569</v>
-      </c>
-      <c r="H42" t="inlineStr">
+      <c r="H42" t="n">
+        <v>569</v>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
+      <c r="J42" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1674,25 +1720,26 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr">
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>1299</v>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="I43" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
+      <c r="J43" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1703,25 +1750,26 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr">
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="G44" t="n">
-        <v>299</v>
-      </c>
-      <c r="H44" t="inlineStr">
+      <c r="H44" t="n">
+        <v>299</v>
+      </c>
+      <c r="I44" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
+      <c r="J44" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1732,25 +1780,26 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr">
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="G45" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G45" t="n">
-        <v>499</v>
-      </c>
-      <c r="H45" t="inlineStr">
+      <c r="H45" t="n">
+        <v>499</v>
+      </c>
+      <c r="I45" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
+      <c r="J45" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1761,25 +1810,26 @@
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr">
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G46" t="n">
-        <v>569</v>
-      </c>
-      <c r="H46" t="inlineStr">
+      <c r="H46" t="n">
+        <v>569</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>https://amzn.in/d/eQdsGNY</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr">
+      <c r="J46" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1790,25 +1840,26 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr">
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G47" t="n">
-        <v>569</v>
-      </c>
-      <c r="H47" t="inlineStr">
+      <c r="H47" t="n">
+        <v>569</v>
+      </c>
+      <c r="I47" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
+      <c r="J47" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1819,25 +1870,26 @@
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr">
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="G48" t="n">
-        <v>299</v>
-      </c>
-      <c r="H48" t="inlineStr">
+      <c r="H48" t="n">
+        <v>299</v>
+      </c>
+      <c r="I48" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="J48" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1848,25 +1900,26 @@
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="G49" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G49" t="n">
-        <v>929</v>
-      </c>
-      <c r="H49" t="inlineStr">
+      <c r="H49" t="n">
+        <v>929</v>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="J49" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1877,50 +1930,52 @@
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr">
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr">
         <is>
           <t>2025-12-18 20:22</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="G50" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="G50" t="n">
-        <v>499</v>
-      </c>
-      <c r="H50" t="inlineStr">
+      <c r="H50" t="n">
+        <v>499</v>
+      </c>
+      <c r="I50" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr">
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr">
         <is>
           <t>2025-12-18 20:24</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="G51" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="G51" t="n">
-        <v>569</v>
-      </c>
-      <c r="H51" t="inlineStr">
+      <c r="H51" t="n">
+        <v>569</v>
+      </c>
+      <c r="I51" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1937,11 +1992,14 @@
       <c r="D52" t="n">
         <v>499</v>
       </c>
-      <c r="E52" t="inlineStr"/>
+      <c r="E52" t="n">
+        <v>499</v>
+      </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1958,11 +2016,14 @@
       <c r="D53" t="n">
         <v>299</v>
       </c>
-      <c r="E53" t="inlineStr"/>
+      <c r="E53" t="n">
+        <v>299</v>
+      </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1979,11 +2040,14 @@
       <c r="D54" t="n">
         <v>299</v>
       </c>
-      <c r="E54" t="inlineStr"/>
+      <c r="E54" t="n">
+        <v>299</v>
+      </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2000,11 +2064,14 @@
       <c r="D55" t="n">
         <v>569</v>
       </c>
-      <c r="E55" t="inlineStr"/>
+      <c r="E55" t="n">
+        <v>569</v>
+      </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2021,11 +2088,14 @@
       <c r="D56" t="n">
         <v>569</v>
       </c>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="n">
+        <v>569</v>
+      </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2034,7 +2104,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1299</v>
+        <v>2997</v>
       </c>
       <c r="C57" t="n">
         <v>1299</v>
@@ -2042,11 +2112,14 @@
       <c r="D57" t="n">
         <v>1299</v>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="n">
+        <v>1299</v>
+      </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2063,11 +2136,14 @@
       <c r="D58" t="n">
         <v>1299</v>
       </c>
-      <c r="E58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>1299</v>
+      </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2084,11 +2160,14 @@
       <c r="D59" t="n">
         <v>1299</v>
       </c>
-      <c r="E59" t="inlineStr"/>
+      <c r="E59" t="n">
+        <v>1299</v>
+      </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2105,11 +2184,14 @@
       <c r="D60" t="n">
         <v>929</v>
       </c>
-      <c r="E60" t="inlineStr"/>
+      <c r="E60" t="n">
+        <v>929</v>
+      </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2126,11 +2208,14 @@
       <c r="D61" t="n">
         <v>499</v>
       </c>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>499</v>
+      </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2147,11 +2232,14 @@
       <c r="D62" t="n">
         <v>569</v>
       </c>
-      <c r="E62" t="inlineStr"/>
+      <c r="E62" t="n">
+        <v>569</v>
+      </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2168,11 +2256,14 @@
       <c r="D63" t="n">
         <v>299</v>
       </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>299</v>
+      </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2189,11 +2280,14 @@
       <c r="D64" t="n">
         <v>499</v>
       </c>
-      <c r="E64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>499</v>
+      </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2210,11 +2304,14 @@
       <c r="D65" t="n">
         <v>299</v>
       </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>299</v>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2222,18 +2319,21 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="n">
+      <c r="B66" t="n">
         <v>2997</v>
       </c>
+      <c r="C66" t="inlineStr"/>
       <c r="D66" t="n">
         <v>2997</v>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>2997</v>
+      </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2241,20 +2341,21 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B67" t="n">
-        <v>499</v>
-      </c>
+      <c r="B67" t="inlineStr"/>
       <c r="C67" t="n">
         <v>499</v>
       </c>
       <c r="D67" t="n">
         <v>499</v>
       </c>
-      <c r="E67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>499</v>
+      </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2271,11 +2372,14 @@
       <c r="D68" t="n">
         <v>499</v>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="n">
+        <v>499</v>
+      </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2283,20 +2387,21 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B69" t="n">
-        <v>929</v>
-      </c>
+      <c r="B69" t="inlineStr"/>
       <c r="C69" t="n">
         <v>929</v>
       </c>
       <c r="D69" t="n">
         <v>929</v>
       </c>
-      <c r="E69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>929</v>
+      </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2313,11 +2418,14 @@
       <c r="D70" t="n">
         <v>929</v>
       </c>
-      <c r="E70" t="inlineStr"/>
+      <c r="E70" t="n">
+        <v>929</v>
+      </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2328,15 +2436,18 @@
       <c r="B71" t="n">
         <v>299</v>
       </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="n">
-        <v>299</v>
-      </c>
-      <c r="E71" t="inlineStr"/>
+      <c r="C71" t="n">
+        <v>299</v>
+      </c>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>299</v>
+      </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2353,11 +2464,14 @@
       <c r="D72" t="n">
         <v>929</v>
       </c>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>929</v>
+      </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2374,11 +2488,14 @@
       <c r="D73" t="n">
         <v>569</v>
       </c>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>569</v>
+      </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2395,11 +2512,14 @@
       <c r="D74" t="n">
         <v>929</v>
       </c>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>929</v>
+      </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2416,11 +2536,14 @@
       <c r="D75" t="n">
         <v>569</v>
       </c>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>569</v>
+      </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2437,11 +2560,14 @@
       <c r="D76" t="n">
         <v>929</v>
       </c>
-      <c r="E76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>929</v>
+      </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Price Update: Fri Dec 19 17:05:20 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,45 +441,50 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-19 16:54</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-19 13:45</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 08:56</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 07:42</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 06:11</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Price Change</t>
         </is>
@@ -491,25 +496,26 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
         <is>
           <t>2025-12-19 05:45</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>929</v>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" t="n">
+        <v>929</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -521,25 +527,26 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>1299</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -551,25 +558,26 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="H4" t="n">
-        <v>299</v>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>299</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -581,25 +589,26 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>2025-12-19 05:47</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="H5" t="n">
-        <v>299</v>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" t="n">
+        <v>299</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -611,25 +620,26 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H6" t="n">
-        <v>499</v>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" t="n">
+        <v>499</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -641,25 +651,26 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>1299</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -671,25 +682,26 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H8" t="n">
-        <v>499</v>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" t="n">
+        <v>499</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -701,25 +713,26 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>2997</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -731,25 +744,26 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H10" t="n">
-        <v>499</v>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" t="n">
+        <v>499</v>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -761,25 +775,26 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H11" t="n">
-        <v>499</v>
-      </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" t="n">
+        <v>499</v>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -791,25 +806,26 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
         <is>
           <t>2025-12-19 05:50</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H12" t="n">
-        <v>929</v>
-      </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" t="n">
+        <v>929</v>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -821,25 +837,26 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H13" t="n">
-        <v>569</v>
-      </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" t="n">
+        <v>569</v>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -851,25 +868,26 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="H14" t="n">
-        <v>299</v>
-      </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" t="n">
+        <v>299</v>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -881,25 +899,26 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H15" t="n">
-        <v>929</v>
-      </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" t="n">
+        <v>929</v>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -911,25 +930,26 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="H16" t="n">
-        <v>299</v>
-      </c>
-      <c r="I16" t="inlineStr">
+      <c r="I16" t="n">
+        <v>299</v>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -941,25 +961,26 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>1299</v>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -971,25 +992,26 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H18" t="n">
-        <v>499</v>
-      </c>
-      <c r="I18" t="inlineStr">
+      <c r="I18" t="n">
+        <v>499</v>
+      </c>
+      <c r="J18" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1001,25 +1023,26 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H19" t="n">
-        <v>569</v>
-      </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" t="n">
+        <v>569</v>
+      </c>
+      <c r="J19" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1031,25 +1054,26 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H20" t="n">
-        <v>929</v>
-      </c>
-      <c r="I20" t="inlineStr">
+      <c r="I20" t="n">
+        <v>929</v>
+      </c>
+      <c r="J20" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1061,25 +1085,26 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H21" t="n">
-        <v>569</v>
-      </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" t="n">
+        <v>569</v>
+      </c>
+      <c r="J21" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1091,25 +1116,26 @@
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
         <is>
           <t>2025-12-19 05:55</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H22" t="n">
-        <v>569</v>
-      </c>
-      <c r="I22" t="inlineStr">
+      <c r="I22" t="n">
+        <v>569</v>
+      </c>
+      <c r="J22" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="K22" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1121,25 +1147,26 @@
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr">
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H23" t="n">
-        <v>929</v>
-      </c>
-      <c r="I23" t="inlineStr">
+      <c r="I23" t="n">
+        <v>929</v>
+      </c>
+      <c r="J23" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1151,25 +1178,26 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="H24" t="n">
-        <v>299</v>
-      </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" t="n">
+        <v>299</v>
+      </c>
+      <c r="J24" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1181,25 +1209,26 @@
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr">
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H25" t="n">
-        <v>499</v>
-      </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" t="n">
+        <v>499</v>
+      </c>
+      <c r="J25" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1211,25 +1240,26 @@
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr">
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H26" t="n">
-        <v>499</v>
-      </c>
-      <c r="I26" t="inlineStr">
+      <c r="I26" t="n">
+        <v>499</v>
+      </c>
+      <c r="J26" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1241,25 +1271,26 @@
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr">
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H27" t="n">
-        <v>929</v>
-      </c>
-      <c r="I27" t="inlineStr">
+      <c r="I27" t="n">
+        <v>929</v>
+      </c>
+      <c r="J27" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1271,25 +1302,26 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H28" t="n">
-        <v>929</v>
-      </c>
-      <c r="I28" t="inlineStr">
+      <c r="I28" t="n">
+        <v>929</v>
+      </c>
+      <c r="J28" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="K28" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1301,25 +1333,26 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
         <is>
           <t>2025-12-19 05:27</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H29" t="n">
-        <v>569</v>
-      </c>
-      <c r="I29" t="inlineStr">
+      <c r="I29" t="n">
+        <v>569</v>
+      </c>
+      <c r="J29" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1331,25 +1364,26 @@
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr">
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H30" t="n">
-        <v>929</v>
-      </c>
-      <c r="I30" t="inlineStr">
+      <c r="I30" t="n">
+        <v>929</v>
+      </c>
+      <c r="J30" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="K30" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1361,25 +1395,26 @@
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr">
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H31" t="n">
-        <v>499</v>
-      </c>
-      <c r="I31" t="inlineStr">
+      <c r="I31" t="n">
+        <v>499</v>
+      </c>
+      <c r="J31" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="K31" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1391,25 +1426,26 @@
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr">
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H32" t="n">
-        <v>929</v>
-      </c>
-      <c r="I32" t="inlineStr">
+      <c r="I32" t="n">
+        <v>929</v>
+      </c>
+      <c r="J32" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="K32" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1421,25 +1457,26 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr">
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="H33" t="n">
-        <v>299</v>
-      </c>
-      <c r="I33" t="inlineStr">
+      <c r="I33" t="n">
+        <v>299</v>
+      </c>
+      <c r="J33" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="K33" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1451,25 +1488,26 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr">
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>1299</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="K34" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1481,25 +1519,26 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H35" t="n">
-        <v>499</v>
-      </c>
-      <c r="I35" t="inlineStr">
+      <c r="I35" t="n">
+        <v>499</v>
+      </c>
+      <c r="J35" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="K35" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1511,25 +1550,26 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr">
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H36" t="n">
-        <v>569</v>
-      </c>
-      <c r="I36" t="inlineStr">
+      <c r="I36" t="n">
+        <v>569</v>
+      </c>
+      <c r="J36" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="K36" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1541,25 +1581,26 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr">
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="H37" t="n">
-        <v>299</v>
-      </c>
-      <c r="I37" t="inlineStr">
+      <c r="I37" t="n">
+        <v>299</v>
+      </c>
+      <c r="J37" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="K37" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1571,25 +1612,26 @@
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr">
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
         <is>
           <t>2025-12-19 05:31</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>1299</v>
       </c>
-      <c r="I38" t="inlineStr">
+      <c r="J38" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="K38" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1601,25 +1643,26 @@
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H39" t="n">
-        <v>929</v>
-      </c>
-      <c r="I39" t="inlineStr">
+      <c r="I39" t="n">
+        <v>929</v>
+      </c>
+      <c r="J39" t="inlineStr">
         <is>
           <t>https://amzn.in/d/7mqmyMs</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="K39" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1631,25 +1674,26 @@
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="H40" t="n">
-        <v>299</v>
-      </c>
-      <c r="I40" t="inlineStr">
+      <c r="I40" t="n">
+        <v>299</v>
+      </c>
+      <c r="J40" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="K40" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1661,25 +1705,26 @@
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr">
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>2997</v>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="J41" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="K41" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1691,25 +1736,26 @@
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr">
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H42" t="n">
-        <v>569</v>
-      </c>
-      <c r="I42" t="inlineStr">
+      <c r="I42" t="n">
+        <v>569</v>
+      </c>
+      <c r="J42" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="K42" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1721,25 +1767,26 @@
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>1299</v>
       </c>
-      <c r="I43" t="inlineStr">
+      <c r="J43" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="K43" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1751,25 +1798,26 @@
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr">
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="H44" t="n">
-        <v>299</v>
-      </c>
-      <c r="I44" t="inlineStr">
+      <c r="I44" t="n">
+        <v>299</v>
+      </c>
+      <c r="J44" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="K44" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1781,25 +1829,26 @@
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr">
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H45" t="n">
-        <v>499</v>
-      </c>
-      <c r="I45" t="inlineStr">
+      <c r="I45" t="n">
+        <v>499</v>
+      </c>
+      <c r="J45" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="K45" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1811,25 +1860,26 @@
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H46" t="n">
-        <v>569</v>
-      </c>
-      <c r="I46" t="inlineStr">
+      <c r="I46" t="n">
+        <v>569</v>
+      </c>
+      <c r="J46" t="inlineStr">
         <is>
           <t>https://amzn.in/d/eQdsGNY</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="K46" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1841,25 +1891,26 @@
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H47" t="n">
-        <v>569</v>
-      </c>
-      <c r="I47" t="inlineStr">
+      <c r="I47" t="n">
+        <v>569</v>
+      </c>
+      <c r="J47" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="J47" t="inlineStr">
+      <c r="K47" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1871,25 +1922,26 @@
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr">
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="H48" t="n">
-        <v>299</v>
-      </c>
-      <c r="I48" t="inlineStr">
+      <c r="I48" t="n">
+        <v>299</v>
+      </c>
+      <c r="J48" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="K48" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1901,25 +1953,26 @@
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr">
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="H49" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H49" t="n">
-        <v>929</v>
-      </c>
-      <c r="I49" t="inlineStr">
+      <c r="I49" t="n">
+        <v>929</v>
+      </c>
+      <c r="J49" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="J49" t="inlineStr">
+      <c r="K49" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1931,25 +1984,26 @@
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr">
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
         <is>
           <t>2025-12-18 20:22</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="H50" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="H50" t="n">
-        <v>499</v>
-      </c>
-      <c r="I50" t="inlineStr">
+      <c r="I50" t="n">
+        <v>499</v>
+      </c>
+      <c r="J50" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
@@ -1957,25 +2011,26 @@
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr">
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
         <is>
           <t>2025-12-18 20:24</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="H51" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="H51" t="n">
-        <v>569</v>
-      </c>
-      <c r="I51" t="inlineStr">
+      <c r="I51" t="n">
+        <v>569</v>
+      </c>
+      <c r="J51" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1995,11 +2050,14 @@
       <c r="E52" t="n">
         <v>499</v>
       </c>
-      <c r="F52" t="inlineStr"/>
+      <c r="F52" t="n">
+        <v>499</v>
+      </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2019,11 +2077,14 @@
       <c r="E53" t="n">
         <v>299</v>
       </c>
-      <c r="F53" t="inlineStr"/>
+      <c r="F53" t="n">
+        <v>299</v>
+      </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2043,11 +2104,14 @@
       <c r="E54" t="n">
         <v>299</v>
       </c>
-      <c r="F54" t="inlineStr"/>
+      <c r="F54" t="n">
+        <v>299</v>
+      </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2067,11 +2131,14 @@
       <c r="E55" t="n">
         <v>569</v>
       </c>
-      <c r="F55" t="inlineStr"/>
+      <c r="F55" t="n">
+        <v>569</v>
+      </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2091,11 +2158,14 @@
       <c r="E56" t="n">
         <v>569</v>
       </c>
-      <c r="F56" t="inlineStr"/>
+      <c r="F56" t="n">
+        <v>569</v>
+      </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2107,7 +2177,7 @@
         <v>2997</v>
       </c>
       <c r="C57" t="n">
-        <v>1299</v>
+        <v>2997</v>
       </c>
       <c r="D57" t="n">
         <v>1299</v>
@@ -2115,11 +2185,14 @@
       <c r="E57" t="n">
         <v>1299</v>
       </c>
-      <c r="F57" t="inlineStr"/>
+      <c r="F57" t="n">
+        <v>1299</v>
+      </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2139,11 +2212,14 @@
       <c r="E58" t="n">
         <v>1299</v>
       </c>
-      <c r="F58" t="inlineStr"/>
+      <c r="F58" t="n">
+        <v>1299</v>
+      </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2163,11 +2239,14 @@
       <c r="E59" t="n">
         <v>1299</v>
       </c>
-      <c r="F59" t="inlineStr"/>
+      <c r="F59" t="n">
+        <v>1299</v>
+      </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2187,11 +2266,14 @@
       <c r="E60" t="n">
         <v>929</v>
       </c>
-      <c r="F60" t="inlineStr"/>
+      <c r="F60" t="n">
+        <v>929</v>
+      </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2211,11 +2293,14 @@
       <c r="E61" t="n">
         <v>499</v>
       </c>
-      <c r="F61" t="inlineStr"/>
+      <c r="F61" t="n">
+        <v>499</v>
+      </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2235,11 +2320,14 @@
       <c r="E62" t="n">
         <v>569</v>
       </c>
-      <c r="F62" t="inlineStr"/>
+      <c r="F62" t="n">
+        <v>569</v>
+      </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2259,11 +2347,14 @@
       <c r="E63" t="n">
         <v>299</v>
       </c>
-      <c r="F63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>299</v>
+      </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2283,11 +2374,14 @@
       <c r="E64" t="n">
         <v>499</v>
       </c>
-      <c r="F64" t="inlineStr"/>
+      <c r="F64" t="n">
+        <v>499</v>
+      </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2307,11 +2401,14 @@
       <c r="E65" t="n">
         <v>299</v>
       </c>
-      <c r="F65" t="inlineStr"/>
+      <c r="F65" t="n">
+        <v>299</v>
+      </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2320,20 +2417,23 @@
         </is>
       </c>
       <c r="B66" t="n">
+        <v>929</v>
+      </c>
+      <c r="C66" t="n">
         <v>2997</v>
       </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="n">
-        <v>2997</v>
-      </c>
+      <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
         <v>2997</v>
       </c>
-      <c r="F66" t="inlineStr"/>
+      <c r="F66" t="n">
+        <v>2997</v>
+      </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2341,21 +2441,24 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="n">
-        <v>499</v>
-      </c>
+      <c r="B67" t="n">
+        <v>499</v>
+      </c>
+      <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
         <v>499</v>
       </c>
       <c r="E67" t="n">
         <v>499</v>
       </c>
-      <c r="F67" t="inlineStr"/>
+      <c r="F67" t="n">
+        <v>499</v>
+      </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2375,11 +2478,14 @@
       <c r="E68" t="n">
         <v>499</v>
       </c>
-      <c r="F68" t="inlineStr"/>
+      <c r="F68" t="n">
+        <v>499</v>
+      </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2387,21 +2493,24 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="n">
-        <v>929</v>
-      </c>
+      <c r="B69" t="n">
+        <v>929</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
       <c r="D69" t="n">
         <v>929</v>
       </c>
       <c r="E69" t="n">
         <v>929</v>
       </c>
-      <c r="F69" t="inlineStr"/>
+      <c r="F69" t="n">
+        <v>929</v>
+      </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2421,11 +2530,14 @@
       <c r="E70" t="n">
         <v>929</v>
       </c>
-      <c r="F70" t="inlineStr"/>
+      <c r="F70" t="n">
+        <v>929</v>
+      </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2439,15 +2551,18 @@
       <c r="C71" t="n">
         <v>299</v>
       </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="n">
-        <v>299</v>
-      </c>
-      <c r="F71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>299</v>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="n">
+        <v>299</v>
+      </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2467,11 +2582,14 @@
       <c r="E72" t="n">
         <v>929</v>
       </c>
-      <c r="F72" t="inlineStr"/>
+      <c r="F72" t="n">
+        <v>929</v>
+      </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2491,11 +2609,14 @@
       <c r="E73" t="n">
         <v>569</v>
       </c>
-      <c r="F73" t="inlineStr"/>
+      <c r="F73" t="n">
+        <v>569</v>
+      </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2515,11 +2636,14 @@
       <c r="E74" t="n">
         <v>929</v>
       </c>
-      <c r="F74" t="inlineStr"/>
+      <c r="F74" t="n">
+        <v>929</v>
+      </c>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2539,11 +2663,14 @@
       <c r="E75" t="n">
         <v>569</v>
       </c>
-      <c r="F75" t="inlineStr"/>
+      <c r="F75" t="n">
+        <v>569</v>
+      </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2563,11 +2690,14 @@
       <c r="E76" t="n">
         <v>929</v>
       </c>
-      <c r="F76" t="inlineStr"/>
+      <c r="F76" t="n">
+        <v>929</v>
+      </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Price Update: Fri Dec 19 20:52:29 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,50 +441,55 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-19 20:41</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-19 16:54</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 13:45</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 08:56</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 07:42</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-19 06:11</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Price Change</t>
         </is>
@@ -497,25 +502,26 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
         <is>
           <t>2025-12-19 05:45</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>929</v>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="n">
+        <v>929</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -528,25 +534,26 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>1299</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -559,25 +566,26 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
         <is>
           <t>2025-12-19 05:46</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>299</v>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" t="n">
+        <v>299</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -590,25 +598,26 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
         <is>
           <t>2025-12-19 05:47</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="I5" t="n">
-        <v>299</v>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" t="n">
+        <v>299</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -621,25 +630,26 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I6" t="n">
-        <v>499</v>
-      </c>
-      <c r="J6" t="inlineStr">
+      <c r="J6" t="n">
+        <v>499</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -652,25 +662,26 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>1299</v>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -683,25 +694,26 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
         <is>
           <t>2025-12-19 05:48</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I8" t="n">
-        <v>499</v>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="J8" t="n">
+        <v>499</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -714,25 +726,26 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr">
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>2997</v>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -745,25 +758,26 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I10" t="n">
-        <v>499</v>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="J10" t="n">
+        <v>499</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -776,25 +790,26 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
         <is>
           <t>2025-12-19 05:49</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I11" t="n">
-        <v>499</v>
-      </c>
-      <c r="J11" t="inlineStr">
+      <c r="J11" t="n">
+        <v>499</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -807,25 +822,26 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
         <is>
           <t>2025-12-19 05:50</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I12" t="n">
-        <v>929</v>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="J12" t="n">
+        <v>929</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -838,25 +854,26 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I13" t="n">
-        <v>569</v>
-      </c>
-      <c r="J13" t="inlineStr">
+      <c r="J13" t="n">
+        <v>569</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -869,25 +886,26 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
         <is>
           <t>2025-12-19 05:51</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="I14" t="n">
-        <v>299</v>
-      </c>
-      <c r="J14" t="inlineStr">
+      <c r="J14" t="n">
+        <v>299</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -900,25 +918,26 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr">
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I15" t="n">
-        <v>929</v>
-      </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" t="n">
+        <v>929</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -931,25 +950,26 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="I16" t="n">
-        <v>299</v>
-      </c>
-      <c r="J16" t="inlineStr">
+      <c r="J16" t="n">
+        <v>299</v>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -962,25 +982,26 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
         <is>
           <t>2025-12-19 05:52</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>1299</v>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -993,25 +1014,26 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr">
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I18" t="n">
-        <v>499</v>
-      </c>
-      <c r="J18" t="inlineStr">
+      <c r="J18" t="n">
+        <v>499</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1024,25 +1046,26 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr">
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
         <is>
           <t>2025-12-19 05:53</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I19" t="n">
-        <v>569</v>
-      </c>
-      <c r="J19" t="inlineStr">
+      <c r="J19" t="n">
+        <v>569</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1055,25 +1078,26 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I20" t="n">
-        <v>929</v>
-      </c>
-      <c r="J20" t="inlineStr">
+      <c r="J20" t="n">
+        <v>929</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1086,25 +1110,26 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
         <is>
           <t>2025-12-19 05:54</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I21" t="n">
-        <v>569</v>
-      </c>
-      <c r="J21" t="inlineStr">
+      <c r="J21" t="n">
+        <v>569</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1117,25 +1142,26 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
         <is>
           <t>2025-12-19 05:55</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I22" t="n">
-        <v>569</v>
-      </c>
-      <c r="J22" t="inlineStr">
+      <c r="J22" t="n">
+        <v>569</v>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1148,25 +1174,26 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I23" t="n">
-        <v>929</v>
-      </c>
-      <c r="J23" t="inlineStr">
+      <c r="J23" t="n">
+        <v>929</v>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1179,25 +1206,26 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
         <is>
           <t>2025-12-19 05:56</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="I24" t="n">
-        <v>299</v>
-      </c>
-      <c r="J24" t="inlineStr">
+      <c r="J24" t="n">
+        <v>299</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1210,25 +1238,26 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I25" t="n">
-        <v>499</v>
-      </c>
-      <c r="J25" t="inlineStr">
+      <c r="J25" t="n">
+        <v>499</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0D9RJyQ</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1241,25 +1270,26 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr">
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
         <is>
           <t>2025-12-19 05:25</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I26" t="n">
-        <v>499</v>
-      </c>
-      <c r="J26" t="inlineStr">
+      <c r="J26" t="n">
+        <v>499</v>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1272,25 +1302,26 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr">
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I27" t="n">
-        <v>929</v>
-      </c>
-      <c r="J27" t="inlineStr">
+      <c r="J27" t="n">
+        <v>929</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>https://amzn.in/d/9Vmpx9L</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1303,25 +1334,26 @@
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr">
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
         <is>
           <t>2025-12-19 05:26</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I28" t="n">
-        <v>929</v>
-      </c>
-      <c r="J28" t="inlineStr">
+      <c r="J28" t="n">
+        <v>929</v>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>https://amzn.in/d/iUJnAAG</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="L28" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1334,25 +1366,26 @@
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr">
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
         <is>
           <t>2025-12-19 05:27</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I29" t="n">
-        <v>569</v>
-      </c>
-      <c r="J29" t="inlineStr">
+      <c r="J29" t="n">
+        <v>569</v>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8Xctx1i</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1365,25 +1398,26 @@
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr">
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I30" t="n">
-        <v>929</v>
-      </c>
-      <c r="J30" t="inlineStr">
+      <c r="J30" t="n">
+        <v>929</v>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>https://amzn.in/d/isCQv09</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="L30" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1396,25 +1430,26 @@
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr">
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
         <is>
           <t>2025-12-19 05:28</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I31" t="n">
-        <v>499</v>
-      </c>
-      <c r="J31" t="inlineStr">
+      <c r="J31" t="n">
+        <v>499</v>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>https://amzn.in/d/4mstrat</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
+      <c r="L31" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1427,25 +1462,26 @@
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr">
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I32" t="n">
-        <v>929</v>
-      </c>
-      <c r="J32" t="inlineStr">
+      <c r="J32" t="n">
+        <v>929</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8D9SlMj</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1458,25 +1494,26 @@
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr">
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="I33" t="n">
-        <v>299</v>
-      </c>
-      <c r="J33" t="inlineStr">
+      <c r="J33" t="n">
+        <v>299</v>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>https://amzn.in/d/axvUrmf</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="L33" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1489,25 +1526,26 @@
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr">
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
         <is>
           <t>2025-12-19 05:29</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>1299</v>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="K34" t="inlineStr">
         <is>
           <t>https://amzn.in/d/1yTk7TG</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="L34" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1520,25 +1558,26 @@
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr">
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I35" t="n">
-        <v>499</v>
-      </c>
-      <c r="J35" t="inlineStr">
+      <c r="J35" t="n">
+        <v>499</v>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>https://amzn.in/d/aNPi1U2</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="L35" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1551,25 +1590,26 @@
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr">
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I36" t="n">
-        <v>569</v>
-      </c>
-      <c r="J36" t="inlineStr">
+      <c r="J36" t="n">
+        <v>569</v>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr">
+      <c r="L36" t="inlineStr">
         <is>
           <t>Stable</t>
         </is>
@@ -1582,25 +1622,26 @@
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr">
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr">
         <is>
           <t>2025-12-19 05:30</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="I37" t="n">
-        <v>299</v>
-      </c>
-      <c r="J37" t="inlineStr">
+      <c r="J37" t="n">
+        <v>299</v>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bqE35ja</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr">
+      <c r="L37" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1613,25 +1654,26 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr">
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
         <is>
           <t>2025-12-19 05:31</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>1299</v>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="K38" t="inlineStr">
         <is>
           <t>https://amzn.in/d/0V4kPll</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr">
+      <c r="L38" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1644,25 +1686,26 @@
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr">
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I39" t="n">
-        <v>929</v>
-      </c>
-      <c r="J39" t="inlineStr">
+      <c r="J39" t="n">
+        <v>929</v>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>https://amzn.in/d/7mqmyMs</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr">
+      <c r="L39" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1675,25 +1718,26 @@
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr">
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
         <is>
           <t>2025-12-19 05:32</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="I40" t="n">
-        <v>299</v>
-      </c>
-      <c r="J40" t="inlineStr">
+      <c r="J40" t="n">
+        <v>299</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>https://amzn.in/d/bGuw5EZ</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr">
+      <c r="L40" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1706,25 +1750,26 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr">
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>2997</v>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="K41" t="inlineStr">
         <is>
           <t>https://amzn.in/d/5fRuGGr</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr">
+      <c r="L41" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1737,25 +1782,26 @@
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr">
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
         <is>
           <t>2025-12-19 05:33</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
+      <c r="I42" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I42" t="n">
-        <v>569</v>
-      </c>
-      <c r="J42" t="inlineStr">
+      <c r="J42" t="n">
+        <v>569</v>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>https://amzn.in/d/amDxu6e</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
+      <c r="L42" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1768,25 +1814,26 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr">
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="I43" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I43" t="n">
+      <c r="J43" t="n">
         <v>1299</v>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="K43" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fCdbdzb</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr">
+      <c r="L43" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1799,25 +1846,26 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr">
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="I44" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="I44" t="n">
-        <v>299</v>
-      </c>
-      <c r="J44" t="inlineStr">
+      <c r="J44" t="n">
+        <v>299</v>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>https://amzn.in/d/i9MHRbf</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="L44" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1830,25 +1878,26 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr">
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
         <is>
           <t>2025-12-19 05:34</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
+      <c r="I45" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I45" t="n">
-        <v>499</v>
-      </c>
-      <c r="J45" t="inlineStr">
+      <c r="J45" t="n">
+        <v>499</v>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>https://amzn.in/d/d8JD7Ef</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr">
+      <c r="L45" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1861,25 +1910,26 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr">
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="I46" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I46" t="n">
-        <v>569</v>
-      </c>
-      <c r="J46" t="inlineStr">
+      <c r="J46" t="n">
+        <v>569</v>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>https://amzn.in/d/eQdsGNY</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr">
+      <c r="L46" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1892,25 +1942,26 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr">
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
         <is>
           <t>2025-12-19 05:35</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
+      <c r="I47" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I47" t="n">
-        <v>569</v>
-      </c>
-      <c r="J47" t="inlineStr">
+      <c r="J47" t="n">
+        <v>569</v>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fETFYB9</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr">
+      <c r="L47" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1923,25 +1974,26 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr">
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="I48" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="I48" t="n">
-        <v>299</v>
-      </c>
-      <c r="J48" t="inlineStr">
+      <c r="J48" t="n">
+        <v>299</v>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>https://amzn.in/d/fGRPZHm</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr">
+      <c r="L48" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1954,25 +2006,26 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr">
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
         <is>
           <t>2025-12-19 05:36</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="I49" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I49" t="n">
-        <v>929</v>
-      </c>
-      <c r="J49" t="inlineStr">
+      <c r="J49" t="n">
+        <v>929</v>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>https://amzn.in/d/27dBhA1</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr">
+      <c r="L49" t="inlineStr">
         <is>
           <t>New Record</t>
         </is>
@@ -1985,25 +2038,26 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr">
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
         <is>
           <t>2025-12-18 20:22</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="I50" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="I50" t="n">
-        <v>499</v>
-      </c>
-      <c r="J50" t="inlineStr">
+      <c r="J50" t="n">
+        <v>499</v>
+      </c>
+      <c r="K50" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8DkcqwJ</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
@@ -2012,25 +2066,26 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr">
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
         <is>
           <t>2025-12-18 20:24</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="I51" t="inlineStr">
         <is>
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="I51" t="n">
-        <v>569</v>
-      </c>
-      <c r="J51" t="inlineStr">
+      <c r="J51" t="n">
+        <v>569</v>
+      </c>
+      <c r="K51" t="inlineStr">
         <is>
           <t>https://amzn.in/d/8MCAq5Z</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2053,11 +2108,14 @@
       <c r="F52" t="n">
         <v>499</v>
       </c>
-      <c r="G52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>499</v>
+      </c>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2080,11 +2138,14 @@
       <c r="F53" t="n">
         <v>299</v>
       </c>
-      <c r="G53" t="inlineStr"/>
+      <c r="G53" t="n">
+        <v>299</v>
+      </c>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2107,11 +2168,14 @@
       <c r="F54" t="n">
         <v>299</v>
       </c>
-      <c r="G54" t="inlineStr"/>
+      <c r="G54" t="n">
+        <v>299</v>
+      </c>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2134,11 +2198,14 @@
       <c r="F55" t="n">
         <v>569</v>
       </c>
-      <c r="G55" t="inlineStr"/>
+      <c r="G55" t="n">
+        <v>569</v>
+      </c>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2161,11 +2228,14 @@
       <c r="F56" t="n">
         <v>569</v>
       </c>
-      <c r="G56" t="inlineStr"/>
+      <c r="G56" t="n">
+        <v>569</v>
+      </c>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2180,7 +2250,7 @@
         <v>2997</v>
       </c>
       <c r="D57" t="n">
-        <v>1299</v>
+        <v>2997</v>
       </c>
       <c r="E57" t="n">
         <v>1299</v>
@@ -2188,11 +2258,14 @@
       <c r="F57" t="n">
         <v>1299</v>
       </c>
-      <c r="G57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>1299</v>
+      </c>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2215,11 +2288,14 @@
       <c r="F58" t="n">
         <v>1299</v>
       </c>
-      <c r="G58" t="inlineStr"/>
+      <c r="G58" t="n">
+        <v>1299</v>
+      </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2242,11 +2318,14 @@
       <c r="F59" t="n">
         <v>1299</v>
       </c>
-      <c r="G59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>1299</v>
+      </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2269,11 +2348,14 @@
       <c r="F60" t="n">
         <v>929</v>
       </c>
-      <c r="G60" t="inlineStr"/>
+      <c r="G60" t="n">
+        <v>929</v>
+      </c>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2296,11 +2378,14 @@
       <c r="F61" t="n">
         <v>499</v>
       </c>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="n">
+        <v>499</v>
+      </c>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2323,11 +2408,14 @@
       <c r="F62" t="n">
         <v>569</v>
       </c>
-      <c r="G62" t="inlineStr"/>
+      <c r="G62" t="n">
+        <v>569</v>
+      </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2350,11 +2438,14 @@
       <c r="F63" t="n">
         <v>299</v>
       </c>
-      <c r="G63" t="inlineStr"/>
+      <c r="G63" t="n">
+        <v>299</v>
+      </c>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2377,11 +2468,14 @@
       <c r="F64" t="n">
         <v>499</v>
       </c>
-      <c r="G64" t="inlineStr"/>
+      <c r="G64" t="n">
+        <v>499</v>
+      </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2404,11 +2498,14 @@
       <c r="F65" t="n">
         <v>299</v>
       </c>
-      <c r="G65" t="inlineStr"/>
+      <c r="G65" t="n">
+        <v>299</v>
+      </c>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2420,20 +2517,23 @@
         <v>929</v>
       </c>
       <c r="C66" t="n">
+        <v>929</v>
+      </c>
+      <c r="D66" t="n">
         <v>2997</v>
       </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="n">
-        <v>2997</v>
-      </c>
+      <c r="E66" t="inlineStr"/>
       <c r="F66" t="n">
         <v>2997</v>
       </c>
-      <c r="G66" t="inlineStr"/>
+      <c r="G66" t="n">
+        <v>2997</v>
+      </c>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2444,21 +2544,24 @@
       <c r="B67" t="n">
         <v>499</v>
       </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="n">
-        <v>499</v>
-      </c>
+      <c r="C67" t="n">
+        <v>499</v>
+      </c>
+      <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
         <v>499</v>
       </c>
       <c r="F67" t="n">
         <v>499</v>
       </c>
-      <c r="G67" t="inlineStr"/>
+      <c r="G67" t="n">
+        <v>499</v>
+      </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2481,11 +2584,14 @@
       <c r="F68" t="n">
         <v>499</v>
       </c>
-      <c r="G68" t="inlineStr"/>
+      <c r="G68" t="n">
+        <v>499</v>
+      </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2496,21 +2602,24 @@
       <c r="B69" t="n">
         <v>929</v>
       </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="n">
-        <v>929</v>
-      </c>
+      <c r="C69" t="n">
+        <v>929</v>
+      </c>
+      <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
         <v>929</v>
       </c>
       <c r="F69" t="n">
         <v>929</v>
       </c>
-      <c r="G69" t="inlineStr"/>
+      <c r="G69" t="n">
+        <v>929</v>
+      </c>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2533,11 +2642,14 @@
       <c r="F70" t="n">
         <v>929</v>
       </c>
-      <c r="G70" t="inlineStr"/>
+      <c r="G70" t="n">
+        <v>929</v>
+      </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2554,15 +2666,18 @@
       <c r="D71" t="n">
         <v>299</v>
       </c>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="n">
-        <v>299</v>
-      </c>
-      <c r="G71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>299</v>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="n">
+        <v>299</v>
+      </c>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2585,11 +2700,14 @@
       <c r="F72" t="n">
         <v>929</v>
       </c>
-      <c r="G72" t="inlineStr"/>
+      <c r="G72" t="n">
+        <v>929</v>
+      </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2612,11 +2730,14 @@
       <c r="F73" t="n">
         <v>569</v>
       </c>
-      <c r="G73" t="inlineStr"/>
+      <c r="G73" t="n">
+        <v>569</v>
+      </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2639,11 +2760,14 @@
       <c r="F74" t="n">
         <v>929</v>
       </c>
-      <c r="G74" t="inlineStr"/>
+      <c r="G74" t="n">
+        <v>929</v>
+      </c>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2666,11 +2790,14 @@
       <c r="F75" t="n">
         <v>569</v>
       </c>
-      <c r="G75" t="inlineStr"/>
+      <c r="G75" t="n">
+        <v>569</v>
+      </c>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2693,11 +2820,14 @@
       <c r="F76" t="n">
         <v>929</v>
       </c>
-      <c r="G76" t="inlineStr"/>
+      <c r="G76" t="n">
+        <v>929</v>
+      </c>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Price Update: Sat Dec 20 17:12:25 UTC 2025
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,6 +435,7 @@
   <cols>
     <col width="197" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -445,6 +446,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-20 22:00</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-20 13:20</t>
         </is>
       </c>
@@ -458,6 +464,9 @@
       <c r="B2" t="n">
         <v>929</v>
       </c>
+      <c r="C2" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +477,9 @@
       <c r="B3" t="n">
         <v>569</v>
       </c>
+      <c r="C3" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -478,6 +490,9 @@
       <c r="B4" t="n">
         <v>299</v>
       </c>
+      <c r="C4" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -488,6 +503,9 @@
       <c r="B5" t="n">
         <v>569</v>
       </c>
+      <c r="C5" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -498,6 +516,9 @@
       <c r="B6" t="n">
         <v>499</v>
       </c>
+      <c r="C6" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -508,6 +529,9 @@
       <c r="B7" t="n">
         <v>569</v>
       </c>
+      <c r="C7" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -518,6 +542,9 @@
       <c r="B8" t="n">
         <v>929</v>
       </c>
+      <c r="C8" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -528,6 +555,9 @@
       <c r="B9" t="n">
         <v>299</v>
       </c>
+      <c r="C9" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -538,6 +568,9 @@
       <c r="B10" t="n">
         <v>299</v>
       </c>
+      <c r="C10" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -548,6 +581,9 @@
       <c r="B11" t="n">
         <v>929</v>
       </c>
+      <c r="C11" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -558,6 +594,9 @@
       <c r="B12" t="n">
         <v>569</v>
       </c>
+      <c r="C12" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -568,6 +607,9 @@
       <c r="B13" t="n">
         <v>569</v>
       </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -578,6 +620,9 @@
       <c r="B14" t="n">
         <v>499</v>
       </c>
+      <c r="C14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -588,6 +633,9 @@
       <c r="B15" t="n">
         <v>499</v>
       </c>
+      <c r="C15" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -598,6 +646,9 @@
       <c r="B16" t="n">
         <v>299</v>
       </c>
+      <c r="C16" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -608,6 +659,9 @@
       <c r="B17" t="n">
         <v>929</v>
       </c>
+      <c r="C17" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -618,6 +672,9 @@
       <c r="B18" t="n">
         <v>499</v>
       </c>
+      <c r="C18" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -626,6 +683,9 @@
         </is>
       </c>
       <c r="B19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="C19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -638,6 +698,9 @@
       <c r="B20" t="n">
         <v>929</v>
       </c>
+      <c r="C20" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -648,6 +711,9 @@
       <c r="B21" t="n">
         <v>499</v>
       </c>
+      <c r="C21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -658,6 +724,9 @@
       <c r="B22" t="n">
         <v>299</v>
       </c>
+      <c r="C22" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -668,6 +737,9 @@
       <c r="B23" t="n">
         <v>1299</v>
       </c>
+      <c r="C23" t="n">
+        <v>1299</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -678,6 +750,9 @@
       <c r="B24" t="n">
         <v>929</v>
       </c>
+      <c r="C24" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -688,6 +763,9 @@
       <c r="B25" t="n">
         <v>929</v>
       </c>
+      <c r="C25" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -696,6 +774,9 @@
         </is>
       </c>
       <c r="B26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-20 17:54
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,7 @@
     <col width="197" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -446,10 +447,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-20 23:18</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -467,6 +473,9 @@
       <c r="C2" t="n">
         <v>929</v>
       </c>
+      <c r="D2" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -480,6 +489,9 @@
       <c r="C3" t="n">
         <v>569</v>
       </c>
+      <c r="D3" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -493,6 +505,9 @@
       <c r="C4" t="n">
         <v>299</v>
       </c>
+      <c r="D4" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -506,6 +521,9 @@
       <c r="C5" t="n">
         <v>569</v>
       </c>
+      <c r="D5" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -519,6 +537,9 @@
       <c r="C6" t="n">
         <v>499</v>
       </c>
+      <c r="D6" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -532,6 +553,9 @@
       <c r="C7" t="n">
         <v>569</v>
       </c>
+      <c r="D7" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -545,6 +569,9 @@
       <c r="C8" t="n">
         <v>929</v>
       </c>
+      <c r="D8" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -558,6 +585,9 @@
       <c r="C9" t="n">
         <v>299</v>
       </c>
+      <c r="D9" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -571,6 +601,9 @@
       <c r="C10" t="n">
         <v>299</v>
       </c>
+      <c r="D10" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -584,6 +617,9 @@
       <c r="C11" t="n">
         <v>929</v>
       </c>
+      <c r="D11" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -597,6 +633,9 @@
       <c r="C12" t="n">
         <v>569</v>
       </c>
+      <c r="D12" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -610,6 +649,9 @@
       <c r="C13" t="n">
         <v>569</v>
       </c>
+      <c r="D13" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -623,6 +665,9 @@
       <c r="C14" t="n">
         <v>499</v>
       </c>
+      <c r="D14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -636,6 +681,9 @@
       <c r="C15" t="n">
         <v>499</v>
       </c>
+      <c r="D15" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -649,6 +697,9 @@
       <c r="C16" t="n">
         <v>299</v>
       </c>
+      <c r="D16" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -662,6 +713,9 @@
       <c r="C17" t="n">
         <v>929</v>
       </c>
+      <c r="D17" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -675,6 +729,9 @@
       <c r="C18" t="n">
         <v>499</v>
       </c>
+      <c r="D18" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -686,6 +743,9 @@
         <v>1497</v>
       </c>
       <c r="C19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="D19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -701,6 +761,9 @@
       <c r="C20" t="n">
         <v>929</v>
       </c>
+      <c r="D20" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -714,6 +777,9 @@
       <c r="C21" t="n">
         <v>499</v>
       </c>
+      <c r="D21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -727,6 +793,9 @@
       <c r="C22" t="n">
         <v>299</v>
       </c>
+      <c r="D22" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -740,6 +809,9 @@
       <c r="C23" t="n">
         <v>1299</v>
       </c>
+      <c r="D23" t="n">
+        <v>1299</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -753,6 +825,9 @@
       <c r="C24" t="n">
         <v>929</v>
       </c>
+      <c r="D24" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -766,6 +841,9 @@
       <c r="C25" t="n">
         <v>929</v>
       </c>
+      <c r="D25" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -777,6 +855,9 @@
         <v>1299</v>
       </c>
       <c r="C26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-20 18:07
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,6 +437,7 @@
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -447,15 +448,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-20 23:33</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -476,6 +482,9 @@
       <c r="D2" t="n">
         <v>929</v>
       </c>
+      <c r="E2" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -492,6 +501,9 @@
       <c r="D3" t="n">
         <v>569</v>
       </c>
+      <c r="E3" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -508,6 +520,9 @@
       <c r="D4" t="n">
         <v>299</v>
       </c>
+      <c r="E4" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -524,6 +539,9 @@
       <c r="D5" t="n">
         <v>569</v>
       </c>
+      <c r="E5" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -540,6 +558,9 @@
       <c r="D6" t="n">
         <v>499</v>
       </c>
+      <c r="E6" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -556,6 +577,9 @@
       <c r="D7" t="n">
         <v>569</v>
       </c>
+      <c r="E7" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -572,6 +596,9 @@
       <c r="D8" t="n">
         <v>929</v>
       </c>
+      <c r="E8" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -588,6 +615,9 @@
       <c r="D9" t="n">
         <v>299</v>
       </c>
+      <c r="E9" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -604,6 +634,9 @@
       <c r="D10" t="n">
         <v>299</v>
       </c>
+      <c r="E10" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -620,6 +653,9 @@
       <c r="D11" t="n">
         <v>929</v>
       </c>
+      <c r="E11" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -636,6 +672,9 @@
       <c r="D12" t="n">
         <v>569</v>
       </c>
+      <c r="E12" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -643,13 +682,14 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
         <v>569</v>
       </c>
       <c r="D13" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -668,6 +708,9 @@
       <c r="D14" t="n">
         <v>499</v>
       </c>
+      <c r="E14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -684,6 +727,9 @@
       <c r="D15" t="n">
         <v>499</v>
       </c>
+      <c r="E15" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -700,6 +746,9 @@
       <c r="D16" t="n">
         <v>299</v>
       </c>
+      <c r="E16" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -716,6 +765,9 @@
       <c r="D17" t="n">
         <v>929</v>
       </c>
+      <c r="E17" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -732,6 +784,9 @@
       <c r="D18" t="n">
         <v>499</v>
       </c>
+      <c r="E18" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -746,6 +801,9 @@
         <v>1497</v>
       </c>
       <c r="D19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="E19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -764,6 +822,9 @@
       <c r="D20" t="n">
         <v>929</v>
       </c>
+      <c r="E20" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -780,6 +841,9 @@
       <c r="D21" t="n">
         <v>499</v>
       </c>
+      <c r="E21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -796,6 +860,9 @@
       <c r="D22" t="n">
         <v>299</v>
       </c>
+      <c r="E22" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -812,6 +879,9 @@
       <c r="D23" t="n">
         <v>1299</v>
       </c>
+      <c r="E23" t="n">
+        <v>1299</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -828,6 +898,9 @@
       <c r="D24" t="n">
         <v>929</v>
       </c>
+      <c r="E24" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -844,6 +917,9 @@
       <c r="D25" t="n">
         <v>929</v>
       </c>
+      <c r="E25" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -858,6 +934,9 @@
         <v>1299</v>
       </c>
       <c r="D26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-20 19:07
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,7 @@
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
     <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -448,20 +449,25 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 00:32</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -485,6 +491,9 @@
       <c r="E2" t="n">
         <v>929</v>
       </c>
+      <c r="F2" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -504,6 +513,9 @@
       <c r="E3" t="n">
         <v>569</v>
       </c>
+      <c r="F3" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -523,6 +535,9 @@
       <c r="E4" t="n">
         <v>299</v>
       </c>
+      <c r="F4" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -542,6 +557,9 @@
       <c r="E5" t="n">
         <v>569</v>
       </c>
+      <c r="F5" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -561,6 +579,9 @@
       <c r="E6" t="n">
         <v>499</v>
       </c>
+      <c r="F6" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -580,6 +601,9 @@
       <c r="E7" t="n">
         <v>569</v>
       </c>
+      <c r="F7" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -599,6 +623,9 @@
       <c r="E8" t="n">
         <v>929</v>
       </c>
+      <c r="F8" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -618,6 +645,9 @@
       <c r="E9" t="n">
         <v>299</v>
       </c>
+      <c r="F9" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -637,6 +667,9 @@
       <c r="E10" t="n">
         <v>299</v>
       </c>
+      <c r="F10" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -656,6 +689,9 @@
       <c r="E11" t="n">
         <v>929</v>
       </c>
+      <c r="F11" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -675,6 +711,9 @@
       <c r="E12" t="n">
         <v>569</v>
       </c>
+      <c r="F12" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -682,14 +721,17 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="n">
+        <v>569</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>569</v>
       </c>
       <c r="E13" t="n">
+        <v>569</v>
+      </c>
+      <c r="F13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -711,6 +753,9 @@
       <c r="E14" t="n">
         <v>499</v>
       </c>
+      <c r="F14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -730,6 +775,9 @@
       <c r="E15" t="n">
         <v>499</v>
       </c>
+      <c r="F15" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -749,6 +797,9 @@
       <c r="E16" t="n">
         <v>299</v>
       </c>
+      <c r="F16" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -768,6 +819,9 @@
       <c r="E17" t="n">
         <v>929</v>
       </c>
+      <c r="F17" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -787,6 +841,9 @@
       <c r="E18" t="n">
         <v>499</v>
       </c>
+      <c r="F18" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -804,6 +861,9 @@
         <v>1497</v>
       </c>
       <c r="E19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="F19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -825,6 +885,9 @@
       <c r="E20" t="n">
         <v>929</v>
       </c>
+      <c r="F20" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -844,6 +907,9 @@
       <c r="E21" t="n">
         <v>499</v>
       </c>
+      <c r="F21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -863,6 +929,9 @@
       <c r="E22" t="n">
         <v>299</v>
       </c>
+      <c r="F22" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -882,6 +951,9 @@
       <c r="E23" t="n">
         <v>1299</v>
       </c>
+      <c r="F23" t="n">
+        <v>1299</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -901,6 +973,9 @@
       <c r="E24" t="n">
         <v>929</v>
       </c>
+      <c r="F24" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -920,6 +995,9 @@
       <c r="E25" t="n">
         <v>929</v>
       </c>
+      <c r="F25" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -937,6 +1015,9 @@
         <v>1299</v>
       </c>
       <c r="E26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-20 19:26
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,7 @@
     <col width="21" customWidth="1" min="4" max="4"/>
     <col width="21" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -449,25 +450,30 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 00:52</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -494,6 +500,9 @@
       <c r="F2" t="n">
         <v>929</v>
       </c>
+      <c r="G2" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -516,6 +525,9 @@
       <c r="F3" t="n">
         <v>569</v>
       </c>
+      <c r="G3" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -538,6 +550,9 @@
       <c r="F4" t="n">
         <v>299</v>
       </c>
+      <c r="G4" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -560,6 +575,9 @@
       <c r="F5" t="n">
         <v>569</v>
       </c>
+      <c r="G5" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -582,6 +600,9 @@
       <c r="F6" t="n">
         <v>499</v>
       </c>
+      <c r="G6" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -604,6 +625,9 @@
       <c r="F7" t="n">
         <v>569</v>
       </c>
+      <c r="G7" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -626,6 +650,9 @@
       <c r="F8" t="n">
         <v>929</v>
       </c>
+      <c r="G8" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -648,6 +675,9 @@
       <c r="F9" t="n">
         <v>299</v>
       </c>
+      <c r="G9" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -670,6 +700,9 @@
       <c r="F10" t="n">
         <v>299</v>
       </c>
+      <c r="G10" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -692,6 +725,9 @@
       <c r="F11" t="n">
         <v>929</v>
       </c>
+      <c r="G11" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -714,6 +750,9 @@
       <c r="F12" t="n">
         <v>569</v>
       </c>
+      <c r="G12" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -724,14 +763,17 @@
       <c r="B13" t="n">
         <v>569</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>569</v>
-      </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>569</v>
       </c>
       <c r="F13" t="n">
+        <v>569</v>
+      </c>
+      <c r="G13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -756,6 +798,9 @@
       <c r="F14" t="n">
         <v>499</v>
       </c>
+      <c r="G14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -778,6 +823,9 @@
       <c r="F15" t="n">
         <v>499</v>
       </c>
+      <c r="G15" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -800,6 +848,9 @@
       <c r="F16" t="n">
         <v>299</v>
       </c>
+      <c r="G16" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -822,6 +873,9 @@
       <c r="F17" t="n">
         <v>929</v>
       </c>
+      <c r="G17" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -844,6 +898,9 @@
       <c r="F18" t="n">
         <v>499</v>
       </c>
+      <c r="G18" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -864,6 +921,9 @@
         <v>1497</v>
       </c>
       <c r="F19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="G19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -888,6 +948,9 @@
       <c r="F20" t="n">
         <v>929</v>
       </c>
+      <c r="G20" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -910,6 +973,9 @@
       <c r="F21" t="n">
         <v>499</v>
       </c>
+      <c r="G21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -932,6 +998,9 @@
       <c r="F22" t="n">
         <v>299</v>
       </c>
+      <c r="G22" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -954,6 +1023,9 @@
       <c r="F23" t="n">
         <v>1299</v>
       </c>
+      <c r="G23" t="n">
+        <v>1299</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -976,6 +1048,9 @@
       <c r="F24" t="n">
         <v>929</v>
       </c>
+      <c r="G24" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -998,6 +1073,9 @@
       <c r="F25" t="n">
         <v>929</v>
       </c>
+      <c r="G25" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1018,6 +1096,9 @@
         <v>1299</v>
       </c>
       <c r="F26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-20 20:41
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +440,7 @@
     <col width="21" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -450,30 +451,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 02:07</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -503,6 +509,9 @@
       <c r="G2" t="n">
         <v>929</v>
       </c>
+      <c r="H2" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -528,6 +537,9 @@
       <c r="G3" t="n">
         <v>569</v>
       </c>
+      <c r="H3" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -553,6 +565,9 @@
       <c r="G4" t="n">
         <v>299</v>
       </c>
+      <c r="H4" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -578,6 +593,9 @@
       <c r="G5" t="n">
         <v>569</v>
       </c>
+      <c r="H5" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -603,6 +621,9 @@
       <c r="G6" t="n">
         <v>499</v>
       </c>
+      <c r="H6" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -628,6 +649,9 @@
       <c r="G7" t="n">
         <v>569</v>
       </c>
+      <c r="H7" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -653,6 +677,9 @@
       <c r="G8" t="n">
         <v>929</v>
       </c>
+      <c r="H8" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -678,6 +705,9 @@
       <c r="G9" t="n">
         <v>299</v>
       </c>
+      <c r="H9" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -703,6 +733,9 @@
       <c r="G10" t="n">
         <v>299</v>
       </c>
+      <c r="H10" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -728,6 +761,9 @@
       <c r="G11" t="n">
         <v>929</v>
       </c>
+      <c r="H11" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -753,6 +789,9 @@
       <c r="G12" t="n">
         <v>569</v>
       </c>
+      <c r="H12" t="n">
+        <v>569</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -766,14 +805,17 @@
       <c r="C13" t="n">
         <v>569</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>569</v>
-      </c>
+      <c r="D13" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>569</v>
       </c>
       <c r="G13" t="n">
+        <v>569</v>
+      </c>
+      <c r="H13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -801,6 +843,9 @@
       <c r="G14" t="n">
         <v>499</v>
       </c>
+      <c r="H14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -826,6 +871,9 @@
       <c r="G15" t="n">
         <v>499</v>
       </c>
+      <c r="H15" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -851,6 +899,9 @@
       <c r="G16" t="n">
         <v>299</v>
       </c>
+      <c r="H16" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -876,6 +927,9 @@
       <c r="G17" t="n">
         <v>929</v>
       </c>
+      <c r="H17" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -901,6 +955,9 @@
       <c r="G18" t="n">
         <v>499</v>
       </c>
+      <c r="H18" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -924,6 +981,9 @@
         <v>1497</v>
       </c>
       <c r="G19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="H19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -951,6 +1011,9 @@
       <c r="G20" t="n">
         <v>929</v>
       </c>
+      <c r="H20" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -976,6 +1039,9 @@
       <c r="G21" t="n">
         <v>499</v>
       </c>
+      <c r="H21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1001,6 +1067,9 @@
       <c r="G22" t="n">
         <v>299</v>
       </c>
+      <c r="H22" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1026,6 +1095,9 @@
       <c r="G23" t="n">
         <v>1299</v>
       </c>
+      <c r="H23" t="n">
+        <v>1299</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1051,6 +1123,9 @@
       <c r="G24" t="n">
         <v>929</v>
       </c>
+      <c r="H24" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1076,6 +1151,9 @@
       <c r="G25" t="n">
         <v>929</v>
       </c>
+      <c r="H25" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1099,6 +1177,9 @@
         <v>1299</v>
       </c>
       <c r="G26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-20 22:45
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,7 @@
     <col width="21" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
+    <col width="21" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -451,35 +452,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 04:09</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -512,6 +518,9 @@
       <c r="H2" t="n">
         <v>929</v>
       </c>
+      <c r="I2" t="n">
+        <v>929</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -519,9 +528,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>569</v>
       </c>
@@ -538,6 +545,9 @@
         <v>569</v>
       </c>
       <c r="H3" t="n">
+        <v>569</v>
+      </c>
+      <c r="I3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -547,9 +557,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>299</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
         <v>299</v>
       </c>
@@ -566,6 +574,9 @@
         <v>299</v>
       </c>
       <c r="H4" t="n">
+        <v>299</v>
+      </c>
+      <c r="I4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -575,9 +586,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>569</v>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
         <v>569</v>
       </c>
@@ -594,6 +603,9 @@
         <v>569</v>
       </c>
       <c r="H5" t="n">
+        <v>569</v>
+      </c>
+      <c r="I5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -603,9 +615,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>499</v>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
         <v>499</v>
       </c>
@@ -622,6 +632,9 @@
         <v>499</v>
       </c>
       <c r="H6" t="n">
+        <v>499</v>
+      </c>
+      <c r="I6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -631,9 +644,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>569</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
         <v>569</v>
       </c>
@@ -650,6 +661,9 @@
         <v>569</v>
       </c>
       <c r="H7" t="n">
+        <v>569</v>
+      </c>
+      <c r="I7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -659,9 +673,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
         <v>929</v>
       </c>
@@ -678,6 +690,9 @@
         <v>929</v>
       </c>
       <c r="H8" t="n">
+        <v>929</v>
+      </c>
+      <c r="I8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -687,9 +702,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>299</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
         <v>299</v>
       </c>
@@ -706,6 +719,9 @@
         <v>299</v>
       </c>
       <c r="H9" t="n">
+        <v>299</v>
+      </c>
+      <c r="I9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -715,9 +731,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
         <v>299</v>
       </c>
@@ -734,6 +748,9 @@
         <v>299</v>
       </c>
       <c r="H10" t="n">
+        <v>299</v>
+      </c>
+      <c r="I10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -743,9 +760,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>929</v>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
         <v>929</v>
       </c>
@@ -762,6 +777,9 @@
         <v>929</v>
       </c>
       <c r="H11" t="n">
+        <v>929</v>
+      </c>
+      <c r="I11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -771,9 +789,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>569</v>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
         <v>569</v>
       </c>
@@ -790,6 +806,9 @@
         <v>569</v>
       </c>
       <c r="H12" t="n">
+        <v>569</v>
+      </c>
+      <c r="I12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -799,23 +818,24 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
         <v>569</v>
       </c>
       <c r="D13" t="n">
         <v>569</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>569</v>
-      </c>
+      <c r="E13" t="n">
+        <v>569</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>569</v>
       </c>
       <c r="H13" t="n">
+        <v>569</v>
+      </c>
+      <c r="I13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -846,6 +866,9 @@
       <c r="H14" t="n">
         <v>499</v>
       </c>
+      <c r="I14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -853,9 +876,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>499</v>
-      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
         <v>499</v>
       </c>
@@ -872,6 +893,9 @@
         <v>499</v>
       </c>
       <c r="H15" t="n">
+        <v>499</v>
+      </c>
+      <c r="I15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -881,9 +905,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
         <v>299</v>
       </c>
@@ -900,6 +922,9 @@
         <v>299</v>
       </c>
       <c r="H16" t="n">
+        <v>299</v>
+      </c>
+      <c r="I16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -909,9 +934,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>929</v>
-      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
         <v>929</v>
       </c>
@@ -928,6 +951,9 @@
         <v>929</v>
       </c>
       <c r="H17" t="n">
+        <v>929</v>
+      </c>
+      <c r="I17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -937,9 +963,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>499</v>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="n">
         <v>499</v>
       </c>
@@ -956,6 +980,9 @@
         <v>499</v>
       </c>
       <c r="H18" t="n">
+        <v>499</v>
+      </c>
+      <c r="I18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -984,6 +1011,9 @@
         <v>1497</v>
       </c>
       <c r="H19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="I19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -993,9 +1023,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>929</v>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="n">
         <v>929</v>
       </c>
@@ -1012,6 +1040,9 @@
         <v>929</v>
       </c>
       <c r="H20" t="n">
+        <v>929</v>
+      </c>
+      <c r="I20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1042,6 +1073,9 @@
       <c r="H21" t="n">
         <v>499</v>
       </c>
+      <c r="I21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1049,9 +1083,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>299</v>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
         <v>299</v>
       </c>
@@ -1068,6 +1100,9 @@
         <v>299</v>
       </c>
       <c r="H22" t="n">
+        <v>299</v>
+      </c>
+      <c r="I22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1077,9 +1112,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
         <v>1299</v>
       </c>
@@ -1096,6 +1129,9 @@
         <v>1299</v>
       </c>
       <c r="H23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1105,9 +1141,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>929</v>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="n">
         <v>929</v>
       </c>
@@ -1124,6 +1158,9 @@
         <v>929</v>
       </c>
       <c r="H24" t="n">
+        <v>929</v>
+      </c>
+      <c r="I24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1133,9 +1170,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>929</v>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
         <v>929</v>
       </c>
@@ -1152,6 +1187,9 @@
         <v>929</v>
       </c>
       <c r="H25" t="n">
+        <v>929</v>
+      </c>
+      <c r="I25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1161,9 +1199,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="n">
         <v>1299</v>
       </c>
@@ -1180,6 +1216,9 @@
         <v>1299</v>
       </c>
       <c r="H26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 04:02
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,7 @@
     <col width="21" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="21" customWidth="1" min="9" max="9"/>
+    <col width="21" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -452,40 +453,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 09:28</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -497,9 +503,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>929</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
         <v>929</v>
       </c>
@@ -519,6 +523,9 @@
         <v>929</v>
       </c>
       <c r="I2" t="n">
+        <v>929</v>
+      </c>
+      <c r="J2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -528,10 +535,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="n">
+        <v>569</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>569</v>
       </c>
@@ -548,6 +555,9 @@
         <v>569</v>
       </c>
       <c r="I3" t="n">
+        <v>569</v>
+      </c>
+      <c r="J3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -557,10 +567,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="n">
-        <v>299</v>
-      </c>
+      <c r="B4" t="n">
+        <v>299</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
         <v>299</v>
       </c>
@@ -577,6 +587,9 @@
         <v>299</v>
       </c>
       <c r="I4" t="n">
+        <v>299</v>
+      </c>
+      <c r="J4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -586,10 +599,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
-        <v>569</v>
-      </c>
+      <c r="B5" t="n">
+        <v>569</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
         <v>569</v>
       </c>
@@ -606,6 +619,9 @@
         <v>569</v>
       </c>
       <c r="I5" t="n">
+        <v>569</v>
+      </c>
+      <c r="J5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -615,10 +631,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="n">
-        <v>499</v>
-      </c>
+      <c r="B6" t="n">
+        <v>499</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
         <v>499</v>
       </c>
@@ -635,6 +651,9 @@
         <v>499</v>
       </c>
       <c r="I6" t="n">
+        <v>499</v>
+      </c>
+      <c r="J6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -644,10 +663,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="n">
-        <v>569</v>
-      </c>
+      <c r="B7" t="n">
+        <v>569</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
         <v>569</v>
       </c>
@@ -664,6 +683,9 @@
         <v>569</v>
       </c>
       <c r="I7" t="n">
+        <v>569</v>
+      </c>
+      <c r="J7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -673,10 +695,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="n">
+        <v>929</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>929</v>
       </c>
@@ -693,6 +715,9 @@
         <v>929</v>
       </c>
       <c r="I8" t="n">
+        <v>929</v>
+      </c>
+      <c r="J8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -702,10 +727,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="n">
-        <v>299</v>
-      </c>
+      <c r="B9" t="n">
+        <v>299</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>299</v>
       </c>
@@ -722,6 +747,9 @@
         <v>299</v>
       </c>
       <c r="I9" t="n">
+        <v>299</v>
+      </c>
+      <c r="J9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -731,10 +759,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="n">
+        <v>299</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>299</v>
       </c>
@@ -751,6 +779,9 @@
         <v>299</v>
       </c>
       <c r="I10" t="n">
+        <v>299</v>
+      </c>
+      <c r="J10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -760,10 +791,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="n">
-        <v>929</v>
-      </c>
+      <c r="B11" t="n">
+        <v>929</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>929</v>
       </c>
@@ -780,6 +811,9 @@
         <v>929</v>
       </c>
       <c r="I11" t="n">
+        <v>929</v>
+      </c>
+      <c r="J11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -789,10 +823,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="n">
-        <v>569</v>
-      </c>
+      <c r="B12" t="n">
+        <v>569</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
         <v>569</v>
       </c>
@@ -809,6 +843,9 @@
         <v>569</v>
       </c>
       <c r="I12" t="n">
+        <v>569</v>
+      </c>
+      <c r="J12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -818,24 +855,27 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="n">
+        <v>569</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>569</v>
       </c>
       <c r="E13" t="n">
         <v>569</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>569</v>
-      </c>
+      <c r="F13" t="n">
+        <v>569</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>569</v>
       </c>
       <c r="I13" t="n">
+        <v>569</v>
+      </c>
+      <c r="J13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -869,6 +909,9 @@
       <c r="I14" t="n">
         <v>499</v>
       </c>
+      <c r="J14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -876,10 +919,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>499</v>
-      </c>
+      <c r="B15" t="n">
+        <v>499</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
         <v>499</v>
       </c>
@@ -896,6 +939,9 @@
         <v>499</v>
       </c>
       <c r="I15" t="n">
+        <v>499</v>
+      </c>
+      <c r="J15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -905,10 +951,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="n">
+        <v>299</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
         <v>299</v>
       </c>
@@ -925,6 +971,9 @@
         <v>299</v>
       </c>
       <c r="I16" t="n">
+        <v>299</v>
+      </c>
+      <c r="J16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -934,10 +983,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="n">
-        <v>929</v>
-      </c>
+      <c r="B17" t="n">
+        <v>929</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
         <v>929</v>
       </c>
@@ -954,6 +1003,9 @@
         <v>929</v>
       </c>
       <c r="I17" t="n">
+        <v>929</v>
+      </c>
+      <c r="J17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -963,10 +1015,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="n">
-        <v>499</v>
-      </c>
+      <c r="B18" t="n">
+        <v>499</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
         <v>499</v>
       </c>
@@ -983,6 +1035,9 @@
         <v>499</v>
       </c>
       <c r="I18" t="n">
+        <v>499</v>
+      </c>
+      <c r="J18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1014,6 +1069,9 @@
         <v>1497</v>
       </c>
       <c r="I19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="J19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1023,10 +1081,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 124 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="n">
-        <v>929</v>
-      </c>
+      <c r="B20" t="n">
+        <v>929</v>
+      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
         <v>929</v>
       </c>
@@ -1043,6 +1101,9 @@
         <v>929</v>
       </c>
       <c r="I20" t="n">
+        <v>929</v>
+      </c>
+      <c r="J20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1076,6 +1137,9 @@
       <c r="I21" t="n">
         <v>499</v>
       </c>
+      <c r="J21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1083,10 +1147,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="n">
-        <v>299</v>
-      </c>
+      <c r="B22" t="n">
+        <v>299</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
         <v>299</v>
       </c>
@@ -1103,6 +1167,9 @@
         <v>299</v>
       </c>
       <c r="I22" t="n">
+        <v>299</v>
+      </c>
+      <c r="J22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1112,10 +1179,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
         <v>1299</v>
       </c>
@@ -1132,6 +1199,9 @@
         <v>1299</v>
       </c>
       <c r="I23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1141,10 +1211,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="n">
-        <v>929</v>
-      </c>
+      <c r="B24" t="n">
+        <v>929</v>
+      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
         <v>929</v>
       </c>
@@ -1161,6 +1231,9 @@
         <v>929</v>
       </c>
       <c r="I24" t="n">
+        <v>929</v>
+      </c>
+      <c r="J24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1170,10 +1243,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="n">
-        <v>929</v>
-      </c>
+      <c r="B25" t="n">
+        <v>929</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
         <v>929</v>
       </c>
@@ -1190,6 +1263,9 @@
         <v>929</v>
       </c>
       <c r="I25" t="n">
+        <v>929</v>
+      </c>
+      <c r="J25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1199,10 +1275,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
         <v>1299</v>
       </c>
@@ -1219,6 +1295,9 @@
         <v>1299</v>
       </c>
       <c r="I26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 05:03
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,7 @@
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="21" customWidth="1" min="9" max="9"/>
     <col width="21" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -453,45 +454,50 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 10:29</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -503,10 +509,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>929</v>
-      </c>
+      <c r="B2" t="n">
+        <v>929</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
         <v>929</v>
       </c>
@@ -526,6 +532,9 @@
         <v>929</v>
       </c>
       <c r="J2" t="n">
+        <v>929</v>
+      </c>
+      <c r="K2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -538,10 +547,10 @@
       <c r="B3" t="n">
         <v>569</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>569</v>
-      </c>
+      <c r="C3" t="n">
+        <v>569</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>569</v>
       </c>
@@ -558,6 +567,9 @@
         <v>569</v>
       </c>
       <c r="J3" t="n">
+        <v>569</v>
+      </c>
+      <c r="K3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -570,10 +582,10 @@
       <c r="B4" t="n">
         <v>299</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="n">
-        <v>299</v>
-      </c>
+      <c r="C4" t="n">
+        <v>299</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>299</v>
       </c>
@@ -590,6 +602,9 @@
         <v>299</v>
       </c>
       <c r="J4" t="n">
+        <v>299</v>
+      </c>
+      <c r="K4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -602,10 +617,10 @@
       <c r="B5" t="n">
         <v>569</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="n">
-        <v>569</v>
-      </c>
+      <c r="C5" t="n">
+        <v>569</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>569</v>
       </c>
@@ -622,6 +637,9 @@
         <v>569</v>
       </c>
       <c r="J5" t="n">
+        <v>569</v>
+      </c>
+      <c r="K5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -634,10 +652,10 @@
       <c r="B6" t="n">
         <v>499</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="n">
-        <v>499</v>
-      </c>
+      <c r="C6" t="n">
+        <v>499</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>499</v>
       </c>
@@ -654,6 +672,9 @@
         <v>499</v>
       </c>
       <c r="J6" t="n">
+        <v>499</v>
+      </c>
+      <c r="K6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -666,10 +687,10 @@
       <c r="B7" t="n">
         <v>569</v>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
-        <v>569</v>
-      </c>
+      <c r="C7" t="n">
+        <v>569</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
         <v>569</v>
       </c>
@@ -686,6 +707,9 @@
         <v>569</v>
       </c>
       <c r="J7" t="n">
+        <v>569</v>
+      </c>
+      <c r="K7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -698,10 +722,10 @@
       <c r="B8" t="n">
         <v>929</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
-        <v>929</v>
-      </c>
+      <c r="C8" t="n">
+        <v>929</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>929</v>
       </c>
@@ -718,6 +742,9 @@
         <v>929</v>
       </c>
       <c r="J8" t="n">
+        <v>929</v>
+      </c>
+      <c r="K8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -730,10 +757,10 @@
       <c r="B9" t="n">
         <v>299</v>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
-        <v>299</v>
-      </c>
+      <c r="C9" t="n">
+        <v>299</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
         <v>299</v>
       </c>
@@ -750,6 +777,9 @@
         <v>299</v>
       </c>
       <c r="J9" t="n">
+        <v>299</v>
+      </c>
+      <c r="K9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -762,10 +792,10 @@
       <c r="B10" t="n">
         <v>299</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>299</v>
-      </c>
+      <c r="C10" t="n">
+        <v>299</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
         <v>299</v>
       </c>
@@ -782,6 +812,9 @@
         <v>299</v>
       </c>
       <c r="J10" t="n">
+        <v>299</v>
+      </c>
+      <c r="K10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -794,10 +827,10 @@
       <c r="B11" t="n">
         <v>929</v>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
-        <v>929</v>
-      </c>
+      <c r="C11" t="n">
+        <v>929</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
         <v>929</v>
       </c>
@@ -814,6 +847,9 @@
         <v>929</v>
       </c>
       <c r="J11" t="n">
+        <v>929</v>
+      </c>
+      <c r="K11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -826,10 +862,10 @@
       <c r="B12" t="n">
         <v>569</v>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="n">
-        <v>569</v>
-      </c>
+      <c r="C12" t="n">
+        <v>569</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
         <v>569</v>
       </c>
@@ -846,6 +882,9 @@
         <v>569</v>
       </c>
       <c r="J12" t="n">
+        <v>569</v>
+      </c>
+      <c r="K12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -858,24 +897,27 @@
       <c r="B13" t="n">
         <v>569</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>569</v>
-      </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>569</v>
       </c>
       <c r="F13" t="n">
         <v>569</v>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>569</v>
-      </c>
+      <c r="G13" t="n">
+        <v>569</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>569</v>
       </c>
       <c r="J13" t="n">
+        <v>569</v>
+      </c>
+      <c r="K13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -912,6 +954,9 @@
       <c r="J14" t="n">
         <v>499</v>
       </c>
+      <c r="K14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -919,13 +964,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>499</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="n">
-        <v>499</v>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>499</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>499</v>
       </c>
@@ -942,6 +985,9 @@
         <v>499</v>
       </c>
       <c r="J15" t="n">
+        <v>499</v>
+      </c>
+      <c r="K15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -954,10 +1000,10 @@
       <c r="B16" t="n">
         <v>299</v>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
-        <v>299</v>
-      </c>
+      <c r="C16" t="n">
+        <v>299</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
         <v>299</v>
       </c>
@@ -974,6 +1020,9 @@
         <v>299</v>
       </c>
       <c r="J16" t="n">
+        <v>299</v>
+      </c>
+      <c r="K16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -986,10 +1035,10 @@
       <c r="B17" t="n">
         <v>929</v>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="n">
-        <v>929</v>
-      </c>
+      <c r="C17" t="n">
+        <v>929</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
         <v>929</v>
       </c>
@@ -1006,6 +1055,9 @@
         <v>929</v>
       </c>
       <c r="J17" t="n">
+        <v>929</v>
+      </c>
+      <c r="K17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1018,10 +1070,10 @@
       <c r="B18" t="n">
         <v>499</v>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="n">
-        <v>499</v>
-      </c>
+      <c r="C18" t="n">
+        <v>499</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>499</v>
       </c>
@@ -1038,6 +1090,9 @@
         <v>499</v>
       </c>
       <c r="J18" t="n">
+        <v>499</v>
+      </c>
+      <c r="K18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1072,6 +1127,9 @@
         <v>1497</v>
       </c>
       <c r="J19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="K19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1084,10 +1142,10 @@
       <c r="B20" t="n">
         <v>929</v>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="n">
-        <v>929</v>
-      </c>
+      <c r="C20" t="n">
+        <v>929</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
         <v>929</v>
       </c>
@@ -1104,6 +1162,9 @@
         <v>929</v>
       </c>
       <c r="J20" t="n">
+        <v>929</v>
+      </c>
+      <c r="K20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1140,6 +1201,9 @@
       <c r="J21" t="n">
         <v>499</v>
       </c>
+      <c r="K21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1150,10 +1214,10 @@
       <c r="B22" t="n">
         <v>299</v>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="n">
-        <v>299</v>
-      </c>
+      <c r="C22" t="n">
+        <v>299</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
         <v>299</v>
       </c>
@@ -1170,6 +1234,9 @@
         <v>299</v>
       </c>
       <c r="J22" t="n">
+        <v>299</v>
+      </c>
+      <c r="K22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1182,10 +1249,10 @@
       <c r="B23" t="n">
         <v>1299</v>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>1299</v>
       </c>
@@ -1202,6 +1269,9 @@
         <v>1299</v>
       </c>
       <c r="J23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1214,10 +1284,10 @@
       <c r="B24" t="n">
         <v>929</v>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="n">
-        <v>929</v>
-      </c>
+      <c r="C24" t="n">
+        <v>929</v>
+      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>929</v>
       </c>
@@ -1234,6 +1304,9 @@
         <v>929</v>
       </c>
       <c r="J24" t="n">
+        <v>929</v>
+      </c>
+      <c r="K24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1246,10 +1319,10 @@
       <c r="B25" t="n">
         <v>929</v>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="n">
-        <v>929</v>
-      </c>
+      <c r="C25" t="n">
+        <v>929</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
         <v>929</v>
       </c>
@@ -1266,6 +1339,9 @@
         <v>929</v>
       </c>
       <c r="J25" t="n">
+        <v>929</v>
+      </c>
+      <c r="K25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1278,10 +1354,10 @@
       <c r="B26" t="n">
         <v>1299</v>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
         <v>1299</v>
       </c>
@@ -1298,6 +1374,9 @@
         <v>1299</v>
       </c>
       <c r="J26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 07:01
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,7 @@
     <col width="21" customWidth="1" min="9" max="9"/>
     <col width="21" customWidth="1" min="10" max="10"/>
     <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -454,50 +455,55 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 12:27</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -512,10 +518,10 @@
       <c r="B2" t="n">
         <v>929</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>929</v>
-      </c>
+      <c r="C2" t="n">
+        <v>929</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>929</v>
       </c>
@@ -535,6 +541,9 @@
         <v>929</v>
       </c>
       <c r="K2" t="n">
+        <v>929</v>
+      </c>
+      <c r="L2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -550,10 +559,10 @@
       <c r="C3" t="n">
         <v>569</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>569</v>
-      </c>
+      <c r="D3" t="n">
+        <v>569</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>569</v>
       </c>
@@ -570,6 +579,9 @@
         <v>569</v>
       </c>
       <c r="K3" t="n">
+        <v>569</v>
+      </c>
+      <c r="L3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -585,10 +597,10 @@
       <c r="C4" t="n">
         <v>299</v>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
-        <v>299</v>
-      </c>
+      <c r="D4" t="n">
+        <v>299</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
         <v>299</v>
       </c>
@@ -605,6 +617,9 @@
         <v>299</v>
       </c>
       <c r="K4" t="n">
+        <v>299</v>
+      </c>
+      <c r="L4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -620,10 +635,10 @@
       <c r="C5" t="n">
         <v>569</v>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="n">
-        <v>569</v>
-      </c>
+      <c r="D5" t="n">
+        <v>569</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>569</v>
       </c>
@@ -640,6 +655,9 @@
         <v>569</v>
       </c>
       <c r="K5" t="n">
+        <v>569</v>
+      </c>
+      <c r="L5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -655,10 +673,10 @@
       <c r="C6" t="n">
         <v>499</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
-        <v>499</v>
-      </c>
+      <c r="D6" t="n">
+        <v>499</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>499</v>
       </c>
@@ -675,6 +693,9 @@
         <v>499</v>
       </c>
       <c r="K6" t="n">
+        <v>499</v>
+      </c>
+      <c r="L6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -690,10 +711,10 @@
       <c r="C7" t="n">
         <v>569</v>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>569</v>
-      </c>
+      <c r="D7" t="n">
+        <v>569</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>569</v>
       </c>
@@ -710,6 +731,9 @@
         <v>569</v>
       </c>
       <c r="K7" t="n">
+        <v>569</v>
+      </c>
+      <c r="L7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -725,10 +749,10 @@
       <c r="C8" t="n">
         <v>929</v>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>929</v>
-      </c>
+      <c r="D8" t="n">
+        <v>929</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>929</v>
       </c>
@@ -745,6 +769,9 @@
         <v>929</v>
       </c>
       <c r="K8" t="n">
+        <v>929</v>
+      </c>
+      <c r="L8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -760,10 +787,10 @@
       <c r="C9" t="n">
         <v>299</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>299</v>
-      </c>
+      <c r="D9" t="n">
+        <v>299</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>299</v>
       </c>
@@ -780,6 +807,9 @@
         <v>299</v>
       </c>
       <c r="K9" t="n">
+        <v>299</v>
+      </c>
+      <c r="L9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -795,10 +825,10 @@
       <c r="C10" t="n">
         <v>299</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>299</v>
-      </c>
+      <c r="D10" t="n">
+        <v>299</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>299</v>
       </c>
@@ -815,6 +845,9 @@
         <v>299</v>
       </c>
       <c r="K10" t="n">
+        <v>299</v>
+      </c>
+      <c r="L10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -825,15 +858,15 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="C11" t="n">
         <v>929</v>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
-        <v>929</v>
-      </c>
+      <c r="D11" t="n">
+        <v>929</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>929</v>
       </c>
@@ -850,6 +883,9 @@
         <v>929</v>
       </c>
       <c r="K11" t="n">
+        <v>929</v>
+      </c>
+      <c r="L11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -865,10 +901,10 @@
       <c r="C12" t="n">
         <v>569</v>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>569</v>
-      </c>
+      <c r="D12" t="n">
+        <v>569</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
         <v>569</v>
       </c>
@@ -885,6 +921,9 @@
         <v>569</v>
       </c>
       <c r="K12" t="n">
+        <v>569</v>
+      </c>
+      <c r="L12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -900,24 +939,27 @@
       <c r="C13" t="n">
         <v>569</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>569</v>
-      </c>
+      <c r="D13" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>569</v>
       </c>
       <c r="G13" t="n">
         <v>569</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>569</v>
-      </c>
+      <c r="H13" t="n">
+        <v>569</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
         <v>569</v>
       </c>
       <c r="K13" t="n">
+        <v>569</v>
+      </c>
+      <c r="L13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -957,6 +999,9 @@
       <c r="K14" t="n">
         <v>499</v>
       </c>
+      <c r="L14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -964,14 +1009,14 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>499</v>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>499</v>
-      </c>
+      <c r="B15" t="n">
+        <v>499</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>499</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
         <v>499</v>
       </c>
@@ -988,6 +1033,9 @@
         <v>499</v>
       </c>
       <c r="K15" t="n">
+        <v>499</v>
+      </c>
+      <c r="L15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1003,10 +1051,10 @@
       <c r="C16" t="n">
         <v>299</v>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>299</v>
-      </c>
+      <c r="D16" t="n">
+        <v>299</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
         <v>299</v>
       </c>
@@ -1023,6 +1071,9 @@
         <v>299</v>
       </c>
       <c r="K16" t="n">
+        <v>299</v>
+      </c>
+      <c r="L16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1038,10 +1089,10 @@
       <c r="C17" t="n">
         <v>929</v>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
-        <v>929</v>
-      </c>
+      <c r="D17" t="n">
+        <v>929</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
         <v>929</v>
       </c>
@@ -1058,6 +1109,9 @@
         <v>929</v>
       </c>
       <c r="K17" t="n">
+        <v>929</v>
+      </c>
+      <c r="L17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1073,10 +1127,10 @@
       <c r="C18" t="n">
         <v>499</v>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="n">
-        <v>499</v>
-      </c>
+      <c r="D18" t="n">
+        <v>499</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
         <v>499</v>
       </c>
@@ -1093,6 +1147,9 @@
         <v>499</v>
       </c>
       <c r="K18" t="n">
+        <v>499</v>
+      </c>
+      <c r="L18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1130,6 +1187,9 @@
         <v>1497</v>
       </c>
       <c r="K19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="L19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1145,10 +1205,10 @@
       <c r="C20" t="n">
         <v>929</v>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="n">
-        <v>929</v>
-      </c>
+      <c r="D20" t="n">
+        <v>929</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
         <v>929</v>
       </c>
@@ -1165,6 +1225,9 @@
         <v>929</v>
       </c>
       <c r="K20" t="n">
+        <v>929</v>
+      </c>
+      <c r="L20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1204,6 +1267,9 @@
       <c r="K21" t="n">
         <v>499</v>
       </c>
+      <c r="L21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1217,10 +1283,10 @@
       <c r="C22" t="n">
         <v>299</v>
       </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="n">
-        <v>299</v>
-      </c>
+      <c r="D22" t="n">
+        <v>299</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
         <v>299</v>
       </c>
@@ -1237,6 +1303,9 @@
         <v>299</v>
       </c>
       <c r="K22" t="n">
+        <v>299</v>
+      </c>
+      <c r="L22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1252,10 +1321,10 @@
       <c r="C23" t="n">
         <v>1299</v>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
         <v>1299</v>
       </c>
@@ -1272,6 +1341,9 @@
         <v>1299</v>
       </c>
       <c r="K23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="L23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1287,10 +1359,10 @@
       <c r="C24" t="n">
         <v>929</v>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="n">
-        <v>929</v>
-      </c>
+      <c r="D24" t="n">
+        <v>929</v>
+      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
         <v>929</v>
       </c>
@@ -1307,6 +1379,9 @@
         <v>929</v>
       </c>
       <c r="K24" t="n">
+        <v>929</v>
+      </c>
+      <c r="L24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1322,10 +1397,10 @@
       <c r="C25" t="n">
         <v>929</v>
       </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="n">
-        <v>929</v>
-      </c>
+      <c r="D25" t="n">
+        <v>929</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
         <v>929</v>
       </c>
@@ -1342,6 +1417,9 @@
         <v>929</v>
       </c>
       <c r="K25" t="n">
+        <v>929</v>
+      </c>
+      <c r="L25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1357,10 +1435,10 @@
       <c r="C26" t="n">
         <v>1299</v>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
         <v>1299</v>
       </c>
@@ -1377,6 +1455,9 @@
         <v>1299</v>
       </c>
       <c r="K26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="L26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 08:54
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,7 @@
     <col width="21" customWidth="1" min="10" max="10"/>
     <col width="21" customWidth="1" min="11" max="11"/>
     <col width="21" customWidth="1" min="12" max="12"/>
+    <col width="21" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -455,55 +456,60 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 14:19</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -515,16 +521,14 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>929</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
         <v>929</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>929</v>
-      </c>
+      <c r="D2" t="n">
+        <v>929</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
         <v>929</v>
       </c>
@@ -544,6 +548,9 @@
         <v>929</v>
       </c>
       <c r="L2" t="n">
+        <v>929</v>
+      </c>
+      <c r="M2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -562,10 +569,10 @@
       <c r="D3" t="n">
         <v>569</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>569</v>
-      </c>
+      <c r="E3" t="n">
+        <v>569</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>569</v>
       </c>
@@ -582,6 +589,9 @@
         <v>569</v>
       </c>
       <c r="L3" t="n">
+        <v>569</v>
+      </c>
+      <c r="M3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -600,10 +610,10 @@
       <c r="D4" t="n">
         <v>299</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>299</v>
-      </c>
+      <c r="E4" t="n">
+        <v>299</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>299</v>
       </c>
@@ -620,6 +630,9 @@
         <v>299</v>
       </c>
       <c r="L4" t="n">
+        <v>299</v>
+      </c>
+      <c r="M4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -638,10 +651,10 @@
       <c r="D5" t="n">
         <v>569</v>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>569</v>
-      </c>
+      <c r="E5" t="n">
+        <v>569</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>569</v>
       </c>
@@ -658,6 +671,9 @@
         <v>569</v>
       </c>
       <c r="L5" t="n">
+        <v>569</v>
+      </c>
+      <c r="M5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -676,10 +692,10 @@
       <c r="D6" t="n">
         <v>499</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>499</v>
-      </c>
+      <c r="E6" t="n">
+        <v>499</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
         <v>499</v>
       </c>
@@ -696,6 +712,9 @@
         <v>499</v>
       </c>
       <c r="L6" t="n">
+        <v>499</v>
+      </c>
+      <c r="M6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -714,10 +733,10 @@
       <c r="D7" t="n">
         <v>569</v>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>569</v>
-      </c>
+      <c r="E7" t="n">
+        <v>569</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>569</v>
       </c>
@@ -734,6 +753,9 @@
         <v>569</v>
       </c>
       <c r="L7" t="n">
+        <v>569</v>
+      </c>
+      <c r="M7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -752,10 +774,10 @@
       <c r="D8" t="n">
         <v>929</v>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>929</v>
-      </c>
+      <c r="E8" t="n">
+        <v>929</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>929</v>
       </c>
@@ -772,6 +794,9 @@
         <v>929</v>
       </c>
       <c r="L8" t="n">
+        <v>929</v>
+      </c>
+      <c r="M8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -790,10 +815,10 @@
       <c r="D9" t="n">
         <v>299</v>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>299</v>
-      </c>
+      <c r="E9" t="n">
+        <v>299</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>299</v>
       </c>
@@ -810,6 +835,9 @@
         <v>299</v>
       </c>
       <c r="L9" t="n">
+        <v>299</v>
+      </c>
+      <c r="M9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -828,10 +856,10 @@
       <c r="D10" t="n">
         <v>299</v>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>299</v>
-      </c>
+      <c r="E10" t="n">
+        <v>299</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>299</v>
       </c>
@@ -848,6 +876,9 @@
         <v>299</v>
       </c>
       <c r="L10" t="n">
+        <v>299</v>
+      </c>
+      <c r="M10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -861,15 +892,15 @@
         <v>2997</v>
       </c>
       <c r="C11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="D11" t="n">
         <v>929</v>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
-        <v>929</v>
-      </c>
+      <c r="E11" t="n">
+        <v>929</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>929</v>
       </c>
@@ -886,6 +917,9 @@
         <v>929</v>
       </c>
       <c r="L11" t="n">
+        <v>929</v>
+      </c>
+      <c r="M11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -904,10 +938,10 @@
       <c r="D12" t="n">
         <v>569</v>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>569</v>
-      </c>
+      <c r="E12" t="n">
+        <v>569</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>569</v>
       </c>
@@ -924,6 +958,9 @@
         <v>569</v>
       </c>
       <c r="L12" t="n">
+        <v>569</v>
+      </c>
+      <c r="M12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -942,24 +979,27 @@
       <c r="D13" t="n">
         <v>569</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>569</v>
-      </c>
+      <c r="E13" t="n">
+        <v>569</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>569</v>
       </c>
       <c r="H13" t="n">
         <v>569</v>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
-        <v>569</v>
-      </c>
+      <c r="I13" t="n">
+        <v>569</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>569</v>
       </c>
       <c r="L13" t="n">
+        <v>569</v>
+      </c>
+      <c r="M13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1002,6 +1042,9 @@
       <c r="L14" t="n">
         <v>499</v>
       </c>
+      <c r="M14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1012,14 +1055,14 @@
       <c r="B15" t="n">
         <v>499</v>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="n">
-        <v>499</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>499</v>
-      </c>
+      <c r="C15" t="n">
+        <v>499</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>499</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
         <v>499</v>
       </c>
@@ -1036,6 +1079,9 @@
         <v>499</v>
       </c>
       <c r="L15" t="n">
+        <v>499</v>
+      </c>
+      <c r="M15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1054,10 +1100,10 @@
       <c r="D16" t="n">
         <v>299</v>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>299</v>
-      </c>
+      <c r="E16" t="n">
+        <v>299</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>299</v>
       </c>
@@ -1074,6 +1120,9 @@
         <v>299</v>
       </c>
       <c r="L16" t="n">
+        <v>299</v>
+      </c>
+      <c r="M16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1092,10 +1141,10 @@
       <c r="D17" t="n">
         <v>929</v>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>929</v>
-      </c>
+      <c r="E17" t="n">
+        <v>929</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
         <v>929</v>
       </c>
@@ -1112,6 +1161,9 @@
         <v>929</v>
       </c>
       <c r="L17" t="n">
+        <v>929</v>
+      </c>
+      <c r="M17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1130,10 +1182,10 @@
       <c r="D18" t="n">
         <v>499</v>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
-        <v>499</v>
-      </c>
+      <c r="E18" t="n">
+        <v>499</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
         <v>499</v>
       </c>
@@ -1150,6 +1202,9 @@
         <v>499</v>
       </c>
       <c r="L18" t="n">
+        <v>499</v>
+      </c>
+      <c r="M18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1190,6 +1245,9 @@
         <v>1497</v>
       </c>
       <c r="L19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="M19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1208,10 +1266,10 @@
       <c r="D20" t="n">
         <v>929</v>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="n">
-        <v>929</v>
-      </c>
+      <c r="E20" t="n">
+        <v>929</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
         <v>929</v>
       </c>
@@ -1228,6 +1286,9 @@
         <v>929</v>
       </c>
       <c r="L20" t="n">
+        <v>929</v>
+      </c>
+      <c r="M20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1270,6 +1331,9 @@
       <c r="L21" t="n">
         <v>499</v>
       </c>
+      <c r="M21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1286,10 +1350,10 @@
       <c r="D22" t="n">
         <v>299</v>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>299</v>
-      </c>
+      <c r="E22" t="n">
+        <v>299</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
         <v>299</v>
       </c>
@@ -1306,6 +1370,9 @@
         <v>299</v>
       </c>
       <c r="L22" t="n">
+        <v>299</v>
+      </c>
+      <c r="M22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1324,10 +1391,10 @@
       <c r="D23" t="n">
         <v>1299</v>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
         <v>1299</v>
       </c>
@@ -1344,6 +1411,9 @@
         <v>1299</v>
       </c>
       <c r="L23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="M23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1362,10 +1432,10 @@
       <c r="D24" t="n">
         <v>929</v>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>929</v>
-      </c>
+      <c r="E24" t="n">
+        <v>929</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
         <v>929</v>
       </c>
@@ -1382,6 +1452,9 @@
         <v>929</v>
       </c>
       <c r="L24" t="n">
+        <v>929</v>
+      </c>
+      <c r="M24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1400,10 +1473,10 @@
       <c r="D25" t="n">
         <v>929</v>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>929</v>
-      </c>
+      <c r="E25" t="n">
+        <v>929</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>929</v>
       </c>
@@ -1420,6 +1493,9 @@
         <v>929</v>
       </c>
       <c r="L25" t="n">
+        <v>929</v>
+      </c>
+      <c r="M25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1438,10 +1514,10 @@
       <c r="D26" t="n">
         <v>1299</v>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
         <v>1299</v>
       </c>
@@ -1458,6 +1534,9 @@
         <v>1299</v>
       </c>
       <c r="L26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="M26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 10:46
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,7 @@
     <col width="21" customWidth="1" min="11" max="11"/>
     <col width="21" customWidth="1" min="12" max="12"/>
     <col width="21" customWidth="1" min="13" max="13"/>
+    <col width="21" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,60 +457,65 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 16:12</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -521,17 +527,17 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>929</v>
-      </c>
+      <c r="B2" t="n">
+        <v>929</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
         <v>929</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>929</v>
-      </c>
+      <c r="E2" t="n">
+        <v>929</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>929</v>
       </c>
@@ -551,6 +557,9 @@
         <v>929</v>
       </c>
       <c r="M2" t="n">
+        <v>929</v>
+      </c>
+      <c r="N2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -572,10 +581,10 @@
       <c r="E3" t="n">
         <v>569</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>569</v>
-      </c>
+      <c r="F3" t="n">
+        <v>569</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>569</v>
       </c>
@@ -592,6 +601,9 @@
         <v>569</v>
       </c>
       <c r="M3" t="n">
+        <v>569</v>
+      </c>
+      <c r="N3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -613,10 +625,10 @@
       <c r="E4" t="n">
         <v>299</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>299</v>
-      </c>
+      <c r="F4" t="n">
+        <v>299</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>299</v>
       </c>
@@ -633,6 +645,9 @@
         <v>299</v>
       </c>
       <c r="M4" t="n">
+        <v>299</v>
+      </c>
+      <c r="N4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -654,10 +669,10 @@
       <c r="E5" t="n">
         <v>569</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>569</v>
-      </c>
+      <c r="F5" t="n">
+        <v>569</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>569</v>
       </c>
@@ -674,6 +689,9 @@
         <v>569</v>
       </c>
       <c r="M5" t="n">
+        <v>569</v>
+      </c>
+      <c r="N5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -695,10 +713,10 @@
       <c r="E6" t="n">
         <v>499</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>499</v>
-      </c>
+      <c r="F6" t="n">
+        <v>499</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>499</v>
       </c>
@@ -715,6 +733,9 @@
         <v>499</v>
       </c>
       <c r="M6" t="n">
+        <v>499</v>
+      </c>
+      <c r="N6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -736,10 +757,10 @@
       <c r="E7" t="n">
         <v>569</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>569</v>
-      </c>
+      <c r="F7" t="n">
+        <v>569</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>569</v>
       </c>
@@ -756,6 +777,9 @@
         <v>569</v>
       </c>
       <c r="M7" t="n">
+        <v>569</v>
+      </c>
+      <c r="N7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -777,10 +801,10 @@
       <c r="E8" t="n">
         <v>929</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>929</v>
-      </c>
+      <c r="F8" t="n">
+        <v>929</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
         <v>929</v>
       </c>
@@ -797,6 +821,9 @@
         <v>929</v>
       </c>
       <c r="M8" t="n">
+        <v>929</v>
+      </c>
+      <c r="N8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -818,10 +845,10 @@
       <c r="E9" t="n">
         <v>299</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>299</v>
-      </c>
+      <c r="F9" t="n">
+        <v>299</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>299</v>
       </c>
@@ -838,6 +865,9 @@
         <v>299</v>
       </c>
       <c r="M9" t="n">
+        <v>299</v>
+      </c>
+      <c r="N9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -859,10 +889,10 @@
       <c r="E10" t="n">
         <v>299</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>299</v>
-      </c>
+      <c r="F10" t="n">
+        <v>299</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>299</v>
       </c>
@@ -879,6 +909,9 @@
         <v>299</v>
       </c>
       <c r="M10" t="n">
+        <v>299</v>
+      </c>
+      <c r="N10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -895,15 +928,15 @@
         <v>2997</v>
       </c>
       <c r="D11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="E11" t="n">
         <v>929</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="n">
-        <v>929</v>
-      </c>
+      <c r="F11" t="n">
+        <v>929</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
         <v>929</v>
       </c>
@@ -920,6 +953,9 @@
         <v>929</v>
       </c>
       <c r="M11" t="n">
+        <v>929</v>
+      </c>
+      <c r="N11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -941,10 +977,10 @@
       <c r="E12" t="n">
         <v>569</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="n">
-        <v>569</v>
-      </c>
+      <c r="F12" t="n">
+        <v>569</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
         <v>569</v>
       </c>
@@ -961,6 +997,9 @@
         <v>569</v>
       </c>
       <c r="M12" t="n">
+        <v>569</v>
+      </c>
+      <c r="N12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -982,24 +1021,27 @@
       <c r="E13" t="n">
         <v>569</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>569</v>
-      </c>
+      <c r="F13" t="n">
+        <v>569</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>569</v>
       </c>
       <c r="I13" t="n">
         <v>569</v>
       </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>569</v>
-      </c>
+      <c r="J13" t="n">
+        <v>569</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
         <v>569</v>
       </c>
       <c r="M13" t="n">
+        <v>569</v>
+      </c>
+      <c r="N13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1045,6 +1087,9 @@
       <c r="M14" t="n">
         <v>499</v>
       </c>
+      <c r="N14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1058,14 +1103,14 @@
       <c r="C15" t="n">
         <v>499</v>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>499</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>499</v>
-      </c>
+      <c r="D15" t="n">
+        <v>499</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>499</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
         <v>499</v>
       </c>
@@ -1082,6 +1127,9 @@
         <v>499</v>
       </c>
       <c r="M15" t="n">
+        <v>499</v>
+      </c>
+      <c r="N15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1103,10 +1151,10 @@
       <c r="E16" t="n">
         <v>299</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>299</v>
-      </c>
+      <c r="F16" t="n">
+        <v>299</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
         <v>299</v>
       </c>
@@ -1123,6 +1171,9 @@
         <v>299</v>
       </c>
       <c r="M16" t="n">
+        <v>299</v>
+      </c>
+      <c r="N16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1144,10 +1195,10 @@
       <c r="E17" t="n">
         <v>929</v>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="n">
-        <v>929</v>
-      </c>
+      <c r="F17" t="n">
+        <v>929</v>
+      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
         <v>929</v>
       </c>
@@ -1164,6 +1215,9 @@
         <v>929</v>
       </c>
       <c r="M17" t="n">
+        <v>929</v>
+      </c>
+      <c r="N17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1185,10 +1239,10 @@
       <c r="E18" t="n">
         <v>499</v>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="n">
-        <v>499</v>
-      </c>
+      <c r="F18" t="n">
+        <v>499</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
         <v>499</v>
       </c>
@@ -1205,6 +1259,9 @@
         <v>499</v>
       </c>
       <c r="M18" t="n">
+        <v>499</v>
+      </c>
+      <c r="N18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1248,6 +1305,9 @@
         <v>1497</v>
       </c>
       <c r="M19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="N19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1269,10 +1329,10 @@
       <c r="E20" t="n">
         <v>929</v>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="n">
-        <v>929</v>
-      </c>
+      <c r="F20" t="n">
+        <v>929</v>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
         <v>929</v>
       </c>
@@ -1289,6 +1349,9 @@
         <v>929</v>
       </c>
       <c r="M20" t="n">
+        <v>929</v>
+      </c>
+      <c r="N20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1334,6 +1397,9 @@
       <c r="M21" t="n">
         <v>499</v>
       </c>
+      <c r="N21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1353,10 +1419,10 @@
       <c r="E22" t="n">
         <v>299</v>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="n">
-        <v>299</v>
-      </c>
+      <c r="F22" t="n">
+        <v>299</v>
+      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
         <v>299</v>
       </c>
@@ -1373,6 +1439,9 @@
         <v>299</v>
       </c>
       <c r="M22" t="n">
+        <v>299</v>
+      </c>
+      <c r="N22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1394,10 +1463,10 @@
       <c r="E23" t="n">
         <v>1299</v>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
         <v>1299</v>
       </c>
@@ -1414,6 +1483,9 @@
         <v>1299</v>
       </c>
       <c r="M23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="N23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1435,10 +1507,10 @@
       <c r="E24" t="n">
         <v>929</v>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="n">
-        <v>929</v>
-      </c>
+      <c r="F24" t="n">
+        <v>929</v>
+      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
         <v>929</v>
       </c>
@@ -1455,6 +1527,9 @@
         <v>929</v>
       </c>
       <c r="M24" t="n">
+        <v>929</v>
+      </c>
+      <c r="N24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1476,10 +1551,10 @@
       <c r="E25" t="n">
         <v>929</v>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
-        <v>929</v>
-      </c>
+      <c r="F25" t="n">
+        <v>929</v>
+      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
         <v>929</v>
       </c>
@@ -1496,6 +1571,9 @@
         <v>929</v>
       </c>
       <c r="M25" t="n">
+        <v>929</v>
+      </c>
+      <c r="N25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1517,10 +1595,10 @@
       <c r="E26" t="n">
         <v>1299</v>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
         <v>1299</v>
       </c>
@@ -1537,6 +1615,9 @@
         <v>1299</v>
       </c>
       <c r="M26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="N26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 13:39
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,7 @@
     <col width="21" customWidth="1" min="12" max="12"/>
     <col width="21" customWidth="1" min="13" max="13"/>
     <col width="21" customWidth="1" min="14" max="14"/>
+    <col width="21" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -457,65 +458,70 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 19:06</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -530,17 +536,17 @@
       <c r="B2" t="n">
         <v>929</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>929</v>
-      </c>
+      <c r="C2" t="n">
+        <v>929</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>929</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>929</v>
-      </c>
+      <c r="F2" t="n">
+        <v>929</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>929</v>
       </c>
@@ -560,6 +566,9 @@
         <v>929</v>
       </c>
       <c r="N2" t="n">
+        <v>929</v>
+      </c>
+      <c r="O2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -584,10 +593,10 @@
       <c r="F3" t="n">
         <v>569</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>569</v>
-      </c>
+      <c r="G3" t="n">
+        <v>569</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>569</v>
       </c>
@@ -604,6 +613,9 @@
         <v>569</v>
       </c>
       <c r="N3" t="n">
+        <v>569</v>
+      </c>
+      <c r="O3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -628,10 +640,10 @@
       <c r="F4" t="n">
         <v>299</v>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>299</v>
-      </c>
+      <c r="G4" t="n">
+        <v>299</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>299</v>
       </c>
@@ -648,6 +660,9 @@
         <v>299</v>
       </c>
       <c r="N4" t="n">
+        <v>299</v>
+      </c>
+      <c r="O4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -672,10 +687,10 @@
       <c r="F5" t="n">
         <v>569</v>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
-        <v>569</v>
-      </c>
+      <c r="G5" t="n">
+        <v>569</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>569</v>
       </c>
@@ -692,6 +707,9 @@
         <v>569</v>
       </c>
       <c r="N5" t="n">
+        <v>569</v>
+      </c>
+      <c r="O5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -716,10 +734,10 @@
       <c r="F6" t="n">
         <v>499</v>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
-        <v>499</v>
-      </c>
+      <c r="G6" t="n">
+        <v>499</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>499</v>
       </c>
@@ -736,6 +754,9 @@
         <v>499</v>
       </c>
       <c r="N6" t="n">
+        <v>499</v>
+      </c>
+      <c r="O6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -760,10 +781,10 @@
       <c r="F7" t="n">
         <v>569</v>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>569</v>
-      </c>
+      <c r="G7" t="n">
+        <v>569</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
         <v>569</v>
       </c>
@@ -780,6 +801,9 @@
         <v>569</v>
       </c>
       <c r="N7" t="n">
+        <v>569</v>
+      </c>
+      <c r="O7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -804,10 +828,10 @@
       <c r="F8" t="n">
         <v>929</v>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>929</v>
-      </c>
+      <c r="G8" t="n">
+        <v>929</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>929</v>
       </c>
@@ -824,6 +848,9 @@
         <v>929</v>
       </c>
       <c r="N8" t="n">
+        <v>929</v>
+      </c>
+      <c r="O8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -848,10 +875,10 @@
       <c r="F9" t="n">
         <v>299</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>299</v>
-      </c>
+      <c r="G9" t="n">
+        <v>299</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>299</v>
       </c>
@@ -868,6 +895,9 @@
         <v>299</v>
       </c>
       <c r="N9" t="n">
+        <v>299</v>
+      </c>
+      <c r="O9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -892,10 +922,10 @@
       <c r="F10" t="n">
         <v>299</v>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>299</v>
-      </c>
+      <c r="G10" t="n">
+        <v>299</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>299</v>
       </c>
@@ -912,6 +942,9 @@
         <v>299</v>
       </c>
       <c r="N10" t="n">
+        <v>299</v>
+      </c>
+      <c r="O10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -931,15 +964,15 @@
         <v>2997</v>
       </c>
       <c r="E11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="F11" t="n">
         <v>929</v>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
-        <v>929</v>
-      </c>
+      <c r="G11" t="n">
+        <v>929</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>929</v>
       </c>
@@ -956,6 +989,9 @@
         <v>929</v>
       </c>
       <c r="N11" t="n">
+        <v>929</v>
+      </c>
+      <c r="O11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -980,10 +1016,10 @@
       <c r="F12" t="n">
         <v>569</v>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="n">
-        <v>569</v>
-      </c>
+      <c r="G12" t="n">
+        <v>569</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
         <v>569</v>
       </c>
@@ -1000,6 +1036,9 @@
         <v>569</v>
       </c>
       <c r="N12" t="n">
+        <v>569</v>
+      </c>
+      <c r="O12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1024,24 +1063,27 @@
       <c r="F13" t="n">
         <v>569</v>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>569</v>
-      </c>
+      <c r="G13" t="n">
+        <v>569</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>569</v>
       </c>
       <c r="J13" t="n">
         <v>569</v>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="n">
-        <v>569</v>
-      </c>
+      <c r="K13" t="n">
+        <v>569</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
         <v>569</v>
       </c>
       <c r="N13" t="n">
+        <v>569</v>
+      </c>
+      <c r="O13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1090,6 +1132,9 @@
       <c r="N14" t="n">
         <v>499</v>
       </c>
+      <c r="O14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1106,14 +1151,14 @@
       <c r="D15" t="n">
         <v>499</v>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>499</v>
-      </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="n">
-        <v>499</v>
-      </c>
+      <c r="E15" t="n">
+        <v>499</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>499</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
         <v>499</v>
       </c>
@@ -1130,6 +1175,9 @@
         <v>499</v>
       </c>
       <c r="N15" t="n">
+        <v>499</v>
+      </c>
+      <c r="O15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1154,10 +1202,10 @@
       <c r="F16" t="n">
         <v>299</v>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="n">
-        <v>299</v>
-      </c>
+      <c r="G16" t="n">
+        <v>299</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
         <v>299</v>
       </c>
@@ -1174,6 +1222,9 @@
         <v>299</v>
       </c>
       <c r="N16" t="n">
+        <v>299</v>
+      </c>
+      <c r="O16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1198,10 +1249,10 @@
       <c r="F17" t="n">
         <v>929</v>
       </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="n">
-        <v>929</v>
-      </c>
+      <c r="G17" t="n">
+        <v>929</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
         <v>929</v>
       </c>
@@ -1218,6 +1269,9 @@
         <v>929</v>
       </c>
       <c r="N17" t="n">
+        <v>929</v>
+      </c>
+      <c r="O17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1242,10 +1296,10 @@
       <c r="F18" t="n">
         <v>499</v>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="n">
-        <v>499</v>
-      </c>
+      <c r="G18" t="n">
+        <v>499</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
         <v>499</v>
       </c>
@@ -1262,6 +1316,9 @@
         <v>499</v>
       </c>
       <c r="N18" t="n">
+        <v>499</v>
+      </c>
+      <c r="O18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1272,7 +1329,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1497</v>
+        <v>465</v>
       </c>
       <c r="C19" t="n">
         <v>1497</v>
@@ -1308,6 +1365,9 @@
         <v>1497</v>
       </c>
       <c r="N19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="O19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1332,10 +1392,10 @@
       <c r="F20" t="n">
         <v>929</v>
       </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="n">
-        <v>929</v>
-      </c>
+      <c r="G20" t="n">
+        <v>929</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
         <v>929</v>
       </c>
@@ -1352,6 +1412,9 @@
         <v>929</v>
       </c>
       <c r="N20" t="n">
+        <v>929</v>
+      </c>
+      <c r="O20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1400,6 +1463,9 @@
       <c r="N21" t="n">
         <v>499</v>
       </c>
+      <c r="O21" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1422,10 +1488,10 @@
       <c r="F22" t="n">
         <v>299</v>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="n">
-        <v>299</v>
-      </c>
+      <c r="G22" t="n">
+        <v>299</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
         <v>299</v>
       </c>
@@ -1442,6 +1508,9 @@
         <v>299</v>
       </c>
       <c r="N22" t="n">
+        <v>299</v>
+      </c>
+      <c r="O22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1466,10 +1535,10 @@
       <c r="F23" t="n">
         <v>1299</v>
       </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
         <v>1299</v>
       </c>
@@ -1486,6 +1555,9 @@
         <v>1299</v>
       </c>
       <c r="N23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="O23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1510,10 +1582,10 @@
       <c r="F24" t="n">
         <v>929</v>
       </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="n">
-        <v>929</v>
-      </c>
+      <c r="G24" t="n">
+        <v>929</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
         <v>929</v>
       </c>
@@ -1530,6 +1602,9 @@
         <v>929</v>
       </c>
       <c r="N24" t="n">
+        <v>929</v>
+      </c>
+      <c r="O24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1554,10 +1629,10 @@
       <c r="F25" t="n">
         <v>929</v>
       </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="n">
-        <v>929</v>
-      </c>
+      <c r="G25" t="n">
+        <v>929</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
         <v>929</v>
       </c>
@@ -1574,6 +1649,9 @@
         <v>929</v>
       </c>
       <c r="N25" t="n">
+        <v>929</v>
+      </c>
+      <c r="O25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1598,10 +1676,10 @@
       <c r="F26" t="n">
         <v>1299</v>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
         <v>1299</v>
       </c>
@@ -1618,6 +1696,9 @@
         <v>1299</v>
       </c>
       <c r="N26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="O26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 14:45
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +448,7 @@
     <col width="21" customWidth="1" min="13" max="13"/>
     <col width="21" customWidth="1" min="14" max="14"/>
     <col width="21" customWidth="1" min="15" max="15"/>
+    <col width="21" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -458,70 +459,75 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 20:09</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -533,23 +539,21 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>929</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
         <v>929</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>929</v>
-      </c>
+      <c r="D2" t="n">
+        <v>929</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
         <v>929</v>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>929</v>
-      </c>
+      <c r="G2" t="n">
+        <v>929</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>929</v>
       </c>
@@ -569,6 +573,9 @@
         <v>929</v>
       </c>
       <c r="O2" t="n">
+        <v>929</v>
+      </c>
+      <c r="P2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -578,9 +585,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>569</v>
       </c>
@@ -596,10 +601,10 @@
       <c r="G3" t="n">
         <v>569</v>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>569</v>
-      </c>
+      <c r="H3" t="n">
+        <v>569</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
         <v>569</v>
       </c>
@@ -616,6 +621,9 @@
         <v>569</v>
       </c>
       <c r="O3" t="n">
+        <v>569</v>
+      </c>
+      <c r="P3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -643,10 +651,10 @@
       <c r="G4" t="n">
         <v>299</v>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>299</v>
-      </c>
+      <c r="H4" t="n">
+        <v>299</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
         <v>299</v>
       </c>
@@ -663,6 +671,9 @@
         <v>299</v>
       </c>
       <c r="O4" t="n">
+        <v>299</v>
+      </c>
+      <c r="P4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -690,10 +701,10 @@
       <c r="G5" t="n">
         <v>569</v>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>569</v>
-      </c>
+      <c r="H5" t="n">
+        <v>569</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="n">
         <v>569</v>
       </c>
@@ -710,6 +721,9 @@
         <v>569</v>
       </c>
       <c r="O5" t="n">
+        <v>569</v>
+      </c>
+      <c r="P5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -737,10 +751,10 @@
       <c r="G6" t="n">
         <v>499</v>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>499</v>
-      </c>
+      <c r="H6" t="n">
+        <v>499</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
         <v>499</v>
       </c>
@@ -757,6 +771,9 @@
         <v>499</v>
       </c>
       <c r="O6" t="n">
+        <v>499</v>
+      </c>
+      <c r="P6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -766,9 +783,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>569</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
         <v>569</v>
       </c>
@@ -784,10 +799,10 @@
       <c r="G7" t="n">
         <v>569</v>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>569</v>
-      </c>
+      <c r="H7" t="n">
+        <v>569</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
         <v>569</v>
       </c>
@@ -804,6 +819,9 @@
         <v>569</v>
       </c>
       <c r="O7" t="n">
+        <v>569</v>
+      </c>
+      <c r="P7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -813,9 +831,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
         <v>929</v>
       </c>
@@ -831,10 +847,10 @@
       <c r="G8" t="n">
         <v>929</v>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
-        <v>929</v>
-      </c>
+      <c r="H8" t="n">
+        <v>929</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
         <v>929</v>
       </c>
@@ -851,6 +867,9 @@
         <v>929</v>
       </c>
       <c r="O8" t="n">
+        <v>929</v>
+      </c>
+      <c r="P8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -878,10 +897,10 @@
       <c r="G9" t="n">
         <v>299</v>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
-        <v>299</v>
-      </c>
+      <c r="H9" t="n">
+        <v>299</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
         <v>299</v>
       </c>
@@ -898,6 +917,9 @@
         <v>299</v>
       </c>
       <c r="O9" t="n">
+        <v>299</v>
+      </c>
+      <c r="P9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -907,9 +929,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
         <v>299</v>
       </c>
@@ -925,10 +945,10 @@
       <c r="G10" t="n">
         <v>299</v>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
-        <v>299</v>
-      </c>
+      <c r="H10" t="n">
+        <v>299</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="n">
         <v>299</v>
       </c>
@@ -945,6 +965,9 @@
         <v>299</v>
       </c>
       <c r="O10" t="n">
+        <v>299</v>
+      </c>
+      <c r="P10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -967,15 +990,15 @@
         <v>2997</v>
       </c>
       <c r="F11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="G11" t="n">
         <v>929</v>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
-        <v>929</v>
-      </c>
+      <c r="H11" t="n">
+        <v>929</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
         <v>929</v>
       </c>
@@ -992,6 +1015,9 @@
         <v>929</v>
       </c>
       <c r="O11" t="n">
+        <v>929</v>
+      </c>
+      <c r="P11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1001,9 +1027,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>569</v>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
         <v>569</v>
       </c>
@@ -1019,10 +1043,10 @@
       <c r="G12" t="n">
         <v>569</v>
       </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
-        <v>569</v>
-      </c>
+      <c r="H12" t="n">
+        <v>569</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="n">
         <v>569</v>
       </c>
@@ -1039,6 +1063,9 @@
         <v>569</v>
       </c>
       <c r="O12" t="n">
+        <v>569</v>
+      </c>
+      <c r="P12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1048,9 +1075,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
         <v>569</v>
       </c>
@@ -1066,24 +1091,27 @@
       <c r="G13" t="n">
         <v>569</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>569</v>
-      </c>
+      <c r="H13" t="n">
+        <v>569</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
         <v>569</v>
       </c>
       <c r="K13" t="n">
         <v>569</v>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>569</v>
-      </c>
+      <c r="L13" t="n">
+        <v>569</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
         <v>569</v>
       </c>
       <c r="O13" t="n">
+        <v>569</v>
+      </c>
+      <c r="P13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1135,6 +1163,9 @@
       <c r="O14" t="n">
         <v>499</v>
       </c>
+      <c r="P14" t="n">
+        <v>499</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1142,9 +1173,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>499</v>
-      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
         <v>499</v>
       </c>
@@ -1154,14 +1183,14 @@
       <c r="E15" t="n">
         <v>499</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>499</v>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
-        <v>499</v>
-      </c>
+      <c r="F15" t="n">
+        <v>499</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>499</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="n">
         <v>499</v>
       </c>
@@ -1178,6 +1207,9 @@
         <v>499</v>
       </c>
       <c r="O15" t="n">
+        <v>499</v>
+      </c>
+      <c r="P15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1205,10 +1237,10 @@
       <c r="G16" t="n">
         <v>299</v>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>299</v>
-      </c>
+      <c r="H16" t="n">
+        <v>299</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
         <v>299</v>
       </c>
@@ -1225,6 +1257,9 @@
         <v>299</v>
       </c>
       <c r="O16" t="n">
+        <v>299</v>
+      </c>
+      <c r="P16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1234,9 +1269,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>929</v>
-      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
         <v>929</v>
       </c>
@@ -1252,10 +1285,10 @@
       <c r="G17" t="n">
         <v>929</v>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="n">
-        <v>929</v>
-      </c>
+      <c r="H17" t="n">
+        <v>929</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="n">
         <v>929</v>
       </c>
@@ -1272,6 +1305,9 @@
         <v>929</v>
       </c>
       <c r="O17" t="n">
+        <v>929</v>
+      </c>
+      <c r="P17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1281,9 +1317,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>499</v>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="n">
         <v>499</v>
       </c>
@@ -1299,10 +1333,10 @@
       <c r="G18" t="n">
         <v>499</v>
       </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="n">
-        <v>499</v>
-      </c>
+      <c r="H18" t="n">
+        <v>499</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="n">
         <v>499</v>
       </c>
@@ -1319,6 +1353,9 @@
         <v>499</v>
       </c>
       <c r="O18" t="n">
+        <v>499</v>
+      </c>
+      <c r="P18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1328,11 +1365,9 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="n">
         <v>465</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1497</v>
       </c>
       <c r="D19" t="n">
         <v>1497</v>
@@ -1368,6 +1403,9 @@
         <v>1497</v>
       </c>
       <c r="O19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="P19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1395,10 +1433,10 @@
       <c r="G20" t="n">
         <v>929</v>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="n">
-        <v>929</v>
-      </c>
+      <c r="H20" t="n">
+        <v>929</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="n">
         <v>929</v>
       </c>
@@ -1415,6 +1453,9 @@
         <v>929</v>
       </c>
       <c r="O20" t="n">
+        <v>929</v>
+      </c>
+      <c r="P20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1424,9 +1465,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
         <v>499</v>
       </c>
@@ -1464,6 +1503,9 @@
         <v>499</v>
       </c>
       <c r="O21" t="n">
+        <v>499</v>
+      </c>
+      <c r="P21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1473,9 +1515,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>299</v>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
         <v>299</v>
       </c>
@@ -1491,10 +1531,10 @@
       <c r="G22" t="n">
         <v>299</v>
       </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="n">
-        <v>299</v>
-      </c>
+      <c r="H22" t="n">
+        <v>299</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="n">
         <v>299</v>
       </c>
@@ -1511,6 +1551,9 @@
         <v>299</v>
       </c>
       <c r="O22" t="n">
+        <v>299</v>
+      </c>
+      <c r="P22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1520,9 +1563,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
         <v>1299</v>
       </c>
@@ -1538,10 +1579,10 @@
       <c r="G23" t="n">
         <v>1299</v>
       </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="n">
         <v>1299</v>
       </c>
@@ -1558,6 +1599,9 @@
         <v>1299</v>
       </c>
       <c r="O23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1585,10 +1629,10 @@
       <c r="G24" t="n">
         <v>929</v>
       </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="n">
-        <v>929</v>
-      </c>
+      <c r="H24" t="n">
+        <v>929</v>
+      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="n">
         <v>929</v>
       </c>
@@ -1605,6 +1649,9 @@
         <v>929</v>
       </c>
       <c r="O24" t="n">
+        <v>929</v>
+      </c>
+      <c r="P24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1632,10 +1679,10 @@
       <c r="G25" t="n">
         <v>929</v>
       </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="n">
-        <v>929</v>
-      </c>
+      <c r="H25" t="n">
+        <v>929</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="n">
         <v>929</v>
       </c>
@@ -1652,6 +1699,9 @@
         <v>929</v>
       </c>
       <c r="O25" t="n">
+        <v>929</v>
+      </c>
+      <c r="P25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1661,9 +1711,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="n">
         <v>1299</v>
       </c>
@@ -1679,10 +1727,10 @@
       <c r="G26" t="n">
         <v>1299</v>
       </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="n">
         <v>1299</v>
       </c>
@@ -1699,6 +1747,9 @@
         <v>1299</v>
       </c>
       <c r="O26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 16:53
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,7 @@
     <col width="21" customWidth="1" min="14" max="14"/>
     <col width="21" customWidth="1" min="15" max="15"/>
     <col width="21" customWidth="1" min="16" max="16"/>
+    <col width="21" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -459,75 +460,80 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-21 22:17</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -540,23 +546,21 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>929</v>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
         <v>929</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>929</v>
-      </c>
+      <c r="E2" t="n">
+        <v>929</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>929</v>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
-        <v>929</v>
-      </c>
+      <c r="H2" t="n">
+        <v>929</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
         <v>929</v>
       </c>
@@ -576,6 +580,9 @@
         <v>929</v>
       </c>
       <c r="P2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -585,10 +592,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="n">
+        <v>569</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>569</v>
       </c>
@@ -604,10 +611,10 @@
       <c r="H3" t="n">
         <v>569</v>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>569</v>
-      </c>
+      <c r="I3" t="n">
+        <v>569</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
         <v>569</v>
       </c>
@@ -624,6 +631,9 @@
         <v>569</v>
       </c>
       <c r="P3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -654,10 +664,10 @@
       <c r="H4" t="n">
         <v>299</v>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="n">
-        <v>299</v>
-      </c>
+      <c r="I4" t="n">
+        <v>299</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
         <v>299</v>
       </c>
@@ -674,6 +684,9 @@
         <v>299</v>
       </c>
       <c r="P4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -704,10 +717,10 @@
       <c r="H5" t="n">
         <v>569</v>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="n">
-        <v>569</v>
-      </c>
+      <c r="I5" t="n">
+        <v>569</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
         <v>569</v>
       </c>
@@ -724,6 +737,9 @@
         <v>569</v>
       </c>
       <c r="P5" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -733,9 +749,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>499</v>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
         <v>499</v>
       </c>
@@ -754,10 +768,10 @@
       <c r="H6" t="n">
         <v>499</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
-        <v>499</v>
-      </c>
+      <c r="I6" t="n">
+        <v>499</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
         <v>499</v>
       </c>
@@ -774,6 +788,9 @@
         <v>499</v>
       </c>
       <c r="P6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -784,9 +801,7 @@
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="n">
-        <v>569</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
         <v>569</v>
       </c>
@@ -802,10 +817,10 @@
       <c r="H7" t="n">
         <v>569</v>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
-        <v>569</v>
-      </c>
+      <c r="I7" t="n">
+        <v>569</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
         <v>569</v>
       </c>
@@ -822,6 +837,9 @@
         <v>569</v>
       </c>
       <c r="P7" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -831,10 +849,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="n">
+        <v>929</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>929</v>
       </c>
@@ -850,10 +868,10 @@
       <c r="H8" t="n">
         <v>929</v>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
-        <v>929</v>
-      </c>
+      <c r="I8" t="n">
+        <v>929</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
         <v>929</v>
       </c>
@@ -870,6 +888,9 @@
         <v>929</v>
       </c>
       <c r="P8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -900,10 +921,10 @@
       <c r="H9" t="n">
         <v>299</v>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
-        <v>299</v>
-      </c>
+      <c r="I9" t="n">
+        <v>299</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
         <v>299</v>
       </c>
@@ -920,6 +941,9 @@
         <v>299</v>
       </c>
       <c r="P9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -929,10 +953,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="n">
+        <v>299</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>299</v>
       </c>
@@ -948,10 +972,10 @@
       <c r="H10" t="n">
         <v>299</v>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>299</v>
-      </c>
+      <c r="I10" t="n">
+        <v>299</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
         <v>299</v>
       </c>
@@ -968,6 +992,9 @@
         <v>299</v>
       </c>
       <c r="P10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -977,9 +1004,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>2997</v>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
         <v>2997</v>
       </c>
@@ -993,15 +1018,15 @@
         <v>2997</v>
       </c>
       <c r="G11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="H11" t="n">
         <v>929</v>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="n">
-        <v>929</v>
-      </c>
+      <c r="I11" t="n">
+        <v>929</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
         <v>929</v>
       </c>
@@ -1018,6 +1043,9 @@
         <v>929</v>
       </c>
       <c r="P11" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1027,10 +1055,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="n">
-        <v>569</v>
-      </c>
+      <c r="B12" t="n">
+        <v>569</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
         <v>569</v>
       </c>
@@ -1046,10 +1074,10 @@
       <c r="H12" t="n">
         <v>569</v>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="n">
-        <v>569</v>
-      </c>
+      <c r="I12" t="n">
+        <v>569</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
         <v>569</v>
       </c>
@@ -1066,6 +1094,9 @@
         <v>569</v>
       </c>
       <c r="P12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1075,10 +1106,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="n">
+        <v>569</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>569</v>
       </c>
@@ -1094,24 +1125,27 @@
       <c r="H13" t="n">
         <v>569</v>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
-        <v>569</v>
-      </c>
+      <c r="I13" t="n">
+        <v>569</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>569</v>
       </c>
       <c r="L13" t="n">
         <v>569</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="n">
-        <v>569</v>
-      </c>
+      <c r="M13" t="n">
+        <v>569</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
         <v>569</v>
       </c>
       <c r="P13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1121,9 +1155,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>499</v>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
         <v>499</v>
       </c>
@@ -1164,6 +1196,9 @@
         <v>499</v>
       </c>
       <c r="P14" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1173,10 +1208,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>499</v>
-      </c>
+      <c r="B15" t="n">
+        <v>499</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
         <v>499</v>
       </c>
@@ -1186,14 +1221,14 @@
       <c r="F15" t="n">
         <v>499</v>
       </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="n">
-        <v>499</v>
-      </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="n">
-        <v>499</v>
-      </c>
+      <c r="G15" t="n">
+        <v>499</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>499</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
         <v>499</v>
       </c>
@@ -1210,6 +1245,9 @@
         <v>499</v>
       </c>
       <c r="P15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1240,10 +1278,10 @@
       <c r="H16" t="n">
         <v>299</v>
       </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="n">
-        <v>299</v>
-      </c>
+      <c r="I16" t="n">
+        <v>299</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
         <v>299</v>
       </c>
@@ -1260,6 +1298,9 @@
         <v>299</v>
       </c>
       <c r="P16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1269,10 +1310,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="n">
-        <v>929</v>
-      </c>
+      <c r="B17" t="n">
+        <v>929</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
         <v>929</v>
       </c>
@@ -1288,10 +1329,10 @@
       <c r="H17" t="n">
         <v>929</v>
       </c>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="n">
-        <v>929</v>
-      </c>
+      <c r="I17" t="n">
+        <v>929</v>
+      </c>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
         <v>929</v>
       </c>
@@ -1308,6 +1349,9 @@
         <v>929</v>
       </c>
       <c r="P17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1318,9 +1362,7 @@
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="n">
-        <v>499</v>
-      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
         <v>499</v>
       </c>
@@ -1336,10 +1378,10 @@
       <c r="H18" t="n">
         <v>499</v>
       </c>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="n">
-        <v>499</v>
-      </c>
+      <c r="I18" t="n">
+        <v>499</v>
+      </c>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
         <v>499</v>
       </c>
@@ -1356,6 +1398,9 @@
         <v>499</v>
       </c>
       <c r="P18" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1366,11 +1411,9 @@
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="n">
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="n">
         <v>465</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1497</v>
       </c>
       <c r="E19" t="n">
         <v>1497</v>
@@ -1406,6 +1449,9 @@
         <v>1497</v>
       </c>
       <c r="P19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="Q19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1436,10 +1482,10 @@
       <c r="H20" t="n">
         <v>929</v>
       </c>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="n">
-        <v>929</v>
-      </c>
+      <c r="I20" t="n">
+        <v>929</v>
+      </c>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
         <v>929</v>
       </c>
@@ -1456,6 +1502,9 @@
         <v>929</v>
       </c>
       <c r="P20" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1465,10 +1514,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="n">
+        <v>499</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>499</v>
       </c>
@@ -1506,6 +1555,9 @@
         <v>499</v>
       </c>
       <c r="P21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1515,10 +1567,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="n">
-        <v>299</v>
-      </c>
+      <c r="B22" t="n">
+        <v>299</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
         <v>299</v>
       </c>
@@ -1534,10 +1586,10 @@
       <c r="H22" t="n">
         <v>299</v>
       </c>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="n">
-        <v>299</v>
-      </c>
+      <c r="I22" t="n">
+        <v>299</v>
+      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
         <v>299</v>
       </c>
@@ -1554,6 +1606,9 @@
         <v>299</v>
       </c>
       <c r="P22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1564,9 +1619,7 @@
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
         <v>1299</v>
       </c>
@@ -1582,10 +1635,10 @@
       <c r="H23" t="n">
         <v>1299</v>
       </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
         <v>1299</v>
       </c>
@@ -1602,6 +1655,9 @@
         <v>1299</v>
       </c>
       <c r="P23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Q23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1611,9 +1667,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>929</v>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="n">
         <v>929</v>
       </c>
@@ -1632,10 +1686,10 @@
       <c r="H24" t="n">
         <v>929</v>
       </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="n">
-        <v>929</v>
-      </c>
+      <c r="I24" t="n">
+        <v>929</v>
+      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
         <v>929</v>
       </c>
@@ -1652,6 +1706,9 @@
         <v>929</v>
       </c>
       <c r="P24" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1661,9 +1718,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>929</v>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
         <v>929</v>
       </c>
@@ -1682,10 +1737,10 @@
       <c r="H25" t="n">
         <v>929</v>
       </c>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="n">
-        <v>929</v>
-      </c>
+      <c r="I25" t="n">
+        <v>929</v>
+      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
         <v>929</v>
       </c>
@@ -1702,6 +1757,9 @@
         <v>929</v>
       </c>
       <c r="P25" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1711,10 +1769,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
         <v>1299</v>
       </c>
@@ -1730,10 +1788,10 @@
       <c r="H26" t="n">
         <v>1299</v>
       </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
         <v>1299</v>
       </c>
@@ -1750,6 +1808,9 @@
         <v>1299</v>
       </c>
       <c r="P26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Q26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 18:59
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,7 @@
     <col width="21" customWidth="1" min="15" max="15"/>
     <col width="21" customWidth="1" min="16" max="16"/>
     <col width="21" customWidth="1" min="17" max="17"/>
+    <col width="21" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -460,80 +461,85 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 00:24</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -545,25 +551,25 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>929</v>
+      </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>929</v>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>929</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>929</v>
-      </c>
+      <c r="F2" t="n">
+        <v>929</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>929</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
-        <v>929</v>
-      </c>
+      <c r="I2" t="n">
+        <v>929</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
         <v>929</v>
       </c>
@@ -583,6 +589,9 @@
         <v>929</v>
       </c>
       <c r="Q2" t="n">
+        <v>929</v>
+      </c>
+      <c r="R2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -592,13 +601,11 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>569</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>569</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>569</v>
       </c>
@@ -614,10 +621,10 @@
       <c r="I3" t="n">
         <v>569</v>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>569</v>
-      </c>
+      <c r="J3" t="n">
+        <v>569</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
         <v>569</v>
       </c>
@@ -634,6 +641,9 @@
         <v>569</v>
       </c>
       <c r="Q3" t="n">
+        <v>569</v>
+      </c>
+      <c r="R3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -643,9 +653,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>299</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
         <v>299</v>
       </c>
@@ -667,10 +675,10 @@
       <c r="I4" t="n">
         <v>299</v>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="n">
-        <v>299</v>
-      </c>
+      <c r="J4" t="n">
+        <v>299</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="n">
         <v>299</v>
       </c>
@@ -687,6 +695,9 @@
         <v>299</v>
       </c>
       <c r="Q4" t="n">
+        <v>299</v>
+      </c>
+      <c r="R4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -720,10 +731,10 @@
       <c r="I5" t="n">
         <v>569</v>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>569</v>
-      </c>
+      <c r="J5" t="n">
+        <v>569</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="n">
         <v>569</v>
       </c>
@@ -740,6 +751,9 @@
         <v>569</v>
       </c>
       <c r="Q5" t="n">
+        <v>569</v>
+      </c>
+      <c r="R5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -749,10 +763,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="n">
-        <v>499</v>
-      </c>
+      <c r="B6" t="n">
+        <v>499</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
         <v>499</v>
       </c>
@@ -771,10 +785,10 @@
       <c r="I6" t="n">
         <v>499</v>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>499</v>
-      </c>
+      <c r="J6" t="n">
+        <v>499</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="n">
         <v>499</v>
       </c>
@@ -791,6 +805,9 @@
         <v>499</v>
       </c>
       <c r="Q6" t="n">
+        <v>499</v>
+      </c>
+      <c r="R6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -802,9 +819,7 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
-        <v>569</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
         <v>569</v>
       </c>
@@ -820,10 +835,10 @@
       <c r="I7" t="n">
         <v>569</v>
       </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>569</v>
-      </c>
+      <c r="J7" t="n">
+        <v>569</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
         <v>569</v>
       </c>
@@ -840,6 +855,9 @@
         <v>569</v>
       </c>
       <c r="Q7" t="n">
+        <v>569</v>
+      </c>
+      <c r="R7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -849,13 +867,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>929</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>929</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>929</v>
       </c>
@@ -871,10 +887,10 @@
       <c r="I8" t="n">
         <v>929</v>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>929</v>
-      </c>
+      <c r="J8" t="n">
+        <v>929</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="n">
         <v>929</v>
       </c>
@@ -891,6 +907,9 @@
         <v>929</v>
       </c>
       <c r="Q8" t="n">
+        <v>929</v>
+      </c>
+      <c r="R8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -900,9 +919,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>299</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
         <v>299</v>
       </c>
@@ -924,10 +941,10 @@
       <c r="I9" t="n">
         <v>299</v>
       </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="n">
-        <v>299</v>
-      </c>
+      <c r="J9" t="n">
+        <v>299</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="n">
         <v>299</v>
       </c>
@@ -944,6 +961,9 @@
         <v>299</v>
       </c>
       <c r="Q9" t="n">
+        <v>299</v>
+      </c>
+      <c r="R9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -953,13 +973,11 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>299</v>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>299</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
         <v>299</v>
       </c>
@@ -975,10 +993,10 @@
       <c r="I10" t="n">
         <v>299</v>
       </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>299</v>
-      </c>
+      <c r="J10" t="n">
+        <v>299</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
         <v>299</v>
       </c>
@@ -995,6 +1013,9 @@
         <v>299</v>
       </c>
       <c r="Q10" t="n">
+        <v>299</v>
+      </c>
+      <c r="R10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1004,10 +1025,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="n">
+      <c r="B11" t="n">
         <v>2997</v>
       </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>2997</v>
       </c>
@@ -1021,15 +1042,15 @@
         <v>2997</v>
       </c>
       <c r="H11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="I11" t="n">
         <v>929</v>
       </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="n">
-        <v>929</v>
-      </c>
+      <c r="J11" t="n">
+        <v>929</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="n">
         <v>929</v>
       </c>
@@ -1046,6 +1067,9 @@
         <v>929</v>
       </c>
       <c r="Q11" t="n">
+        <v>929</v>
+      </c>
+      <c r="R11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1058,10 +1082,10 @@
       <c r="B12" t="n">
         <v>569</v>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="n">
-        <v>569</v>
-      </c>
+      <c r="C12" t="n">
+        <v>569</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
         <v>569</v>
       </c>
@@ -1077,10 +1101,10 @@
       <c r="I12" t="n">
         <v>569</v>
       </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
-        <v>569</v>
-      </c>
+      <c r="J12" t="n">
+        <v>569</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
         <v>569</v>
       </c>
@@ -1097,6 +1121,9 @@
         <v>569</v>
       </c>
       <c r="Q12" t="n">
+        <v>569</v>
+      </c>
+      <c r="R12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1106,13 +1133,11 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>569</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>569</v>
       </c>
@@ -1128,24 +1153,27 @@
       <c r="I13" t="n">
         <v>569</v>
       </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>569</v>
-      </c>
+      <c r="J13" t="n">
+        <v>569</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
         <v>569</v>
       </c>
       <c r="M13" t="n">
         <v>569</v>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="n">
-        <v>569</v>
-      </c>
+      <c r="N13" t="n">
+        <v>569</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
         <v>569</v>
       </c>
       <c r="Q13" t="n">
+        <v>569</v>
+      </c>
+      <c r="R13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1156,9 +1184,7 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="n">
-        <v>499</v>
-      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
         <v>499</v>
       </c>
@@ -1199,6 +1225,9 @@
         <v>499</v>
       </c>
       <c r="Q14" t="n">
+        <v>499</v>
+      </c>
+      <c r="R14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1211,10 +1240,10 @@
       <c r="B15" t="n">
         <v>499</v>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="n">
-        <v>499</v>
-      </c>
+      <c r="C15" t="n">
+        <v>499</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>499</v>
       </c>
@@ -1224,14 +1253,14 @@
       <c r="G15" t="n">
         <v>499</v>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
-        <v>499</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="n">
-        <v>499</v>
-      </c>
+      <c r="H15" t="n">
+        <v>499</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>499</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="n">
         <v>499</v>
       </c>
@@ -1248,6 +1277,9 @@
         <v>499</v>
       </c>
       <c r="Q15" t="n">
+        <v>499</v>
+      </c>
+      <c r="R15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1257,9 +1289,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
         <v>299</v>
       </c>
@@ -1281,10 +1311,10 @@
       <c r="I16" t="n">
         <v>299</v>
       </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="n">
-        <v>299</v>
-      </c>
+      <c r="J16" t="n">
+        <v>299</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="n">
         <v>299</v>
       </c>
@@ -1301,6 +1331,9 @@
         <v>299</v>
       </c>
       <c r="Q16" t="n">
+        <v>299</v>
+      </c>
+      <c r="R16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1313,10 +1346,10 @@
       <c r="B17" t="n">
         <v>929</v>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="n">
-        <v>929</v>
-      </c>
+      <c r="C17" t="n">
+        <v>929</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
         <v>929</v>
       </c>
@@ -1332,10 +1365,10 @@
       <c r="I17" t="n">
         <v>929</v>
       </c>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="n">
-        <v>929</v>
-      </c>
+      <c r="J17" t="n">
+        <v>929</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="n">
         <v>929</v>
       </c>
@@ -1352,6 +1385,9 @@
         <v>929</v>
       </c>
       <c r="Q17" t="n">
+        <v>929</v>
+      </c>
+      <c r="R17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1361,11 +1397,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="n">
+        <v>499</v>
+      </c>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="n">
-        <v>499</v>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>499</v>
       </c>
@@ -1381,10 +1417,10 @@
       <c r="I18" t="n">
         <v>499</v>
       </c>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="n">
-        <v>499</v>
-      </c>
+      <c r="J18" t="n">
+        <v>499</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
       <c r="L18" t="n">
         <v>499</v>
       </c>
@@ -1401,6 +1437,9 @@
         <v>499</v>
       </c>
       <c r="Q18" t="n">
+        <v>499</v>
+      </c>
+      <c r="R18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1410,13 +1449,13 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="n">
+        <v>1497</v>
+      </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="n">
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="n">
         <v>465</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1497</v>
       </c>
       <c r="F19" t="n">
         <v>1497</v>
@@ -1452,6 +1491,9 @@
         <v>1497</v>
       </c>
       <c r="Q19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="R19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1485,10 +1527,10 @@
       <c r="I20" t="n">
         <v>929</v>
       </c>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="n">
-        <v>929</v>
-      </c>
+      <c r="J20" t="n">
+        <v>929</v>
+      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="n">
         <v>929</v>
       </c>
@@ -1505,6 +1547,9 @@
         <v>929</v>
       </c>
       <c r="Q20" t="n">
+        <v>929</v>
+      </c>
+      <c r="R20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1517,10 +1562,10 @@
       <c r="B21" t="n">
         <v>499</v>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
-        <v>499</v>
-      </c>
+      <c r="C21" t="n">
+        <v>499</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
         <v>499</v>
       </c>
@@ -1558,6 +1603,9 @@
         <v>499</v>
       </c>
       <c r="Q21" t="n">
+        <v>499</v>
+      </c>
+      <c r="R21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1567,13 +1615,11 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>299</v>
-      </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="n">
-        <v>299</v>
-      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>299</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
         <v>299</v>
       </c>
@@ -1589,10 +1635,10 @@
       <c r="I22" t="n">
         <v>299</v>
       </c>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="n">
-        <v>299</v>
-      </c>
+      <c r="J22" t="n">
+        <v>299</v>
+      </c>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="n">
         <v>299</v>
       </c>
@@ -1609,6 +1655,9 @@
         <v>299</v>
       </c>
       <c r="Q22" t="n">
+        <v>299</v>
+      </c>
+      <c r="R22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1618,11 +1667,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="n">
+        <v>1299</v>
+      </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>1299</v>
       </c>
@@ -1638,10 +1687,10 @@
       <c r="I23" t="n">
         <v>1299</v>
       </c>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="J23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="n">
         <v>1299</v>
       </c>
@@ -1658,6 +1707,9 @@
         <v>1299</v>
       </c>
       <c r="Q23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="R23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1668,9 +1720,7 @@
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="n">
-        <v>929</v>
-      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
         <v>929</v>
       </c>
@@ -1689,10 +1739,10 @@
       <c r="I24" t="n">
         <v>929</v>
       </c>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="n">
-        <v>929</v>
-      </c>
+      <c r="J24" t="n">
+        <v>929</v>
+      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="n">
         <v>929</v>
       </c>
@@ -1709,6 +1759,9 @@
         <v>929</v>
       </c>
       <c r="Q24" t="n">
+        <v>929</v>
+      </c>
+      <c r="R24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1719,9 +1772,7 @@
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="n">
-        <v>929</v>
-      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
         <v>929</v>
       </c>
@@ -1740,10 +1791,10 @@
       <c r="I25" t="n">
         <v>929</v>
       </c>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="n">
-        <v>929</v>
-      </c>
+      <c r="J25" t="n">
+        <v>929</v>
+      </c>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="n">
         <v>929</v>
       </c>
@@ -1760,6 +1811,9 @@
         <v>929</v>
       </c>
       <c r="Q25" t="n">
+        <v>929</v>
+      </c>
+      <c r="R25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1769,13 +1823,11 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
         <v>1299</v>
       </c>
@@ -1791,10 +1843,10 @@
       <c r="I26" t="n">
         <v>1299</v>
       </c>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="J26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="n">
         <v>1299</v>
       </c>
@@ -1811,6 +1863,9 @@
         <v>1299</v>
       </c>
       <c r="Q26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="R26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 20:44
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,7 @@
     <col width="21" customWidth="1" min="16" max="16"/>
     <col width="21" customWidth="1" min="17" max="17"/>
     <col width="21" customWidth="1" min="18" max="18"/>
+    <col width="21" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -461,85 +462,90 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 02:10</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -554,25 +560,25 @@
       <c r="B2" t="n">
         <v>929</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>929</v>
+      </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>929</v>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
         <v>929</v>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>929</v>
-      </c>
+      <c r="G2" t="n">
+        <v>929</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>929</v>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="n">
-        <v>929</v>
-      </c>
+      <c r="J2" t="n">
+        <v>929</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
         <v>929</v>
       </c>
@@ -592,6 +598,9 @@
         <v>929</v>
       </c>
       <c r="R2" t="n">
+        <v>929</v>
+      </c>
+      <c r="S2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -601,14 +610,14 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>569</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="n">
+        <v>569</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>569</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>569</v>
       </c>
@@ -624,10 +633,10 @@
       <c r="J3" t="n">
         <v>569</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
-        <v>569</v>
-      </c>
+      <c r="K3" t="n">
+        <v>569</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>569</v>
       </c>
@@ -644,6 +653,9 @@
         <v>569</v>
       </c>
       <c r="R3" t="n">
+        <v>569</v>
+      </c>
+      <c r="S3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -653,10 +665,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="n">
-        <v>299</v>
-      </c>
+      <c r="B4" t="n">
+        <v>299</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
         <v>299</v>
       </c>
@@ -678,10 +690,10 @@
       <c r="J4" t="n">
         <v>299</v>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="n">
-        <v>299</v>
-      </c>
+      <c r="K4" t="n">
+        <v>299</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>299</v>
       </c>
@@ -698,6 +710,9 @@
         <v>299</v>
       </c>
       <c r="R4" t="n">
+        <v>299</v>
+      </c>
+      <c r="S4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -734,10 +749,10 @@
       <c r="J5" t="n">
         <v>569</v>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
-        <v>569</v>
-      </c>
+      <c r="K5" t="n">
+        <v>569</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
         <v>569</v>
       </c>
@@ -754,6 +769,9 @@
         <v>569</v>
       </c>
       <c r="R5" t="n">
+        <v>569</v>
+      </c>
+      <c r="S5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -766,10 +784,10 @@
       <c r="B6" t="n">
         <v>499</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="n">
-        <v>499</v>
-      </c>
+      <c r="C6" t="n">
+        <v>499</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>499</v>
       </c>
@@ -788,10 +806,10 @@
       <c r="J6" t="n">
         <v>499</v>
       </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>499</v>
-      </c>
+      <c r="K6" t="n">
+        <v>499</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>499</v>
       </c>
@@ -808,6 +826,9 @@
         <v>499</v>
       </c>
       <c r="R6" t="n">
+        <v>499</v>
+      </c>
+      <c r="S6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -817,12 +838,12 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>569</v>
+      </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>569</v>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>569</v>
       </c>
@@ -838,10 +859,10 @@
       <c r="J7" t="n">
         <v>569</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="n">
-        <v>569</v>
-      </c>
+      <c r="K7" t="n">
+        <v>569</v>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
         <v>569</v>
       </c>
@@ -858,6 +879,9 @@
         <v>569</v>
       </c>
       <c r="R7" t="n">
+        <v>569</v>
+      </c>
+      <c r="S7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -867,14 +891,14 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>929</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="n">
+        <v>929</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>929</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>929</v>
       </c>
@@ -890,10 +914,10 @@
       <c r="J8" t="n">
         <v>929</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="n">
-        <v>929</v>
-      </c>
+      <c r="K8" t="n">
+        <v>929</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
         <v>929</v>
       </c>
@@ -910,6 +934,9 @@
         <v>929</v>
       </c>
       <c r="R8" t="n">
+        <v>929</v>
+      </c>
+      <c r="S8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -919,10 +946,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="n">
-        <v>299</v>
-      </c>
+      <c r="B9" t="n">
+        <v>299</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>299</v>
       </c>
@@ -944,10 +971,10 @@
       <c r="J9" t="n">
         <v>299</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="n">
-        <v>299</v>
-      </c>
+      <c r="K9" t="n">
+        <v>299</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
         <v>299</v>
       </c>
@@ -964,6 +991,9 @@
         <v>299</v>
       </c>
       <c r="R9" t="n">
+        <v>299</v>
+      </c>
+      <c r="S9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -973,14 +1003,14 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="n">
-        <v>299</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="n">
+        <v>299</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>299</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>299</v>
       </c>
@@ -996,10 +1026,10 @@
       <c r="J10" t="n">
         <v>299</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
-        <v>299</v>
-      </c>
+      <c r="K10" t="n">
+        <v>299</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
         <v>299</v>
       </c>
@@ -1016,6 +1046,9 @@
         <v>299</v>
       </c>
       <c r="R10" t="n">
+        <v>299</v>
+      </c>
+      <c r="S10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1028,10 +1061,10 @@
       <c r="B11" t="n">
         <v>2997</v>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
+      <c r="C11" t="n">
         <v>2997</v>
       </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
         <v>2997</v>
       </c>
@@ -1045,15 +1078,15 @@
         <v>2997</v>
       </c>
       <c r="I11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="J11" t="n">
         <v>929</v>
       </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="n">
-        <v>929</v>
-      </c>
+      <c r="K11" t="n">
+        <v>929</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
         <v>929</v>
       </c>
@@ -1070,6 +1103,9 @@
         <v>929</v>
       </c>
       <c r="R11" t="n">
+        <v>929</v>
+      </c>
+      <c r="S11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1085,10 +1121,10 @@
       <c r="C12" t="n">
         <v>569</v>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>569</v>
-      </c>
+      <c r="D12" t="n">
+        <v>569</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
         <v>569</v>
       </c>
@@ -1104,10 +1140,10 @@
       <c r="J12" t="n">
         <v>569</v>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="n">
-        <v>569</v>
-      </c>
+      <c r="K12" t="n">
+        <v>569</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
         <v>569</v>
       </c>
@@ -1124,6 +1160,9 @@
         <v>569</v>
       </c>
       <c r="R12" t="n">
+        <v>569</v>
+      </c>
+      <c r="S12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1133,14 +1172,14 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>569</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="n">
+        <v>569</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>569</v>
       </c>
@@ -1156,24 +1195,27 @@
       <c r="J13" t="n">
         <v>569</v>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="n">
-        <v>569</v>
-      </c>
+      <c r="K13" t="n">
+        <v>569</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
         <v>569</v>
       </c>
       <c r="N13" t="n">
         <v>569</v>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="n">
-        <v>569</v>
-      </c>
+      <c r="O13" t="n">
+        <v>569</v>
+      </c>
+      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="n">
         <v>569</v>
       </c>
       <c r="R13" t="n">
+        <v>569</v>
+      </c>
+      <c r="S13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1183,11 +1225,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>499</v>
+      </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="n">
-        <v>499</v>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>499</v>
       </c>
@@ -1228,6 +1270,9 @@
         <v>499</v>
       </c>
       <c r="R14" t="n">
+        <v>499</v>
+      </c>
+      <c r="S14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1243,10 +1288,10 @@
       <c r="C15" t="n">
         <v>499</v>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>499</v>
-      </c>
+      <c r="D15" t="n">
+        <v>499</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
         <v>499</v>
       </c>
@@ -1256,14 +1301,14 @@
       <c r="H15" t="n">
         <v>499</v>
       </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="n">
-        <v>499</v>
-      </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="n">
-        <v>499</v>
-      </c>
+      <c r="I15" t="n">
+        <v>499</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="n">
+        <v>499</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
         <v>499</v>
       </c>
@@ -1280,6 +1325,9 @@
         <v>499</v>
       </c>
       <c r="R15" t="n">
+        <v>499</v>
+      </c>
+      <c r="S15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1289,10 +1337,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="n">
+        <v>299</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
         <v>299</v>
       </c>
@@ -1314,10 +1362,10 @@
       <c r="J16" t="n">
         <v>299</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="n">
-        <v>299</v>
-      </c>
+      <c r="K16" t="n">
+        <v>299</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
         <v>299</v>
       </c>
@@ -1334,6 +1382,9 @@
         <v>299</v>
       </c>
       <c r="R16" t="n">
+        <v>299</v>
+      </c>
+      <c r="S16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1349,10 +1400,10 @@
       <c r="C17" t="n">
         <v>929</v>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
-        <v>929</v>
-      </c>
+      <c r="D17" t="n">
+        <v>929</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
         <v>929</v>
       </c>
@@ -1368,10 +1419,10 @@
       <c r="J17" t="n">
         <v>929</v>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="n">
-        <v>929</v>
-      </c>
+      <c r="K17" t="n">
+        <v>929</v>
+      </c>
+      <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
         <v>929</v>
       </c>
@@ -1388,6 +1439,9 @@
         <v>929</v>
       </c>
       <c r="R17" t="n">
+        <v>929</v>
+      </c>
+      <c r="S17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1400,11 +1454,11 @@
       <c r="B18" t="n">
         <v>499</v>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>499</v>
+      </c>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="n">
-        <v>499</v>
-      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
         <v>499</v>
       </c>
@@ -1420,10 +1474,10 @@
       <c r="J18" t="n">
         <v>499</v>
       </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="n">
-        <v>499</v>
-      </c>
+      <c r="K18" t="n">
+        <v>499</v>
+      </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
         <v>499</v>
       </c>
@@ -1440,6 +1494,9 @@
         <v>499</v>
       </c>
       <c r="R18" t="n">
+        <v>499</v>
+      </c>
+      <c r="S18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1452,13 +1509,13 @@
       <c r="B19" t="n">
         <v>1497</v>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>1497</v>
+      </c>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="n">
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="n">
         <v>465</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1497</v>
       </c>
       <c r="G19" t="n">
         <v>1497</v>
@@ -1494,6 +1551,9 @@
         <v>1497</v>
       </c>
       <c r="R19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="S19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1530,10 +1590,10 @@
       <c r="J20" t="n">
         <v>929</v>
       </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="n">
-        <v>929</v>
-      </c>
+      <c r="K20" t="n">
+        <v>929</v>
+      </c>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
         <v>929</v>
       </c>
@@ -1550,6 +1610,9 @@
         <v>929</v>
       </c>
       <c r="R20" t="n">
+        <v>929</v>
+      </c>
+      <c r="S20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1565,10 +1628,10 @@
       <c r="C21" t="n">
         <v>499</v>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>499</v>
-      </c>
+      <c r="D21" t="n">
+        <v>499</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
         <v>499</v>
       </c>
@@ -1606,6 +1669,9 @@
         <v>499</v>
       </c>
       <c r="R21" t="n">
+        <v>499</v>
+      </c>
+      <c r="S21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1615,14 +1681,14 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="n">
-        <v>299</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="n">
-        <v>299</v>
-      </c>
+      <c r="B22" t="n">
+        <v>299</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>299</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
         <v>299</v>
       </c>
@@ -1638,10 +1704,10 @@
       <c r="J22" t="n">
         <v>299</v>
       </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="n">
-        <v>299</v>
-      </c>
+      <c r="K22" t="n">
+        <v>299</v>
+      </c>
+      <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
         <v>299</v>
       </c>
@@ -1658,6 +1724,9 @@
         <v>299</v>
       </c>
       <c r="R22" t="n">
+        <v>299</v>
+      </c>
+      <c r="S22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1670,11 +1739,11 @@
       <c r="B23" t="n">
         <v>1299</v>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>1299</v>
+      </c>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
         <v>1299</v>
       </c>
@@ -1690,10 +1759,10 @@
       <c r="J23" t="n">
         <v>1299</v>
       </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="K23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
         <v>1299</v>
       </c>
@@ -1710,6 +1779,9 @@
         <v>1299</v>
       </c>
       <c r="R23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="S23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1719,11 +1791,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="n">
+        <v>929</v>
+      </c>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="n">
-        <v>929</v>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>929</v>
       </c>
@@ -1742,10 +1814,10 @@
       <c r="J24" t="n">
         <v>929</v>
       </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="n">
-        <v>929</v>
-      </c>
+      <c r="K24" t="n">
+        <v>929</v>
+      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
         <v>929</v>
       </c>
@@ -1762,6 +1834,9 @@
         <v>929</v>
       </c>
       <c r="R24" t="n">
+        <v>929</v>
+      </c>
+      <c r="S24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1771,11 +1846,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="n">
+        <v>929</v>
+      </c>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="n">
-        <v>929</v>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
         <v>929</v>
       </c>
@@ -1794,10 +1869,10 @@
       <c r="J25" t="n">
         <v>929</v>
       </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="n">
-        <v>929</v>
-      </c>
+      <c r="K25" t="n">
+        <v>929</v>
+      </c>
+      <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
         <v>929</v>
       </c>
@@ -1814,6 +1889,9 @@
         <v>929</v>
       </c>
       <c r="R25" t="n">
+        <v>929</v>
+      </c>
+      <c r="S25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1823,14 +1901,14 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
         <v>1299</v>
       </c>
@@ -1846,10 +1924,10 @@
       <c r="J26" t="n">
         <v>1299</v>
       </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="K26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
         <v>1299</v>
       </c>
@@ -1866,6 +1944,9 @@
         <v>1299</v>
       </c>
       <c r="R26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="S26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-21 22:44
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,7 @@
     <col width="21" customWidth="1" min="17" max="17"/>
     <col width="21" customWidth="1" min="18" max="18"/>
     <col width="21" customWidth="1" min="19" max="19"/>
+    <col width="21" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -462,90 +463,95 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 04:10</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -563,25 +569,25 @@
       <c r="C2" t="n">
         <v>929</v>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>929</v>
+      </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>929</v>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>929</v>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
-        <v>929</v>
-      </c>
+      <c r="H2" t="n">
+        <v>929</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
         <v>929</v>
       </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="n">
-        <v>929</v>
-      </c>
+      <c r="K2" t="n">
+        <v>929</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
         <v>929</v>
       </c>
@@ -601,6 +607,9 @@
         <v>929</v>
       </c>
       <c r="S2" t="n">
+        <v>929</v>
+      </c>
+      <c r="T2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -613,14 +622,14 @@
       <c r="B3" t="n">
         <v>569</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>569</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>569</v>
-      </c>
+      <c r="C3" t="n">
+        <v>569</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>569</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>569</v>
       </c>
@@ -636,10 +645,10 @@
       <c r="K3" t="n">
         <v>569</v>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>569</v>
-      </c>
+      <c r="L3" t="n">
+        <v>569</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>569</v>
       </c>
@@ -656,6 +665,9 @@
         <v>569</v>
       </c>
       <c r="S3" t="n">
+        <v>569</v>
+      </c>
+      <c r="T3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -668,10 +680,10 @@
       <c r="B4" t="n">
         <v>299</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="n">
-        <v>299</v>
-      </c>
+      <c r="C4" t="n">
+        <v>299</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>299</v>
       </c>
@@ -693,10 +705,10 @@
       <c r="K4" t="n">
         <v>299</v>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>299</v>
-      </c>
+      <c r="L4" t="n">
+        <v>299</v>
+      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
         <v>299</v>
       </c>
@@ -713,6 +725,9 @@
         <v>299</v>
       </c>
       <c r="S4" t="n">
+        <v>299</v>
+      </c>
+      <c r="T4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -752,10 +767,10 @@
       <c r="K5" t="n">
         <v>569</v>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
-        <v>569</v>
-      </c>
+      <c r="L5" t="n">
+        <v>569</v>
+      </c>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
         <v>569</v>
       </c>
@@ -772,6 +787,9 @@
         <v>569</v>
       </c>
       <c r="S5" t="n">
+        <v>569</v>
+      </c>
+      <c r="T5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -787,10 +805,10 @@
       <c r="C6" t="n">
         <v>499</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
-        <v>499</v>
-      </c>
+      <c r="D6" t="n">
+        <v>499</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>499</v>
       </c>
@@ -809,10 +827,10 @@
       <c r="K6" t="n">
         <v>499</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>499</v>
-      </c>
+      <c r="L6" t="n">
+        <v>499</v>
+      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
         <v>499</v>
       </c>
@@ -829,6 +847,9 @@
         <v>499</v>
       </c>
       <c r="S6" t="n">
+        <v>499</v>
+      </c>
+      <c r="T6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -841,12 +862,12 @@
       <c r="B7" t="n">
         <v>569</v>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>569</v>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>569</v>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>569</v>
       </c>
@@ -862,10 +883,10 @@
       <c r="K7" t="n">
         <v>569</v>
       </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="n">
-        <v>569</v>
-      </c>
+      <c r="L7" t="n">
+        <v>569</v>
+      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
         <v>569</v>
       </c>
@@ -882,6 +903,9 @@
         <v>569</v>
       </c>
       <c r="S7" t="n">
+        <v>569</v>
+      </c>
+      <c r="T7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -894,14 +918,14 @@
       <c r="B8" t="n">
         <v>929</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
-        <v>929</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>929</v>
-      </c>
+      <c r="C8" t="n">
+        <v>929</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>929</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>929</v>
       </c>
@@ -917,10 +941,10 @@
       <c r="K8" t="n">
         <v>929</v>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
-        <v>929</v>
-      </c>
+      <c r="L8" t="n">
+        <v>929</v>
+      </c>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
         <v>929</v>
       </c>
@@ -937,6 +961,9 @@
         <v>929</v>
       </c>
       <c r="S8" t="n">
+        <v>929</v>
+      </c>
+      <c r="T8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -949,10 +976,10 @@
       <c r="B9" t="n">
         <v>299</v>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
-        <v>299</v>
-      </c>
+      <c r="C9" t="n">
+        <v>299</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
         <v>299</v>
       </c>
@@ -974,10 +1001,10 @@
       <c r="K9" t="n">
         <v>299</v>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="n">
-        <v>299</v>
-      </c>
+      <c r="L9" t="n">
+        <v>299</v>
+      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
         <v>299</v>
       </c>
@@ -994,6 +1021,9 @@
         <v>299</v>
       </c>
       <c r="S9" t="n">
+        <v>299</v>
+      </c>
+      <c r="T9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1006,14 +1036,14 @@
       <c r="B10" t="n">
         <v>299</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>299</v>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>299</v>
-      </c>
+      <c r="C10" t="n">
+        <v>299</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>299</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>299</v>
       </c>
@@ -1029,10 +1059,10 @@
       <c r="K10" t="n">
         <v>299</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
-        <v>299</v>
-      </c>
+      <c r="L10" t="n">
+        <v>299</v>
+      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
         <v>299</v>
       </c>
@@ -1049,6 +1079,9 @@
         <v>299</v>
       </c>
       <c r="S10" t="n">
+        <v>299</v>
+      </c>
+      <c r="T10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1064,10 +1097,10 @@
       <c r="C11" t="n">
         <v>2997</v>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
+      <c r="D11" t="n">
         <v>2997</v>
       </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>2997</v>
       </c>
@@ -1081,15 +1114,15 @@
         <v>2997</v>
       </c>
       <c r="J11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="K11" t="n">
         <v>929</v>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="n">
-        <v>929</v>
-      </c>
+      <c r="L11" t="n">
+        <v>929</v>
+      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
         <v>929</v>
       </c>
@@ -1106,6 +1139,9 @@
         <v>929</v>
       </c>
       <c r="S11" t="n">
+        <v>929</v>
+      </c>
+      <c r="T11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1124,10 +1160,10 @@
       <c r="D12" t="n">
         <v>569</v>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>569</v>
-      </c>
+      <c r="E12" t="n">
+        <v>569</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>569</v>
       </c>
@@ -1143,10 +1179,10 @@
       <c r="K12" t="n">
         <v>569</v>
       </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="n">
-        <v>569</v>
-      </c>
+      <c r="L12" t="n">
+        <v>569</v>
+      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
         <v>569</v>
       </c>
@@ -1163,6 +1199,9 @@
         <v>569</v>
       </c>
       <c r="S12" t="n">
+        <v>569</v>
+      </c>
+      <c r="T12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1175,14 +1214,14 @@
       <c r="B13" t="n">
         <v>569</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>569</v>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>569</v>
-      </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>569</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>569</v>
       </c>
@@ -1198,24 +1237,27 @@
       <c r="K13" t="n">
         <v>569</v>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>569</v>
-      </c>
+      <c r="L13" t="n">
+        <v>569</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
         <v>569</v>
       </c>
       <c r="O13" t="n">
         <v>569</v>
       </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="n">
-        <v>569</v>
-      </c>
+      <c r="P13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
         <v>569</v>
       </c>
       <c r="S13" t="n">
+        <v>569</v>
+      </c>
+      <c r="T13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1228,11 +1270,11 @@
       <c r="B14" t="n">
         <v>499</v>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>499</v>
+      </c>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>499</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
         <v>499</v>
       </c>
@@ -1273,6 +1315,9 @@
         <v>499</v>
       </c>
       <c r="S14" t="n">
+        <v>499</v>
+      </c>
+      <c r="T14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1291,10 +1336,10 @@
       <c r="D15" t="n">
         <v>499</v>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>499</v>
-      </c>
+      <c r="E15" t="n">
+        <v>499</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
         <v>499</v>
       </c>
@@ -1304,14 +1349,14 @@
       <c r="I15" t="n">
         <v>499</v>
       </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="n">
-        <v>499</v>
-      </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="n">
-        <v>499</v>
-      </c>
+      <c r="J15" t="n">
+        <v>499</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="n">
+        <v>499</v>
+      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
         <v>499</v>
       </c>
@@ -1328,6 +1373,9 @@
         <v>499</v>
       </c>
       <c r="S15" t="n">
+        <v>499</v>
+      </c>
+      <c r="T15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1340,10 +1388,10 @@
       <c r="B16" t="n">
         <v>299</v>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
-        <v>299</v>
-      </c>
+      <c r="C16" t="n">
+        <v>299</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
         <v>299</v>
       </c>
@@ -1365,10 +1413,10 @@
       <c r="K16" t="n">
         <v>299</v>
       </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="n">
-        <v>299</v>
-      </c>
+      <c r="L16" t="n">
+        <v>299</v>
+      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
         <v>299</v>
       </c>
@@ -1385,6 +1433,9 @@
         <v>299</v>
       </c>
       <c r="S16" t="n">
+        <v>299</v>
+      </c>
+      <c r="T16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1403,10 +1454,10 @@
       <c r="D17" t="n">
         <v>929</v>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>929</v>
-      </c>
+      <c r="E17" t="n">
+        <v>929</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
         <v>929</v>
       </c>
@@ -1422,10 +1473,10 @@
       <c r="K17" t="n">
         <v>929</v>
       </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="n">
-        <v>929</v>
-      </c>
+      <c r="L17" t="n">
+        <v>929</v>
+      </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
         <v>929</v>
       </c>
@@ -1442,6 +1493,9 @@
         <v>929</v>
       </c>
       <c r="S17" t="n">
+        <v>929</v>
+      </c>
+      <c r="T17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1457,11 +1511,11 @@
       <c r="C18" t="n">
         <v>499</v>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>499</v>
+      </c>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
-        <v>499</v>
-      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
         <v>499</v>
       </c>
@@ -1477,10 +1531,10 @@
       <c r="K18" t="n">
         <v>499</v>
       </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="n">
-        <v>499</v>
-      </c>
+      <c r="L18" t="n">
+        <v>499</v>
+      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
         <v>499</v>
       </c>
@@ -1497,6 +1551,9 @@
         <v>499</v>
       </c>
       <c r="S18" t="n">
+        <v>499</v>
+      </c>
+      <c r="T18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1512,13 +1569,13 @@
       <c r="C19" t="n">
         <v>1497</v>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>1497</v>
+      </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
         <v>465</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1497</v>
       </c>
       <c r="H19" t="n">
         <v>1497</v>
@@ -1554,6 +1611,9 @@
         <v>1497</v>
       </c>
       <c r="S19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="T19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1593,10 +1653,10 @@
       <c r="K20" t="n">
         <v>929</v>
       </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="n">
-        <v>929</v>
-      </c>
+      <c r="L20" t="n">
+        <v>929</v>
+      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="n">
         <v>929</v>
       </c>
@@ -1613,6 +1673,9 @@
         <v>929</v>
       </c>
       <c r="S20" t="n">
+        <v>929</v>
+      </c>
+      <c r="T20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1631,10 +1694,10 @@
       <c r="D21" t="n">
         <v>499</v>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>499</v>
-      </c>
+      <c r="E21" t="n">
+        <v>499</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
         <v>499</v>
       </c>
@@ -1672,6 +1735,9 @@
         <v>499</v>
       </c>
       <c r="S21" t="n">
+        <v>499</v>
+      </c>
+      <c r="T21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1684,14 +1750,14 @@
       <c r="B22" t="n">
         <v>299</v>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="n">
-        <v>299</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>299</v>
-      </c>
+      <c r="C22" t="n">
+        <v>299</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>299</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
         <v>299</v>
       </c>
@@ -1707,10 +1773,10 @@
       <c r="K22" t="n">
         <v>299</v>
       </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="n">
-        <v>299</v>
-      </c>
+      <c r="L22" t="n">
+        <v>299</v>
+      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
         <v>299</v>
       </c>
@@ -1727,6 +1793,9 @@
         <v>299</v>
       </c>
       <c r="S22" t="n">
+        <v>299</v>
+      </c>
+      <c r="T22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1742,11 +1811,11 @@
       <c r="C23" t="n">
         <v>1299</v>
       </c>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>1299</v>
+      </c>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
         <v>1299</v>
       </c>
@@ -1762,10 +1831,10 @@
       <c r="K23" t="n">
         <v>1299</v>
       </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="L23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="M23" t="inlineStr"/>
       <c r="N23" t="n">
         <v>1299</v>
       </c>
@@ -1782,6 +1851,9 @@
         <v>1299</v>
       </c>
       <c r="S23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="T23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1794,11 +1866,11 @@
       <c r="B24" t="n">
         <v>929</v>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>929</v>
+      </c>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="n">
-        <v>929</v>
-      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
         <v>929</v>
       </c>
@@ -1817,10 +1889,10 @@
       <c r="K24" t="n">
         <v>929</v>
       </c>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="n">
-        <v>929</v>
-      </c>
+      <c r="L24" t="n">
+        <v>929</v>
+      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
         <v>929</v>
       </c>
@@ -1837,6 +1909,9 @@
         <v>929</v>
       </c>
       <c r="S24" t="n">
+        <v>929</v>
+      </c>
+      <c r="T24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1849,11 +1924,11 @@
       <c r="B25" t="n">
         <v>929</v>
       </c>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>929</v>
+      </c>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="n">
-        <v>929</v>
-      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
         <v>929</v>
       </c>
@@ -1872,10 +1947,10 @@
       <c r="K25" t="n">
         <v>929</v>
       </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="n">
-        <v>929</v>
-      </c>
+      <c r="L25" t="n">
+        <v>929</v>
+      </c>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
         <v>929</v>
       </c>
@@ -1892,6 +1967,9 @@
         <v>929</v>
       </c>
       <c r="S25" t="n">
+        <v>929</v>
+      </c>
+      <c r="T25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1904,14 +1982,14 @@
       <c r="B26" t="n">
         <v>1299</v>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
         <v>1299</v>
       </c>
@@ -1927,10 +2005,10 @@
       <c r="K26" t="n">
         <v>1299</v>
       </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="L26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="M26" t="inlineStr"/>
       <c r="N26" t="n">
         <v>1299</v>
       </c>
@@ -1947,6 +2025,9 @@
         <v>1299</v>
       </c>
       <c r="S26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="T26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 04:05
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,7 @@
     <col width="21" customWidth="1" min="18" max="18"/>
     <col width="21" customWidth="1" min="19" max="19"/>
     <col width="21" customWidth="1" min="20" max="20"/>
+    <col width="21" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,95 +464,100 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 09:32</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -572,25 +578,25 @@
       <c r="D2" t="n">
         <v>929</v>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>929</v>
+      </c>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>929</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>929</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
-        <v>929</v>
-      </c>
+      <c r="I2" t="n">
+        <v>929</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
         <v>929</v>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>929</v>
-      </c>
+      <c r="L2" t="n">
+        <v>929</v>
+      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
         <v>929</v>
       </c>
@@ -610,6 +616,9 @@
         <v>929</v>
       </c>
       <c r="T2" t="n">
+        <v>929</v>
+      </c>
+      <c r="U2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -625,14 +634,14 @@
       <c r="C3" t="n">
         <v>569</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>569</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>569</v>
-      </c>
+      <c r="D3" t="n">
+        <v>569</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>569</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>569</v>
       </c>
@@ -648,10 +657,10 @@
       <c r="L3" t="n">
         <v>569</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="n">
-        <v>569</v>
-      </c>
+      <c r="M3" t="n">
+        <v>569</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="n">
         <v>569</v>
       </c>
@@ -668,6 +677,9 @@
         <v>569</v>
       </c>
       <c r="T3" t="n">
+        <v>569</v>
+      </c>
+      <c r="U3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -683,10 +695,10 @@
       <c r="C4" t="n">
         <v>299</v>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
-        <v>299</v>
-      </c>
+      <c r="D4" t="n">
+        <v>299</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
         <v>299</v>
       </c>
@@ -708,10 +720,10 @@
       <c r="L4" t="n">
         <v>299</v>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="n">
-        <v>299</v>
-      </c>
+      <c r="M4" t="n">
+        <v>299</v>
+      </c>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
         <v>299</v>
       </c>
@@ -728,6 +740,9 @@
         <v>299</v>
       </c>
       <c r="T4" t="n">
+        <v>299</v>
+      </c>
+      <c r="U4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -770,10 +785,10 @@
       <c r="L5" t="n">
         <v>569</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="n">
-        <v>569</v>
-      </c>
+      <c r="M5" t="n">
+        <v>569</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
         <v>569</v>
       </c>
@@ -790,6 +805,9 @@
         <v>569</v>
       </c>
       <c r="T5" t="n">
+        <v>569</v>
+      </c>
+      <c r="U5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -808,10 +826,10 @@
       <c r="D6" t="n">
         <v>499</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>499</v>
-      </c>
+      <c r="E6" t="n">
+        <v>499</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
         <v>499</v>
       </c>
@@ -830,10 +848,10 @@
       <c r="L6" t="n">
         <v>499</v>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="n">
-        <v>499</v>
-      </c>
+      <c r="M6" t="n">
+        <v>499</v>
+      </c>
+      <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
         <v>499</v>
       </c>
@@ -850,6 +868,9 @@
         <v>499</v>
       </c>
       <c r="T6" t="n">
+        <v>499</v>
+      </c>
+      <c r="U6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -865,12 +886,12 @@
       <c r="C7" t="n">
         <v>569</v>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>569</v>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>569</v>
-      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>569</v>
       </c>
@@ -886,10 +907,10 @@
       <c r="L7" t="n">
         <v>569</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
-        <v>569</v>
-      </c>
+      <c r="M7" t="n">
+        <v>569</v>
+      </c>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
         <v>569</v>
       </c>
@@ -906,6 +927,9 @@
         <v>569</v>
       </c>
       <c r="T7" t="n">
+        <v>569</v>
+      </c>
+      <c r="U7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -921,14 +945,14 @@
       <c r="C8" t="n">
         <v>929</v>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>929</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>929</v>
-      </c>
+      <c r="D8" t="n">
+        <v>929</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>929</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
         <v>929</v>
       </c>
@@ -944,10 +968,10 @@
       <c r="L8" t="n">
         <v>929</v>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="n">
-        <v>929</v>
-      </c>
+      <c r="M8" t="n">
+        <v>929</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
         <v>929</v>
       </c>
@@ -964,6 +988,9 @@
         <v>929</v>
       </c>
       <c r="T8" t="n">
+        <v>929</v>
+      </c>
+      <c r="U8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -979,10 +1006,10 @@
       <c r="C9" t="n">
         <v>299</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>299</v>
-      </c>
+      <c r="D9" t="n">
+        <v>299</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>299</v>
       </c>
@@ -1004,10 +1031,10 @@
       <c r="L9" t="n">
         <v>299</v>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="n">
-        <v>299</v>
-      </c>
+      <c r="M9" t="n">
+        <v>299</v>
+      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
         <v>299</v>
       </c>
@@ -1024,6 +1051,9 @@
         <v>299</v>
       </c>
       <c r="T9" t="n">
+        <v>299</v>
+      </c>
+      <c r="U9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1039,14 +1069,14 @@
       <c r="C10" t="n">
         <v>299</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>299</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>299</v>
-      </c>
+      <c r="D10" t="n">
+        <v>299</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>299</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>299</v>
       </c>
@@ -1062,10 +1092,10 @@
       <c r="L10" t="n">
         <v>299</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="n">
-        <v>299</v>
-      </c>
+      <c r="M10" t="n">
+        <v>299</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
         <v>299</v>
       </c>
@@ -1082,6 +1112,9 @@
         <v>299</v>
       </c>
       <c r="T10" t="n">
+        <v>299</v>
+      </c>
+      <c r="U10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1100,10 +1133,10 @@
       <c r="D11" t="n">
         <v>2997</v>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
+      <c r="E11" t="n">
         <v>2997</v>
       </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>2997</v>
       </c>
@@ -1117,15 +1150,15 @@
         <v>2997</v>
       </c>
       <c r="K11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="L11" t="n">
         <v>929</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="n">
-        <v>929</v>
-      </c>
+      <c r="M11" t="n">
+        <v>929</v>
+      </c>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
         <v>929</v>
       </c>
@@ -1142,6 +1175,9 @@
         <v>929</v>
       </c>
       <c r="T11" t="n">
+        <v>929</v>
+      </c>
+      <c r="U11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1163,10 +1199,10 @@
       <c r="E12" t="n">
         <v>569</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="n">
-        <v>569</v>
-      </c>
+      <c r="F12" t="n">
+        <v>569</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
         <v>569</v>
       </c>
@@ -1182,10 +1218,10 @@
       <c r="L12" t="n">
         <v>569</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="n">
-        <v>569</v>
-      </c>
+      <c r="M12" t="n">
+        <v>569</v>
+      </c>
+      <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
         <v>569</v>
       </c>
@@ -1202,6 +1238,9 @@
         <v>569</v>
       </c>
       <c r="T12" t="n">
+        <v>569</v>
+      </c>
+      <c r="U12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1217,14 +1256,14 @@
       <c r="C13" t="n">
         <v>569</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>569</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>569</v>
-      </c>
+      <c r="D13" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>569</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>569</v>
       </c>
@@ -1240,24 +1279,27 @@
       <c r="L13" t="n">
         <v>569</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="n">
-        <v>569</v>
-      </c>
+      <c r="M13" t="n">
+        <v>569</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
         <v>569</v>
       </c>
       <c r="P13" t="n">
         <v>569</v>
       </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q13" t="n">
+        <v>569</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
       <c r="S13" t="n">
         <v>569</v>
       </c>
       <c r="T13" t="n">
+        <v>569</v>
+      </c>
+      <c r="U13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1273,11 +1315,11 @@
       <c r="C14" t="n">
         <v>499</v>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>499</v>
+      </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
-        <v>499</v>
-      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>499</v>
       </c>
@@ -1318,6 +1360,9 @@
         <v>499</v>
       </c>
       <c r="T14" t="n">
+        <v>499</v>
+      </c>
+      <c r="U14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1339,10 +1384,10 @@
       <c r="E15" t="n">
         <v>499</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>499</v>
-      </c>
+      <c r="F15" t="n">
+        <v>499</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
         <v>499</v>
       </c>
@@ -1352,14 +1397,14 @@
       <c r="J15" t="n">
         <v>499</v>
       </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="n">
-        <v>499</v>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="n">
-        <v>499</v>
-      </c>
+      <c r="K15" t="n">
+        <v>499</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>499</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
         <v>499</v>
       </c>
@@ -1376,6 +1421,9 @@
         <v>499</v>
       </c>
       <c r="T15" t="n">
+        <v>499</v>
+      </c>
+      <c r="U15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1385,16 +1433,14 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
         <v>299</v>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>299</v>
-      </c>
+      <c r="D16" t="n">
+        <v>299</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
         <v>299</v>
       </c>
@@ -1416,10 +1462,10 @@
       <c r="L16" t="n">
         <v>299</v>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="n">
-        <v>299</v>
-      </c>
+      <c r="M16" t="n">
+        <v>299</v>
+      </c>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
         <v>299</v>
       </c>
@@ -1436,6 +1482,9 @@
         <v>299</v>
       </c>
       <c r="T16" t="n">
+        <v>299</v>
+      </c>
+      <c r="U16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1457,10 +1506,10 @@
       <c r="E17" t="n">
         <v>929</v>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="n">
-        <v>929</v>
-      </c>
+      <c r="F17" t="n">
+        <v>929</v>
+      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
         <v>929</v>
       </c>
@@ -1476,10 +1525,10 @@
       <c r="L17" t="n">
         <v>929</v>
       </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="n">
-        <v>929</v>
-      </c>
+      <c r="M17" t="n">
+        <v>929</v>
+      </c>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
         <v>929</v>
       </c>
@@ -1496,6 +1545,9 @@
         <v>929</v>
       </c>
       <c r="T17" t="n">
+        <v>929</v>
+      </c>
+      <c r="U17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1514,11 +1566,11 @@
       <c r="D18" t="n">
         <v>499</v>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>499</v>
+      </c>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="n">
-        <v>499</v>
-      </c>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
         <v>499</v>
       </c>
@@ -1534,10 +1586,10 @@
       <c r="L18" t="n">
         <v>499</v>
       </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="n">
-        <v>499</v>
-      </c>
+      <c r="M18" t="n">
+        <v>499</v>
+      </c>
+      <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
         <v>499</v>
       </c>
@@ -1554,6 +1606,9 @@
         <v>499</v>
       </c>
       <c r="T18" t="n">
+        <v>499</v>
+      </c>
+      <c r="U18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1564,7 +1619,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="C19" t="n">
         <v>1497</v>
@@ -1572,13 +1627,13 @@
       <c r="D19" t="n">
         <v>1497</v>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>1497</v>
+      </c>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="n">
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="n">
         <v>465</v>
-      </c>
-      <c r="H19" t="n">
-        <v>1497</v>
       </c>
       <c r="I19" t="n">
         <v>1497</v>
@@ -1614,6 +1669,9 @@
         <v>1497</v>
       </c>
       <c r="T19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="U19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1656,10 +1714,10 @@
       <c r="L20" t="n">
         <v>929</v>
       </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="n">
-        <v>929</v>
-      </c>
+      <c r="M20" t="n">
+        <v>929</v>
+      </c>
+      <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
         <v>929</v>
       </c>
@@ -1676,6 +1734,9 @@
         <v>929</v>
       </c>
       <c r="T20" t="n">
+        <v>929</v>
+      </c>
+      <c r="U20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1697,10 +1758,10 @@
       <c r="E21" t="n">
         <v>499</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="n">
-        <v>499</v>
-      </c>
+      <c r="F21" t="n">
+        <v>499</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
         <v>499</v>
       </c>
@@ -1738,6 +1799,9 @@
         <v>499</v>
       </c>
       <c r="T21" t="n">
+        <v>499</v>
+      </c>
+      <c r="U21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1753,14 +1817,14 @@
       <c r="C22" t="n">
         <v>299</v>
       </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="n">
-        <v>299</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="n">
-        <v>299</v>
-      </c>
+      <c r="D22" t="n">
+        <v>299</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>299</v>
+      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
         <v>299</v>
       </c>
@@ -1776,10 +1840,10 @@
       <c r="L22" t="n">
         <v>299</v>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="n">
-        <v>299</v>
-      </c>
+      <c r="M22" t="n">
+        <v>299</v>
+      </c>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
         <v>299</v>
       </c>
@@ -1796,6 +1860,9 @@
         <v>299</v>
       </c>
       <c r="T22" t="n">
+        <v>299</v>
+      </c>
+      <c r="U22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1814,11 +1881,11 @@
       <c r="D23" t="n">
         <v>1299</v>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>1299</v>
+      </c>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
         <v>1299</v>
       </c>
@@ -1834,10 +1901,10 @@
       <c r="L23" t="n">
         <v>1299</v>
       </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="M23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
         <v>1299</v>
       </c>
@@ -1854,6 +1921,9 @@
         <v>1299</v>
       </c>
       <c r="T23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="U23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1869,11 +1939,11 @@
       <c r="C24" t="n">
         <v>929</v>
       </c>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>929</v>
+      </c>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>929</v>
-      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
         <v>929</v>
       </c>
@@ -1892,10 +1962,10 @@
       <c r="L24" t="n">
         <v>929</v>
       </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="n">
-        <v>929</v>
-      </c>
+      <c r="M24" t="n">
+        <v>929</v>
+      </c>
+      <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
         <v>929</v>
       </c>
@@ -1912,6 +1982,9 @@
         <v>929</v>
       </c>
       <c r="T24" t="n">
+        <v>929</v>
+      </c>
+      <c r="U24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1927,11 +2000,11 @@
       <c r="C25" t="n">
         <v>929</v>
       </c>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>929</v>
+      </c>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>929</v>
-      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>929</v>
       </c>
@@ -1950,10 +2023,10 @@
       <c r="L25" t="n">
         <v>929</v>
       </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="n">
-        <v>929</v>
-      </c>
+      <c r="M25" t="n">
+        <v>929</v>
+      </c>
+      <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
         <v>929</v>
       </c>
@@ -1970,6 +2043,9 @@
         <v>929</v>
       </c>
       <c r="T25" t="n">
+        <v>929</v>
+      </c>
+      <c r="U25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1985,14 +2061,14 @@
       <c r="C26" t="n">
         <v>1299</v>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
         <v>1299</v>
       </c>
@@ -2008,10 +2084,10 @@
       <c r="L26" t="n">
         <v>1299</v>
       </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="M26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
         <v>1299</v>
       </c>
@@ -2028,6 +2104,9 @@
         <v>1299</v>
       </c>
       <c r="T26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="U26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 05:06
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,7 @@
     <col width="21" customWidth="1" min="19" max="19"/>
     <col width="21" customWidth="1" min="20" max="20"/>
     <col width="21" customWidth="1" min="21" max="21"/>
+    <col width="21" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -464,100 +465,105 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 10:32</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -581,25 +587,25 @@
       <c r="E2" t="n">
         <v>929</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>929</v>
+      </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>929</v>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>929</v>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="n">
-        <v>929</v>
-      </c>
+      <c r="J2" t="n">
+        <v>929</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
         <v>929</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="n">
-        <v>929</v>
-      </c>
+      <c r="M2" t="n">
+        <v>929</v>
+      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
         <v>929</v>
       </c>
@@ -619,6 +625,9 @@
         <v>929</v>
       </c>
       <c r="U2" t="n">
+        <v>929</v>
+      </c>
+      <c r="V2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -628,23 +637,21 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>569</v>
       </c>
       <c r="D3" t="n">
         <v>569</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>569</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>569</v>
-      </c>
+      <c r="E3" t="n">
+        <v>569</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>569</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>569</v>
       </c>
@@ -660,10 +667,10 @@
       <c r="M3" t="n">
         <v>569</v>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
-        <v>569</v>
-      </c>
+      <c r="N3" t="n">
+        <v>569</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
         <v>569</v>
       </c>
@@ -680,6 +687,9 @@
         <v>569</v>
       </c>
       <c r="U3" t="n">
+        <v>569</v>
+      </c>
+      <c r="V3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -698,10 +708,10 @@
       <c r="D4" t="n">
         <v>299</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>299</v>
-      </c>
+      <c r="E4" t="n">
+        <v>299</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>299</v>
       </c>
@@ -723,10 +733,10 @@
       <c r="M4" t="n">
         <v>299</v>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="n">
-        <v>299</v>
-      </c>
+      <c r="N4" t="n">
+        <v>299</v>
+      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
         <v>299</v>
       </c>
@@ -743,6 +753,9 @@
         <v>299</v>
       </c>
       <c r="U4" t="n">
+        <v>299</v>
+      </c>
+      <c r="V4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -788,10 +801,10 @@
       <c r="M5" t="n">
         <v>569</v>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="n">
-        <v>569</v>
-      </c>
+      <c r="N5" t="n">
+        <v>569</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
         <v>569</v>
       </c>
@@ -808,6 +821,9 @@
         <v>569</v>
       </c>
       <c r="U5" t="n">
+        <v>569</v>
+      </c>
+      <c r="V5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -829,10 +845,10 @@
       <c r="E6" t="n">
         <v>499</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>499</v>
-      </c>
+      <c r="F6" t="n">
+        <v>499</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>499</v>
       </c>
@@ -851,10 +867,10 @@
       <c r="M6" t="n">
         <v>499</v>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="n">
-        <v>499</v>
-      </c>
+      <c r="N6" t="n">
+        <v>499</v>
+      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
         <v>499</v>
       </c>
@@ -871,6 +887,9 @@
         <v>499</v>
       </c>
       <c r="U6" t="n">
+        <v>499</v>
+      </c>
+      <c r="V6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -889,12 +908,12 @@
       <c r="D7" t="n">
         <v>569</v>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>569</v>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>569</v>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
         <v>569</v>
       </c>
@@ -910,10 +929,10 @@
       <c r="M7" t="n">
         <v>569</v>
       </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="n">
-        <v>569</v>
-      </c>
+      <c r="N7" t="n">
+        <v>569</v>
+      </c>
+      <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
         <v>569</v>
       </c>
@@ -930,6 +949,9 @@
         <v>569</v>
       </c>
       <c r="U7" t="n">
+        <v>569</v>
+      </c>
+      <c r="V7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -948,14 +970,14 @@
       <c r="D8" t="n">
         <v>929</v>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>929</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>929</v>
-      </c>
+      <c r="E8" t="n">
+        <v>929</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>929</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>929</v>
       </c>
@@ -971,10 +993,10 @@
       <c r="M8" t="n">
         <v>929</v>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="n">
-        <v>929</v>
-      </c>
+      <c r="N8" t="n">
+        <v>929</v>
+      </c>
+      <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
         <v>929</v>
       </c>
@@ -991,6 +1013,9 @@
         <v>929</v>
       </c>
       <c r="U8" t="n">
+        <v>929</v>
+      </c>
+      <c r="V8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1009,10 +1034,10 @@
       <c r="D9" t="n">
         <v>299</v>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>299</v>
-      </c>
+      <c r="E9" t="n">
+        <v>299</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>299</v>
       </c>
@@ -1034,10 +1059,10 @@
       <c r="M9" t="n">
         <v>299</v>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="n">
-        <v>299</v>
-      </c>
+      <c r="N9" t="n">
+        <v>299</v>
+      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
         <v>299</v>
       </c>
@@ -1054,6 +1079,9 @@
         <v>299</v>
       </c>
       <c r="U9" t="n">
+        <v>299</v>
+      </c>
+      <c r="V9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1072,14 +1100,14 @@
       <c r="D10" t="n">
         <v>299</v>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>299</v>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>299</v>
-      </c>
+      <c r="E10" t="n">
+        <v>299</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>299</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>299</v>
       </c>
@@ -1095,10 +1123,10 @@
       <c r="M10" t="n">
         <v>299</v>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="n">
-        <v>299</v>
-      </c>
+      <c r="N10" t="n">
+        <v>299</v>
+      </c>
+      <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
         <v>299</v>
       </c>
@@ -1115,6 +1143,9 @@
         <v>299</v>
       </c>
       <c r="U10" t="n">
+        <v>299</v>
+      </c>
+      <c r="V10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1136,10 +1167,10 @@
       <c r="E11" t="n">
         <v>2997</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="n">
+      <c r="F11" t="n">
         <v>2997</v>
       </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
         <v>2997</v>
       </c>
@@ -1153,15 +1184,15 @@
         <v>2997</v>
       </c>
       <c r="L11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="M11" t="n">
         <v>929</v>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="n">
-        <v>929</v>
-      </c>
+      <c r="N11" t="n">
+        <v>929</v>
+      </c>
+      <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
         <v>929</v>
       </c>
@@ -1178,6 +1209,9 @@
         <v>929</v>
       </c>
       <c r="U11" t="n">
+        <v>929</v>
+      </c>
+      <c r="V11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1202,10 +1236,10 @@
       <c r="F12" t="n">
         <v>569</v>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="n">
-        <v>569</v>
-      </c>
+      <c r="G12" t="n">
+        <v>569</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
         <v>569</v>
       </c>
@@ -1221,10 +1255,10 @@
       <c r="M12" t="n">
         <v>569</v>
       </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="n">
-        <v>569</v>
-      </c>
+      <c r="N12" t="n">
+        <v>569</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
         <v>569</v>
       </c>
@@ -1241,6 +1275,9 @@
         <v>569</v>
       </c>
       <c r="U12" t="n">
+        <v>569</v>
+      </c>
+      <c r="V12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1259,14 +1296,14 @@
       <c r="D13" t="n">
         <v>569</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>569</v>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>569</v>
-      </c>
+      <c r="E13" t="n">
+        <v>569</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>569</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>569</v>
       </c>
@@ -1282,24 +1319,27 @@
       <c r="M13" t="n">
         <v>569</v>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="n">
-        <v>569</v>
-      </c>
+      <c r="N13" t="n">
+        <v>569</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
         <v>569</v>
       </c>
       <c r="Q13" t="n">
         <v>569</v>
       </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="n">
-        <v>569</v>
-      </c>
+      <c r="R13" t="n">
+        <v>569</v>
+      </c>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
         <v>569</v>
       </c>
       <c r="U13" t="n">
+        <v>569</v>
+      </c>
+      <c r="V13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1318,11 +1358,11 @@
       <c r="D14" t="n">
         <v>499</v>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>499</v>
+      </c>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
-        <v>499</v>
-      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
         <v>499</v>
       </c>
@@ -1363,6 +1403,9 @@
         <v>499</v>
       </c>
       <c r="U14" t="n">
+        <v>499</v>
+      </c>
+      <c r="V14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1387,10 +1430,10 @@
       <c r="F15" t="n">
         <v>499</v>
       </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="n">
-        <v>499</v>
-      </c>
+      <c r="G15" t="n">
+        <v>499</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
         <v>499</v>
       </c>
@@ -1400,14 +1443,14 @@
       <c r="K15" t="n">
         <v>499</v>
       </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="n">
-        <v>499</v>
-      </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="n">
-        <v>499</v>
-      </c>
+      <c r="L15" t="n">
+        <v>499</v>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="n">
+        <v>499</v>
+      </c>
+      <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
         <v>499</v>
       </c>
@@ -1424,6 +1467,9 @@
         <v>499</v>
       </c>
       <c r="U15" t="n">
+        <v>499</v>
+      </c>
+      <c r="V15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1433,17 +1479,17 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="n">
+        <v>299</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
         <v>299</v>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>299</v>
-      </c>
+      <c r="E16" t="n">
+        <v>299</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>299</v>
       </c>
@@ -1465,10 +1511,10 @@
       <c r="M16" t="n">
         <v>299</v>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="n">
-        <v>299</v>
-      </c>
+      <c r="N16" t="n">
+        <v>299</v>
+      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
         <v>299</v>
       </c>
@@ -1485,6 +1531,9 @@
         <v>299</v>
       </c>
       <c r="U16" t="n">
+        <v>299</v>
+      </c>
+      <c r="V16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1509,10 +1558,10 @@
       <c r="F17" t="n">
         <v>929</v>
       </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="n">
-        <v>929</v>
-      </c>
+      <c r="G17" t="n">
+        <v>929</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
         <v>929</v>
       </c>
@@ -1528,10 +1577,10 @@
       <c r="M17" t="n">
         <v>929</v>
       </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="n">
-        <v>929</v>
-      </c>
+      <c r="N17" t="n">
+        <v>929</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
         <v>929</v>
       </c>
@@ -1548,6 +1597,9 @@
         <v>929</v>
       </c>
       <c r="U17" t="n">
+        <v>929</v>
+      </c>
+      <c r="V17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1569,11 +1621,11 @@
       <c r="E18" t="n">
         <v>499</v>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>499</v>
+      </c>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="n">
-        <v>499</v>
-      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
         <v>499</v>
       </c>
@@ -1589,10 +1641,10 @@
       <c r="M18" t="n">
         <v>499</v>
       </c>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="n">
-        <v>499</v>
-      </c>
+      <c r="N18" t="n">
+        <v>499</v>
+      </c>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
         <v>499</v>
       </c>
@@ -1609,6 +1661,9 @@
         <v>499</v>
       </c>
       <c r="U18" t="n">
+        <v>499</v>
+      </c>
+      <c r="V18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1622,7 +1677,7 @@
         <v>1299</v>
       </c>
       <c r="C19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="D19" t="n">
         <v>1497</v>
@@ -1630,13 +1685,13 @@
       <c r="E19" t="n">
         <v>1497</v>
       </c>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>1497</v>
+      </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="n">
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="n">
         <v>465</v>
-      </c>
-      <c r="I19" t="n">
-        <v>1497</v>
       </c>
       <c r="J19" t="n">
         <v>1497</v>
@@ -1672,6 +1727,9 @@
         <v>1497</v>
       </c>
       <c r="U19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="V19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1717,10 +1775,10 @@
       <c r="M20" t="n">
         <v>929</v>
       </c>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="n">
-        <v>929</v>
-      </c>
+      <c r="N20" t="n">
+        <v>929</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
       <c r="P20" t="n">
         <v>929</v>
       </c>
@@ -1737,6 +1795,9 @@
         <v>929</v>
       </c>
       <c r="U20" t="n">
+        <v>929</v>
+      </c>
+      <c r="V20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1761,10 +1822,10 @@
       <c r="F21" t="n">
         <v>499</v>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="n">
-        <v>499</v>
-      </c>
+      <c r="G21" t="n">
+        <v>499</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>499</v>
       </c>
@@ -1802,6 +1863,9 @@
         <v>499</v>
       </c>
       <c r="U21" t="n">
+        <v>499</v>
+      </c>
+      <c r="V21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1820,14 +1884,14 @@
       <c r="D22" t="n">
         <v>299</v>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>299</v>
-      </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="n">
-        <v>299</v>
-      </c>
+      <c r="E22" t="n">
+        <v>299</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>299</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
         <v>299</v>
       </c>
@@ -1843,10 +1907,10 @@
       <c r="M22" t="n">
         <v>299</v>
       </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="n">
-        <v>299</v>
-      </c>
+      <c r="N22" t="n">
+        <v>299</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
       <c r="P22" t="n">
         <v>299</v>
       </c>
@@ -1863,6 +1927,9 @@
         <v>299</v>
       </c>
       <c r="U22" t="n">
+        <v>299</v>
+      </c>
+      <c r="V22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1884,11 +1951,11 @@
       <c r="E23" t="n">
         <v>1299</v>
       </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>1299</v>
+      </c>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
         <v>1299</v>
       </c>
@@ -1904,10 +1971,10 @@
       <c r="M23" t="n">
         <v>1299</v>
       </c>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="N23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="n">
         <v>1299</v>
       </c>
@@ -1924,6 +1991,9 @@
         <v>1299</v>
       </c>
       <c r="U23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="V23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -1942,11 +2012,11 @@
       <c r="D24" t="n">
         <v>929</v>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>929</v>
+      </c>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="n">
-        <v>929</v>
-      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
         <v>929</v>
       </c>
@@ -1965,10 +2035,10 @@
       <c r="M24" t="n">
         <v>929</v>
       </c>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="n">
-        <v>929</v>
-      </c>
+      <c r="N24" t="n">
+        <v>929</v>
+      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
         <v>929</v>
       </c>
@@ -1985,6 +2055,9 @@
         <v>929</v>
       </c>
       <c r="U24" t="n">
+        <v>929</v>
+      </c>
+      <c r="V24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2003,11 +2076,11 @@
       <c r="D25" t="n">
         <v>929</v>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>929</v>
+      </c>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
-        <v>929</v>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
         <v>929</v>
       </c>
@@ -2026,10 +2099,10 @@
       <c r="M25" t="n">
         <v>929</v>
       </c>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="n">
-        <v>929</v>
-      </c>
+      <c r="N25" t="n">
+        <v>929</v>
+      </c>
+      <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
         <v>929</v>
       </c>
@@ -2046,6 +2119,9 @@
         <v>929</v>
       </c>
       <c r="U25" t="n">
+        <v>929</v>
+      </c>
+      <c r="V25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2064,14 +2140,14 @@
       <c r="D26" t="n">
         <v>1299</v>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
         <v>1299</v>
       </c>
@@ -2087,10 +2163,10 @@
       <c r="M26" t="n">
         <v>1299</v>
       </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="N26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
         <v>1299</v>
       </c>
@@ -2107,6 +2183,9 @@
         <v>1299</v>
       </c>
       <c r="U26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="V26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 07:06
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,7 @@
     <col width="21" customWidth="1" min="20" max="20"/>
     <col width="21" customWidth="1" min="21" max="21"/>
     <col width="21" customWidth="1" min="22" max="22"/>
+    <col width="21" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -465,105 +466,110 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 12:32</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -575,9 +581,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>929</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
         <v>929</v>
       </c>
@@ -590,25 +594,25 @@
       <c r="F2" t="n">
         <v>929</v>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>929</v>
+      </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
-        <v>929</v>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
         <v>929</v>
       </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="n">
-        <v>929</v>
-      </c>
+      <c r="K2" t="n">
+        <v>929</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
         <v>929</v>
       </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="n">
-        <v>929</v>
-      </c>
+      <c r="N2" t="n">
+        <v>929</v>
+      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
         <v>929</v>
       </c>
@@ -628,6 +632,9 @@
         <v>929</v>
       </c>
       <c r="V2" t="n">
+        <v>929</v>
+      </c>
+      <c r="W2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -638,23 +645,21 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>569</v>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>569</v>
       </c>
       <c r="E3" t="n">
         <v>569</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>569</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>569</v>
-      </c>
+      <c r="F3" t="n">
+        <v>569</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>569</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
         <v>569</v>
       </c>
@@ -670,10 +675,10 @@
       <c r="N3" t="n">
         <v>569</v>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="n">
-        <v>569</v>
-      </c>
+      <c r="O3" t="n">
+        <v>569</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="n">
         <v>569</v>
       </c>
@@ -690,6 +695,9 @@
         <v>569</v>
       </c>
       <c r="V3" t="n">
+        <v>569</v>
+      </c>
+      <c r="W3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -711,10 +719,10 @@
       <c r="E4" t="n">
         <v>299</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>299</v>
-      </c>
+      <c r="F4" t="n">
+        <v>299</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>299</v>
       </c>
@@ -736,10 +744,10 @@
       <c r="N4" t="n">
         <v>299</v>
       </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="n">
-        <v>299</v>
-      </c>
+      <c r="O4" t="n">
+        <v>299</v>
+      </c>
+      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="n">
         <v>299</v>
       </c>
@@ -756,6 +764,9 @@
         <v>299</v>
       </c>
       <c r="V4" t="n">
+        <v>299</v>
+      </c>
+      <c r="W4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -804,10 +815,10 @@
       <c r="N5" t="n">
         <v>569</v>
       </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="n">
-        <v>569</v>
-      </c>
+      <c r="O5" t="n">
+        <v>569</v>
+      </c>
+      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="n">
         <v>569</v>
       </c>
@@ -824,6 +835,9 @@
         <v>569</v>
       </c>
       <c r="V5" t="n">
+        <v>569</v>
+      </c>
+      <c r="W5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -848,10 +862,10 @@
       <c r="F6" t="n">
         <v>499</v>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
-        <v>499</v>
-      </c>
+      <c r="G6" t="n">
+        <v>499</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>499</v>
       </c>
@@ -870,10 +884,10 @@
       <c r="N6" t="n">
         <v>499</v>
       </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="n">
-        <v>499</v>
-      </c>
+      <c r="O6" t="n">
+        <v>499</v>
+      </c>
+      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="n">
         <v>499</v>
       </c>
@@ -890,6 +904,9 @@
         <v>499</v>
       </c>
       <c r="V6" t="n">
+        <v>499</v>
+      </c>
+      <c r="W6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -911,12 +928,12 @@
       <c r="E7" t="n">
         <v>569</v>
       </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>569</v>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>569</v>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
         <v>569</v>
       </c>
@@ -932,10 +949,10 @@
       <c r="N7" t="n">
         <v>569</v>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="n">
-        <v>569</v>
-      </c>
+      <c r="O7" t="n">
+        <v>569</v>
+      </c>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="n">
         <v>569</v>
       </c>
@@ -952,6 +969,9 @@
         <v>569</v>
       </c>
       <c r="V7" t="n">
+        <v>569</v>
+      </c>
+      <c r="W7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -973,14 +993,14 @@
       <c r="E8" t="n">
         <v>929</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>929</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
-        <v>929</v>
-      </c>
+      <c r="F8" t="n">
+        <v>929</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>929</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
         <v>929</v>
       </c>
@@ -996,10 +1016,10 @@
       <c r="N8" t="n">
         <v>929</v>
       </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="n">
-        <v>929</v>
-      </c>
+      <c r="O8" t="n">
+        <v>929</v>
+      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="n">
         <v>929</v>
       </c>
@@ -1016,6 +1036,9 @@
         <v>929</v>
       </c>
       <c r="V8" t="n">
+        <v>929</v>
+      </c>
+      <c r="W8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1037,10 +1060,10 @@
       <c r="E9" t="n">
         <v>299</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>299</v>
-      </c>
+      <c r="F9" t="n">
+        <v>299</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>299</v>
       </c>
@@ -1062,10 +1085,10 @@
       <c r="N9" t="n">
         <v>299</v>
       </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="n">
-        <v>299</v>
-      </c>
+      <c r="O9" t="n">
+        <v>299</v>
+      </c>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="n">
         <v>299</v>
       </c>
@@ -1082,6 +1105,9 @@
         <v>299</v>
       </c>
       <c r="V9" t="n">
+        <v>299</v>
+      </c>
+      <c r="W9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1103,14 +1129,14 @@
       <c r="E10" t="n">
         <v>299</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>299</v>
-      </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
-        <v>299</v>
-      </c>
+      <c r="F10" t="n">
+        <v>299</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>299</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="n">
         <v>299</v>
       </c>
@@ -1126,10 +1152,10 @@
       <c r="N10" t="n">
         <v>299</v>
       </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="n">
-        <v>299</v>
-      </c>
+      <c r="O10" t="n">
+        <v>299</v>
+      </c>
+      <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
         <v>299</v>
       </c>
@@ -1146,6 +1172,9 @@
         <v>299</v>
       </c>
       <c r="V10" t="n">
+        <v>299</v>
+      </c>
+      <c r="W10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1170,10 +1199,10 @@
       <c r="F11" t="n">
         <v>2997</v>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
+      <c r="G11" t="n">
         <v>2997</v>
       </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>2997</v>
       </c>
@@ -1187,15 +1216,15 @@
         <v>2997</v>
       </c>
       <c r="M11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="N11" t="n">
         <v>929</v>
       </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="n">
-        <v>929</v>
-      </c>
+      <c r="O11" t="n">
+        <v>929</v>
+      </c>
+      <c r="P11" t="inlineStr"/>
       <c r="Q11" t="n">
         <v>929</v>
       </c>
@@ -1212,6 +1241,9 @@
         <v>929</v>
       </c>
       <c r="V11" t="n">
+        <v>929</v>
+      </c>
+      <c r="W11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1239,10 +1271,10 @@
       <c r="G12" t="n">
         <v>569</v>
       </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
-        <v>569</v>
-      </c>
+      <c r="H12" t="n">
+        <v>569</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="n">
         <v>569</v>
       </c>
@@ -1258,10 +1290,10 @@
       <c r="N12" t="n">
         <v>569</v>
       </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="n">
-        <v>569</v>
-      </c>
+      <c r="O12" t="n">
+        <v>569</v>
+      </c>
+      <c r="P12" t="inlineStr"/>
       <c r="Q12" t="n">
         <v>569</v>
       </c>
@@ -1278,6 +1310,9 @@
         <v>569</v>
       </c>
       <c r="V12" t="n">
+        <v>569</v>
+      </c>
+      <c r="W12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1299,14 +1334,14 @@
       <c r="E13" t="n">
         <v>569</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>569</v>
-      </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>569</v>
-      </c>
+      <c r="F13" t="n">
+        <v>569</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>569</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
         <v>569</v>
       </c>
@@ -1322,24 +1357,27 @@
       <c r="N13" t="n">
         <v>569</v>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="n">
-        <v>569</v>
-      </c>
+      <c r="O13" t="n">
+        <v>569</v>
+      </c>
+      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="n">
         <v>569</v>
       </c>
       <c r="R13" t="n">
         <v>569</v>
       </c>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="n">
-        <v>569</v>
-      </c>
+      <c r="S13" t="n">
+        <v>569</v>
+      </c>
+      <c r="T13" t="inlineStr"/>
       <c r="U13" t="n">
         <v>569</v>
       </c>
       <c r="V13" t="n">
+        <v>569</v>
+      </c>
+      <c r="W13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1361,11 +1399,11 @@
       <c r="E14" t="n">
         <v>499</v>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>499</v>
+      </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="n">
-        <v>499</v>
-      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
         <v>499</v>
       </c>
@@ -1406,6 +1444,9 @@
         <v>499</v>
       </c>
       <c r="V14" t="n">
+        <v>499</v>
+      </c>
+      <c r="W14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1433,10 +1474,10 @@
       <c r="G15" t="n">
         <v>499</v>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
-        <v>499</v>
-      </c>
+      <c r="H15" t="n">
+        <v>499</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="n">
         <v>499</v>
       </c>
@@ -1446,14 +1487,14 @@
       <c r="L15" t="n">
         <v>499</v>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="n">
-        <v>499</v>
-      </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="n">
-        <v>499</v>
-      </c>
+      <c r="M15" t="n">
+        <v>499</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="n">
+        <v>499</v>
+      </c>
+      <c r="P15" t="inlineStr"/>
       <c r="Q15" t="n">
         <v>499</v>
       </c>
@@ -1470,6 +1511,9 @@
         <v>499</v>
       </c>
       <c r="V15" t="n">
+        <v>499</v>
+      </c>
+      <c r="W15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1482,17 +1526,17 @@
       <c r="B16" t="n">
         <v>299</v>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
-        <v>299</v>
-      </c>
+      <c r="C16" t="n">
+        <v>299</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
         <v>299</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>299</v>
-      </c>
+      <c r="F16" t="n">
+        <v>299</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
         <v>299</v>
       </c>
@@ -1514,10 +1558,10 @@
       <c r="N16" t="n">
         <v>299</v>
       </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="n">
-        <v>299</v>
-      </c>
+      <c r="O16" t="n">
+        <v>299</v>
+      </c>
+      <c r="P16" t="inlineStr"/>
       <c r="Q16" t="n">
         <v>299</v>
       </c>
@@ -1534,6 +1578,9 @@
         <v>299</v>
       </c>
       <c r="V16" t="n">
+        <v>299</v>
+      </c>
+      <c r="W16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1561,10 +1608,10 @@
       <c r="G17" t="n">
         <v>929</v>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="n">
-        <v>929</v>
-      </c>
+      <c r="H17" t="n">
+        <v>929</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="n">
         <v>929</v>
       </c>
@@ -1580,10 +1627,10 @@
       <c r="N17" t="n">
         <v>929</v>
       </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="n">
-        <v>929</v>
-      </c>
+      <c r="O17" t="n">
+        <v>929</v>
+      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="n">
         <v>929</v>
       </c>
@@ -1600,6 +1647,9 @@
         <v>929</v>
       </c>
       <c r="V17" t="n">
+        <v>929</v>
+      </c>
+      <c r="W17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1624,11 +1674,11 @@
       <c r="F18" t="n">
         <v>499</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>499</v>
+      </c>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="n">
-        <v>499</v>
-      </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="n">
         <v>499</v>
       </c>
@@ -1644,10 +1694,10 @@
       <c r="N18" t="n">
         <v>499</v>
       </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="n">
-        <v>499</v>
-      </c>
+      <c r="O18" t="n">
+        <v>499</v>
+      </c>
+      <c r="P18" t="inlineStr"/>
       <c r="Q18" t="n">
         <v>499</v>
       </c>
@@ -1664,6 +1714,9 @@
         <v>499</v>
       </c>
       <c r="V18" t="n">
+        <v>499</v>
+      </c>
+      <c r="W18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1680,7 +1733,7 @@
         <v>1299</v>
       </c>
       <c r="D19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="E19" t="n">
         <v>1497</v>
@@ -1688,13 +1741,13 @@
       <c r="F19" t="n">
         <v>1497</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>1497</v>
+      </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="n">
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="n">
         <v>465</v>
-      </c>
-      <c r="J19" t="n">
-        <v>1497</v>
       </c>
       <c r="K19" t="n">
         <v>1497</v>
@@ -1730,6 +1783,9 @@
         <v>1497</v>
       </c>
       <c r="V19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="W19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1778,10 +1834,10 @@
       <c r="N20" t="n">
         <v>929</v>
       </c>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="n">
-        <v>929</v>
-      </c>
+      <c r="O20" t="n">
+        <v>929</v>
+      </c>
+      <c r="P20" t="inlineStr"/>
       <c r="Q20" t="n">
         <v>929</v>
       </c>
@@ -1798,6 +1854,9 @@
         <v>929</v>
       </c>
       <c r="V20" t="n">
+        <v>929</v>
+      </c>
+      <c r="W20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1825,10 +1884,10 @@
       <c r="G21" t="n">
         <v>499</v>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="n">
-        <v>499</v>
-      </c>
+      <c r="H21" t="n">
+        <v>499</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
         <v>499</v>
       </c>
@@ -1866,6 +1925,9 @@
         <v>499</v>
       </c>
       <c r="V21" t="n">
+        <v>499</v>
+      </c>
+      <c r="W21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1887,14 +1949,14 @@
       <c r="E22" t="n">
         <v>299</v>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="n">
-        <v>299</v>
-      </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="n">
-        <v>299</v>
-      </c>
+      <c r="F22" t="n">
+        <v>299</v>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="n">
+        <v>299</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="n">
         <v>299</v>
       </c>
@@ -1910,10 +1972,10 @@
       <c r="N22" t="n">
         <v>299</v>
       </c>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="n">
-        <v>299</v>
-      </c>
+      <c r="O22" t="n">
+        <v>299</v>
+      </c>
+      <c r="P22" t="inlineStr"/>
       <c r="Q22" t="n">
         <v>299</v>
       </c>
@@ -1930,6 +1992,9 @@
         <v>299</v>
       </c>
       <c r="V22" t="n">
+        <v>299</v>
+      </c>
+      <c r="W22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1954,11 +2019,11 @@
       <c r="F23" t="n">
         <v>1299</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>1299</v>
+      </c>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="n">
         <v>1299</v>
       </c>
@@ -1974,10 +2039,10 @@
       <c r="N23" t="n">
         <v>1299</v>
       </c>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="O23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P23" t="inlineStr"/>
       <c r="Q23" t="n">
         <v>1299</v>
       </c>
@@ -1994,6 +2059,9 @@
         <v>1299</v>
       </c>
       <c r="V23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="W23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2015,11 +2083,11 @@
       <c r="E24" t="n">
         <v>929</v>
       </c>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>929</v>
+      </c>
       <c r="G24" t="inlineStr"/>
-      <c r="H24" t="n">
-        <v>929</v>
-      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
         <v>929</v>
       </c>
@@ -2038,10 +2106,10 @@
       <c r="N24" t="n">
         <v>929</v>
       </c>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="n">
-        <v>929</v>
-      </c>
+      <c r="O24" t="n">
+        <v>929</v>
+      </c>
+      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="n">
         <v>929</v>
       </c>
@@ -2058,6 +2126,9 @@
         <v>929</v>
       </c>
       <c r="V24" t="n">
+        <v>929</v>
+      </c>
+      <c r="W24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2079,11 +2150,11 @@
       <c r="E25" t="n">
         <v>929</v>
       </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>929</v>
+      </c>
       <c r="G25" t="inlineStr"/>
-      <c r="H25" t="n">
-        <v>929</v>
-      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
         <v>929</v>
       </c>
@@ -2102,10 +2173,10 @@
       <c r="N25" t="n">
         <v>929</v>
       </c>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="n">
-        <v>929</v>
-      </c>
+      <c r="O25" t="n">
+        <v>929</v>
+      </c>
+      <c r="P25" t="inlineStr"/>
       <c r="Q25" t="n">
         <v>929</v>
       </c>
@@ -2122,6 +2193,9 @@
         <v>929</v>
       </c>
       <c r="V25" t="n">
+        <v>929</v>
+      </c>
+      <c r="W25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2143,14 +2217,14 @@
       <c r="E26" t="n">
         <v>1299</v>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="n">
         <v>1299</v>
       </c>
@@ -2166,10 +2240,10 @@
       <c r="N26" t="n">
         <v>1299</v>
       </c>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="O26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P26" t="inlineStr"/>
       <c r="Q26" t="n">
         <v>1299</v>
       </c>
@@ -2186,6 +2260,9 @@
         <v>1299</v>
       </c>
       <c r="V26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="W26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 09:01
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,7 @@
     <col width="21" customWidth="1" min="21" max="21"/>
     <col width="21" customWidth="1" min="22" max="22"/>
     <col width="21" customWidth="1" min="23" max="23"/>
+    <col width="21" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,110 +467,115 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 14:27</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -581,10 +587,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 84 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>929</v>
-      </c>
+      <c r="B2" t="n">
+        <v>929</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
         <v>929</v>
       </c>
@@ -597,25 +603,25 @@
       <c r="G2" t="n">
         <v>929</v>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>929</v>
+      </c>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
-        <v>929</v>
-      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
         <v>929</v>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>929</v>
-      </c>
+      <c r="L2" t="n">
+        <v>929</v>
+      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
         <v>929</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="n">
-        <v>929</v>
-      </c>
+      <c r="O2" t="n">
+        <v>929</v>
+      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="n">
         <v>929</v>
       </c>
@@ -635,6 +641,9 @@
         <v>929</v>
       </c>
       <c r="W2" t="n">
+        <v>929</v>
+      </c>
+      <c r="X2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -646,23 +655,21 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>569</v>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>569</v>
       </c>
       <c r="F3" t="n">
         <v>569</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>569</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>569</v>
-      </c>
+      <c r="G3" t="n">
+        <v>569</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>569</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
         <v>569</v>
       </c>
@@ -678,10 +685,10 @@
       <c r="O3" t="n">
         <v>569</v>
       </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="n">
-        <v>569</v>
-      </c>
+      <c r="P3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
         <v>569</v>
       </c>
@@ -698,6 +705,9 @@
         <v>569</v>
       </c>
       <c r="W3" t="n">
+        <v>569</v>
+      </c>
+      <c r="X3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -722,10 +732,10 @@
       <c r="F4" t="n">
         <v>299</v>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>299</v>
-      </c>
+      <c r="G4" t="n">
+        <v>299</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>299</v>
       </c>
@@ -747,10 +757,10 @@
       <c r="O4" t="n">
         <v>299</v>
       </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="n">
-        <v>299</v>
-      </c>
+      <c r="P4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
         <v>299</v>
       </c>
@@ -767,6 +777,9 @@
         <v>299</v>
       </c>
       <c r="W4" t="n">
+        <v>299</v>
+      </c>
+      <c r="X4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -818,10 +831,10 @@
       <c r="O5" t="n">
         <v>569</v>
       </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="n">
-        <v>569</v>
-      </c>
+      <c r="P5" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
         <v>569</v>
       </c>
@@ -838,6 +851,9 @@
         <v>569</v>
       </c>
       <c r="W5" t="n">
+        <v>569</v>
+      </c>
+      <c r="X5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -865,10 +881,10 @@
       <c r="G6" t="n">
         <v>499</v>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>499</v>
-      </c>
+      <c r="H6" t="n">
+        <v>499</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
         <v>499</v>
       </c>
@@ -887,10 +903,10 @@
       <c r="O6" t="n">
         <v>499</v>
       </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="n">
-        <v>499</v>
-      </c>
+      <c r="P6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
         <v>499</v>
       </c>
@@ -907,6 +923,9 @@
         <v>499</v>
       </c>
       <c r="W6" t="n">
+        <v>499</v>
+      </c>
+      <c r="X6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -931,12 +950,12 @@
       <c r="F7" t="n">
         <v>569</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>569</v>
+      </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
-        <v>569</v>
-      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
         <v>569</v>
       </c>
@@ -952,10 +971,10 @@
       <c r="O7" t="n">
         <v>569</v>
       </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="n">
-        <v>569</v>
-      </c>
+      <c r="P7" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
         <v>569</v>
       </c>
@@ -972,6 +991,9 @@
         <v>569</v>
       </c>
       <c r="W7" t="n">
+        <v>569</v>
+      </c>
+      <c r="X7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -996,14 +1018,14 @@
       <c r="F8" t="n">
         <v>929</v>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>929</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
-        <v>929</v>
-      </c>
+      <c r="G8" t="n">
+        <v>929</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>929</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
         <v>929</v>
       </c>
@@ -1019,10 +1041,10 @@
       <c r="O8" t="n">
         <v>929</v>
       </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="n">
-        <v>929</v>
-      </c>
+      <c r="P8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
         <v>929</v>
       </c>
@@ -1039,6 +1061,9 @@
         <v>929</v>
       </c>
       <c r="W8" t="n">
+        <v>929</v>
+      </c>
+      <c r="X8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1063,10 +1088,10 @@
       <c r="F9" t="n">
         <v>299</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>299</v>
-      </c>
+      <c r="G9" t="n">
+        <v>299</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>299</v>
       </c>
@@ -1088,10 +1113,10 @@
       <c r="O9" t="n">
         <v>299</v>
       </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="n">
-        <v>299</v>
-      </c>
+      <c r="P9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="n">
         <v>299</v>
       </c>
@@ -1108,6 +1133,9 @@
         <v>299</v>
       </c>
       <c r="W9" t="n">
+        <v>299</v>
+      </c>
+      <c r="X9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1132,14 +1160,14 @@
       <c r="F10" t="n">
         <v>299</v>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>299</v>
-      </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>299</v>
-      </c>
+      <c r="G10" t="n">
+        <v>299</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>299</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
         <v>299</v>
       </c>
@@ -1155,10 +1183,10 @@
       <c r="O10" t="n">
         <v>299</v>
       </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="n">
-        <v>299</v>
-      </c>
+      <c r="P10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
         <v>299</v>
       </c>
@@ -1175,6 +1203,9 @@
         <v>299</v>
       </c>
       <c r="W10" t="n">
+        <v>299</v>
+      </c>
+      <c r="X10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1202,10 +1233,10 @@
       <c r="G11" t="n">
         <v>2997</v>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
+      <c r="H11" t="n">
         <v>2997</v>
       </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
         <v>2997</v>
       </c>
@@ -1219,15 +1250,15 @@
         <v>2997</v>
       </c>
       <c r="N11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="O11" t="n">
         <v>929</v>
       </c>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="n">
-        <v>929</v>
-      </c>
+      <c r="P11" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
         <v>929</v>
       </c>
@@ -1244,6 +1275,9 @@
         <v>929</v>
       </c>
       <c r="W11" t="n">
+        <v>929</v>
+      </c>
+      <c r="X11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1274,10 +1308,10 @@
       <c r="H12" t="n">
         <v>569</v>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="n">
-        <v>569</v>
-      </c>
+      <c r="I12" t="n">
+        <v>569</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
         <v>569</v>
       </c>
@@ -1293,10 +1327,10 @@
       <c r="O12" t="n">
         <v>569</v>
       </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="n">
-        <v>569</v>
-      </c>
+      <c r="P12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
         <v>569</v>
       </c>
@@ -1313,6 +1347,9 @@
         <v>569</v>
       </c>
       <c r="W12" t="n">
+        <v>569</v>
+      </c>
+      <c r="X12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1337,14 +1374,14 @@
       <c r="F13" t="n">
         <v>569</v>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>569</v>
-      </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
-        <v>569</v>
-      </c>
+      <c r="G13" t="n">
+        <v>569</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>569</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>569</v>
       </c>
@@ -1360,24 +1397,27 @@
       <c r="O13" t="n">
         <v>569</v>
       </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="n">
-        <v>569</v>
-      </c>
+      <c r="P13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
         <v>569</v>
       </c>
       <c r="S13" t="n">
         <v>569</v>
       </c>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="n">
-        <v>569</v>
-      </c>
+      <c r="T13" t="n">
+        <v>569</v>
+      </c>
+      <c r="U13" t="inlineStr"/>
       <c r="V13" t="n">
         <v>569</v>
       </c>
       <c r="W13" t="n">
+        <v>569</v>
+      </c>
+      <c r="X13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1402,11 +1442,11 @@
       <c r="F14" t="n">
         <v>499</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>499</v>
+      </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="n">
-        <v>499</v>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="n">
         <v>499</v>
       </c>
@@ -1447,6 +1487,9 @@
         <v>499</v>
       </c>
       <c r="W14" t="n">
+        <v>499</v>
+      </c>
+      <c r="X14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1477,10 +1520,10 @@
       <c r="H15" t="n">
         <v>499</v>
       </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="n">
-        <v>499</v>
-      </c>
+      <c r="I15" t="n">
+        <v>499</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
         <v>499</v>
       </c>
@@ -1490,14 +1533,14 @@
       <c r="M15" t="n">
         <v>499</v>
       </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="n">
-        <v>499</v>
-      </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="n">
-        <v>499</v>
-      </c>
+      <c r="N15" t="n">
+        <v>499</v>
+      </c>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="n">
         <v>499</v>
       </c>
@@ -1514,6 +1557,9 @@
         <v>499</v>
       </c>
       <c r="W15" t="n">
+        <v>499</v>
+      </c>
+      <c r="X15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1529,17 +1575,17 @@
       <c r="C16" t="n">
         <v>299</v>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>299</v>
-      </c>
+      <c r="D16" t="n">
+        <v>299</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
         <v>299</v>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="n">
-        <v>299</v>
-      </c>
+      <c r="G16" t="n">
+        <v>299</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
         <v>299</v>
       </c>
@@ -1561,10 +1607,10 @@
       <c r="O16" t="n">
         <v>299</v>
       </c>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="n">
-        <v>299</v>
-      </c>
+      <c r="P16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="n">
         <v>299</v>
       </c>
@@ -1581,6 +1627,9 @@
         <v>299</v>
       </c>
       <c r="W16" t="n">
+        <v>299</v>
+      </c>
+      <c r="X16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1611,10 +1660,10 @@
       <c r="H17" t="n">
         <v>929</v>
       </c>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="n">
-        <v>929</v>
-      </c>
+      <c r="I17" t="n">
+        <v>929</v>
+      </c>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
         <v>929</v>
       </c>
@@ -1630,10 +1679,10 @@
       <c r="O17" t="n">
         <v>929</v>
       </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="n">
-        <v>929</v>
-      </c>
+      <c r="P17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
         <v>929</v>
       </c>
@@ -1650,6 +1699,9 @@
         <v>929</v>
       </c>
       <c r="W17" t="n">
+        <v>929</v>
+      </c>
+      <c r="X17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1677,11 +1729,11 @@
       <c r="G18" t="n">
         <v>499</v>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>499</v>
+      </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="n">
-        <v>499</v>
-      </c>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
         <v>499</v>
       </c>
@@ -1697,10 +1749,10 @@
       <c r="O18" t="n">
         <v>499</v>
       </c>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="n">
-        <v>499</v>
-      </c>
+      <c r="P18" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
         <v>499</v>
       </c>
@@ -1717,6 +1769,9 @@
         <v>499</v>
       </c>
       <c r="W18" t="n">
+        <v>499</v>
+      </c>
+      <c r="X18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1736,7 +1791,7 @@
         <v>1299</v>
       </c>
       <c r="E19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="F19" t="n">
         <v>1497</v>
@@ -1744,13 +1799,13 @@
       <c r="G19" t="n">
         <v>1497</v>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="n">
+        <v>1497</v>
+      </c>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="n">
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="n">
         <v>465</v>
-      </c>
-      <c r="K19" t="n">
-        <v>1497</v>
       </c>
       <c r="L19" t="n">
         <v>1497</v>
@@ -1786,6 +1841,9 @@
         <v>1497</v>
       </c>
       <c r="W19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="X19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1837,10 +1895,10 @@
       <c r="O20" t="n">
         <v>929</v>
       </c>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="n">
-        <v>929</v>
-      </c>
+      <c r="P20" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
         <v>929</v>
       </c>
@@ -1857,6 +1915,9 @@
         <v>929</v>
       </c>
       <c r="W20" t="n">
+        <v>929</v>
+      </c>
+      <c r="X20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1887,10 +1948,10 @@
       <c r="H21" t="n">
         <v>499</v>
       </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>499</v>
-      </c>
+      <c r="I21" t="n">
+        <v>499</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>499</v>
       </c>
@@ -1928,6 +1989,9 @@
         <v>499</v>
       </c>
       <c r="W21" t="n">
+        <v>499</v>
+      </c>
+      <c r="X21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1952,14 +2016,14 @@
       <c r="F22" t="n">
         <v>299</v>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="n">
-        <v>299</v>
-      </c>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="n">
-        <v>299</v>
-      </c>
+      <c r="G22" t="n">
+        <v>299</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>299</v>
+      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
         <v>299</v>
       </c>
@@ -1975,10 +2039,10 @@
       <c r="O22" t="n">
         <v>299</v>
       </c>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="n">
-        <v>299</v>
-      </c>
+      <c r="P22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="n">
         <v>299</v>
       </c>
@@ -1995,6 +2059,9 @@
         <v>299</v>
       </c>
       <c r="W22" t="n">
+        <v>299</v>
+      </c>
+      <c r="X22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2022,11 +2089,11 @@
       <c r="G23" t="n">
         <v>1299</v>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>1299</v>
+      </c>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
         <v>1299</v>
       </c>
@@ -2042,10 +2109,10 @@
       <c r="O23" t="n">
         <v>1299</v>
       </c>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="P23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Q23" t="inlineStr"/>
       <c r="R23" t="n">
         <v>1299</v>
       </c>
@@ -2062,6 +2129,9 @@
         <v>1299</v>
       </c>
       <c r="W23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="X23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2086,11 +2156,11 @@
       <c r="F24" t="n">
         <v>929</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>929</v>
+      </c>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="n">
-        <v>929</v>
-      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="n">
         <v>929</v>
       </c>
@@ -2109,10 +2179,10 @@
       <c r="O24" t="n">
         <v>929</v>
       </c>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="n">
-        <v>929</v>
-      </c>
+      <c r="P24" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="n">
         <v>929</v>
       </c>
@@ -2129,6 +2199,9 @@
         <v>929</v>
       </c>
       <c r="W24" t="n">
+        <v>929</v>
+      </c>
+      <c r="X24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2153,11 +2226,11 @@
       <c r="F25" t="n">
         <v>929</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>929</v>
+      </c>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="n">
-        <v>929</v>
-      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="n">
         <v>929</v>
       </c>
@@ -2176,10 +2249,10 @@
       <c r="O25" t="n">
         <v>929</v>
       </c>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="n">
-        <v>929</v>
-      </c>
+      <c r="P25" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q25" t="inlineStr"/>
       <c r="R25" t="n">
         <v>929</v>
       </c>
@@ -2196,6 +2269,9 @@
         <v>929</v>
       </c>
       <c r="W25" t="n">
+        <v>929</v>
+      </c>
+      <c r="X25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2220,14 +2296,14 @@
       <c r="F26" t="n">
         <v>1299</v>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
         <v>1299</v>
       </c>
@@ -2243,10 +2319,10 @@
       <c r="O26" t="n">
         <v>1299</v>
       </c>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="P26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Q26" t="inlineStr"/>
       <c r="R26" t="n">
         <v>1299</v>
       </c>
@@ -2263,6 +2339,9 @@
         <v>1299</v>
       </c>
       <c r="W26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="X26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 10:52
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X26"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,7 @@
     <col width="21" customWidth="1" min="22" max="22"/>
     <col width="21" customWidth="1" min="23" max="23"/>
     <col width="21" customWidth="1" min="24" max="24"/>
+    <col width="21" customWidth="1" min="25" max="25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -467,115 +468,120 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 16:18</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -590,10 +596,10 @@
       <c r="B2" t="n">
         <v>929</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>929</v>
-      </c>
+      <c r="C2" t="n">
+        <v>929</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>929</v>
       </c>
@@ -606,25 +612,25 @@
       <c r="H2" t="n">
         <v>929</v>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>929</v>
+      </c>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="n">
-        <v>929</v>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
         <v>929</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="n">
-        <v>929</v>
-      </c>
+      <c r="M2" t="n">
+        <v>929</v>
+      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
         <v>929</v>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="n">
-        <v>929</v>
-      </c>
+      <c r="P2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
         <v>929</v>
       </c>
@@ -644,6 +650,9 @@
         <v>929</v>
       </c>
       <c r="X2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -653,26 +662,26 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>569</v>
+      </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>569</v>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>569</v>
       </c>
       <c r="G3" t="n">
         <v>569</v>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>569</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>569</v>
-      </c>
+      <c r="H3" t="n">
+        <v>569</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>569</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
         <v>569</v>
       </c>
@@ -688,10 +697,10 @@
       <c r="P3" t="n">
         <v>569</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q3" t="n">
+        <v>569</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
         <v>569</v>
       </c>
@@ -708,6 +717,9 @@
         <v>569</v>
       </c>
       <c r="X3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -735,10 +747,10 @@
       <c r="G4" t="n">
         <v>299</v>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>299</v>
-      </c>
+      <c r="H4" t="n">
+        <v>299</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
         <v>299</v>
       </c>
@@ -760,10 +772,10 @@
       <c r="P4" t="n">
         <v>299</v>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q4" t="n">
+        <v>299</v>
+      </c>
+      <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
         <v>299</v>
       </c>
@@ -780,6 +792,9 @@
         <v>299</v>
       </c>
       <c r="X4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -834,10 +849,10 @@
       <c r="P5" t="n">
         <v>569</v>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q5" t="n">
+        <v>569</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
       <c r="S5" t="n">
         <v>569</v>
       </c>
@@ -854,6 +869,9 @@
         <v>569</v>
       </c>
       <c r="X5" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -884,10 +902,10 @@
       <c r="H6" t="n">
         <v>499</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
-        <v>499</v>
-      </c>
+      <c r="I6" t="n">
+        <v>499</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
         <v>499</v>
       </c>
@@ -906,10 +924,10 @@
       <c r="P6" t="n">
         <v>499</v>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q6" t="n">
+        <v>499</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
       <c r="S6" t="n">
         <v>499</v>
       </c>
@@ -926,6 +944,9 @@
         <v>499</v>
       </c>
       <c r="X6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -953,12 +974,12 @@
       <c r="G7" t="n">
         <v>569</v>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>569</v>
+      </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>569</v>
-      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
         <v>569</v>
       </c>
@@ -974,10 +995,10 @@
       <c r="P7" t="n">
         <v>569</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q7" t="n">
+        <v>569</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
       <c r="S7" t="n">
         <v>569</v>
       </c>
@@ -994,6 +1015,9 @@
         <v>569</v>
       </c>
       <c r="X7" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1021,14 +1045,14 @@
       <c r="G8" t="n">
         <v>929</v>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
-        <v>929</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>929</v>
-      </c>
+      <c r="H8" t="n">
+        <v>929</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>929</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="n">
         <v>929</v>
       </c>
@@ -1044,10 +1068,10 @@
       <c r="P8" t="n">
         <v>929</v>
       </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q8" t="n">
+        <v>929</v>
+      </c>
+      <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
         <v>929</v>
       </c>
@@ -1064,6 +1088,9 @@
         <v>929</v>
       </c>
       <c r="X8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1091,10 +1118,10 @@
       <c r="G9" t="n">
         <v>299</v>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
-        <v>299</v>
-      </c>
+      <c r="H9" t="n">
+        <v>299</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
         <v>299</v>
       </c>
@@ -1116,10 +1143,10 @@
       <c r="P9" t="n">
         <v>299</v>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q9" t="n">
+        <v>299</v>
+      </c>
+      <c r="R9" t="inlineStr"/>
       <c r="S9" t="n">
         <v>299</v>
       </c>
@@ -1136,6 +1163,9 @@
         <v>299</v>
       </c>
       <c r="X9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1163,14 +1193,14 @@
       <c r="G10" t="n">
         <v>299</v>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
-        <v>299</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>299</v>
-      </c>
+      <c r="H10" t="n">
+        <v>299</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>299</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
         <v>299</v>
       </c>
@@ -1186,10 +1216,10 @@
       <c r="P10" t="n">
         <v>299</v>
       </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q10" t="n">
+        <v>299</v>
+      </c>
+      <c r="R10" t="inlineStr"/>
       <c r="S10" t="n">
         <v>299</v>
       </c>
@@ -1206,6 +1236,9 @@
         <v>299</v>
       </c>
       <c r="X10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1236,10 +1269,10 @@
       <c r="H11" t="n">
         <v>2997</v>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="n">
+      <c r="I11" t="n">
         <v>2997</v>
       </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
         <v>2997</v>
       </c>
@@ -1253,15 +1286,15 @@
         <v>2997</v>
       </c>
       <c r="O11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="P11" t="n">
         <v>929</v>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q11" t="n">
+        <v>929</v>
+      </c>
+      <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
         <v>929</v>
       </c>
@@ -1278,6 +1311,9 @@
         <v>929</v>
       </c>
       <c r="X11" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1311,10 +1347,10 @@
       <c r="I12" t="n">
         <v>569</v>
       </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
-        <v>569</v>
-      </c>
+      <c r="J12" t="n">
+        <v>569</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
         <v>569</v>
       </c>
@@ -1330,10 +1366,10 @@
       <c r="P12" t="n">
         <v>569</v>
       </c>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q12" t="n">
+        <v>569</v>
+      </c>
+      <c r="R12" t="inlineStr"/>
       <c r="S12" t="n">
         <v>569</v>
       </c>
@@ -1350,6 +1386,9 @@
         <v>569</v>
       </c>
       <c r="X12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1377,14 +1416,14 @@
       <c r="G13" t="n">
         <v>569</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>569</v>
-      </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>569</v>
-      </c>
+      <c r="H13" t="n">
+        <v>569</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>569</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
         <v>569</v>
       </c>
@@ -1400,24 +1439,27 @@
       <c r="P13" t="n">
         <v>569</v>
       </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q13" t="n">
+        <v>569</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
       <c r="S13" t="n">
         <v>569</v>
       </c>
       <c r="T13" t="n">
         <v>569</v>
       </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="n">
-        <v>569</v>
-      </c>
+      <c r="U13" t="n">
+        <v>569</v>
+      </c>
+      <c r="V13" t="inlineStr"/>
       <c r="W13" t="n">
         <v>569</v>
       </c>
       <c r="X13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1428,7 +1470,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="C14" t="n">
         <v>499</v>
@@ -1445,11 +1487,11 @@
       <c r="G14" t="n">
         <v>499</v>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>499</v>
+      </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="n">
-        <v>499</v>
-      </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
         <v>499</v>
       </c>
@@ -1490,6 +1532,9 @@
         <v>499</v>
       </c>
       <c r="X14" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1523,10 +1568,10 @@
       <c r="I15" t="n">
         <v>499</v>
       </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="n">
-        <v>499</v>
-      </c>
+      <c r="J15" t="n">
+        <v>499</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="n">
         <v>499</v>
       </c>
@@ -1536,14 +1581,14 @@
       <c r="N15" t="n">
         <v>499</v>
       </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="n">
-        <v>499</v>
-      </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="n">
-        <v>499</v>
-      </c>
+      <c r="O15" t="n">
+        <v>499</v>
+      </c>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="n">
+        <v>499</v>
+      </c>
+      <c r="R15" t="inlineStr"/>
       <c r="S15" t="n">
         <v>499</v>
       </c>
@@ -1560,6 +1605,9 @@
         <v>499</v>
       </c>
       <c r="X15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1578,17 +1626,17 @@
       <c r="D16" t="n">
         <v>299</v>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>299</v>
-      </c>
+      <c r="E16" t="n">
+        <v>299</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>299</v>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>299</v>
-      </c>
+      <c r="H16" t="n">
+        <v>299</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
         <v>299</v>
       </c>
@@ -1610,10 +1658,10 @@
       <c r="P16" t="n">
         <v>299</v>
       </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q16" t="n">
+        <v>299</v>
+      </c>
+      <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
         <v>299</v>
       </c>
@@ -1630,6 +1678,9 @@
         <v>299</v>
       </c>
       <c r="X16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1663,10 +1714,10 @@
       <c r="I17" t="n">
         <v>929</v>
       </c>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="n">
-        <v>929</v>
-      </c>
+      <c r="J17" t="n">
+        <v>929</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="n">
         <v>929</v>
       </c>
@@ -1682,10 +1733,10 @@
       <c r="P17" t="n">
         <v>929</v>
       </c>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q17" t="n">
+        <v>929</v>
+      </c>
+      <c r="R17" t="inlineStr"/>
       <c r="S17" t="n">
         <v>929</v>
       </c>
@@ -1702,6 +1753,9 @@
         <v>929</v>
       </c>
       <c r="X17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1732,11 +1786,11 @@
       <c r="H18" t="n">
         <v>499</v>
       </c>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>499</v>
+      </c>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="n">
-        <v>499</v>
-      </c>
+      <c r="K18" t="inlineStr"/>
       <c r="L18" t="n">
         <v>499</v>
       </c>
@@ -1752,10 +1806,10 @@
       <c r="P18" t="n">
         <v>499</v>
       </c>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q18" t="n">
+        <v>499</v>
+      </c>
+      <c r="R18" t="inlineStr"/>
       <c r="S18" t="n">
         <v>499</v>
       </c>
@@ -1772,6 +1826,9 @@
         <v>499</v>
       </c>
       <c r="X18" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1794,7 +1851,7 @@
         <v>1299</v>
       </c>
       <c r="F19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="G19" t="n">
         <v>1497</v>
@@ -1802,13 +1859,13 @@
       <c r="H19" t="n">
         <v>1497</v>
       </c>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>1497</v>
+      </c>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="n">
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="n">
         <v>465</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1497</v>
       </c>
       <c r="M19" t="n">
         <v>1497</v>
@@ -1844,6 +1901,9 @@
         <v>1497</v>
       </c>
       <c r="X19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="Y19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1898,10 +1958,10 @@
       <c r="P20" t="n">
         <v>929</v>
       </c>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q20" t="n">
+        <v>929</v>
+      </c>
+      <c r="R20" t="inlineStr"/>
       <c r="S20" t="n">
         <v>929</v>
       </c>
@@ -1918,6 +1978,9 @@
         <v>929</v>
       </c>
       <c r="X20" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1951,10 +2014,10 @@
       <c r="I21" t="n">
         <v>499</v>
       </c>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="n">
-        <v>499</v>
-      </c>
+      <c r="J21" t="n">
+        <v>499</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="n">
         <v>499</v>
       </c>
@@ -1992,6 +2055,9 @@
         <v>499</v>
       </c>
       <c r="X21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2019,14 +2085,14 @@
       <c r="G22" t="n">
         <v>299</v>
       </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="n">
-        <v>299</v>
-      </c>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="n">
-        <v>299</v>
-      </c>
+      <c r="H22" t="n">
+        <v>299</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="n">
+        <v>299</v>
+      </c>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="n">
         <v>299</v>
       </c>
@@ -2042,10 +2108,10 @@
       <c r="P22" t="n">
         <v>299</v>
       </c>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q22" t="n">
+        <v>299</v>
+      </c>
+      <c r="R22" t="inlineStr"/>
       <c r="S22" t="n">
         <v>299</v>
       </c>
@@ -2062,6 +2128,9 @@
         <v>299</v>
       </c>
       <c r="X22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2092,11 +2161,11 @@
       <c r="H23" t="n">
         <v>1299</v>
       </c>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>1299</v>
+      </c>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="n">
         <v>1299</v>
       </c>
@@ -2112,10 +2181,10 @@
       <c r="P23" t="n">
         <v>1299</v>
       </c>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Q23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="R23" t="inlineStr"/>
       <c r="S23" t="n">
         <v>1299</v>
       </c>
@@ -2132,6 +2201,9 @@
         <v>1299</v>
       </c>
       <c r="X23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Y23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2159,11 +2231,11 @@
       <c r="G24" t="n">
         <v>929</v>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="n">
+        <v>929</v>
+      </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="n">
-        <v>929</v>
-      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
         <v>929</v>
       </c>
@@ -2182,10 +2254,10 @@
       <c r="P24" t="n">
         <v>929</v>
       </c>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q24" t="n">
+        <v>929</v>
+      </c>
+      <c r="R24" t="inlineStr"/>
       <c r="S24" t="n">
         <v>929</v>
       </c>
@@ -2202,6 +2274,9 @@
         <v>929</v>
       </c>
       <c r="X24" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2229,11 +2304,11 @@
       <c r="G25" t="n">
         <v>929</v>
       </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" t="n">
+        <v>929</v>
+      </c>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="n">
-        <v>929</v>
-      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
         <v>929</v>
       </c>
@@ -2252,10 +2327,10 @@
       <c r="P25" t="n">
         <v>929</v>
       </c>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q25" t="n">
+        <v>929</v>
+      </c>
+      <c r="R25" t="inlineStr"/>
       <c r="S25" t="n">
         <v>929</v>
       </c>
@@ -2272,6 +2347,9 @@
         <v>929</v>
       </c>
       <c r="X25" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2299,14 +2377,14 @@
       <c r="G26" t="n">
         <v>1299</v>
       </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="n">
         <v>1299</v>
       </c>
@@ -2322,10 +2400,10 @@
       <c r="P26" t="n">
         <v>1299</v>
       </c>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Q26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="R26" t="inlineStr"/>
       <c r="S26" t="n">
         <v>1299</v>
       </c>
@@ -2342,6 +2420,9 @@
         <v>1299</v>
       </c>
       <c r="X26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Y26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 13:52
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,6 +458,7 @@
     <col width="21" customWidth="1" min="23" max="23"/>
     <col width="21" customWidth="1" min="24" max="24"/>
     <col width="21" customWidth="1" min="25" max="25"/>
+    <col width="21" customWidth="1" min="26" max="26"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,120 +469,125 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 19:18</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -599,10 +605,10 @@
       <c r="C2" t="n">
         <v>929</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>929</v>
-      </c>
+      <c r="D2" t="n">
+        <v>929</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
         <v>929</v>
       </c>
@@ -615,25 +621,25 @@
       <c r="I2" t="n">
         <v>929</v>
       </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>929</v>
+      </c>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="n">
-        <v>929</v>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
         <v>929</v>
       </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="n">
-        <v>929</v>
-      </c>
+      <c r="N2" t="n">
+        <v>929</v>
+      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
         <v>929</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q2" t="n">
+        <v>929</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
         <v>929</v>
       </c>
@@ -653,6 +659,9 @@
         <v>929</v>
       </c>
       <c r="Y2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -665,26 +674,26 @@
       <c r="B3" t="n">
         <v>569</v>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>569</v>
+      </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>569</v>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>569</v>
       </c>
       <c r="H3" t="n">
         <v>569</v>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>569</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
-        <v>569</v>
-      </c>
+      <c r="I3" t="n">
+        <v>569</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>569</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>569</v>
       </c>
@@ -700,10 +709,10 @@
       <c r="Q3" t="n">
         <v>569</v>
       </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="n">
-        <v>569</v>
-      </c>
+      <c r="R3" t="n">
+        <v>569</v>
+      </c>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="n">
         <v>569</v>
       </c>
@@ -720,6 +729,9 @@
         <v>569</v>
       </c>
       <c r="Y3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -750,10 +762,10 @@
       <c r="H4" t="n">
         <v>299</v>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="n">
-        <v>299</v>
-      </c>
+      <c r="I4" t="n">
+        <v>299</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
         <v>299</v>
       </c>
@@ -775,10 +787,10 @@
       <c r="Q4" t="n">
         <v>299</v>
       </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="n">
-        <v>299</v>
-      </c>
+      <c r="R4" t="n">
+        <v>299</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="n">
         <v>299</v>
       </c>
@@ -795,6 +807,9 @@
         <v>299</v>
       </c>
       <c r="Y4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -852,10 +867,10 @@
       <c r="Q5" t="n">
         <v>569</v>
       </c>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="n">
-        <v>569</v>
-      </c>
+      <c r="R5" t="n">
+        <v>569</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
       <c r="T5" t="n">
         <v>569</v>
       </c>
@@ -872,6 +887,9 @@
         <v>569</v>
       </c>
       <c r="Y5" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -905,10 +923,10 @@
       <c r="I6" t="n">
         <v>499</v>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>499</v>
-      </c>
+      <c r="J6" t="n">
+        <v>499</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="n">
         <v>499</v>
       </c>
@@ -927,10 +945,10 @@
       <c r="Q6" t="n">
         <v>499</v>
       </c>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="n">
-        <v>499</v>
-      </c>
+      <c r="R6" t="n">
+        <v>499</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="n">
         <v>499</v>
       </c>
@@ -947,6 +965,9 @@
         <v>499</v>
       </c>
       <c r="Y6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -977,12 +998,12 @@
       <c r="H7" t="n">
         <v>569</v>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>569</v>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="n">
-        <v>569</v>
-      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
         <v>569</v>
       </c>
@@ -998,10 +1019,10 @@
       <c r="Q7" t="n">
         <v>569</v>
       </c>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="n">
-        <v>569</v>
-      </c>
+      <c r="R7" t="n">
+        <v>569</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="n">
         <v>569</v>
       </c>
@@ -1018,6 +1039,9 @@
         <v>569</v>
       </c>
       <c r="Y7" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1048,14 +1072,14 @@
       <c r="H8" t="n">
         <v>929</v>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
-        <v>929</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="n">
-        <v>929</v>
-      </c>
+      <c r="I8" t="n">
+        <v>929</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>929</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
         <v>929</v>
       </c>
@@ -1071,10 +1095,10 @@
       <c r="Q8" t="n">
         <v>929</v>
       </c>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="n">
-        <v>929</v>
-      </c>
+      <c r="R8" t="n">
+        <v>929</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
       <c r="T8" t="n">
         <v>929</v>
       </c>
@@ -1091,6 +1115,9 @@
         <v>929</v>
       </c>
       <c r="Y8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1121,10 +1148,10 @@
       <c r="H9" t="n">
         <v>299</v>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
-        <v>299</v>
-      </c>
+      <c r="I9" t="n">
+        <v>299</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
         <v>299</v>
       </c>
@@ -1146,10 +1173,10 @@
       <c r="Q9" t="n">
         <v>299</v>
       </c>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="n">
-        <v>299</v>
-      </c>
+      <c r="R9" t="n">
+        <v>299</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="n">
         <v>299</v>
       </c>
@@ -1166,6 +1193,9 @@
         <v>299</v>
       </c>
       <c r="Y9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1196,14 +1226,14 @@
       <c r="H10" t="n">
         <v>299</v>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>299</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
-        <v>299</v>
-      </c>
+      <c r="I10" t="n">
+        <v>299</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>299</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
         <v>299</v>
       </c>
@@ -1219,10 +1249,10 @@
       <c r="Q10" t="n">
         <v>299</v>
       </c>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="n">
-        <v>299</v>
-      </c>
+      <c r="R10" t="n">
+        <v>299</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="n">
         <v>299</v>
       </c>
@@ -1239,6 +1269,9 @@
         <v>299</v>
       </c>
       <c r="Y10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1272,10 +1305,10 @@
       <c r="I11" t="n">
         <v>2997</v>
       </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="n">
+      <c r="J11" t="n">
         <v>2997</v>
       </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="n">
         <v>2997</v>
       </c>
@@ -1289,15 +1322,15 @@
         <v>2997</v>
       </c>
       <c r="P11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="Q11" t="n">
         <v>929</v>
       </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="n">
-        <v>929</v>
-      </c>
+      <c r="R11" t="n">
+        <v>929</v>
+      </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="n">
         <v>929</v>
       </c>
@@ -1314,6 +1347,9 @@
         <v>929</v>
       </c>
       <c r="Y11" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1350,10 +1386,10 @@
       <c r="J12" t="n">
         <v>569</v>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="n">
-        <v>569</v>
-      </c>
+      <c r="K12" t="n">
+        <v>569</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
         <v>569</v>
       </c>
@@ -1369,10 +1405,10 @@
       <c r="Q12" t="n">
         <v>569</v>
       </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="n">
-        <v>569</v>
-      </c>
+      <c r="R12" t="n">
+        <v>569</v>
+      </c>
+      <c r="S12" t="inlineStr"/>
       <c r="T12" t="n">
         <v>569</v>
       </c>
@@ -1389,6 +1425,9 @@
         <v>569</v>
       </c>
       <c r="Y12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1419,14 +1458,14 @@
       <c r="H13" t="n">
         <v>569</v>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
-        <v>569</v>
-      </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="n">
-        <v>569</v>
-      </c>
+      <c r="I13" t="n">
+        <v>569</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>569</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
         <v>569</v>
       </c>
@@ -1442,24 +1481,27 @@
       <c r="Q13" t="n">
         <v>569</v>
       </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="n">
-        <v>569</v>
-      </c>
+      <c r="R13" t="n">
+        <v>569</v>
+      </c>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
         <v>569</v>
       </c>
       <c r="U13" t="n">
         <v>569</v>
       </c>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="n">
-        <v>569</v>
-      </c>
+      <c r="V13" t="n">
+        <v>569</v>
+      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="n">
         <v>569</v>
       </c>
       <c r="Y13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1473,7 +1515,7 @@
         <v>794</v>
       </c>
       <c r="C14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="D14" t="n">
         <v>499</v>
@@ -1490,11 +1532,11 @@
       <c r="H14" t="n">
         <v>499</v>
       </c>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>499</v>
+      </c>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="n">
-        <v>499</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
         <v>499</v>
       </c>
@@ -1535,6 +1577,9 @@
         <v>499</v>
       </c>
       <c r="Y14" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1571,10 +1616,10 @@
       <c r="J15" t="n">
         <v>499</v>
       </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="n">
-        <v>499</v>
-      </c>
+      <c r="K15" t="n">
+        <v>499</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
         <v>499</v>
       </c>
@@ -1584,14 +1629,14 @@
       <c r="O15" t="n">
         <v>499</v>
       </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="n">
-        <v>499</v>
-      </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="n">
-        <v>499</v>
-      </c>
+      <c r="P15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="n">
+        <v>499</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="n">
         <v>499</v>
       </c>
@@ -1608,6 +1653,9 @@
         <v>499</v>
       </c>
       <c r="Y15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1629,17 +1677,17 @@
       <c r="E16" t="n">
         <v>299</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>299</v>
-      </c>
+      <c r="F16" t="n">
+        <v>299</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
         <v>299</v>
       </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="n">
-        <v>299</v>
-      </c>
+      <c r="I16" t="n">
+        <v>299</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
         <v>299</v>
       </c>
@@ -1661,10 +1709,10 @@
       <c r="Q16" t="n">
         <v>299</v>
       </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="n">
-        <v>299</v>
-      </c>
+      <c r="R16" t="n">
+        <v>299</v>
+      </c>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="n">
         <v>299</v>
       </c>
@@ -1681,6 +1729,9 @@
         <v>299</v>
       </c>
       <c r="Y16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1717,10 +1768,10 @@
       <c r="J17" t="n">
         <v>929</v>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="n">
-        <v>929</v>
-      </c>
+      <c r="K17" t="n">
+        <v>929</v>
+      </c>
+      <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
         <v>929</v>
       </c>
@@ -1736,10 +1787,10 @@
       <c r="Q17" t="n">
         <v>929</v>
       </c>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="n">
-        <v>929</v>
-      </c>
+      <c r="R17" t="n">
+        <v>929</v>
+      </c>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="n">
         <v>929</v>
       </c>
@@ -1756,6 +1807,9 @@
         <v>929</v>
       </c>
       <c r="Y17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1789,11 +1843,11 @@
       <c r="I18" t="n">
         <v>499</v>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>499</v>
+      </c>
       <c r="K18" t="inlineStr"/>
-      <c r="L18" t="n">
-        <v>499</v>
-      </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
         <v>499</v>
       </c>
@@ -1809,10 +1863,10 @@
       <c r="Q18" t="n">
         <v>499</v>
       </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="n">
-        <v>499</v>
-      </c>
+      <c r="R18" t="n">
+        <v>499</v>
+      </c>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="n">
         <v>499</v>
       </c>
@@ -1829,6 +1883,9 @@
         <v>499</v>
       </c>
       <c r="Y18" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1854,7 +1911,7 @@
         <v>1299</v>
       </c>
       <c r="G19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="H19" t="n">
         <v>1497</v>
@@ -1862,13 +1919,13 @@
       <c r="I19" t="n">
         <v>1497</v>
       </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>1497</v>
+      </c>
       <c r="K19" t="inlineStr"/>
-      <c r="L19" t="n">
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="n">
         <v>465</v>
-      </c>
-      <c r="M19" t="n">
-        <v>1497</v>
       </c>
       <c r="N19" t="n">
         <v>1497</v>
@@ -1904,6 +1961,9 @@
         <v>1497</v>
       </c>
       <c r="Y19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="Z19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -1961,10 +2021,10 @@
       <c r="Q20" t="n">
         <v>929</v>
       </c>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="n">
-        <v>929</v>
-      </c>
+      <c r="R20" t="n">
+        <v>929</v>
+      </c>
+      <c r="S20" t="inlineStr"/>
       <c r="T20" t="n">
         <v>929</v>
       </c>
@@ -1981,6 +2041,9 @@
         <v>929</v>
       </c>
       <c r="Y20" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1990,9 +2053,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
         <v>499</v>
       </c>
@@ -2017,10 +2078,10 @@
       <c r="J21" t="n">
         <v>499</v>
       </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="n">
-        <v>499</v>
-      </c>
+      <c r="K21" t="n">
+        <v>499</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
         <v>499</v>
       </c>
@@ -2058,6 +2119,9 @@
         <v>499</v>
       </c>
       <c r="Y21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2088,14 +2152,14 @@
       <c r="H22" t="n">
         <v>299</v>
       </c>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="n">
-        <v>299</v>
-      </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="n">
-        <v>299</v>
-      </c>
+      <c r="I22" t="n">
+        <v>299</v>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="n">
+        <v>299</v>
+      </c>
+      <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
         <v>299</v>
       </c>
@@ -2111,10 +2175,10 @@
       <c r="Q22" t="n">
         <v>299</v>
       </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="n">
-        <v>299</v>
-      </c>
+      <c r="R22" t="n">
+        <v>299</v>
+      </c>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="n">
         <v>299</v>
       </c>
@@ -2131,6 +2195,9 @@
         <v>299</v>
       </c>
       <c r="Y22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2164,11 +2231,11 @@
       <c r="I23" t="n">
         <v>1299</v>
       </c>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>1299</v>
+      </c>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
         <v>1299</v>
       </c>
@@ -2184,10 +2251,10 @@
       <c r="Q23" t="n">
         <v>1299</v>
       </c>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="R23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="n">
         <v>1299</v>
       </c>
@@ -2204,6 +2271,9 @@
         <v>1299</v>
       </c>
       <c r="Y23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Z23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2234,11 +2304,11 @@
       <c r="H24" t="n">
         <v>929</v>
       </c>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>929</v>
+      </c>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="n">
-        <v>929</v>
-      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="n">
         <v>929</v>
       </c>
@@ -2257,10 +2327,10 @@
       <c r="Q24" t="n">
         <v>929</v>
       </c>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="n">
-        <v>929</v>
-      </c>
+      <c r="R24" t="n">
+        <v>929</v>
+      </c>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="n">
         <v>929</v>
       </c>
@@ -2277,6 +2347,9 @@
         <v>929</v>
       </c>
       <c r="Y24" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2307,11 +2380,11 @@
       <c r="H25" t="n">
         <v>929</v>
       </c>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>929</v>
+      </c>
       <c r="J25" t="inlineStr"/>
-      <c r="K25" t="n">
-        <v>929</v>
-      </c>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="n">
         <v>929</v>
       </c>
@@ -2330,10 +2403,10 @@
       <c r="Q25" t="n">
         <v>929</v>
       </c>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="n">
-        <v>929</v>
-      </c>
+      <c r="R25" t="n">
+        <v>929</v>
+      </c>
+      <c r="S25" t="inlineStr"/>
       <c r="T25" t="n">
         <v>929</v>
       </c>
@@ -2350,6 +2423,9 @@
         <v>929</v>
       </c>
       <c r="Y25" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2380,14 +2456,14 @@
       <c r="H26" t="n">
         <v>1299</v>
       </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
         <v>1299</v>
       </c>
@@ -2403,10 +2479,10 @@
       <c r="Q26" t="n">
         <v>1299</v>
       </c>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="R26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="n">
         <v>1299</v>
       </c>
@@ -2423,6 +2499,9 @@
         <v>1299</v>
       </c>
       <c r="Y26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Z26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 14:48
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,7 @@
     <col width="21" customWidth="1" min="24" max="24"/>
     <col width="21" customWidth="1" min="25" max="25"/>
     <col width="21" customWidth="1" min="26" max="26"/>
+    <col width="21" customWidth="1" min="27" max="27"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -469,125 +470,130 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 20:14</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -608,10 +614,10 @@
       <c r="D2" t="n">
         <v>929</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>929</v>
-      </c>
+      <c r="E2" t="n">
+        <v>929</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>929</v>
       </c>
@@ -624,25 +630,25 @@
       <c r="J2" t="n">
         <v>929</v>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>929</v>
+      </c>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>929</v>
-      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
         <v>929</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="n">
-        <v>929</v>
-      </c>
+      <c r="O2" t="n">
+        <v>929</v>
+      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="n">
         <v>929</v>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="n">
-        <v>929</v>
-      </c>
+      <c r="R2" t="n">
+        <v>929</v>
+      </c>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="n">
         <v>929</v>
       </c>
@@ -662,6 +668,9 @@
         <v>929</v>
       </c>
       <c r="Z2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -677,26 +686,26 @@
       <c r="C3" t="n">
         <v>569</v>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>569</v>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>569</v>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>569</v>
       </c>
       <c r="I3" t="n">
         <v>569</v>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>569</v>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>569</v>
-      </c>
+      <c r="J3" t="n">
+        <v>569</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>569</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>569</v>
       </c>
@@ -712,10 +721,10 @@
       <c r="R3" t="n">
         <v>569</v>
       </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="n">
-        <v>569</v>
-      </c>
+      <c r="S3" t="n">
+        <v>569</v>
+      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
         <v>569</v>
       </c>
@@ -732,6 +741,9 @@
         <v>569</v>
       </c>
       <c r="Z3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -765,10 +777,10 @@
       <c r="I4" t="n">
         <v>299</v>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="n">
-        <v>299</v>
-      </c>
+      <c r="J4" t="n">
+        <v>299</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="n">
         <v>299</v>
       </c>
@@ -790,10 +802,10 @@
       <c r="R4" t="n">
         <v>299</v>
       </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="n">
-        <v>299</v>
-      </c>
+      <c r="S4" t="n">
+        <v>299</v>
+      </c>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="n">
         <v>299</v>
       </c>
@@ -810,6 +822,9 @@
         <v>299</v>
       </c>
       <c r="Z4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -870,10 +885,10 @@
       <c r="R5" t="n">
         <v>569</v>
       </c>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="n">
-        <v>569</v>
-      </c>
+      <c r="S5" t="n">
+        <v>569</v>
+      </c>
+      <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
         <v>569</v>
       </c>
@@ -890,6 +905,9 @@
         <v>569</v>
       </c>
       <c r="Z5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -926,10 +944,10 @@
       <c r="J6" t="n">
         <v>499</v>
       </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>499</v>
-      </c>
+      <c r="K6" t="n">
+        <v>499</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>499</v>
       </c>
@@ -948,10 +966,10 @@
       <c r="R6" t="n">
         <v>499</v>
       </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="n">
-        <v>499</v>
-      </c>
+      <c r="S6" t="n">
+        <v>499</v>
+      </c>
+      <c r="T6" t="inlineStr"/>
       <c r="U6" t="n">
         <v>499</v>
       </c>
@@ -968,6 +986,9 @@
         <v>499</v>
       </c>
       <c r="Z6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1001,12 +1022,12 @@
       <c r="I7" t="n">
         <v>569</v>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>569</v>
+      </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="n">
-        <v>569</v>
-      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
         <v>569</v>
       </c>
@@ -1022,10 +1043,10 @@
       <c r="R7" t="n">
         <v>569</v>
       </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="n">
-        <v>569</v>
-      </c>
+      <c r="S7" t="n">
+        <v>569</v>
+      </c>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="n">
         <v>569</v>
       </c>
@@ -1042,6 +1063,9 @@
         <v>569</v>
       </c>
       <c r="Z7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1075,14 +1099,14 @@
       <c r="I8" t="n">
         <v>929</v>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>929</v>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
-        <v>929</v>
-      </c>
+      <c r="J8" t="n">
+        <v>929</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>929</v>
+      </c>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
         <v>929</v>
       </c>
@@ -1098,10 +1122,10 @@
       <c r="R8" t="n">
         <v>929</v>
       </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="n">
-        <v>929</v>
-      </c>
+      <c r="S8" t="n">
+        <v>929</v>
+      </c>
+      <c r="T8" t="inlineStr"/>
       <c r="U8" t="n">
         <v>929</v>
       </c>
@@ -1118,6 +1142,9 @@
         <v>929</v>
       </c>
       <c r="Z8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1151,10 +1178,10 @@
       <c r="I9" t="n">
         <v>299</v>
       </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="n">
-        <v>299</v>
-      </c>
+      <c r="J9" t="n">
+        <v>299</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="n">
         <v>299</v>
       </c>
@@ -1176,10 +1203,10 @@
       <c r="R9" t="n">
         <v>299</v>
       </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="n">
-        <v>299</v>
-      </c>
+      <c r="S9" t="n">
+        <v>299</v>
+      </c>
+      <c r="T9" t="inlineStr"/>
       <c r="U9" t="n">
         <v>299</v>
       </c>
@@ -1196,6 +1223,9 @@
         <v>299</v>
       </c>
       <c r="Z9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1229,14 +1259,14 @@
       <c r="I10" t="n">
         <v>299</v>
       </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>299</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
-        <v>299</v>
-      </c>
+      <c r="J10" t="n">
+        <v>299</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>299</v>
+      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
         <v>299</v>
       </c>
@@ -1252,10 +1282,10 @@
       <c r="R10" t="n">
         <v>299</v>
       </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="n">
-        <v>299</v>
-      </c>
+      <c r="S10" t="n">
+        <v>299</v>
+      </c>
+      <c r="T10" t="inlineStr"/>
       <c r="U10" t="n">
         <v>299</v>
       </c>
@@ -1272,6 +1302,9 @@
         <v>299</v>
       </c>
       <c r="Z10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1308,10 +1341,10 @@
       <c r="J11" t="n">
         <v>2997</v>
       </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="n">
+      <c r="K11" t="n">
         <v>2997</v>
       </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
         <v>2997</v>
       </c>
@@ -1325,15 +1358,15 @@
         <v>2997</v>
       </c>
       <c r="Q11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="R11" t="n">
         <v>929</v>
       </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="n">
-        <v>929</v>
-      </c>
+      <c r="S11" t="n">
+        <v>929</v>
+      </c>
+      <c r="T11" t="inlineStr"/>
       <c r="U11" t="n">
         <v>929</v>
       </c>
@@ -1350,6 +1383,9 @@
         <v>929</v>
       </c>
       <c r="Z11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1389,10 +1425,10 @@
       <c r="K12" t="n">
         <v>569</v>
       </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="n">
-        <v>569</v>
-      </c>
+      <c r="L12" t="n">
+        <v>569</v>
+      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
         <v>569</v>
       </c>
@@ -1408,10 +1444,10 @@
       <c r="R12" t="n">
         <v>569</v>
       </c>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="n">
-        <v>569</v>
-      </c>
+      <c r="S12" t="n">
+        <v>569</v>
+      </c>
+      <c r="T12" t="inlineStr"/>
       <c r="U12" t="n">
         <v>569</v>
       </c>
@@ -1428,6 +1464,9 @@
         <v>569</v>
       </c>
       <c r="Z12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1461,14 +1500,14 @@
       <c r="I13" t="n">
         <v>569</v>
       </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>569</v>
-      </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>569</v>
-      </c>
+      <c r="J13" t="n">
+        <v>569</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="n">
+        <v>569</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
         <v>569</v>
       </c>
@@ -1484,24 +1523,27 @@
       <c r="R13" t="n">
         <v>569</v>
       </c>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="n">
-        <v>569</v>
-      </c>
+      <c r="S13" t="n">
+        <v>569</v>
+      </c>
+      <c r="T13" t="inlineStr"/>
       <c r="U13" t="n">
         <v>569</v>
       </c>
       <c r="V13" t="n">
         <v>569</v>
       </c>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="n">
-        <v>569</v>
-      </c>
+      <c r="W13" t="n">
+        <v>569</v>
+      </c>
+      <c r="X13" t="inlineStr"/>
       <c r="Y13" t="n">
         <v>569</v>
       </c>
       <c r="Z13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1518,7 +1560,7 @@
         <v>794</v>
       </c>
       <c r="D14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="E14" t="n">
         <v>499</v>
@@ -1535,11 +1577,11 @@
       <c r="I14" t="n">
         <v>499</v>
       </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>499</v>
+      </c>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" t="n">
-        <v>499</v>
-      </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
         <v>499</v>
       </c>
@@ -1580,6 +1622,9 @@
         <v>499</v>
       </c>
       <c r="Z14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1619,10 +1664,10 @@
       <c r="K15" t="n">
         <v>499</v>
       </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="n">
-        <v>499</v>
-      </c>
+      <c r="L15" t="n">
+        <v>499</v>
+      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
         <v>499</v>
       </c>
@@ -1632,14 +1677,14 @@
       <c r="P15" t="n">
         <v>499</v>
       </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="n">
-        <v>499</v>
-      </c>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q15" t="n">
+        <v>499</v>
+      </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="n">
+        <v>499</v>
+      </c>
+      <c r="T15" t="inlineStr"/>
       <c r="U15" t="n">
         <v>499</v>
       </c>
@@ -1656,6 +1701,9 @@
         <v>499</v>
       </c>
       <c r="Z15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1680,17 +1728,17 @@
       <c r="F16" t="n">
         <v>299</v>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="n">
-        <v>299</v>
-      </c>
+      <c r="G16" t="n">
+        <v>299</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
         <v>299</v>
       </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="n">
-        <v>299</v>
-      </c>
+      <c r="J16" t="n">
+        <v>299</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="n">
         <v>299</v>
       </c>
@@ -1712,10 +1760,10 @@
       <c r="R16" t="n">
         <v>299</v>
       </c>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="n">
-        <v>299</v>
-      </c>
+      <c r="S16" t="n">
+        <v>299</v>
+      </c>
+      <c r="T16" t="inlineStr"/>
       <c r="U16" t="n">
         <v>299</v>
       </c>
@@ -1732,6 +1780,9 @@
         <v>299</v>
       </c>
       <c r="Z16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1771,10 +1822,10 @@
       <c r="K17" t="n">
         <v>929</v>
       </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="n">
-        <v>929</v>
-      </c>
+      <c r="L17" t="n">
+        <v>929</v>
+      </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
         <v>929</v>
       </c>
@@ -1790,10 +1841,10 @@
       <c r="R17" t="n">
         <v>929</v>
       </c>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="n">
-        <v>929</v>
-      </c>
+      <c r="S17" t="n">
+        <v>929</v>
+      </c>
+      <c r="T17" t="inlineStr"/>
       <c r="U17" t="n">
         <v>929</v>
       </c>
@@ -1810,6 +1861,9 @@
         <v>929</v>
       </c>
       <c r="Z17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1846,11 +1900,11 @@
       <c r="J18" t="n">
         <v>499</v>
       </c>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>499</v>
+      </c>
       <c r="L18" t="inlineStr"/>
-      <c r="M18" t="n">
-        <v>499</v>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
         <v>499</v>
       </c>
@@ -1866,10 +1920,10 @@
       <c r="R18" t="n">
         <v>499</v>
       </c>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="n">
-        <v>499</v>
-      </c>
+      <c r="S18" t="n">
+        <v>499</v>
+      </c>
+      <c r="T18" t="inlineStr"/>
       <c r="U18" t="n">
         <v>499</v>
       </c>
@@ -1886,6 +1940,9 @@
         <v>499</v>
       </c>
       <c r="Z18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1914,7 +1971,7 @@
         <v>1299</v>
       </c>
       <c r="H19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="I19" t="n">
         <v>1497</v>
@@ -1922,13 +1979,13 @@
       <c r="J19" t="n">
         <v>1497</v>
       </c>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="n">
+        <v>1497</v>
+      </c>
       <c r="L19" t="inlineStr"/>
-      <c r="M19" t="n">
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="n">
         <v>465</v>
-      </c>
-      <c r="N19" t="n">
-        <v>1497</v>
       </c>
       <c r="O19" t="n">
         <v>1497</v>
@@ -1964,6 +2021,9 @@
         <v>1497</v>
       </c>
       <c r="Z19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AA19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2024,10 +2084,10 @@
       <c r="R20" t="n">
         <v>929</v>
       </c>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="n">
-        <v>929</v>
-      </c>
+      <c r="S20" t="n">
+        <v>929</v>
+      </c>
+      <c r="T20" t="inlineStr"/>
       <c r="U20" t="n">
         <v>929</v>
       </c>
@@ -2044,6 +2104,9 @@
         <v>929</v>
       </c>
       <c r="Z20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2053,10 +2116,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="n">
+        <v>499</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>499</v>
       </c>
@@ -2081,10 +2144,10 @@
       <c r="K21" t="n">
         <v>499</v>
       </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="n">
-        <v>499</v>
-      </c>
+      <c r="L21" t="n">
+        <v>499</v>
+      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
         <v>499</v>
       </c>
@@ -2122,6 +2185,9 @@
         <v>499</v>
       </c>
       <c r="Z21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2155,14 +2221,14 @@
       <c r="I22" t="n">
         <v>299</v>
       </c>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="n">
-        <v>299</v>
-      </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="n">
-        <v>299</v>
-      </c>
+      <c r="J22" t="n">
+        <v>299</v>
+      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="n">
+        <v>299</v>
+      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
         <v>299</v>
       </c>
@@ -2178,10 +2244,10 @@
       <c r="R22" t="n">
         <v>299</v>
       </c>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="n">
-        <v>299</v>
-      </c>
+      <c r="S22" t="n">
+        <v>299</v>
+      </c>
+      <c r="T22" t="inlineStr"/>
       <c r="U22" t="n">
         <v>299</v>
       </c>
@@ -2198,6 +2264,9 @@
         <v>299</v>
       </c>
       <c r="Z22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2234,11 +2303,11 @@
       <c r="J23" t="n">
         <v>1299</v>
       </c>
-      <c r="K23" t="inlineStr"/>
+      <c r="K23" t="n">
+        <v>1299</v>
+      </c>
       <c r="L23" t="inlineStr"/>
-      <c r="M23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="M23" t="inlineStr"/>
       <c r="N23" t="n">
         <v>1299</v>
       </c>
@@ -2254,10 +2323,10 @@
       <c r="R23" t="n">
         <v>1299</v>
       </c>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="S23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="T23" t="inlineStr"/>
       <c r="U23" t="n">
         <v>1299</v>
       </c>
@@ -2274,6 +2343,9 @@
         <v>1299</v>
       </c>
       <c r="Z23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AA23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2307,11 +2379,11 @@
       <c r="I24" t="n">
         <v>929</v>
       </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>929</v>
+      </c>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="n">
-        <v>929</v>
-      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
         <v>929</v>
       </c>
@@ -2330,10 +2402,10 @@
       <c r="R24" t="n">
         <v>929</v>
       </c>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="n">
-        <v>929</v>
-      </c>
+      <c r="S24" t="n">
+        <v>929</v>
+      </c>
+      <c r="T24" t="inlineStr"/>
       <c r="U24" t="n">
         <v>929</v>
       </c>
@@ -2350,6 +2422,9 @@
         <v>929</v>
       </c>
       <c r="Z24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2383,11 +2458,11 @@
       <c r="I25" t="n">
         <v>929</v>
       </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>929</v>
+      </c>
       <c r="K25" t="inlineStr"/>
-      <c r="L25" t="n">
-        <v>929</v>
-      </c>
+      <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
         <v>929</v>
       </c>
@@ -2406,10 +2481,10 @@
       <c r="R25" t="n">
         <v>929</v>
       </c>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="n">
-        <v>929</v>
-      </c>
+      <c r="S25" t="n">
+        <v>929</v>
+      </c>
+      <c r="T25" t="inlineStr"/>
       <c r="U25" t="n">
         <v>929</v>
       </c>
@@ -2426,6 +2501,9 @@
         <v>929</v>
       </c>
       <c r="Z25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2459,14 +2537,14 @@
       <c r="I26" t="n">
         <v>1299</v>
       </c>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="J26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="M26" t="inlineStr"/>
       <c r="N26" t="n">
         <v>1299</v>
       </c>
@@ -2482,10 +2560,10 @@
       <c r="R26" t="n">
         <v>1299</v>
       </c>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="S26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="T26" t="inlineStr"/>
       <c r="U26" t="n">
         <v>1299</v>
       </c>
@@ -2502,6 +2580,9 @@
         <v>1299</v>
       </c>
       <c r="Z26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AA26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 16:59
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA26"/>
+  <dimension ref="A1:AB26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,7 @@
     <col width="21" customWidth="1" min="25" max="25"/>
     <col width="21" customWidth="1" min="26" max="26"/>
     <col width="21" customWidth="1" min="27" max="27"/>
+    <col width="21" customWidth="1" min="28" max="28"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -470,130 +471,135 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-22 22:24</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -617,10 +623,10 @@
       <c r="E2" t="n">
         <v>929</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>929</v>
-      </c>
+      <c r="F2" t="n">
+        <v>929</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>929</v>
       </c>
@@ -633,25 +639,25 @@
       <c r="K2" t="n">
         <v>929</v>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>929</v>
+      </c>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="n">
-        <v>929</v>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
         <v>929</v>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="n">
-        <v>929</v>
-      </c>
+      <c r="P2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
         <v>929</v>
       </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="n">
-        <v>929</v>
-      </c>
+      <c r="S2" t="n">
+        <v>929</v>
+      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
         <v>929</v>
       </c>
@@ -671,6 +677,9 @@
         <v>929</v>
       </c>
       <c r="AA2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -689,26 +698,26 @@
       <c r="D3" t="n">
         <v>569</v>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>569</v>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>569</v>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>569</v>
       </c>
       <c r="J3" t="n">
         <v>569</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
-        <v>569</v>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="n">
-        <v>569</v>
-      </c>
+      <c r="K3" t="n">
+        <v>569</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>569</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="n">
         <v>569</v>
       </c>
@@ -724,10 +733,10 @@
       <c r="S3" t="n">
         <v>569</v>
       </c>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
-        <v>569</v>
-      </c>
+      <c r="T3" t="n">
+        <v>569</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
       <c r="V3" t="n">
         <v>569</v>
       </c>
@@ -744,6 +753,9 @@
         <v>569</v>
       </c>
       <c r="AA3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -780,10 +792,10 @@
       <c r="J4" t="n">
         <v>299</v>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="n">
-        <v>299</v>
-      </c>
+      <c r="K4" t="n">
+        <v>299</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>299</v>
       </c>
@@ -805,10 +817,10 @@
       <c r="S4" t="n">
         <v>299</v>
       </c>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="n">
-        <v>299</v>
-      </c>
+      <c r="T4" t="n">
+        <v>299</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
       <c r="V4" t="n">
         <v>299</v>
       </c>
@@ -825,6 +837,9 @@
         <v>299</v>
       </c>
       <c r="AA4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -888,10 +903,10 @@
       <c r="S5" t="n">
         <v>569</v>
       </c>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="n">
-        <v>569</v>
-      </c>
+      <c r="T5" t="n">
+        <v>569</v>
+      </c>
+      <c r="U5" t="inlineStr"/>
       <c r="V5" t="n">
         <v>569</v>
       </c>
@@ -908,6 +923,9 @@
         <v>569</v>
       </c>
       <c r="AA5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -947,10 +965,10 @@
       <c r="K6" t="n">
         <v>499</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>499</v>
-      </c>
+      <c r="L6" t="n">
+        <v>499</v>
+      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
         <v>499</v>
       </c>
@@ -969,10 +987,10 @@
       <c r="S6" t="n">
         <v>499</v>
       </c>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="n">
-        <v>499</v>
-      </c>
+      <c r="T6" t="n">
+        <v>499</v>
+      </c>
+      <c r="U6" t="inlineStr"/>
       <c r="V6" t="n">
         <v>499</v>
       </c>
@@ -989,6 +1007,9 @@
         <v>499</v>
       </c>
       <c r="AA6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1025,12 +1046,12 @@
       <c r="J7" t="n">
         <v>569</v>
       </c>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>569</v>
+      </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
-        <v>569</v>
-      </c>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
         <v>569</v>
       </c>
@@ -1046,10 +1067,10 @@
       <c r="S7" t="n">
         <v>569</v>
       </c>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="n">
-        <v>569</v>
-      </c>
+      <c r="T7" t="n">
+        <v>569</v>
+      </c>
+      <c r="U7" t="inlineStr"/>
       <c r="V7" t="n">
         <v>569</v>
       </c>
@@ -1066,6 +1087,9 @@
         <v>569</v>
       </c>
       <c r="AA7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1102,14 +1126,14 @@
       <c r="J8" t="n">
         <v>929</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="n">
-        <v>929</v>
-      </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="n">
-        <v>929</v>
-      </c>
+      <c r="K8" t="n">
+        <v>929</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>929</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
         <v>929</v>
       </c>
@@ -1125,10 +1149,10 @@
       <c r="S8" t="n">
         <v>929</v>
       </c>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="n">
-        <v>929</v>
-      </c>
+      <c r="T8" t="n">
+        <v>929</v>
+      </c>
+      <c r="U8" t="inlineStr"/>
       <c r="V8" t="n">
         <v>929</v>
       </c>
@@ -1145,6 +1169,9 @@
         <v>929</v>
       </c>
       <c r="AA8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1181,10 +1208,10 @@
       <c r="J9" t="n">
         <v>299</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="n">
-        <v>299</v>
-      </c>
+      <c r="K9" t="n">
+        <v>299</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
         <v>299</v>
       </c>
@@ -1206,10 +1233,10 @@
       <c r="S9" t="n">
         <v>299</v>
       </c>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="n">
-        <v>299</v>
-      </c>
+      <c r="T9" t="n">
+        <v>299</v>
+      </c>
+      <c r="U9" t="inlineStr"/>
       <c r="V9" t="n">
         <v>299</v>
       </c>
@@ -1226,6 +1253,9 @@
         <v>299</v>
       </c>
       <c r="AA9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1235,9 +1265,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
         <v>299</v>
       </c>
@@ -1262,14 +1290,14 @@
       <c r="J10" t="n">
         <v>299</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
-        <v>299</v>
-      </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="n">
-        <v>299</v>
-      </c>
+      <c r="K10" t="n">
+        <v>299</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>299</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
         <v>299</v>
       </c>
@@ -1285,10 +1313,10 @@
       <c r="S10" t="n">
         <v>299</v>
       </c>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="n">
-        <v>299</v>
-      </c>
+      <c r="T10" t="n">
+        <v>299</v>
+      </c>
+      <c r="U10" t="inlineStr"/>
       <c r="V10" t="n">
         <v>299</v>
       </c>
@@ -1305,6 +1333,9 @@
         <v>299</v>
       </c>
       <c r="AA10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1344,10 +1375,10 @@
       <c r="K11" t="n">
         <v>2997</v>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="n">
+      <c r="L11" t="n">
         <v>2997</v>
       </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
         <v>2997</v>
       </c>
@@ -1361,15 +1392,15 @@
         <v>2997</v>
       </c>
       <c r="R11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="S11" t="n">
         <v>929</v>
       </c>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="n">
-        <v>929</v>
-      </c>
+      <c r="T11" t="n">
+        <v>929</v>
+      </c>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="n">
         <v>929</v>
       </c>
@@ -1386,6 +1417,9 @@
         <v>929</v>
       </c>
       <c r="AA11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1428,10 +1462,10 @@
       <c r="L12" t="n">
         <v>569</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="n">
-        <v>569</v>
-      </c>
+      <c r="M12" t="n">
+        <v>569</v>
+      </c>
+      <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
         <v>569</v>
       </c>
@@ -1447,10 +1481,10 @@
       <c r="S12" t="n">
         <v>569</v>
       </c>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="n">
-        <v>569</v>
-      </c>
+      <c r="T12" t="n">
+        <v>569</v>
+      </c>
+      <c r="U12" t="inlineStr"/>
       <c r="V12" t="n">
         <v>569</v>
       </c>
@@ -1467,6 +1501,9 @@
         <v>569</v>
       </c>
       <c r="AA12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1503,14 +1540,14 @@
       <c r="J13" t="n">
         <v>569</v>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="n">
-        <v>569</v>
-      </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="n">
-        <v>569</v>
-      </c>
+      <c r="K13" t="n">
+        <v>569</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="n">
+        <v>569</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
         <v>569</v>
       </c>
@@ -1526,24 +1563,27 @@
       <c r="S13" t="n">
         <v>569</v>
       </c>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="n">
-        <v>569</v>
-      </c>
+      <c r="T13" t="n">
+        <v>569</v>
+      </c>
+      <c r="U13" t="inlineStr"/>
       <c r="V13" t="n">
         <v>569</v>
       </c>
       <c r="W13" t="n">
         <v>569</v>
       </c>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="n">
-        <v>569</v>
-      </c>
+      <c r="X13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="n">
         <v>569</v>
       </c>
       <c r="AA13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1553,9 +1593,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>794</v>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
         <v>794</v>
       </c>
@@ -1563,7 +1601,7 @@
         <v>794</v>
       </c>
       <c r="E14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="F14" t="n">
         <v>499</v>
@@ -1580,11 +1618,11 @@
       <c r="J14" t="n">
         <v>499</v>
       </c>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>499</v>
+      </c>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="n">
-        <v>499</v>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
         <v>499</v>
       </c>
@@ -1625,6 +1663,9 @@
         <v>499</v>
       </c>
       <c r="AA14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1667,10 +1708,10 @@
       <c r="L15" t="n">
         <v>499</v>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="n">
-        <v>499</v>
-      </c>
+      <c r="M15" t="n">
+        <v>499</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
         <v>499</v>
       </c>
@@ -1680,14 +1721,14 @@
       <c r="Q15" t="n">
         <v>499</v>
       </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="n">
-        <v>499</v>
-      </c>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="n">
-        <v>499</v>
-      </c>
+      <c r="R15" t="n">
+        <v>499</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="n">
+        <v>499</v>
+      </c>
+      <c r="U15" t="inlineStr"/>
       <c r="V15" t="n">
         <v>499</v>
       </c>
@@ -1704,6 +1745,9 @@
         <v>499</v>
       </c>
       <c r="AA15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1731,17 +1775,17 @@
       <c r="G16" t="n">
         <v>299</v>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>299</v>
-      </c>
+      <c r="H16" t="n">
+        <v>299</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
         <v>299</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="n">
-        <v>299</v>
-      </c>
+      <c r="K16" t="n">
+        <v>299</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
         <v>299</v>
       </c>
@@ -1763,10 +1807,10 @@
       <c r="S16" t="n">
         <v>299</v>
       </c>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="n">
-        <v>299</v>
-      </c>
+      <c r="T16" t="n">
+        <v>299</v>
+      </c>
+      <c r="U16" t="inlineStr"/>
       <c r="V16" t="n">
         <v>299</v>
       </c>
@@ -1783,6 +1827,9 @@
         <v>299</v>
       </c>
       <c r="AA16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1825,10 +1872,10 @@
       <c r="L17" t="n">
         <v>929</v>
       </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="n">
-        <v>929</v>
-      </c>
+      <c r="M17" t="n">
+        <v>929</v>
+      </c>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
         <v>929</v>
       </c>
@@ -1844,10 +1891,10 @@
       <c r="S17" t="n">
         <v>929</v>
       </c>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="n">
-        <v>929</v>
-      </c>
+      <c r="T17" t="n">
+        <v>929</v>
+      </c>
+      <c r="U17" t="inlineStr"/>
       <c r="V17" t="n">
         <v>929</v>
       </c>
@@ -1864,6 +1911,9 @@
         <v>929</v>
       </c>
       <c r="AA17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1903,11 +1953,11 @@
       <c r="K18" t="n">
         <v>499</v>
       </c>
-      <c r="L18" t="inlineStr"/>
+      <c r="L18" t="n">
+        <v>499</v>
+      </c>
       <c r="M18" t="inlineStr"/>
-      <c r="N18" t="n">
-        <v>499</v>
-      </c>
+      <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
         <v>499</v>
       </c>
@@ -1923,10 +1973,10 @@
       <c r="S18" t="n">
         <v>499</v>
       </c>
-      <c r="T18" t="inlineStr"/>
-      <c r="U18" t="n">
-        <v>499</v>
-      </c>
+      <c r="T18" t="n">
+        <v>499</v>
+      </c>
+      <c r="U18" t="inlineStr"/>
       <c r="V18" t="n">
         <v>499</v>
       </c>
@@ -1943,6 +1993,9 @@
         <v>499</v>
       </c>
       <c r="AA18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1974,7 +2027,7 @@
         <v>1299</v>
       </c>
       <c r="I19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="J19" t="n">
         <v>1497</v>
@@ -1982,13 +2035,13 @@
       <c r="K19" t="n">
         <v>1497</v>
       </c>
-      <c r="L19" t="inlineStr"/>
+      <c r="L19" t="n">
+        <v>1497</v>
+      </c>
       <c r="M19" t="inlineStr"/>
-      <c r="N19" t="n">
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="n">
         <v>465</v>
-      </c>
-      <c r="O19" t="n">
-        <v>1497</v>
       </c>
       <c r="P19" t="n">
         <v>1497</v>
@@ -2024,6 +2077,9 @@
         <v>1497</v>
       </c>
       <c r="AA19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AB19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2087,10 +2143,10 @@
       <c r="S20" t="n">
         <v>929</v>
       </c>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="n">
-        <v>929</v>
-      </c>
+      <c r="T20" t="n">
+        <v>929</v>
+      </c>
+      <c r="U20" t="inlineStr"/>
       <c r="V20" t="n">
         <v>929</v>
       </c>
@@ -2107,6 +2163,9 @@
         <v>929</v>
       </c>
       <c r="AA20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2119,10 +2178,10 @@
       <c r="B21" t="n">
         <v>499</v>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
-        <v>499</v>
-      </c>
+      <c r="C21" t="n">
+        <v>499</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
         <v>499</v>
       </c>
@@ -2147,10 +2206,10 @@
       <c r="L21" t="n">
         <v>499</v>
       </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="n">
-        <v>499</v>
-      </c>
+      <c r="M21" t="n">
+        <v>499</v>
+      </c>
+      <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
         <v>499</v>
       </c>
@@ -2188,6 +2247,9 @@
         <v>499</v>
       </c>
       <c r="AA21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2224,14 +2286,14 @@
       <c r="J22" t="n">
         <v>299</v>
       </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="n">
-        <v>299</v>
-      </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="n">
-        <v>299</v>
-      </c>
+      <c r="K22" t="n">
+        <v>299</v>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="n">
+        <v>299</v>
+      </c>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
         <v>299</v>
       </c>
@@ -2247,10 +2309,10 @@
       <c r="S22" t="n">
         <v>299</v>
       </c>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="n">
-        <v>299</v>
-      </c>
+      <c r="T22" t="n">
+        <v>299</v>
+      </c>
+      <c r="U22" t="inlineStr"/>
       <c r="V22" t="n">
         <v>299</v>
       </c>
@@ -2267,6 +2329,9 @@
         <v>299</v>
       </c>
       <c r="AA22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2306,11 +2371,11 @@
       <c r="K23" t="n">
         <v>1299</v>
       </c>
-      <c r="L23" t="inlineStr"/>
+      <c r="L23" t="n">
+        <v>1299</v>
+      </c>
       <c r="M23" t="inlineStr"/>
-      <c r="N23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
         <v>1299</v>
       </c>
@@ -2326,10 +2391,10 @@
       <c r="S23" t="n">
         <v>1299</v>
       </c>
-      <c r="T23" t="inlineStr"/>
-      <c r="U23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="T23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="U23" t="inlineStr"/>
       <c r="V23" t="n">
         <v>1299</v>
       </c>
@@ -2346,6 +2411,9 @@
         <v>1299</v>
       </c>
       <c r="AA23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AB23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2382,11 +2450,11 @@
       <c r="J24" t="n">
         <v>929</v>
       </c>
-      <c r="K24" t="inlineStr"/>
+      <c r="K24" t="n">
+        <v>929</v>
+      </c>
       <c r="L24" t="inlineStr"/>
-      <c r="M24" t="n">
-        <v>929</v>
-      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
         <v>929</v>
       </c>
@@ -2405,10 +2473,10 @@
       <c r="S24" t="n">
         <v>929</v>
       </c>
-      <c r="T24" t="inlineStr"/>
-      <c r="U24" t="n">
-        <v>929</v>
-      </c>
+      <c r="T24" t="n">
+        <v>929</v>
+      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="n">
         <v>929</v>
       </c>
@@ -2425,6 +2493,9 @@
         <v>929</v>
       </c>
       <c r="AA24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2461,11 +2532,11 @@
       <c r="J25" t="n">
         <v>929</v>
       </c>
-      <c r="K25" t="inlineStr"/>
+      <c r="K25" t="n">
+        <v>929</v>
+      </c>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="n">
-        <v>929</v>
-      </c>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
         <v>929</v>
       </c>
@@ -2484,10 +2555,10 @@
       <c r="S25" t="n">
         <v>929</v>
       </c>
-      <c r="T25" t="inlineStr"/>
-      <c r="U25" t="n">
-        <v>929</v>
-      </c>
+      <c r="T25" t="n">
+        <v>929</v>
+      </c>
+      <c r="U25" t="inlineStr"/>
       <c r="V25" t="n">
         <v>929</v>
       </c>
@@ -2504,6 +2575,9 @@
         <v>929</v>
       </c>
       <c r="AA25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2540,14 +2614,14 @@
       <c r="J26" t="n">
         <v>1299</v>
       </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="K26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
         <v>1299</v>
       </c>
@@ -2563,10 +2637,10 @@
       <c r="S26" t="n">
         <v>1299</v>
       </c>
-      <c r="T26" t="inlineStr"/>
-      <c r="U26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="T26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="U26" t="inlineStr"/>
       <c r="V26" t="n">
         <v>1299</v>
       </c>
@@ -2583,6 +2657,9 @@
         <v>1299</v>
       </c>
       <c r="AA26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AB26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 19:03
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,7 @@
     <col width="21" customWidth="1" min="26" max="26"/>
     <col width="21" customWidth="1" min="27" max="27"/>
     <col width="21" customWidth="1" min="28" max="28"/>
+    <col width="21" customWidth="1" min="29" max="29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -471,135 +472,140 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 00:28</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -626,10 +632,10 @@
       <c r="F2" t="n">
         <v>929</v>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>929</v>
-      </c>
+      <c r="G2" t="n">
+        <v>929</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>929</v>
       </c>
@@ -642,25 +648,25 @@
       <c r="L2" t="n">
         <v>929</v>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>929</v>
+      </c>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="n">
-        <v>929</v>
-      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
         <v>929</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q2" t="n">
+        <v>929</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
         <v>929</v>
       </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
-        <v>929</v>
-      </c>
+      <c r="T2" t="n">
+        <v>929</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="n">
         <v>929</v>
       </c>
@@ -680,6 +686,9 @@
         <v>929</v>
       </c>
       <c r="AB2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -701,26 +710,26 @@
       <c r="E3" t="n">
         <v>569</v>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>569</v>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>569</v>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
         <v>569</v>
       </c>
       <c r="K3" t="n">
         <v>569</v>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>569</v>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
-        <v>569</v>
-      </c>
+      <c r="L3" t="n">
+        <v>569</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="n">
+        <v>569</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
         <v>569</v>
       </c>
@@ -736,10 +745,10 @@
       <c r="T3" t="n">
         <v>569</v>
       </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="n">
-        <v>569</v>
-      </c>
+      <c r="U3" t="n">
+        <v>569</v>
+      </c>
+      <c r="V3" t="inlineStr"/>
       <c r="W3" t="n">
         <v>569</v>
       </c>
@@ -756,6 +765,9 @@
         <v>569</v>
       </c>
       <c r="AB3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -795,10 +807,10 @@
       <c r="K4" t="n">
         <v>299</v>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>299</v>
-      </c>
+      <c r="L4" t="n">
+        <v>299</v>
+      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
         <v>299</v>
       </c>
@@ -820,10 +832,10 @@
       <c r="T4" t="n">
         <v>299</v>
       </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="n">
-        <v>299</v>
-      </c>
+      <c r="U4" t="n">
+        <v>299</v>
+      </c>
+      <c r="V4" t="inlineStr"/>
       <c r="W4" t="n">
         <v>299</v>
       </c>
@@ -840,6 +852,9 @@
         <v>299</v>
       </c>
       <c r="AB4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -906,10 +921,10 @@
       <c r="T5" t="n">
         <v>569</v>
       </c>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="n">
-        <v>569</v>
-      </c>
+      <c r="U5" t="n">
+        <v>569</v>
+      </c>
+      <c r="V5" t="inlineStr"/>
       <c r="W5" t="n">
         <v>569</v>
       </c>
@@ -926,6 +941,9 @@
         <v>569</v>
       </c>
       <c r="AB5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -968,10 +986,10 @@
       <c r="L6" t="n">
         <v>499</v>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="n">
-        <v>499</v>
-      </c>
+      <c r="M6" t="n">
+        <v>499</v>
+      </c>
+      <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
         <v>499</v>
       </c>
@@ -990,10 +1008,10 @@
       <c r="T6" t="n">
         <v>499</v>
       </c>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="n">
-        <v>499</v>
-      </c>
+      <c r="U6" t="n">
+        <v>499</v>
+      </c>
+      <c r="V6" t="inlineStr"/>
       <c r="W6" t="n">
         <v>499</v>
       </c>
@@ -1010,6 +1028,9 @@
         <v>499</v>
       </c>
       <c r="AB6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1049,12 +1070,12 @@
       <c r="K7" t="n">
         <v>569</v>
       </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>569</v>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="n">
-        <v>569</v>
-      </c>
+      <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
         <v>569</v>
       </c>
@@ -1070,10 +1091,10 @@
       <c r="T7" t="n">
         <v>569</v>
       </c>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="n">
-        <v>569</v>
-      </c>
+      <c r="U7" t="n">
+        <v>569</v>
+      </c>
+      <c r="V7" t="inlineStr"/>
       <c r="W7" t="n">
         <v>569</v>
       </c>
@@ -1090,6 +1111,9 @@
         <v>569</v>
       </c>
       <c r="AB7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1129,14 +1153,14 @@
       <c r="K8" t="n">
         <v>929</v>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
-        <v>929</v>
-      </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="n">
-        <v>929</v>
-      </c>
+      <c r="L8" t="n">
+        <v>929</v>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="n">
+        <v>929</v>
+      </c>
+      <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
         <v>929</v>
       </c>
@@ -1152,10 +1176,10 @@
       <c r="T8" t="n">
         <v>929</v>
       </c>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="n">
-        <v>929</v>
-      </c>
+      <c r="U8" t="n">
+        <v>929</v>
+      </c>
+      <c r="V8" t="inlineStr"/>
       <c r="W8" t="n">
         <v>929</v>
       </c>
@@ -1172,6 +1196,9 @@
         <v>929</v>
       </c>
       <c r="AB8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1211,10 +1238,10 @@
       <c r="K9" t="n">
         <v>299</v>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="n">
-        <v>299</v>
-      </c>
+      <c r="L9" t="n">
+        <v>299</v>
+      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
         <v>299</v>
       </c>
@@ -1236,10 +1263,10 @@
       <c r="T9" t="n">
         <v>299</v>
       </c>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="n">
-        <v>299</v>
-      </c>
+      <c r="U9" t="n">
+        <v>299</v>
+      </c>
+      <c r="V9" t="inlineStr"/>
       <c r="W9" t="n">
         <v>299</v>
       </c>
@@ -1256,6 +1283,9 @@
         <v>299</v>
       </c>
       <c r="AB9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1265,10 +1295,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="n">
+        <v>299</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>299</v>
       </c>
@@ -1293,14 +1323,14 @@
       <c r="K10" t="n">
         <v>299</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
-        <v>299</v>
-      </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="n">
-        <v>299</v>
-      </c>
+      <c r="L10" t="n">
+        <v>299</v>
+      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="n">
+        <v>299</v>
+      </c>
+      <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
         <v>299</v>
       </c>
@@ -1316,10 +1346,10 @@
       <c r="T10" t="n">
         <v>299</v>
       </c>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="n">
-        <v>299</v>
-      </c>
+      <c r="U10" t="n">
+        <v>299</v>
+      </c>
+      <c r="V10" t="inlineStr"/>
       <c r="W10" t="n">
         <v>299</v>
       </c>
@@ -1336,6 +1366,9 @@
         <v>299</v>
       </c>
       <c r="AB10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1378,10 +1411,10 @@
       <c r="L11" t="n">
         <v>2997</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="n">
+      <c r="M11" t="n">
         <v>2997</v>
       </c>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
         <v>2997</v>
       </c>
@@ -1395,15 +1428,15 @@
         <v>2997</v>
       </c>
       <c r="S11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="T11" t="n">
         <v>929</v>
       </c>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="n">
-        <v>929</v>
-      </c>
+      <c r="U11" t="n">
+        <v>929</v>
+      </c>
+      <c r="V11" t="inlineStr"/>
       <c r="W11" t="n">
         <v>929</v>
       </c>
@@ -1420,6 +1453,9 @@
         <v>929</v>
       </c>
       <c r="AB11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1465,10 +1501,10 @@
       <c r="M12" t="n">
         <v>569</v>
       </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="n">
-        <v>569</v>
-      </c>
+      <c r="N12" t="n">
+        <v>569</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
         <v>569</v>
       </c>
@@ -1484,10 +1520,10 @@
       <c r="T12" t="n">
         <v>569</v>
       </c>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="n">
-        <v>569</v>
-      </c>
+      <c r="U12" t="n">
+        <v>569</v>
+      </c>
+      <c r="V12" t="inlineStr"/>
       <c r="W12" t="n">
         <v>569</v>
       </c>
@@ -1504,6 +1540,9 @@
         <v>569</v>
       </c>
       <c r="AB12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1543,14 +1582,14 @@
       <c r="K13" t="n">
         <v>569</v>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>569</v>
-      </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="n">
-        <v>569</v>
-      </c>
+      <c r="L13" t="n">
+        <v>569</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="n">
+        <v>569</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
         <v>569</v>
       </c>
@@ -1566,24 +1605,27 @@
       <c r="T13" t="n">
         <v>569</v>
       </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="n">
-        <v>569</v>
-      </c>
+      <c r="U13" t="n">
+        <v>569</v>
+      </c>
+      <c r="V13" t="inlineStr"/>
       <c r="W13" t="n">
         <v>569</v>
       </c>
       <c r="X13" t="n">
         <v>569</v>
       </c>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
         <v>569</v>
       </c>
       <c r="AB13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1593,10 +1635,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="n">
+      <c r="B14" t="n">
         <v>794</v>
       </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
         <v>794</v>
       </c>
@@ -1604,7 +1646,7 @@
         <v>794</v>
       </c>
       <c r="F14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="G14" t="n">
         <v>499</v>
@@ -1621,11 +1663,11 @@
       <c r="K14" t="n">
         <v>499</v>
       </c>
-      <c r="L14" t="inlineStr"/>
+      <c r="L14" t="n">
+        <v>499</v>
+      </c>
       <c r="M14" t="inlineStr"/>
-      <c r="N14" t="n">
-        <v>499</v>
-      </c>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
         <v>499</v>
       </c>
@@ -1666,6 +1708,9 @@
         <v>499</v>
       </c>
       <c r="AB14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1711,10 +1756,10 @@
       <c r="M15" t="n">
         <v>499</v>
       </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="n">
-        <v>499</v>
-      </c>
+      <c r="N15" t="n">
+        <v>499</v>
+      </c>
+      <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
         <v>499</v>
       </c>
@@ -1724,14 +1769,14 @@
       <c r="R15" t="n">
         <v>499</v>
       </c>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="n">
-        <v>499</v>
-      </c>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="n">
-        <v>499</v>
-      </c>
+      <c r="S15" t="n">
+        <v>499</v>
+      </c>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="n">
+        <v>499</v>
+      </c>
+      <c r="V15" t="inlineStr"/>
       <c r="W15" t="n">
         <v>499</v>
       </c>
@@ -1748,6 +1793,9 @@
         <v>499</v>
       </c>
       <c r="AB15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1778,17 +1826,17 @@
       <c r="H16" t="n">
         <v>299</v>
       </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="n">
-        <v>299</v>
-      </c>
+      <c r="I16" t="n">
+        <v>299</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
         <v>299</v>
       </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="n">
-        <v>299</v>
-      </c>
+      <c r="L16" t="n">
+        <v>299</v>
+      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
         <v>299</v>
       </c>
@@ -1810,10 +1858,10 @@
       <c r="T16" t="n">
         <v>299</v>
       </c>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="n">
-        <v>299</v>
-      </c>
+      <c r="U16" t="n">
+        <v>299</v>
+      </c>
+      <c r="V16" t="inlineStr"/>
       <c r="W16" t="n">
         <v>299</v>
       </c>
@@ -1830,6 +1878,9 @@
         <v>299</v>
       </c>
       <c r="AB16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1875,10 +1926,10 @@
       <c r="M17" t="n">
         <v>929</v>
       </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="n">
-        <v>929</v>
-      </c>
+      <c r="N17" t="n">
+        <v>929</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
         <v>929</v>
       </c>
@@ -1894,10 +1945,10 @@
       <c r="T17" t="n">
         <v>929</v>
       </c>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="n">
-        <v>929</v>
-      </c>
+      <c r="U17" t="n">
+        <v>929</v>
+      </c>
+      <c r="V17" t="inlineStr"/>
       <c r="W17" t="n">
         <v>929</v>
       </c>
@@ -1914,6 +1965,9 @@
         <v>929</v>
       </c>
       <c r="AB17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1956,11 +2010,11 @@
       <c r="L18" t="n">
         <v>499</v>
       </c>
-      <c r="M18" t="inlineStr"/>
+      <c r="M18" t="n">
+        <v>499</v>
+      </c>
       <c r="N18" t="inlineStr"/>
-      <c r="O18" t="n">
-        <v>499</v>
-      </c>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
         <v>499</v>
       </c>
@@ -1976,10 +2030,10 @@
       <c r="T18" t="n">
         <v>499</v>
       </c>
-      <c r="U18" t="inlineStr"/>
-      <c r="V18" t="n">
-        <v>499</v>
-      </c>
+      <c r="U18" t="n">
+        <v>499</v>
+      </c>
+      <c r="V18" t="inlineStr"/>
       <c r="W18" t="n">
         <v>499</v>
       </c>
@@ -1996,6 +2050,9 @@
         <v>499</v>
       </c>
       <c r="AB18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2030,7 +2087,7 @@
         <v>1299</v>
       </c>
       <c r="J19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="K19" t="n">
         <v>1497</v>
@@ -2038,13 +2095,13 @@
       <c r="L19" t="n">
         <v>1497</v>
       </c>
-      <c r="M19" t="inlineStr"/>
+      <c r="M19" t="n">
+        <v>1497</v>
+      </c>
       <c r="N19" t="inlineStr"/>
-      <c r="O19" t="n">
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="n">
         <v>465</v>
-      </c>
-      <c r="P19" t="n">
-        <v>1497</v>
       </c>
       <c r="Q19" t="n">
         <v>1497</v>
@@ -2080,6 +2137,9 @@
         <v>1497</v>
       </c>
       <c r="AB19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AC19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2146,10 +2206,10 @@
       <c r="T20" t="n">
         <v>929</v>
       </c>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="n">
-        <v>929</v>
-      </c>
+      <c r="U20" t="n">
+        <v>929</v>
+      </c>
+      <c r="V20" t="inlineStr"/>
       <c r="W20" t="n">
         <v>929</v>
       </c>
@@ -2166,6 +2226,9 @@
         <v>929</v>
       </c>
       <c r="AB20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2181,10 +2244,10 @@
       <c r="C21" t="n">
         <v>499</v>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>499</v>
-      </c>
+      <c r="D21" t="n">
+        <v>499</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
         <v>499</v>
       </c>
@@ -2209,10 +2272,10 @@
       <c r="M21" t="n">
         <v>499</v>
       </c>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="n">
-        <v>499</v>
-      </c>
+      <c r="N21" t="n">
+        <v>499</v>
+      </c>
+      <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
         <v>499</v>
       </c>
@@ -2250,6 +2313,9 @@
         <v>499</v>
       </c>
       <c r="AB21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2289,14 +2355,14 @@
       <c r="K22" t="n">
         <v>299</v>
       </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="n">
-        <v>299</v>
-      </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="n">
-        <v>299</v>
-      </c>
+      <c r="L22" t="n">
+        <v>299</v>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="n">
+        <v>299</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
       <c r="P22" t="n">
         <v>299</v>
       </c>
@@ -2312,10 +2378,10 @@
       <c r="T22" t="n">
         <v>299</v>
       </c>
-      <c r="U22" t="inlineStr"/>
-      <c r="V22" t="n">
-        <v>299</v>
-      </c>
+      <c r="U22" t="n">
+        <v>299</v>
+      </c>
+      <c r="V22" t="inlineStr"/>
       <c r="W22" t="n">
         <v>299</v>
       </c>
@@ -2332,6 +2398,9 @@
         <v>299</v>
       </c>
       <c r="AB22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2374,11 +2443,11 @@
       <c r="L23" t="n">
         <v>1299</v>
       </c>
-      <c r="M23" t="inlineStr"/>
+      <c r="M23" t="n">
+        <v>1299</v>
+      </c>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="n">
         <v>1299</v>
       </c>
@@ -2394,10 +2463,10 @@
       <c r="T23" t="n">
         <v>1299</v>
       </c>
-      <c r="U23" t="inlineStr"/>
-      <c r="V23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="U23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="V23" t="inlineStr"/>
       <c r="W23" t="n">
         <v>1299</v>
       </c>
@@ -2414,6 +2483,9 @@
         <v>1299</v>
       </c>
       <c r="AB23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AC23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2453,11 +2525,11 @@
       <c r="K24" t="n">
         <v>929</v>
       </c>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" t="n">
+        <v>929</v>
+      </c>
       <c r="M24" t="inlineStr"/>
-      <c r="N24" t="n">
-        <v>929</v>
-      </c>
+      <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
         <v>929</v>
       </c>
@@ -2476,10 +2548,10 @@
       <c r="T24" t="n">
         <v>929</v>
       </c>
-      <c r="U24" t="inlineStr"/>
-      <c r="V24" t="n">
-        <v>929</v>
-      </c>
+      <c r="U24" t="n">
+        <v>929</v>
+      </c>
+      <c r="V24" t="inlineStr"/>
       <c r="W24" t="n">
         <v>929</v>
       </c>
@@ -2496,6 +2568,9 @@
         <v>929</v>
       </c>
       <c r="AB24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2535,11 +2610,11 @@
       <c r="K25" t="n">
         <v>929</v>
       </c>
-      <c r="L25" t="inlineStr"/>
+      <c r="L25" t="n">
+        <v>929</v>
+      </c>
       <c r="M25" t="inlineStr"/>
-      <c r="N25" t="n">
-        <v>929</v>
-      </c>
+      <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
         <v>929</v>
       </c>
@@ -2558,10 +2633,10 @@
       <c r="T25" t="n">
         <v>929</v>
       </c>
-      <c r="U25" t="inlineStr"/>
-      <c r="V25" t="n">
-        <v>929</v>
-      </c>
+      <c r="U25" t="n">
+        <v>929</v>
+      </c>
+      <c r="V25" t="inlineStr"/>
       <c r="W25" t="n">
         <v>929</v>
       </c>
@@ -2578,6 +2653,9 @@
         <v>929</v>
       </c>
       <c r="AB25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2617,14 +2695,14 @@
       <c r="K26" t="n">
         <v>1299</v>
       </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="L26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
         <v>1299</v>
       </c>
@@ -2640,10 +2718,10 @@
       <c r="T26" t="n">
         <v>1299</v>
       </c>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="U26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="V26" t="inlineStr"/>
       <c r="W26" t="n">
         <v>1299</v>
       </c>
@@ -2660,6 +2738,9 @@
         <v>1299</v>
       </c>
       <c r="AB26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AC26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 20:45
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,7 @@
     <col width="21" customWidth="1" min="27" max="27"/>
     <col width="21" customWidth="1" min="28" max="28"/>
     <col width="21" customWidth="1" min="29" max="29"/>
+    <col width="21" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -472,140 +473,145 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 02:12</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -635,10 +641,10 @@
       <c r="G2" t="n">
         <v>929</v>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
-        <v>929</v>
-      </c>
+      <c r="H2" t="n">
+        <v>929</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
         <v>929</v>
       </c>
@@ -651,25 +657,25 @@
       <c r="M2" t="n">
         <v>929</v>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="n">
+        <v>929</v>
+      </c>
       <c r="O2" t="inlineStr"/>
-      <c r="P2" t="n">
-        <v>929</v>
-      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="n">
         <v>929</v>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="n">
-        <v>929</v>
-      </c>
+      <c r="R2" t="n">
+        <v>929</v>
+      </c>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="n">
         <v>929</v>
       </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="n">
-        <v>929</v>
-      </c>
+      <c r="U2" t="n">
+        <v>929</v>
+      </c>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="n">
         <v>929</v>
       </c>
@@ -689,6 +695,9 @@
         <v>929</v>
       </c>
       <c r="AC2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -713,26 +722,26 @@
       <c r="F3" t="n">
         <v>569</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>569</v>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>569</v>
-      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
         <v>569</v>
       </c>
       <c r="L3" t="n">
         <v>569</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="n">
-        <v>569</v>
-      </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="n">
-        <v>569</v>
-      </c>
+      <c r="M3" t="n">
+        <v>569</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="n">
+        <v>569</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="n">
         <v>569</v>
       </c>
@@ -748,10 +757,10 @@
       <c r="U3" t="n">
         <v>569</v>
       </c>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="n">
-        <v>569</v>
-      </c>
+      <c r="V3" t="n">
+        <v>569</v>
+      </c>
+      <c r="W3" t="inlineStr"/>
       <c r="X3" t="n">
         <v>569</v>
       </c>
@@ -768,6 +777,9 @@
         <v>569</v>
       </c>
       <c r="AC3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -810,10 +822,10 @@
       <c r="L4" t="n">
         <v>299</v>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="n">
-        <v>299</v>
-      </c>
+      <c r="M4" t="n">
+        <v>299</v>
+      </c>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
         <v>299</v>
       </c>
@@ -835,10 +847,10 @@
       <c r="U4" t="n">
         <v>299</v>
       </c>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="n">
-        <v>299</v>
-      </c>
+      <c r="V4" t="n">
+        <v>299</v>
+      </c>
+      <c r="W4" t="inlineStr"/>
       <c r="X4" t="n">
         <v>299</v>
       </c>
@@ -855,6 +867,9 @@
         <v>299</v>
       </c>
       <c r="AC4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -924,10 +939,10 @@
       <c r="U5" t="n">
         <v>569</v>
       </c>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="n">
-        <v>569</v>
-      </c>
+      <c r="V5" t="n">
+        <v>569</v>
+      </c>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="n">
         <v>569</v>
       </c>
@@ -944,6 +959,9 @@
         <v>569</v>
       </c>
       <c r="AC5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -989,10 +1007,10 @@
       <c r="M6" t="n">
         <v>499</v>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="n">
-        <v>499</v>
-      </c>
+      <c r="N6" t="n">
+        <v>499</v>
+      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
         <v>499</v>
       </c>
@@ -1011,10 +1029,10 @@
       <c r="U6" t="n">
         <v>499</v>
       </c>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="n">
-        <v>499</v>
-      </c>
+      <c r="V6" t="n">
+        <v>499</v>
+      </c>
+      <c r="W6" t="inlineStr"/>
       <c r="X6" t="n">
         <v>499</v>
       </c>
@@ -1031,6 +1049,9 @@
         <v>499</v>
       </c>
       <c r="AC6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1073,12 +1094,12 @@
       <c r="L7" t="n">
         <v>569</v>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>569</v>
+      </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="n">
-        <v>569</v>
-      </c>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="n">
         <v>569</v>
       </c>
@@ -1094,10 +1115,10 @@
       <c r="U7" t="n">
         <v>569</v>
       </c>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="n">
-        <v>569</v>
-      </c>
+      <c r="V7" t="n">
+        <v>569</v>
+      </c>
+      <c r="W7" t="inlineStr"/>
       <c r="X7" t="n">
         <v>569</v>
       </c>
@@ -1114,6 +1135,9 @@
         <v>569</v>
       </c>
       <c r="AC7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1156,14 +1180,14 @@
       <c r="L8" t="n">
         <v>929</v>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="n">
-        <v>929</v>
-      </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="n">
-        <v>929</v>
-      </c>
+      <c r="M8" t="n">
+        <v>929</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="n">
+        <v>929</v>
+      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="n">
         <v>929</v>
       </c>
@@ -1179,10 +1203,10 @@
       <c r="U8" t="n">
         <v>929</v>
       </c>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="n">
-        <v>929</v>
-      </c>
+      <c r="V8" t="n">
+        <v>929</v>
+      </c>
+      <c r="W8" t="inlineStr"/>
       <c r="X8" t="n">
         <v>929</v>
       </c>
@@ -1199,6 +1223,9 @@
         <v>929</v>
       </c>
       <c r="AC8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1241,10 +1268,10 @@
       <c r="L9" t="n">
         <v>299</v>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="n">
-        <v>299</v>
-      </c>
+      <c r="M9" t="n">
+        <v>299</v>
+      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
         <v>299</v>
       </c>
@@ -1266,10 +1293,10 @@
       <c r="U9" t="n">
         <v>299</v>
       </c>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="n">
-        <v>299</v>
-      </c>
+      <c r="V9" t="n">
+        <v>299</v>
+      </c>
+      <c r="W9" t="inlineStr"/>
       <c r="X9" t="n">
         <v>299</v>
       </c>
@@ -1286,6 +1313,9 @@
         <v>299</v>
       </c>
       <c r="AC9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1298,10 +1328,10 @@
       <c r="B10" t="n">
         <v>299</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>299</v>
-      </c>
+      <c r="C10" t="n">
+        <v>299</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
         <v>299</v>
       </c>
@@ -1326,14 +1356,14 @@
       <c r="L10" t="n">
         <v>299</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="n">
-        <v>299</v>
-      </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="n">
-        <v>299</v>
-      </c>
+      <c r="M10" t="n">
+        <v>299</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="n">
+        <v>299</v>
+      </c>
+      <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
         <v>299</v>
       </c>
@@ -1349,10 +1379,10 @@
       <c r="U10" t="n">
         <v>299</v>
       </c>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="n">
-        <v>299</v>
-      </c>
+      <c r="V10" t="n">
+        <v>299</v>
+      </c>
+      <c r="W10" t="inlineStr"/>
       <c r="X10" t="n">
         <v>299</v>
       </c>
@@ -1369,6 +1399,9 @@
         <v>299</v>
       </c>
       <c r="AC10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1414,10 +1447,10 @@
       <c r="M11" t="n">
         <v>2997</v>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="n">
+      <c r="N11" t="n">
         <v>2997</v>
       </c>
+      <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
         <v>2997</v>
       </c>
@@ -1431,15 +1464,15 @@
         <v>2997</v>
       </c>
       <c r="T11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="U11" t="n">
         <v>929</v>
       </c>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="n">
-        <v>929</v>
-      </c>
+      <c r="V11" t="n">
+        <v>929</v>
+      </c>
+      <c r="W11" t="inlineStr"/>
       <c r="X11" t="n">
         <v>929</v>
       </c>
@@ -1456,6 +1489,9 @@
         <v>929</v>
       </c>
       <c r="AC11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1504,10 +1540,10 @@
       <c r="N12" t="n">
         <v>569</v>
       </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="n">
-        <v>569</v>
-      </c>
+      <c r="O12" t="n">
+        <v>569</v>
+      </c>
+      <c r="P12" t="inlineStr"/>
       <c r="Q12" t="n">
         <v>569</v>
       </c>
@@ -1523,10 +1559,10 @@
       <c r="U12" t="n">
         <v>569</v>
       </c>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="n">
-        <v>569</v>
-      </c>
+      <c r="V12" t="n">
+        <v>569</v>
+      </c>
+      <c r="W12" t="inlineStr"/>
       <c r="X12" t="n">
         <v>569</v>
       </c>
@@ -1543,6 +1579,9 @@
         <v>569</v>
       </c>
       <c r="AC12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1585,14 +1624,14 @@
       <c r="L13" t="n">
         <v>569</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="n">
-        <v>569</v>
-      </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="n">
-        <v>569</v>
-      </c>
+      <c r="M13" t="n">
+        <v>569</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="n">
+        <v>569</v>
+      </c>
+      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="n">
         <v>569</v>
       </c>
@@ -1608,24 +1647,27 @@
       <c r="U13" t="n">
         <v>569</v>
       </c>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="n">
-        <v>569</v>
-      </c>
+      <c r="V13" t="n">
+        <v>569</v>
+      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="n">
         <v>569</v>
       </c>
       <c r="Y13" t="n">
         <v>569</v>
       </c>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="n">
         <v>569</v>
       </c>
       <c r="AC13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1638,10 +1680,10 @@
       <c r="B14" t="n">
         <v>794</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="n">
+      <c r="C14" t="n">
         <v>794</v>
       </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>794</v>
       </c>
@@ -1649,7 +1691,7 @@
         <v>794</v>
       </c>
       <c r="G14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="H14" t="n">
         <v>499</v>
@@ -1666,11 +1708,11 @@
       <c r="L14" t="n">
         <v>499</v>
       </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>499</v>
+      </c>
       <c r="N14" t="inlineStr"/>
-      <c r="O14" t="n">
-        <v>499</v>
-      </c>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
         <v>499</v>
       </c>
@@ -1711,6 +1753,9 @@
         <v>499</v>
       </c>
       <c r="AC14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1759,10 +1804,10 @@
       <c r="N15" t="n">
         <v>499</v>
       </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="n">
-        <v>499</v>
-      </c>
+      <c r="O15" t="n">
+        <v>499</v>
+      </c>
+      <c r="P15" t="inlineStr"/>
       <c r="Q15" t="n">
         <v>499</v>
       </c>
@@ -1772,14 +1817,14 @@
       <c r="S15" t="n">
         <v>499</v>
       </c>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="n">
-        <v>499</v>
-      </c>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="n">
-        <v>499</v>
-      </c>
+      <c r="T15" t="n">
+        <v>499</v>
+      </c>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="n">
+        <v>499</v>
+      </c>
+      <c r="W15" t="inlineStr"/>
       <c r="X15" t="n">
         <v>499</v>
       </c>
@@ -1796,6 +1841,9 @@
         <v>499</v>
       </c>
       <c r="AC15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1829,17 +1877,17 @@
       <c r="I16" t="n">
         <v>299</v>
       </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="n">
-        <v>299</v>
-      </c>
+      <c r="J16" t="n">
+        <v>299</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="n">
         <v>299</v>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="n">
-        <v>299</v>
-      </c>
+      <c r="M16" t="n">
+        <v>299</v>
+      </c>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
         <v>299</v>
       </c>
@@ -1861,10 +1909,10 @@
       <c r="U16" t="n">
         <v>299</v>
       </c>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="n">
-        <v>299</v>
-      </c>
+      <c r="V16" t="n">
+        <v>299</v>
+      </c>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="n">
         <v>299</v>
       </c>
@@ -1881,6 +1929,9 @@
         <v>299</v>
       </c>
       <c r="AC16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1929,10 +1980,10 @@
       <c r="N17" t="n">
         <v>929</v>
       </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="n">
-        <v>929</v>
-      </c>
+      <c r="O17" t="n">
+        <v>929</v>
+      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="n">
         <v>929</v>
       </c>
@@ -1948,10 +1999,10 @@
       <c r="U17" t="n">
         <v>929</v>
       </c>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="n">
-        <v>929</v>
-      </c>
+      <c r="V17" t="n">
+        <v>929</v>
+      </c>
+      <c r="W17" t="inlineStr"/>
       <c r="X17" t="n">
         <v>929</v>
       </c>
@@ -1968,6 +2019,9 @@
         <v>929</v>
       </c>
       <c r="AC17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2013,11 +2067,11 @@
       <c r="M18" t="n">
         <v>499</v>
       </c>
-      <c r="N18" t="inlineStr"/>
+      <c r="N18" t="n">
+        <v>499</v>
+      </c>
       <c r="O18" t="inlineStr"/>
-      <c r="P18" t="n">
-        <v>499</v>
-      </c>
+      <c r="P18" t="inlineStr"/>
       <c r="Q18" t="n">
         <v>499</v>
       </c>
@@ -2033,10 +2087,10 @@
       <c r="U18" t="n">
         <v>499</v>
       </c>
-      <c r="V18" t="inlineStr"/>
-      <c r="W18" t="n">
-        <v>499</v>
-      </c>
+      <c r="V18" t="n">
+        <v>499</v>
+      </c>
+      <c r="W18" t="inlineStr"/>
       <c r="X18" t="n">
         <v>499</v>
       </c>
@@ -2053,6 +2107,9 @@
         <v>499</v>
       </c>
       <c r="AC18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2090,7 +2147,7 @@
         <v>1299</v>
       </c>
       <c r="K19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="L19" t="n">
         <v>1497</v>
@@ -2098,13 +2155,13 @@
       <c r="M19" t="n">
         <v>1497</v>
       </c>
-      <c r="N19" t="inlineStr"/>
+      <c r="N19" t="n">
+        <v>1497</v>
+      </c>
       <c r="O19" t="inlineStr"/>
-      <c r="P19" t="n">
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="n">
         <v>465</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>1497</v>
       </c>
       <c r="R19" t="n">
         <v>1497</v>
@@ -2140,6 +2197,9 @@
         <v>1497</v>
       </c>
       <c r="AC19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AD19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2209,10 +2269,10 @@
       <c r="U20" t="n">
         <v>929</v>
       </c>
-      <c r="V20" t="inlineStr"/>
-      <c r="W20" t="n">
-        <v>929</v>
-      </c>
+      <c r="V20" t="n">
+        <v>929</v>
+      </c>
+      <c r="W20" t="inlineStr"/>
       <c r="X20" t="n">
         <v>929</v>
       </c>
@@ -2229,6 +2289,9 @@
         <v>929</v>
       </c>
       <c r="AC20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2247,10 +2310,10 @@
       <c r="D21" t="n">
         <v>499</v>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>499</v>
-      </c>
+      <c r="E21" t="n">
+        <v>499</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
         <v>499</v>
       </c>
@@ -2275,10 +2338,10 @@
       <c r="N21" t="n">
         <v>499</v>
       </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="n">
-        <v>499</v>
-      </c>
+      <c r="O21" t="n">
+        <v>499</v>
+      </c>
+      <c r="P21" t="inlineStr"/>
       <c r="Q21" t="n">
         <v>499</v>
       </c>
@@ -2316,6 +2379,9 @@
         <v>499</v>
       </c>
       <c r="AC21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2358,14 +2424,14 @@
       <c r="L22" t="n">
         <v>299</v>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="n">
-        <v>299</v>
-      </c>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="n">
-        <v>299</v>
-      </c>
+      <c r="M22" t="n">
+        <v>299</v>
+      </c>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="n">
+        <v>299</v>
+      </c>
+      <c r="P22" t="inlineStr"/>
       <c r="Q22" t="n">
         <v>299</v>
       </c>
@@ -2381,10 +2447,10 @@
       <c r="U22" t="n">
         <v>299</v>
       </c>
-      <c r="V22" t="inlineStr"/>
-      <c r="W22" t="n">
-        <v>299</v>
-      </c>
+      <c r="V22" t="n">
+        <v>299</v>
+      </c>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="n">
         <v>299</v>
       </c>
@@ -2401,6 +2467,9 @@
         <v>299</v>
       </c>
       <c r="AC22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2446,11 +2515,11 @@
       <c r="M23" t="n">
         <v>1299</v>
       </c>
-      <c r="N23" t="inlineStr"/>
+      <c r="N23" t="n">
+        <v>1299</v>
+      </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="P23" t="inlineStr"/>
       <c r="Q23" t="n">
         <v>1299</v>
       </c>
@@ -2466,10 +2535,10 @@
       <c r="U23" t="n">
         <v>1299</v>
       </c>
-      <c r="V23" t="inlineStr"/>
-      <c r="W23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="V23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="W23" t="inlineStr"/>
       <c r="X23" t="n">
         <v>1299</v>
       </c>
@@ -2486,6 +2555,9 @@
         <v>1299</v>
       </c>
       <c r="AC23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AD23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2528,11 +2600,11 @@
       <c r="L24" t="n">
         <v>929</v>
       </c>
-      <c r="M24" t="inlineStr"/>
+      <c r="M24" t="n">
+        <v>929</v>
+      </c>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="n">
-        <v>929</v>
-      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
         <v>929</v>
       </c>
@@ -2551,10 +2623,10 @@
       <c r="U24" t="n">
         <v>929</v>
       </c>
-      <c r="V24" t="inlineStr"/>
-      <c r="W24" t="n">
-        <v>929</v>
-      </c>
+      <c r="V24" t="n">
+        <v>929</v>
+      </c>
+      <c r="W24" t="inlineStr"/>
       <c r="X24" t="n">
         <v>929</v>
       </c>
@@ -2571,6 +2643,9 @@
         <v>929</v>
       </c>
       <c r="AC24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2613,11 +2688,11 @@
       <c r="L25" t="n">
         <v>929</v>
       </c>
-      <c r="M25" t="inlineStr"/>
+      <c r="M25" t="n">
+        <v>929</v>
+      </c>
       <c r="N25" t="inlineStr"/>
-      <c r="O25" t="n">
-        <v>929</v>
-      </c>
+      <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
         <v>929</v>
       </c>
@@ -2636,10 +2711,10 @@
       <c r="U25" t="n">
         <v>929</v>
       </c>
-      <c r="V25" t="inlineStr"/>
-      <c r="W25" t="n">
-        <v>929</v>
-      </c>
+      <c r="V25" t="n">
+        <v>929</v>
+      </c>
+      <c r="W25" t="inlineStr"/>
       <c r="X25" t="n">
         <v>929</v>
       </c>
@@ -2656,6 +2731,9 @@
         <v>929</v>
       </c>
       <c r="AC25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2698,14 +2776,14 @@
       <c r="L26" t="n">
         <v>1299</v>
       </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="M26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P26" t="inlineStr"/>
       <c r="Q26" t="n">
         <v>1299</v>
       </c>
@@ -2721,10 +2799,10 @@
       <c r="U26" t="n">
         <v>1299</v>
       </c>
-      <c r="V26" t="inlineStr"/>
-      <c r="W26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="V26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="n">
         <v>1299</v>
       </c>
@@ -2741,6 +2819,9 @@
         <v>1299</v>
       </c>
       <c r="AC26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AD26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-22 22:46
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,7 @@
     <col width="21" customWidth="1" min="28" max="28"/>
     <col width="21" customWidth="1" min="29" max="29"/>
     <col width="21" customWidth="1" min="30" max="30"/>
+    <col width="21" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -473,145 +474,150 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 04:13</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -644,10 +650,10 @@
       <c r="H2" t="n">
         <v>929</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
-        <v>929</v>
-      </c>
+      <c r="I2" t="n">
+        <v>929</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
         <v>929</v>
       </c>
@@ -660,25 +666,25 @@
       <c r="N2" t="n">
         <v>929</v>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="O2" t="n">
+        <v>929</v>
+      </c>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
         <v>929</v>
       </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="n">
-        <v>929</v>
-      </c>
+      <c r="S2" t="n">
+        <v>929</v>
+      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
         <v>929</v>
       </c>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="n">
-        <v>929</v>
-      </c>
+      <c r="V2" t="n">
+        <v>929</v>
+      </c>
+      <c r="W2" t="inlineStr"/>
       <c r="X2" t="n">
         <v>929</v>
       </c>
@@ -698,6 +704,9 @@
         <v>929</v>
       </c>
       <c r="AD2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -725,26 +734,26 @@
       <c r="G3" t="n">
         <v>569</v>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>569</v>
+      </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>569</v>
-      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
         <v>569</v>
       </c>
       <c r="M3" t="n">
         <v>569</v>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
-        <v>569</v>
-      </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="n">
-        <v>569</v>
-      </c>
+      <c r="N3" t="n">
+        <v>569</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
         <v>569</v>
       </c>
@@ -760,10 +769,10 @@
       <c r="V3" t="n">
         <v>569</v>
       </c>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="n">
-        <v>569</v>
-      </c>
+      <c r="W3" t="n">
+        <v>569</v>
+      </c>
+      <c r="X3" t="inlineStr"/>
       <c r="Y3" t="n">
         <v>569</v>
       </c>
@@ -780,6 +789,9 @@
         <v>569</v>
       </c>
       <c r="AD3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -825,10 +837,10 @@
       <c r="M4" t="n">
         <v>299</v>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="n">
-        <v>299</v>
-      </c>
+      <c r="N4" t="n">
+        <v>299</v>
+      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
         <v>299</v>
       </c>
@@ -850,10 +862,10 @@
       <c r="V4" t="n">
         <v>299</v>
       </c>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="n">
-        <v>299</v>
-      </c>
+      <c r="W4" t="n">
+        <v>299</v>
+      </c>
+      <c r="X4" t="inlineStr"/>
       <c r="Y4" t="n">
         <v>299</v>
       </c>
@@ -870,6 +882,9 @@
         <v>299</v>
       </c>
       <c r="AD4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -942,10 +957,10 @@
       <c r="V5" t="n">
         <v>569</v>
       </c>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="n">
-        <v>569</v>
-      </c>
+      <c r="W5" t="n">
+        <v>569</v>
+      </c>
+      <c r="X5" t="inlineStr"/>
       <c r="Y5" t="n">
         <v>569</v>
       </c>
@@ -962,6 +977,9 @@
         <v>569</v>
       </c>
       <c r="AD5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1010,10 +1028,10 @@
       <c r="N6" t="n">
         <v>499</v>
       </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="n">
-        <v>499</v>
-      </c>
+      <c r="O6" t="n">
+        <v>499</v>
+      </c>
+      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="n">
         <v>499</v>
       </c>
@@ -1032,10 +1050,10 @@
       <c r="V6" t="n">
         <v>499</v>
       </c>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="n">
-        <v>499</v>
-      </c>
+      <c r="W6" t="n">
+        <v>499</v>
+      </c>
+      <c r="X6" t="inlineStr"/>
       <c r="Y6" t="n">
         <v>499</v>
       </c>
@@ -1052,6 +1070,9 @@
         <v>499</v>
       </c>
       <c r="AD6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1097,12 +1118,12 @@
       <c r="M7" t="n">
         <v>569</v>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>569</v>
+      </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
         <v>569</v>
       </c>
@@ -1118,10 +1139,10 @@
       <c r="V7" t="n">
         <v>569</v>
       </c>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="n">
-        <v>569</v>
-      </c>
+      <c r="W7" t="n">
+        <v>569</v>
+      </c>
+      <c r="X7" t="inlineStr"/>
       <c r="Y7" t="n">
         <v>569</v>
       </c>
@@ -1138,6 +1159,9 @@
         <v>569</v>
       </c>
       <c r="AD7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1183,14 +1207,14 @@
       <c r="M8" t="n">
         <v>929</v>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="n">
-        <v>929</v>
-      </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="n">
-        <v>929</v>
-      </c>
+      <c r="N8" t="n">
+        <v>929</v>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
         <v>929</v>
       </c>
@@ -1206,10 +1230,10 @@
       <c r="V8" t="n">
         <v>929</v>
       </c>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="n">
-        <v>929</v>
-      </c>
+      <c r="W8" t="n">
+        <v>929</v>
+      </c>
+      <c r="X8" t="inlineStr"/>
       <c r="Y8" t="n">
         <v>929</v>
       </c>
@@ -1226,6 +1250,9 @@
         <v>929</v>
       </c>
       <c r="AD8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1271,10 +1298,10 @@
       <c r="M9" t="n">
         <v>299</v>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="n">
-        <v>299</v>
-      </c>
+      <c r="N9" t="n">
+        <v>299</v>
+      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
         <v>299</v>
       </c>
@@ -1296,10 +1323,10 @@
       <c r="V9" t="n">
         <v>299</v>
       </c>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="n">
-        <v>299</v>
-      </c>
+      <c r="W9" t="n">
+        <v>299</v>
+      </c>
+      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="n">
         <v>299</v>
       </c>
@@ -1316,6 +1343,9 @@
         <v>299</v>
       </c>
       <c r="AD9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1331,10 +1361,10 @@
       <c r="C10" t="n">
         <v>299</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>299</v>
-      </c>
+      <c r="D10" t="n">
+        <v>299</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>299</v>
       </c>
@@ -1359,14 +1389,14 @@
       <c r="M10" t="n">
         <v>299</v>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="n">
-        <v>299</v>
-      </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="n">
-        <v>299</v>
-      </c>
+      <c r="N10" t="n">
+        <v>299</v>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
         <v>299</v>
       </c>
@@ -1382,10 +1412,10 @@
       <c r="V10" t="n">
         <v>299</v>
       </c>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="n">
-        <v>299</v>
-      </c>
+      <c r="W10" t="n">
+        <v>299</v>
+      </c>
+      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="n">
         <v>299</v>
       </c>
@@ -1402,6 +1432,9 @@
         <v>299</v>
       </c>
       <c r="AD10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1450,10 +1483,10 @@
       <c r="N11" t="n">
         <v>2997</v>
       </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="n">
+      <c r="O11" t="n">
         <v>2997</v>
       </c>
+      <c r="P11" t="inlineStr"/>
       <c r="Q11" t="n">
         <v>2997</v>
       </c>
@@ -1467,15 +1500,15 @@
         <v>2997</v>
       </c>
       <c r="U11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="V11" t="n">
         <v>929</v>
       </c>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="n">
-        <v>929</v>
-      </c>
+      <c r="W11" t="n">
+        <v>929</v>
+      </c>
+      <c r="X11" t="inlineStr"/>
       <c r="Y11" t="n">
         <v>929</v>
       </c>
@@ -1492,6 +1525,9 @@
         <v>929</v>
       </c>
       <c r="AD11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1543,10 +1579,10 @@
       <c r="O12" t="n">
         <v>569</v>
       </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="n">
-        <v>569</v>
-      </c>
+      <c r="P12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
         <v>569</v>
       </c>
@@ -1562,10 +1598,10 @@
       <c r="V12" t="n">
         <v>569</v>
       </c>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="n">
-        <v>569</v>
-      </c>
+      <c r="W12" t="n">
+        <v>569</v>
+      </c>
+      <c r="X12" t="inlineStr"/>
       <c r="Y12" t="n">
         <v>569</v>
       </c>
@@ -1582,6 +1618,9 @@
         <v>569</v>
       </c>
       <c r="AD12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1627,14 +1666,14 @@
       <c r="M13" t="n">
         <v>569</v>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="n">
-        <v>569</v>
-      </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="n">
-        <v>569</v>
-      </c>
+      <c r="N13" t="n">
+        <v>569</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
         <v>569</v>
       </c>
@@ -1650,24 +1689,27 @@
       <c r="V13" t="n">
         <v>569</v>
       </c>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="n">
-        <v>569</v>
-      </c>
+      <c r="W13" t="n">
+        <v>569</v>
+      </c>
+      <c r="X13" t="inlineStr"/>
       <c r="Y13" t="n">
         <v>569</v>
       </c>
       <c r="Z13" t="n">
         <v>569</v>
       </c>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="n">
         <v>569</v>
       </c>
       <c r="AD13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1683,10 +1725,10 @@
       <c r="C14" t="n">
         <v>794</v>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>794</v>
       </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
         <v>794</v>
       </c>
@@ -1694,7 +1736,7 @@
         <v>794</v>
       </c>
       <c r="H14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="I14" t="n">
         <v>499</v>
@@ -1711,11 +1753,11 @@
       <c r="M14" t="n">
         <v>499</v>
       </c>
-      <c r="N14" t="inlineStr"/>
+      <c r="N14" t="n">
+        <v>499</v>
+      </c>
       <c r="O14" t="inlineStr"/>
-      <c r="P14" t="n">
-        <v>499</v>
-      </c>
+      <c r="P14" t="inlineStr"/>
       <c r="Q14" t="n">
         <v>499</v>
       </c>
@@ -1756,6 +1798,9 @@
         <v>499</v>
       </c>
       <c r="AD14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1807,10 +1852,10 @@
       <c r="O15" t="n">
         <v>499</v>
       </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="n">
-        <v>499</v>
-      </c>
+      <c r="P15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="n">
         <v>499</v>
       </c>
@@ -1820,14 +1865,14 @@
       <c r="T15" t="n">
         <v>499</v>
       </c>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="n">
-        <v>499</v>
-      </c>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="n">
-        <v>499</v>
-      </c>
+      <c r="U15" t="n">
+        <v>499</v>
+      </c>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="n">
+        <v>499</v>
+      </c>
+      <c r="X15" t="inlineStr"/>
       <c r="Y15" t="n">
         <v>499</v>
       </c>
@@ -1844,6 +1889,9 @@
         <v>499</v>
       </c>
       <c r="AD15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1880,17 +1928,17 @@
       <c r="J16" t="n">
         <v>299</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="n">
-        <v>299</v>
-      </c>
+      <c r="K16" t="n">
+        <v>299</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
         <v>299</v>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="n">
-        <v>299</v>
-      </c>
+      <c r="N16" t="n">
+        <v>299</v>
+      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
         <v>299</v>
       </c>
@@ -1912,10 +1960,10 @@
       <c r="V16" t="n">
         <v>299</v>
       </c>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="n">
-        <v>299</v>
-      </c>
+      <c r="W16" t="n">
+        <v>299</v>
+      </c>
+      <c r="X16" t="inlineStr"/>
       <c r="Y16" t="n">
         <v>299</v>
       </c>
@@ -1932,6 +1980,9 @@
         <v>299</v>
       </c>
       <c r="AD16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1983,10 +2034,10 @@
       <c r="O17" t="n">
         <v>929</v>
       </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="n">
-        <v>929</v>
-      </c>
+      <c r="P17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
         <v>929</v>
       </c>
@@ -2002,10 +2053,10 @@
       <c r="V17" t="n">
         <v>929</v>
       </c>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="n">
-        <v>929</v>
-      </c>
+      <c r="W17" t="n">
+        <v>929</v>
+      </c>
+      <c r="X17" t="inlineStr"/>
       <c r="Y17" t="n">
         <v>929</v>
       </c>
@@ -2022,6 +2073,9 @@
         <v>929</v>
       </c>
       <c r="AD17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2070,11 +2124,11 @@
       <c r="N18" t="n">
         <v>499</v>
       </c>
-      <c r="O18" t="inlineStr"/>
+      <c r="O18" t="n">
+        <v>499</v>
+      </c>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
         <v>499</v>
       </c>
@@ -2090,10 +2144,10 @@
       <c r="V18" t="n">
         <v>499</v>
       </c>
-      <c r="W18" t="inlineStr"/>
-      <c r="X18" t="n">
-        <v>499</v>
-      </c>
+      <c r="W18" t="n">
+        <v>499</v>
+      </c>
+      <c r="X18" t="inlineStr"/>
       <c r="Y18" t="n">
         <v>499</v>
       </c>
@@ -2110,6 +2164,9 @@
         <v>499</v>
       </c>
       <c r="AD18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2150,7 +2207,7 @@
         <v>1299</v>
       </c>
       <c r="L19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="M19" t="n">
         <v>1497</v>
@@ -2158,13 +2215,13 @@
       <c r="N19" t="n">
         <v>1497</v>
       </c>
-      <c r="O19" t="inlineStr"/>
+      <c r="O19" t="n">
+        <v>1497</v>
+      </c>
       <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="n">
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="n">
         <v>465</v>
-      </c>
-      <c r="R19" t="n">
-        <v>1497</v>
       </c>
       <c r="S19" t="n">
         <v>1497</v>
@@ -2200,6 +2257,9 @@
         <v>1497</v>
       </c>
       <c r="AD19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AE19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2272,10 +2332,10 @@
       <c r="V20" t="n">
         <v>929</v>
       </c>
-      <c r="W20" t="inlineStr"/>
-      <c r="X20" t="n">
-        <v>929</v>
-      </c>
+      <c r="W20" t="n">
+        <v>929</v>
+      </c>
+      <c r="X20" t="inlineStr"/>
       <c r="Y20" t="n">
         <v>929</v>
       </c>
@@ -2292,6 +2352,9 @@
         <v>929</v>
       </c>
       <c r="AD20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2313,10 +2376,10 @@
       <c r="E21" t="n">
         <v>499</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="n">
-        <v>499</v>
-      </c>
+      <c r="F21" t="n">
+        <v>499</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
         <v>499</v>
       </c>
@@ -2341,10 +2404,10 @@
       <c r="O21" t="n">
         <v>499</v>
       </c>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="n">
-        <v>499</v>
-      </c>
+      <c r="P21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
         <v>499</v>
       </c>
@@ -2382,6 +2445,9 @@
         <v>499</v>
       </c>
       <c r="AD21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2427,14 +2493,14 @@
       <c r="M22" t="n">
         <v>299</v>
       </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="n">
-        <v>299</v>
-      </c>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="n">
-        <v>299</v>
-      </c>
+      <c r="N22" t="n">
+        <v>299</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="n">
         <v>299</v>
       </c>
@@ -2450,10 +2516,10 @@
       <c r="V22" t="n">
         <v>299</v>
       </c>
-      <c r="W22" t="inlineStr"/>
-      <c r="X22" t="n">
-        <v>299</v>
-      </c>
+      <c r="W22" t="n">
+        <v>299</v>
+      </c>
+      <c r="X22" t="inlineStr"/>
       <c r="Y22" t="n">
         <v>299</v>
       </c>
@@ -2470,6 +2536,9 @@
         <v>299</v>
       </c>
       <c r="AD22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2518,11 +2587,11 @@
       <c r="N23" t="n">
         <v>1299</v>
       </c>
-      <c r="O23" t="inlineStr"/>
+      <c r="O23" t="n">
+        <v>1299</v>
+      </c>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Q23" t="inlineStr"/>
       <c r="R23" t="n">
         <v>1299</v>
       </c>
@@ -2538,10 +2607,10 @@
       <c r="V23" t="n">
         <v>1299</v>
       </c>
-      <c r="W23" t="inlineStr"/>
-      <c r="X23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="W23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="X23" t="inlineStr"/>
       <c r="Y23" t="n">
         <v>1299</v>
       </c>
@@ -2558,6 +2627,9 @@
         <v>1299</v>
       </c>
       <c r="AD23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AE23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2603,11 +2675,11 @@
       <c r="M24" t="n">
         <v>929</v>
       </c>
-      <c r="N24" t="inlineStr"/>
+      <c r="N24" t="n">
+        <v>929</v>
+      </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="n">
-        <v>929</v>
-      </c>
+      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="n">
         <v>929</v>
       </c>
@@ -2626,10 +2698,10 @@
       <c r="V24" t="n">
         <v>929</v>
       </c>
-      <c r="W24" t="inlineStr"/>
-      <c r="X24" t="n">
-        <v>929</v>
-      </c>
+      <c r="W24" t="n">
+        <v>929</v>
+      </c>
+      <c r="X24" t="inlineStr"/>
       <c r="Y24" t="n">
         <v>929</v>
       </c>
@@ -2646,6 +2718,9 @@
         <v>929</v>
       </c>
       <c r="AD24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2691,11 +2766,11 @@
       <c r="M25" t="n">
         <v>929</v>
       </c>
-      <c r="N25" t="inlineStr"/>
+      <c r="N25" t="n">
+        <v>929</v>
+      </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="n">
-        <v>929</v>
-      </c>
+      <c r="P25" t="inlineStr"/>
       <c r="Q25" t="n">
         <v>929</v>
       </c>
@@ -2714,10 +2789,10 @@
       <c r="V25" t="n">
         <v>929</v>
       </c>
-      <c r="W25" t="inlineStr"/>
-      <c r="X25" t="n">
-        <v>929</v>
-      </c>
+      <c r="W25" t="n">
+        <v>929</v>
+      </c>
+      <c r="X25" t="inlineStr"/>
       <c r="Y25" t="n">
         <v>929</v>
       </c>
@@ -2734,6 +2809,9 @@
         <v>929</v>
       </c>
       <c r="AD25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2779,14 +2857,14 @@
       <c r="M26" t="n">
         <v>1299</v>
       </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="N26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Q26" t="inlineStr"/>
       <c r="R26" t="n">
         <v>1299</v>
       </c>
@@ -2802,10 +2880,10 @@
       <c r="V26" t="n">
         <v>1299</v>
       </c>
-      <c r="W26" t="inlineStr"/>
-      <c r="X26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="W26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="X26" t="inlineStr"/>
       <c r="Y26" t="n">
         <v>1299</v>
       </c>
@@ -2822,6 +2900,9 @@
         <v>1299</v>
       </c>
       <c r="AD26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AE26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 04:00
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE26"/>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,7 @@
     <col width="21" customWidth="1" min="29" max="29"/>
     <col width="21" customWidth="1" min="30" max="30"/>
     <col width="21" customWidth="1" min="31" max="31"/>
+    <col width="21" customWidth="1" min="32" max="32"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -474,150 +475,155 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 09:25</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -653,10 +659,10 @@
       <c r="I2" t="n">
         <v>929</v>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="n">
-        <v>929</v>
-      </c>
+      <c r="J2" t="n">
+        <v>929</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
         <v>929</v>
       </c>
@@ -669,25 +675,25 @@
       <c r="O2" t="n">
         <v>929</v>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>929</v>
+      </c>
       <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="n">
-        <v>929</v>
-      </c>
+      <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
         <v>929</v>
       </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
-        <v>929</v>
-      </c>
+      <c r="T2" t="n">
+        <v>929</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="n">
         <v>929</v>
       </c>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="n">
-        <v>929</v>
-      </c>
+      <c r="W2" t="n">
+        <v>929</v>
+      </c>
+      <c r="X2" t="inlineStr"/>
       <c r="Y2" t="n">
         <v>929</v>
       </c>
@@ -707,6 +713,9 @@
         <v>929</v>
       </c>
       <c r="AE2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -737,26 +746,26 @@
       <c r="H3" t="n">
         <v>569</v>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>569</v>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
-        <v>569</v>
-      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>569</v>
       </c>
       <c r="N3" t="n">
         <v>569</v>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="n">
-        <v>569</v>
-      </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="n">
-        <v>569</v>
-      </c>
+      <c r="O3" t="n">
+        <v>569</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="n">
+        <v>569</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
         <v>569</v>
       </c>
@@ -772,10 +781,10 @@
       <c r="W3" t="n">
         <v>569</v>
       </c>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="n">
-        <v>569</v>
-      </c>
+      <c r="X3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="n">
         <v>569</v>
       </c>
@@ -792,6 +801,9 @@
         <v>569</v>
       </c>
       <c r="AE3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -840,10 +852,10 @@
       <c r="N4" t="n">
         <v>299</v>
       </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="n">
-        <v>299</v>
-      </c>
+      <c r="O4" t="n">
+        <v>299</v>
+      </c>
+      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="n">
         <v>299</v>
       </c>
@@ -865,10 +877,10 @@
       <c r="W4" t="n">
         <v>299</v>
       </c>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="n">
-        <v>299</v>
-      </c>
+      <c r="X4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="n">
         <v>299</v>
       </c>
@@ -885,6 +897,9 @@
         <v>299</v>
       </c>
       <c r="AE4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -960,10 +975,10 @@
       <c r="W5" t="n">
         <v>569</v>
       </c>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="n">
-        <v>569</v>
-      </c>
+      <c r="X5" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="n">
         <v>569</v>
       </c>
@@ -980,6 +995,9 @@
         <v>569</v>
       </c>
       <c r="AE5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1031,10 +1049,10 @@
       <c r="O6" t="n">
         <v>499</v>
       </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="n">
-        <v>499</v>
-      </c>
+      <c r="P6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
         <v>499</v>
       </c>
@@ -1053,10 +1071,10 @@
       <c r="W6" t="n">
         <v>499</v>
       </c>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="n">
-        <v>499</v>
-      </c>
+      <c r="X6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="n">
         <v>499</v>
       </c>
@@ -1073,6 +1091,9 @@
         <v>499</v>
       </c>
       <c r="AE6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1121,12 +1142,12 @@
       <c r="N7" t="n">
         <v>569</v>
       </c>
-      <c r="O7" t="inlineStr"/>
+      <c r="O7" t="n">
+        <v>569</v>
+      </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="n">
-        <v>569</v>
-      </c>
+      <c r="R7" t="inlineStr"/>
       <c r="S7" t="n">
         <v>569</v>
       </c>
@@ -1142,10 +1163,10 @@
       <c r="W7" t="n">
         <v>569</v>
       </c>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="n">
-        <v>569</v>
-      </c>
+      <c r="X7" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="n">
         <v>569</v>
       </c>
@@ -1162,6 +1183,9 @@
         <v>569</v>
       </c>
       <c r="AE7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1210,14 +1234,14 @@
       <c r="N8" t="n">
         <v>929</v>
       </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="n">
-        <v>929</v>
-      </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="n">
-        <v>929</v>
-      </c>
+      <c r="O8" t="n">
+        <v>929</v>
+      </c>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="n">
+        <v>929</v>
+      </c>
+      <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
         <v>929</v>
       </c>
@@ -1233,10 +1257,10 @@
       <c r="W8" t="n">
         <v>929</v>
       </c>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="n">
-        <v>929</v>
-      </c>
+      <c r="X8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="n">
         <v>929</v>
       </c>
@@ -1253,6 +1277,9 @@
         <v>929</v>
       </c>
       <c r="AE8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1301,10 +1328,10 @@
       <c r="N9" t="n">
         <v>299</v>
       </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="n">
-        <v>299</v>
-      </c>
+      <c r="O9" t="n">
+        <v>299</v>
+      </c>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="n">
         <v>299</v>
       </c>
@@ -1326,10 +1353,10 @@
       <c r="W9" t="n">
         <v>299</v>
       </c>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="n">
-        <v>299</v>
-      </c>
+      <c r="X9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="n">
         <v>299</v>
       </c>
@@ -1346,6 +1373,9 @@
         <v>299</v>
       </c>
       <c r="AE9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1364,10 +1394,10 @@
       <c r="D10" t="n">
         <v>299</v>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>299</v>
-      </c>
+      <c r="E10" t="n">
+        <v>299</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>299</v>
       </c>
@@ -1392,14 +1422,14 @@
       <c r="N10" t="n">
         <v>299</v>
       </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="n">
-        <v>299</v>
-      </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="n">
-        <v>299</v>
-      </c>
+      <c r="O10" t="n">
+        <v>299</v>
+      </c>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="n">
+        <v>299</v>
+      </c>
+      <c r="R10" t="inlineStr"/>
       <c r="S10" t="n">
         <v>299</v>
       </c>
@@ -1415,10 +1445,10 @@
       <c r="W10" t="n">
         <v>299</v>
       </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="n">
-        <v>299</v>
-      </c>
+      <c r="X10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="n">
         <v>299</v>
       </c>
@@ -1435,6 +1465,9 @@
         <v>299</v>
       </c>
       <c r="AE10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1486,10 +1519,10 @@
       <c r="O11" t="n">
         <v>2997</v>
       </c>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="n">
+      <c r="P11" t="n">
         <v>2997</v>
       </c>
+      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
         <v>2997</v>
       </c>
@@ -1503,15 +1536,15 @@
         <v>2997</v>
       </c>
       <c r="V11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="W11" t="n">
         <v>929</v>
       </c>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="n">
-        <v>929</v>
-      </c>
+      <c r="X11" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="n">
         <v>929</v>
       </c>
@@ -1528,6 +1561,9 @@
         <v>929</v>
       </c>
       <c r="AE11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1582,10 +1618,10 @@
       <c r="P12" t="n">
         <v>569</v>
       </c>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q12" t="n">
+        <v>569</v>
+      </c>
+      <c r="R12" t="inlineStr"/>
       <c r="S12" t="n">
         <v>569</v>
       </c>
@@ -1601,10 +1637,10 @@
       <c r="W12" t="n">
         <v>569</v>
       </c>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="n">
-        <v>569</v>
-      </c>
+      <c r="X12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="n">
         <v>569</v>
       </c>
@@ -1621,6 +1657,9 @@
         <v>569</v>
       </c>
       <c r="AE12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1669,14 +1708,14 @@
       <c r="N13" t="n">
         <v>569</v>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="n">
-        <v>569</v>
-      </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="n">
-        <v>569</v>
-      </c>
+      <c r="O13" t="n">
+        <v>569</v>
+      </c>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="n">
+        <v>569</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
       <c r="S13" t="n">
         <v>569</v>
       </c>
@@ -1692,24 +1731,27 @@
       <c r="W13" t="n">
         <v>569</v>
       </c>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="n">
-        <v>569</v>
-      </c>
+      <c r="X13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="n">
         <v>569</v>
       </c>
       <c r="AA13" t="n">
         <v>569</v>
       </c>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="n">
         <v>569</v>
       </c>
       <c r="AE13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1728,10 +1770,10 @@
       <c r="D14" t="n">
         <v>794</v>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
+      <c r="E14" t="n">
         <v>794</v>
       </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>794</v>
       </c>
@@ -1739,7 +1781,7 @@
         <v>794</v>
       </c>
       <c r="I14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="J14" t="n">
         <v>499</v>
@@ -1756,11 +1798,11 @@
       <c r="N14" t="n">
         <v>499</v>
       </c>
-      <c r="O14" t="inlineStr"/>
+      <c r="O14" t="n">
+        <v>499</v>
+      </c>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
         <v>499</v>
       </c>
@@ -1801,6 +1843,9 @@
         <v>499</v>
       </c>
       <c r="AE14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1855,10 +1900,10 @@
       <c r="P15" t="n">
         <v>499</v>
       </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q15" t="n">
+        <v>499</v>
+      </c>
+      <c r="R15" t="inlineStr"/>
       <c r="S15" t="n">
         <v>499</v>
       </c>
@@ -1868,14 +1913,14 @@
       <c r="U15" t="n">
         <v>499</v>
       </c>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="n">
-        <v>499</v>
-      </c>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="n">
-        <v>499</v>
-      </c>
+      <c r="V15" t="n">
+        <v>499</v>
+      </c>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="n">
         <v>499</v>
       </c>
@@ -1892,6 +1937,9 @@
         <v>499</v>
       </c>
       <c r="AE15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1931,17 +1979,17 @@
       <c r="K16" t="n">
         <v>299</v>
       </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="n">
-        <v>299</v>
-      </c>
+      <c r="L16" t="n">
+        <v>299</v>
+      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
         <v>299</v>
       </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="n">
-        <v>299</v>
-      </c>
+      <c r="O16" t="n">
+        <v>299</v>
+      </c>
+      <c r="P16" t="inlineStr"/>
       <c r="Q16" t="n">
         <v>299</v>
       </c>
@@ -1963,10 +2011,10 @@
       <c r="W16" t="n">
         <v>299</v>
       </c>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="n">
-        <v>299</v>
-      </c>
+      <c r="X16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="n">
         <v>299</v>
       </c>
@@ -1983,6 +2031,9 @@
         <v>299</v>
       </c>
       <c r="AE16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2037,10 +2088,10 @@
       <c r="P17" t="n">
         <v>929</v>
       </c>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q17" t="n">
+        <v>929</v>
+      </c>
+      <c r="R17" t="inlineStr"/>
       <c r="S17" t="n">
         <v>929</v>
       </c>
@@ -2056,10 +2107,10 @@
       <c r="W17" t="n">
         <v>929</v>
       </c>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="n">
-        <v>929</v>
-      </c>
+      <c r="X17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="n">
         <v>929</v>
       </c>
@@ -2076,6 +2127,9 @@
         <v>929</v>
       </c>
       <c r="AE17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2127,11 +2181,11 @@
       <c r="O18" t="n">
         <v>499</v>
       </c>
-      <c r="P18" t="inlineStr"/>
+      <c r="P18" t="n">
+        <v>499</v>
+      </c>
       <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="n">
-        <v>499</v>
-      </c>
+      <c r="R18" t="inlineStr"/>
       <c r="S18" t="n">
         <v>499</v>
       </c>
@@ -2147,10 +2201,10 @@
       <c r="W18" t="n">
         <v>499</v>
       </c>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="n">
-        <v>499</v>
-      </c>
+      <c r="X18" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="n">
         <v>499</v>
       </c>
@@ -2167,6 +2221,9 @@
         <v>499</v>
       </c>
       <c r="AE18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2210,7 +2267,7 @@
         <v>1299</v>
       </c>
       <c r="M19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="N19" t="n">
         <v>1497</v>
@@ -2218,13 +2275,13 @@
       <c r="O19" t="n">
         <v>1497</v>
       </c>
-      <c r="P19" t="inlineStr"/>
+      <c r="P19" t="n">
+        <v>1497</v>
+      </c>
       <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="n">
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="n">
         <v>465</v>
-      </c>
-      <c r="S19" t="n">
-        <v>1497</v>
       </c>
       <c r="T19" t="n">
         <v>1497</v>
@@ -2260,6 +2317,9 @@
         <v>1497</v>
       </c>
       <c r="AE19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AF19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2335,10 +2395,10 @@
       <c r="W20" t="n">
         <v>929</v>
       </c>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="n">
-        <v>929</v>
-      </c>
+      <c r="X20" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="n">
         <v>929</v>
       </c>
@@ -2355,6 +2415,9 @@
         <v>929</v>
       </c>
       <c r="AE20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2379,10 +2442,10 @@
       <c r="F21" t="n">
         <v>499</v>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="n">
-        <v>499</v>
-      </c>
+      <c r="G21" t="n">
+        <v>499</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>499</v>
       </c>
@@ -2407,10 +2470,10 @@
       <c r="P21" t="n">
         <v>499</v>
       </c>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q21" t="n">
+        <v>499</v>
+      </c>
+      <c r="R21" t="inlineStr"/>
       <c r="S21" t="n">
         <v>499</v>
       </c>
@@ -2448,6 +2511,9 @@
         <v>499</v>
       </c>
       <c r="AE21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2496,14 +2562,14 @@
       <c r="N22" t="n">
         <v>299</v>
       </c>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="n">
-        <v>299</v>
-      </c>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="n">
-        <v>299</v>
-      </c>
+      <c r="O22" t="n">
+        <v>299</v>
+      </c>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="n">
+        <v>299</v>
+      </c>
+      <c r="R22" t="inlineStr"/>
       <c r="S22" t="n">
         <v>299</v>
       </c>
@@ -2519,10 +2585,10 @@
       <c r="W22" t="n">
         <v>299</v>
       </c>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="n">
-        <v>299</v>
-      </c>
+      <c r="X22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="n">
         <v>299</v>
       </c>
@@ -2539,6 +2605,9 @@
         <v>299</v>
       </c>
       <c r="AE22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2590,11 +2659,11 @@
       <c r="O23" t="n">
         <v>1299</v>
       </c>
-      <c r="P23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>1299</v>
+      </c>
       <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="R23" t="inlineStr"/>
       <c r="S23" t="n">
         <v>1299</v>
       </c>
@@ -2610,10 +2679,10 @@
       <c r="W23" t="n">
         <v>1299</v>
       </c>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="X23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="n">
         <v>1299</v>
       </c>
@@ -2630,6 +2699,9 @@
         <v>1299</v>
       </c>
       <c r="AE23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AF23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2678,11 +2750,11 @@
       <c r="N24" t="n">
         <v>929</v>
       </c>
-      <c r="O24" t="inlineStr"/>
+      <c r="O24" t="n">
+        <v>929</v>
+      </c>
       <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="n">
         <v>929</v>
       </c>
@@ -2701,10 +2773,10 @@
       <c r="W24" t="n">
         <v>929</v>
       </c>
-      <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="n">
-        <v>929</v>
-      </c>
+      <c r="X24" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="n">
         <v>929</v>
       </c>
@@ -2721,6 +2793,9 @@
         <v>929</v>
       </c>
       <c r="AE24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2769,11 +2844,11 @@
       <c r="N25" t="n">
         <v>929</v>
       </c>
-      <c r="O25" t="inlineStr"/>
+      <c r="O25" t="n">
+        <v>929</v>
+      </c>
       <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q25" t="inlineStr"/>
       <c r="R25" t="n">
         <v>929</v>
       </c>
@@ -2792,10 +2867,10 @@
       <c r="W25" t="n">
         <v>929</v>
       </c>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="n">
-        <v>929</v>
-      </c>
+      <c r="X25" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="n">
         <v>929</v>
       </c>
@@ -2812,6 +2887,9 @@
         <v>929</v>
       </c>
       <c r="AE25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2860,14 +2938,14 @@
       <c r="N26" t="n">
         <v>1299</v>
       </c>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="O26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="R26" t="inlineStr"/>
       <c r="S26" t="n">
         <v>1299</v>
       </c>
@@ -2883,10 +2961,10 @@
       <c r="W26" t="n">
         <v>1299</v>
       </c>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="X26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="n">
         <v>1299</v>
       </c>
@@ -2903,6 +2981,9 @@
         <v>1299</v>
       </c>
       <c r="AE26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AF26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 05:05
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF26"/>
+  <dimension ref="A1:AG26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,7 @@
     <col width="21" customWidth="1" min="30" max="30"/>
     <col width="21" customWidth="1" min="31" max="31"/>
     <col width="21" customWidth="1" min="32" max="32"/>
+    <col width="21" customWidth="1" min="33" max="33"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -475,155 +476,160 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 10:31</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -662,10 +668,10 @@
       <c r="J2" t="n">
         <v>929</v>
       </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="n">
-        <v>929</v>
-      </c>
+      <c r="K2" t="n">
+        <v>929</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
         <v>929</v>
       </c>
@@ -678,25 +684,25 @@
       <c r="P2" t="n">
         <v>929</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
+      <c r="Q2" t="n">
+        <v>929</v>
+      </c>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="n">
-        <v>929</v>
-      </c>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="n">
         <v>929</v>
       </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="n">
-        <v>929</v>
-      </c>
+      <c r="U2" t="n">
+        <v>929</v>
+      </c>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="n">
         <v>929</v>
       </c>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="n">
-        <v>929</v>
-      </c>
+      <c r="X2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="n">
         <v>929</v>
       </c>
@@ -716,6 +722,9 @@
         <v>929</v>
       </c>
       <c r="AF2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -749,26 +758,26 @@
       <c r="I3" t="n">
         <v>569</v>
       </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>569</v>
+      </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>569</v>
-      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>569</v>
       </c>
       <c r="O3" t="n">
         <v>569</v>
       </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="n">
-        <v>569</v>
-      </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="n">
-        <v>569</v>
-      </c>
+      <c r="P3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="n">
+        <v>569</v>
+      </c>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="n">
         <v>569</v>
       </c>
@@ -784,10 +793,10 @@
       <c r="X3" t="n">
         <v>569</v>
       </c>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
         <v>569</v>
       </c>
@@ -804,6 +813,9 @@
         <v>569</v>
       </c>
       <c r="AF3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -855,10 +867,10 @@
       <c r="O4" t="n">
         <v>299</v>
       </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="n">
-        <v>299</v>
-      </c>
+      <c r="P4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
         <v>299</v>
       </c>
@@ -880,10 +892,10 @@
       <c r="X4" t="n">
         <v>299</v>
       </c>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
         <v>299</v>
       </c>
@@ -900,6 +912,9 @@
         <v>299</v>
       </c>
       <c r="AF4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -978,10 +993,10 @@
       <c r="X5" t="n">
         <v>569</v>
       </c>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y5" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
         <v>569</v>
       </c>
@@ -998,6 +1013,9 @@
         <v>569</v>
       </c>
       <c r="AF5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1052,10 +1070,10 @@
       <c r="P6" t="n">
         <v>499</v>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q6" t="n">
+        <v>499</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
       <c r="S6" t="n">
         <v>499</v>
       </c>
@@ -1074,10 +1092,10 @@
       <c r="X6" t="n">
         <v>499</v>
       </c>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
         <v>499</v>
       </c>
@@ -1094,6 +1112,9 @@
         <v>499</v>
       </c>
       <c r="AF6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1145,12 +1166,12 @@
       <c r="O7" t="n">
         <v>569</v>
       </c>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>569</v>
+      </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="n">
-        <v>569</v>
-      </c>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="n">
         <v>569</v>
       </c>
@@ -1166,10 +1187,10 @@
       <c r="X7" t="n">
         <v>569</v>
       </c>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y7" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
         <v>569</v>
       </c>
@@ -1186,6 +1207,9 @@
         <v>569</v>
       </c>
       <c r="AF7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1237,14 +1261,14 @@
       <c r="O8" t="n">
         <v>929</v>
       </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="n">
-        <v>929</v>
-      </c>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="n">
-        <v>929</v>
-      </c>
+      <c r="P8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="n">
+        <v>929</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
       <c r="T8" t="n">
         <v>929</v>
       </c>
@@ -1260,10 +1284,10 @@
       <c r="X8" t="n">
         <v>929</v>
       </c>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
         <v>929</v>
       </c>
@@ -1280,6 +1304,9 @@
         <v>929</v>
       </c>
       <c r="AF8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1331,10 +1358,10 @@
       <c r="O9" t="n">
         <v>299</v>
       </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="n">
-        <v>299</v>
-      </c>
+      <c r="P9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="n">
         <v>299</v>
       </c>
@@ -1356,10 +1383,10 @@
       <c r="X9" t="n">
         <v>299</v>
       </c>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
         <v>299</v>
       </c>
@@ -1376,6 +1403,9 @@
         <v>299</v>
       </c>
       <c r="AF9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1397,10 +1427,10 @@
       <c r="E10" t="n">
         <v>299</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>299</v>
-      </c>
+      <c r="F10" t="n">
+        <v>299</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>299</v>
       </c>
@@ -1425,14 +1455,14 @@
       <c r="O10" t="n">
         <v>299</v>
       </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="n">
-        <v>299</v>
-      </c>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="n">
-        <v>299</v>
-      </c>
+      <c r="P10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="n">
+        <v>299</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="n">
         <v>299</v>
       </c>
@@ -1448,10 +1478,10 @@
       <c r="X10" t="n">
         <v>299</v>
       </c>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
         <v>299</v>
       </c>
@@ -1468,6 +1498,9 @@
         <v>299</v>
       </c>
       <c r="AF10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1522,10 +1555,10 @@
       <c r="P11" t="n">
         <v>2997</v>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="n">
+      <c r="Q11" t="n">
         <v>2997</v>
       </c>
+      <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
         <v>2997</v>
       </c>
@@ -1539,15 +1572,15 @@
         <v>2997</v>
       </c>
       <c r="W11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="X11" t="n">
         <v>929</v>
       </c>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y11" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
         <v>929</v>
       </c>
@@ -1564,6 +1597,9 @@
         <v>929</v>
       </c>
       <c r="AF11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1621,10 +1657,10 @@
       <c r="Q12" t="n">
         <v>569</v>
       </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="n">
-        <v>569</v>
-      </c>
+      <c r="R12" t="n">
+        <v>569</v>
+      </c>
+      <c r="S12" t="inlineStr"/>
       <c r="T12" t="n">
         <v>569</v>
       </c>
@@ -1640,10 +1676,10 @@
       <c r="X12" t="n">
         <v>569</v>
       </c>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
         <v>569</v>
       </c>
@@ -1660,6 +1696,9 @@
         <v>569</v>
       </c>
       <c r="AF12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1711,14 +1750,14 @@
       <c r="O13" t="n">
         <v>569</v>
       </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="n">
-        <v>569</v>
-      </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="n">
-        <v>569</v>
-      </c>
+      <c r="P13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="n">
+        <v>569</v>
+      </c>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
         <v>569</v>
       </c>
@@ -1734,24 +1773,27 @@
       <c r="X13" t="n">
         <v>569</v>
       </c>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
         <v>569</v>
       </c>
       <c r="AB13" t="n">
         <v>569</v>
       </c>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="n">
         <v>569</v>
       </c>
       <c r="AF13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1773,10 +1815,10 @@
       <c r="E14" t="n">
         <v>794</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
+      <c r="F14" t="n">
         <v>794</v>
       </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
         <v>794</v>
       </c>
@@ -1784,7 +1826,7 @@
         <v>794</v>
       </c>
       <c r="J14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="K14" t="n">
         <v>499</v>
@@ -1801,11 +1843,11 @@
       <c r="O14" t="n">
         <v>499</v>
       </c>
-      <c r="P14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>499</v>
+      </c>
       <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="n">
-        <v>499</v>
-      </c>
+      <c r="R14" t="inlineStr"/>
       <c r="S14" t="n">
         <v>499</v>
       </c>
@@ -1846,6 +1888,9 @@
         <v>499</v>
       </c>
       <c r="AF14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1903,10 +1948,10 @@
       <c r="Q15" t="n">
         <v>499</v>
       </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="n">
-        <v>499</v>
-      </c>
+      <c r="R15" t="n">
+        <v>499</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="n">
         <v>499</v>
       </c>
@@ -1916,14 +1961,14 @@
       <c r="V15" t="n">
         <v>499</v>
       </c>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="n">
-        <v>499</v>
-      </c>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="n">
-        <v>499</v>
-      </c>
+      <c r="W15" t="n">
+        <v>499</v>
+      </c>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
         <v>499</v>
       </c>
@@ -1940,6 +1985,9 @@
         <v>499</v>
       </c>
       <c r="AF15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1982,17 +2030,17 @@
       <c r="L16" t="n">
         <v>299</v>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="n">
-        <v>299</v>
-      </c>
+      <c r="M16" t="n">
+        <v>299</v>
+      </c>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
         <v>299</v>
       </c>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="n">
-        <v>299</v>
-      </c>
+      <c r="P16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="n">
         <v>299</v>
       </c>
@@ -2014,10 +2062,10 @@
       <c r="X16" t="n">
         <v>299</v>
       </c>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
         <v>299</v>
       </c>
@@ -2034,6 +2082,9 @@
         <v>299</v>
       </c>
       <c r="AF16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2091,10 +2142,10 @@
       <c r="Q17" t="n">
         <v>929</v>
       </c>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="n">
-        <v>929</v>
-      </c>
+      <c r="R17" t="n">
+        <v>929</v>
+      </c>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="n">
         <v>929</v>
       </c>
@@ -2110,10 +2161,10 @@
       <c r="X17" t="n">
         <v>929</v>
       </c>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
         <v>929</v>
       </c>
@@ -2130,6 +2181,9 @@
         <v>929</v>
       </c>
       <c r="AF17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2184,11 +2238,11 @@
       <c r="P18" t="n">
         <v>499</v>
       </c>
-      <c r="Q18" t="inlineStr"/>
+      <c r="Q18" t="n">
+        <v>499</v>
+      </c>
       <c r="R18" t="inlineStr"/>
-      <c r="S18" t="n">
-        <v>499</v>
-      </c>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="n">
         <v>499</v>
       </c>
@@ -2204,10 +2258,10 @@
       <c r="X18" t="n">
         <v>499</v>
       </c>
-      <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y18" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
         <v>499</v>
       </c>
@@ -2224,6 +2278,9 @@
         <v>499</v>
       </c>
       <c r="AF18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2270,7 +2327,7 @@
         <v>1299</v>
       </c>
       <c r="N19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="O19" t="n">
         <v>1497</v>
@@ -2278,13 +2335,13 @@
       <c r="P19" t="n">
         <v>1497</v>
       </c>
-      <c r="Q19" t="inlineStr"/>
+      <c r="Q19" t="n">
+        <v>1497</v>
+      </c>
       <c r="R19" t="inlineStr"/>
-      <c r="S19" t="n">
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="n">
         <v>465</v>
-      </c>
-      <c r="T19" t="n">
-        <v>1497</v>
       </c>
       <c r="U19" t="n">
         <v>1497</v>
@@ -2320,6 +2377,9 @@
         <v>1497</v>
       </c>
       <c r="AF19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AG19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2398,10 +2458,10 @@
       <c r="X20" t="n">
         <v>929</v>
       </c>
-      <c r="Y20" t="inlineStr"/>
-      <c r="Z20" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y20" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z20" t="inlineStr"/>
       <c r="AA20" t="n">
         <v>929</v>
       </c>
@@ -2418,6 +2478,9 @@
         <v>929</v>
       </c>
       <c r="AF20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2445,10 +2508,10 @@
       <c r="G21" t="n">
         <v>499</v>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="n">
-        <v>499</v>
-      </c>
+      <c r="H21" t="n">
+        <v>499</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
         <v>499</v>
       </c>
@@ -2473,10 +2536,10 @@
       <c r="Q21" t="n">
         <v>499</v>
       </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="n">
-        <v>499</v>
-      </c>
+      <c r="R21" t="n">
+        <v>499</v>
+      </c>
+      <c r="S21" t="inlineStr"/>
       <c r="T21" t="n">
         <v>499</v>
       </c>
@@ -2514,6 +2577,9 @@
         <v>499</v>
       </c>
       <c r="AF21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2565,14 +2631,14 @@
       <c r="O22" t="n">
         <v>299</v>
       </c>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="n">
-        <v>299</v>
-      </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="n">
-        <v>299</v>
-      </c>
+      <c r="P22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="n">
+        <v>299</v>
+      </c>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="n">
         <v>299</v>
       </c>
@@ -2588,10 +2654,10 @@
       <c r="X22" t="n">
         <v>299</v>
       </c>
-      <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="n">
         <v>299</v>
       </c>
@@ -2608,6 +2674,9 @@
         <v>299</v>
       </c>
       <c r="AF22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2662,11 +2731,11 @@
       <c r="P23" t="n">
         <v>1299</v>
       </c>
-      <c r="Q23" t="inlineStr"/>
+      <c r="Q23" t="n">
+        <v>1299</v>
+      </c>
       <c r="R23" t="inlineStr"/>
-      <c r="S23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="n">
         <v>1299</v>
       </c>
@@ -2682,10 +2751,10 @@
       <c r="X23" t="n">
         <v>1299</v>
       </c>
-      <c r="Y23" t="inlineStr"/>
-      <c r="Z23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Y23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
         <v>1299</v>
       </c>
@@ -2702,6 +2771,9 @@
         <v>1299</v>
       </c>
       <c r="AF23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AG23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2753,11 +2825,11 @@
       <c r="O24" t="n">
         <v>929</v>
       </c>
-      <c r="P24" t="inlineStr"/>
+      <c r="P24" t="n">
+        <v>929</v>
+      </c>
       <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="n">
-        <v>929</v>
-      </c>
+      <c r="R24" t="inlineStr"/>
       <c r="S24" t="n">
         <v>929</v>
       </c>
@@ -2776,10 +2848,10 @@
       <c r="X24" t="n">
         <v>929</v>
       </c>
-      <c r="Y24" t="inlineStr"/>
-      <c r="Z24" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y24" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
         <v>929</v>
       </c>
@@ -2796,6 +2868,9 @@
         <v>929</v>
       </c>
       <c r="AF24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2847,11 +2922,11 @@
       <c r="O25" t="n">
         <v>929</v>
       </c>
-      <c r="P25" t="inlineStr"/>
+      <c r="P25" t="n">
+        <v>929</v>
+      </c>
       <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="n">
-        <v>929</v>
-      </c>
+      <c r="R25" t="inlineStr"/>
       <c r="S25" t="n">
         <v>929</v>
       </c>
@@ -2870,10 +2945,10 @@
       <c r="X25" t="n">
         <v>929</v>
       </c>
-      <c r="Y25" t="inlineStr"/>
-      <c r="Z25" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y25" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
         <v>929</v>
       </c>
@@ -2890,6 +2965,9 @@
         <v>929</v>
       </c>
       <c r="AF25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2941,14 +3019,14 @@
       <c r="O26" t="n">
         <v>1299</v>
       </c>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="P26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="n">
         <v>1299</v>
       </c>
@@ -2964,10 +3042,10 @@
       <c r="X26" t="n">
         <v>1299</v>
       </c>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Y26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
         <v>1299</v>
       </c>
@@ -2984,6 +3062,9 @@
         <v>1299</v>
       </c>
       <c r="AF26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AG26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 07:06
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG26"/>
+  <dimension ref="A1:AH26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,7 @@
     <col width="21" customWidth="1" min="31" max="31"/>
     <col width="21" customWidth="1" min="32" max="32"/>
     <col width="21" customWidth="1" min="33" max="33"/>
+    <col width="21" customWidth="1" min="34" max="34"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -476,160 +477,165 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 12:32</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -671,10 +677,10 @@
       <c r="K2" t="n">
         <v>929</v>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>929</v>
-      </c>
+      <c r="L2" t="n">
+        <v>929</v>
+      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
         <v>929</v>
       </c>
@@ -687,25 +693,25 @@
       <c r="Q2" t="n">
         <v>929</v>
       </c>
-      <c r="R2" t="inlineStr"/>
+      <c r="R2" t="n">
+        <v>929</v>
+      </c>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="n">
-        <v>929</v>
-      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
         <v>929</v>
       </c>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="n">
-        <v>929</v>
-      </c>
+      <c r="V2" t="n">
+        <v>929</v>
+      </c>
+      <c r="W2" t="inlineStr"/>
       <c r="X2" t="n">
         <v>929</v>
       </c>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
         <v>929</v>
       </c>
@@ -725,6 +731,9 @@
         <v>929</v>
       </c>
       <c r="AG2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -761,26 +770,26 @@
       <c r="J3" t="n">
         <v>569</v>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>569</v>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="n">
-        <v>569</v>
-      </c>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="n">
         <v>569</v>
       </c>
       <c r="P3" t="n">
         <v>569</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="n">
-        <v>569</v>
-      </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q3" t="n">
+        <v>569</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="n">
+        <v>569</v>
+      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
         <v>569</v>
       </c>
@@ -796,10 +805,10 @@
       <c r="Y3" t="n">
         <v>569</v>
       </c>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="n">
         <v>569</v>
       </c>
@@ -816,6 +825,9 @@
         <v>569</v>
       </c>
       <c r="AG3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -870,10 +882,10 @@
       <c r="P4" t="n">
         <v>299</v>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q4" t="n">
+        <v>299</v>
+      </c>
+      <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
         <v>299</v>
       </c>
@@ -895,10 +907,10 @@
       <c r="Y4" t="n">
         <v>299</v>
       </c>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="n">
         <v>299</v>
       </c>
@@ -915,6 +927,9 @@
         <v>299</v>
       </c>
       <c r="AG4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -996,10 +1011,10 @@
       <c r="Y5" t="n">
         <v>569</v>
       </c>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="n">
         <v>569</v>
       </c>
@@ -1016,6 +1031,9 @@
         <v>569</v>
       </c>
       <c r="AG5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1073,10 +1091,10 @@
       <c r="Q6" t="n">
         <v>499</v>
       </c>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="n">
-        <v>499</v>
-      </c>
+      <c r="R6" t="n">
+        <v>499</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="n">
         <v>499</v>
       </c>
@@ -1095,10 +1113,10 @@
       <c r="Y6" t="n">
         <v>499</v>
       </c>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="n">
         <v>499</v>
       </c>
@@ -1115,6 +1133,9 @@
         <v>499</v>
       </c>
       <c r="AG6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1169,12 +1190,12 @@
       <c r="P7" t="n">
         <v>569</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
+      <c r="Q7" t="n">
+        <v>569</v>
+      </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
-      <c r="T7" t="n">
-        <v>569</v>
-      </c>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="n">
         <v>569</v>
       </c>
@@ -1190,10 +1211,10 @@
       <c r="Y7" t="n">
         <v>569</v>
       </c>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="n">
         <v>569</v>
       </c>
@@ -1210,6 +1231,9 @@
         <v>569</v>
       </c>
       <c r="AG7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1264,14 +1288,14 @@
       <c r="P8" t="n">
         <v>929</v>
       </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="n">
-        <v>929</v>
-      </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q8" t="n">
+        <v>929</v>
+      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="n">
+        <v>929</v>
+      </c>
+      <c r="T8" t="inlineStr"/>
       <c r="U8" t="n">
         <v>929</v>
       </c>
@@ -1287,10 +1311,10 @@
       <c r="Y8" t="n">
         <v>929</v>
       </c>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="n">
         <v>929</v>
       </c>
@@ -1307,6 +1331,9 @@
         <v>929</v>
       </c>
       <c r="AG8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1361,10 +1388,10 @@
       <c r="P9" t="n">
         <v>299</v>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q9" t="n">
+        <v>299</v>
+      </c>
+      <c r="R9" t="inlineStr"/>
       <c r="S9" t="n">
         <v>299</v>
       </c>
@@ -1386,10 +1413,10 @@
       <c r="Y9" t="n">
         <v>299</v>
       </c>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="n">
         <v>299</v>
       </c>
@@ -1406,6 +1433,9 @@
         <v>299</v>
       </c>
       <c r="AG9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1430,10 +1460,10 @@
       <c r="F10" t="n">
         <v>299</v>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>299</v>
-      </c>
+      <c r="G10" t="n">
+        <v>299</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>299</v>
       </c>
@@ -1458,14 +1488,14 @@
       <c r="P10" t="n">
         <v>299</v>
       </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="n">
-        <v>299</v>
-      </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q10" t="n">
+        <v>299</v>
+      </c>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="n">
+        <v>299</v>
+      </c>
+      <c r="T10" t="inlineStr"/>
       <c r="U10" t="n">
         <v>299</v>
       </c>
@@ -1481,10 +1511,10 @@
       <c r="Y10" t="n">
         <v>299</v>
       </c>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="n">
         <v>299</v>
       </c>
@@ -1501,6 +1531,9 @@
         <v>299</v>
       </c>
       <c r="AG10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1558,10 +1591,10 @@
       <c r="Q11" t="n">
         <v>2997</v>
       </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="n">
+      <c r="R11" t="n">
         <v>2997</v>
       </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="n">
         <v>2997</v>
       </c>
@@ -1575,15 +1608,15 @@
         <v>2997</v>
       </c>
       <c r="X11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="Y11" t="n">
         <v>929</v>
       </c>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="n">
         <v>929</v>
       </c>
@@ -1600,6 +1633,9 @@
         <v>929</v>
       </c>
       <c r="AG11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1660,10 +1696,10 @@
       <c r="R12" t="n">
         <v>569</v>
       </c>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="n">
-        <v>569</v>
-      </c>
+      <c r="S12" t="n">
+        <v>569</v>
+      </c>
+      <c r="T12" t="inlineStr"/>
       <c r="U12" t="n">
         <v>569</v>
       </c>
@@ -1679,10 +1715,10 @@
       <c r="Y12" t="n">
         <v>569</v>
       </c>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="n">
         <v>569</v>
       </c>
@@ -1699,6 +1735,9 @@
         <v>569</v>
       </c>
       <c r="AG12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1753,14 +1792,14 @@
       <c r="P13" t="n">
         <v>569</v>
       </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="n">
-        <v>569</v>
-      </c>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q13" t="n">
+        <v>569</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="n">
+        <v>569</v>
+      </c>
+      <c r="T13" t="inlineStr"/>
       <c r="U13" t="n">
         <v>569</v>
       </c>
@@ -1776,24 +1815,27 @@
       <c r="Y13" t="n">
         <v>569</v>
       </c>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="n">
         <v>569</v>
       </c>
       <c r="AC13" t="n">
         <v>569</v>
       </c>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="n">
         <v>569</v>
       </c>
       <c r="AG13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1818,10 +1860,10 @@
       <c r="F14" t="n">
         <v>794</v>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="n">
+      <c r="G14" t="n">
         <v>794</v>
       </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
         <v>794</v>
       </c>
@@ -1829,7 +1871,7 @@
         <v>794</v>
       </c>
       <c r="K14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="L14" t="n">
         <v>499</v>
@@ -1846,11 +1888,11 @@
       <c r="P14" t="n">
         <v>499</v>
       </c>
-      <c r="Q14" t="inlineStr"/>
+      <c r="Q14" t="n">
+        <v>499</v>
+      </c>
       <c r="R14" t="inlineStr"/>
-      <c r="S14" t="n">
-        <v>499</v>
-      </c>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="n">
         <v>499</v>
       </c>
@@ -1891,6 +1933,9 @@
         <v>499</v>
       </c>
       <c r="AG14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1951,10 +1996,10 @@
       <c r="R15" t="n">
         <v>499</v>
       </c>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="n">
-        <v>499</v>
-      </c>
+      <c r="S15" t="n">
+        <v>499</v>
+      </c>
+      <c r="T15" t="inlineStr"/>
       <c r="U15" t="n">
         <v>499</v>
       </c>
@@ -1964,14 +2009,14 @@
       <c r="W15" t="n">
         <v>499</v>
       </c>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="n">
-        <v>499</v>
-      </c>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="n">
-        <v>499</v>
-      </c>
+      <c r="X15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="n">
         <v>499</v>
       </c>
@@ -1988,6 +2033,9 @@
         <v>499</v>
       </c>
       <c r="AG15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2033,17 +2081,17 @@
       <c r="M16" t="n">
         <v>299</v>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="n">
-        <v>299</v>
-      </c>
+      <c r="N16" t="n">
+        <v>299</v>
+      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
         <v>299</v>
       </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q16" t="n">
+        <v>299</v>
+      </c>
+      <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
         <v>299</v>
       </c>
@@ -2065,10 +2113,10 @@
       <c r="Y16" t="n">
         <v>299</v>
       </c>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="n">
         <v>299</v>
       </c>
@@ -2085,6 +2133,9 @@
         <v>299</v>
       </c>
       <c r="AG16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2145,10 +2196,10 @@
       <c r="R17" t="n">
         <v>929</v>
       </c>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="n">
-        <v>929</v>
-      </c>
+      <c r="S17" t="n">
+        <v>929</v>
+      </c>
+      <c r="T17" t="inlineStr"/>
       <c r="U17" t="n">
         <v>929</v>
       </c>
@@ -2164,10 +2215,10 @@
       <c r="Y17" t="n">
         <v>929</v>
       </c>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="n">
         <v>929</v>
       </c>
@@ -2184,6 +2235,9 @@
         <v>929</v>
       </c>
       <c r="AG17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2241,11 +2295,11 @@
       <c r="Q18" t="n">
         <v>499</v>
       </c>
-      <c r="R18" t="inlineStr"/>
+      <c r="R18" t="n">
+        <v>499</v>
+      </c>
       <c r="S18" t="inlineStr"/>
-      <c r="T18" t="n">
-        <v>499</v>
-      </c>
+      <c r="T18" t="inlineStr"/>
       <c r="U18" t="n">
         <v>499</v>
       </c>
@@ -2261,10 +2315,10 @@
       <c r="Y18" t="n">
         <v>499</v>
       </c>
-      <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="n">
         <v>499</v>
       </c>
@@ -2281,6 +2335,9 @@
         <v>499</v>
       </c>
       <c r="AG18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2330,7 +2387,7 @@
         <v>1299</v>
       </c>
       <c r="O19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="P19" t="n">
         <v>1497</v>
@@ -2338,13 +2395,13 @@
       <c r="Q19" t="n">
         <v>1497</v>
       </c>
-      <c r="R19" t="inlineStr"/>
+      <c r="R19" t="n">
+        <v>1497</v>
+      </c>
       <c r="S19" t="inlineStr"/>
-      <c r="T19" t="n">
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="n">
         <v>465</v>
-      </c>
-      <c r="U19" t="n">
-        <v>1497</v>
       </c>
       <c r="V19" t="n">
         <v>1497</v>
@@ -2380,6 +2437,9 @@
         <v>1497</v>
       </c>
       <c r="AG19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AH19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2461,10 +2521,10 @@
       <c r="Y20" t="n">
         <v>929</v>
       </c>
-      <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="n">
         <v>929</v>
       </c>
@@ -2481,6 +2541,9 @@
         <v>929</v>
       </c>
       <c r="AG20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2511,10 +2574,10 @@
       <c r="H21" t="n">
         <v>499</v>
       </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>499</v>
-      </c>
+      <c r="I21" t="n">
+        <v>499</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>499</v>
       </c>
@@ -2539,10 +2602,10 @@
       <c r="R21" t="n">
         <v>499</v>
       </c>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="n">
-        <v>499</v>
-      </c>
+      <c r="S21" t="n">
+        <v>499</v>
+      </c>
+      <c r="T21" t="inlineStr"/>
       <c r="U21" t="n">
         <v>499</v>
       </c>
@@ -2580,6 +2643,9 @@
         <v>499</v>
       </c>
       <c r="AG21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2634,14 +2700,14 @@
       <c r="P22" t="n">
         <v>299</v>
       </c>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="n">
-        <v>299</v>
-      </c>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q22" t="n">
+        <v>299</v>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="n">
+        <v>299</v>
+      </c>
+      <c r="T22" t="inlineStr"/>
       <c r="U22" t="n">
         <v>299</v>
       </c>
@@ -2657,10 +2723,10 @@
       <c r="Y22" t="n">
         <v>299</v>
       </c>
-      <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="n">
         <v>299</v>
       </c>
@@ -2677,6 +2743,9 @@
         <v>299</v>
       </c>
       <c r="AG22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2734,11 +2803,11 @@
       <c r="Q23" t="n">
         <v>1299</v>
       </c>
-      <c r="R23" t="inlineStr"/>
+      <c r="R23" t="n">
+        <v>1299</v>
+      </c>
       <c r="S23" t="inlineStr"/>
-      <c r="T23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="T23" t="inlineStr"/>
       <c r="U23" t="n">
         <v>1299</v>
       </c>
@@ -2754,10 +2823,10 @@
       <c r="Y23" t="n">
         <v>1299</v>
       </c>
-      <c r="Z23" t="inlineStr"/>
-      <c r="AA23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Z23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="n">
         <v>1299</v>
       </c>
@@ -2774,6 +2843,9 @@
         <v>1299</v>
       </c>
       <c r="AG23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AH23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2828,11 +2900,11 @@
       <c r="P24" t="n">
         <v>929</v>
       </c>
-      <c r="Q24" t="inlineStr"/>
+      <c r="Q24" t="n">
+        <v>929</v>
+      </c>
       <c r="R24" t="inlineStr"/>
-      <c r="S24" t="n">
-        <v>929</v>
-      </c>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="n">
         <v>929</v>
       </c>
@@ -2851,10 +2923,10 @@
       <c r="Y24" t="n">
         <v>929</v>
       </c>
-      <c r="Z24" t="inlineStr"/>
-      <c r="AA24" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="n">
         <v>929</v>
       </c>
@@ -2871,6 +2943,9 @@
         <v>929</v>
       </c>
       <c r="AG24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2925,11 +3000,11 @@
       <c r="P25" t="n">
         <v>929</v>
       </c>
-      <c r="Q25" t="inlineStr"/>
+      <c r="Q25" t="n">
+        <v>929</v>
+      </c>
       <c r="R25" t="inlineStr"/>
-      <c r="S25" t="n">
-        <v>929</v>
-      </c>
+      <c r="S25" t="inlineStr"/>
       <c r="T25" t="n">
         <v>929</v>
       </c>
@@ -2948,10 +3023,10 @@
       <c r="Y25" t="n">
         <v>929</v>
       </c>
-      <c r="Z25" t="inlineStr"/>
-      <c r="AA25" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="n">
         <v>929</v>
       </c>
@@ -2968,6 +3043,9 @@
         <v>929</v>
       </c>
       <c r="AG25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3022,14 +3100,14 @@
       <c r="P26" t="n">
         <v>1299</v>
       </c>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Q26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="T26" t="inlineStr"/>
       <c r="U26" t="n">
         <v>1299</v>
       </c>
@@ -3045,10 +3123,10 @@
       <c r="Y26" t="n">
         <v>1299</v>
       </c>
-      <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Z26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="n">
         <v>1299</v>
       </c>
@@ -3065,6 +3143,9 @@
         <v>1299</v>
       </c>
       <c r="AG26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AH26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 09:02
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH26"/>
+  <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,7 @@
     <col width="21" customWidth="1" min="32" max="32"/>
     <col width="21" customWidth="1" min="33" max="33"/>
     <col width="21" customWidth="1" min="34" max="34"/>
+    <col width="21" customWidth="1" min="35" max="35"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -477,165 +478,170 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 14:27</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -680,10 +686,10 @@
       <c r="L2" t="n">
         <v>929</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="n">
-        <v>929</v>
-      </c>
+      <c r="M2" t="n">
+        <v>929</v>
+      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
         <v>929</v>
       </c>
@@ -696,25 +702,25 @@
       <c r="R2" t="n">
         <v>929</v>
       </c>
-      <c r="S2" t="inlineStr"/>
+      <c r="S2" t="n">
+        <v>929</v>
+      </c>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
-        <v>929</v>
-      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="n">
         <v>929</v>
       </c>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="n">
-        <v>929</v>
-      </c>
+      <c r="W2" t="n">
+        <v>929</v>
+      </c>
+      <c r="X2" t="inlineStr"/>
       <c r="Y2" t="n">
         <v>929</v>
       </c>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="n">
         <v>929</v>
       </c>
@@ -734,6 +740,9 @@
         <v>929</v>
       </c>
       <c r="AH2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -773,26 +782,26 @@
       <c r="K3" t="n">
         <v>569</v>
       </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>569</v>
+      </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
-        <v>569</v>
-      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
         <v>569</v>
       </c>
       <c r="Q3" t="n">
         <v>569</v>
       </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="n">
-        <v>569</v>
-      </c>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
-        <v>569</v>
-      </c>
+      <c r="R3" t="n">
+        <v>569</v>
+      </c>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>569</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
       <c r="V3" t="n">
         <v>569</v>
       </c>
@@ -808,10 +817,10 @@
       <c r="Z3" t="n">
         <v>569</v>
       </c>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="n">
         <v>569</v>
       </c>
@@ -828,6 +837,9 @@
         <v>569</v>
       </c>
       <c r="AH3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -885,10 +897,10 @@
       <c r="Q4" t="n">
         <v>299</v>
       </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="n">
-        <v>299</v>
-      </c>
+      <c r="R4" t="n">
+        <v>299</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="n">
         <v>299</v>
       </c>
@@ -910,10 +922,10 @@
       <c r="Z4" t="n">
         <v>299</v>
       </c>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="n">
         <v>299</v>
       </c>
@@ -930,6 +942,9 @@
         <v>299</v>
       </c>
       <c r="AH4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1014,10 +1029,10 @@
       <c r="Z5" t="n">
         <v>569</v>
       </c>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="n">
         <v>569</v>
       </c>
@@ -1034,6 +1049,9 @@
         <v>569</v>
       </c>
       <c r="AH5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1094,10 +1112,10 @@
       <c r="R6" t="n">
         <v>499</v>
       </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="n">
-        <v>499</v>
-      </c>
+      <c r="S6" t="n">
+        <v>499</v>
+      </c>
+      <c r="T6" t="inlineStr"/>
       <c r="U6" t="n">
         <v>499</v>
       </c>
@@ -1116,10 +1134,10 @@
       <c r="Z6" t="n">
         <v>499</v>
       </c>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="n">
         <v>499</v>
       </c>
@@ -1136,6 +1154,9 @@
         <v>499</v>
       </c>
       <c r="AH6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1193,12 +1214,12 @@
       <c r="Q7" t="n">
         <v>569</v>
       </c>
-      <c r="R7" t="inlineStr"/>
+      <c r="R7" t="n">
+        <v>569</v>
+      </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="n">
-        <v>569</v>
-      </c>
+      <c r="U7" t="inlineStr"/>
       <c r="V7" t="n">
         <v>569</v>
       </c>
@@ -1214,10 +1235,10 @@
       <c r="Z7" t="n">
         <v>569</v>
       </c>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="n">
         <v>569</v>
       </c>
@@ -1234,6 +1255,9 @@
         <v>569</v>
       </c>
       <c r="AH7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1291,14 +1315,14 @@
       <c r="Q8" t="n">
         <v>929</v>
       </c>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="n">
-        <v>929</v>
-      </c>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="n">
-        <v>929</v>
-      </c>
+      <c r="R8" t="n">
+        <v>929</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="n">
+        <v>929</v>
+      </c>
+      <c r="U8" t="inlineStr"/>
       <c r="V8" t="n">
         <v>929</v>
       </c>
@@ -1314,10 +1338,10 @@
       <c r="Z8" t="n">
         <v>929</v>
       </c>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="n">
         <v>929</v>
       </c>
@@ -1334,6 +1358,9 @@
         <v>929</v>
       </c>
       <c r="AH8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1391,10 +1418,10 @@
       <c r="Q9" t="n">
         <v>299</v>
       </c>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="n">
-        <v>299</v>
-      </c>
+      <c r="R9" t="n">
+        <v>299</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="n">
         <v>299</v>
       </c>
@@ -1416,10 +1443,10 @@
       <c r="Z9" t="n">
         <v>299</v>
       </c>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="n">
         <v>299</v>
       </c>
@@ -1436,6 +1463,9 @@
         <v>299</v>
       </c>
       <c r="AH9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1463,10 +1493,10 @@
       <c r="G10" t="n">
         <v>299</v>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
-        <v>299</v>
-      </c>
+      <c r="H10" t="n">
+        <v>299</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="n">
         <v>299</v>
       </c>
@@ -1491,14 +1521,14 @@
       <c r="Q10" t="n">
         <v>299</v>
       </c>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="n">
-        <v>299</v>
-      </c>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="n">
-        <v>299</v>
-      </c>
+      <c r="R10" t="n">
+        <v>299</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="n">
+        <v>299</v>
+      </c>
+      <c r="U10" t="inlineStr"/>
       <c r="V10" t="n">
         <v>299</v>
       </c>
@@ -1514,10 +1544,10 @@
       <c r="Z10" t="n">
         <v>299</v>
       </c>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="n">
         <v>299</v>
       </c>
@@ -1534,6 +1564,9 @@
         <v>299</v>
       </c>
       <c r="AH10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1594,10 +1627,10 @@
       <c r="R11" t="n">
         <v>2997</v>
       </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="n">
+      <c r="S11" t="n">
         <v>2997</v>
       </c>
+      <c r="T11" t="inlineStr"/>
       <c r="U11" t="n">
         <v>2997</v>
       </c>
@@ -1611,15 +1644,15 @@
         <v>2997</v>
       </c>
       <c r="Y11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="Z11" t="n">
         <v>929</v>
       </c>
-      <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="n">
         <v>929</v>
       </c>
@@ -1636,6 +1669,9 @@
         <v>929</v>
       </c>
       <c r="AH11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1699,10 +1735,10 @@
       <c r="S12" t="n">
         <v>569</v>
       </c>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="n">
-        <v>569</v>
-      </c>
+      <c r="T12" t="n">
+        <v>569</v>
+      </c>
+      <c r="U12" t="inlineStr"/>
       <c r="V12" t="n">
         <v>569</v>
       </c>
@@ -1718,10 +1754,10 @@
       <c r="Z12" t="n">
         <v>569</v>
       </c>
-      <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="n">
         <v>569</v>
       </c>
@@ -1738,6 +1774,9 @@
         <v>569</v>
       </c>
       <c r="AH12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1747,9 +1786,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
         <v>569</v>
       </c>
@@ -1795,14 +1832,14 @@
       <c r="Q13" t="n">
         <v>569</v>
       </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="n">
-        <v>569</v>
-      </c>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="n">
-        <v>569</v>
-      </c>
+      <c r="R13" t="n">
+        <v>569</v>
+      </c>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="n">
+        <v>569</v>
+      </c>
+      <c r="U13" t="inlineStr"/>
       <c r="V13" t="n">
         <v>569</v>
       </c>
@@ -1818,24 +1855,27 @@
       <c r="Z13" t="n">
         <v>569</v>
       </c>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="n">
         <v>569</v>
       </c>
       <c r="AD13" t="n">
         <v>569</v>
       </c>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF13" t="inlineStr"/>
       <c r="AG13" t="n">
         <v>569</v>
       </c>
       <c r="AH13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1863,10 +1903,10 @@
       <c r="G14" t="n">
         <v>794</v>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="n">
+      <c r="H14" t="n">
         <v>794</v>
       </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="n">
         <v>794</v>
       </c>
@@ -1874,7 +1914,7 @@
         <v>794</v>
       </c>
       <c r="L14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="M14" t="n">
         <v>499</v>
@@ -1891,11 +1931,11 @@
       <c r="Q14" t="n">
         <v>499</v>
       </c>
-      <c r="R14" t="inlineStr"/>
+      <c r="R14" t="n">
+        <v>499</v>
+      </c>
       <c r="S14" t="inlineStr"/>
-      <c r="T14" t="n">
-        <v>499</v>
-      </c>
+      <c r="T14" t="inlineStr"/>
       <c r="U14" t="n">
         <v>499</v>
       </c>
@@ -1936,6 +1976,9 @@
         <v>499</v>
       </c>
       <c r="AH14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1999,10 +2042,10 @@
       <c r="S15" t="n">
         <v>499</v>
       </c>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="n">
-        <v>499</v>
-      </c>
+      <c r="T15" t="n">
+        <v>499</v>
+      </c>
+      <c r="U15" t="inlineStr"/>
       <c r="V15" t="n">
         <v>499</v>
       </c>
@@ -2012,14 +2055,14 @@
       <c r="X15" t="n">
         <v>499</v>
       </c>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="n">
         <v>499</v>
       </c>
@@ -2036,6 +2079,9 @@
         <v>499</v>
       </c>
       <c r="AH15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2084,17 +2130,17 @@
       <c r="N16" t="n">
         <v>299</v>
       </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="n">
-        <v>299</v>
-      </c>
+      <c r="O16" t="n">
+        <v>299</v>
+      </c>
+      <c r="P16" t="inlineStr"/>
       <c r="Q16" t="n">
         <v>299</v>
       </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="n">
-        <v>299</v>
-      </c>
+      <c r="R16" t="n">
+        <v>299</v>
+      </c>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="n">
         <v>299</v>
       </c>
@@ -2116,10 +2162,10 @@
       <c r="Z16" t="n">
         <v>299</v>
       </c>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="n">
         <v>299</v>
       </c>
@@ -2136,6 +2182,9 @@
         <v>299</v>
       </c>
       <c r="AH16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2199,10 +2248,10 @@
       <c r="S17" t="n">
         <v>929</v>
       </c>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="n">
-        <v>929</v>
-      </c>
+      <c r="T17" t="n">
+        <v>929</v>
+      </c>
+      <c r="U17" t="inlineStr"/>
       <c r="V17" t="n">
         <v>929</v>
       </c>
@@ -2218,10 +2267,10 @@
       <c r="Z17" t="n">
         <v>929</v>
       </c>
-      <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="n">
         <v>929</v>
       </c>
@@ -2238,6 +2287,9 @@
         <v>929</v>
       </c>
       <c r="AH17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2298,11 +2350,11 @@
       <c r="R18" t="n">
         <v>499</v>
       </c>
-      <c r="S18" t="inlineStr"/>
+      <c r="S18" t="n">
+        <v>499</v>
+      </c>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="n">
-        <v>499</v>
-      </c>
+      <c r="U18" t="inlineStr"/>
       <c r="V18" t="n">
         <v>499</v>
       </c>
@@ -2318,10 +2370,10 @@
       <c r="Z18" t="n">
         <v>499</v>
       </c>
-      <c r="AA18" t="inlineStr"/>
-      <c r="AB18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="n">
         <v>499</v>
       </c>
@@ -2338,6 +2390,9 @@
         <v>499</v>
       </c>
       <c r="AH18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2390,7 +2445,7 @@
         <v>1299</v>
       </c>
       <c r="P19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="Q19" t="n">
         <v>1497</v>
@@ -2398,13 +2453,13 @@
       <c r="R19" t="n">
         <v>1497</v>
       </c>
-      <c r="S19" t="inlineStr"/>
+      <c r="S19" t="n">
+        <v>1497</v>
+      </c>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="n">
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="n">
         <v>465</v>
-      </c>
-      <c r="V19" t="n">
-        <v>1497</v>
       </c>
       <c r="W19" t="n">
         <v>1497</v>
@@ -2440,6 +2495,9 @@
         <v>1497</v>
       </c>
       <c r="AH19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AI19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2524,10 +2582,10 @@
       <c r="Z20" t="n">
         <v>929</v>
       </c>
-      <c r="AA20" t="inlineStr"/>
-      <c r="AB20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="n">
         <v>929</v>
       </c>
@@ -2544,6 +2602,9 @@
         <v>929</v>
       </c>
       <c r="AH20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2577,10 +2638,10 @@
       <c r="I21" t="n">
         <v>499</v>
       </c>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="n">
-        <v>499</v>
-      </c>
+      <c r="J21" t="n">
+        <v>499</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="n">
         <v>499</v>
       </c>
@@ -2605,10 +2666,10 @@
       <c r="S21" t="n">
         <v>499</v>
       </c>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="n">
-        <v>499</v>
-      </c>
+      <c r="T21" t="n">
+        <v>499</v>
+      </c>
+      <c r="U21" t="inlineStr"/>
       <c r="V21" t="n">
         <v>499</v>
       </c>
@@ -2646,6 +2707,9 @@
         <v>499</v>
       </c>
       <c r="AH21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2703,14 +2767,14 @@
       <c r="Q22" t="n">
         <v>299</v>
       </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="n">
-        <v>299</v>
-      </c>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="n">
-        <v>299</v>
-      </c>
+      <c r="R22" t="n">
+        <v>299</v>
+      </c>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="n">
+        <v>299</v>
+      </c>
+      <c r="U22" t="inlineStr"/>
       <c r="V22" t="n">
         <v>299</v>
       </c>
@@ -2726,10 +2790,10 @@
       <c r="Z22" t="n">
         <v>299</v>
       </c>
-      <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="n">
         <v>299</v>
       </c>
@@ -2746,6 +2810,9 @@
         <v>299</v>
       </c>
       <c r="AH22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2806,11 +2873,11 @@
       <c r="R23" t="n">
         <v>1299</v>
       </c>
-      <c r="S23" t="inlineStr"/>
+      <c r="S23" t="n">
+        <v>1299</v>
+      </c>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="U23" t="inlineStr"/>
       <c r="V23" t="n">
         <v>1299</v>
       </c>
@@ -2826,10 +2893,10 @@
       <c r="Z23" t="n">
         <v>1299</v>
       </c>
-      <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AA23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="n">
         <v>1299</v>
       </c>
@@ -2846,6 +2913,9 @@
         <v>1299</v>
       </c>
       <c r="AH23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AI23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2903,11 +2973,11 @@
       <c r="Q24" t="n">
         <v>929</v>
       </c>
-      <c r="R24" t="inlineStr"/>
+      <c r="R24" t="n">
+        <v>929</v>
+      </c>
       <c r="S24" t="inlineStr"/>
-      <c r="T24" t="n">
-        <v>929</v>
-      </c>
+      <c r="T24" t="inlineStr"/>
       <c r="U24" t="n">
         <v>929</v>
       </c>
@@ -2926,10 +2996,10 @@
       <c r="Z24" t="n">
         <v>929</v>
       </c>
-      <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="n">
         <v>929</v>
       </c>
@@ -2946,6 +3016,9 @@
         <v>929</v>
       </c>
       <c r="AH24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3003,11 +3076,11 @@
       <c r="Q25" t="n">
         <v>929</v>
       </c>
-      <c r="R25" t="inlineStr"/>
+      <c r="R25" t="n">
+        <v>929</v>
+      </c>
       <c r="S25" t="inlineStr"/>
-      <c r="T25" t="n">
-        <v>929</v>
-      </c>
+      <c r="T25" t="inlineStr"/>
       <c r="U25" t="n">
         <v>929</v>
       </c>
@@ -3026,10 +3099,10 @@
       <c r="Z25" t="n">
         <v>929</v>
       </c>
-      <c r="AA25" t="inlineStr"/>
-      <c r="AB25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="n">
         <v>929</v>
       </c>
@@ -3046,6 +3119,9 @@
         <v>929</v>
       </c>
       <c r="AH25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3103,14 +3179,14 @@
       <c r="Q26" t="n">
         <v>1299</v>
       </c>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="T26" t="inlineStr"/>
-      <c r="U26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="R26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="U26" t="inlineStr"/>
       <c r="V26" t="n">
         <v>1299</v>
       </c>
@@ -3126,10 +3202,10 @@
       <c r="Z26" t="n">
         <v>1299</v>
       </c>
-      <c r="AA26" t="inlineStr"/>
-      <c r="AB26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AA26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
         <v>1299</v>
       </c>
@@ -3146,6 +3222,9 @@
         <v>1299</v>
       </c>
       <c r="AH26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AI26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 10:54
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI26"/>
+  <dimension ref="A1:AJ26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,7 @@
     <col width="21" customWidth="1" min="33" max="33"/>
     <col width="21" customWidth="1" min="34" max="34"/>
     <col width="21" customWidth="1" min="35" max="35"/>
+    <col width="21" customWidth="1" min="36" max="36"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -478,170 +479,175 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 16:20</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -689,10 +695,10 @@
       <c r="M2" t="n">
         <v>929</v>
       </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="n">
-        <v>929</v>
-      </c>
+      <c r="N2" t="n">
+        <v>929</v>
+      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
         <v>929</v>
       </c>
@@ -705,25 +711,25 @@
       <c r="S2" t="n">
         <v>929</v>
       </c>
-      <c r="T2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>929</v>
+      </c>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" t="n">
-        <v>929</v>
-      </c>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="n">
         <v>929</v>
       </c>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="n">
-        <v>929</v>
-      </c>
+      <c r="X2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="n">
         <v>929</v>
       </c>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="n">
         <v>929</v>
       </c>
@@ -743,6 +749,9 @@
         <v>929</v>
       </c>
       <c r="AI2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -785,26 +794,26 @@
       <c r="L3" t="n">
         <v>569</v>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>569</v>
+      </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
-      <c r="P3" t="n">
-        <v>569</v>
-      </c>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="n">
         <v>569</v>
       </c>
       <c r="R3" t="n">
         <v>569</v>
       </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="n">
-        <v>569</v>
-      </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="n">
-        <v>569</v>
-      </c>
+      <c r="S3" t="n">
+        <v>569</v>
+      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="n">
+        <v>569</v>
+      </c>
+      <c r="V3" t="inlineStr"/>
       <c r="W3" t="n">
         <v>569</v>
       </c>
@@ -820,10 +829,10 @@
       <c r="AA3" t="n">
         <v>569</v>
       </c>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="n">
         <v>569</v>
       </c>
@@ -840,6 +849,9 @@
         <v>569</v>
       </c>
       <c r="AI3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -900,10 +912,10 @@
       <c r="R4" t="n">
         <v>299</v>
       </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="n">
-        <v>299</v>
-      </c>
+      <c r="S4" t="n">
+        <v>299</v>
+      </c>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="n">
         <v>299</v>
       </c>
@@ -925,10 +937,10 @@
       <c r="AA4" t="n">
         <v>299</v>
       </c>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="n">
         <v>299</v>
       </c>
@@ -945,6 +957,9 @@
         <v>299</v>
       </c>
       <c r="AI4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1032,10 +1047,10 @@
       <c r="AA5" t="n">
         <v>569</v>
       </c>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC5" t="inlineStr"/>
       <c r="AD5" t="n">
         <v>569</v>
       </c>
@@ -1052,6 +1067,9 @@
         <v>569</v>
       </c>
       <c r="AI5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1115,10 +1133,10 @@
       <c r="S6" t="n">
         <v>499</v>
       </c>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="n">
-        <v>499</v>
-      </c>
+      <c r="T6" t="n">
+        <v>499</v>
+      </c>
+      <c r="U6" t="inlineStr"/>
       <c r="V6" t="n">
         <v>499</v>
       </c>
@@ -1137,10 +1155,10 @@
       <c r="AA6" t="n">
         <v>499</v>
       </c>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC6" t="inlineStr"/>
       <c r="AD6" t="n">
         <v>499</v>
       </c>
@@ -1157,6 +1175,9 @@
         <v>499</v>
       </c>
       <c r="AI6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1217,12 +1238,12 @@
       <c r="R7" t="n">
         <v>569</v>
       </c>
-      <c r="S7" t="inlineStr"/>
+      <c r="S7" t="n">
+        <v>569</v>
+      </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
-      <c r="V7" t="n">
-        <v>569</v>
-      </c>
+      <c r="V7" t="inlineStr"/>
       <c r="W7" t="n">
         <v>569</v>
       </c>
@@ -1238,10 +1259,10 @@
       <c r="AA7" t="n">
         <v>569</v>
       </c>
-      <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="n">
         <v>569</v>
       </c>
@@ -1258,6 +1279,9 @@
         <v>569</v>
       </c>
       <c r="AI7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1318,14 +1342,14 @@
       <c r="R8" t="n">
         <v>929</v>
       </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="n">
-        <v>929</v>
-      </c>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="n">
-        <v>929</v>
-      </c>
+      <c r="S8" t="n">
+        <v>929</v>
+      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="n">
+        <v>929</v>
+      </c>
+      <c r="V8" t="inlineStr"/>
       <c r="W8" t="n">
         <v>929</v>
       </c>
@@ -1341,10 +1365,10 @@
       <c r="AA8" t="n">
         <v>929</v>
       </c>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC8" t="inlineStr"/>
       <c r="AD8" t="n">
         <v>929</v>
       </c>
@@ -1361,6 +1385,9 @@
         <v>929</v>
       </c>
       <c r="AI8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1421,10 +1448,10 @@
       <c r="R9" t="n">
         <v>299</v>
       </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="n">
-        <v>299</v>
-      </c>
+      <c r="S9" t="n">
+        <v>299</v>
+      </c>
+      <c r="T9" t="inlineStr"/>
       <c r="U9" t="n">
         <v>299</v>
       </c>
@@ -1446,10 +1473,10 @@
       <c r="AA9" t="n">
         <v>299</v>
       </c>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC9" t="inlineStr"/>
       <c r="AD9" t="n">
         <v>299</v>
       </c>
@@ -1466,6 +1493,9 @@
         <v>299</v>
       </c>
       <c r="AI9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1496,10 +1526,10 @@
       <c r="H10" t="n">
         <v>299</v>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>299</v>
-      </c>
+      <c r="I10" t="n">
+        <v>299</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
         <v>299</v>
       </c>
@@ -1524,14 +1554,14 @@
       <c r="R10" t="n">
         <v>299</v>
       </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="n">
-        <v>299</v>
-      </c>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="n">
-        <v>299</v>
-      </c>
+      <c r="S10" t="n">
+        <v>299</v>
+      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="n">
+        <v>299</v>
+      </c>
+      <c r="V10" t="inlineStr"/>
       <c r="W10" t="n">
         <v>299</v>
       </c>
@@ -1547,10 +1577,10 @@
       <c r="AA10" t="n">
         <v>299</v>
       </c>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="n">
         <v>299</v>
       </c>
@@ -1567,6 +1597,9 @@
         <v>299</v>
       </c>
       <c r="AI10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1630,10 +1663,10 @@
       <c r="S11" t="n">
         <v>2997</v>
       </c>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="n">
+      <c r="T11" t="n">
         <v>2997</v>
       </c>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="n">
         <v>2997</v>
       </c>
@@ -1647,15 +1680,15 @@
         <v>2997</v>
       </c>
       <c r="Z11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AA11" t="n">
         <v>929</v>
       </c>
-      <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="n">
         <v>929</v>
       </c>
@@ -1672,6 +1705,9 @@
         <v>929</v>
       </c>
       <c r="AI11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1738,10 +1774,10 @@
       <c r="T12" t="n">
         <v>569</v>
       </c>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="n">
-        <v>569</v>
-      </c>
+      <c r="U12" t="n">
+        <v>569</v>
+      </c>
+      <c r="V12" t="inlineStr"/>
       <c r="W12" t="n">
         <v>569</v>
       </c>
@@ -1757,10 +1793,10 @@
       <c r="AA12" t="n">
         <v>569</v>
       </c>
-      <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC12" t="inlineStr"/>
       <c r="AD12" t="n">
         <v>569</v>
       </c>
@@ -1777,6 +1813,9 @@
         <v>569</v>
       </c>
       <c r="AI12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1786,10 +1825,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="n">
+        <v>569</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>569</v>
       </c>
@@ -1835,14 +1874,14 @@
       <c r="R13" t="n">
         <v>569</v>
       </c>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="n">
-        <v>569</v>
-      </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="n">
-        <v>569</v>
-      </c>
+      <c r="S13" t="n">
+        <v>569</v>
+      </c>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="n">
+        <v>569</v>
+      </c>
+      <c r="V13" t="inlineStr"/>
       <c r="W13" t="n">
         <v>569</v>
       </c>
@@ -1858,24 +1897,27 @@
       <c r="AA13" t="n">
         <v>569</v>
       </c>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="n">
         <v>569</v>
       </c>
       <c r="AE13" t="n">
         <v>569</v>
       </c>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="n">
         <v>569</v>
       </c>
       <c r="AI13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1906,10 +1948,10 @@
       <c r="H14" t="n">
         <v>794</v>
       </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="n">
+      <c r="I14" t="n">
         <v>794</v>
       </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
         <v>794</v>
       </c>
@@ -1917,7 +1959,7 @@
         <v>794</v>
       </c>
       <c r="M14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="N14" t="n">
         <v>499</v>
@@ -1934,11 +1976,11 @@
       <c r="R14" t="n">
         <v>499</v>
       </c>
-      <c r="S14" t="inlineStr"/>
+      <c r="S14" t="n">
+        <v>499</v>
+      </c>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="n">
-        <v>499</v>
-      </c>
+      <c r="U14" t="inlineStr"/>
       <c r="V14" t="n">
         <v>499</v>
       </c>
@@ -1979,6 +2021,9 @@
         <v>499</v>
       </c>
       <c r="AI14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2045,10 +2090,10 @@
       <c r="T15" t="n">
         <v>499</v>
       </c>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="n">
-        <v>499</v>
-      </c>
+      <c r="U15" t="n">
+        <v>499</v>
+      </c>
+      <c r="V15" t="inlineStr"/>
       <c r="W15" t="n">
         <v>499</v>
       </c>
@@ -2058,14 +2103,14 @@
       <c r="Y15" t="n">
         <v>499</v>
       </c>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="n">
         <v>499</v>
       </c>
@@ -2082,6 +2127,9 @@
         <v>499</v>
       </c>
       <c r="AI15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2133,17 +2181,17 @@
       <c r="O16" t="n">
         <v>299</v>
       </c>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="n">
-        <v>299</v>
-      </c>
+      <c r="P16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="n">
         <v>299</v>
       </c>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="n">
-        <v>299</v>
-      </c>
+      <c r="S16" t="n">
+        <v>299</v>
+      </c>
+      <c r="T16" t="inlineStr"/>
       <c r="U16" t="n">
         <v>299</v>
       </c>
@@ -2165,10 +2213,10 @@
       <c r="AA16" t="n">
         <v>299</v>
       </c>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="n">
         <v>299</v>
       </c>
@@ -2185,6 +2233,9 @@
         <v>299</v>
       </c>
       <c r="AI16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2251,10 +2302,10 @@
       <c r="T17" t="n">
         <v>929</v>
       </c>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="n">
-        <v>929</v>
-      </c>
+      <c r="U17" t="n">
+        <v>929</v>
+      </c>
+      <c r="V17" t="inlineStr"/>
       <c r="W17" t="n">
         <v>929</v>
       </c>
@@ -2270,10 +2321,10 @@
       <c r="AA17" t="n">
         <v>929</v>
       </c>
-      <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC17" t="inlineStr"/>
       <c r="AD17" t="n">
         <v>929</v>
       </c>
@@ -2290,6 +2341,9 @@
         <v>929</v>
       </c>
       <c r="AI17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2353,11 +2407,11 @@
       <c r="S18" t="n">
         <v>499</v>
       </c>
-      <c r="T18" t="inlineStr"/>
+      <c r="T18" t="n">
+        <v>499</v>
+      </c>
       <c r="U18" t="inlineStr"/>
-      <c r="V18" t="n">
-        <v>499</v>
-      </c>
+      <c r="V18" t="inlineStr"/>
       <c r="W18" t="n">
         <v>499</v>
       </c>
@@ -2373,10 +2427,10 @@
       <c r="AA18" t="n">
         <v>499</v>
       </c>
-      <c r="AB18" t="inlineStr"/>
-      <c r="AC18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC18" t="inlineStr"/>
       <c r="AD18" t="n">
         <v>499</v>
       </c>
@@ -2393,6 +2447,9 @@
         <v>499</v>
       </c>
       <c r="AI18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2448,7 +2505,7 @@
         <v>1299</v>
       </c>
       <c r="Q19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="R19" t="n">
         <v>1497</v>
@@ -2456,13 +2513,13 @@
       <c r="S19" t="n">
         <v>1497</v>
       </c>
-      <c r="T19" t="inlineStr"/>
+      <c r="T19" t="n">
+        <v>1497</v>
+      </c>
       <c r="U19" t="inlineStr"/>
-      <c r="V19" t="n">
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="n">
         <v>465</v>
-      </c>
-      <c r="W19" t="n">
-        <v>1497</v>
       </c>
       <c r="X19" t="n">
         <v>1497</v>
@@ -2498,6 +2555,9 @@
         <v>1497</v>
       </c>
       <c r="AI19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AJ19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2585,10 +2645,10 @@
       <c r="AA20" t="n">
         <v>929</v>
       </c>
-      <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC20" t="inlineStr"/>
       <c r="AD20" t="n">
         <v>929</v>
       </c>
@@ -2605,6 +2665,9 @@
         <v>929</v>
       </c>
       <c r="AI20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2641,10 +2704,10 @@
       <c r="J21" t="n">
         <v>499</v>
       </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="n">
-        <v>499</v>
-      </c>
+      <c r="K21" t="n">
+        <v>499</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
         <v>499</v>
       </c>
@@ -2669,10 +2732,10 @@
       <c r="T21" t="n">
         <v>499</v>
       </c>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="n">
-        <v>499</v>
-      </c>
+      <c r="U21" t="n">
+        <v>499</v>
+      </c>
+      <c r="V21" t="inlineStr"/>
       <c r="W21" t="n">
         <v>499</v>
       </c>
@@ -2710,6 +2773,9 @@
         <v>499</v>
       </c>
       <c r="AI21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2770,14 +2836,14 @@
       <c r="R22" t="n">
         <v>299</v>
       </c>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="n">
-        <v>299</v>
-      </c>
-      <c r="U22" t="inlineStr"/>
-      <c r="V22" t="n">
-        <v>299</v>
-      </c>
+      <c r="S22" t="n">
+        <v>299</v>
+      </c>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="n">
+        <v>299</v>
+      </c>
+      <c r="V22" t="inlineStr"/>
       <c r="W22" t="n">
         <v>299</v>
       </c>
@@ -2793,10 +2859,10 @@
       <c r="AA22" t="n">
         <v>299</v>
       </c>
-      <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC22" t="inlineStr"/>
       <c r="AD22" t="n">
         <v>299</v>
       </c>
@@ -2813,6 +2879,9 @@
         <v>299</v>
       </c>
       <c r="AI22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2876,11 +2945,11 @@
       <c r="S23" t="n">
         <v>1299</v>
       </c>
-      <c r="T23" t="inlineStr"/>
+      <c r="T23" t="n">
+        <v>1299</v>
+      </c>
       <c r="U23" t="inlineStr"/>
-      <c r="V23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="V23" t="inlineStr"/>
       <c r="W23" t="n">
         <v>1299</v>
       </c>
@@ -2896,10 +2965,10 @@
       <c r="AA23" t="n">
         <v>1299</v>
       </c>
-      <c r="AB23" t="inlineStr"/>
-      <c r="AC23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AB23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="n">
         <v>1299</v>
       </c>
@@ -2916,6 +2985,9 @@
         <v>1299</v>
       </c>
       <c r="AI23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AJ23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -2976,11 +3048,11 @@
       <c r="R24" t="n">
         <v>929</v>
       </c>
-      <c r="S24" t="inlineStr"/>
+      <c r="S24" t="n">
+        <v>929</v>
+      </c>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="n">
-        <v>929</v>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="n">
         <v>929</v>
       </c>
@@ -2999,10 +3071,10 @@
       <c r="AA24" t="n">
         <v>929</v>
       </c>
-      <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="n">
         <v>929</v>
       </c>
@@ -3019,6 +3091,9 @@
         <v>929</v>
       </c>
       <c r="AI24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3079,11 +3154,11 @@
       <c r="R25" t="n">
         <v>929</v>
       </c>
-      <c r="S25" t="inlineStr"/>
+      <c r="S25" t="n">
+        <v>929</v>
+      </c>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="n">
-        <v>929</v>
-      </c>
+      <c r="U25" t="inlineStr"/>
       <c r="V25" t="n">
         <v>929</v>
       </c>
@@ -3102,10 +3177,10 @@
       <c r="AA25" t="n">
         <v>929</v>
       </c>
-      <c r="AB25" t="inlineStr"/>
-      <c r="AC25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC25" t="inlineStr"/>
       <c r="AD25" t="n">
         <v>929</v>
       </c>
@@ -3122,6 +3197,9 @@
         <v>929</v>
       </c>
       <c r="AI25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3182,14 +3260,14 @@
       <c r="R26" t="n">
         <v>1299</v>
       </c>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="S26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="V26" t="inlineStr"/>
       <c r="W26" t="n">
         <v>1299</v>
       </c>
@@ -3205,10 +3283,10 @@
       <c r="AA26" t="n">
         <v>1299</v>
       </c>
-      <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AB26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AC26" t="inlineStr"/>
       <c r="AD26" t="n">
         <v>1299</v>
       </c>
@@ -3225,6 +3303,9 @@
         <v>1299</v>
       </c>
       <c r="AI26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AJ26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 13:54
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ26"/>
+  <dimension ref="A1:AK26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,7 @@
     <col width="21" customWidth="1" min="34" max="34"/>
     <col width="21" customWidth="1" min="35" max="35"/>
     <col width="21" customWidth="1" min="36" max="36"/>
+    <col width="21" customWidth="1" min="37" max="37"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -479,175 +480,180 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 19:20</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -698,10 +704,10 @@
       <c r="N2" t="n">
         <v>929</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="n">
-        <v>929</v>
-      </c>
+      <c r="O2" t="n">
+        <v>929</v>
+      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="n">
         <v>929</v>
       </c>
@@ -714,25 +720,25 @@
       <c r="T2" t="n">
         <v>929</v>
       </c>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="n">
+        <v>929</v>
+      </c>
       <c r="V2" t="inlineStr"/>
-      <c r="W2" t="n">
-        <v>929</v>
-      </c>
+      <c r="W2" t="inlineStr"/>
       <c r="X2" t="n">
         <v>929</v>
       </c>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
         <v>929</v>
       </c>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="n">
         <v>929</v>
       </c>
@@ -752,6 +758,9 @@
         <v>929</v>
       </c>
       <c r="AJ2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -797,26 +806,26 @@
       <c r="M3" t="n">
         <v>569</v>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="n">
+        <v>569</v>
+      </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
         <v>569</v>
       </c>
       <c r="S3" t="n">
         <v>569</v>
       </c>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
-        <v>569</v>
-      </c>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="n">
-        <v>569</v>
-      </c>
+      <c r="T3" t="n">
+        <v>569</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="n">
+        <v>569</v>
+      </c>
+      <c r="W3" t="inlineStr"/>
       <c r="X3" t="n">
         <v>569</v>
       </c>
@@ -832,10 +841,10 @@
       <c r="AB3" t="n">
         <v>569</v>
       </c>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="n">
         <v>569</v>
       </c>
@@ -852,6 +861,9 @@
         <v>569</v>
       </c>
       <c r="AJ3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -915,10 +927,10 @@
       <c r="S4" t="n">
         <v>299</v>
       </c>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="n">
-        <v>299</v>
-      </c>
+      <c r="T4" t="n">
+        <v>299</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
       <c r="V4" t="n">
         <v>299</v>
       </c>
@@ -940,10 +952,10 @@
       <c r="AB4" t="n">
         <v>299</v>
       </c>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="n">
         <v>299</v>
       </c>
@@ -960,6 +972,9 @@
         <v>299</v>
       </c>
       <c r="AJ4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1050,10 +1065,10 @@
       <c r="AB5" t="n">
         <v>569</v>
       </c>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="n">
         <v>569</v>
       </c>
@@ -1070,6 +1085,9 @@
         <v>569</v>
       </c>
       <c r="AJ5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1136,10 +1154,10 @@
       <c r="T6" t="n">
         <v>499</v>
       </c>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="n">
-        <v>499</v>
-      </c>
+      <c r="U6" t="n">
+        <v>499</v>
+      </c>
+      <c r="V6" t="inlineStr"/>
       <c r="W6" t="n">
         <v>499</v>
       </c>
@@ -1158,10 +1176,10 @@
       <c r="AB6" t="n">
         <v>499</v>
       </c>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="n">
         <v>499</v>
       </c>
@@ -1178,6 +1196,9 @@
         <v>499</v>
       </c>
       <c r="AJ6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1241,12 +1262,12 @@
       <c r="S7" t="n">
         <v>569</v>
       </c>
-      <c r="T7" t="inlineStr"/>
+      <c r="T7" t="n">
+        <v>569</v>
+      </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
-      <c r="W7" t="n">
-        <v>569</v>
-      </c>
+      <c r="W7" t="inlineStr"/>
       <c r="X7" t="n">
         <v>569</v>
       </c>
@@ -1262,10 +1283,10 @@
       <c r="AB7" t="n">
         <v>569</v>
       </c>
-      <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="n">
         <v>569</v>
       </c>
@@ -1282,6 +1303,9 @@
         <v>569</v>
       </c>
       <c r="AJ7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1345,14 +1369,14 @@
       <c r="S8" t="n">
         <v>929</v>
       </c>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="n">
-        <v>929</v>
-      </c>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="n">
-        <v>929</v>
-      </c>
+      <c r="T8" t="n">
+        <v>929</v>
+      </c>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="n">
+        <v>929</v>
+      </c>
+      <c r="W8" t="inlineStr"/>
       <c r="X8" t="n">
         <v>929</v>
       </c>
@@ -1368,10 +1392,10 @@
       <c r="AB8" t="n">
         <v>929</v>
       </c>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD8" t="inlineStr"/>
       <c r="AE8" t="n">
         <v>929</v>
       </c>
@@ -1388,6 +1412,9 @@
         <v>929</v>
       </c>
       <c r="AJ8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1451,10 +1478,10 @@
       <c r="S9" t="n">
         <v>299</v>
       </c>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="n">
-        <v>299</v>
-      </c>
+      <c r="T9" t="n">
+        <v>299</v>
+      </c>
+      <c r="U9" t="inlineStr"/>
       <c r="V9" t="n">
         <v>299</v>
       </c>
@@ -1476,10 +1503,10 @@
       <c r="AB9" t="n">
         <v>299</v>
       </c>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="n">
         <v>299</v>
       </c>
@@ -1496,6 +1523,9 @@
         <v>299</v>
       </c>
       <c r="AJ9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1529,10 +1559,10 @@
       <c r="I10" t="n">
         <v>299</v>
       </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>299</v>
-      </c>
+      <c r="J10" t="n">
+        <v>299</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
         <v>299</v>
       </c>
@@ -1557,14 +1587,14 @@
       <c r="S10" t="n">
         <v>299</v>
       </c>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="n">
-        <v>299</v>
-      </c>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="n">
-        <v>299</v>
-      </c>
+      <c r="T10" t="n">
+        <v>299</v>
+      </c>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="n">
+        <v>299</v>
+      </c>
+      <c r="W10" t="inlineStr"/>
       <c r="X10" t="n">
         <v>299</v>
       </c>
@@ -1580,10 +1610,10 @@
       <c r="AB10" t="n">
         <v>299</v>
       </c>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="n">
         <v>299</v>
       </c>
@@ -1600,6 +1630,9 @@
         <v>299</v>
       </c>
       <c r="AJ10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1666,10 +1699,10 @@
       <c r="T11" t="n">
         <v>2997</v>
       </c>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="n">
+      <c r="U11" t="n">
         <v>2997</v>
       </c>
+      <c r="V11" t="inlineStr"/>
       <c r="W11" t="n">
         <v>2997</v>
       </c>
@@ -1683,15 +1716,15 @@
         <v>2997</v>
       </c>
       <c r="AA11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AB11" t="n">
         <v>929</v>
       </c>
-      <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="n">
         <v>929</v>
       </c>
@@ -1708,6 +1741,9 @@
         <v>929</v>
       </c>
       <c r="AJ11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1777,10 +1813,10 @@
       <c r="U12" t="n">
         <v>569</v>
       </c>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="n">
-        <v>569</v>
-      </c>
+      <c r="V12" t="n">
+        <v>569</v>
+      </c>
+      <c r="W12" t="inlineStr"/>
       <c r="X12" t="n">
         <v>569</v>
       </c>
@@ -1796,10 +1832,10 @@
       <c r="AB12" t="n">
         <v>569</v>
       </c>
-      <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD12" t="inlineStr"/>
       <c r="AE12" t="n">
         <v>569</v>
       </c>
@@ -1816,6 +1852,9 @@
         <v>569</v>
       </c>
       <c r="AJ12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1828,10 +1867,10 @@
       <c r="B13" t="n">
         <v>569</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>569</v>
-      </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>569</v>
       </c>
@@ -1877,14 +1916,14 @@
       <c r="S13" t="n">
         <v>569</v>
       </c>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="n">
-        <v>569</v>
-      </c>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="n">
-        <v>569</v>
-      </c>
+      <c r="T13" t="n">
+        <v>569</v>
+      </c>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="n">
+        <v>569</v>
+      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="n">
         <v>569</v>
       </c>
@@ -1900,24 +1939,27 @@
       <c r="AB13" t="n">
         <v>569</v>
       </c>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="n">
         <v>569</v>
       </c>
       <c r="AF13" t="n">
         <v>569</v>
       </c>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH13" t="inlineStr"/>
       <c r="AI13" t="n">
         <v>569</v>
       </c>
       <c r="AJ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1951,10 +1993,10 @@
       <c r="I14" t="n">
         <v>794</v>
       </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="n">
+      <c r="J14" t="n">
         <v>794</v>
       </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
         <v>794</v>
       </c>
@@ -1962,7 +2004,7 @@
         <v>794</v>
       </c>
       <c r="N14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="O14" t="n">
         <v>499</v>
@@ -1979,11 +2021,11 @@
       <c r="S14" t="n">
         <v>499</v>
       </c>
-      <c r="T14" t="inlineStr"/>
+      <c r="T14" t="n">
+        <v>499</v>
+      </c>
       <c r="U14" t="inlineStr"/>
-      <c r="V14" t="n">
-        <v>499</v>
-      </c>
+      <c r="V14" t="inlineStr"/>
       <c r="W14" t="n">
         <v>499</v>
       </c>
@@ -2024,6 +2066,9 @@
         <v>499</v>
       </c>
       <c r="AJ14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2093,10 +2138,10 @@
       <c r="U15" t="n">
         <v>499</v>
       </c>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="n">
-        <v>499</v>
-      </c>
+      <c r="V15" t="n">
+        <v>499</v>
+      </c>
+      <c r="W15" t="inlineStr"/>
       <c r="X15" t="n">
         <v>499</v>
       </c>
@@ -2106,14 +2151,14 @@
       <c r="Z15" t="n">
         <v>499</v>
       </c>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AC15" t="inlineStr"/>
-      <c r="AD15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB15" t="inlineStr"/>
+      <c r="AC15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="n">
         <v>499</v>
       </c>
@@ -2130,6 +2175,9 @@
         <v>499</v>
       </c>
       <c r="AJ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2184,17 +2232,17 @@
       <c r="P16" t="n">
         <v>299</v>
       </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q16" t="n">
+        <v>299</v>
+      </c>
+      <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
         <v>299</v>
       </c>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="n">
-        <v>299</v>
-      </c>
+      <c r="T16" t="n">
+        <v>299</v>
+      </c>
+      <c r="U16" t="inlineStr"/>
       <c r="V16" t="n">
         <v>299</v>
       </c>
@@ -2216,10 +2264,10 @@
       <c r="AB16" t="n">
         <v>299</v>
       </c>
-      <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="n">
         <v>299</v>
       </c>
@@ -2236,6 +2284,9 @@
         <v>299</v>
       </c>
       <c r="AJ16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2305,10 +2356,10 @@
       <c r="U17" t="n">
         <v>929</v>
       </c>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="n">
-        <v>929</v>
-      </c>
+      <c r="V17" t="n">
+        <v>929</v>
+      </c>
+      <c r="W17" t="inlineStr"/>
       <c r="X17" t="n">
         <v>929</v>
       </c>
@@ -2324,10 +2375,10 @@
       <c r="AB17" t="n">
         <v>929</v>
       </c>
-      <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="n">
         <v>929</v>
       </c>
@@ -2344,6 +2395,9 @@
         <v>929</v>
       </c>
       <c r="AJ17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2410,11 +2464,11 @@
       <c r="T18" t="n">
         <v>499</v>
       </c>
-      <c r="U18" t="inlineStr"/>
+      <c r="U18" t="n">
+        <v>499</v>
+      </c>
       <c r="V18" t="inlineStr"/>
-      <c r="W18" t="n">
-        <v>499</v>
-      </c>
+      <c r="W18" t="inlineStr"/>
       <c r="X18" t="n">
         <v>499</v>
       </c>
@@ -2430,10 +2484,10 @@
       <c r="AB18" t="n">
         <v>499</v>
       </c>
-      <c r="AC18" t="inlineStr"/>
-      <c r="AD18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD18" t="inlineStr"/>
       <c r="AE18" t="n">
         <v>499</v>
       </c>
@@ -2450,6 +2504,9 @@
         <v>499</v>
       </c>
       <c r="AJ18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2508,7 +2565,7 @@
         <v>1299</v>
       </c>
       <c r="R19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="S19" t="n">
         <v>1497</v>
@@ -2516,13 +2573,13 @@
       <c r="T19" t="n">
         <v>1497</v>
       </c>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="n">
+        <v>1497</v>
+      </c>
       <c r="V19" t="inlineStr"/>
-      <c r="W19" t="n">
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="n">
         <v>465</v>
-      </c>
-      <c r="X19" t="n">
-        <v>1497</v>
       </c>
       <c r="Y19" t="n">
         <v>1497</v>
@@ -2558,6 +2615,9 @@
         <v>1497</v>
       </c>
       <c r="AJ19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AK19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2648,10 +2708,10 @@
       <c r="AB20" t="n">
         <v>929</v>
       </c>
-      <c r="AC20" t="inlineStr"/>
-      <c r="AD20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD20" t="inlineStr"/>
       <c r="AE20" t="n">
         <v>929</v>
       </c>
@@ -2668,6 +2728,9 @@
         <v>929</v>
       </c>
       <c r="AJ20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2707,10 +2770,10 @@
       <c r="K21" t="n">
         <v>499</v>
       </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="n">
-        <v>499</v>
-      </c>
+      <c r="L21" t="n">
+        <v>499</v>
+      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
         <v>499</v>
       </c>
@@ -2735,10 +2798,10 @@
       <c r="U21" t="n">
         <v>499</v>
       </c>
-      <c r="V21" t="inlineStr"/>
-      <c r="W21" t="n">
-        <v>499</v>
-      </c>
+      <c r="V21" t="n">
+        <v>499</v>
+      </c>
+      <c r="W21" t="inlineStr"/>
       <c r="X21" t="n">
         <v>499</v>
       </c>
@@ -2776,6 +2839,9 @@
         <v>499</v>
       </c>
       <c r="AJ21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2839,14 +2905,14 @@
       <c r="S22" t="n">
         <v>299</v>
       </c>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="n">
-        <v>299</v>
-      </c>
-      <c r="V22" t="inlineStr"/>
-      <c r="W22" t="n">
-        <v>299</v>
-      </c>
+      <c r="T22" t="n">
+        <v>299</v>
+      </c>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="n">
+        <v>299</v>
+      </c>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="n">
         <v>299</v>
       </c>
@@ -2862,10 +2928,10 @@
       <c r="AB22" t="n">
         <v>299</v>
       </c>
-      <c r="AC22" t="inlineStr"/>
-      <c r="AD22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD22" t="inlineStr"/>
       <c r="AE22" t="n">
         <v>299</v>
       </c>
@@ -2882,6 +2948,9 @@
         <v>299</v>
       </c>
       <c r="AJ22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2948,11 +3017,11 @@
       <c r="T23" t="n">
         <v>1299</v>
       </c>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="n">
+        <v>1299</v>
+      </c>
       <c r="V23" t="inlineStr"/>
-      <c r="W23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="W23" t="inlineStr"/>
       <c r="X23" t="n">
         <v>1299</v>
       </c>
@@ -2968,10 +3037,10 @@
       <c r="AB23" t="n">
         <v>1299</v>
       </c>
-      <c r="AC23" t="inlineStr"/>
-      <c r="AD23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AC23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="n">
         <v>1299</v>
       </c>
@@ -2988,6 +3057,9 @@
         <v>1299</v>
       </c>
       <c r="AJ23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AK23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3051,11 +3123,11 @@
       <c r="S24" t="n">
         <v>929</v>
       </c>
-      <c r="T24" t="inlineStr"/>
+      <c r="T24" t="n">
+        <v>929</v>
+      </c>
       <c r="U24" t="inlineStr"/>
-      <c r="V24" t="n">
-        <v>929</v>
-      </c>
+      <c r="V24" t="inlineStr"/>
       <c r="W24" t="n">
         <v>929</v>
       </c>
@@ -3074,10 +3146,10 @@
       <c r="AB24" t="n">
         <v>929</v>
       </c>
-      <c r="AC24" t="inlineStr"/>
-      <c r="AD24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="n">
         <v>929</v>
       </c>
@@ -3094,6 +3166,9 @@
         <v>929</v>
       </c>
       <c r="AJ24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3157,11 +3232,11 @@
       <c r="S25" t="n">
         <v>929</v>
       </c>
-      <c r="T25" t="inlineStr"/>
+      <c r="T25" t="n">
+        <v>929</v>
+      </c>
       <c r="U25" t="inlineStr"/>
-      <c r="V25" t="n">
-        <v>929</v>
-      </c>
+      <c r="V25" t="inlineStr"/>
       <c r="W25" t="n">
         <v>929</v>
       </c>
@@ -3180,10 +3255,10 @@
       <c r="AB25" t="n">
         <v>929</v>
       </c>
-      <c r="AC25" t="inlineStr"/>
-      <c r="AD25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD25" t="inlineStr"/>
       <c r="AE25" t="n">
         <v>929</v>
       </c>
@@ -3200,6 +3275,9 @@
         <v>929</v>
       </c>
       <c r="AJ25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3263,14 +3341,14 @@
       <c r="S26" t="n">
         <v>1299</v>
       </c>
-      <c r="T26" t="inlineStr"/>
-      <c r="U26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="V26" t="inlineStr"/>
-      <c r="W26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="T26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="n">
         <v>1299</v>
       </c>
@@ -3286,10 +3364,10 @@
       <c r="AB26" t="n">
         <v>1299</v>
       </c>
-      <c r="AC26" t="inlineStr"/>
-      <c r="AD26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AC26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AD26" t="inlineStr"/>
       <c r="AE26" t="n">
         <v>1299</v>
       </c>
@@ -3306,6 +3384,9 @@
         <v>1299</v>
       </c>
       <c r="AJ26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AK26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 14:51
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AL26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +470,7 @@
     <col width="21" customWidth="1" min="35" max="35"/>
     <col width="21" customWidth="1" min="36" max="36"/>
     <col width="21" customWidth="1" min="37" max="37"/>
+    <col width="21" customWidth="1" min="38" max="38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -480,180 +481,185 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 20:17</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -707,10 +713,10 @@
       <c r="O2" t="n">
         <v>929</v>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="n">
-        <v>929</v>
-      </c>
+      <c r="P2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
         <v>929</v>
       </c>
@@ -723,25 +729,25 @@
       <c r="U2" t="n">
         <v>929</v>
       </c>
-      <c r="V2" t="inlineStr"/>
+      <c r="V2" t="n">
+        <v>929</v>
+      </c>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" t="n">
-        <v>929</v>
-      </c>
+      <c r="X2" t="inlineStr"/>
       <c r="Y2" t="n">
         <v>929</v>
       </c>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="n">
         <v>929</v>
       </c>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="n">
         <v>929</v>
       </c>
@@ -761,6 +767,9 @@
         <v>929</v>
       </c>
       <c r="AK2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -809,26 +818,26 @@
       <c r="N3" t="n">
         <v>569</v>
       </c>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="n">
+        <v>569</v>
+      </c>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="n">
-        <v>569</v>
-      </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
         <v>569</v>
       </c>
       <c r="T3" t="n">
         <v>569</v>
       </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="n">
-        <v>569</v>
-      </c>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="n">
-        <v>569</v>
-      </c>
+      <c r="U3" t="n">
+        <v>569</v>
+      </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="n">
+        <v>569</v>
+      </c>
+      <c r="X3" t="inlineStr"/>
       <c r="Y3" t="n">
         <v>569</v>
       </c>
@@ -844,10 +853,10 @@
       <c r="AC3" t="n">
         <v>569</v>
       </c>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="n">
         <v>569</v>
       </c>
@@ -864,6 +873,9 @@
         <v>569</v>
       </c>
       <c r="AK3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -930,10 +942,10 @@
       <c r="T4" t="n">
         <v>299</v>
       </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="n">
-        <v>299</v>
-      </c>
+      <c r="U4" t="n">
+        <v>299</v>
+      </c>
+      <c r="V4" t="inlineStr"/>
       <c r="W4" t="n">
         <v>299</v>
       </c>
@@ -955,10 +967,10 @@
       <c r="AC4" t="n">
         <v>299</v>
       </c>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="n">
         <v>299</v>
       </c>
@@ -975,6 +987,9 @@
         <v>299</v>
       </c>
       <c r="AK4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1068,10 +1083,10 @@
       <c r="AC5" t="n">
         <v>569</v>
       </c>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="n">
         <v>569</v>
       </c>
@@ -1088,6 +1103,9 @@
         <v>569</v>
       </c>
       <c r="AK5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1157,10 +1175,10 @@
       <c r="U6" t="n">
         <v>499</v>
       </c>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="n">
-        <v>499</v>
-      </c>
+      <c r="V6" t="n">
+        <v>499</v>
+      </c>
+      <c r="W6" t="inlineStr"/>
       <c r="X6" t="n">
         <v>499</v>
       </c>
@@ -1179,10 +1197,10 @@
       <c r="AC6" t="n">
         <v>499</v>
       </c>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="n">
         <v>499</v>
       </c>
@@ -1199,6 +1217,9 @@
         <v>499</v>
       </c>
       <c r="AK6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1265,12 +1286,12 @@
       <c r="T7" t="n">
         <v>569</v>
       </c>
-      <c r="U7" t="inlineStr"/>
+      <c r="U7" t="n">
+        <v>569</v>
+      </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
-      <c r="X7" t="n">
-        <v>569</v>
-      </c>
+      <c r="X7" t="inlineStr"/>
       <c r="Y7" t="n">
         <v>569</v>
       </c>
@@ -1286,10 +1307,10 @@
       <c r="AC7" t="n">
         <v>569</v>
       </c>
-      <c r="AD7" t="inlineStr"/>
-      <c r="AE7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="n">
         <v>569</v>
       </c>
@@ -1306,6 +1327,9 @@
         <v>569</v>
       </c>
       <c r="AK7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1372,14 +1396,14 @@
       <c r="T8" t="n">
         <v>929</v>
       </c>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="n">
-        <v>929</v>
-      </c>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="n">
-        <v>929</v>
-      </c>
+      <c r="U8" t="n">
+        <v>929</v>
+      </c>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="n">
+        <v>929</v>
+      </c>
+      <c r="X8" t="inlineStr"/>
       <c r="Y8" t="n">
         <v>929</v>
       </c>
@@ -1395,10 +1419,10 @@
       <c r="AC8" t="n">
         <v>929</v>
       </c>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="n">
         <v>929</v>
       </c>
@@ -1415,6 +1439,9 @@
         <v>929</v>
       </c>
       <c r="AK8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1481,10 +1508,10 @@
       <c r="T9" t="n">
         <v>299</v>
       </c>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="n">
-        <v>299</v>
-      </c>
+      <c r="U9" t="n">
+        <v>299</v>
+      </c>
+      <c r="V9" t="inlineStr"/>
       <c r="W9" t="n">
         <v>299</v>
       </c>
@@ -1506,10 +1533,10 @@
       <c r="AC9" t="n">
         <v>299</v>
       </c>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="n">
         <v>299</v>
       </c>
@@ -1526,6 +1553,9 @@
         <v>299</v>
       </c>
       <c r="AK9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1562,10 +1592,10 @@
       <c r="J10" t="n">
         <v>299</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
-        <v>299</v>
-      </c>
+      <c r="K10" t="n">
+        <v>299</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
         <v>299</v>
       </c>
@@ -1590,14 +1620,14 @@
       <c r="T10" t="n">
         <v>299</v>
       </c>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="n">
-        <v>299</v>
-      </c>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="n">
-        <v>299</v>
-      </c>
+      <c r="U10" t="n">
+        <v>299</v>
+      </c>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="n">
+        <v>299</v>
+      </c>
+      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="n">
         <v>299</v>
       </c>
@@ -1613,10 +1643,10 @@
       <c r="AC10" t="n">
         <v>299</v>
       </c>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="n">
         <v>299</v>
       </c>
@@ -1633,6 +1663,9 @@
         <v>299</v>
       </c>
       <c r="AK10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1702,10 +1735,10 @@
       <c r="U11" t="n">
         <v>2997</v>
       </c>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="n">
+      <c r="V11" t="n">
         <v>2997</v>
       </c>
+      <c r="W11" t="inlineStr"/>
       <c r="X11" t="n">
         <v>2997</v>
       </c>
@@ -1719,15 +1752,15 @@
         <v>2997</v>
       </c>
       <c r="AB11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AC11" t="n">
         <v>929</v>
       </c>
-      <c r="AD11" t="inlineStr"/>
-      <c r="AE11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="n">
         <v>929</v>
       </c>
@@ -1744,6 +1777,9 @@
         <v>929</v>
       </c>
       <c r="AK11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1816,10 +1852,10 @@
       <c r="V12" t="n">
         <v>569</v>
       </c>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="n">
-        <v>569</v>
-      </c>
+      <c r="W12" t="n">
+        <v>569</v>
+      </c>
+      <c r="X12" t="inlineStr"/>
       <c r="Y12" t="n">
         <v>569</v>
       </c>
@@ -1835,10 +1871,10 @@
       <c r="AC12" t="n">
         <v>569</v>
       </c>
-      <c r="AD12" t="inlineStr"/>
-      <c r="AE12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="n">
         <v>569</v>
       </c>
@@ -1855,6 +1891,9 @@
         <v>569</v>
       </c>
       <c r="AK12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1870,10 +1909,10 @@
       <c r="C13" t="n">
         <v>569</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>569</v>
-      </c>
+      <c r="D13" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>569</v>
       </c>
@@ -1919,14 +1958,14 @@
       <c r="T13" t="n">
         <v>569</v>
       </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="n">
-        <v>569</v>
-      </c>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="n">
-        <v>569</v>
-      </c>
+      <c r="U13" t="n">
+        <v>569</v>
+      </c>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="n">
+        <v>569</v>
+      </c>
+      <c r="X13" t="inlineStr"/>
       <c r="Y13" t="n">
         <v>569</v>
       </c>
@@ -1942,24 +1981,27 @@
       <c r="AC13" t="n">
         <v>569</v>
       </c>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="n">
         <v>569</v>
       </c>
       <c r="AG13" t="n">
         <v>569</v>
       </c>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI13" t="inlineStr"/>
       <c r="AJ13" t="n">
         <v>569</v>
       </c>
       <c r="AK13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1996,10 +2038,10 @@
       <c r="J14" t="n">
         <v>794</v>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="n">
+      <c r="K14" t="n">
         <v>794</v>
       </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
         <v>794</v>
       </c>
@@ -2007,7 +2049,7 @@
         <v>794</v>
       </c>
       <c r="O14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="P14" t="n">
         <v>499</v>
@@ -2024,11 +2066,11 @@
       <c r="T14" t="n">
         <v>499</v>
       </c>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="n">
+        <v>499</v>
+      </c>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="n">
-        <v>499</v>
-      </c>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="n">
         <v>499</v>
       </c>
@@ -2069,6 +2111,9 @@
         <v>499</v>
       </c>
       <c r="AK14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2141,10 +2186,10 @@
       <c r="V15" t="n">
         <v>499</v>
       </c>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="n">
-        <v>499</v>
-      </c>
+      <c r="W15" t="n">
+        <v>499</v>
+      </c>
+      <c r="X15" t="inlineStr"/>
       <c r="Y15" t="n">
         <v>499</v>
       </c>
@@ -2154,14 +2199,14 @@
       <c r="AA15" t="n">
         <v>499</v>
       </c>
-      <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="n">
         <v>499</v>
       </c>
@@ -2178,6 +2223,9 @@
         <v>499</v>
       </c>
       <c r="AK15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2235,17 +2283,17 @@
       <c r="Q16" t="n">
         <v>299</v>
       </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="n">
-        <v>299</v>
-      </c>
+      <c r="R16" t="n">
+        <v>299</v>
+      </c>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="n">
         <v>299</v>
       </c>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="n">
-        <v>299</v>
-      </c>
+      <c r="U16" t="n">
+        <v>299</v>
+      </c>
+      <c r="V16" t="inlineStr"/>
       <c r="W16" t="n">
         <v>299</v>
       </c>
@@ -2267,10 +2315,10 @@
       <c r="AC16" t="n">
         <v>299</v>
       </c>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="n">
         <v>299</v>
       </c>
@@ -2287,6 +2335,9 @@
         <v>299</v>
       </c>
       <c r="AK16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2359,10 +2410,10 @@
       <c r="V17" t="n">
         <v>929</v>
       </c>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="n">
-        <v>929</v>
-      </c>
+      <c r="W17" t="n">
+        <v>929</v>
+      </c>
+      <c r="X17" t="inlineStr"/>
       <c r="Y17" t="n">
         <v>929</v>
       </c>
@@ -2378,10 +2429,10 @@
       <c r="AC17" t="n">
         <v>929</v>
       </c>
-      <c r="AD17" t="inlineStr"/>
-      <c r="AE17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="n">
         <v>929</v>
       </c>
@@ -2398,6 +2449,9 @@
         <v>929</v>
       </c>
       <c r="AK17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2467,11 +2521,11 @@
       <c r="U18" t="n">
         <v>499</v>
       </c>
-      <c r="V18" t="inlineStr"/>
+      <c r="V18" t="n">
+        <v>499</v>
+      </c>
       <c r="W18" t="inlineStr"/>
-      <c r="X18" t="n">
-        <v>499</v>
-      </c>
+      <c r="X18" t="inlineStr"/>
       <c r="Y18" t="n">
         <v>499</v>
       </c>
@@ -2487,10 +2541,10 @@
       <c r="AC18" t="n">
         <v>499</v>
       </c>
-      <c r="AD18" t="inlineStr"/>
-      <c r="AE18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="n">
         <v>499</v>
       </c>
@@ -2507,6 +2561,9 @@
         <v>499</v>
       </c>
       <c r="AK18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2568,7 +2625,7 @@
         <v>1299</v>
       </c>
       <c r="S19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="T19" t="n">
         <v>1497</v>
@@ -2576,13 +2633,13 @@
       <c r="U19" t="n">
         <v>1497</v>
       </c>
-      <c r="V19" t="inlineStr"/>
+      <c r="V19" t="n">
+        <v>1497</v>
+      </c>
       <c r="W19" t="inlineStr"/>
-      <c r="X19" t="n">
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="n">
         <v>465</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>1497</v>
       </c>
       <c r="Z19" t="n">
         <v>1497</v>
@@ -2618,6 +2675,9 @@
         <v>1497</v>
       </c>
       <c r="AK19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AL19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2711,10 +2771,10 @@
       <c r="AC20" t="n">
         <v>929</v>
       </c>
-      <c r="AD20" t="inlineStr"/>
-      <c r="AE20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="n">
         <v>929</v>
       </c>
@@ -2731,6 +2791,9 @@
         <v>929</v>
       </c>
       <c r="AK20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2773,10 +2836,10 @@
       <c r="L21" t="n">
         <v>499</v>
       </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="n">
-        <v>499</v>
-      </c>
+      <c r="M21" t="n">
+        <v>499</v>
+      </c>
+      <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
         <v>499</v>
       </c>
@@ -2801,10 +2864,10 @@
       <c r="V21" t="n">
         <v>499</v>
       </c>
-      <c r="W21" t="inlineStr"/>
-      <c r="X21" t="n">
-        <v>499</v>
-      </c>
+      <c r="W21" t="n">
+        <v>499</v>
+      </c>
+      <c r="X21" t="inlineStr"/>
       <c r="Y21" t="n">
         <v>499</v>
       </c>
@@ -2842,6 +2905,9 @@
         <v>499</v>
       </c>
       <c r="AK21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2908,14 +2974,14 @@
       <c r="T22" t="n">
         <v>299</v>
       </c>
-      <c r="U22" t="inlineStr"/>
-      <c r="V22" t="n">
-        <v>299</v>
-      </c>
-      <c r="W22" t="inlineStr"/>
-      <c r="X22" t="n">
-        <v>299</v>
-      </c>
+      <c r="U22" t="n">
+        <v>299</v>
+      </c>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="n">
+        <v>299</v>
+      </c>
+      <c r="X22" t="inlineStr"/>
       <c r="Y22" t="n">
         <v>299</v>
       </c>
@@ -2931,10 +2997,10 @@
       <c r="AC22" t="n">
         <v>299</v>
       </c>
-      <c r="AD22" t="inlineStr"/>
-      <c r="AE22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="n">
         <v>299</v>
       </c>
@@ -2951,6 +3017,9 @@
         <v>299</v>
       </c>
       <c r="AK22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3020,11 +3089,11 @@
       <c r="U23" t="n">
         <v>1299</v>
       </c>
-      <c r="V23" t="inlineStr"/>
+      <c r="V23" t="n">
+        <v>1299</v>
+      </c>
       <c r="W23" t="inlineStr"/>
-      <c r="X23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="X23" t="inlineStr"/>
       <c r="Y23" t="n">
         <v>1299</v>
       </c>
@@ -3040,10 +3109,10 @@
       <c r="AC23" t="n">
         <v>1299</v>
       </c>
-      <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AD23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AE23" t="inlineStr"/>
       <c r="AF23" t="n">
         <v>1299</v>
       </c>
@@ -3060,6 +3129,9 @@
         <v>1299</v>
       </c>
       <c r="AK23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AL23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3126,11 +3198,11 @@
       <c r="T24" t="n">
         <v>929</v>
       </c>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="n">
+        <v>929</v>
+      </c>
       <c r="V24" t="inlineStr"/>
-      <c r="W24" t="n">
-        <v>929</v>
-      </c>
+      <c r="W24" t="inlineStr"/>
       <c r="X24" t="n">
         <v>929</v>
       </c>
@@ -3149,10 +3221,10 @@
       <c r="AC24" t="n">
         <v>929</v>
       </c>
-      <c r="AD24" t="inlineStr"/>
-      <c r="AE24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE24" t="inlineStr"/>
       <c r="AF24" t="n">
         <v>929</v>
       </c>
@@ -3169,6 +3241,9 @@
         <v>929</v>
       </c>
       <c r="AK24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3235,11 +3310,11 @@
       <c r="T25" t="n">
         <v>929</v>
       </c>
-      <c r="U25" t="inlineStr"/>
+      <c r="U25" t="n">
+        <v>929</v>
+      </c>
       <c r="V25" t="inlineStr"/>
-      <c r="W25" t="n">
-        <v>929</v>
-      </c>
+      <c r="W25" t="inlineStr"/>
       <c r="X25" t="n">
         <v>929</v>
       </c>
@@ -3258,10 +3333,10 @@
       <c r="AC25" t="n">
         <v>929</v>
       </c>
-      <c r="AD25" t="inlineStr"/>
-      <c r="AE25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="n">
         <v>929</v>
       </c>
@@ -3278,6 +3353,9 @@
         <v>929</v>
       </c>
       <c r="AK25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3344,14 +3422,14 @@
       <c r="T26" t="n">
         <v>1299</v>
       </c>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="W26" t="inlineStr"/>
-      <c r="X26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="U26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="X26" t="inlineStr"/>
       <c r="Y26" t="n">
         <v>1299</v>
       </c>
@@ -3367,10 +3445,10 @@
       <c r="AC26" t="n">
         <v>1299</v>
       </c>
-      <c r="AD26" t="inlineStr"/>
-      <c r="AE26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AD26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="n">
         <v>1299</v>
       </c>
@@ -3387,6 +3465,9 @@
         <v>1299</v>
       </c>
       <c r="AK26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AL26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 16:59
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL26"/>
+  <dimension ref="A1:AM26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,7 @@
     <col width="21" customWidth="1" min="36" max="36"/>
     <col width="21" customWidth="1" min="37" max="37"/>
     <col width="21" customWidth="1" min="38" max="38"/>
+    <col width="21" customWidth="1" min="39" max="39"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -481,185 +482,190 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-23 22:26</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -716,10 +722,10 @@
       <c r="P2" t="n">
         <v>929</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Q2" t="n">
+        <v>929</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
         <v>929</v>
       </c>
@@ -732,25 +738,25 @@
       <c r="V2" t="n">
         <v>929</v>
       </c>
-      <c r="W2" t="inlineStr"/>
+      <c r="W2" t="n">
+        <v>929</v>
+      </c>
       <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="n">
         <v>929</v>
       </c>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="n">
         <v>929</v>
       </c>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="n">
         <v>929</v>
       </c>
@@ -770,6 +776,9 @@
         <v>929</v>
       </c>
       <c r="AL2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -821,26 +830,26 @@
       <c r="O3" t="n">
         <v>569</v>
       </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>569</v>
+      </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="n">
-        <v>569</v>
-      </c>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="n">
         <v>569</v>
       </c>
       <c r="U3" t="n">
         <v>569</v>
       </c>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="n">
-        <v>569</v>
-      </c>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="n">
-        <v>569</v>
-      </c>
+      <c r="V3" t="n">
+        <v>569</v>
+      </c>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="n">
         <v>569</v>
       </c>
@@ -856,10 +865,10 @@
       <c r="AD3" t="n">
         <v>569</v>
       </c>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="n">
         <v>569</v>
       </c>
@@ -876,6 +885,9 @@
         <v>569</v>
       </c>
       <c r="AL3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -945,10 +957,10 @@
       <c r="U4" t="n">
         <v>299</v>
       </c>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="n">
-        <v>299</v>
-      </c>
+      <c r="V4" t="n">
+        <v>299</v>
+      </c>
+      <c r="W4" t="inlineStr"/>
       <c r="X4" t="n">
         <v>299</v>
       </c>
@@ -970,10 +982,10 @@
       <c r="AD4" t="n">
         <v>299</v>
       </c>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="n">
         <v>299</v>
       </c>
@@ -990,6 +1002,9 @@
         <v>299</v>
       </c>
       <c r="AL4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1086,10 +1101,10 @@
       <c r="AD5" t="n">
         <v>569</v>
       </c>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="n">
         <v>569</v>
       </c>
@@ -1106,6 +1121,9 @@
         <v>569</v>
       </c>
       <c r="AL5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1178,10 +1196,10 @@
       <c r="V6" t="n">
         <v>499</v>
       </c>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="n">
-        <v>499</v>
-      </c>
+      <c r="W6" t="n">
+        <v>499</v>
+      </c>
+      <c r="X6" t="inlineStr"/>
       <c r="Y6" t="n">
         <v>499</v>
       </c>
@@ -1200,10 +1218,10 @@
       <c r="AD6" t="n">
         <v>499</v>
       </c>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="n">
         <v>499</v>
       </c>
@@ -1220,6 +1238,9 @@
         <v>499</v>
       </c>
       <c r="AL6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1289,12 +1310,12 @@
       <c r="U7" t="n">
         <v>569</v>
       </c>
-      <c r="V7" t="inlineStr"/>
+      <c r="V7" t="n">
+        <v>569</v>
+      </c>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="n">
         <v>569</v>
       </c>
@@ -1310,10 +1331,10 @@
       <c r="AD7" t="n">
         <v>569</v>
       </c>
-      <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="n">
         <v>569</v>
       </c>
@@ -1330,6 +1351,9 @@
         <v>569</v>
       </c>
       <c r="AL7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1399,14 +1423,14 @@
       <c r="U8" t="n">
         <v>929</v>
       </c>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="n">
-        <v>929</v>
-      </c>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="n">
-        <v>929</v>
-      </c>
+      <c r="V8" t="n">
+        <v>929</v>
+      </c>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="n">
         <v>929</v>
       </c>
@@ -1422,10 +1446,10 @@
       <c r="AD8" t="n">
         <v>929</v>
       </c>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="n">
         <v>929</v>
       </c>
@@ -1442,6 +1466,9 @@
         <v>929</v>
       </c>
       <c r="AL8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1511,10 +1538,10 @@
       <c r="U9" t="n">
         <v>299</v>
       </c>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="n">
-        <v>299</v>
-      </c>
+      <c r="V9" t="n">
+        <v>299</v>
+      </c>
+      <c r="W9" t="inlineStr"/>
       <c r="X9" t="n">
         <v>299</v>
       </c>
@@ -1536,10 +1563,10 @@
       <c r="AD9" t="n">
         <v>299</v>
       </c>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="n">
         <v>299</v>
       </c>
@@ -1556,6 +1583,9 @@
         <v>299</v>
       </c>
       <c r="AL9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1595,10 +1625,10 @@
       <c r="K10" t="n">
         <v>299</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
-        <v>299</v>
-      </c>
+      <c r="L10" t="n">
+        <v>299</v>
+      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
         <v>299</v>
       </c>
@@ -1623,14 +1653,14 @@
       <c r="U10" t="n">
         <v>299</v>
       </c>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="n">
-        <v>299</v>
-      </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="n">
-        <v>299</v>
-      </c>
+      <c r="V10" t="n">
+        <v>299</v>
+      </c>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="n">
         <v>299</v>
       </c>
@@ -1646,10 +1676,10 @@
       <c r="AD10" t="n">
         <v>299</v>
       </c>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF10" t="inlineStr"/>
       <c r="AG10" t="n">
         <v>299</v>
       </c>
@@ -1666,6 +1696,9 @@
         <v>299</v>
       </c>
       <c r="AL10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1738,10 +1771,10 @@
       <c r="V11" t="n">
         <v>2997</v>
       </c>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="n">
+      <c r="W11" t="n">
         <v>2997</v>
       </c>
+      <c r="X11" t="inlineStr"/>
       <c r="Y11" t="n">
         <v>2997</v>
       </c>
@@ -1755,15 +1788,15 @@
         <v>2997</v>
       </c>
       <c r="AC11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AD11" t="n">
         <v>929</v>
       </c>
-      <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF11" t="inlineStr"/>
       <c r="AG11" t="n">
         <v>929</v>
       </c>
@@ -1780,6 +1813,9 @@
         <v>929</v>
       </c>
       <c r="AL11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1855,10 +1891,10 @@
       <c r="W12" t="n">
         <v>569</v>
       </c>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="n">
-        <v>569</v>
-      </c>
+      <c r="X12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="n">
         <v>569</v>
       </c>
@@ -1874,10 +1910,10 @@
       <c r="AD12" t="n">
         <v>569</v>
       </c>
-      <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF12" t="inlineStr"/>
       <c r="AG12" t="n">
         <v>569</v>
       </c>
@@ -1894,6 +1930,9 @@
         <v>569</v>
       </c>
       <c r="AL12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1912,10 +1951,10 @@
       <c r="D13" t="n">
         <v>569</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>569</v>
-      </c>
+      <c r="E13" t="n">
+        <v>569</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>569</v>
       </c>
@@ -1961,14 +2000,14 @@
       <c r="U13" t="n">
         <v>569</v>
       </c>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="n">
-        <v>569</v>
-      </c>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="n">
-        <v>569</v>
-      </c>
+      <c r="V13" t="n">
+        <v>569</v>
+      </c>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="n">
         <v>569</v>
       </c>
@@ -1984,24 +2023,27 @@
       <c r="AD13" t="n">
         <v>569</v>
       </c>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF13" t="inlineStr"/>
       <c r="AG13" t="n">
         <v>569</v>
       </c>
       <c r="AH13" t="n">
         <v>569</v>
       </c>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="n">
         <v>569</v>
       </c>
       <c r="AL13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2041,10 +2083,10 @@
       <c r="K14" t="n">
         <v>794</v>
       </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="n">
+      <c r="L14" t="n">
         <v>794</v>
       </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
         <v>794</v>
       </c>
@@ -2052,7 +2094,7 @@
         <v>794</v>
       </c>
       <c r="P14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="Q14" t="n">
         <v>499</v>
@@ -2069,11 +2111,11 @@
       <c r="U14" t="n">
         <v>499</v>
       </c>
-      <c r="V14" t="inlineStr"/>
+      <c r="V14" t="n">
+        <v>499</v>
+      </c>
       <c r="W14" t="inlineStr"/>
-      <c r="X14" t="n">
-        <v>499</v>
-      </c>
+      <c r="X14" t="inlineStr"/>
       <c r="Y14" t="n">
         <v>499</v>
       </c>
@@ -2114,6 +2156,9 @@
         <v>499</v>
       </c>
       <c r="AL14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2189,10 +2234,10 @@
       <c r="W15" t="n">
         <v>499</v>
       </c>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="n">
-        <v>499</v>
-      </c>
+      <c r="X15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="n">
         <v>499</v>
       </c>
@@ -2202,14 +2247,14 @@
       <c r="AB15" t="n">
         <v>499</v>
       </c>
-      <c r="AC15" t="inlineStr"/>
-      <c r="AD15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF15" t="inlineStr"/>
       <c r="AG15" t="n">
         <v>499</v>
       </c>
@@ -2226,6 +2271,9 @@
         <v>499</v>
       </c>
       <c r="AL15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2286,17 +2334,17 @@
       <c r="R16" t="n">
         <v>299</v>
       </c>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="n">
-        <v>299</v>
-      </c>
+      <c r="S16" t="n">
+        <v>299</v>
+      </c>
+      <c r="T16" t="inlineStr"/>
       <c r="U16" t="n">
         <v>299</v>
       </c>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="n">
-        <v>299</v>
-      </c>
+      <c r="V16" t="n">
+        <v>299</v>
+      </c>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="n">
         <v>299</v>
       </c>
@@ -2318,10 +2366,10 @@
       <c r="AD16" t="n">
         <v>299</v>
       </c>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF16" t="inlineStr"/>
       <c r="AG16" t="n">
         <v>299</v>
       </c>
@@ -2338,6 +2386,9 @@
         <v>299</v>
       </c>
       <c r="AL16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2413,10 +2464,10 @@
       <c r="W17" t="n">
         <v>929</v>
       </c>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="n">
-        <v>929</v>
-      </c>
+      <c r="X17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="n">
         <v>929</v>
       </c>
@@ -2432,10 +2483,10 @@
       <c r="AD17" t="n">
         <v>929</v>
       </c>
-      <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF17" t="inlineStr"/>
       <c r="AG17" t="n">
         <v>929</v>
       </c>
@@ -2452,6 +2503,9 @@
         <v>929</v>
       </c>
       <c r="AL17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2524,11 +2578,11 @@
       <c r="V18" t="n">
         <v>499</v>
       </c>
-      <c r="W18" t="inlineStr"/>
+      <c r="W18" t="n">
+        <v>499</v>
+      </c>
       <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="n">
         <v>499</v>
       </c>
@@ -2544,10 +2598,10 @@
       <c r="AD18" t="n">
         <v>499</v>
       </c>
-      <c r="AE18" t="inlineStr"/>
-      <c r="AF18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF18" t="inlineStr"/>
       <c r="AG18" t="n">
         <v>499</v>
       </c>
@@ -2564,6 +2618,9 @@
         <v>499</v>
       </c>
       <c r="AL18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2628,7 +2685,7 @@
         <v>1299</v>
       </c>
       <c r="T19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="U19" t="n">
         <v>1497</v>
@@ -2636,13 +2693,13 @@
       <c r="V19" t="n">
         <v>1497</v>
       </c>
-      <c r="W19" t="inlineStr"/>
+      <c r="W19" t="n">
+        <v>1497</v>
+      </c>
       <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="n">
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="n">
         <v>465</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>1497</v>
       </c>
       <c r="AA19" t="n">
         <v>1497</v>
@@ -2678,6 +2735,9 @@
         <v>1497</v>
       </c>
       <c r="AL19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AM19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2774,10 +2834,10 @@
       <c r="AD20" t="n">
         <v>929</v>
       </c>
-      <c r="AE20" t="inlineStr"/>
-      <c r="AF20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF20" t="inlineStr"/>
       <c r="AG20" t="n">
         <v>929</v>
       </c>
@@ -2794,6 +2854,9 @@
         <v>929</v>
       </c>
       <c r="AL20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2839,10 +2902,10 @@
       <c r="M21" t="n">
         <v>499</v>
       </c>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="n">
-        <v>499</v>
-      </c>
+      <c r="N21" t="n">
+        <v>499</v>
+      </c>
+      <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
         <v>499</v>
       </c>
@@ -2867,10 +2930,10 @@
       <c r="W21" t="n">
         <v>499</v>
       </c>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="n">
-        <v>499</v>
-      </c>
+      <c r="X21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="n">
         <v>499</v>
       </c>
@@ -2908,6 +2971,9 @@
         <v>499</v>
       </c>
       <c r="AL21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2977,14 +3043,14 @@
       <c r="U22" t="n">
         <v>299</v>
       </c>
-      <c r="V22" t="inlineStr"/>
-      <c r="W22" t="n">
-        <v>299</v>
-      </c>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="n">
-        <v>299</v>
-      </c>
+      <c r="V22" t="n">
+        <v>299</v>
+      </c>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="n">
         <v>299</v>
       </c>
@@ -3000,10 +3066,10 @@
       <c r="AD22" t="n">
         <v>299</v>
       </c>
-      <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF22" t="inlineStr"/>
       <c r="AG22" t="n">
         <v>299</v>
       </c>
@@ -3020,6 +3086,9 @@
         <v>299</v>
       </c>
       <c r="AL22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3092,11 +3161,11 @@
       <c r="V23" t="n">
         <v>1299</v>
       </c>
-      <c r="W23" t="inlineStr"/>
+      <c r="W23" t="n">
+        <v>1299</v>
+      </c>
       <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="n">
         <v>1299</v>
       </c>
@@ -3112,10 +3181,10 @@
       <c r="AD23" t="n">
         <v>1299</v>
       </c>
-      <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AE23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AF23" t="inlineStr"/>
       <c r="AG23" t="n">
         <v>1299</v>
       </c>
@@ -3132,6 +3201,9 @@
         <v>1299</v>
       </c>
       <c r="AL23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AM23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3201,11 +3273,11 @@
       <c r="U24" t="n">
         <v>929</v>
       </c>
-      <c r="V24" t="inlineStr"/>
+      <c r="V24" t="n">
+        <v>929</v>
+      </c>
       <c r="W24" t="inlineStr"/>
-      <c r="X24" t="n">
-        <v>929</v>
-      </c>
+      <c r="X24" t="inlineStr"/>
       <c r="Y24" t="n">
         <v>929</v>
       </c>
@@ -3224,10 +3296,10 @@
       <c r="AD24" t="n">
         <v>929</v>
       </c>
-      <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF24" t="inlineStr"/>
       <c r="AG24" t="n">
         <v>929</v>
       </c>
@@ -3244,6 +3316,9 @@
         <v>929</v>
       </c>
       <c r="AL24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3313,11 +3388,11 @@
       <c r="U25" t="n">
         <v>929</v>
       </c>
-      <c r="V25" t="inlineStr"/>
+      <c r="V25" t="n">
+        <v>929</v>
+      </c>
       <c r="W25" t="inlineStr"/>
-      <c r="X25" t="n">
-        <v>929</v>
-      </c>
+      <c r="X25" t="inlineStr"/>
       <c r="Y25" t="n">
         <v>929</v>
       </c>
@@ -3336,10 +3411,10 @@
       <c r="AD25" t="n">
         <v>929</v>
       </c>
-      <c r="AE25" t="inlineStr"/>
-      <c r="AF25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF25" t="inlineStr"/>
       <c r="AG25" t="n">
         <v>929</v>
       </c>
@@ -3356,6 +3431,9 @@
         <v>929</v>
       </c>
       <c r="AL25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3425,14 +3503,14 @@
       <c r="U26" t="n">
         <v>1299</v>
       </c>
-      <c r="V26" t="inlineStr"/>
-      <c r="W26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="V26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="n">
         <v>1299</v>
       </c>
@@ -3448,10 +3526,10 @@
       <c r="AD26" t="n">
         <v>1299</v>
       </c>
-      <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AE26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AF26" t="inlineStr"/>
       <c r="AG26" t="n">
         <v>1299</v>
       </c>
@@ -3468,6 +3546,9 @@
         <v>1299</v>
       </c>
       <c r="AL26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AM26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 19:03
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AN26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +472,7 @@
     <col width="21" customWidth="1" min="37" max="37"/>
     <col width="21" customWidth="1" min="38" max="38"/>
     <col width="21" customWidth="1" min="39" max="39"/>
+    <col width="21" customWidth="1" min="40" max="40"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -482,190 +483,195 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 00:29</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -725,10 +731,10 @@
       <c r="Q2" t="n">
         <v>929</v>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="n">
-        <v>929</v>
-      </c>
+      <c r="R2" t="n">
+        <v>929</v>
+      </c>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="n">
         <v>929</v>
       </c>
@@ -741,25 +747,25 @@
       <c r="W2" t="n">
         <v>929</v>
       </c>
-      <c r="X2" t="inlineStr"/>
+      <c r="X2" t="n">
+        <v>929</v>
+      </c>
       <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
         <v>929</v>
       </c>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="n">
         <v>929</v>
       </c>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
         <v>929</v>
       </c>
@@ -779,6 +785,9 @@
         <v>929</v>
       </c>
       <c r="AM2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -788,9 +797,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>569</v>
       </c>
@@ -833,26 +840,26 @@
       <c r="P3" t="n">
         <v>569</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
+      <c r="Q3" t="n">
+        <v>569</v>
+      </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="n">
-        <v>569</v>
-      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
         <v>569</v>
       </c>
       <c r="V3" t="n">
         <v>569</v>
       </c>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="n">
-        <v>569</v>
-      </c>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="n">
-        <v>569</v>
-      </c>
+      <c r="W3" t="n">
+        <v>569</v>
+      </c>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
         <v>569</v>
       </c>
@@ -868,10 +875,10 @@
       <c r="AE3" t="n">
         <v>569</v>
       </c>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="n">
         <v>569</v>
       </c>
@@ -888,6 +895,9 @@
         <v>569</v>
       </c>
       <c r="AM3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -960,10 +970,10 @@
       <c r="V4" t="n">
         <v>299</v>
       </c>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="n">
-        <v>299</v>
-      </c>
+      <c r="W4" t="n">
+        <v>299</v>
+      </c>
+      <c r="X4" t="inlineStr"/>
       <c r="Y4" t="n">
         <v>299</v>
       </c>
@@ -985,10 +995,10 @@
       <c r="AE4" t="n">
         <v>299</v>
       </c>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="n">
         <v>299</v>
       </c>
@@ -1005,6 +1015,9 @@
         <v>299</v>
       </c>
       <c r="AM4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1104,10 +1117,10 @@
       <c r="AE5" t="n">
         <v>569</v>
       </c>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="n">
         <v>569</v>
       </c>
@@ -1124,6 +1137,9 @@
         <v>569</v>
       </c>
       <c r="AM5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1199,10 +1215,10 @@
       <c r="W6" t="n">
         <v>499</v>
       </c>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="n">
-        <v>499</v>
-      </c>
+      <c r="X6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="n">
         <v>499</v>
       </c>
@@ -1221,10 +1237,10 @@
       <c r="AE6" t="n">
         <v>499</v>
       </c>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="n">
         <v>499</v>
       </c>
@@ -1241,6 +1257,9 @@
         <v>499</v>
       </c>
       <c r="AM6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1313,12 +1332,12 @@
       <c r="V7" t="n">
         <v>569</v>
       </c>
-      <c r="W7" t="inlineStr"/>
+      <c r="W7" t="n">
+        <v>569</v>
+      </c>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
         <v>569</v>
       </c>
@@ -1334,10 +1353,10 @@
       <c r="AE7" t="n">
         <v>569</v>
       </c>
-      <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="n">
         <v>569</v>
       </c>
@@ -1354,6 +1373,9 @@
         <v>569</v>
       </c>
       <c r="AM7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1426,14 +1448,14 @@
       <c r="V8" t="n">
         <v>929</v>
       </c>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="n">
-        <v>929</v>
-      </c>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="n">
-        <v>929</v>
-      </c>
+      <c r="W8" t="n">
+        <v>929</v>
+      </c>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
         <v>929</v>
       </c>
@@ -1449,10 +1471,10 @@
       <c r="AE8" t="n">
         <v>929</v>
       </c>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="n">
         <v>929</v>
       </c>
@@ -1469,6 +1491,9 @@
         <v>929</v>
       </c>
       <c r="AM8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1541,10 +1566,10 @@
       <c r="V9" t="n">
         <v>299</v>
       </c>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="n">
-        <v>299</v>
-      </c>
+      <c r="W9" t="n">
+        <v>299</v>
+      </c>
+      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="n">
         <v>299</v>
       </c>
@@ -1566,10 +1591,10 @@
       <c r="AE9" t="n">
         <v>299</v>
       </c>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="n">
         <v>299</v>
       </c>
@@ -1586,6 +1611,9 @@
         <v>299</v>
       </c>
       <c r="AM9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1628,10 +1656,10 @@
       <c r="L10" t="n">
         <v>299</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="n">
-        <v>299</v>
-      </c>
+      <c r="M10" t="n">
+        <v>299</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
         <v>299</v>
       </c>
@@ -1656,14 +1684,14 @@
       <c r="V10" t="n">
         <v>299</v>
       </c>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="n">
-        <v>299</v>
-      </c>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="n">
-        <v>299</v>
-      </c>
+      <c r="W10" t="n">
+        <v>299</v>
+      </c>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
         <v>299</v>
       </c>
@@ -1679,10 +1707,10 @@
       <c r="AE10" t="n">
         <v>299</v>
       </c>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG10" t="inlineStr"/>
       <c r="AH10" t="n">
         <v>299</v>
       </c>
@@ -1699,6 +1727,9 @@
         <v>299</v>
       </c>
       <c r="AM10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1774,10 +1805,10 @@
       <c r="W11" t="n">
         <v>2997</v>
       </c>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="n">
+      <c r="X11" t="n">
         <v>2997</v>
       </c>
+      <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="n">
         <v>2997</v>
       </c>
@@ -1791,15 +1822,15 @@
         <v>2997</v>
       </c>
       <c r="AD11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AE11" t="n">
         <v>929</v>
       </c>
-      <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="n">
         <v>929</v>
       </c>
@@ -1816,6 +1847,9 @@
         <v>929</v>
       </c>
       <c r="AM11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1894,10 +1928,10 @@
       <c r="X12" t="n">
         <v>569</v>
       </c>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y12" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
         <v>569</v>
       </c>
@@ -1913,10 +1947,10 @@
       <c r="AE12" t="n">
         <v>569</v>
       </c>
-      <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="n">
         <v>569</v>
       </c>
@@ -1933,6 +1967,9 @@
         <v>569</v>
       </c>
       <c r="AM12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1954,10 +1991,10 @@
       <c r="E13" t="n">
         <v>569</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>569</v>
-      </c>
+      <c r="F13" t="n">
+        <v>569</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>569</v>
       </c>
@@ -2003,14 +2040,14 @@
       <c r="V13" t="n">
         <v>569</v>
       </c>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="n">
-        <v>569</v>
-      </c>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="n">
-        <v>569</v>
-      </c>
+      <c r="W13" t="n">
+        <v>569</v>
+      </c>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
         <v>569</v>
       </c>
@@ -2026,24 +2063,27 @@
       <c r="AE13" t="n">
         <v>569</v>
       </c>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="n">
         <v>569</v>
       </c>
       <c r="AI13" t="n">
         <v>569</v>
       </c>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="n">
         <v>569</v>
       </c>
       <c r="AM13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2086,10 +2126,10 @@
       <c r="L14" t="n">
         <v>794</v>
       </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="n">
+      <c r="M14" t="n">
         <v>794</v>
       </c>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
         <v>794</v>
       </c>
@@ -2097,7 +2137,7 @@
         <v>794</v>
       </c>
       <c r="Q14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="R14" t="n">
         <v>499</v>
@@ -2114,11 +2154,11 @@
       <c r="V14" t="n">
         <v>499</v>
       </c>
-      <c r="W14" t="inlineStr"/>
+      <c r="W14" t="n">
+        <v>499</v>
+      </c>
       <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="n">
         <v>499</v>
       </c>
@@ -2159,6 +2199,9 @@
         <v>499</v>
       </c>
       <c r="AM14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2237,10 +2280,10 @@
       <c r="X15" t="n">
         <v>499</v>
       </c>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y15" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
         <v>499</v>
       </c>
@@ -2250,14 +2293,14 @@
       <c r="AC15" t="n">
         <v>499</v>
       </c>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="n">
         <v>499</v>
       </c>
@@ -2274,6 +2317,9 @@
         <v>499</v>
       </c>
       <c r="AM15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2337,17 +2383,17 @@
       <c r="S16" t="n">
         <v>299</v>
       </c>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="n">
-        <v>299</v>
-      </c>
+      <c r="T16" t="n">
+        <v>299</v>
+      </c>
+      <c r="U16" t="inlineStr"/>
       <c r="V16" t="n">
         <v>299</v>
       </c>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="n">
-        <v>299</v>
-      </c>
+      <c r="W16" t="n">
+        <v>299</v>
+      </c>
+      <c r="X16" t="inlineStr"/>
       <c r="Y16" t="n">
         <v>299</v>
       </c>
@@ -2369,10 +2415,10 @@
       <c r="AE16" t="n">
         <v>299</v>
       </c>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="n">
         <v>299</v>
       </c>
@@ -2389,6 +2435,9 @@
         <v>299</v>
       </c>
       <c r="AM16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2467,10 +2516,10 @@
       <c r="X17" t="n">
         <v>929</v>
       </c>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y17" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
         <v>929</v>
       </c>
@@ -2486,10 +2535,10 @@
       <c r="AE17" t="n">
         <v>929</v>
       </c>
-      <c r="AF17" t="inlineStr"/>
-      <c r="AG17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="n">
         <v>929</v>
       </c>
@@ -2506,6 +2555,9 @@
         <v>929</v>
       </c>
       <c r="AM17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2581,11 +2633,11 @@
       <c r="W18" t="n">
         <v>499</v>
       </c>
-      <c r="X18" t="inlineStr"/>
+      <c r="X18" t="n">
+        <v>499</v>
+      </c>
       <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
         <v>499</v>
       </c>
@@ -2601,10 +2653,10 @@
       <c r="AE18" t="n">
         <v>499</v>
       </c>
-      <c r="AF18" t="inlineStr"/>
-      <c r="AG18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="n">
         <v>499</v>
       </c>
@@ -2621,6 +2673,9 @@
         <v>499</v>
       </c>
       <c r="AM18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2688,7 +2743,7 @@
         <v>1299</v>
       </c>
       <c r="U19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="V19" t="n">
         <v>1497</v>
@@ -2696,13 +2751,13 @@
       <c r="W19" t="n">
         <v>1497</v>
       </c>
-      <c r="X19" t="inlineStr"/>
+      <c r="X19" t="n">
+        <v>1497</v>
+      </c>
       <c r="Y19" t="inlineStr"/>
-      <c r="Z19" t="n">
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="n">
         <v>465</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>1497</v>
       </c>
       <c r="AB19" t="n">
         <v>1497</v>
@@ -2738,6 +2793,9 @@
         <v>1497</v>
       </c>
       <c r="AM19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AN19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2837,10 +2895,10 @@
       <c r="AE20" t="n">
         <v>929</v>
       </c>
-      <c r="AF20" t="inlineStr"/>
-      <c r="AG20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG20" t="inlineStr"/>
       <c r="AH20" t="n">
         <v>929</v>
       </c>
@@ -2857,6 +2915,9 @@
         <v>929</v>
       </c>
       <c r="AM20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2905,10 +2966,10 @@
       <c r="N21" t="n">
         <v>499</v>
       </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="n">
-        <v>499</v>
-      </c>
+      <c r="O21" t="n">
+        <v>499</v>
+      </c>
+      <c r="P21" t="inlineStr"/>
       <c r="Q21" t="n">
         <v>499</v>
       </c>
@@ -2933,10 +2994,10 @@
       <c r="X21" t="n">
         <v>499</v>
       </c>
-      <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="n">
         <v>499</v>
       </c>
@@ -2974,6 +3035,9 @@
         <v>499</v>
       </c>
       <c r="AM21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3046,14 +3110,14 @@
       <c r="V22" t="n">
         <v>299</v>
       </c>
-      <c r="W22" t="inlineStr"/>
-      <c r="X22" t="n">
-        <v>299</v>
-      </c>
-      <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="n">
-        <v>299</v>
-      </c>
+      <c r="W22" t="n">
+        <v>299</v>
+      </c>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="n">
         <v>299</v>
       </c>
@@ -3069,10 +3133,10 @@
       <c r="AE22" t="n">
         <v>299</v>
       </c>
-      <c r="AF22" t="inlineStr"/>
-      <c r="AG22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="n">
         <v>299</v>
       </c>
@@ -3089,6 +3153,9 @@
         <v>299</v>
       </c>
       <c r="AM22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3164,11 +3231,11 @@
       <c r="W23" t="n">
         <v>1299</v>
       </c>
-      <c r="X23" t="inlineStr"/>
+      <c r="X23" t="n">
+        <v>1299</v>
+      </c>
       <c r="Y23" t="inlineStr"/>
-      <c r="Z23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
         <v>1299</v>
       </c>
@@ -3184,10 +3251,10 @@
       <c r="AE23" t="n">
         <v>1299</v>
       </c>
-      <c r="AF23" t="inlineStr"/>
-      <c r="AG23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AF23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="n">
         <v>1299</v>
       </c>
@@ -3204,6 +3271,9 @@
         <v>1299</v>
       </c>
       <c r="AM23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AN23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3276,11 +3346,11 @@
       <c r="V24" t="n">
         <v>929</v>
       </c>
-      <c r="W24" t="inlineStr"/>
+      <c r="W24" t="n">
+        <v>929</v>
+      </c>
       <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="n">
         <v>929</v>
       </c>
@@ -3299,10 +3369,10 @@
       <c r="AE24" t="n">
         <v>929</v>
       </c>
-      <c r="AF24" t="inlineStr"/>
-      <c r="AG24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="n">
         <v>929</v>
       </c>
@@ -3319,6 +3389,9 @@
         <v>929</v>
       </c>
       <c r="AM24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3391,11 +3464,11 @@
       <c r="V25" t="n">
         <v>929</v>
       </c>
-      <c r="W25" t="inlineStr"/>
+      <c r="W25" t="n">
+        <v>929</v>
+      </c>
       <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="n">
         <v>929</v>
       </c>
@@ -3414,10 +3487,10 @@
       <c r="AE25" t="n">
         <v>929</v>
       </c>
-      <c r="AF25" t="inlineStr"/>
-      <c r="AG25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG25" t="inlineStr"/>
       <c r="AH25" t="n">
         <v>929</v>
       </c>
@@ -3434,6 +3507,9 @@
         <v>929</v>
       </c>
       <c r="AM25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3506,14 +3582,14 @@
       <c r="V26" t="n">
         <v>1299</v>
       </c>
-      <c r="W26" t="inlineStr"/>
-      <c r="X26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="W26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
         <v>1299</v>
       </c>
@@ -3529,10 +3605,10 @@
       <c r="AE26" t="n">
         <v>1299</v>
       </c>
-      <c r="AF26" t="inlineStr"/>
-      <c r="AG26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AF26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AG26" t="inlineStr"/>
       <c r="AH26" t="n">
         <v>1299</v>
       </c>
@@ -3549,6 +3625,9 @@
         <v>1299</v>
       </c>
       <c r="AM26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AN26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 20:45
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN26"/>
+  <dimension ref="A1:AO26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +473,7 @@
     <col width="21" customWidth="1" min="38" max="38"/>
     <col width="21" customWidth="1" min="39" max="39"/>
     <col width="21" customWidth="1" min="40" max="40"/>
+    <col width="21" customWidth="1" min="41" max="41"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -483,195 +484,200 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 02:11</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -734,10 +740,10 @@
       <c r="R2" t="n">
         <v>929</v>
       </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="n">
-        <v>929</v>
-      </c>
+      <c r="S2" t="n">
+        <v>929</v>
+      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
         <v>929</v>
       </c>
@@ -750,25 +756,25 @@
       <c r="X2" t="n">
         <v>929</v>
       </c>
-      <c r="Y2" t="inlineStr"/>
+      <c r="Y2" t="n">
+        <v>929</v>
+      </c>
       <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="n">
         <v>929</v>
       </c>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="n">
         <v>929</v>
       </c>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="n">
         <v>929</v>
       </c>
@@ -788,6 +794,9 @@
         <v>929</v>
       </c>
       <c r="AN2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -797,10 +806,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="n">
+        <v>569</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>569</v>
       </c>
@@ -843,26 +852,26 @@
       <c r="Q3" t="n">
         <v>569</v>
       </c>
-      <c r="R3" t="inlineStr"/>
+      <c r="R3" t="n">
+        <v>569</v>
+      </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
-        <v>569</v>
-      </c>
+      <c r="U3" t="inlineStr"/>
       <c r="V3" t="n">
         <v>569</v>
       </c>
       <c r="W3" t="n">
         <v>569</v>
       </c>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="n">
-        <v>569</v>
-      </c>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="n">
-        <v>569</v>
-      </c>
+      <c r="X3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="n">
         <v>569</v>
       </c>
@@ -878,10 +887,10 @@
       <c r="AF3" t="n">
         <v>569</v>
       </c>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH3" t="inlineStr"/>
       <c r="AI3" t="n">
         <v>569</v>
       </c>
@@ -898,6 +907,9 @@
         <v>569</v>
       </c>
       <c r="AN3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -973,10 +985,10 @@
       <c r="W4" t="n">
         <v>299</v>
       </c>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="n">
-        <v>299</v>
-      </c>
+      <c r="X4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="n">
         <v>299</v>
       </c>
@@ -998,10 +1010,10 @@
       <c r="AF4" t="n">
         <v>299</v>
       </c>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH4" t="inlineStr"/>
       <c r="AI4" t="n">
         <v>299</v>
       </c>
@@ -1018,6 +1030,9 @@
         <v>299</v>
       </c>
       <c r="AN4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1120,10 +1135,10 @@
       <c r="AF5" t="n">
         <v>569</v>
       </c>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH5" t="inlineStr"/>
       <c r="AI5" t="n">
         <v>569</v>
       </c>
@@ -1140,6 +1155,9 @@
         <v>569</v>
       </c>
       <c r="AN5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1218,10 +1236,10 @@
       <c r="X6" t="n">
         <v>499</v>
       </c>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y6" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
         <v>499</v>
       </c>
@@ -1240,10 +1258,10 @@
       <c r="AF6" t="n">
         <v>499</v>
       </c>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH6" t="inlineStr"/>
       <c r="AI6" t="n">
         <v>499</v>
       </c>
@@ -1260,6 +1278,9 @@
         <v>499</v>
       </c>
       <c r="AN6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1335,12 +1356,12 @@
       <c r="W7" t="n">
         <v>569</v>
       </c>
-      <c r="X7" t="inlineStr"/>
+      <c r="X7" t="n">
+        <v>569</v>
+      </c>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="n">
         <v>569</v>
       </c>
@@ -1356,10 +1377,10 @@
       <c r="AF7" t="n">
         <v>569</v>
       </c>
-      <c r="AG7" t="inlineStr"/>
-      <c r="AH7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH7" t="inlineStr"/>
       <c r="AI7" t="n">
         <v>569</v>
       </c>
@@ -1376,6 +1397,9 @@
         <v>569</v>
       </c>
       <c r="AN7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1451,14 +1475,14 @@
       <c r="W8" t="n">
         <v>929</v>
       </c>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="n">
-        <v>929</v>
-      </c>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="n">
-        <v>929</v>
-      </c>
+      <c r="X8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="n">
         <v>929</v>
       </c>
@@ -1474,10 +1498,10 @@
       <c r="AF8" t="n">
         <v>929</v>
       </c>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH8" t="inlineStr"/>
       <c r="AI8" t="n">
         <v>929</v>
       </c>
@@ -1494,6 +1518,9 @@
         <v>929</v>
       </c>
       <c r="AN8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1569,10 +1596,10 @@
       <c r="W9" t="n">
         <v>299</v>
       </c>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="n">
-        <v>299</v>
-      </c>
+      <c r="X9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="n">
         <v>299</v>
       </c>
@@ -1594,10 +1621,10 @@
       <c r="AF9" t="n">
         <v>299</v>
       </c>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH9" t="inlineStr"/>
       <c r="AI9" t="n">
         <v>299</v>
       </c>
@@ -1614,6 +1641,9 @@
         <v>299</v>
       </c>
       <c r="AN9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1659,10 +1689,10 @@
       <c r="M10" t="n">
         <v>299</v>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="n">
-        <v>299</v>
-      </c>
+      <c r="N10" t="n">
+        <v>299</v>
+      </c>
+      <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
         <v>299</v>
       </c>
@@ -1687,14 +1717,14 @@
       <c r="W10" t="n">
         <v>299</v>
       </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="n">
-        <v>299</v>
-      </c>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="n">
-        <v>299</v>
-      </c>
+      <c r="X10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="n">
         <v>299</v>
       </c>
@@ -1710,10 +1740,10 @@
       <c r="AF10" t="n">
         <v>299</v>
       </c>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH10" t="inlineStr"/>
       <c r="AI10" t="n">
         <v>299</v>
       </c>
@@ -1730,6 +1760,9 @@
         <v>299</v>
       </c>
       <c r="AN10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1808,10 +1841,10 @@
       <c r="X11" t="n">
         <v>2997</v>
       </c>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="n">
+      <c r="Y11" t="n">
         <v>2997</v>
       </c>
+      <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
         <v>2997</v>
       </c>
@@ -1825,15 +1858,15 @@
         <v>2997</v>
       </c>
       <c r="AE11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AF11" t="n">
         <v>929</v>
       </c>
-      <c r="AG11" t="inlineStr"/>
-      <c r="AH11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH11" t="inlineStr"/>
       <c r="AI11" t="n">
         <v>929</v>
       </c>
@@ -1850,6 +1883,9 @@
         <v>929</v>
       </c>
       <c r="AN11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1931,10 +1967,10 @@
       <c r="Y12" t="n">
         <v>569</v>
       </c>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="n">
         <v>569</v>
       </c>
@@ -1950,10 +1986,10 @@
       <c r="AF12" t="n">
         <v>569</v>
       </c>
-      <c r="AG12" t="inlineStr"/>
-      <c r="AH12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH12" t="inlineStr"/>
       <c r="AI12" t="n">
         <v>569</v>
       </c>
@@ -1970,6 +2006,9 @@
         <v>569</v>
       </c>
       <c r="AN12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1994,10 +2033,10 @@
       <c r="F13" t="n">
         <v>569</v>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>569</v>
-      </c>
+      <c r="G13" t="n">
+        <v>569</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>569</v>
       </c>
@@ -2043,14 +2082,14 @@
       <c r="W13" t="n">
         <v>569</v>
       </c>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="n">
-        <v>569</v>
-      </c>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="n">
-        <v>569</v>
-      </c>
+      <c r="X13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="n">
         <v>569</v>
       </c>
@@ -2066,24 +2105,27 @@
       <c r="AF13" t="n">
         <v>569</v>
       </c>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH13" t="inlineStr"/>
       <c r="AI13" t="n">
         <v>569</v>
       </c>
       <c r="AJ13" t="n">
         <v>569</v>
       </c>
-      <c r="AK13" t="inlineStr"/>
-      <c r="AL13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="n">
         <v>569</v>
       </c>
       <c r="AN13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2129,10 +2171,10 @@
       <c r="M14" t="n">
         <v>794</v>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="n">
+      <c r="N14" t="n">
         <v>794</v>
       </c>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
         <v>794</v>
       </c>
@@ -2140,7 +2182,7 @@
         <v>794</v>
       </c>
       <c r="R14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="S14" t="n">
         <v>499</v>
@@ -2157,11 +2199,11 @@
       <c r="W14" t="n">
         <v>499</v>
       </c>
-      <c r="X14" t="inlineStr"/>
+      <c r="X14" t="n">
+        <v>499</v>
+      </c>
       <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
         <v>499</v>
       </c>
@@ -2202,6 +2244,9 @@
         <v>499</v>
       </c>
       <c r="AN14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2283,10 +2328,10 @@
       <c r="Y15" t="n">
         <v>499</v>
       </c>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="n">
         <v>499</v>
       </c>
@@ -2296,14 +2341,14 @@
       <c r="AD15" t="n">
         <v>499</v>
       </c>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AG15" t="inlineStr"/>
-      <c r="AH15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH15" t="inlineStr"/>
       <c r="AI15" t="n">
         <v>499</v>
       </c>
@@ -2320,6 +2365,9 @@
         <v>499</v>
       </c>
       <c r="AN15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2386,17 +2434,17 @@
       <c r="T16" t="n">
         <v>299</v>
       </c>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="n">
-        <v>299</v>
-      </c>
+      <c r="U16" t="n">
+        <v>299</v>
+      </c>
+      <c r="V16" t="inlineStr"/>
       <c r="W16" t="n">
         <v>299</v>
       </c>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="n">
-        <v>299</v>
-      </c>
+      <c r="X16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="n">
         <v>299</v>
       </c>
@@ -2418,10 +2466,10 @@
       <c r="AF16" t="n">
         <v>299</v>
       </c>
-      <c r="AG16" t="inlineStr"/>
-      <c r="AH16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH16" t="inlineStr"/>
       <c r="AI16" t="n">
         <v>299</v>
       </c>
@@ -2438,6 +2486,9 @@
         <v>299</v>
       </c>
       <c r="AN16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2519,10 +2570,10 @@
       <c r="Y17" t="n">
         <v>929</v>
       </c>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="n">
         <v>929</v>
       </c>
@@ -2538,10 +2589,10 @@
       <c r="AF17" t="n">
         <v>929</v>
       </c>
-      <c r="AG17" t="inlineStr"/>
-      <c r="AH17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH17" t="inlineStr"/>
       <c r="AI17" t="n">
         <v>929</v>
       </c>
@@ -2558,6 +2609,9 @@
         <v>929</v>
       </c>
       <c r="AN17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2636,11 +2690,11 @@
       <c r="X18" t="n">
         <v>499</v>
       </c>
-      <c r="Y18" t="inlineStr"/>
+      <c r="Y18" t="n">
+        <v>499</v>
+      </c>
       <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="n">
         <v>499</v>
       </c>
@@ -2656,10 +2710,10 @@
       <c r="AF18" t="n">
         <v>499</v>
       </c>
-      <c r="AG18" t="inlineStr"/>
-      <c r="AH18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH18" t="inlineStr"/>
       <c r="AI18" t="n">
         <v>499</v>
       </c>
@@ -2676,6 +2730,9 @@
         <v>499</v>
       </c>
       <c r="AN18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2746,7 +2803,7 @@
         <v>1299</v>
       </c>
       <c r="V19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="W19" t="n">
         <v>1497</v>
@@ -2754,13 +2811,13 @@
       <c r="X19" t="n">
         <v>1497</v>
       </c>
-      <c r="Y19" t="inlineStr"/>
+      <c r="Y19" t="n">
+        <v>1497</v>
+      </c>
       <c r="Z19" t="inlineStr"/>
-      <c r="AA19" t="n">
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="n">
         <v>465</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>1497</v>
       </c>
       <c r="AC19" t="n">
         <v>1497</v>
@@ -2796,6 +2853,9 @@
         <v>1497</v>
       </c>
       <c r="AN19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AO19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2898,10 +2958,10 @@
       <c r="AF20" t="n">
         <v>929</v>
       </c>
-      <c r="AG20" t="inlineStr"/>
-      <c r="AH20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH20" t="inlineStr"/>
       <c r="AI20" t="n">
         <v>929</v>
       </c>
@@ -2918,6 +2978,9 @@
         <v>929</v>
       </c>
       <c r="AN20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2969,10 +3032,10 @@
       <c r="O21" t="n">
         <v>499</v>
       </c>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="n">
-        <v>499</v>
-      </c>
+      <c r="P21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
         <v>499</v>
       </c>
@@ -2997,10 +3060,10 @@
       <c r="Y21" t="n">
         <v>499</v>
       </c>
-      <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="n">
         <v>499</v>
       </c>
@@ -3038,6 +3101,9 @@
         <v>499</v>
       </c>
       <c r="AN21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3113,14 +3179,14 @@
       <c r="W22" t="n">
         <v>299</v>
       </c>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="n">
-        <v>299</v>
-      </c>
-      <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="n">
-        <v>299</v>
-      </c>
+      <c r="X22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="n">
         <v>299</v>
       </c>
@@ -3136,10 +3202,10 @@
       <c r="AF22" t="n">
         <v>299</v>
       </c>
-      <c r="AG22" t="inlineStr"/>
-      <c r="AH22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH22" t="inlineStr"/>
       <c r="AI22" t="n">
         <v>299</v>
       </c>
@@ -3156,6 +3222,9 @@
         <v>299</v>
       </c>
       <c r="AN22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3234,11 +3303,11 @@
       <c r="X23" t="n">
         <v>1299</v>
       </c>
-      <c r="Y23" t="inlineStr"/>
+      <c r="Y23" t="n">
+        <v>1299</v>
+      </c>
       <c r="Z23" t="inlineStr"/>
-      <c r="AA23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="n">
         <v>1299</v>
       </c>
@@ -3254,10 +3323,10 @@
       <c r="AF23" t="n">
         <v>1299</v>
       </c>
-      <c r="AG23" t="inlineStr"/>
-      <c r="AH23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AG23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="n">
         <v>1299</v>
       </c>
@@ -3274,6 +3343,9 @@
         <v>1299</v>
       </c>
       <c r="AN23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AO23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3349,11 +3421,11 @@
       <c r="W24" t="n">
         <v>929</v>
       </c>
-      <c r="X24" t="inlineStr"/>
+      <c r="X24" t="n">
+        <v>929</v>
+      </c>
       <c r="Y24" t="inlineStr"/>
-      <c r="Z24" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
         <v>929</v>
       </c>
@@ -3372,10 +3444,10 @@
       <c r="AF24" t="n">
         <v>929</v>
       </c>
-      <c r="AG24" t="inlineStr"/>
-      <c r="AH24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="n">
         <v>929</v>
       </c>
@@ -3392,6 +3464,9 @@
         <v>929</v>
       </c>
       <c r="AN24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3467,11 +3542,11 @@
       <c r="W25" t="n">
         <v>929</v>
       </c>
-      <c r="X25" t="inlineStr"/>
+      <c r="X25" t="n">
+        <v>929</v>
+      </c>
       <c r="Y25" t="inlineStr"/>
-      <c r="Z25" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
         <v>929</v>
       </c>
@@ -3490,10 +3565,10 @@
       <c r="AF25" t="n">
         <v>929</v>
       </c>
-      <c r="AG25" t="inlineStr"/>
-      <c r="AH25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH25" t="inlineStr"/>
       <c r="AI25" t="n">
         <v>929</v>
       </c>
@@ -3510,6 +3585,9 @@
         <v>929</v>
       </c>
       <c r="AN25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3585,14 +3663,14 @@
       <c r="W26" t="n">
         <v>1299</v>
       </c>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="X26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="n">
         <v>1299</v>
       </c>
@@ -3608,10 +3686,10 @@
       <c r="AF26" t="n">
         <v>1299</v>
       </c>
-      <c r="AG26" t="inlineStr"/>
-      <c r="AH26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AG26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AH26" t="inlineStr"/>
       <c r="AI26" t="n">
         <v>1299</v>
       </c>
@@ -3628,6 +3706,9 @@
         <v>1299</v>
       </c>
       <c r="AN26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AO26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-23 22:45
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO26"/>
+  <dimension ref="A1:AP26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,7 @@
     <col width="21" customWidth="1" min="39" max="39"/>
     <col width="21" customWidth="1" min="40" max="40"/>
     <col width="21" customWidth="1" min="41" max="41"/>
+    <col width="21" customWidth="1" min="42" max="42"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -484,200 +485,205 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 04:11</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -743,10 +749,10 @@
       <c r="S2" t="n">
         <v>929</v>
       </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
-        <v>929</v>
-      </c>
+      <c r="T2" t="n">
+        <v>929</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="n">
         <v>929</v>
       </c>
@@ -759,25 +765,25 @@
       <c r="Y2" t="n">
         <v>929</v>
       </c>
-      <c r="Z2" t="inlineStr"/>
+      <c r="Z2" t="n">
+        <v>929</v>
+      </c>
       <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="n">
         <v>929</v>
       </c>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="n">
         <v>929</v>
       </c>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="n">
         <v>929</v>
       </c>
@@ -797,6 +803,9 @@
         <v>929</v>
       </c>
       <c r="AO2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -809,10 +818,10 @@
       <c r="B3" t="n">
         <v>569</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>569</v>
-      </c>
+      <c r="C3" t="n">
+        <v>569</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>569</v>
       </c>
@@ -855,26 +864,26 @@
       <c r="R3" t="n">
         <v>569</v>
       </c>
-      <c r="S3" t="inlineStr"/>
+      <c r="S3" t="n">
+        <v>569</v>
+      </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
-      <c r="V3" t="n">
-        <v>569</v>
-      </c>
+      <c r="V3" t="inlineStr"/>
       <c r="W3" t="n">
         <v>569</v>
       </c>
       <c r="X3" t="n">
         <v>569</v>
       </c>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="n">
         <v>569</v>
       </c>
@@ -890,10 +899,10 @@
       <c r="AG3" t="n">
         <v>569</v>
       </c>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="n">
         <v>569</v>
       </c>
@@ -910,6 +919,9 @@
         <v>569</v>
       </c>
       <c r="AO3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -988,10 +1000,10 @@
       <c r="X4" t="n">
         <v>299</v>
       </c>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y4" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
         <v>299</v>
       </c>
@@ -1013,10 +1025,10 @@
       <c r="AG4" t="n">
         <v>299</v>
       </c>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI4" t="inlineStr"/>
       <c r="AJ4" t="n">
         <v>299</v>
       </c>
@@ -1033,6 +1045,9 @@
         <v>299</v>
       </c>
       <c r="AO4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1042,9 +1057,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>569</v>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
         <v>569</v>
       </c>
@@ -1138,10 +1151,10 @@
       <c r="AG5" t="n">
         <v>569</v>
       </c>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI5" t="inlineStr"/>
       <c r="AJ5" t="n">
         <v>569</v>
       </c>
@@ -1158,6 +1171,9 @@
         <v>569</v>
       </c>
       <c r="AO5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1239,10 +1255,10 @@
       <c r="Y6" t="n">
         <v>499</v>
       </c>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="n">
         <v>499</v>
       </c>
@@ -1261,10 +1277,10 @@
       <c r="AG6" t="n">
         <v>499</v>
       </c>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AH6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="n">
         <v>499</v>
       </c>
@@ -1281,6 +1297,9 @@
         <v>499</v>
       </c>
       <c r="AO6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1359,12 +1378,12 @@
       <c r="X7" t="n">
         <v>569</v>
       </c>
-      <c r="Y7" t="inlineStr"/>
+      <c r="Y7" t="n">
+        <v>569</v>
+      </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="n">
         <v>569</v>
       </c>
@@ -1380,10 +1399,10 @@
       <c r="AG7" t="n">
         <v>569</v>
       </c>
-      <c r="AH7" t="inlineStr"/>
-      <c r="AI7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI7" t="inlineStr"/>
       <c r="AJ7" t="n">
         <v>569</v>
       </c>
@@ -1400,6 +1419,9 @@
         <v>569</v>
       </c>
       <c r="AO7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1478,14 +1500,14 @@
       <c r="X8" t="n">
         <v>929</v>
       </c>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y8" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="n">
         <v>929</v>
       </c>
@@ -1501,10 +1523,10 @@
       <c r="AG8" t="n">
         <v>929</v>
       </c>
-      <c r="AH8" t="inlineStr"/>
-      <c r="AI8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI8" t="inlineStr"/>
       <c r="AJ8" t="n">
         <v>929</v>
       </c>
@@ -1521,6 +1543,9 @@
         <v>929</v>
       </c>
       <c r="AO8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1599,10 +1624,10 @@
       <c r="X9" t="n">
         <v>299</v>
       </c>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y9" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
         <v>299</v>
       </c>
@@ -1624,10 +1649,10 @@
       <c r="AG9" t="n">
         <v>299</v>
       </c>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI9" t="inlineStr"/>
       <c r="AJ9" t="n">
         <v>299</v>
       </c>
@@ -1644,6 +1669,9 @@
         <v>299</v>
       </c>
       <c r="AO9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1692,10 +1720,10 @@
       <c r="N10" t="n">
         <v>299</v>
       </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="n">
-        <v>299</v>
-      </c>
+      <c r="O10" t="n">
+        <v>299</v>
+      </c>
+      <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
         <v>299</v>
       </c>
@@ -1720,14 +1748,14 @@
       <c r="X10" t="n">
         <v>299</v>
       </c>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="n">
         <v>299</v>
       </c>
@@ -1743,10 +1771,10 @@
       <c r="AG10" t="n">
         <v>299</v>
       </c>
-      <c r="AH10" t="inlineStr"/>
-      <c r="AI10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI10" t="inlineStr"/>
       <c r="AJ10" t="n">
         <v>299</v>
       </c>
@@ -1763,6 +1791,9 @@
         <v>299</v>
       </c>
       <c r="AO10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1844,10 +1875,10 @@
       <c r="Y11" t="n">
         <v>2997</v>
       </c>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="n">
+      <c r="Z11" t="n">
         <v>2997</v>
       </c>
+      <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="n">
         <v>2997</v>
       </c>
@@ -1861,15 +1892,15 @@
         <v>2997</v>
       </c>
       <c r="AF11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AG11" t="n">
         <v>929</v>
       </c>
-      <c r="AH11" t="inlineStr"/>
-      <c r="AI11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI11" t="inlineStr"/>
       <c r="AJ11" t="n">
         <v>929</v>
       </c>
@@ -1886,6 +1917,9 @@
         <v>929</v>
       </c>
       <c r="AO11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1970,10 +2004,10 @@
       <c r="Z12" t="n">
         <v>569</v>
       </c>
-      <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="n">
         <v>569</v>
       </c>
@@ -1989,10 +2023,10 @@
       <c r="AG12" t="n">
         <v>569</v>
       </c>
-      <c r="AH12" t="inlineStr"/>
-      <c r="AI12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI12" t="inlineStr"/>
       <c r="AJ12" t="n">
         <v>569</v>
       </c>
@@ -2009,6 +2043,9 @@
         <v>569</v>
       </c>
       <c r="AO12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2036,10 +2073,10 @@
       <c r="G13" t="n">
         <v>569</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>569</v>
-      </c>
+      <c r="H13" t="n">
+        <v>569</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
         <v>569</v>
       </c>
@@ -2085,14 +2122,14 @@
       <c r="X13" t="n">
         <v>569</v>
       </c>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="n">
         <v>569</v>
       </c>
@@ -2108,24 +2145,27 @@
       <c r="AG13" t="n">
         <v>569</v>
       </c>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI13" t="inlineStr"/>
       <c r="AJ13" t="n">
         <v>569</v>
       </c>
       <c r="AK13" t="n">
         <v>569</v>
       </c>
-      <c r="AL13" t="inlineStr"/>
-      <c r="AM13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM13" t="inlineStr"/>
       <c r="AN13" t="n">
         <v>569</v>
       </c>
       <c r="AO13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2174,10 +2214,10 @@
       <c r="N14" t="n">
         <v>794</v>
       </c>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="n">
+      <c r="O14" t="n">
         <v>794</v>
       </c>
+      <c r="P14" t="inlineStr"/>
       <c r="Q14" t="n">
         <v>794</v>
       </c>
@@ -2185,7 +2225,7 @@
         <v>794</v>
       </c>
       <c r="S14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="T14" t="n">
         <v>499</v>
@@ -2202,11 +2242,11 @@
       <c r="X14" t="n">
         <v>499</v>
       </c>
-      <c r="Y14" t="inlineStr"/>
+      <c r="Y14" t="n">
+        <v>499</v>
+      </c>
       <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="n">
         <v>499</v>
       </c>
@@ -2247,6 +2287,9 @@
         <v>499</v>
       </c>
       <c r="AO14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2331,10 +2374,10 @@
       <c r="Z15" t="n">
         <v>499</v>
       </c>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="n">
         <v>499</v>
       </c>
@@ -2344,14 +2387,14 @@
       <c r="AE15" t="n">
         <v>499</v>
       </c>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AH15" t="inlineStr"/>
-      <c r="AI15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI15" t="inlineStr"/>
       <c r="AJ15" t="n">
         <v>499</v>
       </c>
@@ -2368,6 +2411,9 @@
         <v>499</v>
       </c>
       <c r="AO15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2437,17 +2483,17 @@
       <c r="U16" t="n">
         <v>299</v>
       </c>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="n">
-        <v>299</v>
-      </c>
+      <c r="V16" t="n">
+        <v>299</v>
+      </c>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="n">
         <v>299</v>
       </c>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
         <v>299</v>
       </c>
@@ -2469,10 +2515,10 @@
       <c r="AG16" t="n">
         <v>299</v>
       </c>
-      <c r="AH16" t="inlineStr"/>
-      <c r="AI16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI16" t="inlineStr"/>
       <c r="AJ16" t="n">
         <v>299</v>
       </c>
@@ -2489,6 +2535,9 @@
         <v>299</v>
       </c>
       <c r="AO16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2573,10 +2622,10 @@
       <c r="Z17" t="n">
         <v>929</v>
       </c>
-      <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="n">
         <v>929</v>
       </c>
@@ -2592,10 +2641,10 @@
       <c r="AG17" t="n">
         <v>929</v>
       </c>
-      <c r="AH17" t="inlineStr"/>
-      <c r="AI17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI17" t="inlineStr"/>
       <c r="AJ17" t="n">
         <v>929</v>
       </c>
@@ -2612,6 +2661,9 @@
         <v>929</v>
       </c>
       <c r="AO17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2693,11 +2745,11 @@
       <c r="Y18" t="n">
         <v>499</v>
       </c>
-      <c r="Z18" t="inlineStr"/>
+      <c r="Z18" t="n">
+        <v>499</v>
+      </c>
       <c r="AA18" t="inlineStr"/>
-      <c r="AB18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="n">
         <v>499</v>
       </c>
@@ -2713,10 +2765,10 @@
       <c r="AG18" t="n">
         <v>499</v>
       </c>
-      <c r="AH18" t="inlineStr"/>
-      <c r="AI18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AH18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI18" t="inlineStr"/>
       <c r="AJ18" t="n">
         <v>499</v>
       </c>
@@ -2733,6 +2785,9 @@
         <v>499</v>
       </c>
       <c r="AO18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2806,7 +2861,7 @@
         <v>1299</v>
       </c>
       <c r="W19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="X19" t="n">
         <v>1497</v>
@@ -2814,13 +2869,13 @@
       <c r="Y19" t="n">
         <v>1497</v>
       </c>
-      <c r="Z19" t="inlineStr"/>
+      <c r="Z19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AA19" t="inlineStr"/>
-      <c r="AB19" t="n">
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="n">
         <v>465</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>1497</v>
       </c>
       <c r="AD19" t="n">
         <v>1497</v>
@@ -2856,6 +2911,9 @@
         <v>1497</v>
       </c>
       <c r="AO19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AP19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -2961,10 +3019,10 @@
       <c r="AG20" t="n">
         <v>929</v>
       </c>
-      <c r="AH20" t="inlineStr"/>
-      <c r="AI20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI20" t="inlineStr"/>
       <c r="AJ20" t="n">
         <v>929</v>
       </c>
@@ -2981,6 +3039,9 @@
         <v>929</v>
       </c>
       <c r="AO20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3035,10 +3096,10 @@
       <c r="P21" t="n">
         <v>499</v>
       </c>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="n">
-        <v>499</v>
-      </c>
+      <c r="Q21" t="n">
+        <v>499</v>
+      </c>
+      <c r="R21" t="inlineStr"/>
       <c r="S21" t="n">
         <v>499</v>
       </c>
@@ -3063,10 +3124,10 @@
       <c r="Z21" t="n">
         <v>499</v>
       </c>
-      <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="n">
         <v>499</v>
       </c>
@@ -3104,6 +3165,9 @@
         <v>499</v>
       </c>
       <c r="AO21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3182,14 +3246,14 @@
       <c r="X22" t="n">
         <v>299</v>
       </c>
-      <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y22" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="n">
         <v>299</v>
       </c>
@@ -3205,10 +3269,10 @@
       <c r="AG22" t="n">
         <v>299</v>
       </c>
-      <c r="AH22" t="inlineStr"/>
-      <c r="AI22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI22" t="inlineStr"/>
       <c r="AJ22" t="n">
         <v>299</v>
       </c>
@@ -3225,6 +3289,9 @@
         <v>299</v>
       </c>
       <c r="AO22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3306,11 +3373,11 @@
       <c r="Y23" t="n">
         <v>1299</v>
       </c>
-      <c r="Z23" t="inlineStr"/>
+      <c r="Z23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="n">
         <v>1299</v>
       </c>
@@ -3326,10 +3393,10 @@
       <c r="AG23" t="n">
         <v>1299</v>
       </c>
-      <c r="AH23" t="inlineStr"/>
-      <c r="AI23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AH23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AI23" t="inlineStr"/>
       <c r="AJ23" t="n">
         <v>1299</v>
       </c>
@@ -3346,6 +3413,9 @@
         <v>1299</v>
       </c>
       <c r="AO23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AP23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3424,11 +3494,11 @@
       <c r="X24" t="n">
         <v>929</v>
       </c>
-      <c r="Y24" t="inlineStr"/>
+      <c r="Y24" t="n">
+        <v>929</v>
+      </c>
       <c r="Z24" t="inlineStr"/>
-      <c r="AA24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="n">
         <v>929</v>
       </c>
@@ -3447,10 +3517,10 @@
       <c r="AG24" t="n">
         <v>929</v>
       </c>
-      <c r="AH24" t="inlineStr"/>
-      <c r="AI24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI24" t="inlineStr"/>
       <c r="AJ24" t="n">
         <v>929</v>
       </c>
@@ -3467,6 +3537,9 @@
         <v>929</v>
       </c>
       <c r="AO24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3545,11 +3618,11 @@
       <c r="X25" t="n">
         <v>929</v>
       </c>
-      <c r="Y25" t="inlineStr"/>
+      <c r="Y25" t="n">
+        <v>929</v>
+      </c>
       <c r="Z25" t="inlineStr"/>
-      <c r="AA25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="n">
         <v>929</v>
       </c>
@@ -3568,10 +3641,10 @@
       <c r="AG25" t="n">
         <v>929</v>
       </c>
-      <c r="AH25" t="inlineStr"/>
-      <c r="AI25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI25" t="inlineStr"/>
       <c r="AJ25" t="n">
         <v>929</v>
       </c>
@@ -3588,6 +3661,9 @@
         <v>929</v>
       </c>
       <c r="AO25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3666,14 +3742,14 @@
       <c r="X26" t="n">
         <v>1299</v>
       </c>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AA26" t="inlineStr"/>
-      <c r="AB26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Y26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
         <v>1299</v>
       </c>
@@ -3689,10 +3765,10 @@
       <c r="AG26" t="n">
         <v>1299</v>
       </c>
-      <c r="AH26" t="inlineStr"/>
-      <c r="AI26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AH26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AI26" t="inlineStr"/>
       <c r="AJ26" t="n">
         <v>1299</v>
       </c>
@@ -3709,6 +3785,9 @@
         <v>1299</v>
       </c>
       <c r="AO26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AP26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 03:57
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP26"/>
+  <dimension ref="A1:AQ26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,7 @@
     <col width="21" customWidth="1" min="40" max="40"/>
     <col width="21" customWidth="1" min="41" max="41"/>
     <col width="21" customWidth="1" min="42" max="42"/>
+    <col width="21" customWidth="1" min="43" max="43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -485,205 +486,210 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 09:22</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -752,10 +758,10 @@
       <c r="T2" t="n">
         <v>929</v>
       </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="n">
-        <v>929</v>
-      </c>
+      <c r="U2" t="n">
+        <v>929</v>
+      </c>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="n">
         <v>929</v>
       </c>
@@ -768,25 +774,25 @@
       <c r="Z2" t="n">
         <v>929</v>
       </c>
-      <c r="AA2" t="inlineStr"/>
+      <c r="AA2" t="n">
+        <v>929</v>
+      </c>
       <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="n">
         <v>929</v>
       </c>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
         <v>929</v>
       </c>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="n">
         <v>929</v>
       </c>
@@ -806,6 +812,9 @@
         <v>929</v>
       </c>
       <c r="AP2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -821,10 +830,10 @@
       <c r="C3" t="n">
         <v>569</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>569</v>
-      </c>
+      <c r="D3" t="n">
+        <v>569</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>569</v>
       </c>
@@ -867,26 +876,26 @@
       <c r="S3" t="n">
         <v>569</v>
       </c>
-      <c r="T3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>569</v>
+      </c>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
-      <c r="W3" t="n">
-        <v>569</v>
-      </c>
+      <c r="W3" t="inlineStr"/>
       <c r="X3" t="n">
         <v>569</v>
       </c>
       <c r="Y3" t="n">
         <v>569</v>
       </c>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="n">
         <v>569</v>
       </c>
@@ -902,10 +911,10 @@
       <c r="AH3" t="n">
         <v>569</v>
       </c>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="n">
         <v>569</v>
       </c>
@@ -922,6 +931,9 @@
         <v>569</v>
       </c>
       <c r="AP3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1003,10 +1015,10 @@
       <c r="Y4" t="n">
         <v>299</v>
       </c>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="n">
         <v>299</v>
       </c>
@@ -1028,10 +1040,10 @@
       <c r="AH4" t="n">
         <v>299</v>
       </c>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="n">
         <v>299</v>
       </c>
@@ -1048,6 +1060,9 @@
         <v>299</v>
       </c>
       <c r="AP4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1057,10 +1072,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
-        <v>569</v>
-      </c>
+      <c r="B5" t="n">
+        <v>569</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
         <v>569</v>
       </c>
@@ -1154,10 +1169,10 @@
       <c r="AH5" t="n">
         <v>569</v>
       </c>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="n">
         <v>569</v>
       </c>
@@ -1174,6 +1189,9 @@
         <v>569</v>
       </c>
       <c r="AP5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1258,10 +1276,10 @@
       <c r="Z6" t="n">
         <v>499</v>
       </c>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="n">
         <v>499</v>
       </c>
@@ -1280,10 +1298,10 @@
       <c r="AH6" t="n">
         <v>499</v>
       </c>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AI6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="n">
         <v>499</v>
       </c>
@@ -1300,6 +1318,9 @@
         <v>499</v>
       </c>
       <c r="AP6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1381,12 +1402,12 @@
       <c r="Y7" t="n">
         <v>569</v>
       </c>
-      <c r="Z7" t="inlineStr"/>
+      <c r="Z7" t="n">
+        <v>569</v>
+      </c>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="n">
         <v>569</v>
       </c>
@@ -1402,10 +1423,10 @@
       <c r="AH7" t="n">
         <v>569</v>
       </c>
-      <c r="AI7" t="inlineStr"/>
-      <c r="AJ7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="n">
         <v>569</v>
       </c>
@@ -1422,6 +1443,9 @@
         <v>569</v>
       </c>
       <c r="AP7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1503,14 +1527,14 @@
       <c r="Y8" t="n">
         <v>929</v>
       </c>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC8" t="inlineStr"/>
       <c r="AD8" t="n">
         <v>929</v>
       </c>
@@ -1526,10 +1550,10 @@
       <c r="AH8" t="n">
         <v>929</v>
       </c>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="n">
         <v>929</v>
       </c>
@@ -1546,6 +1570,9 @@
         <v>929</v>
       </c>
       <c r="AP8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1627,10 +1654,10 @@
       <c r="Y9" t="n">
         <v>299</v>
       </c>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="n">
         <v>299</v>
       </c>
@@ -1652,10 +1679,10 @@
       <c r="AH9" t="n">
         <v>299</v>
       </c>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="n">
         <v>299</v>
       </c>
@@ -1672,6 +1699,9 @@
         <v>299</v>
       </c>
       <c r="AP9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1723,10 +1753,10 @@
       <c r="O10" t="n">
         <v>299</v>
       </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="n">
-        <v>299</v>
-      </c>
+      <c r="P10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
         <v>299</v>
       </c>
@@ -1751,14 +1781,14 @@
       <c r="Y10" t="n">
         <v>299</v>
       </c>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="n">
         <v>299</v>
       </c>
@@ -1774,10 +1804,10 @@
       <c r="AH10" t="n">
         <v>299</v>
       </c>
-      <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ10" t="inlineStr"/>
       <c r="AK10" t="n">
         <v>299</v>
       </c>
@@ -1794,6 +1824,9 @@
         <v>299</v>
       </c>
       <c r="AP10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1878,10 +1911,10 @@
       <c r="Z11" t="n">
         <v>2997</v>
       </c>
-      <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="n">
+      <c r="AA11" t="n">
         <v>2997</v>
       </c>
+      <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="n">
         <v>2997</v>
       </c>
@@ -1895,15 +1928,15 @@
         <v>2997</v>
       </c>
       <c r="AG11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AH11" t="n">
         <v>929</v>
       </c>
-      <c r="AI11" t="inlineStr"/>
-      <c r="AJ11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ11" t="inlineStr"/>
       <c r="AK11" t="n">
         <v>929</v>
       </c>
@@ -1920,6 +1953,9 @@
         <v>929</v>
       </c>
       <c r="AP11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2007,10 +2043,10 @@
       <c r="AA12" t="n">
         <v>569</v>
       </c>
-      <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC12" t="inlineStr"/>
       <c r="AD12" t="n">
         <v>569</v>
       </c>
@@ -2026,10 +2062,10 @@
       <c r="AH12" t="n">
         <v>569</v>
       </c>
-      <c r="AI12" t="inlineStr"/>
-      <c r="AJ12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ12" t="inlineStr"/>
       <c r="AK12" t="n">
         <v>569</v>
       </c>
@@ -2046,6 +2082,9 @@
         <v>569</v>
       </c>
       <c r="AP12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2076,10 +2115,10 @@
       <c r="H13" t="n">
         <v>569</v>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
-        <v>569</v>
-      </c>
+      <c r="I13" t="n">
+        <v>569</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>569</v>
       </c>
@@ -2125,14 +2164,14 @@
       <c r="Y13" t="n">
         <v>569</v>
       </c>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="n">
         <v>569</v>
       </c>
@@ -2148,24 +2187,27 @@
       <c r="AH13" t="n">
         <v>569</v>
       </c>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="n">
         <v>569</v>
       </c>
       <c r="AL13" t="n">
         <v>569</v>
       </c>
-      <c r="AM13" t="inlineStr"/>
-      <c r="AN13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN13" t="inlineStr"/>
       <c r="AO13" t="n">
         <v>569</v>
       </c>
       <c r="AP13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2217,10 +2259,10 @@
       <c r="O14" t="n">
         <v>794</v>
       </c>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="n">
+      <c r="P14" t="n">
         <v>794</v>
       </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
         <v>794</v>
       </c>
@@ -2228,7 +2270,7 @@
         <v>794</v>
       </c>
       <c r="T14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="U14" t="n">
         <v>499</v>
@@ -2245,11 +2287,11 @@
       <c r="Y14" t="n">
         <v>499</v>
       </c>
-      <c r="Z14" t="inlineStr"/>
+      <c r="Z14" t="n">
+        <v>499</v>
+      </c>
       <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="n">
         <v>499</v>
       </c>
@@ -2290,6 +2332,9 @@
         <v>499</v>
       </c>
       <c r="AP14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2377,10 +2422,10 @@
       <c r="AA15" t="n">
         <v>499</v>
       </c>
-      <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="n">
         <v>499</v>
       </c>
@@ -2390,14 +2435,14 @@
       <c r="AF15" t="n">
         <v>499</v>
       </c>
-      <c r="AG15" t="inlineStr"/>
-      <c r="AH15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AI15" t="inlineStr"/>
-      <c r="AJ15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ15" t="inlineStr"/>
       <c r="AK15" t="n">
         <v>499</v>
       </c>
@@ -2414,6 +2459,9 @@
         <v>499</v>
       </c>
       <c r="AP15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2486,17 +2534,17 @@
       <c r="V16" t="n">
         <v>299</v>
       </c>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="n">
-        <v>299</v>
-      </c>
+      <c r="W16" t="n">
+        <v>299</v>
+      </c>
+      <c r="X16" t="inlineStr"/>
       <c r="Y16" t="n">
         <v>299</v>
       </c>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="n">
         <v>299</v>
       </c>
@@ -2518,10 +2566,10 @@
       <c r="AH16" t="n">
         <v>299</v>
       </c>
-      <c r="AI16" t="inlineStr"/>
-      <c r="AJ16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ16" t="inlineStr"/>
       <c r="AK16" t="n">
         <v>299</v>
       </c>
@@ -2538,6 +2586,9 @@
         <v>299</v>
       </c>
       <c r="AP16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2625,10 +2676,10 @@
       <c r="AA17" t="n">
         <v>929</v>
       </c>
-      <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC17" t="inlineStr"/>
       <c r="AD17" t="n">
         <v>929</v>
       </c>
@@ -2644,10 +2695,10 @@
       <c r="AH17" t="n">
         <v>929</v>
       </c>
-      <c r="AI17" t="inlineStr"/>
-      <c r="AJ17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ17" t="inlineStr"/>
       <c r="AK17" t="n">
         <v>929</v>
       </c>
@@ -2664,6 +2715,9 @@
         <v>929</v>
       </c>
       <c r="AP17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2748,11 +2802,11 @@
       <c r="Z18" t="n">
         <v>499</v>
       </c>
-      <c r="AA18" t="inlineStr"/>
+      <c r="AA18" t="n">
+        <v>499</v>
+      </c>
       <c r="AB18" t="inlineStr"/>
-      <c r="AC18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC18" t="inlineStr"/>
       <c r="AD18" t="n">
         <v>499</v>
       </c>
@@ -2768,10 +2822,10 @@
       <c r="AH18" t="n">
         <v>499</v>
       </c>
-      <c r="AI18" t="inlineStr"/>
-      <c r="AJ18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AI18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ18" t="inlineStr"/>
       <c r="AK18" t="n">
         <v>499</v>
       </c>
@@ -2788,6 +2842,9 @@
         <v>499</v>
       </c>
       <c r="AP18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2864,7 +2921,7 @@
         <v>1299</v>
       </c>
       <c r="X19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="Y19" t="n">
         <v>1497</v>
@@ -2872,13 +2929,13 @@
       <c r="Z19" t="n">
         <v>1497</v>
       </c>
-      <c r="AA19" t="inlineStr"/>
+      <c r="AA19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AB19" t="inlineStr"/>
-      <c r="AC19" t="n">
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="n">
         <v>465</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>1497</v>
       </c>
       <c r="AE19" t="n">
         <v>1497</v>
@@ -2914,6 +2971,9 @@
         <v>1497</v>
       </c>
       <c r="AP19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AQ19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3022,10 +3082,10 @@
       <c r="AH20" t="n">
         <v>929</v>
       </c>
-      <c r="AI20" t="inlineStr"/>
-      <c r="AJ20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ20" t="inlineStr"/>
       <c r="AK20" t="n">
         <v>929</v>
       </c>
@@ -3042,6 +3102,9 @@
         <v>929</v>
       </c>
       <c r="AP20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3099,10 +3162,10 @@
       <c r="Q21" t="n">
         <v>499</v>
       </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="n">
-        <v>499</v>
-      </c>
+      <c r="R21" t="n">
+        <v>499</v>
+      </c>
+      <c r="S21" t="inlineStr"/>
       <c r="T21" t="n">
         <v>499</v>
       </c>
@@ -3127,10 +3190,10 @@
       <c r="AA21" t="n">
         <v>499</v>
       </c>
-      <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="n">
         <v>499</v>
       </c>
@@ -3168,6 +3231,9 @@
         <v>499</v>
       </c>
       <c r="AP21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3249,14 +3315,14 @@
       <c r="Y22" t="n">
         <v>299</v>
       </c>
-      <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC22" t="inlineStr"/>
       <c r="AD22" t="n">
         <v>299</v>
       </c>
@@ -3272,10 +3338,10 @@
       <c r="AH22" t="n">
         <v>299</v>
       </c>
-      <c r="AI22" t="inlineStr"/>
-      <c r="AJ22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ22" t="inlineStr"/>
       <c r="AK22" t="n">
         <v>299</v>
       </c>
@@ -3292,6 +3358,9 @@
         <v>299</v>
       </c>
       <c r="AP22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3376,11 +3445,11 @@
       <c r="Z23" t="n">
         <v>1299</v>
       </c>
-      <c r="AA23" t="inlineStr"/>
+      <c r="AA23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AB23" t="inlineStr"/>
-      <c r="AC23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="n">
         <v>1299</v>
       </c>
@@ -3396,10 +3465,10 @@
       <c r="AH23" t="n">
         <v>1299</v>
       </c>
-      <c r="AI23" t="inlineStr"/>
-      <c r="AJ23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AI23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AJ23" t="inlineStr"/>
       <c r="AK23" t="n">
         <v>1299</v>
       </c>
@@ -3416,6 +3485,9 @@
         <v>1299</v>
       </c>
       <c r="AP23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AQ23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3497,11 +3569,11 @@
       <c r="Y24" t="n">
         <v>929</v>
       </c>
-      <c r="Z24" t="inlineStr"/>
+      <c r="Z24" t="n">
+        <v>929</v>
+      </c>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="n">
         <v>929</v>
       </c>
@@ -3520,10 +3592,10 @@
       <c r="AH24" t="n">
         <v>929</v>
       </c>
-      <c r="AI24" t="inlineStr"/>
-      <c r="AJ24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ24" t="inlineStr"/>
       <c r="AK24" t="n">
         <v>929</v>
       </c>
@@ -3540,6 +3612,9 @@
         <v>929</v>
       </c>
       <c r="AP24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3549,9 +3624,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>929</v>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
         <v>929</v>
       </c>
@@ -3621,11 +3694,11 @@
       <c r="Y25" t="n">
         <v>929</v>
       </c>
-      <c r="Z25" t="inlineStr"/>
+      <c r="Z25" t="n">
+        <v>929</v>
+      </c>
       <c r="AA25" t="inlineStr"/>
-      <c r="AB25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="n">
         <v>929</v>
       </c>
@@ -3644,10 +3717,10 @@
       <c r="AH25" t="n">
         <v>929</v>
       </c>
-      <c r="AI25" t="inlineStr"/>
-      <c r="AJ25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ25" t="inlineStr"/>
       <c r="AK25" t="n">
         <v>929</v>
       </c>
@@ -3664,6 +3737,9 @@
         <v>929</v>
       </c>
       <c r="AP25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3745,14 +3821,14 @@
       <c r="Y26" t="n">
         <v>1299</v>
       </c>
-      <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="Z26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AC26" t="inlineStr"/>
       <c r="AD26" t="n">
         <v>1299</v>
       </c>
@@ -3768,10 +3844,10 @@
       <c r="AH26" t="n">
         <v>1299</v>
       </c>
-      <c r="AI26" t="inlineStr"/>
-      <c r="AJ26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AI26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AJ26" t="inlineStr"/>
       <c r="AK26" t="n">
         <v>1299</v>
       </c>
@@ -3788,6 +3864,9 @@
         <v>1299</v>
       </c>
       <c r="AP26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AQ26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 05:04
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ26"/>
+  <dimension ref="A1:AR26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,7 @@
     <col width="21" customWidth="1" min="41" max="41"/>
     <col width="21" customWidth="1" min="42" max="42"/>
     <col width="21" customWidth="1" min="43" max="43"/>
+    <col width="21" customWidth="1" min="44" max="44"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -486,210 +487,215 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 10:30</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -761,10 +767,10 @@
       <c r="U2" t="n">
         <v>929</v>
       </c>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="n">
-        <v>929</v>
-      </c>
+      <c r="V2" t="n">
+        <v>929</v>
+      </c>
+      <c r="W2" t="inlineStr"/>
       <c r="X2" t="n">
         <v>929</v>
       </c>
@@ -777,25 +783,25 @@
       <c r="AA2" t="n">
         <v>929</v>
       </c>
-      <c r="AB2" t="inlineStr"/>
+      <c r="AB2" t="n">
+        <v>929</v>
+      </c>
       <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="n">
         <v>929</v>
       </c>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="n">
         <v>929</v>
       </c>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="n">
         <v>929</v>
       </c>
@@ -815,6 +821,9 @@
         <v>929</v>
       </c>
       <c r="AQ2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -833,10 +842,10 @@
       <c r="D3" t="n">
         <v>569</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>569</v>
-      </c>
+      <c r="E3" t="n">
+        <v>569</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>569</v>
       </c>
@@ -879,26 +888,26 @@
       <c r="T3" t="n">
         <v>569</v>
       </c>
-      <c r="U3" t="inlineStr"/>
+      <c r="U3" t="n">
+        <v>569</v>
+      </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
-      <c r="X3" t="n">
-        <v>569</v>
-      </c>
+      <c r="X3" t="inlineStr"/>
       <c r="Y3" t="n">
         <v>569</v>
       </c>
       <c r="Z3" t="n">
         <v>569</v>
       </c>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="n">
         <v>569</v>
       </c>
@@ -914,10 +923,10 @@
       <c r="AI3" t="n">
         <v>569</v>
       </c>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="n">
         <v>569</v>
       </c>
@@ -934,6 +943,9 @@
         <v>569</v>
       </c>
       <c r="AQ3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1018,10 +1030,10 @@
       <c r="Z4" t="n">
         <v>299</v>
       </c>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="n">
         <v>299</v>
       </c>
@@ -1043,10 +1055,10 @@
       <c r="AI4" t="n">
         <v>299</v>
       </c>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="n">
         <v>299</v>
       </c>
@@ -1063,6 +1075,9 @@
         <v>299</v>
       </c>
       <c r="AQ4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1075,10 +1090,10 @@
       <c r="B5" t="n">
         <v>569</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="n">
-        <v>569</v>
-      </c>
+      <c r="C5" t="n">
+        <v>569</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>569</v>
       </c>
@@ -1172,10 +1187,10 @@
       <c r="AI5" t="n">
         <v>569</v>
       </c>
-      <c r="AJ5" t="inlineStr"/>
-      <c r="AK5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="n">
         <v>569</v>
       </c>
@@ -1192,6 +1207,9 @@
         <v>569</v>
       </c>
       <c r="AQ5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1279,10 +1297,10 @@
       <c r="AA6" t="n">
         <v>499</v>
       </c>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC6" t="inlineStr"/>
       <c r="AD6" t="n">
         <v>499</v>
       </c>
@@ -1301,10 +1319,10 @@
       <c r="AI6" t="n">
         <v>499</v>
       </c>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AJ6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="n">
         <v>499</v>
       </c>
@@ -1321,6 +1339,9 @@
         <v>499</v>
       </c>
       <c r="AQ6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1405,12 +1426,12 @@
       <c r="Z7" t="n">
         <v>569</v>
       </c>
-      <c r="AA7" t="inlineStr"/>
+      <c r="AA7" t="n">
+        <v>569</v>
+      </c>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="n">
         <v>569</v>
       </c>
@@ -1426,10 +1447,10 @@
       <c r="AI7" t="n">
         <v>569</v>
       </c>
-      <c r="AJ7" t="inlineStr"/>
-      <c r="AK7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="n">
         <v>569</v>
       </c>
@@ -1446,6 +1467,9 @@
         <v>569</v>
       </c>
       <c r="AQ7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1530,14 +1554,14 @@
       <c r="Z8" t="n">
         <v>929</v>
       </c>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD8" t="inlineStr"/>
       <c r="AE8" t="n">
         <v>929</v>
       </c>
@@ -1553,10 +1577,10 @@
       <c r="AI8" t="n">
         <v>929</v>
       </c>
-      <c r="AJ8" t="inlineStr"/>
-      <c r="AK8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="n">
         <v>929</v>
       </c>
@@ -1573,6 +1597,9 @@
         <v>929</v>
       </c>
       <c r="AQ8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1657,10 +1684,10 @@
       <c r="Z9" t="n">
         <v>299</v>
       </c>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="n">
         <v>299</v>
       </c>
@@ -1682,10 +1709,10 @@
       <c r="AI9" t="n">
         <v>299</v>
       </c>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="n">
         <v>299</v>
       </c>
@@ -1702,6 +1729,9 @@
         <v>299</v>
       </c>
       <c r="AQ9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1756,10 +1786,10 @@
       <c r="P10" t="n">
         <v>299</v>
       </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Q10" t="n">
+        <v>299</v>
+      </c>
+      <c r="R10" t="inlineStr"/>
       <c r="S10" t="n">
         <v>299</v>
       </c>
@@ -1784,14 +1814,14 @@
       <c r="Z10" t="n">
         <v>299</v>
       </c>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="n">
         <v>299</v>
       </c>
@@ -1807,10 +1837,10 @@
       <c r="AI10" t="n">
         <v>299</v>
       </c>
-      <c r="AJ10" t="inlineStr"/>
-      <c r="AK10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="n">
         <v>299</v>
       </c>
@@ -1827,6 +1857,9 @@
         <v>299</v>
       </c>
       <c r="AQ10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1914,10 +1947,10 @@
       <c r="AA11" t="n">
         <v>2997</v>
       </c>
-      <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="n">
+      <c r="AB11" t="n">
         <v>2997</v>
       </c>
+      <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="n">
         <v>2997</v>
       </c>
@@ -1931,15 +1964,15 @@
         <v>2997</v>
       </c>
       <c r="AH11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AI11" t="n">
         <v>929</v>
       </c>
-      <c r="AJ11" t="inlineStr"/>
-      <c r="AK11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="n">
         <v>929</v>
       </c>
@@ -1956,6 +1989,9 @@
         <v>929</v>
       </c>
       <c r="AQ11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2046,10 +2082,10 @@
       <c r="AB12" t="n">
         <v>569</v>
       </c>
-      <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD12" t="inlineStr"/>
       <c r="AE12" t="n">
         <v>569</v>
       </c>
@@ -2065,10 +2101,10 @@
       <c r="AI12" t="n">
         <v>569</v>
       </c>
-      <c r="AJ12" t="inlineStr"/>
-      <c r="AK12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="n">
         <v>569</v>
       </c>
@@ -2085,6 +2121,9 @@
         <v>569</v>
       </c>
       <c r="AQ12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2118,10 +2157,10 @@
       <c r="I13" t="n">
         <v>569</v>
       </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>569</v>
-      </c>
+      <c r="J13" t="n">
+        <v>569</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
         <v>569</v>
       </c>
@@ -2167,14 +2206,14 @@
       <c r="Z13" t="n">
         <v>569</v>
       </c>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="n">
         <v>569</v>
       </c>
@@ -2190,24 +2229,27 @@
       <c r="AI13" t="n">
         <v>569</v>
       </c>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="n">
         <v>569</v>
       </c>
       <c r="AM13" t="n">
         <v>569</v>
       </c>
-      <c r="AN13" t="inlineStr"/>
-      <c r="AO13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO13" t="inlineStr"/>
       <c r="AP13" t="n">
         <v>569</v>
       </c>
       <c r="AQ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2262,10 +2304,10 @@
       <c r="P14" t="n">
         <v>794</v>
       </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="n">
+      <c r="Q14" t="n">
         <v>794</v>
       </c>
+      <c r="R14" t="inlineStr"/>
       <c r="S14" t="n">
         <v>794</v>
       </c>
@@ -2273,7 +2315,7 @@
         <v>794</v>
       </c>
       <c r="U14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="V14" t="n">
         <v>499</v>
@@ -2290,11 +2332,11 @@
       <c r="Z14" t="n">
         <v>499</v>
       </c>
-      <c r="AA14" t="inlineStr"/>
+      <c r="AA14" t="n">
+        <v>499</v>
+      </c>
       <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="n">
         <v>499</v>
       </c>
@@ -2335,6 +2377,9 @@
         <v>499</v>
       </c>
       <c r="AQ14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2425,10 +2470,10 @@
       <c r="AB15" t="n">
         <v>499</v>
       </c>
-      <c r="AC15" t="inlineStr"/>
-      <c r="AD15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="n">
         <v>499</v>
       </c>
@@ -2438,14 +2483,14 @@
       <c r="AG15" t="n">
         <v>499</v>
       </c>
-      <c r="AH15" t="inlineStr"/>
-      <c r="AI15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AJ15" t="inlineStr"/>
-      <c r="AK15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AH15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="n">
         <v>499</v>
       </c>
@@ -2462,6 +2507,9 @@
         <v>499</v>
       </c>
       <c r="AQ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2537,17 +2585,17 @@
       <c r="W16" t="n">
         <v>299</v>
       </c>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="n">
-        <v>299</v>
-      </c>
+      <c r="X16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="n">
         <v>299</v>
       </c>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="n">
         <v>299</v>
       </c>
@@ -2569,10 +2617,10 @@
       <c r="AI16" t="n">
         <v>299</v>
       </c>
-      <c r="AJ16" t="inlineStr"/>
-      <c r="AK16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="n">
         <v>299</v>
       </c>
@@ -2589,6 +2637,9 @@
         <v>299</v>
       </c>
       <c r="AQ16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2679,10 +2730,10 @@
       <c r="AB17" t="n">
         <v>929</v>
       </c>
-      <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="n">
         <v>929</v>
       </c>
@@ -2698,10 +2749,10 @@
       <c r="AI17" t="n">
         <v>929</v>
       </c>
-      <c r="AJ17" t="inlineStr"/>
-      <c r="AK17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="n">
         <v>929</v>
       </c>
@@ -2718,6 +2769,9 @@
         <v>929</v>
       </c>
       <c r="AQ17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2805,11 +2859,11 @@
       <c r="AA18" t="n">
         <v>499</v>
       </c>
-      <c r="AB18" t="inlineStr"/>
+      <c r="AB18" t="n">
+        <v>499</v>
+      </c>
       <c r="AC18" t="inlineStr"/>
-      <c r="AD18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD18" t="inlineStr"/>
       <c r="AE18" t="n">
         <v>499</v>
       </c>
@@ -2825,10 +2879,10 @@
       <c r="AI18" t="n">
         <v>499</v>
       </c>
-      <c r="AJ18" t="inlineStr"/>
-      <c r="AK18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AJ18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="n">
         <v>499</v>
       </c>
@@ -2845,6 +2899,9 @@
         <v>499</v>
       </c>
       <c r="AQ18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2924,7 +2981,7 @@
         <v>1299</v>
       </c>
       <c r="Y19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="Z19" t="n">
         <v>1497</v>
@@ -2932,13 +2989,13 @@
       <c r="AA19" t="n">
         <v>1497</v>
       </c>
-      <c r="AB19" t="inlineStr"/>
+      <c r="AB19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AC19" t="inlineStr"/>
-      <c r="AD19" t="n">
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="n">
         <v>465</v>
-      </c>
-      <c r="AE19" t="n">
-        <v>1497</v>
       </c>
       <c r="AF19" t="n">
         <v>1497</v>
@@ -2974,6 +3031,9 @@
         <v>1497</v>
       </c>
       <c r="AQ19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AR19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3085,10 +3145,10 @@
       <c r="AI20" t="n">
         <v>929</v>
       </c>
-      <c r="AJ20" t="inlineStr"/>
-      <c r="AK20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK20" t="inlineStr"/>
       <c r="AL20" t="n">
         <v>929</v>
       </c>
@@ -3105,6 +3165,9 @@
         <v>929</v>
       </c>
       <c r="AQ20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3165,10 +3228,10 @@
       <c r="R21" t="n">
         <v>499</v>
       </c>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="n">
-        <v>499</v>
-      </c>
+      <c r="S21" t="n">
+        <v>499</v>
+      </c>
+      <c r="T21" t="inlineStr"/>
       <c r="U21" t="n">
         <v>499</v>
       </c>
@@ -3193,10 +3256,10 @@
       <c r="AB21" t="n">
         <v>499</v>
       </c>
-      <c r="AC21" t="inlineStr"/>
-      <c r="AD21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="n">
         <v>499</v>
       </c>
@@ -3234,6 +3297,9 @@
         <v>499</v>
       </c>
       <c r="AQ21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3318,14 +3384,14 @@
       <c r="Z22" t="n">
         <v>299</v>
       </c>
-      <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AC22" t="inlineStr"/>
-      <c r="AD22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB22" t="inlineStr"/>
+      <c r="AC22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD22" t="inlineStr"/>
       <c r="AE22" t="n">
         <v>299</v>
       </c>
@@ -3341,10 +3407,10 @@
       <c r="AI22" t="n">
         <v>299</v>
       </c>
-      <c r="AJ22" t="inlineStr"/>
-      <c r="AK22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="n">
         <v>299</v>
       </c>
@@ -3361,6 +3427,9 @@
         <v>299</v>
       </c>
       <c r="AQ22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3448,11 +3517,11 @@
       <c r="AA23" t="n">
         <v>1299</v>
       </c>
-      <c r="AB23" t="inlineStr"/>
+      <c r="AB23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AC23" t="inlineStr"/>
-      <c r="AD23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="n">
         <v>1299</v>
       </c>
@@ -3468,10 +3537,10 @@
       <c r="AI23" t="n">
         <v>1299</v>
       </c>
-      <c r="AJ23" t="inlineStr"/>
-      <c r="AK23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AJ23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AK23" t="inlineStr"/>
       <c r="AL23" t="n">
         <v>1299</v>
       </c>
@@ -3488,6 +3557,9 @@
         <v>1299</v>
       </c>
       <c r="AQ23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AR23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3572,11 +3644,11 @@
       <c r="Z24" t="n">
         <v>929</v>
       </c>
-      <c r="AA24" t="inlineStr"/>
+      <c r="AA24" t="n">
+        <v>929</v>
+      </c>
       <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="n">
         <v>929</v>
       </c>
@@ -3595,10 +3667,10 @@
       <c r="AI24" t="n">
         <v>929</v>
       </c>
-      <c r="AJ24" t="inlineStr"/>
-      <c r="AK24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK24" t="inlineStr"/>
       <c r="AL24" t="n">
         <v>929</v>
       </c>
@@ -3615,6 +3687,9 @@
         <v>929</v>
       </c>
       <c r="AQ24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3624,10 +3699,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="n">
-        <v>929</v>
-      </c>
+      <c r="B25" t="n">
+        <v>929</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
         <v>929</v>
       </c>
@@ -3697,11 +3772,11 @@
       <c r="Z25" t="n">
         <v>929</v>
       </c>
-      <c r="AA25" t="inlineStr"/>
+      <c r="AA25" t="n">
+        <v>929</v>
+      </c>
       <c r="AB25" t="inlineStr"/>
-      <c r="AC25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC25" t="inlineStr"/>
       <c r="AD25" t="n">
         <v>929</v>
       </c>
@@ -3720,10 +3795,10 @@
       <c r="AI25" t="n">
         <v>929</v>
       </c>
-      <c r="AJ25" t="inlineStr"/>
-      <c r="AK25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK25" t="inlineStr"/>
       <c r="AL25" t="n">
         <v>929</v>
       </c>
@@ -3740,6 +3815,9 @@
         <v>929</v>
       </c>
       <c r="AQ25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3749,9 +3827,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="n">
         <v>1299</v>
       </c>
@@ -3824,14 +3900,14 @@
       <c r="Z26" t="n">
         <v>1299</v>
       </c>
-      <c r="AA26" t="inlineStr"/>
-      <c r="AB26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AC26" t="inlineStr"/>
-      <c r="AD26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AA26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AB26" t="inlineStr"/>
+      <c r="AC26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AD26" t="inlineStr"/>
       <c r="AE26" t="n">
         <v>1299</v>
       </c>
@@ -3847,10 +3923,10 @@
       <c r="AI26" t="n">
         <v>1299</v>
       </c>
-      <c r="AJ26" t="inlineStr"/>
-      <c r="AK26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AJ26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AK26" t="inlineStr"/>
       <c r="AL26" t="n">
         <v>1299</v>
       </c>
@@ -3867,6 +3943,9 @@
         <v>1299</v>
       </c>
       <c r="AQ26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AR26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 07:05
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR26"/>
+  <dimension ref="A1:AS26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,7 @@
     <col width="21" customWidth="1" min="42" max="42"/>
     <col width="21" customWidth="1" min="43" max="43"/>
     <col width="21" customWidth="1" min="44" max="44"/>
+    <col width="21" customWidth="1" min="45" max="45"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -487,215 +488,220 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 12:31</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -770,10 +776,10 @@
       <c r="V2" t="n">
         <v>929</v>
       </c>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="n">
-        <v>929</v>
-      </c>
+      <c r="W2" t="n">
+        <v>929</v>
+      </c>
+      <c r="X2" t="inlineStr"/>
       <c r="Y2" t="n">
         <v>929</v>
       </c>
@@ -786,25 +792,25 @@
       <c r="AB2" t="n">
         <v>929</v>
       </c>
-      <c r="AC2" t="inlineStr"/>
+      <c r="AC2" t="n">
+        <v>929</v>
+      </c>
       <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="n">
         <v>929</v>
       </c>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="n">
         <v>929</v>
       </c>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="n">
         <v>929</v>
       </c>
@@ -824,6 +830,9 @@
         <v>929</v>
       </c>
       <c r="AR2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -845,10 +854,10 @@
       <c r="E3" t="n">
         <v>569</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>569</v>
-      </c>
+      <c r="F3" t="n">
+        <v>569</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>569</v>
       </c>
@@ -891,26 +900,26 @@
       <c r="U3" t="n">
         <v>569</v>
       </c>
-      <c r="V3" t="inlineStr"/>
+      <c r="V3" t="n">
+        <v>569</v>
+      </c>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="n">
         <v>569</v>
       </c>
       <c r="AA3" t="n">
         <v>569</v>
       </c>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="n">
         <v>569</v>
       </c>
@@ -926,10 +935,10 @@
       <c r="AJ3" t="n">
         <v>569</v>
       </c>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="n">
         <v>569</v>
       </c>
@@ -946,6 +955,9 @@
         <v>569</v>
       </c>
       <c r="AR3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1033,10 +1045,10 @@
       <c r="AA4" t="n">
         <v>299</v>
       </c>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="n">
         <v>299</v>
       </c>
@@ -1058,10 +1070,10 @@
       <c r="AJ4" t="n">
         <v>299</v>
       </c>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="n">
         <v>299</v>
       </c>
@@ -1078,6 +1090,9 @@
         <v>299</v>
       </c>
       <c r="AR4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1093,10 +1108,10 @@
       <c r="C5" t="n">
         <v>569</v>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="n">
-        <v>569</v>
-      </c>
+      <c r="D5" t="n">
+        <v>569</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>569</v>
       </c>
@@ -1190,10 +1205,10 @@
       <c r="AJ5" t="n">
         <v>569</v>
       </c>
-      <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL5" t="inlineStr"/>
       <c r="AM5" t="n">
         <v>569</v>
       </c>
@@ -1210,6 +1225,9 @@
         <v>569</v>
       </c>
       <c r="AR5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1300,10 +1318,10 @@
       <c r="AB6" t="n">
         <v>499</v>
       </c>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="n">
         <v>499</v>
       </c>
@@ -1322,10 +1340,10 @@
       <c r="AJ6" t="n">
         <v>499</v>
       </c>
-      <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AK6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL6" t="inlineStr"/>
       <c r="AM6" t="n">
         <v>499</v>
       </c>
@@ -1342,6 +1360,9 @@
         <v>499</v>
       </c>
       <c r="AR6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1429,12 +1450,12 @@
       <c r="AA7" t="n">
         <v>569</v>
       </c>
-      <c r="AB7" t="inlineStr"/>
+      <c r="AB7" t="n">
+        <v>569</v>
+      </c>
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr"/>
-      <c r="AE7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="n">
         <v>569</v>
       </c>
@@ -1450,10 +1471,10 @@
       <c r="AJ7" t="n">
         <v>569</v>
       </c>
-      <c r="AK7" t="inlineStr"/>
-      <c r="AL7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="n">
         <v>569</v>
       </c>
@@ -1470,6 +1491,9 @@
         <v>569</v>
       </c>
       <c r="AR7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1557,14 +1581,14 @@
       <c r="AA8" t="n">
         <v>929</v>
       </c>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="n">
         <v>929</v>
       </c>
@@ -1580,10 +1604,10 @@
       <c r="AJ8" t="n">
         <v>929</v>
       </c>
-      <c r="AK8" t="inlineStr"/>
-      <c r="AL8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="n">
         <v>929</v>
       </c>
@@ -1600,6 +1624,9 @@
         <v>929</v>
       </c>
       <c r="AR8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1687,10 +1714,10 @@
       <c r="AA9" t="n">
         <v>299</v>
       </c>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC9" t="inlineStr"/>
       <c r="AD9" t="n">
         <v>299</v>
       </c>
@@ -1712,10 +1739,10 @@
       <c r="AJ9" t="n">
         <v>299</v>
       </c>
-      <c r="AK9" t="inlineStr"/>
-      <c r="AL9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="n">
         <v>299</v>
       </c>
@@ -1732,6 +1759,9 @@
         <v>299</v>
       </c>
       <c r="AR9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1789,10 +1819,10 @@
       <c r="Q10" t="n">
         <v>299</v>
       </c>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="n">
-        <v>299</v>
-      </c>
+      <c r="R10" t="n">
+        <v>299</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="n">
         <v>299</v>
       </c>
@@ -1817,14 +1847,14 @@
       <c r="AA10" t="n">
         <v>299</v>
       </c>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="n">
         <v>299</v>
       </c>
@@ -1840,10 +1870,10 @@
       <c r="AJ10" t="n">
         <v>299</v>
       </c>
-      <c r="AK10" t="inlineStr"/>
-      <c r="AL10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL10" t="inlineStr"/>
       <c r="AM10" t="n">
         <v>299</v>
       </c>
@@ -1860,6 +1890,9 @@
         <v>299</v>
       </c>
       <c r="AR10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1950,10 +1983,10 @@
       <c r="AB11" t="n">
         <v>2997</v>
       </c>
-      <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="n">
+      <c r="AC11" t="n">
         <v>2997</v>
       </c>
+      <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="n">
         <v>2997</v>
       </c>
@@ -1967,15 +2000,15 @@
         <v>2997</v>
       </c>
       <c r="AI11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AJ11" t="n">
         <v>929</v>
       </c>
-      <c r="AK11" t="inlineStr"/>
-      <c r="AL11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL11" t="inlineStr"/>
       <c r="AM11" t="n">
         <v>929</v>
       </c>
@@ -1992,6 +2025,9 @@
         <v>929</v>
       </c>
       <c r="AR11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2085,10 +2121,10 @@
       <c r="AC12" t="n">
         <v>569</v>
       </c>
-      <c r="AD12" t="inlineStr"/>
-      <c r="AE12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="n">
         <v>569</v>
       </c>
@@ -2104,10 +2140,10 @@
       <c r="AJ12" t="n">
         <v>569</v>
       </c>
-      <c r="AK12" t="inlineStr"/>
-      <c r="AL12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="n">
         <v>569</v>
       </c>
@@ -2124,6 +2160,9 @@
         <v>569</v>
       </c>
       <c r="AR12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2160,10 +2199,10 @@
       <c r="J13" t="n">
         <v>569</v>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="n">
-        <v>569</v>
-      </c>
+      <c r="K13" t="n">
+        <v>569</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
         <v>569</v>
       </c>
@@ -2209,14 +2248,14 @@
       <c r="AA13" t="n">
         <v>569</v>
       </c>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="n">
         <v>569</v>
       </c>
@@ -2232,24 +2271,27 @@
       <c r="AJ13" t="n">
         <v>569</v>
       </c>
-      <c r="AK13" t="inlineStr"/>
-      <c r="AL13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="n">
         <v>569</v>
       </c>
       <c r="AN13" t="n">
         <v>569</v>
       </c>
-      <c r="AO13" t="inlineStr"/>
-      <c r="AP13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP13" t="inlineStr"/>
       <c r="AQ13" t="n">
         <v>569</v>
       </c>
       <c r="AR13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2307,10 +2349,10 @@
       <c r="Q14" t="n">
         <v>794</v>
       </c>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="n">
+      <c r="R14" t="n">
         <v>794</v>
       </c>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="n">
         <v>794</v>
       </c>
@@ -2318,7 +2360,7 @@
         <v>794</v>
       </c>
       <c r="V14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="W14" t="n">
         <v>499</v>
@@ -2335,11 +2377,11 @@
       <c r="AA14" t="n">
         <v>499</v>
       </c>
-      <c r="AB14" t="inlineStr"/>
+      <c r="AB14" t="n">
+        <v>499</v>
+      </c>
       <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="n">
         <v>499</v>
       </c>
@@ -2380,6 +2422,9 @@
         <v>499</v>
       </c>
       <c r="AR14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2473,10 +2518,10 @@
       <c r="AC15" t="n">
         <v>499</v>
       </c>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="n">
         <v>499</v>
       </c>
@@ -2486,14 +2531,14 @@
       <c r="AH15" t="n">
         <v>499</v>
       </c>
-      <c r="AI15" t="inlineStr"/>
-      <c r="AJ15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AK15" t="inlineStr"/>
-      <c r="AL15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AI15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ15" t="inlineStr"/>
+      <c r="AK15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="n">
         <v>499</v>
       </c>
@@ -2510,6 +2555,9 @@
         <v>499</v>
       </c>
       <c r="AR15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2588,17 +2636,17 @@
       <c r="X16" t="n">
         <v>299</v>
       </c>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y16" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
         <v>299</v>
       </c>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="n">
         <v>299</v>
       </c>
@@ -2620,10 +2668,10 @@
       <c r="AJ16" t="n">
         <v>299</v>
       </c>
-      <c r="AK16" t="inlineStr"/>
-      <c r="AL16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="n">
         <v>299</v>
       </c>
@@ -2640,6 +2688,9 @@
         <v>299</v>
       </c>
       <c r="AR16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2733,10 +2784,10 @@
       <c r="AC17" t="n">
         <v>929</v>
       </c>
-      <c r="AD17" t="inlineStr"/>
-      <c r="AE17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="n">
         <v>929</v>
       </c>
@@ -2752,10 +2803,10 @@
       <c r="AJ17" t="n">
         <v>929</v>
       </c>
-      <c r="AK17" t="inlineStr"/>
-      <c r="AL17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL17" t="inlineStr"/>
       <c r="AM17" t="n">
         <v>929</v>
       </c>
@@ -2772,6 +2823,9 @@
         <v>929</v>
       </c>
       <c r="AR17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2862,11 +2916,11 @@
       <c r="AB18" t="n">
         <v>499</v>
       </c>
-      <c r="AC18" t="inlineStr"/>
+      <c r="AC18" t="n">
+        <v>499</v>
+      </c>
       <c r="AD18" t="inlineStr"/>
-      <c r="AE18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="n">
         <v>499</v>
       </c>
@@ -2882,10 +2936,10 @@
       <c r="AJ18" t="n">
         <v>499</v>
       </c>
-      <c r="AK18" t="inlineStr"/>
-      <c r="AL18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AK18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL18" t="inlineStr"/>
       <c r="AM18" t="n">
         <v>499</v>
       </c>
@@ -2902,6 +2956,9 @@
         <v>499</v>
       </c>
       <c r="AR18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2984,7 +3041,7 @@
         <v>1299</v>
       </c>
       <c r="Z19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AA19" t="n">
         <v>1497</v>
@@ -2992,13 +3049,13 @@
       <c r="AB19" t="n">
         <v>1497</v>
       </c>
-      <c r="AC19" t="inlineStr"/>
+      <c r="AC19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AD19" t="inlineStr"/>
-      <c r="AE19" t="n">
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="n">
         <v>465</v>
-      </c>
-      <c r="AF19" t="n">
-        <v>1497</v>
       </c>
       <c r="AG19" t="n">
         <v>1497</v>
@@ -3034,6 +3091,9 @@
         <v>1497</v>
       </c>
       <c r="AR19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AS19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3148,10 +3208,10 @@
       <c r="AJ20" t="n">
         <v>929</v>
       </c>
-      <c r="AK20" t="inlineStr"/>
-      <c r="AL20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL20" t="inlineStr"/>
       <c r="AM20" t="n">
         <v>929</v>
       </c>
@@ -3168,6 +3228,9 @@
         <v>929</v>
       </c>
       <c r="AR20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3231,10 +3294,10 @@
       <c r="S21" t="n">
         <v>499</v>
       </c>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="n">
-        <v>499</v>
-      </c>
+      <c r="T21" t="n">
+        <v>499</v>
+      </c>
+      <c r="U21" t="inlineStr"/>
       <c r="V21" t="n">
         <v>499</v>
       </c>
@@ -3259,10 +3322,10 @@
       <c r="AC21" t="n">
         <v>499</v>
       </c>
-      <c r="AD21" t="inlineStr"/>
-      <c r="AE21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="n">
         <v>499</v>
       </c>
@@ -3300,6 +3363,9 @@
         <v>499</v>
       </c>
       <c r="AR21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3387,14 +3453,14 @@
       <c r="AA22" t="n">
         <v>299</v>
       </c>
-      <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AD22" t="inlineStr"/>
-      <c r="AE22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="n">
         <v>299</v>
       </c>
@@ -3410,10 +3476,10 @@
       <c r="AJ22" t="n">
         <v>299</v>
       </c>
-      <c r="AK22" t="inlineStr"/>
-      <c r="AL22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL22" t="inlineStr"/>
       <c r="AM22" t="n">
         <v>299</v>
       </c>
@@ -3430,6 +3496,9 @@
         <v>299</v>
       </c>
       <c r="AR22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3520,11 +3589,11 @@
       <c r="AB23" t="n">
         <v>1299</v>
       </c>
-      <c r="AC23" t="inlineStr"/>
+      <c r="AC23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AE23" t="inlineStr"/>
       <c r="AF23" t="n">
         <v>1299</v>
       </c>
@@ -3540,10 +3609,10 @@
       <c r="AJ23" t="n">
         <v>1299</v>
       </c>
-      <c r="AK23" t="inlineStr"/>
-      <c r="AL23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AK23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AL23" t="inlineStr"/>
       <c r="AM23" t="n">
         <v>1299</v>
       </c>
@@ -3560,6 +3629,9 @@
         <v>1299</v>
       </c>
       <c r="AR23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AS23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3647,11 +3719,11 @@
       <c r="AA24" t="n">
         <v>929</v>
       </c>
-      <c r="AB24" t="inlineStr"/>
+      <c r="AB24" t="n">
+        <v>929</v>
+      </c>
       <c r="AC24" t="inlineStr"/>
-      <c r="AD24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="n">
         <v>929</v>
       </c>
@@ -3670,10 +3742,10 @@
       <c r="AJ24" t="n">
         <v>929</v>
       </c>
-      <c r="AK24" t="inlineStr"/>
-      <c r="AL24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL24" t="inlineStr"/>
       <c r="AM24" t="n">
         <v>929</v>
       </c>
@@ -3690,6 +3762,9 @@
         <v>929</v>
       </c>
       <c r="AR24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3702,10 +3777,10 @@
       <c r="B25" t="n">
         <v>929</v>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="n">
-        <v>929</v>
-      </c>
+      <c r="C25" t="n">
+        <v>929</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
         <v>929</v>
       </c>
@@ -3775,11 +3850,11 @@
       <c r="AA25" t="n">
         <v>929</v>
       </c>
-      <c r="AB25" t="inlineStr"/>
+      <c r="AB25" t="n">
+        <v>929</v>
+      </c>
       <c r="AC25" t="inlineStr"/>
-      <c r="AD25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD25" t="inlineStr"/>
       <c r="AE25" t="n">
         <v>929</v>
       </c>
@@ -3798,10 +3873,10 @@
       <c r="AJ25" t="n">
         <v>929</v>
       </c>
-      <c r="AK25" t="inlineStr"/>
-      <c r="AL25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL25" t="inlineStr"/>
       <c r="AM25" t="n">
         <v>929</v>
       </c>
@@ -3818,6 +3893,9 @@
         <v>929</v>
       </c>
       <c r="AR25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3827,10 +3905,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
         <v>1299</v>
       </c>
@@ -3903,14 +3981,14 @@
       <c r="AA26" t="n">
         <v>1299</v>
       </c>
-      <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AD26" t="inlineStr"/>
-      <c r="AE26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AB26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="n">
         <v>1299</v>
       </c>
@@ -3926,10 +4004,10 @@
       <c r="AJ26" t="n">
         <v>1299</v>
       </c>
-      <c r="AK26" t="inlineStr"/>
-      <c r="AL26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AK26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AL26" t="inlineStr"/>
       <c r="AM26" t="n">
         <v>1299</v>
       </c>
@@ -3946,6 +4024,9 @@
         <v>1299</v>
       </c>
       <c r="AR26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AS26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 09:02
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS26"/>
+  <dimension ref="A1:AT26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,6 +478,7 @@
     <col width="21" customWidth="1" min="43" max="43"/>
     <col width="21" customWidth="1" min="44" max="44"/>
     <col width="21" customWidth="1" min="45" max="45"/>
+    <col width="21" customWidth="1" min="46" max="46"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -488,220 +489,225 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 14:28</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -779,10 +785,10 @@
       <c r="W2" t="n">
         <v>929</v>
       </c>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="n">
-        <v>929</v>
-      </c>
+      <c r="X2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="n">
         <v>929</v>
       </c>
@@ -795,25 +801,25 @@
       <c r="AC2" t="n">
         <v>929</v>
       </c>
-      <c r="AD2" t="inlineStr"/>
+      <c r="AD2" t="n">
+        <v>929</v>
+      </c>
       <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
         <v>929</v>
       </c>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="n">
         <v>929</v>
       </c>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="n">
         <v>929</v>
       </c>
@@ -833,6 +839,9 @@
         <v>929</v>
       </c>
       <c r="AS2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -857,10 +866,10 @@
       <c r="F3" t="n">
         <v>569</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>569</v>
-      </c>
+      <c r="G3" t="n">
+        <v>569</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>569</v>
       </c>
@@ -903,26 +912,26 @@
       <c r="V3" t="n">
         <v>569</v>
       </c>
-      <c r="W3" t="inlineStr"/>
+      <c r="W3" t="n">
+        <v>569</v>
+      </c>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
         <v>569</v>
       </c>
       <c r="AB3" t="n">
         <v>569</v>
       </c>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="n">
         <v>569</v>
       </c>
@@ -938,10 +947,10 @@
       <c r="AK3" t="n">
         <v>569</v>
       </c>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="n">
         <v>569</v>
       </c>
@@ -958,6 +967,9 @@
         <v>569</v>
       </c>
       <c r="AS3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1048,10 +1060,10 @@
       <c r="AB4" t="n">
         <v>299</v>
       </c>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="n">
         <v>299</v>
       </c>
@@ -1073,10 +1085,10 @@
       <c r="AK4" t="n">
         <v>299</v>
       </c>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM4" t="inlineStr"/>
       <c r="AN4" t="n">
         <v>299</v>
       </c>
@@ -1093,6 +1105,9 @@
         <v>299</v>
       </c>
       <c r="AS4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1111,10 +1126,10 @@
       <c r="D5" t="n">
         <v>569</v>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>569</v>
-      </c>
+      <c r="E5" t="n">
+        <v>569</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>569</v>
       </c>
@@ -1208,10 +1223,10 @@
       <c r="AK5" t="n">
         <v>569</v>
       </c>
-      <c r="AL5" t="inlineStr"/>
-      <c r="AM5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM5" t="inlineStr"/>
       <c r="AN5" t="n">
         <v>569</v>
       </c>
@@ -1228,6 +1243,9 @@
         <v>569</v>
       </c>
       <c r="AS5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1321,10 +1339,10 @@
       <c r="AC6" t="n">
         <v>499</v>
       </c>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="n">
         <v>499</v>
       </c>
@@ -1343,10 +1361,10 @@
       <c r="AK6" t="n">
         <v>499</v>
       </c>
-      <c r="AL6" t="inlineStr"/>
-      <c r="AM6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AL6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="n">
         <v>499</v>
       </c>
@@ -1363,6 +1381,9 @@
         <v>499</v>
       </c>
       <c r="AS6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1453,12 +1474,12 @@
       <c r="AB7" t="n">
         <v>569</v>
       </c>
-      <c r="AC7" t="inlineStr"/>
+      <c r="AC7" t="n">
+        <v>569</v>
+      </c>
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="n">
         <v>569</v>
       </c>
@@ -1474,10 +1495,10 @@
       <c r="AK7" t="n">
         <v>569</v>
       </c>
-      <c r="AL7" t="inlineStr"/>
-      <c r="AM7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="n">
         <v>569</v>
       </c>
@@ -1494,6 +1515,9 @@
         <v>569</v>
       </c>
       <c r="AS7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1584,14 +1608,14 @@
       <c r="AB8" t="n">
         <v>929</v>
       </c>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="n">
         <v>929</v>
       </c>
@@ -1607,10 +1631,10 @@
       <c r="AK8" t="n">
         <v>929</v>
       </c>
-      <c r="AL8" t="inlineStr"/>
-      <c r="AM8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="n">
         <v>929</v>
       </c>
@@ -1627,6 +1651,9 @@
         <v>929</v>
       </c>
       <c r="AS8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1717,10 +1744,10 @@
       <c r="AB9" t="n">
         <v>299</v>
       </c>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="n">
         <v>299</v>
       </c>
@@ -1742,10 +1769,10 @@
       <c r="AK9" t="n">
         <v>299</v>
       </c>
-      <c r="AL9" t="inlineStr"/>
-      <c r="AM9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM9" t="inlineStr"/>
       <c r="AN9" t="n">
         <v>299</v>
       </c>
@@ -1762,6 +1789,9 @@
         <v>299</v>
       </c>
       <c r="AS9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1822,10 +1852,10 @@
       <c r="R10" t="n">
         <v>299</v>
       </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="n">
-        <v>299</v>
-      </c>
+      <c r="S10" t="n">
+        <v>299</v>
+      </c>
+      <c r="T10" t="inlineStr"/>
       <c r="U10" t="n">
         <v>299</v>
       </c>
@@ -1850,14 +1880,14 @@
       <c r="AB10" t="n">
         <v>299</v>
       </c>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF10" t="inlineStr"/>
       <c r="AG10" t="n">
         <v>299</v>
       </c>
@@ -1873,10 +1903,10 @@
       <c r="AK10" t="n">
         <v>299</v>
       </c>
-      <c r="AL10" t="inlineStr"/>
-      <c r="AM10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM10" t="inlineStr"/>
       <c r="AN10" t="n">
         <v>299</v>
       </c>
@@ -1893,6 +1923,9 @@
         <v>299</v>
       </c>
       <c r="AS10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1986,10 +2019,10 @@
       <c r="AC11" t="n">
         <v>2997</v>
       </c>
-      <c r="AD11" t="inlineStr"/>
-      <c r="AE11" t="n">
+      <c r="AD11" t="n">
         <v>2997</v>
       </c>
+      <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="n">
         <v>2997</v>
       </c>
@@ -2003,15 +2036,15 @@
         <v>2997</v>
       </c>
       <c r="AJ11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AK11" t="n">
         <v>929</v>
       </c>
-      <c r="AL11" t="inlineStr"/>
-      <c r="AM11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM11" t="inlineStr"/>
       <c r="AN11" t="n">
         <v>929</v>
       </c>
@@ -2028,6 +2061,9 @@
         <v>929</v>
       </c>
       <c r="AS11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2124,10 +2160,10 @@
       <c r="AD12" t="n">
         <v>569</v>
       </c>
-      <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF12" t="inlineStr"/>
       <c r="AG12" t="n">
         <v>569</v>
       </c>
@@ -2143,10 +2179,10 @@
       <c r="AK12" t="n">
         <v>569</v>
       </c>
-      <c r="AL12" t="inlineStr"/>
-      <c r="AM12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM12" t="inlineStr"/>
       <c r="AN12" t="n">
         <v>569</v>
       </c>
@@ -2163,6 +2199,9 @@
         <v>569</v>
       </c>
       <c r="AS12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2202,10 +2241,10 @@
       <c r="K13" t="n">
         <v>569</v>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>569</v>
-      </c>
+      <c r="L13" t="n">
+        <v>569</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
         <v>569</v>
       </c>
@@ -2251,14 +2290,14 @@
       <c r="AB13" t="n">
         <v>569</v>
       </c>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF13" t="inlineStr"/>
       <c r="AG13" t="n">
         <v>569</v>
       </c>
@@ -2274,24 +2313,27 @@
       <c r="AK13" t="n">
         <v>569</v>
       </c>
-      <c r="AL13" t="inlineStr"/>
-      <c r="AM13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM13" t="inlineStr"/>
       <c r="AN13" t="n">
         <v>569</v>
       </c>
       <c r="AO13" t="n">
         <v>569</v>
       </c>
-      <c r="AP13" t="inlineStr"/>
-      <c r="AQ13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ13" t="inlineStr"/>
       <c r="AR13" t="n">
         <v>569</v>
       </c>
       <c r="AS13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2352,10 +2394,10 @@
       <c r="R14" t="n">
         <v>794</v>
       </c>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="n">
+      <c r="S14" t="n">
         <v>794</v>
       </c>
+      <c r="T14" t="inlineStr"/>
       <c r="U14" t="n">
         <v>794</v>
       </c>
@@ -2363,7 +2405,7 @@
         <v>794</v>
       </c>
       <c r="W14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="X14" t="n">
         <v>499</v>
@@ -2380,11 +2422,11 @@
       <c r="AB14" t="n">
         <v>499</v>
       </c>
-      <c r="AC14" t="inlineStr"/>
+      <c r="AC14" t="n">
+        <v>499</v>
+      </c>
       <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="n">
         <v>499</v>
       </c>
@@ -2425,6 +2467,9 @@
         <v>499</v>
       </c>
       <c r="AS14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2521,10 +2566,10 @@
       <c r="AD15" t="n">
         <v>499</v>
       </c>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF15" t="inlineStr"/>
       <c r="AG15" t="n">
         <v>499</v>
       </c>
@@ -2534,14 +2579,14 @@
       <c r="AI15" t="n">
         <v>499</v>
       </c>
-      <c r="AJ15" t="inlineStr"/>
-      <c r="AK15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AL15" t="inlineStr"/>
-      <c r="AM15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AJ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM15" t="inlineStr"/>
       <c r="AN15" t="n">
         <v>499</v>
       </c>
@@ -2558,6 +2603,9 @@
         <v>499</v>
       </c>
       <c r="AS15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2639,17 +2687,17 @@
       <c r="Y16" t="n">
         <v>299</v>
       </c>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="n">
         <v>299</v>
       </c>
-      <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="n">
         <v>299</v>
       </c>
@@ -2671,10 +2719,10 @@
       <c r="AK16" t="n">
         <v>299</v>
       </c>
-      <c r="AL16" t="inlineStr"/>
-      <c r="AM16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM16" t="inlineStr"/>
       <c r="AN16" t="n">
         <v>299</v>
       </c>
@@ -2691,6 +2739,9 @@
         <v>299</v>
       </c>
       <c r="AS16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2787,10 +2838,10 @@
       <c r="AD17" t="n">
         <v>929</v>
       </c>
-      <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF17" t="inlineStr"/>
       <c r="AG17" t="n">
         <v>929</v>
       </c>
@@ -2806,10 +2857,10 @@
       <c r="AK17" t="n">
         <v>929</v>
       </c>
-      <c r="AL17" t="inlineStr"/>
-      <c r="AM17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM17" t="inlineStr"/>
       <c r="AN17" t="n">
         <v>929</v>
       </c>
@@ -2826,6 +2877,9 @@
         <v>929</v>
       </c>
       <c r="AS17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2919,11 +2973,11 @@
       <c r="AC18" t="n">
         <v>499</v>
       </c>
-      <c r="AD18" t="inlineStr"/>
+      <c r="AD18" t="n">
+        <v>499</v>
+      </c>
       <c r="AE18" t="inlineStr"/>
-      <c r="AF18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF18" t="inlineStr"/>
       <c r="AG18" t="n">
         <v>499</v>
       </c>
@@ -2939,10 +2993,10 @@
       <c r="AK18" t="n">
         <v>499</v>
       </c>
-      <c r="AL18" t="inlineStr"/>
-      <c r="AM18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AL18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM18" t="inlineStr"/>
       <c r="AN18" t="n">
         <v>499</v>
       </c>
@@ -2959,6 +3013,9 @@
         <v>499</v>
       </c>
       <c r="AS18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3044,7 +3101,7 @@
         <v>1299</v>
       </c>
       <c r="AA19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AB19" t="n">
         <v>1497</v>
@@ -3052,13 +3109,13 @@
       <c r="AC19" t="n">
         <v>1497</v>
       </c>
-      <c r="AD19" t="inlineStr"/>
+      <c r="AD19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AE19" t="inlineStr"/>
-      <c r="AF19" t="n">
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="n">
         <v>465</v>
-      </c>
-      <c r="AG19" t="n">
-        <v>1497</v>
       </c>
       <c r="AH19" t="n">
         <v>1497</v>
@@ -3094,6 +3151,9 @@
         <v>1497</v>
       </c>
       <c r="AS19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AT19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3211,10 +3271,10 @@
       <c r="AK20" t="n">
         <v>929</v>
       </c>
-      <c r="AL20" t="inlineStr"/>
-      <c r="AM20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM20" t="inlineStr"/>
       <c r="AN20" t="n">
         <v>929</v>
       </c>
@@ -3231,6 +3291,9 @@
         <v>929</v>
       </c>
       <c r="AS20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3240,9 +3303,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
         <v>499</v>
       </c>
@@ -3297,10 +3358,10 @@
       <c r="T21" t="n">
         <v>499</v>
       </c>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="n">
-        <v>499</v>
-      </c>
+      <c r="U21" t="n">
+        <v>499</v>
+      </c>
+      <c r="V21" t="inlineStr"/>
       <c r="W21" t="n">
         <v>499</v>
       </c>
@@ -3325,10 +3386,10 @@
       <c r="AD21" t="n">
         <v>499</v>
       </c>
-      <c r="AE21" t="inlineStr"/>
-      <c r="AF21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF21" t="inlineStr"/>
       <c r="AG21" t="n">
         <v>499</v>
       </c>
@@ -3366,6 +3427,9 @@
         <v>499</v>
       </c>
       <c r="AS21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3456,14 +3520,14 @@
       <c r="AB22" t="n">
         <v>299</v>
       </c>
-      <c r="AC22" t="inlineStr"/>
-      <c r="AD22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF22" t="inlineStr"/>
       <c r="AG22" t="n">
         <v>299</v>
       </c>
@@ -3479,10 +3543,10 @@
       <c r="AK22" t="n">
         <v>299</v>
       </c>
-      <c r="AL22" t="inlineStr"/>
-      <c r="AM22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM22" t="inlineStr"/>
       <c r="AN22" t="n">
         <v>299</v>
       </c>
@@ -3499,6 +3563,9 @@
         <v>299</v>
       </c>
       <c r="AS22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3592,11 +3659,11 @@
       <c r="AC23" t="n">
         <v>1299</v>
       </c>
-      <c r="AD23" t="inlineStr"/>
+      <c r="AD23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AF23" t="inlineStr"/>
       <c r="AG23" t="n">
         <v>1299</v>
       </c>
@@ -3612,10 +3679,10 @@
       <c r="AK23" t="n">
         <v>1299</v>
       </c>
-      <c r="AL23" t="inlineStr"/>
-      <c r="AM23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AL23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AM23" t="inlineStr"/>
       <c r="AN23" t="n">
         <v>1299</v>
       </c>
@@ -3632,6 +3699,9 @@
         <v>1299</v>
       </c>
       <c r="AS23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AT23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3722,11 +3792,11 @@
       <c r="AB24" t="n">
         <v>929</v>
       </c>
-      <c r="AC24" t="inlineStr"/>
+      <c r="AC24" t="n">
+        <v>929</v>
+      </c>
       <c r="AD24" t="inlineStr"/>
-      <c r="AE24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE24" t="inlineStr"/>
       <c r="AF24" t="n">
         <v>929</v>
       </c>
@@ -3745,10 +3815,10 @@
       <c r="AK24" t="n">
         <v>929</v>
       </c>
-      <c r="AL24" t="inlineStr"/>
-      <c r="AM24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM24" t="inlineStr"/>
       <c r="AN24" t="n">
         <v>929</v>
       </c>
@@ -3765,6 +3835,9 @@
         <v>929</v>
       </c>
       <c r="AS24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3780,10 +3853,10 @@
       <c r="C25" t="n">
         <v>929</v>
       </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="n">
-        <v>929</v>
-      </c>
+      <c r="D25" t="n">
+        <v>929</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
         <v>929</v>
       </c>
@@ -3853,11 +3926,11 @@
       <c r="AB25" t="n">
         <v>929</v>
       </c>
-      <c r="AC25" t="inlineStr"/>
+      <c r="AC25" t="n">
+        <v>929</v>
+      </c>
       <c r="AD25" t="inlineStr"/>
-      <c r="AE25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="n">
         <v>929</v>
       </c>
@@ -3876,10 +3949,10 @@
       <c r="AK25" t="n">
         <v>929</v>
       </c>
-      <c r="AL25" t="inlineStr"/>
-      <c r="AM25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM25" t="inlineStr"/>
       <c r="AN25" t="n">
         <v>929</v>
       </c>
@@ -3896,6 +3969,9 @@
         <v>929</v>
       </c>
       <c r="AS25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3908,10 +3984,10 @@
       <c r="B26" t="n">
         <v>1299</v>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
         <v>1299</v>
       </c>
@@ -3984,14 +4060,14 @@
       <c r="AB26" t="n">
         <v>1299</v>
       </c>
-      <c r="AC26" t="inlineStr"/>
-      <c r="AD26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AC26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AF26" t="inlineStr"/>
       <c r="AG26" t="n">
         <v>1299</v>
       </c>
@@ -4007,10 +4083,10 @@
       <c r="AK26" t="n">
         <v>1299</v>
       </c>
-      <c r="AL26" t="inlineStr"/>
-      <c r="AM26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AL26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AM26" t="inlineStr"/>
       <c r="AN26" t="n">
         <v>1299</v>
       </c>
@@ -4027,6 +4103,9 @@
         <v>1299</v>
       </c>
       <c r="AS26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AT26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 10:50
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT26"/>
+  <dimension ref="A1:AU26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,7 @@
     <col width="21" customWidth="1" min="44" max="44"/>
     <col width="21" customWidth="1" min="45" max="45"/>
     <col width="21" customWidth="1" min="46" max="46"/>
+    <col width="21" customWidth="1" min="47" max="47"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -489,225 +490,230 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 16:16</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -788,10 +794,10 @@
       <c r="X2" t="n">
         <v>929</v>
       </c>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Y2" t="n">
+        <v>929</v>
+      </c>
+      <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
         <v>929</v>
       </c>
@@ -804,25 +810,25 @@
       <c r="AD2" t="n">
         <v>929</v>
       </c>
-      <c r="AE2" t="inlineStr"/>
+      <c r="AE2" t="n">
+        <v>929</v>
+      </c>
       <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="n">
         <v>929</v>
       </c>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="n">
         <v>929</v>
       </c>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="n">
         <v>929</v>
       </c>
@@ -842,6 +848,9 @@
         <v>929</v>
       </c>
       <c r="AT2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -869,10 +878,10 @@
       <c r="G3" t="n">
         <v>569</v>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>569</v>
-      </c>
+      <c r="H3" t="n">
+        <v>569</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
         <v>569</v>
       </c>
@@ -915,26 +924,26 @@
       <c r="W3" t="n">
         <v>569</v>
       </c>
-      <c r="X3" t="inlineStr"/>
+      <c r="X3" t="n">
+        <v>569</v>
+      </c>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="n">
         <v>569</v>
       </c>
       <c r="AC3" t="n">
         <v>569</v>
       </c>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="n">
         <v>569</v>
       </c>
@@ -950,10 +959,10 @@
       <c r="AL3" t="n">
         <v>569</v>
       </c>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN3" t="inlineStr"/>
       <c r="AO3" t="n">
         <v>569</v>
       </c>
@@ -970,6 +979,9 @@
         <v>569</v>
       </c>
       <c r="AT3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1063,10 +1075,10 @@
       <c r="AC4" t="n">
         <v>299</v>
       </c>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="n">
         <v>299</v>
       </c>
@@ -1088,10 +1100,10 @@
       <c r="AL4" t="n">
         <v>299</v>
       </c>
-      <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN4" t="inlineStr"/>
       <c r="AO4" t="n">
         <v>299</v>
       </c>
@@ -1108,6 +1120,9 @@
         <v>299</v>
       </c>
       <c r="AT4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1129,10 +1144,10 @@
       <c r="E5" t="n">
         <v>569</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>569</v>
-      </c>
+      <c r="F5" t="n">
+        <v>569</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>569</v>
       </c>
@@ -1226,10 +1241,10 @@
       <c r="AL5" t="n">
         <v>569</v>
       </c>
-      <c r="AM5" t="inlineStr"/>
-      <c r="AN5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN5" t="inlineStr"/>
       <c r="AO5" t="n">
         <v>569</v>
       </c>
@@ -1246,6 +1261,9 @@
         <v>569</v>
       </c>
       <c r="AT5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1342,10 +1360,10 @@
       <c r="AD6" t="n">
         <v>499</v>
       </c>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="n">
         <v>499</v>
       </c>
@@ -1364,10 +1382,10 @@
       <c r="AL6" t="n">
         <v>499</v>
       </c>
-      <c r="AM6" t="inlineStr"/>
-      <c r="AN6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AM6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN6" t="inlineStr"/>
       <c r="AO6" t="n">
         <v>499</v>
       </c>
@@ -1384,6 +1402,9 @@
         <v>499</v>
       </c>
       <c r="AT6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1477,12 +1498,12 @@
       <c r="AC7" t="n">
         <v>569</v>
       </c>
-      <c r="AD7" t="inlineStr"/>
+      <c r="AD7" t="n">
+        <v>569</v>
+      </c>
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="n">
         <v>569</v>
       </c>
@@ -1498,10 +1519,10 @@
       <c r="AL7" t="n">
         <v>569</v>
       </c>
-      <c r="AM7" t="inlineStr"/>
-      <c r="AN7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN7" t="inlineStr"/>
       <c r="AO7" t="n">
         <v>569</v>
       </c>
@@ -1518,6 +1539,9 @@
         <v>569</v>
       </c>
       <c r="AT7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1611,14 +1635,14 @@
       <c r="AC8" t="n">
         <v>929</v>
       </c>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="n">
         <v>929</v>
       </c>
@@ -1634,10 +1658,10 @@
       <c r="AL8" t="n">
         <v>929</v>
       </c>
-      <c r="AM8" t="inlineStr"/>
-      <c r="AN8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN8" t="inlineStr"/>
       <c r="AO8" t="n">
         <v>929</v>
       </c>
@@ -1654,6 +1678,9 @@
         <v>929</v>
       </c>
       <c r="AT8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1747,10 +1774,10 @@
       <c r="AC9" t="n">
         <v>299</v>
       </c>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="n">
         <v>299</v>
       </c>
@@ -1772,10 +1799,10 @@
       <c r="AL9" t="n">
         <v>299</v>
       </c>
-      <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN9" t="inlineStr"/>
       <c r="AO9" t="n">
         <v>299</v>
       </c>
@@ -1792,6 +1819,9 @@
         <v>299</v>
       </c>
       <c r="AT9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1855,10 +1885,10 @@
       <c r="S10" t="n">
         <v>299</v>
       </c>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="n">
-        <v>299</v>
-      </c>
+      <c r="T10" t="n">
+        <v>299</v>
+      </c>
+      <c r="U10" t="inlineStr"/>
       <c r="V10" t="n">
         <v>299</v>
       </c>
@@ -1883,14 +1913,14 @@
       <c r="AC10" t="n">
         <v>299</v>
       </c>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG10" t="inlineStr"/>
       <c r="AH10" t="n">
         <v>299</v>
       </c>
@@ -1906,10 +1936,10 @@
       <c r="AL10" t="n">
         <v>299</v>
       </c>
-      <c r="AM10" t="inlineStr"/>
-      <c r="AN10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN10" t="inlineStr"/>
       <c r="AO10" t="n">
         <v>299</v>
       </c>
@@ -1926,6 +1956,9 @@
         <v>299</v>
       </c>
       <c r="AT10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2022,10 +2055,10 @@
       <c r="AD11" t="n">
         <v>2997</v>
       </c>
-      <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="n">
+      <c r="AE11" t="n">
         <v>2997</v>
       </c>
+      <c r="AF11" t="inlineStr"/>
       <c r="AG11" t="n">
         <v>2997</v>
       </c>
@@ -2039,15 +2072,15 @@
         <v>2997</v>
       </c>
       <c r="AK11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AL11" t="n">
         <v>929</v>
       </c>
-      <c r="AM11" t="inlineStr"/>
-      <c r="AN11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN11" t="inlineStr"/>
       <c r="AO11" t="n">
         <v>929</v>
       </c>
@@ -2064,6 +2097,9 @@
         <v>929</v>
       </c>
       <c r="AT11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2163,10 +2199,10 @@
       <c r="AE12" t="n">
         <v>569</v>
       </c>
-      <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="n">
         <v>569</v>
       </c>
@@ -2182,10 +2218,10 @@
       <c r="AL12" t="n">
         <v>569</v>
       </c>
-      <c r="AM12" t="inlineStr"/>
-      <c r="AN12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN12" t="inlineStr"/>
       <c r="AO12" t="n">
         <v>569</v>
       </c>
@@ -2202,6 +2238,9 @@
         <v>569</v>
       </c>
       <c r="AT12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2244,10 +2283,10 @@
       <c r="L13" t="n">
         <v>569</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="n">
-        <v>569</v>
-      </c>
+      <c r="M13" t="n">
+        <v>569</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
         <v>569</v>
       </c>
@@ -2293,14 +2332,14 @@
       <c r="AC13" t="n">
         <v>569</v>
       </c>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="n">
         <v>569</v>
       </c>
@@ -2316,24 +2355,27 @@
       <c r="AL13" t="n">
         <v>569</v>
       </c>
-      <c r="AM13" t="inlineStr"/>
-      <c r="AN13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN13" t="inlineStr"/>
       <c r="AO13" t="n">
         <v>569</v>
       </c>
       <c r="AP13" t="n">
         <v>569</v>
       </c>
-      <c r="AQ13" t="inlineStr"/>
-      <c r="AR13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AQ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR13" t="inlineStr"/>
       <c r="AS13" t="n">
         <v>569</v>
       </c>
       <c r="AT13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2397,10 +2439,10 @@
       <c r="S14" t="n">
         <v>794</v>
       </c>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="n">
+      <c r="T14" t="n">
         <v>794</v>
       </c>
+      <c r="U14" t="inlineStr"/>
       <c r="V14" t="n">
         <v>794</v>
       </c>
@@ -2408,7 +2450,7 @@
         <v>794</v>
       </c>
       <c r="X14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="Y14" t="n">
         <v>499</v>
@@ -2425,11 +2467,11 @@
       <c r="AC14" t="n">
         <v>499</v>
       </c>
-      <c r="AD14" t="inlineStr"/>
+      <c r="AD14" t="n">
+        <v>499</v>
+      </c>
       <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF14" t="inlineStr"/>
       <c r="AG14" t="n">
         <v>499</v>
       </c>
@@ -2470,6 +2512,9 @@
         <v>499</v>
       </c>
       <c r="AT14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2569,10 +2614,10 @@
       <c r="AE15" t="n">
         <v>499</v>
       </c>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="n">
         <v>499</v>
       </c>
@@ -2582,14 +2627,14 @@
       <c r="AJ15" t="n">
         <v>499</v>
       </c>
-      <c r="AK15" t="inlineStr"/>
-      <c r="AL15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AK15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL15" t="inlineStr"/>
+      <c r="AM15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN15" t="inlineStr"/>
       <c r="AO15" t="n">
         <v>499</v>
       </c>
@@ -2606,6 +2651,9 @@
         <v>499</v>
       </c>
       <c r="AT15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2690,17 +2738,17 @@
       <c r="Z16" t="n">
         <v>299</v>
       </c>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="n">
         <v>299</v>
       </c>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="n">
         <v>299</v>
       </c>
@@ -2722,10 +2770,10 @@
       <c r="AL16" t="n">
         <v>299</v>
       </c>
-      <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN16" t="inlineStr"/>
       <c r="AO16" t="n">
         <v>299</v>
       </c>
@@ -2742,6 +2790,9 @@
         <v>299</v>
       </c>
       <c r="AT16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2841,10 +2892,10 @@
       <c r="AE17" t="n">
         <v>929</v>
       </c>
-      <c r="AF17" t="inlineStr"/>
-      <c r="AG17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="n">
         <v>929</v>
       </c>
@@ -2860,10 +2911,10 @@
       <c r="AL17" t="n">
         <v>929</v>
       </c>
-      <c r="AM17" t="inlineStr"/>
-      <c r="AN17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN17" t="inlineStr"/>
       <c r="AO17" t="n">
         <v>929</v>
       </c>
@@ -2880,6 +2931,9 @@
         <v>929</v>
       </c>
       <c r="AT17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2976,11 +3030,11 @@
       <c r="AD18" t="n">
         <v>499</v>
       </c>
-      <c r="AE18" t="inlineStr"/>
+      <c r="AE18" t="n">
+        <v>499</v>
+      </c>
       <c r="AF18" t="inlineStr"/>
-      <c r="AG18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="n">
         <v>499</v>
       </c>
@@ -2996,10 +3050,10 @@
       <c r="AL18" t="n">
         <v>499</v>
       </c>
-      <c r="AM18" t="inlineStr"/>
-      <c r="AN18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AM18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN18" t="inlineStr"/>
       <c r="AO18" t="n">
         <v>499</v>
       </c>
@@ -3016,6 +3070,9 @@
         <v>499</v>
       </c>
       <c r="AT18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3104,7 +3161,7 @@
         <v>1299</v>
       </c>
       <c r="AB19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AC19" t="n">
         <v>1497</v>
@@ -3112,13 +3169,13 @@
       <c r="AD19" t="n">
         <v>1497</v>
       </c>
-      <c r="AE19" t="inlineStr"/>
+      <c r="AE19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AF19" t="inlineStr"/>
-      <c r="AG19" t="n">
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="n">
         <v>465</v>
-      </c>
-      <c r="AH19" t="n">
-        <v>1497</v>
       </c>
       <c r="AI19" t="n">
         <v>1497</v>
@@ -3154,6 +3211,9 @@
         <v>1497</v>
       </c>
       <c r="AT19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AU19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3274,10 +3334,10 @@
       <c r="AL20" t="n">
         <v>929</v>
       </c>
-      <c r="AM20" t="inlineStr"/>
-      <c r="AN20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN20" t="inlineStr"/>
       <c r="AO20" t="n">
         <v>929</v>
       </c>
@@ -3294,6 +3354,9 @@
         <v>929</v>
       </c>
       <c r="AT20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3303,10 +3366,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="n">
+        <v>499</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>499</v>
       </c>
@@ -3361,10 +3424,10 @@
       <c r="U21" t="n">
         <v>499</v>
       </c>
-      <c r="V21" t="inlineStr"/>
-      <c r="W21" t="n">
-        <v>499</v>
-      </c>
+      <c r="V21" t="n">
+        <v>499</v>
+      </c>
+      <c r="W21" t="inlineStr"/>
       <c r="X21" t="n">
         <v>499</v>
       </c>
@@ -3389,10 +3452,10 @@
       <c r="AE21" t="n">
         <v>499</v>
       </c>
-      <c r="AF21" t="inlineStr"/>
-      <c r="AG21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG21" t="inlineStr"/>
       <c r="AH21" t="n">
         <v>499</v>
       </c>
@@ -3430,6 +3493,9 @@
         <v>499</v>
       </c>
       <c r="AT21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3523,14 +3589,14 @@
       <c r="AC22" t="n">
         <v>299</v>
       </c>
-      <c r="AD22" t="inlineStr"/>
-      <c r="AE22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AF22" t="inlineStr"/>
-      <c r="AG22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="n">
         <v>299</v>
       </c>
@@ -3546,10 +3612,10 @@
       <c r="AL22" t="n">
         <v>299</v>
       </c>
-      <c r="AM22" t="inlineStr"/>
-      <c r="AN22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN22" t="inlineStr"/>
       <c r="AO22" t="n">
         <v>299</v>
       </c>
@@ -3566,6 +3632,9 @@
         <v>299</v>
       </c>
       <c r="AT22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3662,11 +3731,11 @@
       <c r="AD23" t="n">
         <v>1299</v>
       </c>
-      <c r="AE23" t="inlineStr"/>
+      <c r="AE23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AF23" t="inlineStr"/>
-      <c r="AG23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="n">
         <v>1299</v>
       </c>
@@ -3682,10 +3751,10 @@
       <c r="AL23" t="n">
         <v>1299</v>
       </c>
-      <c r="AM23" t="inlineStr"/>
-      <c r="AN23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AM23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AN23" t="inlineStr"/>
       <c r="AO23" t="n">
         <v>1299</v>
       </c>
@@ -3702,6 +3771,9 @@
         <v>1299</v>
       </c>
       <c r="AT23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AU23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3795,11 +3867,11 @@
       <c r="AC24" t="n">
         <v>929</v>
       </c>
-      <c r="AD24" t="inlineStr"/>
+      <c r="AD24" t="n">
+        <v>929</v>
+      </c>
       <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF24" t="inlineStr"/>
       <c r="AG24" t="n">
         <v>929</v>
       </c>
@@ -3818,10 +3890,10 @@
       <c r="AL24" t="n">
         <v>929</v>
       </c>
-      <c r="AM24" t="inlineStr"/>
-      <c r="AN24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN24" t="inlineStr"/>
       <c r="AO24" t="n">
         <v>929</v>
       </c>
@@ -3838,6 +3910,9 @@
         <v>929</v>
       </c>
       <c r="AT24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3856,10 +3931,10 @@
       <c r="D25" t="n">
         <v>929</v>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>929</v>
-      </c>
+      <c r="E25" t="n">
+        <v>929</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>929</v>
       </c>
@@ -3929,11 +4004,11 @@
       <c r="AC25" t="n">
         <v>929</v>
       </c>
-      <c r="AD25" t="inlineStr"/>
+      <c r="AD25" t="n">
+        <v>929</v>
+      </c>
       <c r="AE25" t="inlineStr"/>
-      <c r="AF25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF25" t="inlineStr"/>
       <c r="AG25" t="n">
         <v>929</v>
       </c>
@@ -3952,10 +4027,10 @@
       <c r="AL25" t="n">
         <v>929</v>
       </c>
-      <c r="AM25" t="inlineStr"/>
-      <c r="AN25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN25" t="inlineStr"/>
       <c r="AO25" t="n">
         <v>929</v>
       </c>
@@ -3972,6 +4047,9 @@
         <v>929</v>
       </c>
       <c r="AT25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3987,10 +4065,10 @@
       <c r="C26" t="n">
         <v>1299</v>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
         <v>1299</v>
       </c>
@@ -4063,14 +4141,14 @@
       <c r="AC26" t="n">
         <v>1299</v>
       </c>
-      <c r="AD26" t="inlineStr"/>
-      <c r="AE26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AF26" t="inlineStr"/>
-      <c r="AG26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AD26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AE26" t="inlineStr"/>
+      <c r="AF26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AG26" t="inlineStr"/>
       <c r="AH26" t="n">
         <v>1299</v>
       </c>
@@ -4086,10 +4164,10 @@
       <c r="AL26" t="n">
         <v>1299</v>
       </c>
-      <c r="AM26" t="inlineStr"/>
-      <c r="AN26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AM26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AN26" t="inlineStr"/>
       <c r="AO26" t="n">
         <v>1299</v>
       </c>
@@ -4106,6 +4184,9 @@
         <v>1299</v>
       </c>
       <c r="AT26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AU26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 13:50
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU26"/>
+  <dimension ref="A1:AV26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,7 @@
     <col width="21" customWidth="1" min="45" max="45"/>
     <col width="21" customWidth="1" min="46" max="46"/>
     <col width="21" customWidth="1" min="47" max="47"/>
+    <col width="21" customWidth="1" min="48" max="48"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -490,230 +491,235 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 19:14</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -797,10 +803,10 @@
       <c r="Y2" t="n">
         <v>929</v>
       </c>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="n">
-        <v>929</v>
-      </c>
+      <c r="Z2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="n">
         <v>929</v>
       </c>
@@ -813,25 +819,25 @@
       <c r="AE2" t="n">
         <v>929</v>
       </c>
-      <c r="AF2" t="inlineStr"/>
+      <c r="AF2" t="n">
+        <v>929</v>
+      </c>
       <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="n">
         <v>929</v>
       </c>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="n">
         <v>929</v>
       </c>
-      <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN2" t="inlineStr"/>
       <c r="AO2" t="n">
         <v>929</v>
       </c>
@@ -851,6 +857,9 @@
         <v>929</v>
       </c>
       <c r="AU2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -860,9 +869,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>569</v>
       </c>
@@ -881,10 +888,10 @@
       <c r="H3" t="n">
         <v>569</v>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>569</v>
-      </c>
+      <c r="I3" t="n">
+        <v>569</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
         <v>569</v>
       </c>
@@ -927,26 +934,26 @@
       <c r="X3" t="n">
         <v>569</v>
       </c>
-      <c r="Y3" t="inlineStr"/>
+      <c r="Y3" t="n">
+        <v>569</v>
+      </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="n">
         <v>569</v>
       </c>
       <c r="AD3" t="n">
         <v>569</v>
       </c>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH3" t="inlineStr"/>
       <c r="AI3" t="n">
         <v>569</v>
       </c>
@@ -962,10 +969,10 @@
       <c r="AM3" t="n">
         <v>569</v>
       </c>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO3" t="inlineStr"/>
       <c r="AP3" t="n">
         <v>569</v>
       </c>
@@ -982,6 +989,9 @@
         <v>569</v>
       </c>
       <c r="AU3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1078,10 +1088,10 @@
       <c r="AD4" t="n">
         <v>299</v>
       </c>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="n">
         <v>299</v>
       </c>
@@ -1103,10 +1113,10 @@
       <c r="AM4" t="n">
         <v>299</v>
       </c>
-      <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO4" t="inlineStr"/>
       <c r="AP4" t="n">
         <v>299</v>
       </c>
@@ -1123,6 +1133,9 @@
         <v>299</v>
       </c>
       <c r="AU4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1147,10 +1160,10 @@
       <c r="F5" t="n">
         <v>569</v>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
-        <v>569</v>
-      </c>
+      <c r="G5" t="n">
+        <v>569</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>569</v>
       </c>
@@ -1244,10 +1257,10 @@
       <c r="AM5" t="n">
         <v>569</v>
       </c>
-      <c r="AN5" t="inlineStr"/>
-      <c r="AO5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO5" t="inlineStr"/>
       <c r="AP5" t="n">
         <v>569</v>
       </c>
@@ -1264,6 +1277,9 @@
         <v>569</v>
       </c>
       <c r="AU5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1273,9 +1289,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>499</v>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
         <v>499</v>
       </c>
@@ -1363,10 +1377,10 @@
       <c r="AE6" t="n">
         <v>499</v>
       </c>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="n">
         <v>499</v>
       </c>
@@ -1385,10 +1399,10 @@
       <c r="AM6" t="n">
         <v>499</v>
       </c>
-      <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AN6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO6" t="inlineStr"/>
       <c r="AP6" t="n">
         <v>499</v>
       </c>
@@ -1405,6 +1419,9 @@
         <v>499</v>
       </c>
       <c r="AU6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1414,9 +1431,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>569</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
         <v>569</v>
       </c>
@@ -1501,12 +1516,12 @@
       <c r="AD7" t="n">
         <v>569</v>
       </c>
-      <c r="AE7" t="inlineStr"/>
+      <c r="AE7" t="n">
+        <v>569</v>
+      </c>
       <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
-      <c r="AH7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH7" t="inlineStr"/>
       <c r="AI7" t="n">
         <v>569</v>
       </c>
@@ -1522,10 +1537,10 @@
       <c r="AM7" t="n">
         <v>569</v>
       </c>
-      <c r="AN7" t="inlineStr"/>
-      <c r="AO7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO7" t="inlineStr"/>
       <c r="AP7" t="n">
         <v>569</v>
       </c>
@@ -1542,6 +1557,9 @@
         <v>569</v>
       </c>
       <c r="AU7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1551,9 +1569,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
         <v>929</v>
       </c>
@@ -1638,14 +1654,14 @@
       <c r="AD8" t="n">
         <v>929</v>
       </c>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH8" t="inlineStr"/>
       <c r="AI8" t="n">
         <v>929</v>
       </c>
@@ -1661,10 +1677,10 @@
       <c r="AM8" t="n">
         <v>929</v>
       </c>
-      <c r="AN8" t="inlineStr"/>
-      <c r="AO8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO8" t="inlineStr"/>
       <c r="AP8" t="n">
         <v>929</v>
       </c>
@@ -1681,6 +1697,9 @@
         <v>929</v>
       </c>
       <c r="AU8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1777,10 +1796,10 @@
       <c r="AD9" t="n">
         <v>299</v>
       </c>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="n">
         <v>299</v>
       </c>
@@ -1802,10 +1821,10 @@
       <c r="AM9" t="n">
         <v>299</v>
       </c>
-      <c r="AN9" t="inlineStr"/>
-      <c r="AO9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO9" t="inlineStr"/>
       <c r="AP9" t="n">
         <v>299</v>
       </c>
@@ -1822,6 +1841,9 @@
         <v>299</v>
       </c>
       <c r="AU9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1831,9 +1853,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
         <v>299</v>
       </c>
@@ -1888,10 +1908,10 @@
       <c r="T10" t="n">
         <v>299</v>
       </c>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="n">
-        <v>299</v>
-      </c>
+      <c r="U10" t="n">
+        <v>299</v>
+      </c>
+      <c r="V10" t="inlineStr"/>
       <c r="W10" t="n">
         <v>299</v>
       </c>
@@ -1916,14 +1936,14 @@
       <c r="AD10" t="n">
         <v>299</v>
       </c>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH10" t="inlineStr"/>
       <c r="AI10" t="n">
         <v>299</v>
       </c>
@@ -1939,10 +1959,10 @@
       <c r="AM10" t="n">
         <v>299</v>
       </c>
-      <c r="AN10" t="inlineStr"/>
-      <c r="AO10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO10" t="inlineStr"/>
       <c r="AP10" t="n">
         <v>299</v>
       </c>
@@ -1959,6 +1979,9 @@
         <v>299</v>
       </c>
       <c r="AU10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2058,10 +2081,10 @@
       <c r="AE11" t="n">
         <v>2997</v>
       </c>
-      <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="n">
+      <c r="AF11" t="n">
         <v>2997</v>
       </c>
+      <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="n">
         <v>2997</v>
       </c>
@@ -2075,15 +2098,15 @@
         <v>2997</v>
       </c>
       <c r="AL11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AM11" t="n">
         <v>929</v>
       </c>
-      <c r="AN11" t="inlineStr"/>
-      <c r="AO11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO11" t="inlineStr"/>
       <c r="AP11" t="n">
         <v>929</v>
       </c>
@@ -2100,6 +2123,9 @@
         <v>929</v>
       </c>
       <c r="AU11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2202,10 +2228,10 @@
       <c r="AF12" t="n">
         <v>569</v>
       </c>
-      <c r="AG12" t="inlineStr"/>
-      <c r="AH12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH12" t="inlineStr"/>
       <c r="AI12" t="n">
         <v>569</v>
       </c>
@@ -2221,10 +2247,10 @@
       <c r="AM12" t="n">
         <v>569</v>
       </c>
-      <c r="AN12" t="inlineStr"/>
-      <c r="AO12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO12" t="inlineStr"/>
       <c r="AP12" t="n">
         <v>569</v>
       </c>
@@ -2241,6 +2267,9 @@
         <v>569</v>
       </c>
       <c r="AU12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2286,10 +2315,10 @@
       <c r="M13" t="n">
         <v>569</v>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="n">
-        <v>569</v>
-      </c>
+      <c r="N13" t="n">
+        <v>569</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
         <v>569</v>
       </c>
@@ -2335,14 +2364,14 @@
       <c r="AD13" t="n">
         <v>569</v>
       </c>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH13" t="inlineStr"/>
       <c r="AI13" t="n">
         <v>569</v>
       </c>
@@ -2358,24 +2387,27 @@
       <c r="AM13" t="n">
         <v>569</v>
       </c>
-      <c r="AN13" t="inlineStr"/>
-      <c r="AO13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO13" t="inlineStr"/>
       <c r="AP13" t="n">
         <v>569</v>
       </c>
       <c r="AQ13" t="n">
         <v>569</v>
       </c>
-      <c r="AR13" t="inlineStr"/>
-      <c r="AS13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AR13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS13" t="inlineStr"/>
       <c r="AT13" t="n">
         <v>569</v>
       </c>
       <c r="AU13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2385,9 +2417,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>794</v>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
         <v>794</v>
       </c>
@@ -2442,10 +2472,10 @@
       <c r="T14" t="n">
         <v>794</v>
       </c>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="n">
+      <c r="U14" t="n">
         <v>794</v>
       </c>
+      <c r="V14" t="inlineStr"/>
       <c r="W14" t="n">
         <v>794</v>
       </c>
@@ -2453,7 +2483,7 @@
         <v>794</v>
       </c>
       <c r="Y14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="Z14" t="n">
         <v>499</v>
@@ -2470,11 +2500,11 @@
       <c r="AD14" t="n">
         <v>499</v>
       </c>
-      <c r="AE14" t="inlineStr"/>
+      <c r="AE14" t="n">
+        <v>499</v>
+      </c>
       <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="n">
         <v>499</v>
       </c>
@@ -2515,6 +2545,9 @@
         <v>499</v>
       </c>
       <c r="AU14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2524,9 +2557,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>499</v>
-      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
         <v>499</v>
       </c>
@@ -2617,10 +2648,10 @@
       <c r="AF15" t="n">
         <v>499</v>
       </c>
-      <c r="AG15" t="inlineStr"/>
-      <c r="AH15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH15" t="inlineStr"/>
       <c r="AI15" t="n">
         <v>499</v>
       </c>
@@ -2630,14 +2661,14 @@
       <c r="AK15" t="n">
         <v>499</v>
       </c>
-      <c r="AL15" t="inlineStr"/>
-      <c r="AM15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AN15" t="inlineStr"/>
-      <c r="AO15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AL15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO15" t="inlineStr"/>
       <c r="AP15" t="n">
         <v>499</v>
       </c>
@@ -2654,6 +2685,9 @@
         <v>499</v>
       </c>
       <c r="AU15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2741,17 +2775,17 @@
       <c r="AA16" t="n">
         <v>299</v>
       </c>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="n">
         <v>299</v>
       </c>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF16" t="inlineStr"/>
       <c r="AG16" t="n">
         <v>299</v>
       </c>
@@ -2773,10 +2807,10 @@
       <c r="AM16" t="n">
         <v>299</v>
       </c>
-      <c r="AN16" t="inlineStr"/>
-      <c r="AO16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO16" t="inlineStr"/>
       <c r="AP16" t="n">
         <v>299</v>
       </c>
@@ -2793,6 +2827,9 @@
         <v>299</v>
       </c>
       <c r="AU16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2895,10 +2932,10 @@
       <c r="AF17" t="n">
         <v>929</v>
       </c>
-      <c r="AG17" t="inlineStr"/>
-      <c r="AH17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH17" t="inlineStr"/>
       <c r="AI17" t="n">
         <v>929</v>
       </c>
@@ -2914,10 +2951,10 @@
       <c r="AM17" t="n">
         <v>929</v>
       </c>
-      <c r="AN17" t="inlineStr"/>
-      <c r="AO17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO17" t="inlineStr"/>
       <c r="AP17" t="n">
         <v>929</v>
       </c>
@@ -2934,6 +2971,9 @@
         <v>929</v>
       </c>
       <c r="AU17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2943,9 +2983,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>499</v>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="n">
         <v>499</v>
       </c>
@@ -3033,11 +3071,11 @@
       <c r="AE18" t="n">
         <v>499</v>
       </c>
-      <c r="AF18" t="inlineStr"/>
+      <c r="AF18" t="n">
+        <v>499</v>
+      </c>
       <c r="AG18" t="inlineStr"/>
-      <c r="AH18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AH18" t="inlineStr"/>
       <c r="AI18" t="n">
         <v>499</v>
       </c>
@@ -3053,10 +3091,10 @@
       <c r="AM18" t="n">
         <v>499</v>
       </c>
-      <c r="AN18" t="inlineStr"/>
-      <c r="AO18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AN18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO18" t="inlineStr"/>
       <c r="AP18" t="n">
         <v>499</v>
       </c>
@@ -3073,6 +3111,9 @@
         <v>499</v>
       </c>
       <c r="AU18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3082,9 +3123,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
         <v>1299</v>
       </c>
@@ -3164,7 +3203,7 @@
         <v>1299</v>
       </c>
       <c r="AC19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AD19" t="n">
         <v>1497</v>
@@ -3172,13 +3211,13 @@
       <c r="AE19" t="n">
         <v>1497</v>
       </c>
-      <c r="AF19" t="inlineStr"/>
+      <c r="AF19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AG19" t="inlineStr"/>
-      <c r="AH19" t="n">
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="n">
         <v>465</v>
-      </c>
-      <c r="AI19" t="n">
-        <v>1497</v>
       </c>
       <c r="AJ19" t="n">
         <v>1497</v>
@@ -3214,6 +3253,9 @@
         <v>1497</v>
       </c>
       <c r="AU19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AV19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3337,10 +3379,10 @@
       <c r="AM20" t="n">
         <v>929</v>
       </c>
-      <c r="AN20" t="inlineStr"/>
-      <c r="AO20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO20" t="inlineStr"/>
       <c r="AP20" t="n">
         <v>929</v>
       </c>
@@ -3357,6 +3399,9 @@
         <v>929</v>
       </c>
       <c r="AU20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3369,10 +3414,10 @@
       <c r="B21" t="n">
         <v>499</v>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
-        <v>499</v>
-      </c>
+      <c r="C21" t="n">
+        <v>499</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
         <v>499</v>
       </c>
@@ -3427,10 +3472,10 @@
       <c r="V21" t="n">
         <v>499</v>
       </c>
-      <c r="W21" t="inlineStr"/>
-      <c r="X21" t="n">
-        <v>499</v>
-      </c>
+      <c r="W21" t="n">
+        <v>499</v>
+      </c>
+      <c r="X21" t="inlineStr"/>
       <c r="Y21" t="n">
         <v>499</v>
       </c>
@@ -3455,10 +3500,10 @@
       <c r="AF21" t="n">
         <v>499</v>
       </c>
-      <c r="AG21" t="inlineStr"/>
-      <c r="AH21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH21" t="inlineStr"/>
       <c r="AI21" t="n">
         <v>499</v>
       </c>
@@ -3496,6 +3541,9 @@
         <v>499</v>
       </c>
       <c r="AU21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3592,14 +3640,14 @@
       <c r="AD22" t="n">
         <v>299</v>
       </c>
-      <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AG22" t="inlineStr"/>
-      <c r="AH22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH22" t="inlineStr"/>
       <c r="AI22" t="n">
         <v>299</v>
       </c>
@@ -3615,10 +3663,10 @@
       <c r="AM22" t="n">
         <v>299</v>
       </c>
-      <c r="AN22" t="inlineStr"/>
-      <c r="AO22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO22" t="inlineStr"/>
       <c r="AP22" t="n">
         <v>299</v>
       </c>
@@ -3635,6 +3683,9 @@
         <v>299</v>
       </c>
       <c r="AU22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3644,9 +3695,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
         <v>1299</v>
       </c>
@@ -3734,11 +3783,11 @@
       <c r="AE23" t="n">
         <v>1299</v>
       </c>
-      <c r="AF23" t="inlineStr"/>
+      <c r="AF23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AG23" t="inlineStr"/>
-      <c r="AH23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="n">
         <v>1299</v>
       </c>
@@ -3754,10 +3803,10 @@
       <c r="AM23" t="n">
         <v>1299</v>
       </c>
-      <c r="AN23" t="inlineStr"/>
-      <c r="AO23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AN23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AO23" t="inlineStr"/>
       <c r="AP23" t="n">
         <v>1299</v>
       </c>
@@ -3774,6 +3823,9 @@
         <v>1299</v>
       </c>
       <c r="AU23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AV23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3783,9 +3835,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>929</v>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="n">
         <v>929</v>
       </c>
@@ -3870,11 +3920,11 @@
       <c r="AD24" t="n">
         <v>929</v>
       </c>
-      <c r="AE24" t="inlineStr"/>
+      <c r="AE24" t="n">
+        <v>929</v>
+      </c>
       <c r="AF24" t="inlineStr"/>
-      <c r="AG24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="n">
         <v>929</v>
       </c>
@@ -3893,10 +3943,10 @@
       <c r="AM24" t="n">
         <v>929</v>
       </c>
-      <c r="AN24" t="inlineStr"/>
-      <c r="AO24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO24" t="inlineStr"/>
       <c r="AP24" t="n">
         <v>929</v>
       </c>
@@ -3913,6 +3963,9 @@
         <v>929</v>
       </c>
       <c r="AU24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3922,9 +3975,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>929</v>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
         <v>929</v>
       </c>
@@ -3934,10 +3985,10 @@
       <c r="E25" t="n">
         <v>929</v>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
-        <v>929</v>
-      </c>
+      <c r="F25" t="n">
+        <v>929</v>
+      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
         <v>929</v>
       </c>
@@ -4007,11 +4058,11 @@
       <c r="AD25" t="n">
         <v>929</v>
       </c>
-      <c r="AE25" t="inlineStr"/>
+      <c r="AE25" t="n">
+        <v>929</v>
+      </c>
       <c r="AF25" t="inlineStr"/>
-      <c r="AG25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG25" t="inlineStr"/>
       <c r="AH25" t="n">
         <v>929</v>
       </c>
@@ -4030,10 +4081,10 @@
       <c r="AM25" t="n">
         <v>929</v>
       </c>
-      <c r="AN25" t="inlineStr"/>
-      <c r="AO25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO25" t="inlineStr"/>
       <c r="AP25" t="n">
         <v>929</v>
       </c>
@@ -4050,6 +4101,9 @@
         <v>929</v>
       </c>
       <c r="AU25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4068,10 +4122,10 @@
       <c r="D26" t="n">
         <v>1299</v>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
         <v>1299</v>
       </c>
@@ -4144,14 +4198,14 @@
       <c r="AD26" t="n">
         <v>1299</v>
       </c>
-      <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AG26" t="inlineStr"/>
-      <c r="AH26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AE26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AH26" t="inlineStr"/>
       <c r="AI26" t="n">
         <v>1299</v>
       </c>
@@ -4167,10 +4221,10 @@
       <c r="AM26" t="n">
         <v>1299</v>
       </c>
-      <c r="AN26" t="inlineStr"/>
-      <c r="AO26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AN26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AO26" t="inlineStr"/>
       <c r="AP26" t="n">
         <v>1299</v>
       </c>
@@ -4187,6 +4241,9 @@
         <v>1299</v>
       </c>
       <c r="AU26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AV26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 14:47
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV26"/>
+  <dimension ref="A1:AW26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,7 @@
     <col width="21" customWidth="1" min="46" max="46"/>
     <col width="21" customWidth="1" min="47" max="47"/>
     <col width="21" customWidth="1" min="48" max="48"/>
+    <col width="21" customWidth="1" min="49" max="49"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -491,235 +492,240 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 20:12</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -806,10 +812,10 @@
       <c r="Z2" t="n">
         <v>929</v>
       </c>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AA2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="n">
         <v>929</v>
       </c>
@@ -822,25 +828,25 @@
       <c r="AF2" t="n">
         <v>929</v>
       </c>
-      <c r="AG2" t="inlineStr"/>
+      <c r="AG2" t="n">
+        <v>929</v>
+      </c>
       <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="n">
         <v>929</v>
       </c>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="n">
         <v>929</v>
       </c>
-      <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="n">
         <v>929</v>
       </c>
@@ -860,6 +866,9 @@
         <v>929</v>
       </c>
       <c r="AV2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -869,10 +878,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="n">
+        <v>569</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>569</v>
       </c>
@@ -891,10 +900,10 @@
       <c r="I3" t="n">
         <v>569</v>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>569</v>
-      </c>
+      <c r="J3" t="n">
+        <v>569</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
         <v>569</v>
       </c>
@@ -937,26 +946,26 @@
       <c r="Y3" t="n">
         <v>569</v>
       </c>
-      <c r="Z3" t="inlineStr"/>
+      <c r="Z3" t="n">
+        <v>569</v>
+      </c>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="n">
         <v>569</v>
       </c>
       <c r="AE3" t="n">
         <v>569</v>
       </c>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="n">
         <v>569</v>
       </c>
@@ -972,10 +981,10 @@
       <c r="AN3" t="n">
         <v>569</v>
       </c>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP3" t="inlineStr"/>
       <c r="AQ3" t="n">
         <v>569</v>
       </c>
@@ -992,6 +1001,9 @@
         <v>569</v>
       </c>
       <c r="AV3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1091,10 +1103,10 @@
       <c r="AE4" t="n">
         <v>299</v>
       </c>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="n">
         <v>299</v>
       </c>
@@ -1116,10 +1128,10 @@
       <c r="AN4" t="n">
         <v>299</v>
       </c>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP4" t="inlineStr"/>
       <c r="AQ4" t="n">
         <v>299</v>
       </c>
@@ -1136,6 +1148,9 @@
         <v>299</v>
       </c>
       <c r="AV4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1163,10 +1178,10 @@
       <c r="G5" t="n">
         <v>569</v>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>569</v>
-      </c>
+      <c r="H5" t="n">
+        <v>569</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="n">
         <v>569</v>
       </c>
@@ -1260,10 +1275,10 @@
       <c r="AN5" t="n">
         <v>569</v>
       </c>
-      <c r="AO5" t="inlineStr"/>
-      <c r="AP5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP5" t="inlineStr"/>
       <c r="AQ5" t="n">
         <v>569</v>
       </c>
@@ -1280,6 +1295,9 @@
         <v>569</v>
       </c>
       <c r="AV5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1290,9 +1308,7 @@
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="n">
-        <v>499</v>
-      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
         <v>499</v>
       </c>
@@ -1380,10 +1396,10 @@
       <c r="AF6" t="n">
         <v>499</v>
       </c>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH6" t="inlineStr"/>
       <c r="AI6" t="n">
         <v>499</v>
       </c>
@@ -1402,10 +1418,10 @@
       <c r="AN6" t="n">
         <v>499</v>
       </c>
-      <c r="AO6" t="inlineStr"/>
-      <c r="AP6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AO6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP6" t="inlineStr"/>
       <c r="AQ6" t="n">
         <v>499</v>
       </c>
@@ -1422,6 +1438,9 @@
         <v>499</v>
       </c>
       <c r="AV6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1431,10 +1450,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="n">
-        <v>569</v>
-      </c>
+      <c r="B7" t="n">
+        <v>569</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
         <v>569</v>
       </c>
@@ -1519,12 +1538,12 @@
       <c r="AE7" t="n">
         <v>569</v>
       </c>
-      <c r="AF7" t="inlineStr"/>
+      <c r="AF7" t="n">
+        <v>569</v>
+      </c>
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr"/>
-      <c r="AI7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI7" t="inlineStr"/>
       <c r="AJ7" t="n">
         <v>569</v>
       </c>
@@ -1540,10 +1559,10 @@
       <c r="AN7" t="n">
         <v>569</v>
       </c>
-      <c r="AO7" t="inlineStr"/>
-      <c r="AP7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP7" t="inlineStr"/>
       <c r="AQ7" t="n">
         <v>569</v>
       </c>
@@ -1560,6 +1579,9 @@
         <v>569</v>
       </c>
       <c r="AV7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1569,10 +1591,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="n">
+        <v>929</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>929</v>
       </c>
@@ -1657,14 +1679,14 @@
       <c r="AE8" t="n">
         <v>929</v>
       </c>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AH8" t="inlineStr"/>
-      <c r="AI8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI8" t="inlineStr"/>
       <c r="AJ8" t="n">
         <v>929</v>
       </c>
@@ -1680,10 +1702,10 @@
       <c r="AN8" t="n">
         <v>929</v>
       </c>
-      <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP8" t="inlineStr"/>
       <c r="AQ8" t="n">
         <v>929</v>
       </c>
@@ -1700,6 +1722,9 @@
         <v>929</v>
       </c>
       <c r="AV8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1709,9 +1734,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>299</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
         <v>299</v>
       </c>
@@ -1799,10 +1822,10 @@
       <c r="AE9" t="n">
         <v>299</v>
       </c>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="n">
         <v>299</v>
       </c>
@@ -1824,10 +1847,10 @@
       <c r="AN9" t="n">
         <v>299</v>
       </c>
-      <c r="AO9" t="inlineStr"/>
-      <c r="AP9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP9" t="inlineStr"/>
       <c r="AQ9" t="n">
         <v>299</v>
       </c>
@@ -1844,6 +1867,9 @@
         <v>299</v>
       </c>
       <c r="AV9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1854,9 +1880,7 @@
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="n">
-        <v>299</v>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>299</v>
       </c>
@@ -1911,10 +1935,10 @@
       <c r="U10" t="n">
         <v>299</v>
       </c>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="n">
-        <v>299</v>
-      </c>
+      <c r="V10" t="n">
+        <v>299</v>
+      </c>
+      <c r="W10" t="inlineStr"/>
       <c r="X10" t="n">
         <v>299</v>
       </c>
@@ -1939,14 +1963,14 @@
       <c r="AE10" t="n">
         <v>299</v>
       </c>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AH10" t="inlineStr"/>
-      <c r="AI10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI10" t="inlineStr"/>
       <c r="AJ10" t="n">
         <v>299</v>
       </c>
@@ -1962,10 +1986,10 @@
       <c r="AN10" t="n">
         <v>299</v>
       </c>
-      <c r="AO10" t="inlineStr"/>
-      <c r="AP10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP10" t="inlineStr"/>
       <c r="AQ10" t="n">
         <v>299</v>
       </c>
@@ -1982,6 +2006,9 @@
         <v>299</v>
       </c>
       <c r="AV10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2084,10 +2111,10 @@
       <c r="AF11" t="n">
         <v>2997</v>
       </c>
-      <c r="AG11" t="inlineStr"/>
-      <c r="AH11" t="n">
+      <c r="AG11" t="n">
         <v>2997</v>
       </c>
+      <c r="AH11" t="inlineStr"/>
       <c r="AI11" t="n">
         <v>2997</v>
       </c>
@@ -2101,15 +2128,15 @@
         <v>2997</v>
       </c>
       <c r="AM11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AN11" t="n">
         <v>929</v>
       </c>
-      <c r="AO11" t="inlineStr"/>
-      <c r="AP11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP11" t="inlineStr"/>
       <c r="AQ11" t="n">
         <v>929</v>
       </c>
@@ -2126,6 +2153,9 @@
         <v>929</v>
       </c>
       <c r="AV11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2231,10 +2261,10 @@
       <c r="AG12" t="n">
         <v>569</v>
       </c>
-      <c r="AH12" t="inlineStr"/>
-      <c r="AI12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI12" t="inlineStr"/>
       <c r="AJ12" t="n">
         <v>569</v>
       </c>
@@ -2250,10 +2280,10 @@
       <c r="AN12" t="n">
         <v>569</v>
       </c>
-      <c r="AO12" t="inlineStr"/>
-      <c r="AP12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP12" t="inlineStr"/>
       <c r="AQ12" t="n">
         <v>569</v>
       </c>
@@ -2270,6 +2300,9 @@
         <v>569</v>
       </c>
       <c r="AV12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2279,9 +2312,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
         <v>569</v>
       </c>
@@ -2318,10 +2349,10 @@
       <c r="N13" t="n">
         <v>569</v>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="n">
-        <v>569</v>
-      </c>
+      <c r="O13" t="n">
+        <v>569</v>
+      </c>
+      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="n">
         <v>569</v>
       </c>
@@ -2367,14 +2398,14 @@
       <c r="AE13" t="n">
         <v>569</v>
       </c>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI13" t="inlineStr"/>
       <c r="AJ13" t="n">
         <v>569</v>
       </c>
@@ -2390,24 +2421,27 @@
       <c r="AN13" t="n">
         <v>569</v>
       </c>
-      <c r="AO13" t="inlineStr"/>
-      <c r="AP13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP13" t="inlineStr"/>
       <c r="AQ13" t="n">
         <v>569</v>
       </c>
       <c r="AR13" t="n">
         <v>569</v>
       </c>
-      <c r="AS13" t="inlineStr"/>
-      <c r="AT13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AS13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT13" t="inlineStr"/>
       <c r="AU13" t="n">
         <v>569</v>
       </c>
       <c r="AV13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2417,10 +2451,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="n">
+      <c r="B14" t="n">
         <v>794</v>
       </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
         <v>794</v>
       </c>
@@ -2475,10 +2509,10 @@
       <c r="U14" t="n">
         <v>794</v>
       </c>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="n">
+      <c r="V14" t="n">
         <v>794</v>
       </c>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="n">
         <v>794</v>
       </c>
@@ -2486,7 +2520,7 @@
         <v>794</v>
       </c>
       <c r="Z14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AA14" t="n">
         <v>499</v>
@@ -2503,11 +2537,11 @@
       <c r="AE14" t="n">
         <v>499</v>
       </c>
-      <c r="AF14" t="inlineStr"/>
+      <c r="AF14" t="n">
+        <v>499</v>
+      </c>
       <c r="AG14" t="inlineStr"/>
-      <c r="AH14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AH14" t="inlineStr"/>
       <c r="AI14" t="n">
         <v>499</v>
       </c>
@@ -2548,6 +2582,9 @@
         <v>499</v>
       </c>
       <c r="AV14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2558,9 +2595,7 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>499</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
         <v>499</v>
       </c>
@@ -2651,10 +2686,10 @@
       <c r="AG15" t="n">
         <v>499</v>
       </c>
-      <c r="AH15" t="inlineStr"/>
-      <c r="AI15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AH15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI15" t="inlineStr"/>
       <c r="AJ15" t="n">
         <v>499</v>
       </c>
@@ -2664,14 +2699,14 @@
       <c r="AL15" t="n">
         <v>499</v>
       </c>
-      <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AO15" t="inlineStr"/>
-      <c r="AP15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AM15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN15" t="inlineStr"/>
+      <c r="AO15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP15" t="inlineStr"/>
       <c r="AQ15" t="n">
         <v>499</v>
       </c>
@@ -2688,6 +2723,9 @@
         <v>499</v>
       </c>
       <c r="AV15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2697,9 +2735,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
         <v>299</v>
       </c>
@@ -2778,17 +2814,17 @@
       <c r="AB16" t="n">
         <v>299</v>
       </c>
-      <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="n">
         <v>299</v>
       </c>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="n">
         <v>299</v>
       </c>
@@ -2810,10 +2846,10 @@
       <c r="AN16" t="n">
         <v>299</v>
       </c>
-      <c r="AO16" t="inlineStr"/>
-      <c r="AP16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP16" t="inlineStr"/>
       <c r="AQ16" t="n">
         <v>299</v>
       </c>
@@ -2830,6 +2866,9 @@
         <v>299</v>
       </c>
       <c r="AV16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2935,10 +2974,10 @@
       <c r="AG17" t="n">
         <v>929</v>
       </c>
-      <c r="AH17" t="inlineStr"/>
-      <c r="AI17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI17" t="inlineStr"/>
       <c r="AJ17" t="n">
         <v>929</v>
       </c>
@@ -2954,10 +2993,10 @@
       <c r="AN17" t="n">
         <v>929</v>
       </c>
-      <c r="AO17" t="inlineStr"/>
-      <c r="AP17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP17" t="inlineStr"/>
       <c r="AQ17" t="n">
         <v>929</v>
       </c>
@@ -2974,6 +3013,9 @@
         <v>929</v>
       </c>
       <c r="AV17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2984,9 +3026,7 @@
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="n">
-        <v>499</v>
-      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
         <v>499</v>
       </c>
@@ -3074,11 +3114,11 @@
       <c r="AF18" t="n">
         <v>499</v>
       </c>
-      <c r="AG18" t="inlineStr"/>
+      <c r="AG18" t="n">
+        <v>499</v>
+      </c>
       <c r="AH18" t="inlineStr"/>
-      <c r="AI18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AI18" t="inlineStr"/>
       <c r="AJ18" t="n">
         <v>499</v>
       </c>
@@ -3094,10 +3134,10 @@
       <c r="AN18" t="n">
         <v>499</v>
       </c>
-      <c r="AO18" t="inlineStr"/>
-      <c r="AP18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AO18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP18" t="inlineStr"/>
       <c r="AQ18" t="n">
         <v>499</v>
       </c>
@@ -3114,6 +3154,9 @@
         <v>499</v>
       </c>
       <c r="AV18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3123,10 +3166,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
         <v>1299</v>
       </c>
@@ -3206,7 +3249,7 @@
         <v>1299</v>
       </c>
       <c r="AD19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AE19" t="n">
         <v>1497</v>
@@ -3214,13 +3257,13 @@
       <c r="AF19" t="n">
         <v>1497</v>
       </c>
-      <c r="AG19" t="inlineStr"/>
+      <c r="AG19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AH19" t="inlineStr"/>
-      <c r="AI19" t="n">
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="n">
         <v>465</v>
-      </c>
-      <c r="AJ19" t="n">
-        <v>1497</v>
       </c>
       <c r="AK19" t="n">
         <v>1497</v>
@@ -3256,6 +3299,9 @@
         <v>1497</v>
       </c>
       <c r="AV19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AW19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3382,10 +3428,10 @@
       <c r="AN20" t="n">
         <v>929</v>
       </c>
-      <c r="AO20" t="inlineStr"/>
-      <c r="AP20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP20" t="inlineStr"/>
       <c r="AQ20" t="n">
         <v>929</v>
       </c>
@@ -3402,6 +3448,9 @@
         <v>929</v>
       </c>
       <c r="AV20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3411,16 +3460,14 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
         <v>499</v>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>499</v>
-      </c>
+      <c r="D21" t="n">
+        <v>499</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
         <v>499</v>
       </c>
@@ -3475,10 +3522,10 @@
       <c r="W21" t="n">
         <v>499</v>
       </c>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="n">
-        <v>499</v>
-      </c>
+      <c r="X21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="n">
         <v>499</v>
       </c>
@@ -3503,10 +3550,10 @@
       <c r="AG21" t="n">
         <v>499</v>
       </c>
-      <c r="AH21" t="inlineStr"/>
-      <c r="AI21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AH21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI21" t="inlineStr"/>
       <c r="AJ21" t="n">
         <v>499</v>
       </c>
@@ -3544,6 +3591,9 @@
         <v>499</v>
       </c>
       <c r="AV21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3643,14 +3693,14 @@
       <c r="AE22" t="n">
         <v>299</v>
       </c>
-      <c r="AF22" t="inlineStr"/>
-      <c r="AG22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AH22" t="inlineStr"/>
-      <c r="AI22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI22" t="inlineStr"/>
       <c r="AJ22" t="n">
         <v>299</v>
       </c>
@@ -3666,10 +3716,10 @@
       <c r="AN22" t="n">
         <v>299</v>
       </c>
-      <c r="AO22" t="inlineStr"/>
-      <c r="AP22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP22" t="inlineStr"/>
       <c r="AQ22" t="n">
         <v>299</v>
       </c>
@@ -3686,6 +3736,9 @@
         <v>299</v>
       </c>
       <c r="AV22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3696,9 +3749,7 @@
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
         <v>1299</v>
       </c>
@@ -3786,11 +3837,11 @@
       <c r="AF23" t="n">
         <v>1299</v>
       </c>
-      <c r="AG23" t="inlineStr"/>
+      <c r="AG23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AH23" t="inlineStr"/>
-      <c r="AI23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AI23" t="inlineStr"/>
       <c r="AJ23" t="n">
         <v>1299</v>
       </c>
@@ -3806,10 +3857,10 @@
       <c r="AN23" t="n">
         <v>1299</v>
       </c>
-      <c r="AO23" t="inlineStr"/>
-      <c r="AP23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AO23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AP23" t="inlineStr"/>
       <c r="AQ23" t="n">
         <v>1299</v>
       </c>
@@ -3826,6 +3877,9 @@
         <v>1299</v>
       </c>
       <c r="AV23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AW23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3836,9 +3890,7 @@
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="n">
-        <v>929</v>
-      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
         <v>929</v>
       </c>
@@ -3923,11 +3975,11 @@
       <c r="AE24" t="n">
         <v>929</v>
       </c>
-      <c r="AF24" t="inlineStr"/>
+      <c r="AF24" t="n">
+        <v>929</v>
+      </c>
       <c r="AG24" t="inlineStr"/>
-      <c r="AH24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="n">
         <v>929</v>
       </c>
@@ -3946,10 +3998,10 @@
       <c r="AN24" t="n">
         <v>929</v>
       </c>
-      <c r="AO24" t="inlineStr"/>
-      <c r="AP24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP24" t="inlineStr"/>
       <c r="AQ24" t="n">
         <v>929</v>
       </c>
@@ -3966,6 +4018,9 @@
         <v>929</v>
       </c>
       <c r="AV24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3976,9 +4031,7 @@
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="n">
-        <v>929</v>
-      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
         <v>929</v>
       </c>
@@ -3988,10 +4041,10 @@
       <c r="F25" t="n">
         <v>929</v>
       </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="n">
-        <v>929</v>
-      </c>
+      <c r="G25" t="n">
+        <v>929</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
         <v>929</v>
       </c>
@@ -4061,11 +4114,11 @@
       <c r="AE25" t="n">
         <v>929</v>
       </c>
-      <c r="AF25" t="inlineStr"/>
+      <c r="AF25" t="n">
+        <v>929</v>
+      </c>
       <c r="AG25" t="inlineStr"/>
-      <c r="AH25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH25" t="inlineStr"/>
       <c r="AI25" t="n">
         <v>929</v>
       </c>
@@ -4084,10 +4137,10 @@
       <c r="AN25" t="n">
         <v>929</v>
       </c>
-      <c r="AO25" t="inlineStr"/>
-      <c r="AP25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP25" t="inlineStr"/>
       <c r="AQ25" t="n">
         <v>929</v>
       </c>
@@ -4104,6 +4157,9 @@
         <v>929</v>
       </c>
       <c r="AV25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4113,9 +4169,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="n">
         <v>1299</v>
       </c>
@@ -4125,10 +4179,10 @@
       <c r="E26" t="n">
         <v>1299</v>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
         <v>1299</v>
       </c>
@@ -4201,14 +4255,14 @@
       <c r="AE26" t="n">
         <v>1299</v>
       </c>
-      <c r="AF26" t="inlineStr"/>
-      <c r="AG26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AH26" t="inlineStr"/>
-      <c r="AI26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AF26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AI26" t="inlineStr"/>
       <c r="AJ26" t="n">
         <v>1299</v>
       </c>
@@ -4224,10 +4278,10 @@
       <c r="AN26" t="n">
         <v>1299</v>
       </c>
-      <c r="AO26" t="inlineStr"/>
-      <c r="AP26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AO26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AP26" t="inlineStr"/>
       <c r="AQ26" t="n">
         <v>1299</v>
       </c>
@@ -4244,6 +4298,9 @@
         <v>1299</v>
       </c>
       <c r="AV26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AW26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 16:55
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW26"/>
+  <dimension ref="A1:AX26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,6 +482,7 @@
     <col width="21" customWidth="1" min="47" max="47"/>
     <col width="21" customWidth="1" min="48" max="48"/>
     <col width="21" customWidth="1" min="49" max="49"/>
+    <col width="21" customWidth="1" min="50" max="50"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -492,240 +493,245 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-24 22:22</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -815,10 +821,10 @@
       <c r="AA2" t="n">
         <v>929</v>
       </c>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AB2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="n">
         <v>929</v>
       </c>
@@ -831,25 +837,25 @@
       <c r="AG2" t="n">
         <v>929</v>
       </c>
-      <c r="AH2" t="inlineStr"/>
+      <c r="AH2" t="n">
+        <v>929</v>
+      </c>
       <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="n">
         <v>929</v>
       </c>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="n">
         <v>929</v>
       </c>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="n">
         <v>929</v>
       </c>
@@ -869,6 +875,9 @@
         <v>929</v>
       </c>
       <c r="AW2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -881,10 +890,10 @@
       <c r="B3" t="n">
         <v>569</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>569</v>
-      </c>
+      <c r="C3" t="n">
+        <v>569</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>569</v>
       </c>
@@ -903,10 +912,10 @@
       <c r="J3" t="n">
         <v>569</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
-        <v>569</v>
-      </c>
+      <c r="K3" t="n">
+        <v>569</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>569</v>
       </c>
@@ -949,26 +958,26 @@
       <c r="Z3" t="n">
         <v>569</v>
       </c>
-      <c r="AA3" t="inlineStr"/>
+      <c r="AA3" t="n">
+        <v>569</v>
+      </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="n">
         <v>569</v>
       </c>
       <c r="AF3" t="n">
         <v>569</v>
       </c>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="n">
         <v>569</v>
       </c>
@@ -984,10 +993,10 @@
       <c r="AO3" t="n">
         <v>569</v>
       </c>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ3" t="inlineStr"/>
       <c r="AR3" t="n">
         <v>569</v>
       </c>
@@ -1004,6 +1013,9 @@
         <v>569</v>
       </c>
       <c r="AW3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1106,10 +1118,10 @@
       <c r="AF4" t="n">
         <v>299</v>
       </c>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH4" t="inlineStr"/>
       <c r="AI4" t="n">
         <v>299</v>
       </c>
@@ -1131,10 +1143,10 @@
       <c r="AO4" t="n">
         <v>299</v>
       </c>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AP4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ4" t="inlineStr"/>
       <c r="AR4" t="n">
         <v>299</v>
       </c>
@@ -1151,6 +1163,9 @@
         <v>299</v>
       </c>
       <c r="AW4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1181,10 +1196,10 @@
       <c r="H5" t="n">
         <v>569</v>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="n">
-        <v>569</v>
-      </c>
+      <c r="I5" t="n">
+        <v>569</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
         <v>569</v>
       </c>
@@ -1278,10 +1293,10 @@
       <c r="AO5" t="n">
         <v>569</v>
       </c>
-      <c r="AP5" t="inlineStr"/>
-      <c r="AQ5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ5" t="inlineStr"/>
       <c r="AR5" t="n">
         <v>569</v>
       </c>
@@ -1298,6 +1313,9 @@
         <v>569</v>
       </c>
       <c r="AW5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1307,11 +1325,11 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>499</v>
+      </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="n">
-        <v>499</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>499</v>
       </c>
@@ -1399,10 +1417,10 @@
       <c r="AG6" t="n">
         <v>499</v>
       </c>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AH6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="n">
         <v>499</v>
       </c>
@@ -1421,10 +1439,10 @@
       <c r="AO6" t="n">
         <v>499</v>
       </c>
-      <c r="AP6" t="inlineStr"/>
-      <c r="AQ6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AP6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ6" t="inlineStr"/>
       <c r="AR6" t="n">
         <v>499</v>
       </c>
@@ -1441,6 +1459,9 @@
         <v>499</v>
       </c>
       <c r="AW6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AX6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1453,10 +1474,10 @@
       <c r="B7" t="n">
         <v>569</v>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
-        <v>569</v>
-      </c>
+      <c r="C7" t="n">
+        <v>569</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
         <v>569</v>
       </c>
@@ -1541,12 +1562,12 @@
       <c r="AF7" t="n">
         <v>569</v>
       </c>
-      <c r="AG7" t="inlineStr"/>
+      <c r="AG7" t="n">
+        <v>569</v>
+      </c>
       <c r="AH7" t="inlineStr"/>
       <c r="AI7" t="inlineStr"/>
-      <c r="AJ7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="n">
         <v>569</v>
       </c>
@@ -1562,10 +1583,10 @@
       <c r="AO7" t="n">
         <v>569</v>
       </c>
-      <c r="AP7" t="inlineStr"/>
-      <c r="AQ7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ7" t="inlineStr"/>
       <c r="AR7" t="n">
         <v>569</v>
       </c>
@@ -1582,6 +1603,9 @@
         <v>569</v>
       </c>
       <c r="AW7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1594,10 +1618,10 @@
       <c r="B8" t="n">
         <v>929</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
-        <v>929</v>
-      </c>
+      <c r="C8" t="n">
+        <v>929</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>929</v>
       </c>
@@ -1682,14 +1706,14 @@
       <c r="AF8" t="n">
         <v>929</v>
       </c>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="n">
         <v>929</v>
       </c>
@@ -1705,10 +1729,10 @@
       <c r="AO8" t="n">
         <v>929</v>
       </c>
-      <c r="AP8" t="inlineStr"/>
-      <c r="AQ8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ8" t="inlineStr"/>
       <c r="AR8" t="n">
         <v>929</v>
       </c>
@@ -1725,6 +1749,9 @@
         <v>929</v>
       </c>
       <c r="AW8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1734,10 +1761,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="n">
-        <v>299</v>
-      </c>
+      <c r="B9" t="n">
+        <v>299</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>299</v>
       </c>
@@ -1825,10 +1852,10 @@
       <c r="AF9" t="n">
         <v>299</v>
       </c>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH9" t="inlineStr"/>
       <c r="AI9" t="n">
         <v>299</v>
       </c>
@@ -1850,10 +1877,10 @@
       <c r="AO9" t="n">
         <v>299</v>
       </c>
-      <c r="AP9" t="inlineStr"/>
-      <c r="AQ9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AP9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ9" t="inlineStr"/>
       <c r="AR9" t="n">
         <v>299</v>
       </c>
@@ -1870,6 +1897,9 @@
         <v>299</v>
       </c>
       <c r="AW9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1879,11 +1909,11 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>299</v>
+      </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>299</v>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
         <v>299</v>
       </c>
@@ -1938,10 +1968,10 @@
       <c r="V10" t="n">
         <v>299</v>
       </c>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="n">
-        <v>299</v>
-      </c>
+      <c r="W10" t="n">
+        <v>299</v>
+      </c>
+      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="n">
         <v>299</v>
       </c>
@@ -1966,14 +1996,14 @@
       <c r="AF10" t="n">
         <v>299</v>
       </c>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ10" t="inlineStr"/>
       <c r="AK10" t="n">
         <v>299</v>
       </c>
@@ -1989,10 +2019,10 @@
       <c r="AO10" t="n">
         <v>299</v>
       </c>
-      <c r="AP10" t="inlineStr"/>
-      <c r="AQ10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AP10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ10" t="inlineStr"/>
       <c r="AR10" t="n">
         <v>299</v>
       </c>
@@ -2009,6 +2039,9 @@
         <v>299</v>
       </c>
       <c r="AW10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2114,10 +2147,10 @@
       <c r="AG11" t="n">
         <v>2997</v>
       </c>
-      <c r="AH11" t="inlineStr"/>
-      <c r="AI11" t="n">
+      <c r="AH11" t="n">
         <v>2997</v>
       </c>
+      <c r="AI11" t="inlineStr"/>
       <c r="AJ11" t="n">
         <v>2997</v>
       </c>
@@ -2131,15 +2164,15 @@
         <v>2997</v>
       </c>
       <c r="AN11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AO11" t="n">
         <v>929</v>
       </c>
-      <c r="AP11" t="inlineStr"/>
-      <c r="AQ11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ11" t="inlineStr"/>
       <c r="AR11" t="n">
         <v>929</v>
       </c>
@@ -2156,6 +2189,9 @@
         <v>929</v>
       </c>
       <c r="AW11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2264,10 +2300,10 @@
       <c r="AH12" t="n">
         <v>569</v>
       </c>
-      <c r="AI12" t="inlineStr"/>
-      <c r="AJ12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ12" t="inlineStr"/>
       <c r="AK12" t="n">
         <v>569</v>
       </c>
@@ -2283,10 +2319,10 @@
       <c r="AO12" t="n">
         <v>569</v>
       </c>
-      <c r="AP12" t="inlineStr"/>
-      <c r="AQ12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ12" t="inlineStr"/>
       <c r="AR12" t="n">
         <v>569</v>
       </c>
@@ -2303,6 +2339,9 @@
         <v>569</v>
       </c>
       <c r="AW12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2312,10 +2351,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="n">
+        <v>569</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>569</v>
       </c>
@@ -2352,10 +2391,10 @@
       <c r="O13" t="n">
         <v>569</v>
       </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="n">
-        <v>569</v>
-      </c>
+      <c r="P13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
         <v>569</v>
       </c>
@@ -2401,14 +2440,14 @@
       <c r="AF13" t="n">
         <v>569</v>
       </c>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="n">
         <v>569</v>
       </c>
@@ -2424,24 +2463,27 @@
       <c r="AO13" t="n">
         <v>569</v>
       </c>
-      <c r="AP13" t="inlineStr"/>
-      <c r="AQ13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ13" t="inlineStr"/>
       <c r="AR13" t="n">
         <v>569</v>
       </c>
       <c r="AS13" t="n">
         <v>569</v>
       </c>
-      <c r="AT13" t="inlineStr"/>
-      <c r="AU13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AT13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU13" t="inlineStr"/>
       <c r="AV13" t="n">
         <v>569</v>
       </c>
       <c r="AW13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2454,10 +2496,10 @@
       <c r="B14" t="n">
         <v>794</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="n">
+      <c r="C14" t="n">
         <v>794</v>
       </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>794</v>
       </c>
@@ -2512,10 +2554,10 @@
       <c r="V14" t="n">
         <v>794</v>
       </c>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="n">
+      <c r="W14" t="n">
         <v>794</v>
       </c>
+      <c r="X14" t="inlineStr"/>
       <c r="Y14" t="n">
         <v>794</v>
       </c>
@@ -2523,7 +2565,7 @@
         <v>794</v>
       </c>
       <c r="AA14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AB14" t="n">
         <v>499</v>
@@ -2540,11 +2582,11 @@
       <c r="AF14" t="n">
         <v>499</v>
       </c>
-      <c r="AG14" t="inlineStr"/>
+      <c r="AG14" t="n">
+        <v>499</v>
+      </c>
       <c r="AH14" t="inlineStr"/>
-      <c r="AI14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AI14" t="inlineStr"/>
       <c r="AJ14" t="n">
         <v>499</v>
       </c>
@@ -2585,6 +2627,9 @@
         <v>499</v>
       </c>
       <c r="AW14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AX14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2594,11 +2639,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>499</v>
+      </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="n">
-        <v>499</v>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>499</v>
       </c>
@@ -2689,10 +2734,10 @@
       <c r="AH15" t="n">
         <v>499</v>
       </c>
-      <c r="AI15" t="inlineStr"/>
-      <c r="AJ15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AI15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ15" t="inlineStr"/>
       <c r="AK15" t="n">
         <v>499</v>
       </c>
@@ -2702,14 +2747,14 @@
       <c r="AM15" t="n">
         <v>499</v>
       </c>
-      <c r="AN15" t="inlineStr"/>
-      <c r="AO15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AP15" t="inlineStr"/>
-      <c r="AQ15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AN15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ15" t="inlineStr"/>
       <c r="AR15" t="n">
         <v>499</v>
       </c>
@@ -2726,6 +2771,9 @@
         <v>499</v>
       </c>
       <c r="AW15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AX15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2735,10 +2783,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="n">
+        <v>299</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
         <v>299</v>
       </c>
@@ -2817,17 +2865,17 @@
       <c r="AC16" t="n">
         <v>299</v>
       </c>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="n">
         <v>299</v>
       </c>
-      <c r="AG16" t="inlineStr"/>
-      <c r="AH16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH16" t="inlineStr"/>
       <c r="AI16" t="n">
         <v>299</v>
       </c>
@@ -2849,10 +2897,10 @@
       <c r="AO16" t="n">
         <v>299</v>
       </c>
-      <c r="AP16" t="inlineStr"/>
-      <c r="AQ16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AP16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ16" t="inlineStr"/>
       <c r="AR16" t="n">
         <v>299</v>
       </c>
@@ -2869,6 +2917,9 @@
         <v>299</v>
       </c>
       <c r="AW16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2977,10 +3028,10 @@
       <c r="AH17" t="n">
         <v>929</v>
       </c>
-      <c r="AI17" t="inlineStr"/>
-      <c r="AJ17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ17" t="inlineStr"/>
       <c r="AK17" t="n">
         <v>929</v>
       </c>
@@ -2996,10 +3047,10 @@
       <c r="AO17" t="n">
         <v>929</v>
       </c>
-      <c r="AP17" t="inlineStr"/>
-      <c r="AQ17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ17" t="inlineStr"/>
       <c r="AR17" t="n">
         <v>929</v>
       </c>
@@ -3016,6 +3067,9 @@
         <v>929</v>
       </c>
       <c r="AW17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3025,11 +3079,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="n">
+        <v>499</v>
+      </c>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="n">
-        <v>499</v>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>499</v>
       </c>
@@ -3117,11 +3171,11 @@
       <c r="AG18" t="n">
         <v>499</v>
       </c>
-      <c r="AH18" t="inlineStr"/>
+      <c r="AH18" t="n">
+        <v>499</v>
+      </c>
       <c r="AI18" t="inlineStr"/>
-      <c r="AJ18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AJ18" t="inlineStr"/>
       <c r="AK18" t="n">
         <v>499</v>
       </c>
@@ -3137,10 +3191,10 @@
       <c r="AO18" t="n">
         <v>499</v>
       </c>
-      <c r="AP18" t="inlineStr"/>
-      <c r="AQ18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AP18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ18" t="inlineStr"/>
       <c r="AR18" t="n">
         <v>499</v>
       </c>
@@ -3157,6 +3211,9 @@
         <v>499</v>
       </c>
       <c r="AW18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AX18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3169,10 +3226,10 @@
       <c r="B19" t="n">
         <v>1299</v>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>1299</v>
       </c>
@@ -3252,7 +3309,7 @@
         <v>1299</v>
       </c>
       <c r="AE19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AF19" t="n">
         <v>1497</v>
@@ -3260,13 +3317,13 @@
       <c r="AG19" t="n">
         <v>1497</v>
       </c>
-      <c r="AH19" t="inlineStr"/>
+      <c r="AH19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AI19" t="inlineStr"/>
-      <c r="AJ19" t="n">
+      <c r="AJ19" t="inlineStr"/>
+      <c r="AK19" t="n">
         <v>465</v>
-      </c>
-      <c r="AK19" t="n">
-        <v>1497</v>
       </c>
       <c r="AL19" t="n">
         <v>1497</v>
@@ -3302,6 +3359,9 @@
         <v>1497</v>
       </c>
       <c r="AW19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AX19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3431,10 +3491,10 @@
       <c r="AO20" t="n">
         <v>929</v>
       </c>
-      <c r="AP20" t="inlineStr"/>
-      <c r="AQ20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ20" t="inlineStr"/>
       <c r="AR20" t="n">
         <v>929</v>
       </c>
@@ -3451,6 +3511,9 @@
         <v>929</v>
       </c>
       <c r="AW20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3460,17 +3523,17 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="n">
+        <v>499</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>499</v>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>499</v>
-      </c>
+      <c r="E21" t="n">
+        <v>499</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
         <v>499</v>
       </c>
@@ -3525,10 +3588,10 @@
       <c r="X21" t="n">
         <v>499</v>
       </c>
-      <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="n">
-        <v>499</v>
-      </c>
+      <c r="Y21" t="n">
+        <v>499</v>
+      </c>
+      <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="n">
         <v>499</v>
       </c>
@@ -3553,10 +3616,10 @@
       <c r="AH21" t="n">
         <v>499</v>
       </c>
-      <c r="AI21" t="inlineStr"/>
-      <c r="AJ21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AI21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ21" t="inlineStr"/>
       <c r="AK21" t="n">
         <v>499</v>
       </c>
@@ -3594,6 +3657,9 @@
         <v>499</v>
       </c>
       <c r="AW21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AX21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3696,14 +3762,14 @@
       <c r="AF22" t="n">
         <v>299</v>
       </c>
-      <c r="AG22" t="inlineStr"/>
-      <c r="AH22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AI22" t="inlineStr"/>
-      <c r="AJ22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ22" t="inlineStr"/>
       <c r="AK22" t="n">
         <v>299</v>
       </c>
@@ -3719,10 +3785,10 @@
       <c r="AO22" t="n">
         <v>299</v>
       </c>
-      <c r="AP22" t="inlineStr"/>
-      <c r="AQ22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AP22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ22" t="inlineStr"/>
       <c r="AR22" t="n">
         <v>299</v>
       </c>
@@ -3739,6 +3805,9 @@
         <v>299</v>
       </c>
       <c r="AW22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3748,11 +3817,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="n">
+        <v>1299</v>
+      </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>1299</v>
       </c>
@@ -3840,11 +3909,11 @@
       <c r="AG23" t="n">
         <v>1299</v>
       </c>
-      <c r="AH23" t="inlineStr"/>
+      <c r="AH23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AI23" t="inlineStr"/>
-      <c r="AJ23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AJ23" t="inlineStr"/>
       <c r="AK23" t="n">
         <v>1299</v>
       </c>
@@ -3860,10 +3929,10 @@
       <c r="AO23" t="n">
         <v>1299</v>
       </c>
-      <c r="AP23" t="inlineStr"/>
-      <c r="AQ23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AP23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AQ23" t="inlineStr"/>
       <c r="AR23" t="n">
         <v>1299</v>
       </c>
@@ -3880,6 +3949,9 @@
         <v>1299</v>
       </c>
       <c r="AW23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AX23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3889,11 +3961,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 186 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="n">
+        <v>929</v>
+      </c>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="n">
-        <v>929</v>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>929</v>
       </c>
@@ -3978,11 +4050,11 @@
       <c r="AF24" t="n">
         <v>929</v>
       </c>
-      <c r="AG24" t="inlineStr"/>
+      <c r="AG24" t="n">
+        <v>929</v>
+      </c>
       <c r="AH24" t="inlineStr"/>
-      <c r="AI24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI24" t="inlineStr"/>
       <c r="AJ24" t="n">
         <v>929</v>
       </c>
@@ -4001,10 +4073,10 @@
       <c r="AO24" t="n">
         <v>929</v>
       </c>
-      <c r="AP24" t="inlineStr"/>
-      <c r="AQ24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ24" t="inlineStr"/>
       <c r="AR24" t="n">
         <v>929</v>
       </c>
@@ -4021,6 +4093,9 @@
         <v>929</v>
       </c>
       <c r="AW24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4030,11 +4105,11 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="n">
+        <v>929</v>
+      </c>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="n">
-        <v>929</v>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
         <v>929</v>
       </c>
@@ -4044,10 +4119,10 @@
       <c r="G25" t="n">
         <v>929</v>
       </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="n">
-        <v>929</v>
-      </c>
+      <c r="H25" t="n">
+        <v>929</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="n">
         <v>929</v>
       </c>
@@ -4117,11 +4192,11 @@
       <c r="AF25" t="n">
         <v>929</v>
       </c>
-      <c r="AG25" t="inlineStr"/>
+      <c r="AG25" t="n">
+        <v>929</v>
+      </c>
       <c r="AH25" t="inlineStr"/>
-      <c r="AI25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI25" t="inlineStr"/>
       <c r="AJ25" t="n">
         <v>929</v>
       </c>
@@ -4140,10 +4215,10 @@
       <c r="AO25" t="n">
         <v>929</v>
       </c>
-      <c r="AP25" t="inlineStr"/>
-      <c r="AQ25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ25" t="inlineStr"/>
       <c r="AR25" t="n">
         <v>929</v>
       </c>
@@ -4160,6 +4235,9 @@
         <v>929</v>
       </c>
       <c r="AW25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4169,10 +4247,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
         <v>1299</v>
       </c>
@@ -4182,10 +4260,10 @@
       <c r="F26" t="n">
         <v>1299</v>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
         <v>1299</v>
       </c>
@@ -4258,14 +4336,14 @@
       <c r="AF26" t="n">
         <v>1299</v>
       </c>
-      <c r="AG26" t="inlineStr"/>
-      <c r="AH26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AI26" t="inlineStr"/>
-      <c r="AJ26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AG26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AJ26" t="inlineStr"/>
       <c r="AK26" t="n">
         <v>1299</v>
       </c>
@@ -4281,10 +4359,10 @@
       <c r="AO26" t="n">
         <v>1299</v>
       </c>
-      <c r="AP26" t="inlineStr"/>
-      <c r="AQ26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AP26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AQ26" t="inlineStr"/>
       <c r="AR26" t="n">
         <v>1299</v>
       </c>
@@ -4301,6 +4379,9 @@
         <v>1299</v>
       </c>
       <c r="AW26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AX26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 19:02
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX26"/>
+  <dimension ref="A1:AY26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,7 @@
     <col width="21" customWidth="1" min="48" max="48"/>
     <col width="21" customWidth="1" min="49" max="49"/>
     <col width="21" customWidth="1" min="50" max="50"/>
+    <col width="21" customWidth="1" min="51" max="51"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -493,245 +494,250 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 00:27</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -824,10 +830,10 @@
       <c r="AB2" t="n">
         <v>929</v>
       </c>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AC2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="n">
         <v>929</v>
       </c>
@@ -840,25 +846,25 @@
       <c r="AH2" t="n">
         <v>929</v>
       </c>
-      <c r="AI2" t="inlineStr"/>
+      <c r="AI2" t="n">
+        <v>929</v>
+      </c>
       <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="n">
         <v>929</v>
       </c>
-      <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN2" t="inlineStr"/>
       <c r="AO2" t="n">
         <v>929</v>
       </c>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="n">
         <v>929</v>
       </c>
@@ -878,6 +884,9 @@
         <v>929</v>
       </c>
       <c r="AX2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -893,10 +902,10 @@
       <c r="C3" t="n">
         <v>569</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>569</v>
-      </c>
+      <c r="D3" t="n">
+        <v>569</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>569</v>
       </c>
@@ -915,10 +924,10 @@
       <c r="K3" t="n">
         <v>569</v>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>569</v>
-      </c>
+      <c r="L3" t="n">
+        <v>569</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>569</v>
       </c>
@@ -961,26 +970,26 @@
       <c r="AA3" t="n">
         <v>569</v>
       </c>
-      <c r="AB3" t="inlineStr"/>
+      <c r="AB3" t="n">
+        <v>569</v>
+      </c>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="n">
         <v>569</v>
       </c>
       <c r="AG3" t="n">
         <v>569</v>
       </c>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="n">
         <v>569</v>
       </c>
@@ -996,10 +1005,10 @@
       <c r="AP3" t="n">
         <v>569</v>
       </c>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AQ3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR3" t="inlineStr"/>
       <c r="AS3" t="n">
         <v>569</v>
       </c>
@@ -1016,6 +1025,9 @@
         <v>569</v>
       </c>
       <c r="AX3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1025,9 +1037,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>299</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
         <v>299</v>
       </c>
@@ -1121,10 +1131,10 @@
       <c r="AG4" t="n">
         <v>299</v>
       </c>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI4" t="inlineStr"/>
       <c r="AJ4" t="n">
         <v>299</v>
       </c>
@@ -1146,10 +1156,10 @@
       <c r="AP4" t="n">
         <v>299</v>
       </c>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AQ4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR4" t="inlineStr"/>
       <c r="AS4" t="n">
         <v>299</v>
       </c>
@@ -1166,6 +1176,9 @@
         <v>299</v>
       </c>
       <c r="AX4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1175,9 +1188,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>569</v>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
         <v>569</v>
       </c>
@@ -1199,10 +1210,10 @@
       <c r="I5" t="n">
         <v>569</v>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>569</v>
-      </c>
+      <c r="J5" t="n">
+        <v>569</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="n">
         <v>569</v>
       </c>
@@ -1296,10 +1307,10 @@
       <c r="AP5" t="n">
         <v>569</v>
       </c>
-      <c r="AQ5" t="inlineStr"/>
-      <c r="AR5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AQ5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="n">
         <v>569</v>
       </c>
@@ -1316,6 +1327,9 @@
         <v>569</v>
       </c>
       <c r="AX5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1325,14 +1339,12 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>499</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>499</v>
+      </c>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
-        <v>499</v>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>499</v>
       </c>
@@ -1420,10 +1432,10 @@
       <c r="AH6" t="n">
         <v>499</v>
       </c>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AI6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="n">
         <v>499</v>
       </c>
@@ -1442,10 +1454,10 @@
       <c r="AP6" t="n">
         <v>499</v>
       </c>
-      <c r="AQ6" t="inlineStr"/>
-      <c r="AR6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AQ6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR6" t="inlineStr"/>
       <c r="AS6" t="n">
         <v>499</v>
       </c>
@@ -1462,6 +1474,9 @@
         <v>499</v>
       </c>
       <c r="AX6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AY6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1477,10 +1492,10 @@
       <c r="C7" t="n">
         <v>569</v>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>569</v>
-      </c>
+      <c r="D7" t="n">
+        <v>569</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>569</v>
       </c>
@@ -1565,12 +1580,12 @@
       <c r="AG7" t="n">
         <v>569</v>
       </c>
-      <c r="AH7" t="inlineStr"/>
+      <c r="AH7" t="n">
+        <v>569</v>
+      </c>
       <c r="AI7" t="inlineStr"/>
       <c r="AJ7" t="inlineStr"/>
-      <c r="AK7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="n">
         <v>569</v>
       </c>
@@ -1586,10 +1601,10 @@
       <c r="AP7" t="n">
         <v>569</v>
       </c>
-      <c r="AQ7" t="inlineStr"/>
-      <c r="AR7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AQ7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR7" t="inlineStr"/>
       <c r="AS7" t="n">
         <v>569</v>
       </c>
@@ -1606,6 +1621,9 @@
         <v>569</v>
       </c>
       <c r="AX7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1621,10 +1639,10 @@
       <c r="C8" t="n">
         <v>929</v>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>929</v>
-      </c>
+      <c r="D8" t="n">
+        <v>929</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>929</v>
       </c>
@@ -1709,14 +1727,14 @@
       <c r="AG8" t="n">
         <v>929</v>
       </c>
-      <c r="AH8" t="inlineStr"/>
-      <c r="AI8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AJ8" t="inlineStr"/>
-      <c r="AK8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="n">
         <v>929</v>
       </c>
@@ -1732,10 +1750,10 @@
       <c r="AP8" t="n">
         <v>929</v>
       </c>
-      <c r="AQ8" t="inlineStr"/>
-      <c r="AR8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR8" t="inlineStr"/>
       <c r="AS8" t="n">
         <v>929</v>
       </c>
@@ -1752,6 +1770,9 @@
         <v>929</v>
       </c>
       <c r="AX8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1764,10 +1785,10 @@
       <c r="B9" t="n">
         <v>299</v>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
-        <v>299</v>
-      </c>
+      <c r="C9" t="n">
+        <v>299</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
         <v>299</v>
       </c>
@@ -1855,10 +1876,10 @@
       <c r="AG9" t="n">
         <v>299</v>
       </c>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI9" t="inlineStr"/>
       <c r="AJ9" t="n">
         <v>299</v>
       </c>
@@ -1880,10 +1901,10 @@
       <c r="AP9" t="n">
         <v>299</v>
       </c>
-      <c r="AQ9" t="inlineStr"/>
-      <c r="AR9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AQ9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR9" t="inlineStr"/>
       <c r="AS9" t="n">
         <v>299</v>
       </c>
@@ -1900,6 +1921,9 @@
         <v>299</v>
       </c>
       <c r="AX9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1912,11 +1936,11 @@
       <c r="B10" t="n">
         <v>299</v>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>299</v>
+      </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>299</v>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>299</v>
       </c>
@@ -1971,10 +1995,10 @@
       <c r="W10" t="n">
         <v>299</v>
       </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="n">
-        <v>299</v>
-      </c>
+      <c r="X10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="n">
         <v>299</v>
       </c>
@@ -1999,14 +2023,14 @@
       <c r="AG10" t="n">
         <v>299</v>
       </c>
-      <c r="AH10" t="inlineStr"/>
-      <c r="AI10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AJ10" t="inlineStr"/>
-      <c r="AK10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="n">
         <v>299</v>
       </c>
@@ -2022,10 +2046,10 @@
       <c r="AP10" t="n">
         <v>299</v>
       </c>
-      <c r="AQ10" t="inlineStr"/>
-      <c r="AR10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AQ10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR10" t="inlineStr"/>
       <c r="AS10" t="n">
         <v>299</v>
       </c>
@@ -2042,6 +2066,9 @@
         <v>299</v>
       </c>
       <c r="AX10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2150,10 +2177,10 @@
       <c r="AH11" t="n">
         <v>2997</v>
       </c>
-      <c r="AI11" t="inlineStr"/>
-      <c r="AJ11" t="n">
+      <c r="AI11" t="n">
         <v>2997</v>
       </c>
+      <c r="AJ11" t="inlineStr"/>
       <c r="AK11" t="n">
         <v>2997</v>
       </c>
@@ -2167,15 +2194,15 @@
         <v>2997</v>
       </c>
       <c r="AO11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AP11" t="n">
         <v>929</v>
       </c>
-      <c r="AQ11" t="inlineStr"/>
-      <c r="AR11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR11" t="inlineStr"/>
       <c r="AS11" t="n">
         <v>929</v>
       </c>
@@ -2192,6 +2219,9 @@
         <v>929</v>
       </c>
       <c r="AX11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2303,10 +2333,10 @@
       <c r="AI12" t="n">
         <v>569</v>
       </c>
-      <c r="AJ12" t="inlineStr"/>
-      <c r="AK12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="n">
         <v>569</v>
       </c>
@@ -2322,10 +2352,10 @@
       <c r="AP12" t="n">
         <v>569</v>
       </c>
-      <c r="AQ12" t="inlineStr"/>
-      <c r="AR12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AQ12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR12" t="inlineStr"/>
       <c r="AS12" t="n">
         <v>569</v>
       </c>
@@ -2342,6 +2372,9 @@
         <v>569</v>
       </c>
       <c r="AX12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2354,10 +2387,10 @@
       <c r="B13" t="n">
         <v>569</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>569</v>
-      </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>569</v>
       </c>
@@ -2394,10 +2427,10 @@
       <c r="P13" t="n">
         <v>569</v>
       </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q13" t="n">
+        <v>569</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
       <c r="S13" t="n">
         <v>569</v>
       </c>
@@ -2443,14 +2476,14 @@
       <c r="AG13" t="n">
         <v>569</v>
       </c>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="n">
         <v>569</v>
       </c>
@@ -2466,24 +2499,27 @@
       <c r="AP13" t="n">
         <v>569</v>
       </c>
-      <c r="AQ13" t="inlineStr"/>
-      <c r="AR13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AQ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR13" t="inlineStr"/>
       <c r="AS13" t="n">
         <v>569</v>
       </c>
       <c r="AT13" t="n">
         <v>569</v>
       </c>
-      <c r="AU13" t="inlineStr"/>
-      <c r="AV13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AU13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV13" t="inlineStr"/>
       <c r="AW13" t="n">
         <v>569</v>
       </c>
       <c r="AX13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2493,16 +2529,14 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>794</v>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
         <v>794</v>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>794</v>
       </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
         <v>794</v>
       </c>
@@ -2557,10 +2591,10 @@
       <c r="W14" t="n">
         <v>794</v>
       </c>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="n">
+      <c r="X14" t="n">
         <v>794</v>
       </c>
+      <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="n">
         <v>794</v>
       </c>
@@ -2568,7 +2602,7 @@
         <v>794</v>
       </c>
       <c r="AB14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AC14" t="n">
         <v>499</v>
@@ -2585,11 +2619,11 @@
       <c r="AG14" t="n">
         <v>499</v>
       </c>
-      <c r="AH14" t="inlineStr"/>
+      <c r="AH14" t="n">
+        <v>499</v>
+      </c>
       <c r="AI14" t="inlineStr"/>
-      <c r="AJ14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AJ14" t="inlineStr"/>
       <c r="AK14" t="n">
         <v>499</v>
       </c>
@@ -2630,6 +2664,9 @@
         <v>499</v>
       </c>
       <c r="AX14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AY14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2639,14 +2676,12 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>499</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>499</v>
+      </c>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>499</v>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
         <v>499</v>
       </c>
@@ -2737,10 +2772,10 @@
       <c r="AI15" t="n">
         <v>499</v>
       </c>
-      <c r="AJ15" t="inlineStr"/>
-      <c r="AK15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AJ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="n">
         <v>499</v>
       </c>
@@ -2750,14 +2785,14 @@
       <c r="AN15" t="n">
         <v>499</v>
       </c>
-      <c r="AO15" t="inlineStr"/>
-      <c r="AP15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AQ15" t="inlineStr"/>
-      <c r="AR15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AO15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR15" t="inlineStr"/>
       <c r="AS15" t="n">
         <v>499</v>
       </c>
@@ -2774,6 +2809,9 @@
         <v>499</v>
       </c>
       <c r="AX15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AY15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2783,13 +2821,11 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>299</v>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>299</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
         <v>299</v>
       </c>
@@ -2868,17 +2904,17 @@
       <c r="AD16" t="n">
         <v>299</v>
       </c>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF16" t="inlineStr"/>
       <c r="AG16" t="n">
         <v>299</v>
       </c>
-      <c r="AH16" t="inlineStr"/>
-      <c r="AI16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI16" t="inlineStr"/>
       <c r="AJ16" t="n">
         <v>299</v>
       </c>
@@ -2900,10 +2936,10 @@
       <c r="AP16" t="n">
         <v>299</v>
       </c>
-      <c r="AQ16" t="inlineStr"/>
-      <c r="AR16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AQ16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR16" t="inlineStr"/>
       <c r="AS16" t="n">
         <v>299</v>
       </c>
@@ -2920,6 +2956,9 @@
         <v>299</v>
       </c>
       <c r="AX16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3031,10 +3070,10 @@
       <c r="AI17" t="n">
         <v>929</v>
       </c>
-      <c r="AJ17" t="inlineStr"/>
-      <c r="AK17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="n">
         <v>929</v>
       </c>
@@ -3050,10 +3089,10 @@
       <c r="AP17" t="n">
         <v>929</v>
       </c>
-      <c r="AQ17" t="inlineStr"/>
-      <c r="AR17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR17" t="inlineStr"/>
       <c r="AS17" t="n">
         <v>929</v>
       </c>
@@ -3070,6 +3109,9 @@
         <v>929</v>
       </c>
       <c r="AX17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3082,11 +3124,11 @@
       <c r="B18" t="n">
         <v>499</v>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>499</v>
+      </c>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="n">
-        <v>499</v>
-      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
         <v>499</v>
       </c>
@@ -3174,11 +3216,11 @@
       <c r="AH18" t="n">
         <v>499</v>
       </c>
-      <c r="AI18" t="inlineStr"/>
+      <c r="AI18" t="n">
+        <v>499</v>
+      </c>
       <c r="AJ18" t="inlineStr"/>
-      <c r="AK18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="n">
         <v>499</v>
       </c>
@@ -3194,10 +3236,10 @@
       <c r="AP18" t="n">
         <v>499</v>
       </c>
-      <c r="AQ18" t="inlineStr"/>
-      <c r="AR18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AQ18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR18" t="inlineStr"/>
       <c r="AS18" t="n">
         <v>499</v>
       </c>
@@ -3214,6 +3256,9 @@
         <v>499</v>
       </c>
       <c r="AX18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AY18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3223,16 +3268,14 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
         <v>1299</v>
       </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
         <v>1299</v>
       </c>
@@ -3312,7 +3355,7 @@
         <v>1299</v>
       </c>
       <c r="AF19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AG19" t="n">
         <v>1497</v>
@@ -3320,13 +3363,13 @@
       <c r="AH19" t="n">
         <v>1497</v>
       </c>
-      <c r="AI19" t="inlineStr"/>
+      <c r="AI19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AJ19" t="inlineStr"/>
-      <c r="AK19" t="n">
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="n">
         <v>465</v>
-      </c>
-      <c r="AL19" t="n">
-        <v>1497</v>
       </c>
       <c r="AM19" t="n">
         <v>1497</v>
@@ -3362,6 +3405,9 @@
         <v>1497</v>
       </c>
       <c r="AX19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AY19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3494,10 +3540,10 @@
       <c r="AP20" t="n">
         <v>929</v>
       </c>
-      <c r="AQ20" t="inlineStr"/>
-      <c r="AR20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR20" t="inlineStr"/>
       <c r="AS20" t="n">
         <v>929</v>
       </c>
@@ -3514,6 +3560,9 @@
         <v>929</v>
       </c>
       <c r="AX20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3526,17 +3575,17 @@
       <c r="B21" t="n">
         <v>499</v>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
-        <v>499</v>
-      </c>
+      <c r="C21" t="n">
+        <v>499</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
         <v>499</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="n">
-        <v>499</v>
-      </c>
+      <c r="F21" t="n">
+        <v>499</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
         <v>499</v>
       </c>
@@ -3591,10 +3640,10 @@
       <c r="Y21" t="n">
         <v>499</v>
       </c>
-      <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="n">
-        <v>499</v>
-      </c>
+      <c r="Z21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="n">
         <v>499</v>
       </c>
@@ -3619,10 +3668,10 @@
       <c r="AI21" t="n">
         <v>499</v>
       </c>
-      <c r="AJ21" t="inlineStr"/>
-      <c r="AK21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AJ21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="n">
         <v>499</v>
       </c>
@@ -3660,6 +3709,9 @@
         <v>499</v>
       </c>
       <c r="AX21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AY21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3669,9 +3721,7 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>299</v>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
         <v>299</v>
       </c>
@@ -3765,14 +3815,14 @@
       <c r="AG22" t="n">
         <v>299</v>
       </c>
-      <c r="AH22" t="inlineStr"/>
-      <c r="AI22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AJ22" t="inlineStr"/>
-      <c r="AK22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI22" t="inlineStr"/>
+      <c r="AJ22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="n">
         <v>299</v>
       </c>
@@ -3788,10 +3838,10 @@
       <c r="AP22" t="n">
         <v>299</v>
       </c>
-      <c r="AQ22" t="inlineStr"/>
-      <c r="AR22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AQ22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR22" t="inlineStr"/>
       <c r="AS22" t="n">
         <v>299</v>
       </c>
@@ -3808,6 +3858,9 @@
         <v>299</v>
       </c>
       <c r="AX22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3820,11 +3873,11 @@
       <c r="B23" t="n">
         <v>1299</v>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>1299</v>
+      </c>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
         <v>1299</v>
       </c>
@@ -3912,11 +3965,11 @@
       <c r="AH23" t="n">
         <v>1299</v>
       </c>
-      <c r="AI23" t="inlineStr"/>
+      <c r="AI23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AJ23" t="inlineStr"/>
-      <c r="AK23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AK23" t="inlineStr"/>
       <c r="AL23" t="n">
         <v>1299</v>
       </c>
@@ -3932,10 +3985,10 @@
       <c r="AP23" t="n">
         <v>1299</v>
       </c>
-      <c r="AQ23" t="inlineStr"/>
-      <c r="AR23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AQ23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AR23" t="inlineStr"/>
       <c r="AS23" t="n">
         <v>1299</v>
       </c>
@@ -3952,6 +4005,9 @@
         <v>1299</v>
       </c>
       <c r="AX23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AY23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -3964,11 +4020,11 @@
       <c r="B24" t="n">
         <v>929</v>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>929</v>
+      </c>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="n">
-        <v>929</v>
-      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
         <v>929</v>
       </c>
@@ -4053,11 +4109,11 @@
       <c r="AG24" t="n">
         <v>929</v>
       </c>
-      <c r="AH24" t="inlineStr"/>
+      <c r="AH24" t="n">
+        <v>929</v>
+      </c>
       <c r="AI24" t="inlineStr"/>
-      <c r="AJ24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ24" t="inlineStr"/>
       <c r="AK24" t="n">
         <v>929</v>
       </c>
@@ -4076,10 +4132,10 @@
       <c r="AP24" t="n">
         <v>929</v>
       </c>
-      <c r="AQ24" t="inlineStr"/>
-      <c r="AR24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR24" t="inlineStr"/>
       <c r="AS24" t="n">
         <v>929</v>
       </c>
@@ -4096,6 +4152,9 @@
         <v>929</v>
       </c>
       <c r="AX24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4108,11 +4167,11 @@
       <c r="B25" t="n">
         <v>929</v>
       </c>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>929</v>
+      </c>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="n">
-        <v>929</v>
-      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
         <v>929</v>
       </c>
@@ -4122,10 +4181,10 @@
       <c r="H25" t="n">
         <v>929</v>
       </c>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="n">
-        <v>929</v>
-      </c>
+      <c r="I25" t="n">
+        <v>929</v>
+      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
         <v>929</v>
       </c>
@@ -4195,11 +4254,11 @@
       <c r="AG25" t="n">
         <v>929</v>
       </c>
-      <c r="AH25" t="inlineStr"/>
+      <c r="AH25" t="n">
+        <v>929</v>
+      </c>
       <c r="AI25" t="inlineStr"/>
-      <c r="AJ25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ25" t="inlineStr"/>
       <c r="AK25" t="n">
         <v>929</v>
       </c>
@@ -4218,10 +4277,10 @@
       <c r="AP25" t="n">
         <v>929</v>
       </c>
-      <c r="AQ25" t="inlineStr"/>
-      <c r="AR25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR25" t="inlineStr"/>
       <c r="AS25" t="n">
         <v>929</v>
       </c>
@@ -4238,6 +4297,9 @@
         <v>929</v>
       </c>
       <c r="AX25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4250,10 +4312,10 @@
       <c r="B26" t="n">
         <v>1299</v>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
         <v>1299</v>
       </c>
@@ -4263,10 +4325,10 @@
       <c r="G26" t="n">
         <v>1299</v>
       </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="n">
         <v>1299</v>
       </c>
@@ -4339,14 +4401,14 @@
       <c r="AG26" t="n">
         <v>1299</v>
       </c>
-      <c r="AH26" t="inlineStr"/>
-      <c r="AI26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AJ26" t="inlineStr"/>
-      <c r="AK26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AH26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AI26" t="inlineStr"/>
+      <c r="AJ26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AK26" t="inlineStr"/>
       <c r="AL26" t="n">
         <v>1299</v>
       </c>
@@ -4362,10 +4424,10 @@
       <c r="AP26" t="n">
         <v>1299</v>
       </c>
-      <c r="AQ26" t="inlineStr"/>
-      <c r="AR26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AQ26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AR26" t="inlineStr"/>
       <c r="AS26" t="n">
         <v>1299</v>
       </c>
@@ -4382,6 +4444,9 @@
         <v>1299</v>
       </c>
       <c r="AX26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AY26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 20:47
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY26"/>
+  <dimension ref="A1:AZ26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,7 @@
     <col width="21" customWidth="1" min="49" max="49"/>
     <col width="21" customWidth="1" min="50" max="50"/>
     <col width="21" customWidth="1" min="51" max="51"/>
+    <col width="21" customWidth="1" min="52" max="52"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -494,250 +495,255 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 02:11</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-25 00:27</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -833,10 +839,10 @@
       <c r="AC2" t="n">
         <v>929</v>
       </c>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AD2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="n">
         <v>929</v>
       </c>
@@ -849,25 +855,25 @@
       <c r="AI2" t="n">
         <v>929</v>
       </c>
-      <c r="AJ2" t="inlineStr"/>
+      <c r="AJ2" t="n">
+        <v>929</v>
+      </c>
       <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="n">
         <v>929</v>
       </c>
-      <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="n">
         <v>929</v>
       </c>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="n">
         <v>929</v>
       </c>
@@ -887,6 +893,9 @@
         <v>929</v>
       </c>
       <c r="AY2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AZ2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -896,19 +905,17 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>569</v>
       </c>
       <c r="D3" t="n">
         <v>569</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>569</v>
-      </c>
+      <c r="E3" t="n">
+        <v>569</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>569</v>
       </c>
@@ -927,10 +934,10 @@
       <c r="L3" t="n">
         <v>569</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="n">
-        <v>569</v>
-      </c>
+      <c r="M3" t="n">
+        <v>569</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="n">
         <v>569</v>
       </c>
@@ -973,26 +980,26 @@
       <c r="AB3" t="n">
         <v>569</v>
       </c>
-      <c r="AC3" t="inlineStr"/>
+      <c r="AC3" t="n">
+        <v>569</v>
+      </c>
       <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="n">
         <v>569</v>
       </c>
       <c r="AH3" t="n">
         <v>569</v>
       </c>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="n">
         <v>569</v>
       </c>
@@ -1008,10 +1015,10 @@
       <c r="AQ3" t="n">
         <v>569</v>
       </c>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AR3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS3" t="inlineStr"/>
       <c r="AT3" t="n">
         <v>569</v>
       </c>
@@ -1028,6 +1035,9 @@
         <v>569</v>
       </c>
       <c r="AY3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AZ3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1037,10 +1047,10 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XL, 28, count)</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="n">
-        <v>299</v>
-      </c>
+      <c r="B4" t="n">
+        <v>299</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
         <v>299</v>
       </c>
@@ -1134,10 +1144,10 @@
       <c r="AH4" t="n">
         <v>299</v>
       </c>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="n">
         <v>299</v>
       </c>
@@ -1159,10 +1169,10 @@
       <c r="AQ4" t="n">
         <v>299</v>
       </c>
-      <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AR4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS4" t="inlineStr"/>
       <c r="AT4" t="n">
         <v>299</v>
       </c>
@@ -1179,6 +1189,9 @@
         <v>299</v>
       </c>
       <c r="AY4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AZ4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1189,9 +1202,7 @@
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
-        <v>569</v>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
         <v>569</v>
       </c>
@@ -1213,10 +1224,10 @@
       <c r="J5" t="n">
         <v>569</v>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
-        <v>569</v>
-      </c>
+      <c r="K5" t="n">
+        <v>569</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
         <v>569</v>
       </c>
@@ -1310,10 +1321,10 @@
       <c r="AQ5" t="n">
         <v>569</v>
       </c>
-      <c r="AR5" t="inlineStr"/>
-      <c r="AS5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AR5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS5" t="inlineStr"/>
       <c r="AT5" t="n">
         <v>569</v>
       </c>
@@ -1330,6 +1341,9 @@
         <v>569</v>
       </c>
       <c r="AY5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AZ5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1339,15 +1353,15 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 42 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="n">
-        <v>499</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>499</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>499</v>
+      </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>499</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
         <v>499</v>
       </c>
@@ -1435,10 +1449,10 @@
       <c r="AI6" t="n">
         <v>499</v>
       </c>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AJ6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="n">
         <v>499</v>
       </c>
@@ -1457,10 +1471,10 @@
       <c r="AQ6" t="n">
         <v>499</v>
       </c>
-      <c r="AR6" t="inlineStr"/>
-      <c r="AS6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AR6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS6" t="inlineStr"/>
       <c r="AT6" t="n">
         <v>499</v>
       </c>
@@ -1477,6 +1491,9 @@
         <v>499</v>
       </c>
       <c r="AY6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AZ6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1486,19 +1503,17 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>569</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
         <v>569</v>
       </c>
       <c r="D7" t="n">
         <v>569</v>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>569</v>
-      </c>
+      <c r="E7" t="n">
+        <v>569</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>569</v>
       </c>
@@ -1583,12 +1598,12 @@
       <c r="AH7" t="n">
         <v>569</v>
       </c>
-      <c r="AI7" t="inlineStr"/>
+      <c r="AI7" t="n">
+        <v>569</v>
+      </c>
       <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
-      <c r="AL7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="n">
         <v>569</v>
       </c>
@@ -1604,10 +1619,10 @@
       <c r="AQ7" t="n">
         <v>569</v>
       </c>
-      <c r="AR7" t="inlineStr"/>
-      <c r="AS7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AR7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS7" t="inlineStr"/>
       <c r="AT7" t="n">
         <v>569</v>
       </c>
@@ -1624,6 +1639,9 @@
         <v>569</v>
       </c>
       <c r="AY7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AZ7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1633,19 +1651,17 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
         <v>929</v>
       </c>
       <c r="D8" t="n">
         <v>929</v>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>929</v>
-      </c>
+      <c r="E8" t="n">
+        <v>929</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>929</v>
       </c>
@@ -1730,14 +1746,14 @@
       <c r="AH8" t="n">
         <v>929</v>
       </c>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AK8" t="inlineStr"/>
-      <c r="AL8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="n">
         <v>929</v>
       </c>
@@ -1753,10 +1769,10 @@
       <c r="AQ8" t="n">
         <v>929</v>
       </c>
-      <c r="AR8" t="inlineStr"/>
-      <c r="AS8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS8" t="inlineStr"/>
       <c r="AT8" t="n">
         <v>929</v>
       </c>
@@ -1773,6 +1789,9 @@
         <v>929</v>
       </c>
       <c r="AY8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AZ8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1782,16 +1801,14 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>299</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
         <v>299</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>299</v>
-      </c>
+      <c r="D9" t="n">
+        <v>299</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>299</v>
       </c>
@@ -1879,10 +1896,10 @@
       <c r="AH9" t="n">
         <v>299</v>
       </c>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="n">
         <v>299</v>
       </c>
@@ -1904,10 +1921,10 @@
       <c r="AQ9" t="n">
         <v>299</v>
       </c>
-      <c r="AR9" t="inlineStr"/>
-      <c r="AS9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AR9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS9" t="inlineStr"/>
       <c r="AT9" t="n">
         <v>299</v>
       </c>
@@ -1924,6 +1941,9 @@
         <v>299</v>
       </c>
       <c r="AY9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AZ9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1933,17 +1953,15 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
         <v>299</v>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>299</v>
+      </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>299</v>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>299</v>
       </c>
@@ -1998,10 +2016,10 @@
       <c r="X10" t="n">
         <v>299</v>
       </c>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Y10" t="n">
+        <v>299</v>
+      </c>
+      <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
         <v>299</v>
       </c>
@@ -2026,14 +2044,14 @@
       <c r="AH10" t="n">
         <v>299</v>
       </c>
-      <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AK10" t="inlineStr"/>
-      <c r="AL10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL10" t="inlineStr"/>
       <c r="AM10" t="n">
         <v>299</v>
       </c>
@@ -2049,10 +2067,10 @@
       <c r="AQ10" t="n">
         <v>299</v>
       </c>
-      <c r="AR10" t="inlineStr"/>
-      <c r="AS10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AR10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS10" t="inlineStr"/>
       <c r="AT10" t="n">
         <v>299</v>
       </c>
@@ -2069,6 +2087,9 @@
         <v>299</v>
       </c>
       <c r="AY10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AZ10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2078,9 +2099,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>2997</v>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
         <v>2997</v>
       </c>
@@ -2180,10 +2199,10 @@
       <c r="AI11" t="n">
         <v>2997</v>
       </c>
-      <c r="AJ11" t="inlineStr"/>
-      <c r="AK11" t="n">
+      <c r="AJ11" t="n">
         <v>2997</v>
       </c>
+      <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="n">
         <v>2997</v>
       </c>
@@ -2197,15 +2216,15 @@
         <v>2997</v>
       </c>
       <c r="AP11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AQ11" t="n">
         <v>929</v>
       </c>
-      <c r="AR11" t="inlineStr"/>
-      <c r="AS11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS11" t="inlineStr"/>
       <c r="AT11" t="n">
         <v>929</v>
       </c>
@@ -2222,6 +2241,9 @@
         <v>929</v>
       </c>
       <c r="AY11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AZ11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2231,9 +2253,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>569</v>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
         <v>569</v>
       </c>
@@ -2336,10 +2356,10 @@
       <c r="AJ12" t="n">
         <v>569</v>
       </c>
-      <c r="AK12" t="inlineStr"/>
-      <c r="AL12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="n">
         <v>569</v>
       </c>
@@ -2355,10 +2375,10 @@
       <c r="AQ12" t="n">
         <v>569</v>
       </c>
-      <c r="AR12" t="inlineStr"/>
-      <c r="AS12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AR12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS12" t="inlineStr"/>
       <c r="AT12" t="n">
         <v>569</v>
       </c>
@@ -2375,6 +2395,9 @@
         <v>569</v>
       </c>
       <c r="AY12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AZ12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2384,16 +2407,14 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
         <v>569</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>569</v>
-      </c>
+      <c r="D13" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>569</v>
       </c>
@@ -2430,10 +2451,10 @@
       <c r="Q13" t="n">
         <v>569</v>
       </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="n">
-        <v>569</v>
-      </c>
+      <c r="R13" t="n">
+        <v>569</v>
+      </c>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
         <v>569</v>
       </c>
@@ -2479,14 +2500,14 @@
       <c r="AH13" t="n">
         <v>569</v>
       </c>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AK13" t="inlineStr"/>
-      <c r="AL13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="n">
         <v>569</v>
       </c>
@@ -2502,24 +2523,27 @@
       <c r="AQ13" t="n">
         <v>569</v>
       </c>
-      <c r="AR13" t="inlineStr"/>
-      <c r="AS13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AR13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS13" t="inlineStr"/>
       <c r="AT13" t="n">
         <v>569</v>
       </c>
       <c r="AU13" t="n">
         <v>569</v>
       </c>
-      <c r="AV13" t="inlineStr"/>
-      <c r="AW13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AV13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW13" t="inlineStr"/>
       <c r="AX13" t="n">
         <v>569</v>
       </c>
       <c r="AY13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AZ13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2529,17 +2553,17 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 78 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="n">
+      <c r="B14" t="n">
         <v>794</v>
       </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
         <v>794</v>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
+      <c r="E14" t="n">
         <v>794</v>
       </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>794</v>
       </c>
@@ -2594,10 +2618,10 @@
       <c r="X14" t="n">
         <v>794</v>
       </c>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="n">
+      <c r="Y14" t="n">
         <v>794</v>
       </c>
+      <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
         <v>794</v>
       </c>
@@ -2605,7 +2629,7 @@
         <v>794</v>
       </c>
       <c r="AC14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AD14" t="n">
         <v>499</v>
@@ -2622,11 +2646,11 @@
       <c r="AH14" t="n">
         <v>499</v>
       </c>
-      <c r="AI14" t="inlineStr"/>
+      <c r="AI14" t="n">
+        <v>499</v>
+      </c>
       <c r="AJ14" t="inlineStr"/>
-      <c r="AK14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AK14" t="inlineStr"/>
       <c r="AL14" t="n">
         <v>499</v>
       </c>
@@ -2667,6 +2691,9 @@
         <v>499</v>
       </c>
       <c r="AY14" t="n">
+        <v>499</v>
+      </c>
+      <c r="AZ14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2677,14 +2704,12 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>499</v>
-      </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>499</v>
+      </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>499</v>
-      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
         <v>499</v>
       </c>
@@ -2775,10 +2800,10 @@
       <c r="AJ15" t="n">
         <v>499</v>
       </c>
-      <c r="AK15" t="inlineStr"/>
-      <c r="AL15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AK15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="n">
         <v>499</v>
       </c>
@@ -2788,14 +2813,14 @@
       <c r="AO15" t="n">
         <v>499</v>
       </c>
-      <c r="AP15" t="inlineStr"/>
-      <c r="AQ15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AR15" t="inlineStr"/>
-      <c r="AS15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AP15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS15" t="inlineStr"/>
       <c r="AT15" t="n">
         <v>499</v>
       </c>
@@ -2812,6 +2837,9 @@
         <v>499</v>
       </c>
       <c r="AY15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AZ15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2821,14 +2849,14 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (S, 40, count)</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="n">
-        <v>299</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>299</v>
-      </c>
+      <c r="B16" t="n">
+        <v>299</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="n">
+        <v>299</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
         <v>299</v>
       </c>
@@ -2907,17 +2935,17 @@
       <c r="AE16" t="n">
         <v>299</v>
       </c>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AF16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="n">
         <v>299</v>
       </c>
-      <c r="AI16" t="inlineStr"/>
-      <c r="AJ16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ16" t="inlineStr"/>
       <c r="AK16" t="n">
         <v>299</v>
       </c>
@@ -2939,10 +2967,10 @@
       <c r="AQ16" t="n">
         <v>299</v>
       </c>
-      <c r="AR16" t="inlineStr"/>
-      <c r="AS16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AR16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS16" t="inlineStr"/>
       <c r="AT16" t="n">
         <v>299</v>
       </c>
@@ -2959,6 +2987,9 @@
         <v>299</v>
       </c>
       <c r="AY16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AZ16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2968,9 +2999,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>929</v>
-      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
         <v>929</v>
       </c>
@@ -3073,10 +3102,10 @@
       <c r="AJ17" t="n">
         <v>929</v>
       </c>
-      <c r="AK17" t="inlineStr"/>
-      <c r="AL17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL17" t="inlineStr"/>
       <c r="AM17" t="n">
         <v>929</v>
       </c>
@@ -3092,10 +3121,10 @@
       <c r="AQ17" t="n">
         <v>929</v>
       </c>
-      <c r="AR17" t="inlineStr"/>
-      <c r="AS17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS17" t="inlineStr"/>
       <c r="AT17" t="n">
         <v>929</v>
       </c>
@@ -3112,6 +3141,9 @@
         <v>929</v>
       </c>
       <c r="AY17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AZ17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3121,17 +3153,15 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>499</v>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="n">
         <v>499</v>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>499</v>
+      </c>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
-        <v>499</v>
-      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
         <v>499</v>
       </c>
@@ -3219,11 +3249,11 @@
       <c r="AI18" t="n">
         <v>499</v>
       </c>
-      <c r="AJ18" t="inlineStr"/>
+      <c r="AJ18" t="n">
+        <v>499</v>
+      </c>
       <c r="AK18" t="inlineStr"/>
-      <c r="AL18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AL18" t="inlineStr"/>
       <c r="AM18" t="n">
         <v>499</v>
       </c>
@@ -3239,10 +3269,10 @@
       <c r="AQ18" t="n">
         <v>499</v>
       </c>
-      <c r="AR18" t="inlineStr"/>
-      <c r="AS18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AR18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS18" t="inlineStr"/>
       <c r="AT18" t="n">
         <v>499</v>
       </c>
@@ -3259,6 +3289,9 @@
         <v>499</v>
       </c>
       <c r="AY18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AZ18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3269,16 +3302,14 @@
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
         <v>1299</v>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
         <v>1299</v>
       </c>
@@ -3358,7 +3389,7 @@
         <v>1299</v>
       </c>
       <c r="AG19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AH19" t="n">
         <v>1497</v>
@@ -3366,13 +3397,13 @@
       <c r="AI19" t="n">
         <v>1497</v>
       </c>
-      <c r="AJ19" t="inlineStr"/>
+      <c r="AJ19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AK19" t="inlineStr"/>
-      <c r="AL19" t="n">
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="n">
         <v>465</v>
-      </c>
-      <c r="AM19" t="n">
-        <v>1497</v>
       </c>
       <c r="AN19" t="n">
         <v>1497</v>
@@ -3408,6 +3439,9 @@
         <v>1497</v>
       </c>
       <c r="AY19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="AZ19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3543,10 +3577,10 @@
       <c r="AQ20" t="n">
         <v>929</v>
       </c>
-      <c r="AR20" t="inlineStr"/>
-      <c r="AS20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS20" t="inlineStr"/>
       <c r="AT20" t="n">
         <v>929</v>
       </c>
@@ -3563,6 +3597,9 @@
         <v>929</v>
       </c>
       <c r="AY20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AZ20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3572,23 +3609,21 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
         <v>499</v>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>499</v>
-      </c>
+      <c r="D21" t="n">
+        <v>499</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
         <v>499</v>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="n">
-        <v>499</v>
-      </c>
+      <c r="G21" t="n">
+        <v>499</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>499</v>
       </c>
@@ -3643,10 +3678,10 @@
       <c r="Z21" t="n">
         <v>499</v>
       </c>
-      <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AA21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="n">
         <v>499</v>
       </c>
@@ -3671,10 +3706,10 @@
       <c r="AJ21" t="n">
         <v>499</v>
       </c>
-      <c r="AK21" t="inlineStr"/>
-      <c r="AL21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AK21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="n">
         <v>499</v>
       </c>
@@ -3712,6 +3747,9 @@
         <v>499</v>
       </c>
       <c r="AY21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AZ21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3722,9 +3760,7 @@
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" t="n">
-        <v>299</v>
-      </c>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
         <v>299</v>
       </c>
@@ -3818,14 +3854,14 @@
       <c r="AH22" t="n">
         <v>299</v>
       </c>
-      <c r="AI22" t="inlineStr"/>
-      <c r="AJ22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AK22" t="inlineStr"/>
-      <c r="AL22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ22" t="inlineStr"/>
+      <c r="AK22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL22" t="inlineStr"/>
       <c r="AM22" t="n">
         <v>299</v>
       </c>
@@ -3841,10 +3877,10 @@
       <c r="AQ22" t="n">
         <v>299</v>
       </c>
-      <c r="AR22" t="inlineStr"/>
-      <c r="AS22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AR22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AS22" t="inlineStr"/>
       <c r="AT22" t="n">
         <v>299</v>
       </c>
@@ -3861,6 +3897,9 @@
         <v>299</v>
       </c>
       <c r="AY22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AZ22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3870,17 +3909,15 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
         <v>1299</v>
       </c>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>1299</v>
+      </c>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
         <v>1299</v>
       </c>
@@ -3968,11 +4005,11 @@
       <c r="AI23" t="n">
         <v>1299</v>
       </c>
-      <c r="AJ23" t="inlineStr"/>
+      <c r="AJ23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AK23" t="inlineStr"/>
-      <c r="AL23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AL23" t="inlineStr"/>
       <c r="AM23" t="n">
         <v>1299</v>
       </c>
@@ -3988,10 +4025,10 @@
       <c r="AQ23" t="n">
         <v>1299</v>
       </c>
-      <c r="AR23" t="inlineStr"/>
-      <c r="AS23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AR23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AS23" t="inlineStr"/>
       <c r="AT23" t="n">
         <v>1299</v>
       </c>
@@ -4008,6 +4045,9 @@
         <v>1299</v>
       </c>
       <c r="AY23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AZ23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -4023,11 +4063,11 @@
       <c r="C24" t="n">
         <v>929</v>
       </c>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>929</v>
+      </c>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>929</v>
-      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
         <v>929</v>
       </c>
@@ -4112,11 +4152,11 @@
       <c r="AH24" t="n">
         <v>929</v>
       </c>
-      <c r="AI24" t="inlineStr"/>
+      <c r="AI24" t="n">
+        <v>929</v>
+      </c>
       <c r="AJ24" t="inlineStr"/>
-      <c r="AK24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK24" t="inlineStr"/>
       <c r="AL24" t="n">
         <v>929</v>
       </c>
@@ -4135,10 +4175,10 @@
       <c r="AQ24" t="n">
         <v>929</v>
       </c>
-      <c r="AR24" t="inlineStr"/>
-      <c r="AS24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS24" t="inlineStr"/>
       <c r="AT24" t="n">
         <v>929</v>
       </c>
@@ -4155,6 +4195,9 @@
         <v>929</v>
       </c>
       <c r="AY24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AZ24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4164,17 +4207,15 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>929</v>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
         <v>929</v>
       </c>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>929</v>
+      </c>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>929</v>
-      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>929</v>
       </c>
@@ -4184,10 +4225,10 @@
       <c r="I25" t="n">
         <v>929</v>
       </c>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="n">
-        <v>929</v>
-      </c>
+      <c r="J25" t="n">
+        <v>929</v>
+      </c>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="n">
         <v>929</v>
       </c>
@@ -4257,11 +4298,11 @@
       <c r="AH25" t="n">
         <v>929</v>
       </c>
-      <c r="AI25" t="inlineStr"/>
+      <c r="AI25" t="n">
+        <v>929</v>
+      </c>
       <c r="AJ25" t="inlineStr"/>
-      <c r="AK25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK25" t="inlineStr"/>
       <c r="AL25" t="n">
         <v>929</v>
       </c>
@@ -4280,10 +4321,10 @@
       <c r="AQ25" t="n">
         <v>929</v>
       </c>
-      <c r="AR25" t="inlineStr"/>
-      <c r="AS25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS25" t="inlineStr"/>
       <c r="AT25" t="n">
         <v>929</v>
       </c>
@@ -4300,6 +4341,9 @@
         <v>929</v>
       </c>
       <c r="AY25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AZ25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4315,10 +4359,10 @@
       <c r="C26" t="n">
         <v>1299</v>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
         <v>1299</v>
       </c>
@@ -4328,10 +4372,10 @@
       <c r="H26" t="n">
         <v>1299</v>
       </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
         <v>1299</v>
       </c>
@@ -4404,14 +4448,14 @@
       <c r="AH26" t="n">
         <v>1299</v>
       </c>
-      <c r="AI26" t="inlineStr"/>
-      <c r="AJ26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AK26" t="inlineStr"/>
-      <c r="AL26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AI26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AJ26" t="inlineStr"/>
+      <c r="AK26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AL26" t="inlineStr"/>
       <c r="AM26" t="n">
         <v>1299</v>
       </c>
@@ -4427,10 +4471,10 @@
       <c r="AQ26" t="n">
         <v>1299</v>
       </c>
-      <c r="AR26" t="inlineStr"/>
-      <c r="AS26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AR26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AS26" t="inlineStr"/>
       <c r="AT26" t="n">
         <v>1299</v>
       </c>
@@ -4447,6 +4491,9 @@
         <v>1299</v>
       </c>
       <c r="AY26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AZ26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-24 22:46
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ26"/>
+  <dimension ref="A1:BA26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,7 @@
     <col width="21" customWidth="1" min="50" max="50"/>
     <col width="21" customWidth="1" min="51" max="51"/>
     <col width="21" customWidth="1" min="52" max="52"/>
+    <col width="21" customWidth="1" min="53" max="53"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -495,255 +496,260 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 04:11</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-25 02:11</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 00:27</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -842,10 +848,10 @@
       <c r="AD2" t="n">
         <v>929</v>
       </c>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AE2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
         <v>929</v>
       </c>
@@ -858,25 +864,25 @@
       <c r="AJ2" t="n">
         <v>929</v>
       </c>
-      <c r="AK2" t="inlineStr"/>
+      <c r="AK2" t="n">
+        <v>929</v>
+      </c>
       <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="n">
         <v>929</v>
       </c>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="n">
         <v>929</v>
       </c>
-      <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="n">
         <v>929</v>
       </c>
@@ -896,6 +902,9 @@
         <v>929</v>
       </c>
       <c r="AZ2" t="n">
+        <v>929</v>
+      </c>
+      <c r="BA2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -905,20 +914,20 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Newborn/Extra Small (NB/XS) Size (0-5kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>569</v>
-      </c>
+      <c r="B3" t="n">
+        <v>569</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>569</v>
       </c>
       <c r="E3" t="n">
         <v>569</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>569</v>
-      </c>
+      <c r="F3" t="n">
+        <v>569</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>569</v>
       </c>
@@ -937,10 +946,10 @@
       <c r="M3" t="n">
         <v>569</v>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
-        <v>569</v>
-      </c>
+      <c r="N3" t="n">
+        <v>569</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
         <v>569</v>
       </c>
@@ -983,26 +992,26 @@
       <c r="AC3" t="n">
         <v>569</v>
       </c>
-      <c r="AD3" t="inlineStr"/>
+      <c r="AD3" t="n">
+        <v>569</v>
+      </c>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="n">
         <v>569</v>
       </c>
       <c r="AI3" t="n">
         <v>569</v>
       </c>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="n">
         <v>569</v>
       </c>
@@ -1018,10 +1027,10 @@
       <c r="AR3" t="n">
         <v>569</v>
       </c>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AS3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT3" t="inlineStr"/>
       <c r="AU3" t="n">
         <v>569</v>
       </c>
@@ -1038,6 +1047,9 @@
         <v>569</v>
       </c>
       <c r="AZ3" t="n">
+        <v>569</v>
+      </c>
+      <c r="BA3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1050,10 +1062,10 @@
       <c r="B4" t="n">
         <v>299</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="n">
-        <v>299</v>
-      </c>
+      <c r="C4" t="n">
+        <v>299</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>299</v>
       </c>
@@ -1147,10 +1159,10 @@
       <c r="AI4" t="n">
         <v>299</v>
       </c>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="n">
         <v>299</v>
       </c>
@@ -1172,10 +1184,10 @@
       <c r="AR4" t="n">
         <v>299</v>
       </c>
-      <c r="AS4" t="inlineStr"/>
-      <c r="AT4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AS4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT4" t="inlineStr"/>
       <c r="AU4" t="n">
         <v>299</v>
       </c>
@@ -1192,6 +1204,9 @@
         <v>299</v>
       </c>
       <c r="AZ4" t="n">
+        <v>299</v>
+      </c>
+      <c r="BA4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1201,11 +1216,11 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>569</v>
+      </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="n">
-        <v>569</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>569</v>
       </c>
@@ -1227,10 +1242,10 @@
       <c r="K5" t="n">
         <v>569</v>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
-        <v>569</v>
-      </c>
+      <c r="L5" t="n">
+        <v>569</v>
+      </c>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
         <v>569</v>
       </c>
@@ -1324,10 +1339,10 @@
       <c r="AR5" t="n">
         <v>569</v>
       </c>
-      <c r="AS5" t="inlineStr"/>
-      <c r="AT5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AS5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT5" t="inlineStr"/>
       <c r="AU5" t="n">
         <v>569</v>
       </c>
@@ -1344,6 +1359,9 @@
         <v>569</v>
       </c>
       <c r="AZ5" t="n">
+        <v>569</v>
+      </c>
+      <c r="BA5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1356,15 +1374,15 @@
       <c r="B6" t="n">
         <v>499</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="n">
-        <v>499</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>499</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>499</v>
+      </c>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>499</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>499</v>
       </c>
@@ -1452,10 +1470,10 @@
       <c r="AJ6" t="n">
         <v>499</v>
       </c>
-      <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AK6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AL6" t="inlineStr"/>
       <c r="AM6" t="n">
         <v>499</v>
       </c>
@@ -1474,10 +1492,10 @@
       <c r="AR6" t="n">
         <v>499</v>
       </c>
-      <c r="AS6" t="inlineStr"/>
-      <c r="AT6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AS6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT6" t="inlineStr"/>
       <c r="AU6" t="n">
         <v>499</v>
       </c>
@@ -1494,6 +1512,9 @@
         <v>499</v>
       </c>
       <c r="AZ6" t="n">
+        <v>499</v>
+      </c>
+      <c r="BA6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1503,20 +1524,20 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Small (S) Size (3-8 kg), 64 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="n">
-        <v>569</v>
-      </c>
+      <c r="B7" t="n">
+        <v>569</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
         <v>569</v>
       </c>
       <c r="E7" t="n">
         <v>569</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>569</v>
-      </c>
+      <c r="F7" t="n">
+        <v>569</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>569</v>
       </c>
@@ -1601,12 +1622,12 @@
       <c r="AI7" t="n">
         <v>569</v>
       </c>
-      <c r="AJ7" t="inlineStr"/>
+      <c r="AJ7" t="n">
+        <v>569</v>
+      </c>
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr"/>
-      <c r="AM7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="n">
         <v>569</v>
       </c>
@@ -1622,10 +1643,10 @@
       <c r="AR7" t="n">
         <v>569</v>
       </c>
-      <c r="AS7" t="inlineStr"/>
-      <c r="AT7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AS7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT7" t="inlineStr"/>
       <c r="AU7" t="n">
         <v>569</v>
       </c>
@@ -1642,6 +1663,9 @@
         <v>569</v>
       </c>
       <c r="AZ7" t="n">
+        <v>569</v>
+      </c>
+      <c r="BA7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1651,20 +1675,20 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 108 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>929</v>
-      </c>
+      <c r="B8" t="n">
+        <v>929</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>929</v>
       </c>
       <c r="E8" t="n">
         <v>929</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>929</v>
-      </c>
+      <c r="F8" t="n">
+        <v>929</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
         <v>929</v>
       </c>
@@ -1749,14 +1773,14 @@
       <c r="AI8" t="n">
         <v>929</v>
       </c>
-      <c r="AJ8" t="inlineStr"/>
-      <c r="AK8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AL8" t="inlineStr"/>
-      <c r="AM8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="n">
         <v>929</v>
       </c>
@@ -1772,10 +1796,10 @@
       <c r="AR8" t="n">
         <v>929</v>
       </c>
-      <c r="AS8" t="inlineStr"/>
-      <c r="AT8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT8" t="inlineStr"/>
       <c r="AU8" t="n">
         <v>929</v>
       </c>
@@ -1792,6 +1816,9 @@
         <v>929</v>
       </c>
       <c r="AZ8" t="n">
+        <v>929</v>
+      </c>
+      <c r="BA8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1801,17 +1828,17 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (M, 36, count)</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="n">
-        <v>299</v>
-      </c>
+      <c r="B9" t="n">
+        <v>299</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>299</v>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>299</v>
-      </c>
+      <c r="E9" t="n">
+        <v>299</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>299</v>
       </c>
@@ -1899,10 +1926,10 @@
       <c r="AI9" t="n">
         <v>299</v>
       </c>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="n">
         <v>299</v>
       </c>
@@ -1924,10 +1951,10 @@
       <c r="AR9" t="n">
         <v>299</v>
       </c>
-      <c r="AS9" t="inlineStr"/>
-      <c r="AT9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AS9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT9" t="inlineStr"/>
       <c r="AU9" t="n">
         <v>299</v>
       </c>
@@ -1944,6 +1971,9 @@
         <v>299</v>
       </c>
       <c r="AZ9" t="n">
+        <v>299</v>
+      </c>
+      <c r="BA9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1953,18 +1983,18 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (XXL, 22, count)</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="n">
-        <v>299</v>
-      </c>
+      <c r="B10" t="n">
+        <v>299</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>299</v>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>299</v>
+      </c>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>299</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>299</v>
       </c>
@@ -2019,10 +2049,10 @@
       <c r="Y10" t="n">
         <v>299</v>
       </c>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="n">
-        <v>299</v>
-      </c>
+      <c r="Z10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="n">
         <v>299</v>
       </c>
@@ -2047,14 +2077,14 @@
       <c r="AI10" t="n">
         <v>299</v>
       </c>
-      <c r="AJ10" t="inlineStr"/>
-      <c r="AK10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AL10" t="inlineStr"/>
-      <c r="AM10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM10" t="inlineStr"/>
       <c r="AN10" t="n">
         <v>299</v>
       </c>
@@ -2070,10 +2100,10 @@
       <c r="AR10" t="n">
         <v>299</v>
       </c>
-      <c r="AS10" t="inlineStr"/>
-      <c r="AT10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AS10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT10" t="inlineStr"/>
       <c r="AU10" t="n">
         <v>299</v>
       </c>
@@ -2090,6 +2120,9 @@
         <v>299</v>
       </c>
       <c r="AZ10" t="n">
+        <v>299</v>
+      </c>
+      <c r="BA10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2099,10 +2132,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 234 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="n">
+      <c r="B11" t="n">
         <v>2997</v>
       </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>2997</v>
       </c>
@@ -2202,10 +2235,10 @@
       <c r="AJ11" t="n">
         <v>2997</v>
       </c>
-      <c r="AK11" t="inlineStr"/>
-      <c r="AL11" t="n">
+      <c r="AK11" t="n">
         <v>2997</v>
       </c>
+      <c r="AL11" t="inlineStr"/>
       <c r="AM11" t="n">
         <v>2997</v>
       </c>
@@ -2219,15 +2252,15 @@
         <v>2997</v>
       </c>
       <c r="AQ11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AR11" t="n">
         <v>929</v>
       </c>
-      <c r="AS11" t="inlineStr"/>
-      <c r="AT11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT11" t="inlineStr"/>
       <c r="AU11" t="n">
         <v>929</v>
       </c>
@@ -2244,6 +2277,9 @@
         <v>929</v>
       </c>
       <c r="AZ11" t="n">
+        <v>929</v>
+      </c>
+      <c r="BA11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2253,10 +2289,10 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Medium (M) Size (6-11 kg), 56 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="n">
-        <v>569</v>
-      </c>
+      <c r="B12" t="n">
+        <v>569</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
         <v>569</v>
       </c>
@@ -2359,10 +2395,10 @@
       <c r="AK12" t="n">
         <v>569</v>
       </c>
-      <c r="AL12" t="inlineStr"/>
-      <c r="AM12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM12" t="inlineStr"/>
       <c r="AN12" t="n">
         <v>569</v>
       </c>
@@ -2378,10 +2414,10 @@
       <c r="AR12" t="n">
         <v>569</v>
       </c>
-      <c r="AS12" t="inlineStr"/>
-      <c r="AT12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AS12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT12" t="inlineStr"/>
       <c r="AU12" t="n">
         <v>569</v>
       </c>
@@ -2398,6 +2434,9 @@
         <v>569</v>
       </c>
       <c r="AZ12" t="n">
+        <v>569</v>
+      </c>
+      <c r="BA12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2407,17 +2446,17 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="n">
+        <v>569</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>569</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>569</v>
-      </c>
+      <c r="E13" t="n">
+        <v>569</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>569</v>
       </c>
@@ -2454,10 +2493,10 @@
       <c r="R13" t="n">
         <v>569</v>
       </c>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="n">
-        <v>569</v>
-      </c>
+      <c r="S13" t="n">
+        <v>569</v>
+      </c>
+      <c r="T13" t="inlineStr"/>
       <c r="U13" t="n">
         <v>569</v>
       </c>
@@ -2503,14 +2542,14 @@
       <c r="AI13" t="n">
         <v>569</v>
       </c>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AL13" t="inlineStr"/>
-      <c r="AM13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM13" t="inlineStr"/>
       <c r="AN13" t="n">
         <v>569</v>
       </c>
@@ -2526,24 +2565,27 @@
       <c r="AR13" t="n">
         <v>569</v>
       </c>
-      <c r="AS13" t="inlineStr"/>
-      <c r="AT13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AS13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT13" t="inlineStr"/>
       <c r="AU13" t="n">
         <v>569</v>
       </c>
       <c r="AV13" t="n">
         <v>569</v>
       </c>
-      <c r="AW13" t="inlineStr"/>
-      <c r="AX13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AW13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX13" t="inlineStr"/>
       <c r="AY13" t="n">
         <v>569</v>
       </c>
       <c r="AZ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BA13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2556,17 +2598,17 @@
       <c r="B14" t="n">
         <v>794</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="n">
+      <c r="C14" t="n">
         <v>794</v>
       </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>794</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
+      <c r="F14" t="n">
         <v>794</v>
       </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
         <v>794</v>
       </c>
@@ -2621,10 +2663,10 @@
       <c r="Y14" t="n">
         <v>794</v>
       </c>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="n">
+      <c r="Z14" t="n">
         <v>794</v>
       </c>
+      <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="n">
         <v>794</v>
       </c>
@@ -2632,7 +2674,7 @@
         <v>794</v>
       </c>
       <c r="AD14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AE14" t="n">
         <v>499</v>
@@ -2649,11 +2691,11 @@
       <c r="AI14" t="n">
         <v>499</v>
       </c>
-      <c r="AJ14" t="inlineStr"/>
+      <c r="AJ14" t="n">
+        <v>499</v>
+      </c>
       <c r="AK14" t="inlineStr"/>
-      <c r="AL14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AL14" t="inlineStr"/>
       <c r="AM14" t="n">
         <v>499</v>
       </c>
@@ -2694,6 +2736,9 @@
         <v>499</v>
       </c>
       <c r="AZ14" t="n">
+        <v>499</v>
+      </c>
+      <c r="BA14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2703,16 +2748,16 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 72 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>499</v>
+      </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="n">
-        <v>499</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>499</v>
+      </c>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>499</v>
-      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
         <v>499</v>
       </c>
@@ -2803,10 +2848,10 @@
       <c r="AK15" t="n">
         <v>499</v>
       </c>
-      <c r="AL15" t="inlineStr"/>
-      <c r="AM15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AL15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM15" t="inlineStr"/>
       <c r="AN15" t="n">
         <v>499</v>
       </c>
@@ -2816,14 +2861,14 @@
       <c r="AP15" t="n">
         <v>499</v>
       </c>
-      <c r="AQ15" t="inlineStr"/>
-      <c r="AR15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AS15" t="inlineStr"/>
-      <c r="AT15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AQ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR15" t="inlineStr"/>
+      <c r="AS15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT15" t="inlineStr"/>
       <c r="AU15" t="n">
         <v>499</v>
       </c>
@@ -2840,6 +2885,9 @@
         <v>499</v>
       </c>
       <c r="AZ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="BA15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2852,14 +2900,14 @@
       <c r="B16" t="n">
         <v>299</v>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
-        <v>299</v>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>299</v>
-      </c>
+      <c r="C16" t="n">
+        <v>299</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>299</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>299</v>
       </c>
@@ -2938,17 +2986,17 @@
       <c r="AF16" t="n">
         <v>299</v>
       </c>
-      <c r="AG16" t="inlineStr"/>
-      <c r="AH16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AG16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AH16" t="inlineStr"/>
       <c r="AI16" t="n">
         <v>299</v>
       </c>
-      <c r="AJ16" t="inlineStr"/>
-      <c r="AK16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="n">
         <v>299</v>
       </c>
@@ -2970,10 +3018,10 @@
       <c r="AR16" t="n">
         <v>299</v>
       </c>
-      <c r="AS16" t="inlineStr"/>
-      <c r="AT16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AS16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT16" t="inlineStr"/>
       <c r="AU16" t="n">
         <v>299</v>
       </c>
@@ -2990,6 +3038,9 @@
         <v>299</v>
       </c>
       <c r="AZ16" t="n">
+        <v>299</v>
+      </c>
+      <c r="BA16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2999,10 +3050,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Small (S) Size (4-8 kg), 156 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="n">
-        <v>929</v>
-      </c>
+      <c r="B17" t="n">
+        <v>929</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
         <v>929</v>
       </c>
@@ -3105,10 +3156,10 @@
       <c r="AK17" t="n">
         <v>929</v>
       </c>
-      <c r="AL17" t="inlineStr"/>
-      <c r="AM17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM17" t="inlineStr"/>
       <c r="AN17" t="n">
         <v>929</v>
       </c>
@@ -3124,10 +3175,10 @@
       <c r="AR17" t="n">
         <v>929</v>
       </c>
-      <c r="AS17" t="inlineStr"/>
-      <c r="AT17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT17" t="inlineStr"/>
       <c r="AU17" t="n">
         <v>929</v>
       </c>
@@ -3144,6 +3195,9 @@
         <v>929</v>
       </c>
       <c r="AZ17" t="n">
+        <v>929</v>
+      </c>
+      <c r="BA17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3153,18 +3207,18 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 54 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="n">
-        <v>499</v>
-      </c>
+      <c r="B18" t="n">
+        <v>499</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
         <v>499</v>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>499</v>
+      </c>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="n">
-        <v>499</v>
-      </c>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
         <v>499</v>
       </c>
@@ -3252,11 +3306,11 @@
       <c r="AJ18" t="n">
         <v>499</v>
       </c>
-      <c r="AK18" t="inlineStr"/>
+      <c r="AK18" t="n">
+        <v>499</v>
+      </c>
       <c r="AL18" t="inlineStr"/>
-      <c r="AM18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AM18" t="inlineStr"/>
       <c r="AN18" t="n">
         <v>499</v>
       </c>
@@ -3272,10 +3326,10 @@
       <c r="AR18" t="n">
         <v>499</v>
       </c>
-      <c r="AS18" t="inlineStr"/>
-      <c r="AT18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AS18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT18" t="inlineStr"/>
       <c r="AU18" t="n">
         <v>499</v>
       </c>
@@ -3292,6 +3346,9 @@
         <v>499</v>
       </c>
       <c r="AZ18" t="n">
+        <v>499</v>
+      </c>
+      <c r="BA18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3301,18 +3358,18 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="n">
+        <v>1299</v>
+      </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>1299</v>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
         <v>1299</v>
       </c>
@@ -3392,7 +3449,7 @@
         <v>1299</v>
       </c>
       <c r="AH19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AI19" t="n">
         <v>1497</v>
@@ -3400,13 +3457,13 @@
       <c r="AJ19" t="n">
         <v>1497</v>
       </c>
-      <c r="AK19" t="inlineStr"/>
+      <c r="AK19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AL19" t="inlineStr"/>
-      <c r="AM19" t="n">
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="n">
         <v>465</v>
-      </c>
-      <c r="AN19" t="n">
-        <v>1497</v>
       </c>
       <c r="AO19" t="n">
         <v>1497</v>
@@ -3442,6 +3499,9 @@
         <v>1497</v>
       </c>
       <c r="AZ19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="BA19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3580,10 +3640,10 @@
       <c r="AR20" t="n">
         <v>929</v>
       </c>
-      <c r="AS20" t="inlineStr"/>
-      <c r="AT20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT20" t="inlineStr"/>
       <c r="AU20" t="n">
         <v>929</v>
       </c>
@@ -3600,6 +3660,9 @@
         <v>929</v>
       </c>
       <c r="AZ20" t="n">
+        <v>929</v>
+      </c>
+      <c r="BA20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3609,24 +3672,24 @@
           <t>Jr. Sr. Baby Diaper Pants | Large (L) Size (9-14 kg), 62 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>499</v>
-      </c>
+      <c r="B21" t="n">
+        <v>499</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>499</v>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>499</v>
-      </c>
+      <c r="E21" t="n">
+        <v>499</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
         <v>499</v>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="n">
-        <v>499</v>
-      </c>
+      <c r="H21" t="n">
+        <v>499</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
         <v>499</v>
       </c>
@@ -3681,10 +3744,10 @@
       <c r="AA21" t="n">
         <v>499</v>
       </c>
-      <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AB21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="n">
         <v>499</v>
       </c>
@@ -3709,10 +3772,10 @@
       <c r="AK21" t="n">
         <v>499</v>
       </c>
-      <c r="AL21" t="inlineStr"/>
-      <c r="AM21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AL21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM21" t="inlineStr"/>
       <c r="AN21" t="n">
         <v>499</v>
       </c>
@@ -3750,6 +3813,9 @@
         <v>499</v>
       </c>
       <c r="AZ21" t="n">
+        <v>499</v>
+      </c>
+      <c r="BA21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3759,11 +3825,11 @@
           <t>Jr. Sr. Baby Diaper Pants | 10-12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy (L, 32, count)</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="n">
+        <v>299</v>
+      </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="n">
-        <v>299</v>
-      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
         <v>299</v>
       </c>
@@ -3857,14 +3923,14 @@
       <c r="AI22" t="n">
         <v>299</v>
       </c>
-      <c r="AJ22" t="inlineStr"/>
-      <c r="AK22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AL22" t="inlineStr"/>
-      <c r="AM22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK22" t="inlineStr"/>
+      <c r="AL22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM22" t="inlineStr"/>
       <c r="AN22" t="n">
         <v>299</v>
       </c>
@@ -3880,10 +3946,10 @@
       <c r="AR22" t="n">
         <v>299</v>
       </c>
-      <c r="AS22" t="inlineStr"/>
-      <c r="AT22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AS22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AT22" t="inlineStr"/>
       <c r="AU22" t="n">
         <v>299</v>
       </c>
@@ -3900,6 +3966,9 @@
         <v>299</v>
       </c>
       <c r="AZ22" t="n">
+        <v>299</v>
+      </c>
+      <c r="BA22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3909,18 +3978,18 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 216 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
         <v>1299</v>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>1299</v>
+      </c>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
         <v>1299</v>
       </c>
@@ -4008,11 +4077,11 @@
       <c r="AJ23" t="n">
         <v>1299</v>
       </c>
-      <c r="AK23" t="inlineStr"/>
+      <c r="AK23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AL23" t="inlineStr"/>
-      <c r="AM23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AM23" t="inlineStr"/>
       <c r="AN23" t="n">
         <v>1299</v>
       </c>
@@ -4028,10 +4097,10 @@
       <c r="AR23" t="n">
         <v>1299</v>
       </c>
-      <c r="AS23" t="inlineStr"/>
-      <c r="AT23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AS23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AT23" t="inlineStr"/>
       <c r="AU23" t="n">
         <v>1299</v>
       </c>
@@ -4048,6 +4117,9 @@
         <v>1299</v>
       </c>
       <c r="AZ23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BA23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -4066,11 +4138,11 @@
       <c r="D24" t="n">
         <v>929</v>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>929</v>
+      </c>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="n">
-        <v>929</v>
-      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
         <v>929</v>
       </c>
@@ -4155,11 +4227,11 @@
       <c r="AI24" t="n">
         <v>929</v>
       </c>
-      <c r="AJ24" t="inlineStr"/>
+      <c r="AJ24" t="n">
+        <v>929</v>
+      </c>
       <c r="AK24" t="inlineStr"/>
-      <c r="AL24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL24" t="inlineStr"/>
       <c r="AM24" t="n">
         <v>929</v>
       </c>
@@ -4178,10 +4250,10 @@
       <c r="AR24" t="n">
         <v>929</v>
       </c>
-      <c r="AS24" t="inlineStr"/>
-      <c r="AT24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT24" t="inlineStr"/>
       <c r="AU24" t="n">
         <v>929</v>
       </c>
@@ -4198,6 +4270,9 @@
         <v>929</v>
       </c>
       <c r="AZ24" t="n">
+        <v>929</v>
+      </c>
+      <c r="BA24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4207,18 +4282,18 @@
           <t>Jr. Sr. Baby Diaper Pants | Medium (M) Size (7-12 kg), 144 Count | Pack of 2 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="n">
-        <v>929</v>
-      </c>
+      <c r="B25" t="n">
+        <v>929</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
         <v>929</v>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>929</v>
+      </c>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
-        <v>929</v>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
         <v>929</v>
       </c>
@@ -4228,10 +4303,10 @@
       <c r="J25" t="n">
         <v>929</v>
       </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="n">
-        <v>929</v>
-      </c>
+      <c r="K25" t="n">
+        <v>929</v>
+      </c>
+      <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
         <v>929</v>
       </c>
@@ -4301,11 +4376,11 @@
       <c r="AI25" t="n">
         <v>929</v>
       </c>
-      <c r="AJ25" t="inlineStr"/>
+      <c r="AJ25" t="n">
+        <v>929</v>
+      </c>
       <c r="AK25" t="inlineStr"/>
-      <c r="AL25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL25" t="inlineStr"/>
       <c r="AM25" t="n">
         <v>929</v>
       </c>
@@ -4324,10 +4399,10 @@
       <c r="AR25" t="n">
         <v>929</v>
       </c>
-      <c r="AS25" t="inlineStr"/>
-      <c r="AT25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT25" t="inlineStr"/>
       <c r="AU25" t="n">
         <v>929</v>
       </c>
@@ -4344,6 +4419,9 @@
         <v>929</v>
       </c>
       <c r="AZ25" t="n">
+        <v>929</v>
+      </c>
+      <c r="BA25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4362,10 +4440,10 @@
       <c r="D26" t="n">
         <v>1299</v>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
         <v>1299</v>
       </c>
@@ -4375,10 +4453,10 @@
       <c r="I26" t="n">
         <v>1299</v>
       </c>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="J26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="n">
         <v>1299</v>
       </c>
@@ -4451,14 +4529,14 @@
       <c r="AI26" t="n">
         <v>1299</v>
       </c>
-      <c r="AJ26" t="inlineStr"/>
-      <c r="AK26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AL26" t="inlineStr"/>
-      <c r="AM26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AJ26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AK26" t="inlineStr"/>
+      <c r="AL26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AM26" t="inlineStr"/>
       <c r="AN26" t="n">
         <v>1299</v>
       </c>
@@ -4474,10 +4552,10 @@
       <c r="AR26" t="n">
         <v>1299</v>
       </c>
-      <c r="AS26" t="inlineStr"/>
-      <c r="AT26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AS26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AT26" t="inlineStr"/>
       <c r="AU26" t="n">
         <v>1299</v>
       </c>
@@ -4494,6 +4572,9 @@
         <v>1299</v>
       </c>
       <c r="AZ26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BA26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-25 03:59
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA26"/>
+  <dimension ref="A1:BB26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,7 @@
     <col width="21" customWidth="1" min="51" max="51"/>
     <col width="21" customWidth="1" min="52" max="52"/>
     <col width="21" customWidth="1" min="53" max="53"/>
+    <col width="21" customWidth="1" min="54" max="54"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -496,260 +497,265 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 09:25</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-25 04:11</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 02:11</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 00:27</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -851,10 +857,10 @@
       <c r="AE2" t="n">
         <v>929</v>
       </c>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AF2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="n">
         <v>929</v>
       </c>
@@ -867,25 +873,25 @@
       <c r="AK2" t="n">
         <v>929</v>
       </c>
-      <c r="AL2" t="inlineStr"/>
+      <c r="AL2" t="n">
+        <v>929</v>
+      </c>
       <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN2" t="inlineStr"/>
       <c r="AO2" t="n">
         <v>929</v>
       </c>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="n">
         <v>929</v>
       </c>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT2" t="inlineStr"/>
       <c r="AU2" t="n">
         <v>929</v>
       </c>
@@ -905,6 +911,9 @@
         <v>929</v>
       </c>
       <c r="BA2" t="n">
+        <v>929</v>
+      </c>
+      <c r="BB2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -917,20 +926,20 @@
       <c r="B3" t="n">
         <v>569</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>569</v>
-      </c>
+      <c r="C3" t="n">
+        <v>569</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>569</v>
       </c>
       <c r="F3" t="n">
         <v>569</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>569</v>
-      </c>
+      <c r="G3" t="n">
+        <v>569</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>569</v>
       </c>
@@ -949,10 +958,10 @@
       <c r="N3" t="n">
         <v>569</v>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="n">
-        <v>569</v>
-      </c>
+      <c r="O3" t="n">
+        <v>569</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="n">
         <v>569</v>
       </c>
@@ -995,26 +1004,26 @@
       <c r="AD3" t="n">
         <v>569</v>
       </c>
-      <c r="AE3" t="inlineStr"/>
+      <c r="AE3" t="n">
+        <v>569</v>
+      </c>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AH3" t="inlineStr"/>
       <c r="AI3" t="n">
         <v>569</v>
       </c>
       <c r="AJ3" t="n">
         <v>569</v>
       </c>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN3" t="inlineStr"/>
       <c r="AO3" t="n">
         <v>569</v>
       </c>
@@ -1030,10 +1039,10 @@
       <c r="AS3" t="n">
         <v>569</v>
       </c>
-      <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AT3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU3" t="inlineStr"/>
       <c r="AV3" t="n">
         <v>569</v>
       </c>
@@ -1050,6 +1059,9 @@
         <v>569</v>
       </c>
       <c r="BA3" t="n">
+        <v>569</v>
+      </c>
+      <c r="BB3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1065,10 +1077,10 @@
       <c r="C4" t="n">
         <v>299</v>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
-        <v>299</v>
-      </c>
+      <c r="D4" t="n">
+        <v>299</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
         <v>299</v>
       </c>
@@ -1162,10 +1174,10 @@
       <c r="AJ4" t="n">
         <v>299</v>
       </c>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="n">
         <v>299</v>
       </c>
@@ -1187,10 +1199,10 @@
       <c r="AS4" t="n">
         <v>299</v>
       </c>
-      <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AT4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU4" t="inlineStr"/>
       <c r="AV4" t="n">
         <v>299</v>
       </c>
@@ -1207,6 +1219,9 @@
         <v>299</v>
       </c>
       <c r="BA4" t="n">
+        <v>299</v>
+      </c>
+      <c r="BB4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1219,11 +1234,11 @@
       <c r="B5" t="n">
         <v>569</v>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>569</v>
+      </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="n">
-        <v>569</v>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>569</v>
       </c>
@@ -1245,10 +1260,10 @@
       <c r="L5" t="n">
         <v>569</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="n">
-        <v>569</v>
-      </c>
+      <c r="M5" t="n">
+        <v>569</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
         <v>569</v>
       </c>
@@ -1342,10 +1357,10 @@
       <c r="AS5" t="n">
         <v>569</v>
       </c>
-      <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AT5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU5" t="inlineStr"/>
       <c r="AV5" t="n">
         <v>569</v>
       </c>
@@ -1362,6 +1377,9 @@
         <v>569</v>
       </c>
       <c r="BA5" t="n">
+        <v>569</v>
+      </c>
+      <c r="BB5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1377,15 +1395,15 @@
       <c r="C6" t="n">
         <v>499</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
-        <v>499</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>499</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>499</v>
+      </c>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
-        <v>499</v>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>499</v>
       </c>
@@ -1473,10 +1491,10 @@
       <c r="AK6" t="n">
         <v>499</v>
       </c>
-      <c r="AL6" t="inlineStr"/>
-      <c r="AM6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AL6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="n">
         <v>499</v>
       </c>
@@ -1495,10 +1513,10 @@
       <c r="AS6" t="n">
         <v>499</v>
       </c>
-      <c r="AT6" t="inlineStr"/>
-      <c r="AU6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AT6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU6" t="inlineStr"/>
       <c r="AV6" t="n">
         <v>499</v>
       </c>
@@ -1515,6 +1533,9 @@
         <v>499</v>
       </c>
       <c r="BA6" t="n">
+        <v>499</v>
+      </c>
+      <c r="BB6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1527,20 +1548,20 @@
       <c r="B7" t="n">
         <v>569</v>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
-        <v>569</v>
-      </c>
+      <c r="C7" t="n">
+        <v>569</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
         <v>569</v>
       </c>
       <c r="F7" t="n">
         <v>569</v>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>569</v>
-      </c>
+      <c r="G7" t="n">
+        <v>569</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
         <v>569</v>
       </c>
@@ -1625,12 +1646,12 @@
       <c r="AJ7" t="n">
         <v>569</v>
       </c>
-      <c r="AK7" t="inlineStr"/>
+      <c r="AK7" t="n">
+        <v>569</v>
+      </c>
       <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="inlineStr"/>
-      <c r="AN7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN7" t="inlineStr"/>
       <c r="AO7" t="n">
         <v>569</v>
       </c>
@@ -1646,10 +1667,10 @@
       <c r="AS7" t="n">
         <v>569</v>
       </c>
-      <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AT7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU7" t="inlineStr"/>
       <c r="AV7" t="n">
         <v>569</v>
       </c>
@@ -1666,6 +1687,9 @@
         <v>569</v>
       </c>
       <c r="BA7" t="n">
+        <v>569</v>
+      </c>
+      <c r="BB7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1678,20 +1702,20 @@
       <c r="B8" t="n">
         <v>929</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
-        <v>929</v>
-      </c>
+      <c r="C8" t="n">
+        <v>929</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>929</v>
       </c>
       <c r="F8" t="n">
         <v>929</v>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>929</v>
-      </c>
+      <c r="G8" t="n">
+        <v>929</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>929</v>
       </c>
@@ -1776,14 +1800,14 @@
       <c r="AJ8" t="n">
         <v>929</v>
       </c>
-      <c r="AK8" t="inlineStr"/>
-      <c r="AL8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AM8" t="inlineStr"/>
-      <c r="AN8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN8" t="inlineStr"/>
       <c r="AO8" t="n">
         <v>929</v>
       </c>
@@ -1799,10 +1823,10 @@
       <c r="AS8" t="n">
         <v>929</v>
       </c>
-      <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AT8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU8" t="inlineStr"/>
       <c r="AV8" t="n">
         <v>929</v>
       </c>
@@ -1819,6 +1843,9 @@
         <v>929</v>
       </c>
       <c r="BA8" t="n">
+        <v>929</v>
+      </c>
+      <c r="BB8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1831,17 +1858,17 @@
       <c r="B9" t="n">
         <v>299</v>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
-        <v>299</v>
-      </c>
+      <c r="C9" t="n">
+        <v>299</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
         <v>299</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>299</v>
-      </c>
+      <c r="F9" t="n">
+        <v>299</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>299</v>
       </c>
@@ -1929,10 +1956,10 @@
       <c r="AJ9" t="n">
         <v>299</v>
       </c>
-      <c r="AK9" t="inlineStr"/>
-      <c r="AL9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="n">
         <v>299</v>
       </c>
@@ -1954,10 +1981,10 @@
       <c r="AS9" t="n">
         <v>299</v>
       </c>
-      <c r="AT9" t="inlineStr"/>
-      <c r="AU9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AT9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU9" t="inlineStr"/>
       <c r="AV9" t="n">
         <v>299</v>
       </c>
@@ -1974,6 +2001,9 @@
         <v>299</v>
       </c>
       <c r="BA9" t="n">
+        <v>299</v>
+      </c>
+      <c r="BB9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1986,18 +2016,18 @@
       <c r="B10" t="n">
         <v>299</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>299</v>
-      </c>
+      <c r="C10" t="n">
+        <v>299</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
         <v>299</v>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>299</v>
+      </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>299</v>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>299</v>
       </c>
@@ -2052,10 +2082,10 @@
       <c r="Z10" t="n">
         <v>299</v>
       </c>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AA10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="n">
         <v>299</v>
       </c>
@@ -2080,14 +2110,14 @@
       <c r="AJ10" t="n">
         <v>299</v>
       </c>
-      <c r="AK10" t="inlineStr"/>
-      <c r="AL10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AM10" t="inlineStr"/>
-      <c r="AN10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN10" t="inlineStr"/>
       <c r="AO10" t="n">
         <v>299</v>
       </c>
@@ -2103,10 +2133,10 @@
       <c r="AS10" t="n">
         <v>299</v>
       </c>
-      <c r="AT10" t="inlineStr"/>
-      <c r="AU10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AT10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU10" t="inlineStr"/>
       <c r="AV10" t="n">
         <v>299</v>
       </c>
@@ -2123,6 +2153,9 @@
         <v>299</v>
       </c>
       <c r="BA10" t="n">
+        <v>299</v>
+      </c>
+      <c r="BB10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2135,10 +2168,10 @@
       <c r="B11" t="n">
         <v>2997</v>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
+      <c r="C11" t="n">
         <v>2997</v>
       </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
         <v>2997</v>
       </c>
@@ -2238,10 +2271,10 @@
       <c r="AK11" t="n">
         <v>2997</v>
       </c>
-      <c r="AL11" t="inlineStr"/>
-      <c r="AM11" t="n">
+      <c r="AL11" t="n">
         <v>2997</v>
       </c>
+      <c r="AM11" t="inlineStr"/>
       <c r="AN11" t="n">
         <v>2997</v>
       </c>
@@ -2255,15 +2288,15 @@
         <v>2997</v>
       </c>
       <c r="AR11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AS11" t="n">
         <v>929</v>
       </c>
-      <c r="AT11" t="inlineStr"/>
-      <c r="AU11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AT11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU11" t="inlineStr"/>
       <c r="AV11" t="n">
         <v>929</v>
       </c>
@@ -2280,6 +2313,9 @@
         <v>929</v>
       </c>
       <c r="BA11" t="n">
+        <v>929</v>
+      </c>
+      <c r="BB11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2292,10 +2328,10 @@
       <c r="B12" t="n">
         <v>569</v>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="n">
-        <v>569</v>
-      </c>
+      <c r="C12" t="n">
+        <v>569</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
         <v>569</v>
       </c>
@@ -2398,10 +2434,10 @@
       <c r="AL12" t="n">
         <v>569</v>
       </c>
-      <c r="AM12" t="inlineStr"/>
-      <c r="AN12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN12" t="inlineStr"/>
       <c r="AO12" t="n">
         <v>569</v>
       </c>
@@ -2417,10 +2453,10 @@
       <c r="AS12" t="n">
         <v>569</v>
       </c>
-      <c r="AT12" t="inlineStr"/>
-      <c r="AU12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AT12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU12" t="inlineStr"/>
       <c r="AV12" t="n">
         <v>569</v>
       </c>
@@ -2437,6 +2473,9 @@
         <v>569</v>
       </c>
       <c r="BA12" t="n">
+        <v>569</v>
+      </c>
+      <c r="BB12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2449,17 +2488,17 @@
       <c r="B13" t="n">
         <v>569</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>569</v>
-      </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>569</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>569</v>
-      </c>
+      <c r="F13" t="n">
+        <v>569</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>569</v>
       </c>
@@ -2496,10 +2535,10 @@
       <c r="S13" t="n">
         <v>569</v>
       </c>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="n">
-        <v>569</v>
-      </c>
+      <c r="T13" t="n">
+        <v>569</v>
+      </c>
+      <c r="U13" t="inlineStr"/>
       <c r="V13" t="n">
         <v>569</v>
       </c>
@@ -2545,14 +2584,14 @@
       <c r="AJ13" t="n">
         <v>569</v>
       </c>
-      <c r="AK13" t="inlineStr"/>
-      <c r="AL13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AM13" t="inlineStr"/>
-      <c r="AN13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN13" t="inlineStr"/>
       <c r="AO13" t="n">
         <v>569</v>
       </c>
@@ -2568,24 +2607,27 @@
       <c r="AS13" t="n">
         <v>569</v>
       </c>
-      <c r="AT13" t="inlineStr"/>
-      <c r="AU13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AT13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AU13" t="inlineStr"/>
       <c r="AV13" t="n">
         <v>569</v>
       </c>
       <c r="AW13" t="n">
         <v>569</v>
       </c>
-      <c r="AX13" t="inlineStr"/>
-      <c r="AY13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AX13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY13" t="inlineStr"/>
       <c r="AZ13" t="n">
         <v>569</v>
       </c>
       <c r="BA13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BB13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2601,17 +2643,17 @@
       <c r="C14" t="n">
         <v>794</v>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>794</v>
       </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
         <v>794</v>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="n">
+      <c r="G14" t="n">
         <v>794</v>
       </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
         <v>794</v>
       </c>
@@ -2666,10 +2708,10 @@
       <c r="Z14" t="n">
         <v>794</v>
       </c>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="n">
+      <c r="AA14" t="n">
         <v>794</v>
       </c>
+      <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="n">
         <v>794</v>
       </c>
@@ -2677,7 +2719,7 @@
         <v>794</v>
       </c>
       <c r="AE14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AF14" t="n">
         <v>499</v>
@@ -2694,11 +2736,11 @@
       <c r="AJ14" t="n">
         <v>499</v>
       </c>
-      <c r="AK14" t="inlineStr"/>
+      <c r="AK14" t="n">
+        <v>499</v>
+      </c>
       <c r="AL14" t="inlineStr"/>
-      <c r="AM14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AM14" t="inlineStr"/>
       <c r="AN14" t="n">
         <v>499</v>
       </c>
@@ -2739,6 +2781,9 @@
         <v>499</v>
       </c>
       <c r="BA14" t="n">
+        <v>499</v>
+      </c>
+      <c r="BB14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2751,16 +2796,16 @@
       <c r="B15" t="n">
         <v>499</v>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>499</v>
+      </c>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>499</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>499</v>
+      </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="n">
-        <v>499</v>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
         <v>499</v>
       </c>
@@ -2851,10 +2896,10 @@
       <c r="AL15" t="n">
         <v>499</v>
       </c>
-      <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AM15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN15" t="inlineStr"/>
       <c r="AO15" t="n">
         <v>499</v>
       </c>
@@ -2864,14 +2909,14 @@
       <c r="AQ15" t="n">
         <v>499</v>
       </c>
-      <c r="AR15" t="inlineStr"/>
-      <c r="AS15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AT15" t="inlineStr"/>
-      <c r="AU15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AR15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AS15" t="inlineStr"/>
+      <c r="AT15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU15" t="inlineStr"/>
       <c r="AV15" t="n">
         <v>499</v>
       </c>
@@ -2888,6 +2933,9 @@
         <v>499</v>
       </c>
       <c r="BA15" t="n">
+        <v>499</v>
+      </c>
+      <c r="BB15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2903,14 +2951,14 @@
       <c r="C16" t="n">
         <v>299</v>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>299</v>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>299</v>
-      </c>
+      <c r="D16" t="n">
+        <v>299</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>299</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
         <v>299</v>
       </c>
@@ -2989,17 +3037,17 @@
       <c r="AG16" t="n">
         <v>299</v>
       </c>
-      <c r="AH16" t="inlineStr"/>
-      <c r="AI16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AH16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AI16" t="inlineStr"/>
       <c r="AJ16" t="n">
         <v>299</v>
       </c>
-      <c r="AK16" t="inlineStr"/>
-      <c r="AL16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="n">
         <v>299</v>
       </c>
@@ -3021,10 +3069,10 @@
       <c r="AS16" t="n">
         <v>299</v>
       </c>
-      <c r="AT16" t="inlineStr"/>
-      <c r="AU16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AT16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU16" t="inlineStr"/>
       <c r="AV16" t="n">
         <v>299</v>
       </c>
@@ -3041,6 +3089,9 @@
         <v>299</v>
       </c>
       <c r="BA16" t="n">
+        <v>299</v>
+      </c>
+      <c r="BB16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3053,10 +3104,10 @@
       <c r="B17" t="n">
         <v>929</v>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="n">
-        <v>929</v>
-      </c>
+      <c r="C17" t="n">
+        <v>929</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
         <v>929</v>
       </c>
@@ -3159,10 +3210,10 @@
       <c r="AL17" t="n">
         <v>929</v>
       </c>
-      <c r="AM17" t="inlineStr"/>
-      <c r="AN17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN17" t="inlineStr"/>
       <c r="AO17" t="n">
         <v>929</v>
       </c>
@@ -3178,10 +3229,10 @@
       <c r="AS17" t="n">
         <v>929</v>
       </c>
-      <c r="AT17" t="inlineStr"/>
-      <c r="AU17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AT17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU17" t="inlineStr"/>
       <c r="AV17" t="n">
         <v>929</v>
       </c>
@@ -3198,6 +3249,9 @@
         <v>929</v>
       </c>
       <c r="BA17" t="n">
+        <v>929</v>
+      </c>
+      <c r="BB17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3210,18 +3264,18 @@
       <c r="B18" t="n">
         <v>499</v>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="n">
-        <v>499</v>
-      </c>
+      <c r="C18" t="n">
+        <v>499</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>499</v>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>499</v>
+      </c>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="n">
-        <v>499</v>
-      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
         <v>499</v>
       </c>
@@ -3309,11 +3363,11 @@
       <c r="AK18" t="n">
         <v>499</v>
       </c>
-      <c r="AL18" t="inlineStr"/>
+      <c r="AL18" t="n">
+        <v>499</v>
+      </c>
       <c r="AM18" t="inlineStr"/>
-      <c r="AN18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AN18" t="inlineStr"/>
       <c r="AO18" t="n">
         <v>499</v>
       </c>
@@ -3329,10 +3383,10 @@
       <c r="AS18" t="n">
         <v>499</v>
       </c>
-      <c r="AT18" t="inlineStr"/>
-      <c r="AU18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AT18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU18" t="inlineStr"/>
       <c r="AV18" t="n">
         <v>499</v>
       </c>
@@ -3349,6 +3403,9 @@
         <v>499</v>
       </c>
       <c r="BA18" t="n">
+        <v>499</v>
+      </c>
+      <c r="BB18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3361,18 +3418,18 @@
       <c r="B19" t="n">
         <v>1299</v>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>1299</v>
+      </c>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
         <v>1299</v>
       </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
         <v>1299</v>
       </c>
@@ -3452,7 +3509,7 @@
         <v>1299</v>
       </c>
       <c r="AI19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AJ19" t="n">
         <v>1497</v>
@@ -3460,13 +3517,13 @@
       <c r="AK19" t="n">
         <v>1497</v>
       </c>
-      <c r="AL19" t="inlineStr"/>
+      <c r="AL19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AM19" t="inlineStr"/>
-      <c r="AN19" t="n">
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="n">
         <v>465</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>1497</v>
       </c>
       <c r="AP19" t="n">
         <v>1497</v>
@@ -3502,6 +3559,9 @@
         <v>1497</v>
       </c>
       <c r="BA19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="BB19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3643,10 +3703,10 @@
       <c r="AS20" t="n">
         <v>929</v>
       </c>
-      <c r="AT20" t="inlineStr"/>
-      <c r="AU20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AT20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU20" t="inlineStr"/>
       <c r="AV20" t="n">
         <v>929</v>
       </c>
@@ -3663,6 +3723,9 @@
         <v>929</v>
       </c>
       <c r="BA20" t="n">
+        <v>929</v>
+      </c>
+      <c r="BB20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3675,24 +3738,24 @@
       <c r="B21" t="n">
         <v>499</v>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
-        <v>499</v>
-      </c>
+      <c r="C21" t="n">
+        <v>499</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
         <v>499</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="n">
-        <v>499</v>
-      </c>
+      <c r="F21" t="n">
+        <v>499</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
         <v>499</v>
       </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>499</v>
-      </c>
+      <c r="I21" t="n">
+        <v>499</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>499</v>
       </c>
@@ -3747,10 +3810,10 @@
       <c r="AB21" t="n">
         <v>499</v>
       </c>
-      <c r="AC21" t="inlineStr"/>
-      <c r="AD21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AC21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="n">
         <v>499</v>
       </c>
@@ -3775,10 +3838,10 @@
       <c r="AL21" t="n">
         <v>499</v>
       </c>
-      <c r="AM21" t="inlineStr"/>
-      <c r="AN21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AM21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN21" t="inlineStr"/>
       <c r="AO21" t="n">
         <v>499</v>
       </c>
@@ -3816,6 +3879,9 @@
         <v>499</v>
       </c>
       <c r="BA21" t="n">
+        <v>499</v>
+      </c>
+      <c r="BB21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3828,11 +3894,11 @@
       <c r="B22" t="n">
         <v>299</v>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>299</v>
+      </c>
       <c r="D22" t="inlineStr"/>
-      <c r="E22" t="n">
-        <v>299</v>
-      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
         <v>299</v>
       </c>
@@ -3926,14 +3992,14 @@
       <c r="AJ22" t="n">
         <v>299</v>
       </c>
-      <c r="AK22" t="inlineStr"/>
-      <c r="AL22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AM22" t="inlineStr"/>
-      <c r="AN22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL22" t="inlineStr"/>
+      <c r="AM22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN22" t="inlineStr"/>
       <c r="AO22" t="n">
         <v>299</v>
       </c>
@@ -3949,10 +4015,10 @@
       <c r="AS22" t="n">
         <v>299</v>
       </c>
-      <c r="AT22" t="inlineStr"/>
-      <c r="AU22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AT22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AU22" t="inlineStr"/>
       <c r="AV22" t="n">
         <v>299</v>
       </c>
@@ -3969,6 +4035,9 @@
         <v>299</v>
       </c>
       <c r="BA22" t="n">
+        <v>299</v>
+      </c>
+      <c r="BB22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3981,18 +4050,18 @@
       <c r="B23" t="n">
         <v>1299</v>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>1299</v>
       </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>1299</v>
+      </c>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
         <v>1299</v>
       </c>
@@ -4080,11 +4149,11 @@
       <c r="AK23" t="n">
         <v>1299</v>
       </c>
-      <c r="AL23" t="inlineStr"/>
+      <c r="AL23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AM23" t="inlineStr"/>
-      <c r="AN23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AN23" t="inlineStr"/>
       <c r="AO23" t="n">
         <v>1299</v>
       </c>
@@ -4100,10 +4169,10 @@
       <c r="AS23" t="n">
         <v>1299</v>
       </c>
-      <c r="AT23" t="inlineStr"/>
-      <c r="AU23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AT23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AU23" t="inlineStr"/>
       <c r="AV23" t="n">
         <v>1299</v>
       </c>
@@ -4120,6 +4189,9 @@
         <v>1299</v>
       </c>
       <c r="BA23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BB23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -4141,11 +4213,11 @@
       <c r="E24" t="n">
         <v>929</v>
       </c>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>929</v>
+      </c>
       <c r="G24" t="inlineStr"/>
-      <c r="H24" t="n">
-        <v>929</v>
-      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
         <v>929</v>
       </c>
@@ -4230,11 +4302,11 @@
       <c r="AJ24" t="n">
         <v>929</v>
       </c>
-      <c r="AK24" t="inlineStr"/>
+      <c r="AK24" t="n">
+        <v>929</v>
+      </c>
       <c r="AL24" t="inlineStr"/>
-      <c r="AM24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM24" t="inlineStr"/>
       <c r="AN24" t="n">
         <v>929</v>
       </c>
@@ -4253,10 +4325,10 @@
       <c r="AS24" t="n">
         <v>929</v>
       </c>
-      <c r="AT24" t="inlineStr"/>
-      <c r="AU24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AT24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU24" t="inlineStr"/>
       <c r="AV24" t="n">
         <v>929</v>
       </c>
@@ -4273,6 +4345,9 @@
         <v>929</v>
       </c>
       <c r="BA24" t="n">
+        <v>929</v>
+      </c>
+      <c r="BB24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4285,18 +4360,18 @@
       <c r="B25" t="n">
         <v>929</v>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="n">
-        <v>929</v>
-      </c>
+      <c r="C25" t="n">
+        <v>929</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
         <v>929</v>
       </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>929</v>
+      </c>
       <c r="G25" t="inlineStr"/>
-      <c r="H25" t="n">
-        <v>929</v>
-      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
         <v>929</v>
       </c>
@@ -4306,10 +4381,10 @@
       <c r="K25" t="n">
         <v>929</v>
       </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="n">
-        <v>929</v>
-      </c>
+      <c r="L25" t="n">
+        <v>929</v>
+      </c>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
         <v>929</v>
       </c>
@@ -4379,11 +4454,11 @@
       <c r="AJ25" t="n">
         <v>929</v>
       </c>
-      <c r="AK25" t="inlineStr"/>
+      <c r="AK25" t="n">
+        <v>929</v>
+      </c>
       <c r="AL25" t="inlineStr"/>
-      <c r="AM25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM25" t="inlineStr"/>
       <c r="AN25" t="n">
         <v>929</v>
       </c>
@@ -4402,10 +4477,10 @@
       <c r="AS25" t="n">
         <v>929</v>
       </c>
-      <c r="AT25" t="inlineStr"/>
-      <c r="AU25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AT25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU25" t="inlineStr"/>
       <c r="AV25" t="n">
         <v>929</v>
       </c>
@@ -4422,6 +4497,9 @@
         <v>929</v>
       </c>
       <c r="BA25" t="n">
+        <v>929</v>
+      </c>
+      <c r="BB25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4431,9 +4509,7 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="n">
         <v>1299</v>
       </c>
@@ -4443,10 +4519,10 @@
       <c r="E26" t="n">
         <v>1299</v>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
         <v>1299</v>
       </c>
@@ -4456,10 +4532,10 @@
       <c r="J26" t="n">
         <v>1299</v>
       </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="K26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
         <v>1299</v>
       </c>
@@ -4532,14 +4608,14 @@
       <c r="AJ26" t="n">
         <v>1299</v>
       </c>
-      <c r="AK26" t="inlineStr"/>
-      <c r="AL26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AM26" t="inlineStr"/>
-      <c r="AN26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AK26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AL26" t="inlineStr"/>
+      <c r="AM26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AN26" t="inlineStr"/>
       <c r="AO26" t="n">
         <v>1299</v>
       </c>
@@ -4555,10 +4631,10 @@
       <c r="AS26" t="n">
         <v>1299</v>
       </c>
-      <c r="AT26" t="inlineStr"/>
-      <c r="AU26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AT26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AU26" t="inlineStr"/>
       <c r="AV26" t="n">
         <v>1299</v>
       </c>
@@ -4575,6 +4651,9 @@
         <v>1299</v>
       </c>
       <c r="BA26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BB26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-25 05:05
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB26"/>
+  <dimension ref="A1:BC26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +487,7 @@
     <col width="21" customWidth="1" min="52" max="52"/>
     <col width="21" customWidth="1" min="53" max="53"/>
     <col width="21" customWidth="1" min="54" max="54"/>
+    <col width="21" customWidth="1" min="55" max="55"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -497,265 +498,270 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 10:31</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-25 09:25</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 04:11</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 02:11</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 00:27</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -860,10 +866,10 @@
       <c r="AF2" t="n">
         <v>929</v>
       </c>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AG2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="n">
         <v>929</v>
       </c>
@@ -876,25 +882,25 @@
       <c r="AL2" t="n">
         <v>929</v>
       </c>
-      <c r="AM2" t="inlineStr"/>
+      <c r="AM2" t="n">
+        <v>929</v>
+      </c>
       <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="n">
         <v>929</v>
       </c>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="n">
         <v>929</v>
       </c>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AT2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="n">
         <v>929</v>
       </c>
@@ -914,6 +920,9 @@
         <v>929</v>
       </c>
       <c r="BB2" t="n">
+        <v>929</v>
+      </c>
+      <c r="BC2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -929,20 +938,20 @@
       <c r="C3" t="n">
         <v>569</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>569</v>
-      </c>
+      <c r="D3" t="n">
+        <v>569</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>569</v>
       </c>
       <c r="G3" t="n">
         <v>569</v>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>569</v>
-      </c>
+      <c r="H3" t="n">
+        <v>569</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
         <v>569</v>
       </c>
@@ -961,10 +970,10 @@
       <c r="O3" t="n">
         <v>569</v>
       </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="n">
-        <v>569</v>
-      </c>
+      <c r="P3" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
         <v>569</v>
       </c>
@@ -1007,26 +1016,26 @@
       <c r="AE3" t="n">
         <v>569</v>
       </c>
-      <c r="AF3" t="inlineStr"/>
+      <c r="AF3" t="n">
+        <v>569</v>
+      </c>
       <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="n">
         <v>569</v>
       </c>
       <c r="AK3" t="n">
         <v>569</v>
       </c>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO3" t="inlineStr"/>
       <c r="AP3" t="n">
         <v>569</v>
       </c>
@@ -1042,10 +1051,10 @@
       <c r="AT3" t="n">
         <v>569</v>
       </c>
-      <c r="AU3" t="inlineStr"/>
-      <c r="AV3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AU3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV3" t="inlineStr"/>
       <c r="AW3" t="n">
         <v>569</v>
       </c>
@@ -1062,6 +1071,9 @@
         <v>569</v>
       </c>
       <c r="BB3" t="n">
+        <v>569</v>
+      </c>
+      <c r="BC3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1080,10 +1092,10 @@
       <c r="D4" t="n">
         <v>299</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>299</v>
-      </c>
+      <c r="E4" t="n">
+        <v>299</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>299</v>
       </c>
@@ -1177,10 +1189,10 @@
       <c r="AK4" t="n">
         <v>299</v>
       </c>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM4" t="inlineStr"/>
       <c r="AN4" t="n">
         <v>299</v>
       </c>
@@ -1202,10 +1214,10 @@
       <c r="AT4" t="n">
         <v>299</v>
       </c>
-      <c r="AU4" t="inlineStr"/>
-      <c r="AV4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AU4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV4" t="inlineStr"/>
       <c r="AW4" t="n">
         <v>299</v>
       </c>
@@ -1222,6 +1234,9 @@
         <v>299</v>
       </c>
       <c r="BB4" t="n">
+        <v>299</v>
+      </c>
+      <c r="BC4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1237,11 +1252,11 @@
       <c r="C5" t="n">
         <v>569</v>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>569</v>
+      </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>569</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>569</v>
       </c>
@@ -1263,10 +1278,10 @@
       <c r="M5" t="n">
         <v>569</v>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="n">
-        <v>569</v>
-      </c>
+      <c r="N5" t="n">
+        <v>569</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
         <v>569</v>
       </c>
@@ -1360,10 +1375,10 @@
       <c r="AT5" t="n">
         <v>569</v>
       </c>
-      <c r="AU5" t="inlineStr"/>
-      <c r="AV5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AU5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="n">
         <v>569</v>
       </c>
@@ -1380,6 +1395,9 @@
         <v>569</v>
       </c>
       <c r="BB5" t="n">
+        <v>569</v>
+      </c>
+      <c r="BC5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1398,15 +1416,15 @@
       <c r="D6" t="n">
         <v>499</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>499</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>499</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>499</v>
+      </c>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>499</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
         <v>499</v>
       </c>
@@ -1494,10 +1512,10 @@
       <c r="AL6" t="n">
         <v>499</v>
       </c>
-      <c r="AM6" t="inlineStr"/>
-      <c r="AN6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AM6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AN6" t="inlineStr"/>
       <c r="AO6" t="n">
         <v>499</v>
       </c>
@@ -1516,10 +1534,10 @@
       <c r="AT6" t="n">
         <v>499</v>
       </c>
-      <c r="AU6" t="inlineStr"/>
-      <c r="AV6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AU6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV6" t="inlineStr"/>
       <c r="AW6" t="n">
         <v>499</v>
       </c>
@@ -1536,6 +1554,9 @@
         <v>499</v>
       </c>
       <c r="BB6" t="n">
+        <v>499</v>
+      </c>
+      <c r="BC6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1551,20 +1572,20 @@
       <c r="C7" t="n">
         <v>569</v>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>569</v>
-      </c>
+      <c r="D7" t="n">
+        <v>569</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>569</v>
       </c>
       <c r="G7" t="n">
         <v>569</v>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>569</v>
-      </c>
+      <c r="H7" t="n">
+        <v>569</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
         <v>569</v>
       </c>
@@ -1649,12 +1670,12 @@
       <c r="AK7" t="n">
         <v>569</v>
       </c>
-      <c r="AL7" t="inlineStr"/>
+      <c r="AL7" t="n">
+        <v>569</v>
+      </c>
       <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="inlineStr"/>
-      <c r="AO7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO7" t="inlineStr"/>
       <c r="AP7" t="n">
         <v>569</v>
       </c>
@@ -1670,10 +1691,10 @@
       <c r="AT7" t="n">
         <v>569</v>
       </c>
-      <c r="AU7" t="inlineStr"/>
-      <c r="AV7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AU7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV7" t="inlineStr"/>
       <c r="AW7" t="n">
         <v>569</v>
       </c>
@@ -1690,6 +1711,9 @@
         <v>569</v>
       </c>
       <c r="BB7" t="n">
+        <v>569</v>
+      </c>
+      <c r="BC7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1705,20 +1729,20 @@
       <c r="C8" t="n">
         <v>929</v>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>929</v>
-      </c>
+      <c r="D8" t="n">
+        <v>929</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>929</v>
       </c>
       <c r="G8" t="n">
         <v>929</v>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
-        <v>929</v>
-      </c>
+      <c r="H8" t="n">
+        <v>929</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
         <v>929</v>
       </c>
@@ -1803,14 +1827,14 @@
       <c r="AK8" t="n">
         <v>929</v>
       </c>
-      <c r="AL8" t="inlineStr"/>
-      <c r="AM8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AN8" t="inlineStr"/>
-      <c r="AO8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AL8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO8" t="inlineStr"/>
       <c r="AP8" t="n">
         <v>929</v>
       </c>
@@ -1826,10 +1850,10 @@
       <c r="AT8" t="n">
         <v>929</v>
       </c>
-      <c r="AU8" t="inlineStr"/>
-      <c r="AV8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AU8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV8" t="inlineStr"/>
       <c r="AW8" t="n">
         <v>929</v>
       </c>
@@ -1846,6 +1870,9 @@
         <v>929</v>
       </c>
       <c r="BB8" t="n">
+        <v>929</v>
+      </c>
+      <c r="BC8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1861,17 +1888,17 @@
       <c r="C9" t="n">
         <v>299</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>299</v>
-      </c>
+      <c r="D9" t="n">
+        <v>299</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>299</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>299</v>
-      </c>
+      <c r="G9" t="n">
+        <v>299</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>299</v>
       </c>
@@ -1959,10 +1986,10 @@
       <c r="AK9" t="n">
         <v>299</v>
       </c>
-      <c r="AL9" t="inlineStr"/>
-      <c r="AM9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM9" t="inlineStr"/>
       <c r="AN9" t="n">
         <v>299</v>
       </c>
@@ -1984,10 +2011,10 @@
       <c r="AT9" t="n">
         <v>299</v>
       </c>
-      <c r="AU9" t="inlineStr"/>
-      <c r="AV9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AU9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV9" t="inlineStr"/>
       <c r="AW9" t="n">
         <v>299</v>
       </c>
@@ -2004,6 +2031,9 @@
         <v>299</v>
       </c>
       <c r="BB9" t="n">
+        <v>299</v>
+      </c>
+      <c r="BC9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2019,18 +2049,18 @@
       <c r="C10" t="n">
         <v>299</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>299</v>
-      </c>
+      <c r="D10" t="n">
+        <v>299</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>299</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>299</v>
+      </c>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
-        <v>299</v>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="n">
         <v>299</v>
       </c>
@@ -2085,10 +2115,10 @@
       <c r="AA10" t="n">
         <v>299</v>
       </c>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AB10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="n">
         <v>299</v>
       </c>
@@ -2113,14 +2143,14 @@
       <c r="AK10" t="n">
         <v>299</v>
       </c>
-      <c r="AL10" t="inlineStr"/>
-      <c r="AM10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AN10" t="inlineStr"/>
-      <c r="AO10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO10" t="inlineStr"/>
       <c r="AP10" t="n">
         <v>299</v>
       </c>
@@ -2136,10 +2166,10 @@
       <c r="AT10" t="n">
         <v>299</v>
       </c>
-      <c r="AU10" t="inlineStr"/>
-      <c r="AV10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AU10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV10" t="inlineStr"/>
       <c r="AW10" t="n">
         <v>299</v>
       </c>
@@ -2156,6 +2186,9 @@
         <v>299</v>
       </c>
       <c r="BB10" t="n">
+        <v>299</v>
+      </c>
+      <c r="BC10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2171,10 +2204,10 @@
       <c r="C11" t="n">
         <v>2997</v>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
+      <c r="D11" t="n">
         <v>2997</v>
       </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>2997</v>
       </c>
@@ -2274,10 +2307,10 @@
       <c r="AL11" t="n">
         <v>2997</v>
       </c>
-      <c r="AM11" t="inlineStr"/>
-      <c r="AN11" t="n">
+      <c r="AM11" t="n">
         <v>2997</v>
       </c>
+      <c r="AN11" t="inlineStr"/>
       <c r="AO11" t="n">
         <v>2997</v>
       </c>
@@ -2291,15 +2324,15 @@
         <v>2997</v>
       </c>
       <c r="AS11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AT11" t="n">
         <v>929</v>
       </c>
-      <c r="AU11" t="inlineStr"/>
-      <c r="AV11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AU11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV11" t="inlineStr"/>
       <c r="AW11" t="n">
         <v>929</v>
       </c>
@@ -2316,6 +2349,9 @@
         <v>929</v>
       </c>
       <c r="BB11" t="n">
+        <v>929</v>
+      </c>
+      <c r="BC11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2331,10 +2367,10 @@
       <c r="C12" t="n">
         <v>569</v>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>569</v>
-      </c>
+      <c r="D12" t="n">
+        <v>569</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
         <v>569</v>
       </c>
@@ -2437,10 +2473,10 @@
       <c r="AM12" t="n">
         <v>569</v>
       </c>
-      <c r="AN12" t="inlineStr"/>
-      <c r="AO12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO12" t="inlineStr"/>
       <c r="AP12" t="n">
         <v>569</v>
       </c>
@@ -2456,10 +2492,10 @@
       <c r="AT12" t="n">
         <v>569</v>
       </c>
-      <c r="AU12" t="inlineStr"/>
-      <c r="AV12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AU12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV12" t="inlineStr"/>
       <c r="AW12" t="n">
         <v>569</v>
       </c>
@@ -2476,6 +2512,9 @@
         <v>569</v>
       </c>
       <c r="BB12" t="n">
+        <v>569</v>
+      </c>
+      <c r="BC12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2491,17 +2530,17 @@
       <c r="C13" t="n">
         <v>569</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>569</v>
-      </c>
+      <c r="D13" t="n">
+        <v>569</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>569</v>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>569</v>
-      </c>
+      <c r="G13" t="n">
+        <v>569</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>569</v>
       </c>
@@ -2538,10 +2577,10 @@
       <c r="T13" t="n">
         <v>569</v>
       </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="n">
-        <v>569</v>
-      </c>
+      <c r="U13" t="n">
+        <v>569</v>
+      </c>
+      <c r="V13" t="inlineStr"/>
       <c r="W13" t="n">
         <v>569</v>
       </c>
@@ -2587,14 +2626,14 @@
       <c r="AK13" t="n">
         <v>569</v>
       </c>
-      <c r="AL13" t="inlineStr"/>
-      <c r="AM13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AN13" t="inlineStr"/>
-      <c r="AO13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO13" t="inlineStr"/>
       <c r="AP13" t="n">
         <v>569</v>
       </c>
@@ -2610,24 +2649,27 @@
       <c r="AT13" t="n">
         <v>569</v>
       </c>
-      <c r="AU13" t="inlineStr"/>
-      <c r="AV13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AU13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV13" t="inlineStr"/>
       <c r="AW13" t="n">
         <v>569</v>
       </c>
       <c r="AX13" t="n">
         <v>569</v>
       </c>
-      <c r="AY13" t="inlineStr"/>
-      <c r="AZ13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AY13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AZ13" t="inlineStr"/>
       <c r="BA13" t="n">
         <v>569</v>
       </c>
       <c r="BB13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BC13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2646,17 +2688,17 @@
       <c r="D14" t="n">
         <v>794</v>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
+      <c r="E14" t="n">
         <v>794</v>
       </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>794</v>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="n">
+      <c r="H14" t="n">
         <v>794</v>
       </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="n">
         <v>794</v>
       </c>
@@ -2711,10 +2753,10 @@
       <c r="AA14" t="n">
         <v>794</v>
       </c>
-      <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="n">
+      <c r="AB14" t="n">
         <v>794</v>
       </c>
+      <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="n">
         <v>794</v>
       </c>
@@ -2722,7 +2764,7 @@
         <v>794</v>
       </c>
       <c r="AF14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AG14" t="n">
         <v>499</v>
@@ -2739,11 +2781,11 @@
       <c r="AK14" t="n">
         <v>499</v>
       </c>
-      <c r="AL14" t="inlineStr"/>
+      <c r="AL14" t="n">
+        <v>499</v>
+      </c>
       <c r="AM14" t="inlineStr"/>
-      <c r="AN14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AN14" t="inlineStr"/>
       <c r="AO14" t="n">
         <v>499</v>
       </c>
@@ -2784,6 +2826,9 @@
         <v>499</v>
       </c>
       <c r="BB14" t="n">
+        <v>499</v>
+      </c>
+      <c r="BC14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2799,16 +2844,16 @@
       <c r="C15" t="n">
         <v>499</v>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>499</v>
+      </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>499</v>
-      </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>499</v>
+      </c>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
-        <v>499</v>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="n">
         <v>499</v>
       </c>
@@ -2899,10 +2944,10 @@
       <c r="AM15" t="n">
         <v>499</v>
       </c>
-      <c r="AN15" t="inlineStr"/>
-      <c r="AO15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AN15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO15" t="inlineStr"/>
       <c r="AP15" t="n">
         <v>499</v>
       </c>
@@ -2912,14 +2957,14 @@
       <c r="AR15" t="n">
         <v>499</v>
       </c>
-      <c r="AS15" t="inlineStr"/>
-      <c r="AT15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AU15" t="inlineStr"/>
-      <c r="AV15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AS15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT15" t="inlineStr"/>
+      <c r="AU15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV15" t="inlineStr"/>
       <c r="AW15" t="n">
         <v>499</v>
       </c>
@@ -2936,6 +2981,9 @@
         <v>499</v>
       </c>
       <c r="BB15" t="n">
+        <v>499</v>
+      </c>
+      <c r="BC15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2954,14 +3002,14 @@
       <c r="D16" t="n">
         <v>299</v>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>299</v>
-      </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="n">
-        <v>299</v>
-      </c>
+      <c r="E16" t="n">
+        <v>299</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>299</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
         <v>299</v>
       </c>
@@ -3040,17 +3088,17 @@
       <c r="AH16" t="n">
         <v>299</v>
       </c>
-      <c r="AI16" t="inlineStr"/>
-      <c r="AJ16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AI16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AJ16" t="inlineStr"/>
       <c r="AK16" t="n">
         <v>299</v>
       </c>
-      <c r="AL16" t="inlineStr"/>
-      <c r="AM16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM16" t="inlineStr"/>
       <c r="AN16" t="n">
         <v>299</v>
       </c>
@@ -3072,10 +3120,10 @@
       <c r="AT16" t="n">
         <v>299</v>
       </c>
-      <c r="AU16" t="inlineStr"/>
-      <c r="AV16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AU16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV16" t="inlineStr"/>
       <c r="AW16" t="n">
         <v>299</v>
       </c>
@@ -3092,6 +3140,9 @@
         <v>299</v>
       </c>
       <c r="BB16" t="n">
+        <v>299</v>
+      </c>
+      <c r="BC16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3107,10 +3158,10 @@
       <c r="C17" t="n">
         <v>929</v>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
-        <v>929</v>
-      </c>
+      <c r="D17" t="n">
+        <v>929</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
         <v>929</v>
       </c>
@@ -3213,10 +3264,10 @@
       <c r="AM17" t="n">
         <v>929</v>
       </c>
-      <c r="AN17" t="inlineStr"/>
-      <c r="AO17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO17" t="inlineStr"/>
       <c r="AP17" t="n">
         <v>929</v>
       </c>
@@ -3232,10 +3283,10 @@
       <c r="AT17" t="n">
         <v>929</v>
       </c>
-      <c r="AU17" t="inlineStr"/>
-      <c r="AV17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AU17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV17" t="inlineStr"/>
       <c r="AW17" t="n">
         <v>929</v>
       </c>
@@ -3252,6 +3303,9 @@
         <v>929</v>
       </c>
       <c r="BB17" t="n">
+        <v>929</v>
+      </c>
+      <c r="BC17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3267,18 +3321,18 @@
       <c r="C18" t="n">
         <v>499</v>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="n">
-        <v>499</v>
-      </c>
+      <c r="D18" t="n">
+        <v>499</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
         <v>499</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>499</v>
+      </c>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="n">
-        <v>499</v>
-      </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="n">
         <v>499</v>
       </c>
@@ -3366,11 +3420,11 @@
       <c r="AL18" t="n">
         <v>499</v>
       </c>
-      <c r="AM18" t="inlineStr"/>
+      <c r="AM18" t="n">
+        <v>499</v>
+      </c>
       <c r="AN18" t="inlineStr"/>
-      <c r="AO18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AO18" t="inlineStr"/>
       <c r="AP18" t="n">
         <v>499</v>
       </c>
@@ -3386,10 +3440,10 @@
       <c r="AT18" t="n">
         <v>499</v>
       </c>
-      <c r="AU18" t="inlineStr"/>
-      <c r="AV18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AU18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV18" t="inlineStr"/>
       <c r="AW18" t="n">
         <v>499</v>
       </c>
@@ -3406,6 +3460,9 @@
         <v>499</v>
       </c>
       <c r="BB18" t="n">
+        <v>499</v>
+      </c>
+      <c r="BC18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3421,18 +3478,18 @@
       <c r="C19" t="n">
         <v>1299</v>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>1299</v>
+      </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
         <v>1299</v>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="n">
         <v>1299</v>
       </c>
@@ -3512,7 +3569,7 @@
         <v>1299</v>
       </c>
       <c r="AJ19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AK19" t="n">
         <v>1497</v>
@@ -3520,13 +3577,13 @@
       <c r="AL19" t="n">
         <v>1497</v>
       </c>
-      <c r="AM19" t="inlineStr"/>
+      <c r="AM19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AN19" t="inlineStr"/>
-      <c r="AO19" t="n">
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="n">
         <v>465</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>1497</v>
       </c>
       <c r="AQ19" t="n">
         <v>1497</v>
@@ -3562,6 +3619,9 @@
         <v>1497</v>
       </c>
       <c r="BB19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="BC19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3572,7 +3632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>929</v>
+        <v>569</v>
       </c>
       <c r="C20" t="n">
         <v>929</v>
@@ -3706,10 +3766,10 @@
       <c r="AT20" t="n">
         <v>929</v>
       </c>
-      <c r="AU20" t="inlineStr"/>
-      <c r="AV20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AU20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV20" t="inlineStr"/>
       <c r="AW20" t="n">
         <v>929</v>
       </c>
@@ -3726,6 +3786,9 @@
         <v>929</v>
       </c>
       <c r="BB20" t="n">
+        <v>929</v>
+      </c>
+      <c r="BC20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3741,24 +3804,24 @@
       <c r="C21" t="n">
         <v>499</v>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>499</v>
-      </c>
+      <c r="D21" t="n">
+        <v>499</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
         <v>499</v>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="n">
-        <v>499</v>
-      </c>
+      <c r="G21" t="n">
+        <v>499</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>499</v>
       </c>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="n">
-        <v>499</v>
-      </c>
+      <c r="J21" t="n">
+        <v>499</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="n">
         <v>499</v>
       </c>
@@ -3813,10 +3876,10 @@
       <c r="AC21" t="n">
         <v>499</v>
       </c>
-      <c r="AD21" t="inlineStr"/>
-      <c r="AE21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AD21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="n">
         <v>499</v>
       </c>
@@ -3841,10 +3904,10 @@
       <c r="AM21" t="n">
         <v>499</v>
       </c>
-      <c r="AN21" t="inlineStr"/>
-      <c r="AO21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AN21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO21" t="inlineStr"/>
       <c r="AP21" t="n">
         <v>499</v>
       </c>
@@ -3882,6 +3945,9 @@
         <v>499</v>
       </c>
       <c r="BB21" t="n">
+        <v>499</v>
+      </c>
+      <c r="BC21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3897,11 +3963,11 @@
       <c r="C22" t="n">
         <v>299</v>
       </c>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>299</v>
+      </c>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>299</v>
-      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
         <v>299</v>
       </c>
@@ -3995,14 +4061,14 @@
       <c r="AK22" t="n">
         <v>299</v>
       </c>
-      <c r="AL22" t="inlineStr"/>
-      <c r="AM22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AN22" t="inlineStr"/>
-      <c r="AO22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO22" t="inlineStr"/>
       <c r="AP22" t="n">
         <v>299</v>
       </c>
@@ -4018,10 +4084,10 @@
       <c r="AT22" t="n">
         <v>299</v>
       </c>
-      <c r="AU22" t="inlineStr"/>
-      <c r="AV22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AU22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AV22" t="inlineStr"/>
       <c r="AW22" t="n">
         <v>299</v>
       </c>
@@ -4038,6 +4104,9 @@
         <v>299</v>
       </c>
       <c r="BB22" t="n">
+        <v>299</v>
+      </c>
+      <c r="BC22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -4053,18 +4122,18 @@
       <c r="C23" t="n">
         <v>1299</v>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
         <v>1299</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>1299</v>
+      </c>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="n">
         <v>1299</v>
       </c>
@@ -4152,11 +4221,11 @@
       <c r="AL23" t="n">
         <v>1299</v>
       </c>
-      <c r="AM23" t="inlineStr"/>
+      <c r="AM23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AN23" t="inlineStr"/>
-      <c r="AO23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AO23" t="inlineStr"/>
       <c r="AP23" t="n">
         <v>1299</v>
       </c>
@@ -4172,10 +4241,10 @@
       <c r="AT23" t="n">
         <v>1299</v>
       </c>
-      <c r="AU23" t="inlineStr"/>
-      <c r="AV23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AU23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AV23" t="inlineStr"/>
       <c r="AW23" t="n">
         <v>1299</v>
       </c>
@@ -4192,6 +4261,9 @@
         <v>1299</v>
       </c>
       <c r="BB23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BC23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -4202,7 +4274,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>929</v>
+        <v>569</v>
       </c>
       <c r="C24" t="n">
         <v>929</v>
@@ -4216,11 +4288,11 @@
       <c r="F24" t="n">
         <v>929</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>929</v>
+      </c>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="n">
-        <v>929</v>
-      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="n">
         <v>929</v>
       </c>
@@ -4305,11 +4377,11 @@
       <c r="AK24" t="n">
         <v>929</v>
       </c>
-      <c r="AL24" t="inlineStr"/>
+      <c r="AL24" t="n">
+        <v>929</v>
+      </c>
       <c r="AM24" t="inlineStr"/>
-      <c r="AN24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN24" t="inlineStr"/>
       <c r="AO24" t="n">
         <v>929</v>
       </c>
@@ -4328,10 +4400,10 @@
       <c r="AT24" t="n">
         <v>929</v>
       </c>
-      <c r="AU24" t="inlineStr"/>
-      <c r="AV24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AU24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV24" t="inlineStr"/>
       <c r="AW24" t="n">
         <v>929</v>
       </c>
@@ -4348,6 +4420,9 @@
         <v>929</v>
       </c>
       <c r="BB24" t="n">
+        <v>929</v>
+      </c>
+      <c r="BC24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4363,18 +4438,18 @@
       <c r="C25" t="n">
         <v>929</v>
       </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="n">
-        <v>929</v>
-      </c>
+      <c r="D25" t="n">
+        <v>929</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
         <v>929</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>929</v>
+      </c>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="n">
-        <v>929</v>
-      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="n">
         <v>929</v>
       </c>
@@ -4384,10 +4459,10 @@
       <c r="L25" t="n">
         <v>929</v>
       </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="n">
-        <v>929</v>
-      </c>
+      <c r="M25" t="n">
+        <v>929</v>
+      </c>
+      <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
         <v>929</v>
       </c>
@@ -4457,11 +4532,11 @@
       <c r="AK25" t="n">
         <v>929</v>
       </c>
-      <c r="AL25" t="inlineStr"/>
+      <c r="AL25" t="n">
+        <v>929</v>
+      </c>
       <c r="AM25" t="inlineStr"/>
-      <c r="AN25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN25" t="inlineStr"/>
       <c r="AO25" t="n">
         <v>929</v>
       </c>
@@ -4480,10 +4555,10 @@
       <c r="AT25" t="n">
         <v>929</v>
       </c>
-      <c r="AU25" t="inlineStr"/>
-      <c r="AV25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AU25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV25" t="inlineStr"/>
       <c r="AW25" t="n">
         <v>929</v>
       </c>
@@ -4500,6 +4575,9 @@
         <v>929</v>
       </c>
       <c r="BB25" t="n">
+        <v>929</v>
+      </c>
+      <c r="BC25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4509,10 +4587,10 @@
           <t>Jr. Sr. Baby Diaper Pants | XXL Size (15-25 kg), 126 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
         <v>1299</v>
       </c>
@@ -4522,10 +4600,10 @@
       <c r="F26" t="n">
         <v>1299</v>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
         <v>1299</v>
       </c>
@@ -4535,10 +4613,10 @@
       <c r="K26" t="n">
         <v>1299</v>
       </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="L26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="M26" t="inlineStr"/>
       <c r="N26" t="n">
         <v>1299</v>
       </c>
@@ -4611,14 +4689,14 @@
       <c r="AK26" t="n">
         <v>1299</v>
       </c>
-      <c r="AL26" t="inlineStr"/>
-      <c r="AM26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AN26" t="inlineStr"/>
-      <c r="AO26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AL26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AM26" t="inlineStr"/>
+      <c r="AN26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AO26" t="inlineStr"/>
       <c r="AP26" t="n">
         <v>1299</v>
       </c>
@@ -4634,10 +4712,10 @@
       <c r="AT26" t="n">
         <v>1299</v>
       </c>
-      <c r="AU26" t="inlineStr"/>
-      <c r="AV26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AU26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AV26" t="inlineStr"/>
       <c r="AW26" t="n">
         <v>1299</v>
       </c>
@@ -4654,6 +4732,9 @@
         <v>1299</v>
       </c>
       <c r="BB26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BC26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-25 07:04
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC26"/>
+  <dimension ref="A1:BD26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,6 +488,7 @@
     <col width="21" customWidth="1" min="53" max="53"/>
     <col width="21" customWidth="1" min="54" max="54"/>
     <col width="21" customWidth="1" min="55" max="55"/>
+    <col width="21" customWidth="1" min="56" max="56"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -498,270 +499,275 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 12:29</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-25 10:31</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 09:25</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 04:11</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 02:11</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 00:27</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -869,10 +875,10 @@
       <c r="AG2" t="n">
         <v>929</v>
       </c>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AH2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="n">
         <v>929</v>
       </c>
@@ -885,25 +891,25 @@
       <c r="AM2" t="n">
         <v>929</v>
       </c>
-      <c r="AN2" t="inlineStr"/>
+      <c r="AN2" t="n">
+        <v>929</v>
+      </c>
       <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="n">
         <v>929</v>
       </c>
-      <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="n">
         <v>929</v>
       </c>
-      <c r="AU2" t="inlineStr"/>
-      <c r="AV2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AU2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="n">
         <v>929</v>
       </c>
@@ -923,6 +929,9 @@
         <v>929</v>
       </c>
       <c r="BC2" t="n">
+        <v>929</v>
+      </c>
+      <c r="BD2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -941,20 +950,20 @@
       <c r="D3" t="n">
         <v>569</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>569</v>
-      </c>
+      <c r="E3" t="n">
+        <v>569</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>569</v>
       </c>
       <c r="H3" t="n">
         <v>569</v>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>569</v>
-      </c>
+      <c r="I3" t="n">
+        <v>569</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
         <v>569</v>
       </c>
@@ -973,10 +982,10 @@
       <c r="P3" t="n">
         <v>569</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q3" t="n">
+        <v>569</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
         <v>569</v>
       </c>
@@ -1019,26 +1028,26 @@
       <c r="AF3" t="n">
         <v>569</v>
       </c>
-      <c r="AG3" t="inlineStr"/>
+      <c r="AG3" t="n">
+        <v>569</v>
+      </c>
       <c r="AH3" t="inlineStr"/>
       <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="n">
         <v>569</v>
       </c>
       <c r="AL3" t="n">
         <v>569</v>
       </c>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP3" t="inlineStr"/>
       <c r="AQ3" t="n">
         <v>569</v>
       </c>
@@ -1054,10 +1063,10 @@
       <c r="AU3" t="n">
         <v>569</v>
       </c>
-      <c r="AV3" t="inlineStr"/>
-      <c r="AW3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AV3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW3" t="inlineStr"/>
       <c r="AX3" t="n">
         <v>569</v>
       </c>
@@ -1074,6 +1083,9 @@
         <v>569</v>
       </c>
       <c r="BC3" t="n">
+        <v>569</v>
+      </c>
+      <c r="BD3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1095,10 +1107,10 @@
       <c r="E4" t="n">
         <v>299</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>299</v>
-      </c>
+      <c r="F4" t="n">
+        <v>299</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>299</v>
       </c>
@@ -1192,10 +1204,10 @@
       <c r="AL4" t="n">
         <v>299</v>
       </c>
-      <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN4" t="inlineStr"/>
       <c r="AO4" t="n">
         <v>299</v>
       </c>
@@ -1217,10 +1229,10 @@
       <c r="AU4" t="n">
         <v>299</v>
       </c>
-      <c r="AV4" t="inlineStr"/>
-      <c r="AW4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AV4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW4" t="inlineStr"/>
       <c r="AX4" t="n">
         <v>299</v>
       </c>
@@ -1237,6 +1249,9 @@
         <v>299</v>
       </c>
       <c r="BC4" t="n">
+        <v>299</v>
+      </c>
+      <c r="BD4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1255,11 +1270,11 @@
       <c r="D5" t="n">
         <v>569</v>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>569</v>
+      </c>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>569</v>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>569</v>
       </c>
@@ -1281,10 +1296,10 @@
       <c r="N5" t="n">
         <v>569</v>
       </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="n">
-        <v>569</v>
-      </c>
+      <c r="O5" t="n">
+        <v>569</v>
+      </c>
+      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="n">
         <v>569</v>
       </c>
@@ -1378,10 +1393,10 @@
       <c r="AU5" t="n">
         <v>569</v>
       </c>
-      <c r="AV5" t="inlineStr"/>
-      <c r="AW5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AV5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW5" t="inlineStr"/>
       <c r="AX5" t="n">
         <v>569</v>
       </c>
@@ -1398,6 +1413,9 @@
         <v>569</v>
       </c>
       <c r="BC5" t="n">
+        <v>569</v>
+      </c>
+      <c r="BD5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1419,15 +1437,15 @@
       <c r="E6" t="n">
         <v>499</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>499</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>499</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>499</v>
+      </c>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
-        <v>499</v>
-      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
         <v>499</v>
       </c>
@@ -1515,10 +1533,10 @@
       <c r="AM6" t="n">
         <v>499</v>
       </c>
-      <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AN6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AO6" t="inlineStr"/>
       <c r="AP6" t="n">
         <v>499</v>
       </c>
@@ -1537,10 +1555,10 @@
       <c r="AU6" t="n">
         <v>499</v>
       </c>
-      <c r="AV6" t="inlineStr"/>
-      <c r="AW6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AV6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW6" t="inlineStr"/>
       <c r="AX6" t="n">
         <v>499</v>
       </c>
@@ -1557,6 +1575,9 @@
         <v>499</v>
       </c>
       <c r="BC6" t="n">
+        <v>499</v>
+      </c>
+      <c r="BD6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1575,20 +1596,20 @@
       <c r="D7" t="n">
         <v>569</v>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>569</v>
-      </c>
+      <c r="E7" t="n">
+        <v>569</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>569</v>
       </c>
       <c r="H7" t="n">
         <v>569</v>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
-        <v>569</v>
-      </c>
+      <c r="I7" t="n">
+        <v>569</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
         <v>569</v>
       </c>
@@ -1673,12 +1694,12 @@
       <c r="AL7" t="n">
         <v>569</v>
       </c>
-      <c r="AM7" t="inlineStr"/>
+      <c r="AM7" t="n">
+        <v>569</v>
+      </c>
       <c r="AN7" t="inlineStr"/>
       <c r="AO7" t="inlineStr"/>
-      <c r="AP7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP7" t="inlineStr"/>
       <c r="AQ7" t="n">
         <v>569</v>
       </c>
@@ -1694,10 +1715,10 @@
       <c r="AU7" t="n">
         <v>569</v>
       </c>
-      <c r="AV7" t="inlineStr"/>
-      <c r="AW7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AV7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW7" t="inlineStr"/>
       <c r="AX7" t="n">
         <v>569</v>
       </c>
@@ -1714,6 +1735,9 @@
         <v>569</v>
       </c>
       <c r="BC7" t="n">
+        <v>569</v>
+      </c>
+      <c r="BD7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1732,20 +1756,20 @@
       <c r="D8" t="n">
         <v>929</v>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>929</v>
-      </c>
+      <c r="E8" t="n">
+        <v>929</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>929</v>
       </c>
       <c r="H8" t="n">
         <v>929</v>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
-        <v>929</v>
-      </c>
+      <c r="I8" t="n">
+        <v>929</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
         <v>929</v>
       </c>
@@ -1830,14 +1854,14 @@
       <c r="AL8" t="n">
         <v>929</v>
       </c>
-      <c r="AM8" t="inlineStr"/>
-      <c r="AN8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AM8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP8" t="inlineStr"/>
       <c r="AQ8" t="n">
         <v>929</v>
       </c>
@@ -1853,10 +1877,10 @@
       <c r="AU8" t="n">
         <v>929</v>
       </c>
-      <c r="AV8" t="inlineStr"/>
-      <c r="AW8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AV8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW8" t="inlineStr"/>
       <c r="AX8" t="n">
         <v>929</v>
       </c>
@@ -1873,6 +1897,9 @@
         <v>929</v>
       </c>
       <c r="BC8" t="n">
+        <v>929</v>
+      </c>
+      <c r="BD8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1891,17 +1918,17 @@
       <c r="D9" t="n">
         <v>299</v>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>299</v>
-      </c>
+      <c r="E9" t="n">
+        <v>299</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>299</v>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
-        <v>299</v>
-      </c>
+      <c r="H9" t="n">
+        <v>299</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
         <v>299</v>
       </c>
@@ -1989,10 +2016,10 @@
       <c r="AL9" t="n">
         <v>299</v>
       </c>
-      <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN9" t="inlineStr"/>
       <c r="AO9" t="n">
         <v>299</v>
       </c>
@@ -2014,10 +2041,10 @@
       <c r="AU9" t="n">
         <v>299</v>
       </c>
-      <c r="AV9" t="inlineStr"/>
-      <c r="AW9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AV9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW9" t="inlineStr"/>
       <c r="AX9" t="n">
         <v>299</v>
       </c>
@@ -2034,6 +2061,9 @@
         <v>299</v>
       </c>
       <c r="BC9" t="n">
+        <v>299</v>
+      </c>
+      <c r="BD9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2052,18 +2082,18 @@
       <c r="D10" t="n">
         <v>299</v>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>299</v>
-      </c>
+      <c r="E10" t="n">
+        <v>299</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>299</v>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>299</v>
+      </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>299</v>
-      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
         <v>299</v>
       </c>
@@ -2118,10 +2148,10 @@
       <c r="AB10" t="n">
         <v>299</v>
       </c>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AC10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="n">
         <v>299</v>
       </c>
@@ -2146,14 +2176,14 @@
       <c r="AL10" t="n">
         <v>299</v>
       </c>
-      <c r="AM10" t="inlineStr"/>
-      <c r="AN10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AO10" t="inlineStr"/>
-      <c r="AP10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP10" t="inlineStr"/>
       <c r="AQ10" t="n">
         <v>299</v>
       </c>
@@ -2169,10 +2199,10 @@
       <c r="AU10" t="n">
         <v>299</v>
       </c>
-      <c r="AV10" t="inlineStr"/>
-      <c r="AW10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AV10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW10" t="inlineStr"/>
       <c r="AX10" t="n">
         <v>299</v>
       </c>
@@ -2189,6 +2219,9 @@
         <v>299</v>
       </c>
       <c r="BC10" t="n">
+        <v>299</v>
+      </c>
+      <c r="BD10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2207,10 +2240,10 @@
       <c r="D11" t="n">
         <v>2997</v>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
+      <c r="E11" t="n">
         <v>2997</v>
       </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>2997</v>
       </c>
@@ -2310,10 +2343,10 @@
       <c r="AM11" t="n">
         <v>2997</v>
       </c>
-      <c r="AN11" t="inlineStr"/>
-      <c r="AO11" t="n">
+      <c r="AN11" t="n">
         <v>2997</v>
       </c>
+      <c r="AO11" t="inlineStr"/>
       <c r="AP11" t="n">
         <v>2997</v>
       </c>
@@ -2327,15 +2360,15 @@
         <v>2997</v>
       </c>
       <c r="AT11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AU11" t="n">
         <v>929</v>
       </c>
-      <c r="AV11" t="inlineStr"/>
-      <c r="AW11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AV11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW11" t="inlineStr"/>
       <c r="AX11" t="n">
         <v>929</v>
       </c>
@@ -2352,6 +2385,9 @@
         <v>929</v>
       </c>
       <c r="BC11" t="n">
+        <v>929</v>
+      </c>
+      <c r="BD11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2370,10 +2406,10 @@
       <c r="D12" t="n">
         <v>569</v>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>569</v>
-      </c>
+      <c r="E12" t="n">
+        <v>569</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>569</v>
       </c>
@@ -2476,10 +2512,10 @@
       <c r="AN12" t="n">
         <v>569</v>
       </c>
-      <c r="AO12" t="inlineStr"/>
-      <c r="AP12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP12" t="inlineStr"/>
       <c r="AQ12" t="n">
         <v>569</v>
       </c>
@@ -2495,10 +2531,10 @@
       <c r="AU12" t="n">
         <v>569</v>
       </c>
-      <c r="AV12" t="inlineStr"/>
-      <c r="AW12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AV12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW12" t="inlineStr"/>
       <c r="AX12" t="n">
         <v>569</v>
       </c>
@@ -2515,6 +2551,9 @@
         <v>569</v>
       </c>
       <c r="BC12" t="n">
+        <v>569</v>
+      </c>
+      <c r="BD12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2524,26 +2563,24 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
         <v>569</v>
       </c>
       <c r="D13" t="n">
         <v>569</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>569</v>
-      </c>
+      <c r="E13" t="n">
+        <v>569</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>569</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>569</v>
-      </c>
+      <c r="H13" t="n">
+        <v>569</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
         <v>569</v>
       </c>
@@ -2580,10 +2617,10 @@
       <c r="U13" t="n">
         <v>569</v>
       </c>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="n">
-        <v>569</v>
-      </c>
+      <c r="V13" t="n">
+        <v>569</v>
+      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="n">
         <v>569</v>
       </c>
@@ -2629,14 +2666,14 @@
       <c r="AL13" t="n">
         <v>569</v>
       </c>
-      <c r="AM13" t="inlineStr"/>
-      <c r="AN13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AO13" t="inlineStr"/>
-      <c r="AP13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AN13" t="inlineStr"/>
+      <c r="AO13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP13" t="inlineStr"/>
       <c r="AQ13" t="n">
         <v>569</v>
       </c>
@@ -2652,24 +2689,27 @@
       <c r="AU13" t="n">
         <v>569</v>
       </c>
-      <c r="AV13" t="inlineStr"/>
-      <c r="AW13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AV13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AW13" t="inlineStr"/>
       <c r="AX13" t="n">
         <v>569</v>
       </c>
       <c r="AY13" t="n">
         <v>569</v>
       </c>
-      <c r="AZ13" t="inlineStr"/>
-      <c r="BA13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AZ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BA13" t="inlineStr"/>
       <c r="BB13" t="n">
         <v>569</v>
       </c>
       <c r="BC13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BD13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2691,17 +2731,17 @@
       <c r="E14" t="n">
         <v>794</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
+      <c r="F14" t="n">
         <v>794</v>
       </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
         <v>794</v>
       </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="n">
+      <c r="I14" t="n">
         <v>794</v>
       </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
         <v>794</v>
       </c>
@@ -2756,10 +2796,10 @@
       <c r="AB14" t="n">
         <v>794</v>
       </c>
-      <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="n">
+      <c r="AC14" t="n">
         <v>794</v>
       </c>
+      <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="n">
         <v>794</v>
       </c>
@@ -2767,7 +2807,7 @@
         <v>794</v>
       </c>
       <c r="AG14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AH14" t="n">
         <v>499</v>
@@ -2784,11 +2824,11 @@
       <c r="AL14" t="n">
         <v>499</v>
       </c>
-      <c r="AM14" t="inlineStr"/>
+      <c r="AM14" t="n">
+        <v>499</v>
+      </c>
       <c r="AN14" t="inlineStr"/>
-      <c r="AO14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AO14" t="inlineStr"/>
       <c r="AP14" t="n">
         <v>499</v>
       </c>
@@ -2829,6 +2869,9 @@
         <v>499</v>
       </c>
       <c r="BC14" t="n">
+        <v>499</v>
+      </c>
+      <c r="BD14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2847,16 +2890,16 @@
       <c r="D15" t="n">
         <v>499</v>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>499</v>
+      </c>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>499</v>
-      </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>499</v>
+      </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="n">
-        <v>499</v>
-      </c>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
         <v>499</v>
       </c>
@@ -2947,10 +2990,10 @@
       <c r="AN15" t="n">
         <v>499</v>
       </c>
-      <c r="AO15" t="inlineStr"/>
-      <c r="AP15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AO15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP15" t="inlineStr"/>
       <c r="AQ15" t="n">
         <v>499</v>
       </c>
@@ -2960,14 +3003,14 @@
       <c r="AS15" t="n">
         <v>499</v>
       </c>
-      <c r="AT15" t="inlineStr"/>
-      <c r="AU15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AV15" t="inlineStr"/>
-      <c r="AW15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AT15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AU15" t="inlineStr"/>
+      <c r="AV15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW15" t="inlineStr"/>
       <c r="AX15" t="n">
         <v>499</v>
       </c>
@@ -2984,6 +3027,9 @@
         <v>499</v>
       </c>
       <c r="BC15" t="n">
+        <v>499</v>
+      </c>
+      <c r="BD15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3005,14 +3051,14 @@
       <c r="E16" t="n">
         <v>299</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>299</v>
-      </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>299</v>
-      </c>
+      <c r="F16" t="n">
+        <v>299</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>299</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
         <v>299</v>
       </c>
@@ -3091,17 +3137,17 @@
       <c r="AI16" t="n">
         <v>299</v>
       </c>
-      <c r="AJ16" t="inlineStr"/>
-      <c r="AK16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AJ16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="n">
         <v>299</v>
       </c>
-      <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN16" t="inlineStr"/>
       <c r="AO16" t="n">
         <v>299</v>
       </c>
@@ -3123,10 +3169,10 @@
       <c r="AU16" t="n">
         <v>299</v>
       </c>
-      <c r="AV16" t="inlineStr"/>
-      <c r="AW16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AV16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW16" t="inlineStr"/>
       <c r="AX16" t="n">
         <v>299</v>
       </c>
@@ -3143,6 +3189,9 @@
         <v>299</v>
       </c>
       <c r="BC16" t="n">
+        <v>299</v>
+      </c>
+      <c r="BD16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3161,10 +3210,10 @@
       <c r="D17" t="n">
         <v>929</v>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>929</v>
-      </c>
+      <c r="E17" t="n">
+        <v>929</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
         <v>929</v>
       </c>
@@ -3267,10 +3316,10 @@
       <c r="AN17" t="n">
         <v>929</v>
       </c>
-      <c r="AO17" t="inlineStr"/>
-      <c r="AP17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP17" t="inlineStr"/>
       <c r="AQ17" t="n">
         <v>929</v>
       </c>
@@ -3286,10 +3335,10 @@
       <c r="AU17" t="n">
         <v>929</v>
       </c>
-      <c r="AV17" t="inlineStr"/>
-      <c r="AW17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AV17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW17" t="inlineStr"/>
       <c r="AX17" t="n">
         <v>929</v>
       </c>
@@ -3306,6 +3355,9 @@
         <v>929</v>
       </c>
       <c r="BC17" t="n">
+        <v>929</v>
+      </c>
+      <c r="BD17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3324,18 +3376,18 @@
       <c r="D18" t="n">
         <v>499</v>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
-        <v>499</v>
-      </c>
+      <c r="E18" t="n">
+        <v>499</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
         <v>499</v>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>499</v>
+      </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="n">
-        <v>499</v>
-      </c>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
         <v>499</v>
       </c>
@@ -3423,11 +3475,11 @@
       <c r="AM18" t="n">
         <v>499</v>
       </c>
-      <c r="AN18" t="inlineStr"/>
+      <c r="AN18" t="n">
+        <v>499</v>
+      </c>
       <c r="AO18" t="inlineStr"/>
-      <c r="AP18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AP18" t="inlineStr"/>
       <c r="AQ18" t="n">
         <v>499</v>
       </c>
@@ -3443,10 +3495,10 @@
       <c r="AU18" t="n">
         <v>499</v>
       </c>
-      <c r="AV18" t="inlineStr"/>
-      <c r="AW18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AV18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW18" t="inlineStr"/>
       <c r="AX18" t="n">
         <v>499</v>
       </c>
@@ -3463,6 +3515,9 @@
         <v>499</v>
       </c>
       <c r="BC18" t="n">
+        <v>499</v>
+      </c>
+      <c r="BD18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3481,18 +3536,18 @@
       <c r="D19" t="n">
         <v>1299</v>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>1299</v>
+      </c>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
         <v>1299</v>
       </c>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
         <v>1299</v>
       </c>
@@ -3572,7 +3627,7 @@
         <v>1299</v>
       </c>
       <c r="AK19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AL19" t="n">
         <v>1497</v>
@@ -3580,13 +3635,13 @@
       <c r="AM19" t="n">
         <v>1497</v>
       </c>
-      <c r="AN19" t="inlineStr"/>
+      <c r="AN19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AO19" t="inlineStr"/>
-      <c r="AP19" t="n">
+      <c r="AP19" t="inlineStr"/>
+      <c r="AQ19" t="n">
         <v>465</v>
-      </c>
-      <c r="AQ19" t="n">
-        <v>1497</v>
       </c>
       <c r="AR19" t="n">
         <v>1497</v>
@@ -3622,6 +3677,9 @@
         <v>1497</v>
       </c>
       <c r="BC19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="BD19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3635,7 +3693,7 @@
         <v>569</v>
       </c>
       <c r="C20" t="n">
-        <v>929</v>
+        <v>569</v>
       </c>
       <c r="D20" t="n">
         <v>929</v>
@@ -3769,10 +3827,10 @@
       <c r="AU20" t="n">
         <v>929</v>
       </c>
-      <c r="AV20" t="inlineStr"/>
-      <c r="AW20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AV20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW20" t="inlineStr"/>
       <c r="AX20" t="n">
         <v>929</v>
       </c>
@@ -3789,6 +3847,9 @@
         <v>929</v>
       </c>
       <c r="BC20" t="n">
+        <v>929</v>
+      </c>
+      <c r="BD20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3807,24 +3868,24 @@
       <c r="D21" t="n">
         <v>499</v>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>499</v>
-      </c>
+      <c r="E21" t="n">
+        <v>499</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
         <v>499</v>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="n">
-        <v>499</v>
-      </c>
+      <c r="H21" t="n">
+        <v>499</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
         <v>499</v>
       </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="n">
-        <v>499</v>
-      </c>
+      <c r="K21" t="n">
+        <v>499</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
         <v>499</v>
       </c>
@@ -3879,10 +3940,10 @@
       <c r="AD21" t="n">
         <v>499</v>
       </c>
-      <c r="AE21" t="inlineStr"/>
-      <c r="AF21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AE21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AF21" t="inlineStr"/>
       <c r="AG21" t="n">
         <v>499</v>
       </c>
@@ -3907,10 +3968,10 @@
       <c r="AN21" t="n">
         <v>499</v>
       </c>
-      <c r="AO21" t="inlineStr"/>
-      <c r="AP21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AO21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP21" t="inlineStr"/>
       <c r="AQ21" t="n">
         <v>499</v>
       </c>
@@ -3948,6 +4009,9 @@
         <v>499</v>
       </c>
       <c r="BC21" t="n">
+        <v>499</v>
+      </c>
+      <c r="BD21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3966,11 +4030,11 @@
       <c r="D22" t="n">
         <v>299</v>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>299</v>
+      </c>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="n">
-        <v>299</v>
-      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
         <v>299</v>
       </c>
@@ -4064,14 +4128,14 @@
       <c r="AL22" t="n">
         <v>299</v>
       </c>
-      <c r="AM22" t="inlineStr"/>
-      <c r="AN22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AO22" t="inlineStr"/>
-      <c r="AP22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AM22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AN22" t="inlineStr"/>
+      <c r="AO22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP22" t="inlineStr"/>
       <c r="AQ22" t="n">
         <v>299</v>
       </c>
@@ -4087,10 +4151,10 @@
       <c r="AU22" t="n">
         <v>299</v>
       </c>
-      <c r="AV22" t="inlineStr"/>
-      <c r="AW22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AV22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AW22" t="inlineStr"/>
       <c r="AX22" t="n">
         <v>299</v>
       </c>
@@ -4107,6 +4171,9 @@
         <v>299</v>
       </c>
       <c r="BC22" t="n">
+        <v>299</v>
+      </c>
+      <c r="BD22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -4125,18 +4192,18 @@
       <c r="D23" t="n">
         <v>1299</v>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
         <v>1299</v>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>1299</v>
+      </c>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
         <v>1299</v>
       </c>
@@ -4224,11 +4291,11 @@
       <c r="AM23" t="n">
         <v>1299</v>
       </c>
-      <c r="AN23" t="inlineStr"/>
+      <c r="AN23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AO23" t="inlineStr"/>
-      <c r="AP23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AP23" t="inlineStr"/>
       <c r="AQ23" t="n">
         <v>1299</v>
       </c>
@@ -4244,10 +4311,10 @@
       <c r="AU23" t="n">
         <v>1299</v>
       </c>
-      <c r="AV23" t="inlineStr"/>
-      <c r="AW23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AV23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AW23" t="inlineStr"/>
       <c r="AX23" t="n">
         <v>1299</v>
       </c>
@@ -4264,6 +4331,9 @@
         <v>1299</v>
       </c>
       <c r="BC23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BD23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -4277,7 +4347,7 @@
         <v>569</v>
       </c>
       <c r="C24" t="n">
-        <v>929</v>
+        <v>569</v>
       </c>
       <c r="D24" t="n">
         <v>929</v>
@@ -4291,11 +4361,11 @@
       <c r="G24" t="n">
         <v>929</v>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="n">
+        <v>929</v>
+      </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="n">
-        <v>929</v>
-      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
         <v>929</v>
       </c>
@@ -4380,11 +4450,11 @@
       <c r="AL24" t="n">
         <v>929</v>
       </c>
-      <c r="AM24" t="inlineStr"/>
+      <c r="AM24" t="n">
+        <v>929</v>
+      </c>
       <c r="AN24" t="inlineStr"/>
-      <c r="AO24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO24" t="inlineStr"/>
       <c r="AP24" t="n">
         <v>929</v>
       </c>
@@ -4403,10 +4473,10 @@
       <c r="AU24" t="n">
         <v>929</v>
       </c>
-      <c r="AV24" t="inlineStr"/>
-      <c r="AW24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AV24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW24" t="inlineStr"/>
       <c r="AX24" t="n">
         <v>929</v>
       </c>
@@ -4423,6 +4493,9 @@
         <v>929</v>
       </c>
       <c r="BC24" t="n">
+        <v>929</v>
+      </c>
+      <c r="BD24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4441,18 +4514,18 @@
       <c r="D25" t="n">
         <v>929</v>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>929</v>
-      </c>
+      <c r="E25" t="n">
+        <v>929</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>929</v>
       </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" t="n">
+        <v>929</v>
+      </c>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="n">
-        <v>929</v>
-      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
         <v>929</v>
       </c>
@@ -4462,10 +4535,10 @@
       <c r="M25" t="n">
         <v>929</v>
       </c>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="n">
-        <v>929</v>
-      </c>
+      <c r="N25" t="n">
+        <v>929</v>
+      </c>
+      <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
         <v>929</v>
       </c>
@@ -4535,11 +4608,11 @@
       <c r="AL25" t="n">
         <v>929</v>
       </c>
-      <c r="AM25" t="inlineStr"/>
+      <c r="AM25" t="n">
+        <v>929</v>
+      </c>
       <c r="AN25" t="inlineStr"/>
-      <c r="AO25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO25" t="inlineStr"/>
       <c r="AP25" t="n">
         <v>929</v>
       </c>
@@ -4558,10 +4631,10 @@
       <c r="AU25" t="n">
         <v>929</v>
       </c>
-      <c r="AV25" t="inlineStr"/>
-      <c r="AW25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AV25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW25" t="inlineStr"/>
       <c r="AX25" t="n">
         <v>929</v>
       </c>
@@ -4578,6 +4651,9 @@
         <v>929</v>
       </c>
       <c r="BC25" t="n">
+        <v>929</v>
+      </c>
+      <c r="BD25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4590,10 +4666,10 @@
       <c r="B26" t="n">
         <v>1299</v>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="C26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
         <v>1299</v>
       </c>
@@ -4603,10 +4679,10 @@
       <c r="G26" t="n">
         <v>1299</v>
       </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="n">
         <v>1299</v>
       </c>
@@ -4616,10 +4692,10 @@
       <c r="L26" t="n">
         <v>1299</v>
       </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="M26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
         <v>1299</v>
       </c>
@@ -4692,14 +4768,14 @@
       <c r="AL26" t="n">
         <v>1299</v>
       </c>
-      <c r="AM26" t="inlineStr"/>
-      <c r="AN26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AO26" t="inlineStr"/>
-      <c r="AP26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AM26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AN26" t="inlineStr"/>
+      <c r="AO26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AP26" t="inlineStr"/>
       <c r="AQ26" t="n">
         <v>1299</v>
       </c>
@@ -4715,10 +4791,10 @@
       <c r="AU26" t="n">
         <v>1299</v>
       </c>
-      <c r="AV26" t="inlineStr"/>
-      <c r="AW26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AV26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AW26" t="inlineStr"/>
       <c r="AX26" t="n">
         <v>1299</v>
       </c>
@@ -4735,6 +4811,9 @@
         <v>1299</v>
       </c>
       <c r="BC26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BD26" t="n">
         <v>1299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IST price update 2025-12-25 08:39
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD26"/>
+  <dimension ref="A1:BE30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="197" customWidth="1" min="1" max="1"/>
+    <col width="204" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
@@ -489,6 +489,7 @@
     <col width="21" customWidth="1" min="54" max="54"/>
     <col width="21" customWidth="1" min="55" max="55"/>
     <col width="21" customWidth="1" min="56" max="56"/>
+    <col width="21" customWidth="1" min="57" max="57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -499,275 +500,280 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 14:04</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-25 12:29</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 10:31</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 09:25</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 04:11</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 02:11</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 00:27</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -878,10 +884,10 @@
       <c r="AH2" t="n">
         <v>929</v>
       </c>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AI2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="n">
         <v>929</v>
       </c>
@@ -894,25 +900,25 @@
       <c r="AN2" t="n">
         <v>929</v>
       </c>
-      <c r="AO2" t="inlineStr"/>
+      <c r="AO2" t="n">
+        <v>929</v>
+      </c>
       <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="n">
         <v>929</v>
       </c>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AT2" t="inlineStr"/>
       <c r="AU2" t="n">
         <v>929</v>
       </c>
-      <c r="AV2" t="inlineStr"/>
-      <c r="AW2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AV2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="n">
         <v>929</v>
       </c>
@@ -932,6 +938,9 @@
         <v>929</v>
       </c>
       <c r="BD2" t="n">
+        <v>929</v>
+      </c>
+      <c r="BE2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -953,20 +962,20 @@
       <c r="E3" t="n">
         <v>569</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>569</v>
-      </c>
+      <c r="F3" t="n">
+        <v>569</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>569</v>
       </c>
       <c r="I3" t="n">
         <v>569</v>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>569</v>
-      </c>
+      <c r="J3" t="n">
+        <v>569</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
         <v>569</v>
       </c>
@@ -985,10 +994,10 @@
       <c r="Q3" t="n">
         <v>569</v>
       </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="n">
-        <v>569</v>
-      </c>
+      <c r="R3" t="n">
+        <v>569</v>
+      </c>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="n">
         <v>569</v>
       </c>
@@ -1031,26 +1040,26 @@
       <c r="AG3" t="n">
         <v>569</v>
       </c>
-      <c r="AH3" t="inlineStr"/>
+      <c r="AH3" t="n">
+        <v>569</v>
+      </c>
       <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="n">
         <v>569</v>
       </c>
       <c r="AM3" t="n">
         <v>569</v>
       </c>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ3" t="inlineStr"/>
       <c r="AR3" t="n">
         <v>569</v>
       </c>
@@ -1066,10 +1075,10 @@
       <c r="AV3" t="n">
         <v>569</v>
       </c>
-      <c r="AW3" t="inlineStr"/>
-      <c r="AX3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AW3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX3" t="inlineStr"/>
       <c r="AY3" t="n">
         <v>569</v>
       </c>
@@ -1086,6 +1095,9 @@
         <v>569</v>
       </c>
       <c r="BD3" t="n">
+        <v>569</v>
+      </c>
+      <c r="BE3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1110,10 +1122,10 @@
       <c r="F4" t="n">
         <v>299</v>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>299</v>
-      </c>
+      <c r="G4" t="n">
+        <v>299</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>299</v>
       </c>
@@ -1207,10 +1219,10 @@
       <c r="AM4" t="n">
         <v>299</v>
       </c>
-      <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO4" t="inlineStr"/>
       <c r="AP4" t="n">
         <v>299</v>
       </c>
@@ -1232,10 +1244,10 @@
       <c r="AV4" t="n">
         <v>299</v>
       </c>
-      <c r="AW4" t="inlineStr"/>
-      <c r="AX4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AW4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX4" t="inlineStr"/>
       <c r="AY4" t="n">
         <v>299</v>
       </c>
@@ -1252,6 +1264,9 @@
         <v>299</v>
       </c>
       <c r="BD4" t="n">
+        <v>299</v>
+      </c>
+      <c r="BE4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1273,11 +1288,11 @@
       <c r="E5" t="n">
         <v>569</v>
       </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>569</v>
+      </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
-        <v>569</v>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>569</v>
       </c>
@@ -1299,10 +1314,10 @@
       <c r="O5" t="n">
         <v>569</v>
       </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="n">
-        <v>569</v>
-      </c>
+      <c r="P5" t="n">
+        <v>569</v>
+      </c>
+      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
         <v>569</v>
       </c>
@@ -1396,10 +1411,10 @@
       <c r="AV5" t="n">
         <v>569</v>
       </c>
-      <c r="AW5" t="inlineStr"/>
-      <c r="AX5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AW5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX5" t="inlineStr"/>
       <c r="AY5" t="n">
         <v>569</v>
       </c>
@@ -1416,6 +1431,9 @@
         <v>569</v>
       </c>
       <c r="BD5" t="n">
+        <v>569</v>
+      </c>
+      <c r="BE5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1440,15 +1458,15 @@
       <c r="F6" t="n">
         <v>499</v>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
-        <v>499</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>499</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>499</v>
+      </c>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>499</v>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="n">
         <v>499</v>
       </c>
@@ -1536,10 +1554,10 @@
       <c r="AN6" t="n">
         <v>499</v>
       </c>
-      <c r="AO6" t="inlineStr"/>
-      <c r="AP6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AO6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AP6" t="inlineStr"/>
       <c r="AQ6" t="n">
         <v>499</v>
       </c>
@@ -1558,10 +1576,10 @@
       <c r="AV6" t="n">
         <v>499</v>
       </c>
-      <c r="AW6" t="inlineStr"/>
-      <c r="AX6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AW6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AX6" t="inlineStr"/>
       <c r="AY6" t="n">
         <v>499</v>
       </c>
@@ -1578,6 +1596,9 @@
         <v>499</v>
       </c>
       <c r="BD6" t="n">
+        <v>499</v>
+      </c>
+      <c r="BE6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1599,20 +1620,20 @@
       <c r="E7" t="n">
         <v>569</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>569</v>
-      </c>
+      <c r="F7" t="n">
+        <v>569</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>569</v>
       </c>
       <c r="I7" t="n">
         <v>569</v>
       </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>569</v>
-      </c>
+      <c r="J7" t="n">
+        <v>569</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
         <v>569</v>
       </c>
@@ -1697,12 +1718,12 @@
       <c r="AM7" t="n">
         <v>569</v>
       </c>
-      <c r="AN7" t="inlineStr"/>
+      <c r="AN7" t="n">
+        <v>569</v>
+      </c>
       <c r="AO7" t="inlineStr"/>
       <c r="AP7" t="inlineStr"/>
-      <c r="AQ7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AQ7" t="inlineStr"/>
       <c r="AR7" t="n">
         <v>569</v>
       </c>
@@ -1718,10 +1739,10 @@
       <c r="AV7" t="n">
         <v>569</v>
       </c>
-      <c r="AW7" t="inlineStr"/>
-      <c r="AX7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AW7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX7" t="inlineStr"/>
       <c r="AY7" t="n">
         <v>569</v>
       </c>
@@ -1738,6 +1759,9 @@
         <v>569</v>
       </c>
       <c r="BD7" t="n">
+        <v>569</v>
+      </c>
+      <c r="BE7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1759,20 +1783,20 @@
       <c r="E8" t="n">
         <v>929</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>929</v>
-      </c>
+      <c r="F8" t="n">
+        <v>929</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
         <v>929</v>
       </c>
       <c r="I8" t="n">
         <v>929</v>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>929</v>
-      </c>
+      <c r="J8" t="n">
+        <v>929</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="n">
         <v>929</v>
       </c>
@@ -1857,14 +1881,14 @@
       <c r="AM8" t="n">
         <v>929</v>
       </c>
-      <c r="AN8" t="inlineStr"/>
-      <c r="AO8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AP8" t="inlineStr"/>
-      <c r="AQ8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AN8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ8" t="inlineStr"/>
       <c r="AR8" t="n">
         <v>929</v>
       </c>
@@ -1880,10 +1904,10 @@
       <c r="AV8" t="n">
         <v>929</v>
       </c>
-      <c r="AW8" t="inlineStr"/>
-      <c r="AX8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AW8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX8" t="inlineStr"/>
       <c r="AY8" t="n">
         <v>929</v>
       </c>
@@ -1900,6 +1924,9 @@
         <v>929</v>
       </c>
       <c r="BD8" t="n">
+        <v>929</v>
+      </c>
+      <c r="BE8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1921,17 +1948,17 @@
       <c r="E9" t="n">
         <v>299</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>299</v>
-      </c>
+      <c r="F9" t="n">
+        <v>299</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>299</v>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
-        <v>299</v>
-      </c>
+      <c r="I9" t="n">
+        <v>299</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
         <v>299</v>
       </c>
@@ -2019,10 +2046,10 @@
       <c r="AM9" t="n">
         <v>299</v>
       </c>
-      <c r="AN9" t="inlineStr"/>
-      <c r="AO9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO9" t="inlineStr"/>
       <c r="AP9" t="n">
         <v>299</v>
       </c>
@@ -2044,10 +2071,10 @@
       <c r="AV9" t="n">
         <v>299</v>
       </c>
-      <c r="AW9" t="inlineStr"/>
-      <c r="AX9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AW9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX9" t="inlineStr"/>
       <c r="AY9" t="n">
         <v>299</v>
       </c>
@@ -2064,6 +2091,9 @@
         <v>299</v>
       </c>
       <c r="BD9" t="n">
+        <v>299</v>
+      </c>
+      <c r="BE9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2085,18 +2115,18 @@
       <c r="E10" t="n">
         <v>299</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>299</v>
-      </c>
+      <c r="F10" t="n">
+        <v>299</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>299</v>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>299</v>
+      </c>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>299</v>
-      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
         <v>299</v>
       </c>
@@ -2151,10 +2181,10 @@
       <c r="AC10" t="n">
         <v>299</v>
       </c>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AD10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="n">
         <v>299</v>
       </c>
@@ -2179,14 +2209,14 @@
       <c r="AM10" t="n">
         <v>299</v>
       </c>
-      <c r="AN10" t="inlineStr"/>
-      <c r="AO10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AP10" t="inlineStr"/>
-      <c r="AQ10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ10" t="inlineStr"/>
       <c r="AR10" t="n">
         <v>299</v>
       </c>
@@ -2202,10 +2232,10 @@
       <c r="AV10" t="n">
         <v>299</v>
       </c>
-      <c r="AW10" t="inlineStr"/>
-      <c r="AX10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AW10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX10" t="inlineStr"/>
       <c r="AY10" t="n">
         <v>299</v>
       </c>
@@ -2222,6 +2252,9 @@
         <v>299</v>
       </c>
       <c r="BD10" t="n">
+        <v>299</v>
+      </c>
+      <c r="BE10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2243,10 +2276,10 @@
       <c r="E11" t="n">
         <v>2997</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="n">
+      <c r="F11" t="n">
         <v>2997</v>
       </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
         <v>2997</v>
       </c>
@@ -2346,10 +2379,10 @@
       <c r="AN11" t="n">
         <v>2997</v>
       </c>
-      <c r="AO11" t="inlineStr"/>
-      <c r="AP11" t="n">
+      <c r="AO11" t="n">
         <v>2997</v>
       </c>
+      <c r="AP11" t="inlineStr"/>
       <c r="AQ11" t="n">
         <v>2997</v>
       </c>
@@ -2363,15 +2396,15 @@
         <v>2997</v>
       </c>
       <c r="AU11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AV11" t="n">
         <v>929</v>
       </c>
-      <c r="AW11" t="inlineStr"/>
-      <c r="AX11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AW11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX11" t="inlineStr"/>
       <c r="AY11" t="n">
         <v>929</v>
       </c>
@@ -2388,6 +2421,9 @@
         <v>929</v>
       </c>
       <c r="BD11" t="n">
+        <v>929</v>
+      </c>
+      <c r="BE11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2409,10 +2445,10 @@
       <c r="E12" t="n">
         <v>569</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="n">
-        <v>569</v>
-      </c>
+      <c r="F12" t="n">
+        <v>569</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
         <v>569</v>
       </c>
@@ -2515,10 +2551,10 @@
       <c r="AO12" t="n">
         <v>569</v>
       </c>
-      <c r="AP12" t="inlineStr"/>
-      <c r="AQ12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ12" t="inlineStr"/>
       <c r="AR12" t="n">
         <v>569</v>
       </c>
@@ -2534,10 +2570,10 @@
       <c r="AV12" t="n">
         <v>569</v>
       </c>
-      <c r="AW12" t="inlineStr"/>
-      <c r="AX12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AW12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX12" t="inlineStr"/>
       <c r="AY12" t="n">
         <v>569</v>
       </c>
@@ -2554,6 +2590,9 @@
         <v>569</v>
       </c>
       <c r="BD12" t="n">
+        <v>569</v>
+      </c>
+      <c r="BE12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2563,27 +2602,27 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Large (L) Size (9-14 kg), 48 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="n">
-        <v>569</v>
-      </c>
+      <c r="B13" t="n">
+        <v>569</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
         <v>569</v>
       </c>
       <c r="E13" t="n">
         <v>569</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="n">
-        <v>569</v>
-      </c>
+      <c r="F13" t="n">
+        <v>569</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>569</v>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
-        <v>569</v>
-      </c>
+      <c r="I13" t="n">
+        <v>569</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>569</v>
       </c>
@@ -2620,10 +2659,10 @@
       <c r="V13" t="n">
         <v>569</v>
       </c>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="n">
-        <v>569</v>
-      </c>
+      <c r="W13" t="n">
+        <v>569</v>
+      </c>
+      <c r="X13" t="inlineStr"/>
       <c r="Y13" t="n">
         <v>569</v>
       </c>
@@ -2669,14 +2708,14 @@
       <c r="AM13" t="n">
         <v>569</v>
       </c>
-      <c r="AN13" t="inlineStr"/>
-      <c r="AO13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AP13" t="inlineStr"/>
-      <c r="AQ13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AN13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ13" t="inlineStr"/>
       <c r="AR13" t="n">
         <v>569</v>
       </c>
@@ -2692,24 +2731,27 @@
       <c r="AV13" t="n">
         <v>569</v>
       </c>
-      <c r="AW13" t="inlineStr"/>
-      <c r="AX13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AW13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AX13" t="inlineStr"/>
       <c r="AY13" t="n">
         <v>569</v>
       </c>
       <c r="AZ13" t="n">
         <v>569</v>
       </c>
-      <c r="BA13" t="inlineStr"/>
-      <c r="BB13" t="n">
-        <v>569</v>
-      </c>
+      <c r="BA13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BB13" t="inlineStr"/>
       <c r="BC13" t="n">
         <v>569</v>
       </c>
       <c r="BD13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BE13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2734,17 +2776,17 @@
       <c r="F14" t="n">
         <v>794</v>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="n">
+      <c r="G14" t="n">
         <v>794</v>
       </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
         <v>794</v>
       </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="n">
+      <c r="J14" t="n">
         <v>794</v>
       </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
         <v>794</v>
       </c>
@@ -2799,10 +2841,10 @@
       <c r="AC14" t="n">
         <v>794</v>
       </c>
-      <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="n">
+      <c r="AD14" t="n">
         <v>794</v>
       </c>
+      <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="n">
         <v>794</v>
       </c>
@@ -2810,7 +2852,7 @@
         <v>794</v>
       </c>
       <c r="AH14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AI14" t="n">
         <v>499</v>
@@ -2827,11 +2869,11 @@
       <c r="AM14" t="n">
         <v>499</v>
       </c>
-      <c r="AN14" t="inlineStr"/>
+      <c r="AN14" t="n">
+        <v>499</v>
+      </c>
       <c r="AO14" t="inlineStr"/>
-      <c r="AP14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AP14" t="inlineStr"/>
       <c r="AQ14" t="n">
         <v>499</v>
       </c>
@@ -2872,6 +2914,9 @@
         <v>499</v>
       </c>
       <c r="BD14" t="n">
+        <v>499</v>
+      </c>
+      <c r="BE14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2893,16 +2938,16 @@
       <c r="E15" t="n">
         <v>499</v>
       </c>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>499</v>
+      </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="n">
-        <v>499</v>
-      </c>
-      <c r="I15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>499</v>
+      </c>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="n">
-        <v>499</v>
-      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="n">
         <v>499</v>
       </c>
@@ -2993,10 +3038,10 @@
       <c r="AO15" t="n">
         <v>499</v>
       </c>
-      <c r="AP15" t="inlineStr"/>
-      <c r="AQ15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AP15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ15" t="inlineStr"/>
       <c r="AR15" t="n">
         <v>499</v>
       </c>
@@ -3006,14 +3051,14 @@
       <c r="AT15" t="n">
         <v>499</v>
       </c>
-      <c r="AU15" t="inlineStr"/>
-      <c r="AV15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AW15" t="inlineStr"/>
-      <c r="AX15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AU15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AV15" t="inlineStr"/>
+      <c r="AW15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AX15" t="inlineStr"/>
       <c r="AY15" t="n">
         <v>499</v>
       </c>
@@ -3030,6 +3075,9 @@
         <v>499</v>
       </c>
       <c r="BD15" t="n">
+        <v>499</v>
+      </c>
+      <c r="BE15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3054,14 +3102,14 @@
       <c r="F16" t="n">
         <v>299</v>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="n">
-        <v>299</v>
-      </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="n">
-        <v>299</v>
-      </c>
+      <c r="G16" t="n">
+        <v>299</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>299</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
         <v>299</v>
       </c>
@@ -3140,17 +3188,17 @@
       <c r="AJ16" t="n">
         <v>299</v>
       </c>
-      <c r="AK16" t="inlineStr"/>
-      <c r="AL16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AK16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="n">
         <v>299</v>
       </c>
-      <c r="AN16" t="inlineStr"/>
-      <c r="AO16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO16" t="inlineStr"/>
       <c r="AP16" t="n">
         <v>299</v>
       </c>
@@ -3172,10 +3220,10 @@
       <c r="AV16" t="n">
         <v>299</v>
       </c>
-      <c r="AW16" t="inlineStr"/>
-      <c r="AX16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AW16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX16" t="inlineStr"/>
       <c r="AY16" t="n">
         <v>299</v>
       </c>
@@ -3192,6 +3240,9 @@
         <v>299</v>
       </c>
       <c r="BD16" t="n">
+        <v>299</v>
+      </c>
+      <c r="BE16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3213,10 +3264,10 @@
       <c r="E17" t="n">
         <v>929</v>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="n">
-        <v>929</v>
-      </c>
+      <c r="F17" t="n">
+        <v>929</v>
+      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
         <v>929</v>
       </c>
@@ -3319,10 +3370,10 @@
       <c r="AO17" t="n">
         <v>929</v>
       </c>
-      <c r="AP17" t="inlineStr"/>
-      <c r="AQ17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AQ17" t="inlineStr"/>
       <c r="AR17" t="n">
         <v>929</v>
       </c>
@@ -3338,10 +3389,10 @@
       <c r="AV17" t="n">
         <v>929</v>
       </c>
-      <c r="AW17" t="inlineStr"/>
-      <c r="AX17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AW17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX17" t="inlineStr"/>
       <c r="AY17" t="n">
         <v>929</v>
       </c>
@@ -3358,6 +3409,9 @@
         <v>929</v>
       </c>
       <c r="BD17" t="n">
+        <v>929</v>
+      </c>
+      <c r="BE17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3379,18 +3433,18 @@
       <c r="E18" t="n">
         <v>499</v>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="n">
-        <v>499</v>
-      </c>
+      <c r="F18" t="n">
+        <v>499</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
         <v>499</v>
       </c>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>499</v>
+      </c>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="n">
-        <v>499</v>
-      </c>
+      <c r="K18" t="inlineStr"/>
       <c r="L18" t="n">
         <v>499</v>
       </c>
@@ -3478,11 +3532,11 @@
       <c r="AN18" t="n">
         <v>499</v>
       </c>
-      <c r="AO18" t="inlineStr"/>
+      <c r="AO18" t="n">
+        <v>499</v>
+      </c>
       <c r="AP18" t="inlineStr"/>
-      <c r="AQ18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AQ18" t="inlineStr"/>
       <c r="AR18" t="n">
         <v>499</v>
       </c>
@@ -3498,10 +3552,10 @@
       <c r="AV18" t="n">
         <v>499</v>
       </c>
-      <c r="AW18" t="inlineStr"/>
-      <c r="AX18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AW18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AX18" t="inlineStr"/>
       <c r="AY18" t="n">
         <v>499</v>
       </c>
@@ -3518,6 +3572,9 @@
         <v>499</v>
       </c>
       <c r="BD18" t="n">
+        <v>499</v>
+      </c>
+      <c r="BE18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3527,9 +3584,7 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
         <v>1299</v>
       </c>
@@ -3539,18 +3594,18 @@
       <c r="E19" t="n">
         <v>1299</v>
       </c>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>1299</v>
+      </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
         <v>1299</v>
       </c>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="J19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="n">
         <v>1299</v>
       </c>
@@ -3630,7 +3685,7 @@
         <v>1299</v>
       </c>
       <c r="AL19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AM19" t="n">
         <v>1497</v>
@@ -3638,13 +3693,13 @@
       <c r="AN19" t="n">
         <v>1497</v>
       </c>
-      <c r="AO19" t="inlineStr"/>
+      <c r="AO19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AP19" t="inlineStr"/>
-      <c r="AQ19" t="n">
+      <c r="AQ19" t="inlineStr"/>
+      <c r="AR19" t="n">
         <v>465</v>
-      </c>
-      <c r="AR19" t="n">
-        <v>1497</v>
       </c>
       <c r="AS19" t="n">
         <v>1497</v>
@@ -3680,6 +3735,9 @@
         <v>1497</v>
       </c>
       <c r="BD19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="BE19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3696,7 +3754,7 @@
         <v>569</v>
       </c>
       <c r="D20" t="n">
-        <v>929</v>
+        <v>569</v>
       </c>
       <c r="E20" t="n">
         <v>929</v>
@@ -3830,10 +3888,10 @@
       <c r="AV20" t="n">
         <v>929</v>
       </c>
-      <c r="AW20" t="inlineStr"/>
-      <c r="AX20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AW20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX20" t="inlineStr"/>
       <c r="AY20" t="n">
         <v>929</v>
       </c>
@@ -3850,6 +3908,9 @@
         <v>929</v>
       </c>
       <c r="BD20" t="n">
+        <v>929</v>
+      </c>
+      <c r="BE20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3871,24 +3932,24 @@
       <c r="E21" t="n">
         <v>499</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="n">
-        <v>499</v>
-      </c>
+      <c r="F21" t="n">
+        <v>499</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
         <v>499</v>
       </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>499</v>
-      </c>
+      <c r="I21" t="n">
+        <v>499</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>499</v>
       </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="n">
-        <v>499</v>
-      </c>
+      <c r="L21" t="n">
+        <v>499</v>
+      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
         <v>499</v>
       </c>
@@ -3943,10 +4004,10 @@
       <c r="AE21" t="n">
         <v>499</v>
       </c>
-      <c r="AF21" t="inlineStr"/>
-      <c r="AG21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AF21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AG21" t="inlineStr"/>
       <c r="AH21" t="n">
         <v>499</v>
       </c>
@@ -3971,10 +4032,10 @@
       <c r="AO21" t="n">
         <v>499</v>
       </c>
-      <c r="AP21" t="inlineStr"/>
-      <c r="AQ21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AP21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ21" t="inlineStr"/>
       <c r="AR21" t="n">
         <v>499</v>
       </c>
@@ -4012,6 +4073,9 @@
         <v>499</v>
       </c>
       <c r="BD21" t="n">
+        <v>499</v>
+      </c>
+      <c r="BE21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -4033,11 +4097,11 @@
       <c r="E22" t="n">
         <v>299</v>
       </c>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>299</v>
+      </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="n">
-        <v>299</v>
-      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
         <v>299</v>
       </c>
@@ -4131,14 +4195,14 @@
       <c r="AM22" t="n">
         <v>299</v>
       </c>
-      <c r="AN22" t="inlineStr"/>
-      <c r="AO22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AP22" t="inlineStr"/>
-      <c r="AQ22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AN22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AO22" t="inlineStr"/>
+      <c r="AP22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ22" t="inlineStr"/>
       <c r="AR22" t="n">
         <v>299</v>
       </c>
@@ -4154,10 +4218,10 @@
       <c r="AV22" t="n">
         <v>299</v>
       </c>
-      <c r="AW22" t="inlineStr"/>
-      <c r="AX22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AW22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AX22" t="inlineStr"/>
       <c r="AY22" t="n">
         <v>299</v>
       </c>
@@ -4174,6 +4238,9 @@
         <v>299</v>
       </c>
       <c r="BD22" t="n">
+        <v>299</v>
+      </c>
+      <c r="BE22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -4195,18 +4262,18 @@
       <c r="E23" t="n">
         <v>1299</v>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="F23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
         <v>1299</v>
       </c>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>1299</v>
+      </c>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="n">
         <v>1299</v>
       </c>
@@ -4294,11 +4361,11 @@
       <c r="AN23" t="n">
         <v>1299</v>
       </c>
-      <c r="AO23" t="inlineStr"/>
+      <c r="AO23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AP23" t="inlineStr"/>
-      <c r="AQ23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AQ23" t="inlineStr"/>
       <c r="AR23" t="n">
         <v>1299</v>
       </c>
@@ -4314,10 +4381,10 @@
       <c r="AV23" t="n">
         <v>1299</v>
       </c>
-      <c r="AW23" t="inlineStr"/>
-      <c r="AX23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AW23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AX23" t="inlineStr"/>
       <c r="AY23" t="n">
         <v>1299</v>
       </c>
@@ -4334,6 +4401,9 @@
         <v>1299</v>
       </c>
       <c r="BD23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BE23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -4350,7 +4420,7 @@
         <v>569</v>
       </c>
       <c r="D24" t="n">
-        <v>929</v>
+        <v>569</v>
       </c>
       <c r="E24" t="n">
         <v>929</v>
@@ -4364,11 +4434,11 @@
       <c r="H24" t="n">
         <v>929</v>
       </c>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>929</v>
+      </c>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="n">
-        <v>929</v>
-      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="n">
         <v>929</v>
       </c>
@@ -4453,11 +4523,11 @@
       <c r="AM24" t="n">
         <v>929</v>
       </c>
-      <c r="AN24" t="inlineStr"/>
+      <c r="AN24" t="n">
+        <v>929</v>
+      </c>
       <c r="AO24" t="inlineStr"/>
-      <c r="AP24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP24" t="inlineStr"/>
       <c r="AQ24" t="n">
         <v>929</v>
       </c>
@@ -4476,10 +4546,10 @@
       <c r="AV24" t="n">
         <v>929</v>
       </c>
-      <c r="AW24" t="inlineStr"/>
-      <c r="AX24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AW24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX24" t="inlineStr"/>
       <c r="AY24" t="n">
         <v>929</v>
       </c>
@@ -4496,6 +4566,9 @@
         <v>929</v>
       </c>
       <c r="BD24" t="n">
+        <v>929</v>
+      </c>
+      <c r="BE24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4517,18 +4590,18 @@
       <c r="E25" t="n">
         <v>929</v>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
-        <v>929</v>
-      </c>
+      <c r="F25" t="n">
+        <v>929</v>
+      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
         <v>929</v>
       </c>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>929</v>
+      </c>
       <c r="J25" t="inlineStr"/>
-      <c r="K25" t="n">
-        <v>929</v>
-      </c>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="n">
         <v>929</v>
       </c>
@@ -4538,10 +4611,10 @@
       <c r="N25" t="n">
         <v>929</v>
       </c>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="n">
-        <v>929</v>
-      </c>
+      <c r="O25" t="n">
+        <v>929</v>
+      </c>
+      <c r="P25" t="inlineStr"/>
       <c r="Q25" t="n">
         <v>929</v>
       </c>
@@ -4611,11 +4684,11 @@
       <c r="AM25" t="n">
         <v>929</v>
       </c>
-      <c r="AN25" t="inlineStr"/>
+      <c r="AN25" t="n">
+        <v>929</v>
+      </c>
       <c r="AO25" t="inlineStr"/>
-      <c r="AP25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AP25" t="inlineStr"/>
       <c r="AQ25" t="n">
         <v>929</v>
       </c>
@@ -4634,10 +4707,10 @@
       <c r="AV25" t="n">
         <v>929</v>
       </c>
-      <c r="AW25" t="inlineStr"/>
-      <c r="AX25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AW25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX25" t="inlineStr"/>
       <c r="AY25" t="n">
         <v>929</v>
       </c>
@@ -4654,6 +4727,9 @@
         <v>929</v>
       </c>
       <c r="BD25" t="n">
+        <v>929</v>
+      </c>
+      <c r="BE25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4669,10 +4745,10 @@
       <c r="C26" t="n">
         <v>1299</v>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="D26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
         <v>1299</v>
       </c>
@@ -4682,10 +4758,10 @@
       <c r="H26" t="n">
         <v>1299</v>
       </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
         <v>1299</v>
       </c>
@@ -4695,10 +4771,10 @@
       <c r="M26" t="n">
         <v>1299</v>
       </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="N26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
         <v>1299</v>
       </c>
@@ -4771,14 +4847,14 @@
       <c r="AM26" t="n">
         <v>1299</v>
       </c>
-      <c r="AN26" t="inlineStr"/>
-      <c r="AO26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AP26" t="inlineStr"/>
-      <c r="AQ26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AN26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AO26" t="inlineStr"/>
+      <c r="AP26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AQ26" t="inlineStr"/>
       <c r="AR26" t="n">
         <v>1299</v>
       </c>
@@ -4794,10 +4870,10 @@
       <c r="AV26" t="n">
         <v>1299</v>
       </c>
-      <c r="AW26" t="inlineStr"/>
-      <c r="AX26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AW26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AX26" t="inlineStr"/>
       <c r="AY26" t="n">
         <v>1299</v>
       </c>
@@ -4816,6 +4892,269 @@
       <c r="BD26" t="n">
         <v>1299</v>
       </c>
+      <c r="BE26" t="n">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Adult Diaper Pants Style | Medium (M) Size 10 Counts | Waist 24"-40" (61-102cm)| Upto 12 hr Absorption Protection | Unisex with Wetness Indicator | Odour Control &amp; Goodness of Aloe Vera</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>199</v>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
+      <c r="AI27" t="inlineStr"/>
+      <c r="AJ27" t="inlineStr"/>
+      <c r="AK27" t="inlineStr"/>
+      <c r="AL27" t="inlineStr"/>
+      <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr"/>
+      <c r="AO27" t="inlineStr"/>
+      <c r="AP27" t="inlineStr"/>
+      <c r="AQ27" t="inlineStr"/>
+      <c r="AR27" t="inlineStr"/>
+      <c r="AS27" t="inlineStr"/>
+      <c r="AT27" t="inlineStr"/>
+      <c r="AU27" t="inlineStr"/>
+      <c r="AV27" t="inlineStr"/>
+      <c r="AW27" t="inlineStr"/>
+      <c r="AX27" t="inlineStr"/>
+      <c r="AY27" t="inlineStr"/>
+      <c r="AZ27" t="inlineStr"/>
+      <c r="BA27" t="inlineStr"/>
+      <c r="BB27" t="inlineStr"/>
+      <c r="BC27" t="inlineStr"/>
+      <c r="BD27" t="inlineStr"/>
+      <c r="BE27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Adult Diaper Pants Style | Medium (M) Size 30 Counts | Waist 24"-40" (61-102cm)| Upto 12 hr Absorption Protection | Unisex with Wetness Indicator | Odour Control &amp; Goodness of Aloe Vera</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>213</v>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
+      <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" t="inlineStr"/>
+      <c r="AK28" t="inlineStr"/>
+      <c r="AL28" t="inlineStr"/>
+      <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr"/>
+      <c r="AO28" t="inlineStr"/>
+      <c r="AP28" t="inlineStr"/>
+      <c r="AQ28" t="inlineStr"/>
+      <c r="AR28" t="inlineStr"/>
+      <c r="AS28" t="inlineStr"/>
+      <c r="AT28" t="inlineStr"/>
+      <c r="AU28" t="inlineStr"/>
+      <c r="AV28" t="inlineStr"/>
+      <c r="AW28" t="inlineStr"/>
+      <c r="AX28" t="inlineStr"/>
+      <c r="AY28" t="inlineStr"/>
+      <c r="AZ28" t="inlineStr"/>
+      <c r="BA28" t="inlineStr"/>
+      <c r="BB28" t="inlineStr"/>
+      <c r="BC28" t="inlineStr"/>
+      <c r="BD28" t="inlineStr"/>
+      <c r="BE28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Adult Diaper Pants Style | Extra Large (XL) Size 10 Counts | Waist 34"-59" (86-150cm)| Upto 12 hr Absorption Protection | Unisex with Wetness Indicator | Odour Control &amp; Goodness of Aloe Vera</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>251</v>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
+      <c r="AI29" t="inlineStr"/>
+      <c r="AJ29" t="inlineStr"/>
+      <c r="AK29" t="inlineStr"/>
+      <c r="AL29" t="inlineStr"/>
+      <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr"/>
+      <c r="AO29" t="inlineStr"/>
+      <c r="AP29" t="inlineStr"/>
+      <c r="AQ29" t="inlineStr"/>
+      <c r="AR29" t="inlineStr"/>
+      <c r="AS29" t="inlineStr"/>
+      <c r="AT29" t="inlineStr"/>
+      <c r="AU29" t="inlineStr"/>
+      <c r="AV29" t="inlineStr"/>
+      <c r="AW29" t="inlineStr"/>
+      <c r="AX29" t="inlineStr"/>
+      <c r="AY29" t="inlineStr"/>
+      <c r="AZ29" t="inlineStr"/>
+      <c r="BA29" t="inlineStr"/>
+      <c r="BB29" t="inlineStr"/>
+      <c r="BC29" t="inlineStr"/>
+      <c r="BD29" t="inlineStr"/>
+      <c r="BE29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Adult Diaper Pants Style | Large (L) Size 30 Counts | Waist 30"-50" (76-127cm)| Upto 12 hr Absorption Protection | Unisex with Wetness Indicator | Odour Control &amp; Goodness of Aloe Vera</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>231</v>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr"/>
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="inlineStr"/>
+      <c r="AJ30" t="inlineStr"/>
+      <c r="AK30" t="inlineStr"/>
+      <c r="AL30" t="inlineStr"/>
+      <c r="AM30" t="inlineStr"/>
+      <c r="AN30" t="inlineStr"/>
+      <c r="AO30" t="inlineStr"/>
+      <c r="AP30" t="inlineStr"/>
+      <c r="AQ30" t="inlineStr"/>
+      <c r="AR30" t="inlineStr"/>
+      <c r="AS30" t="inlineStr"/>
+      <c r="AT30" t="inlineStr"/>
+      <c r="AU30" t="inlineStr"/>
+      <c r="AV30" t="inlineStr"/>
+      <c r="AW30" t="inlineStr"/>
+      <c r="AX30" t="inlineStr"/>
+      <c r="AY30" t="inlineStr"/>
+      <c r="AZ30" t="inlineStr"/>
+      <c r="BA30" t="inlineStr"/>
+      <c r="BB30" t="inlineStr"/>
+      <c r="BC30" t="inlineStr"/>
+      <c r="BD30" t="inlineStr"/>
+      <c r="BE30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
IST price update 2025-12-25 08:53
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BE30"/>
+  <dimension ref="A1:BF32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,7 @@
     <col width="21" customWidth="1" min="55" max="55"/>
     <col width="21" customWidth="1" min="56" max="56"/>
     <col width="21" customWidth="1" min="57" max="57"/>
+    <col width="21" customWidth="1" min="58" max="58"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -500,280 +501,285 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 14:18</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-25 14:04</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 12:29</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 10:31</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 09:25</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 04:11</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 02:11</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 00:27</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -887,10 +893,10 @@
       <c r="AI2" t="n">
         <v>929</v>
       </c>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AJ2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="n">
         <v>929</v>
       </c>
@@ -903,25 +909,25 @@
       <c r="AO2" t="n">
         <v>929</v>
       </c>
-      <c r="AP2" t="inlineStr"/>
+      <c r="AP2" t="n">
+        <v>929</v>
+      </c>
       <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="n">
         <v>929</v>
       </c>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AT2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="n">
         <v>929</v>
       </c>
-      <c r="AW2" t="inlineStr"/>
-      <c r="AX2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AW2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AX2" t="inlineStr"/>
       <c r="AY2" t="n">
         <v>929</v>
       </c>
@@ -941,6 +947,9 @@
         <v>929</v>
       </c>
       <c r="BE2" t="n">
+        <v>929</v>
+      </c>
+      <c r="BF2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -965,20 +974,20 @@
       <c r="F3" t="n">
         <v>569</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>569</v>
-      </c>
+      <c r="G3" t="n">
+        <v>569</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>569</v>
       </c>
       <c r="J3" t="n">
         <v>569</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
-        <v>569</v>
-      </c>
+      <c r="K3" t="n">
+        <v>569</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>569</v>
       </c>
@@ -997,10 +1006,10 @@
       <c r="R3" t="n">
         <v>569</v>
       </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="n">
-        <v>569</v>
-      </c>
+      <c r="S3" t="n">
+        <v>569</v>
+      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
         <v>569</v>
       </c>
@@ -1043,26 +1052,26 @@
       <c r="AH3" t="n">
         <v>569</v>
       </c>
-      <c r="AI3" t="inlineStr"/>
+      <c r="AI3" t="n">
+        <v>569</v>
+      </c>
       <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="n">
         <v>569</v>
       </c>
       <c r="AN3" t="n">
         <v>569</v>
       </c>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR3" t="inlineStr"/>
       <c r="AS3" t="n">
         <v>569</v>
       </c>
@@ -1078,10 +1087,10 @@
       <c r="AW3" t="n">
         <v>569</v>
       </c>
-      <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AX3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY3" t="inlineStr"/>
       <c r="AZ3" t="n">
         <v>569</v>
       </c>
@@ -1098,6 +1107,9 @@
         <v>569</v>
       </c>
       <c r="BE3" t="n">
+        <v>569</v>
+      </c>
+      <c r="BF3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1125,10 +1137,10 @@
       <c r="G4" t="n">
         <v>299</v>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>299</v>
-      </c>
+      <c r="H4" t="n">
+        <v>299</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
         <v>299</v>
       </c>
@@ -1222,10 +1234,10 @@
       <c r="AN4" t="n">
         <v>299</v>
       </c>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP4" t="inlineStr"/>
       <c r="AQ4" t="n">
         <v>299</v>
       </c>
@@ -1247,10 +1259,10 @@
       <c r="AW4" t="n">
         <v>299</v>
       </c>
-      <c r="AX4" t="inlineStr"/>
-      <c r="AY4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AX4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY4" t="inlineStr"/>
       <c r="AZ4" t="n">
         <v>299</v>
       </c>
@@ -1267,6 +1279,9 @@
         <v>299</v>
       </c>
       <c r="BE4" t="n">
+        <v>299</v>
+      </c>
+      <c r="BF4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1291,11 +1306,11 @@
       <c r="F5" t="n">
         <v>569</v>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>569</v>
+      </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>569</v>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="n">
         <v>569</v>
       </c>
@@ -1317,10 +1332,10 @@
       <c r="P5" t="n">
         <v>569</v>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="n">
-        <v>569</v>
-      </c>
+      <c r="Q5" t="n">
+        <v>569</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
       <c r="S5" t="n">
         <v>569</v>
       </c>
@@ -1414,10 +1429,10 @@
       <c r="AW5" t="n">
         <v>569</v>
       </c>
-      <c r="AX5" t="inlineStr"/>
-      <c r="AY5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AX5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY5" t="inlineStr"/>
       <c r="AZ5" t="n">
         <v>569</v>
       </c>
@@ -1434,6 +1449,9 @@
         <v>569</v>
       </c>
       <c r="BE5" t="n">
+        <v>569</v>
+      </c>
+      <c r="BF5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1461,15 +1479,15 @@
       <c r="G6" t="n">
         <v>499</v>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>499</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>499</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>499</v>
+      </c>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>499</v>
-      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>499</v>
       </c>
@@ -1557,10 +1575,10 @@
       <c r="AO6" t="n">
         <v>499</v>
       </c>
-      <c r="AP6" t="inlineStr"/>
-      <c r="AQ6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AP6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AQ6" t="inlineStr"/>
       <c r="AR6" t="n">
         <v>499</v>
       </c>
@@ -1579,10 +1597,10 @@
       <c r="AW6" t="n">
         <v>499</v>
       </c>
-      <c r="AX6" t="inlineStr"/>
-      <c r="AY6" t="n">
-        <v>499</v>
-      </c>
+      <c r="AX6" t="n">
+        <v>499</v>
+      </c>
+      <c r="AY6" t="inlineStr"/>
       <c r="AZ6" t="n">
         <v>499</v>
       </c>
@@ -1599,6 +1617,9 @@
         <v>499</v>
       </c>
       <c r="BE6" t="n">
+        <v>499</v>
+      </c>
+      <c r="BF6" t="n">
         <v>499</v>
       </c>
     </row>
@@ -1623,20 +1644,20 @@
       <c r="F7" t="n">
         <v>569</v>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>569</v>
-      </c>
+      <c r="G7" t="n">
+        <v>569</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
         <v>569</v>
       </c>
       <c r="J7" t="n">
         <v>569</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="n">
-        <v>569</v>
-      </c>
+      <c r="K7" t="n">
+        <v>569</v>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
         <v>569</v>
       </c>
@@ -1721,12 +1742,12 @@
       <c r="AN7" t="n">
         <v>569</v>
       </c>
-      <c r="AO7" t="inlineStr"/>
+      <c r="AO7" t="n">
+        <v>569</v>
+      </c>
       <c r="AP7" t="inlineStr"/>
       <c r="AQ7" t="inlineStr"/>
-      <c r="AR7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AR7" t="inlineStr"/>
       <c r="AS7" t="n">
         <v>569</v>
       </c>
@@ -1742,10 +1763,10 @@
       <c r="AW7" t="n">
         <v>569</v>
       </c>
-      <c r="AX7" t="inlineStr"/>
-      <c r="AY7" t="n">
-        <v>569</v>
-      </c>
+      <c r="AX7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY7" t="inlineStr"/>
       <c r="AZ7" t="n">
         <v>569</v>
       </c>
@@ -1762,6 +1783,9 @@
         <v>569</v>
       </c>
       <c r="BE7" t="n">
+        <v>569</v>
+      </c>
+      <c r="BF7" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1786,20 +1810,20 @@
       <c r="F8" t="n">
         <v>929</v>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>929</v>
-      </c>
+      <c r="G8" t="n">
+        <v>929</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>929</v>
       </c>
       <c r="J8" t="n">
         <v>929</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="n">
-        <v>929</v>
-      </c>
+      <c r="K8" t="n">
+        <v>929</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
         <v>929</v>
       </c>
@@ -1884,14 +1908,14 @@
       <c r="AN8" t="n">
         <v>929</v>
       </c>
-      <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="n">
-        <v>929</v>
-      </c>
-      <c r="AQ8" t="inlineStr"/>
-      <c r="AR8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AO8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR8" t="inlineStr"/>
       <c r="AS8" t="n">
         <v>929</v>
       </c>
@@ -1907,10 +1931,10 @@
       <c r="AW8" t="n">
         <v>929</v>
       </c>
-      <c r="AX8" t="inlineStr"/>
-      <c r="AY8" t="n">
-        <v>929</v>
-      </c>
+      <c r="AX8" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY8" t="inlineStr"/>
       <c r="AZ8" t="n">
         <v>929</v>
       </c>
@@ -1927,6 +1951,9 @@
         <v>929</v>
       </c>
       <c r="BE8" t="n">
+        <v>929</v>
+      </c>
+      <c r="BF8" t="n">
         <v>929</v>
       </c>
     </row>
@@ -1951,17 +1978,17 @@
       <c r="F9" t="n">
         <v>299</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>299</v>
-      </c>
+      <c r="G9" t="n">
+        <v>299</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>299</v>
       </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="n">
-        <v>299</v>
-      </c>
+      <c r="J9" t="n">
+        <v>299</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="n">
         <v>299</v>
       </c>
@@ -2049,10 +2076,10 @@
       <c r="AN9" t="n">
         <v>299</v>
       </c>
-      <c r="AO9" t="inlineStr"/>
-      <c r="AP9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP9" t="inlineStr"/>
       <c r="AQ9" t="n">
         <v>299</v>
       </c>
@@ -2074,10 +2101,10 @@
       <c r="AW9" t="n">
         <v>299</v>
       </c>
-      <c r="AX9" t="inlineStr"/>
-      <c r="AY9" t="n">
-        <v>299</v>
-      </c>
+      <c r="AX9" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY9" t="inlineStr"/>
       <c r="AZ9" t="n">
         <v>299</v>
       </c>
@@ -2094,6 +2121,9 @@
         <v>299</v>
       </c>
       <c r="BE9" t="n">
+        <v>299</v>
+      </c>
+      <c r="BF9" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2118,18 +2148,18 @@
       <c r="F10" t="n">
         <v>299</v>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>299</v>
-      </c>
+      <c r="G10" t="n">
+        <v>299</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>299</v>
       </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>299</v>
+      </c>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
-        <v>299</v>
-      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
         <v>299</v>
       </c>
@@ -2184,10 +2214,10 @@
       <c r="AD10" t="n">
         <v>299</v>
       </c>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AE10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AF10" t="inlineStr"/>
       <c r="AG10" t="n">
         <v>299</v>
       </c>
@@ -2212,14 +2242,14 @@
       <c r="AN10" t="n">
         <v>299</v>
       </c>
-      <c r="AO10" t="inlineStr"/>
-      <c r="AP10" t="n">
-        <v>299</v>
-      </c>
-      <c r="AQ10" t="inlineStr"/>
-      <c r="AR10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR10" t="inlineStr"/>
       <c r="AS10" t="n">
         <v>299</v>
       </c>
@@ -2235,10 +2265,10 @@
       <c r="AW10" t="n">
         <v>299</v>
       </c>
-      <c r="AX10" t="inlineStr"/>
-      <c r="AY10" t="n">
-        <v>299</v>
-      </c>
+      <c r="AX10" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY10" t="inlineStr"/>
       <c r="AZ10" t="n">
         <v>299</v>
       </c>
@@ -2255,6 +2285,9 @@
         <v>299</v>
       </c>
       <c r="BE10" t="n">
+        <v>299</v>
+      </c>
+      <c r="BF10" t="n">
         <v>299</v>
       </c>
     </row>
@@ -2279,10 +2312,10 @@
       <c r="F11" t="n">
         <v>2997</v>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
+      <c r="G11" t="n">
         <v>2997</v>
       </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>2997</v>
       </c>
@@ -2382,10 +2415,10 @@
       <c r="AO11" t="n">
         <v>2997</v>
       </c>
-      <c r="AP11" t="inlineStr"/>
-      <c r="AQ11" t="n">
+      <c r="AP11" t="n">
         <v>2997</v>
       </c>
+      <c r="AQ11" t="inlineStr"/>
       <c r="AR11" t="n">
         <v>2997</v>
       </c>
@@ -2399,15 +2432,15 @@
         <v>2997</v>
       </c>
       <c r="AV11" t="n">
-        <v>929</v>
+        <v>2997</v>
       </c>
       <c r="AW11" t="n">
         <v>929</v>
       </c>
-      <c r="AX11" t="inlineStr"/>
-      <c r="AY11" t="n">
-        <v>929</v>
-      </c>
+      <c r="AX11" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY11" t="inlineStr"/>
       <c r="AZ11" t="n">
         <v>929</v>
       </c>
@@ -2424,6 +2457,9 @@
         <v>929</v>
       </c>
       <c r="BE11" t="n">
+        <v>929</v>
+      </c>
+      <c r="BF11" t="n">
         <v>929</v>
       </c>
     </row>
@@ -2448,10 +2484,10 @@
       <c r="F12" t="n">
         <v>569</v>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="n">
-        <v>569</v>
-      </c>
+      <c r="G12" t="n">
+        <v>569</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
         <v>569</v>
       </c>
@@ -2554,10 +2590,10 @@
       <c r="AP12" t="n">
         <v>569</v>
       </c>
-      <c r="AQ12" t="inlineStr"/>
-      <c r="AR12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AQ12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR12" t="inlineStr"/>
       <c r="AS12" t="n">
         <v>569</v>
       </c>
@@ -2573,10 +2609,10 @@
       <c r="AW12" t="n">
         <v>569</v>
       </c>
-      <c r="AX12" t="inlineStr"/>
-      <c r="AY12" t="n">
-        <v>569</v>
-      </c>
+      <c r="AX12" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY12" t="inlineStr"/>
       <c r="AZ12" t="n">
         <v>569</v>
       </c>
@@ -2593,6 +2629,9 @@
         <v>569</v>
       </c>
       <c r="BE12" t="n">
+        <v>569</v>
+      </c>
+      <c r="BF12" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2605,27 +2644,27 @@
       <c r="B13" t="n">
         <v>569</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>569</v>
-      </c>
+      <c r="C13" t="n">
+        <v>569</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>569</v>
       </c>
       <c r="F13" t="n">
         <v>569</v>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>569</v>
-      </c>
+      <c r="G13" t="n">
+        <v>569</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>569</v>
       </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>569</v>
-      </c>
+      <c r="J13" t="n">
+        <v>569</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
         <v>569</v>
       </c>
@@ -2662,10 +2701,10 @@
       <c r="W13" t="n">
         <v>569</v>
       </c>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="n">
-        <v>569</v>
-      </c>
+      <c r="X13" t="n">
+        <v>569</v>
+      </c>
+      <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="n">
         <v>569</v>
       </c>
@@ -2711,14 +2750,14 @@
       <c r="AN13" t="n">
         <v>569</v>
       </c>
-      <c r="AO13" t="inlineStr"/>
-      <c r="AP13" t="n">
-        <v>569</v>
-      </c>
-      <c r="AQ13" t="inlineStr"/>
-      <c r="AR13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AO13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AR13" t="inlineStr"/>
       <c r="AS13" t="n">
         <v>569</v>
       </c>
@@ -2734,24 +2773,27 @@
       <c r="AW13" t="n">
         <v>569</v>
       </c>
-      <c r="AX13" t="inlineStr"/>
-      <c r="AY13" t="n">
-        <v>569</v>
-      </c>
+      <c r="AX13" t="n">
+        <v>569</v>
+      </c>
+      <c r="AY13" t="inlineStr"/>
       <c r="AZ13" t="n">
         <v>569</v>
       </c>
       <c r="BA13" t="n">
         <v>569</v>
       </c>
-      <c r="BB13" t="inlineStr"/>
-      <c r="BC13" t="n">
-        <v>569</v>
-      </c>
+      <c r="BB13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BC13" t="inlineStr"/>
       <c r="BD13" t="n">
         <v>569</v>
       </c>
       <c r="BE13" t="n">
+        <v>569</v>
+      </c>
+      <c r="BF13" t="n">
         <v>569</v>
       </c>
     </row>
@@ -2779,17 +2821,17 @@
       <c r="G14" t="n">
         <v>794</v>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="n">
+      <c r="H14" t="n">
         <v>794</v>
       </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="n">
         <v>794</v>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="n">
+      <c r="K14" t="n">
         <v>794</v>
       </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
         <v>794</v>
       </c>
@@ -2844,10 +2886,10 @@
       <c r="AD14" t="n">
         <v>794</v>
       </c>
-      <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="n">
+      <c r="AE14" t="n">
         <v>794</v>
       </c>
+      <c r="AF14" t="inlineStr"/>
       <c r="AG14" t="n">
         <v>794</v>
       </c>
@@ -2855,7 +2897,7 @@
         <v>794</v>
       </c>
       <c r="AI14" t="n">
-        <v>499</v>
+        <v>794</v>
       </c>
       <c r="AJ14" t="n">
         <v>499</v>
@@ -2872,11 +2914,11 @@
       <c r="AN14" t="n">
         <v>499</v>
       </c>
-      <c r="AO14" t="inlineStr"/>
+      <c r="AO14" t="n">
+        <v>499</v>
+      </c>
       <c r="AP14" t="inlineStr"/>
-      <c r="AQ14" t="n">
-        <v>499</v>
-      </c>
+      <c r="AQ14" t="inlineStr"/>
       <c r="AR14" t="n">
         <v>499</v>
       </c>
@@ -2917,6 +2959,9 @@
         <v>499</v>
       </c>
       <c r="BE14" t="n">
+        <v>499</v>
+      </c>
+      <c r="BF14" t="n">
         <v>499</v>
       </c>
     </row>
@@ -2941,16 +2986,16 @@
       <c r="F15" t="n">
         <v>499</v>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>499</v>
+      </c>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
-        <v>499</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>499</v>
+      </c>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="n">
-        <v>499</v>
-      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
         <v>499</v>
       </c>
@@ -3041,10 +3086,10 @@
       <c r="AP15" t="n">
         <v>499</v>
       </c>
-      <c r="AQ15" t="inlineStr"/>
-      <c r="AR15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AQ15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR15" t="inlineStr"/>
       <c r="AS15" t="n">
         <v>499</v>
       </c>
@@ -3054,14 +3099,14 @@
       <c r="AU15" t="n">
         <v>499</v>
       </c>
-      <c r="AV15" t="inlineStr"/>
-      <c r="AW15" t="n">
-        <v>499</v>
-      </c>
-      <c r="AX15" t="inlineStr"/>
-      <c r="AY15" t="n">
-        <v>499</v>
-      </c>
+      <c r="AV15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AW15" t="inlineStr"/>
+      <c r="AX15" t="n">
+        <v>499</v>
+      </c>
+      <c r="AY15" t="inlineStr"/>
       <c r="AZ15" t="n">
         <v>499</v>
       </c>
@@ -3078,6 +3123,9 @@
         <v>499</v>
       </c>
       <c r="BE15" t="n">
+        <v>499</v>
+      </c>
+      <c r="BF15" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3105,14 +3153,14 @@
       <c r="G16" t="n">
         <v>299</v>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>299</v>
-      </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="n">
-        <v>299</v>
-      </c>
+      <c r="H16" t="n">
+        <v>299</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>299</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="n">
         <v>299</v>
       </c>
@@ -3191,17 +3239,17 @@
       <c r="AK16" t="n">
         <v>299</v>
       </c>
-      <c r="AL16" t="inlineStr"/>
-      <c r="AM16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AL16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AM16" t="inlineStr"/>
       <c r="AN16" t="n">
         <v>299</v>
       </c>
-      <c r="AO16" t="inlineStr"/>
-      <c r="AP16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP16" t="inlineStr"/>
       <c r="AQ16" t="n">
         <v>299</v>
       </c>
@@ -3223,10 +3271,10 @@
       <c r="AW16" t="n">
         <v>299</v>
       </c>
-      <c r="AX16" t="inlineStr"/>
-      <c r="AY16" t="n">
-        <v>299</v>
-      </c>
+      <c r="AX16" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY16" t="inlineStr"/>
       <c r="AZ16" t="n">
         <v>299</v>
       </c>
@@ -3243,6 +3291,9 @@
         <v>299</v>
       </c>
       <c r="BE16" t="n">
+        <v>299</v>
+      </c>
+      <c r="BF16" t="n">
         <v>299</v>
       </c>
     </row>
@@ -3267,10 +3318,10 @@
       <c r="F17" t="n">
         <v>929</v>
       </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="n">
-        <v>929</v>
-      </c>
+      <c r="G17" t="n">
+        <v>929</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
         <v>929</v>
       </c>
@@ -3373,10 +3424,10 @@
       <c r="AP17" t="n">
         <v>929</v>
       </c>
-      <c r="AQ17" t="inlineStr"/>
-      <c r="AR17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AR17" t="inlineStr"/>
       <c r="AS17" t="n">
         <v>929</v>
       </c>
@@ -3392,10 +3443,10 @@
       <c r="AW17" t="n">
         <v>929</v>
       </c>
-      <c r="AX17" t="inlineStr"/>
-      <c r="AY17" t="n">
-        <v>929</v>
-      </c>
+      <c r="AX17" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY17" t="inlineStr"/>
       <c r="AZ17" t="n">
         <v>929</v>
       </c>
@@ -3412,6 +3463,9 @@
         <v>929</v>
       </c>
       <c r="BE17" t="n">
+        <v>929</v>
+      </c>
+      <c r="BF17" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3436,18 +3490,18 @@
       <c r="F18" t="n">
         <v>499</v>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="n">
-        <v>499</v>
-      </c>
+      <c r="G18" t="n">
+        <v>499</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
         <v>499</v>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>499</v>
+      </c>
       <c r="K18" t="inlineStr"/>
-      <c r="L18" t="n">
-        <v>499</v>
-      </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
         <v>499</v>
       </c>
@@ -3535,11 +3589,11 @@
       <c r="AO18" t="n">
         <v>499</v>
       </c>
-      <c r="AP18" t="inlineStr"/>
+      <c r="AP18" t="n">
+        <v>499</v>
+      </c>
       <c r="AQ18" t="inlineStr"/>
-      <c r="AR18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AR18" t="inlineStr"/>
       <c r="AS18" t="n">
         <v>499</v>
       </c>
@@ -3555,10 +3609,10 @@
       <c r="AW18" t="n">
         <v>499</v>
       </c>
-      <c r="AX18" t="inlineStr"/>
-      <c r="AY18" t="n">
-        <v>499</v>
-      </c>
+      <c r="AX18" t="n">
+        <v>499</v>
+      </c>
+      <c r="AY18" t="inlineStr"/>
       <c r="AZ18" t="n">
         <v>499</v>
       </c>
@@ -3575,6 +3629,9 @@
         <v>499</v>
       </c>
       <c r="BE18" t="n">
+        <v>499</v>
+      </c>
+      <c r="BF18" t="n">
         <v>499</v>
       </c>
     </row>
@@ -3584,10 +3641,10 @@
           <t>Jr. Sr. Baby Diaper Pants | Extra Large (XL) Size (12-17 kg), 162 Count | Pack of 3 | Upto 12 hr Absorption with Advanced Leak Protection | Safe For Babies Skin | Soft, Secure &amp; Comfy</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="B19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
         <v>1299</v>
       </c>
@@ -3597,18 +3654,18 @@
       <c r="F19" t="n">
         <v>1299</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>1299</v>
+      </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="n">
         <v>1299</v>
       </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="n">
-        <v>1299</v>
-      </c>
+      <c r="K19" t="n">
+        <v>1299</v>
+      </c>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
         <v>1299</v>
       </c>
@@ -3688,7 +3745,7 @@
         <v>1299</v>
       </c>
       <c r="AM19" t="n">
-        <v>1497</v>
+        <v>1299</v>
       </c>
       <c r="AN19" t="n">
         <v>1497</v>
@@ -3696,13 +3753,13 @@
       <c r="AO19" t="n">
         <v>1497</v>
       </c>
-      <c r="AP19" t="inlineStr"/>
+      <c r="AP19" t="n">
+        <v>1497</v>
+      </c>
       <c r="AQ19" t="inlineStr"/>
-      <c r="AR19" t="n">
+      <c r="AR19" t="inlineStr"/>
+      <c r="AS19" t="n">
         <v>465</v>
-      </c>
-      <c r="AS19" t="n">
-        <v>1497</v>
       </c>
       <c r="AT19" t="n">
         <v>1497</v>
@@ -3738,6 +3795,9 @@
         <v>1497</v>
       </c>
       <c r="BE19" t="n">
+        <v>1497</v>
+      </c>
+      <c r="BF19" t="n">
         <v>2997</v>
       </c>
     </row>
@@ -3757,7 +3817,7 @@
         <v>569</v>
       </c>
       <c r="E20" t="n">
-        <v>929</v>
+        <v>569</v>
       </c>
       <c r="F20" t="n">
         <v>929</v>
@@ -3891,10 +3951,10 @@
       <c r="AW20" t="n">
         <v>929</v>
       </c>
-      <c r="AX20" t="inlineStr"/>
-      <c r="AY20" t="n">
-        <v>929</v>
-      </c>
+      <c r="AX20" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY20" t="inlineStr"/>
       <c r="AZ20" t="n">
         <v>929</v>
       </c>
@@ -3911,6 +3971,9 @@
         <v>929</v>
       </c>
       <c r="BE20" t="n">
+        <v>929</v>
+      </c>
+      <c r="BF20" t="n">
         <v>929</v>
       </c>
     </row>
@@ -3935,24 +3998,24 @@
       <c r="F21" t="n">
         <v>499</v>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="n">
-        <v>499</v>
-      </c>
+      <c r="G21" t="n">
+        <v>499</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>499</v>
       </c>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="n">
-        <v>499</v>
-      </c>
+      <c r="J21" t="n">
+        <v>499</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="n">
         <v>499</v>
       </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="n">
-        <v>499</v>
-      </c>
+      <c r="M21" t="n">
+        <v>499</v>
+      </c>
+      <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
         <v>499</v>
       </c>
@@ -4007,10 +4070,10 @@
       <c r="AF21" t="n">
         <v>499</v>
       </c>
-      <c r="AG21" t="inlineStr"/>
-      <c r="AH21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AG21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AH21" t="inlineStr"/>
       <c r="AI21" t="n">
         <v>499</v>
       </c>
@@ -4035,10 +4098,10 @@
       <c r="AP21" t="n">
         <v>499</v>
       </c>
-      <c r="AQ21" t="inlineStr"/>
-      <c r="AR21" t="n">
-        <v>499</v>
-      </c>
+      <c r="AQ21" t="n">
+        <v>499</v>
+      </c>
+      <c r="AR21" t="inlineStr"/>
       <c r="AS21" t="n">
         <v>499</v>
       </c>
@@ -4076,6 +4139,9 @@
         <v>499</v>
       </c>
       <c r="BE21" t="n">
+        <v>499</v>
+      </c>
+      <c r="BF21" t="n">
         <v>499</v>
       </c>
     </row>
@@ -4100,11 +4166,11 @@
       <c r="F22" t="n">
         <v>299</v>
       </c>
-      <c r="G22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>299</v>
+      </c>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="n">
-        <v>299</v>
-      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="n">
         <v>299</v>
       </c>
@@ -4198,14 +4264,14 @@
       <c r="AN22" t="n">
         <v>299</v>
       </c>
-      <c r="AO22" t="inlineStr"/>
-      <c r="AP22" t="n">
-        <v>299</v>
-      </c>
-      <c r="AQ22" t="inlineStr"/>
-      <c r="AR22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AO22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AP22" t="inlineStr"/>
+      <c r="AQ22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AR22" t="inlineStr"/>
       <c r="AS22" t="n">
         <v>299</v>
       </c>
@@ -4221,10 +4287,10 @@
       <c r="AW22" t="n">
         <v>299</v>
       </c>
-      <c r="AX22" t="inlineStr"/>
-      <c r="AY22" t="n">
-        <v>299</v>
-      </c>
+      <c r="AX22" t="n">
+        <v>299</v>
+      </c>
+      <c r="AY22" t="inlineStr"/>
       <c r="AZ22" t="n">
         <v>299</v>
       </c>
@@ -4241,6 +4307,9 @@
         <v>299</v>
       </c>
       <c r="BE22" t="n">
+        <v>299</v>
+      </c>
+      <c r="BF22" t="n">
         <v>299</v>
       </c>
     </row>
@@ -4265,18 +4334,18 @@
       <c r="F23" t="n">
         <v>1299</v>
       </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="G23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
         <v>1299</v>
       </c>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>1299</v>
+      </c>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
         <v>1299</v>
       </c>
@@ -4364,11 +4433,11 @@
       <c r="AO23" t="n">
         <v>1299</v>
       </c>
-      <c r="AP23" t="inlineStr"/>
+      <c r="AP23" t="n">
+        <v>1299</v>
+      </c>
       <c r="AQ23" t="inlineStr"/>
-      <c r="AR23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AR23" t="inlineStr"/>
       <c r="AS23" t="n">
         <v>1299</v>
       </c>
@@ -4384,10 +4453,10 @@
       <c r="AW23" t="n">
         <v>1299</v>
       </c>
-      <c r="AX23" t="inlineStr"/>
-      <c r="AY23" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AX23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AY23" t="inlineStr"/>
       <c r="AZ23" t="n">
         <v>1299</v>
       </c>
@@ -4404,6 +4473,9 @@
         <v>1299</v>
       </c>
       <c r="BE23" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BF23" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -4423,7 +4495,7 @@
         <v>569</v>
       </c>
       <c r="E24" t="n">
-        <v>929</v>
+        <v>569</v>
       </c>
       <c r="F24" t="n">
         <v>929</v>
@@ -4437,11 +4509,11 @@
       <c r="I24" t="n">
         <v>929</v>
       </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>929</v>
+      </c>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="n">
-        <v>929</v>
-      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
         <v>929</v>
       </c>
@@ -4526,11 +4598,11 @@
       <c r="AN24" t="n">
         <v>929</v>
       </c>
-      <c r="AO24" t="inlineStr"/>
+      <c r="AO24" t="n">
+        <v>929</v>
+      </c>
       <c r="AP24" t="inlineStr"/>
-      <c r="AQ24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ24" t="inlineStr"/>
       <c r="AR24" t="n">
         <v>929</v>
       </c>
@@ -4549,10 +4621,10 @@
       <c r="AW24" t="n">
         <v>929</v>
       </c>
-      <c r="AX24" t="inlineStr"/>
-      <c r="AY24" t="n">
-        <v>929</v>
-      </c>
+      <c r="AX24" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY24" t="inlineStr"/>
       <c r="AZ24" t="n">
         <v>929</v>
       </c>
@@ -4569,6 +4641,9 @@
         <v>929</v>
       </c>
       <c r="BE24" t="n">
+        <v>929</v>
+      </c>
+      <c r="BF24" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4593,18 +4668,18 @@
       <c r="F25" t="n">
         <v>929</v>
       </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="n">
-        <v>929</v>
-      </c>
+      <c r="G25" t="n">
+        <v>929</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
         <v>929</v>
       </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>929</v>
+      </c>
       <c r="K25" t="inlineStr"/>
-      <c r="L25" t="n">
-        <v>929</v>
-      </c>
+      <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
         <v>929</v>
       </c>
@@ -4614,10 +4689,10 @@
       <c r="O25" t="n">
         <v>929</v>
       </c>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="n">
-        <v>929</v>
-      </c>
+      <c r="P25" t="n">
+        <v>929</v>
+      </c>
+      <c r="Q25" t="inlineStr"/>
       <c r="R25" t="n">
         <v>929</v>
       </c>
@@ -4687,11 +4762,11 @@
       <c r="AN25" t="n">
         <v>929</v>
       </c>
-      <c r="AO25" t="inlineStr"/>
+      <c r="AO25" t="n">
+        <v>929</v>
+      </c>
       <c r="AP25" t="inlineStr"/>
-      <c r="AQ25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AQ25" t="inlineStr"/>
       <c r="AR25" t="n">
         <v>929</v>
       </c>
@@ -4710,10 +4785,10 @@
       <c r="AW25" t="n">
         <v>929</v>
       </c>
-      <c r="AX25" t="inlineStr"/>
-      <c r="AY25" t="n">
-        <v>929</v>
-      </c>
+      <c r="AX25" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY25" t="inlineStr"/>
       <c r="AZ25" t="n">
         <v>929</v>
       </c>
@@ -4730,6 +4805,9 @@
         <v>929</v>
       </c>
       <c r="BE25" t="n">
+        <v>929</v>
+      </c>
+      <c r="BF25" t="n">
         <v>929</v>
       </c>
     </row>
@@ -4748,10 +4826,10 @@
       <c r="D26" t="n">
         <v>1299</v>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="E26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
         <v>1299</v>
       </c>
@@ -4761,10 +4839,10 @@
       <c r="I26" t="n">
         <v>1299</v>
       </c>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="J26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="n">
         <v>1299</v>
       </c>
@@ -4774,10 +4852,10 @@
       <c r="N26" t="n">
         <v>1299</v>
       </c>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="O26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="P26" t="inlineStr"/>
       <c r="Q26" t="n">
         <v>1299</v>
       </c>
@@ -4850,14 +4928,14 @@
       <c r="AN26" t="n">
         <v>1299</v>
       </c>
-      <c r="AO26" t="inlineStr"/>
-      <c r="AP26" t="n">
-        <v>1299</v>
-      </c>
-      <c r="AQ26" t="inlineStr"/>
-      <c r="AR26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AO26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AP26" t="inlineStr"/>
+      <c r="AQ26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AR26" t="inlineStr"/>
       <c r="AS26" t="n">
         <v>1299</v>
       </c>
@@ -4873,10 +4951,10 @@
       <c r="AW26" t="n">
         <v>1299</v>
       </c>
-      <c r="AX26" t="inlineStr"/>
-      <c r="AY26" t="n">
-        <v>1299</v>
-      </c>
+      <c r="AX26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AY26" t="inlineStr"/>
       <c r="AZ26" t="n">
         <v>1299</v>
       </c>
@@ -4893,6 +4971,9 @@
         <v>1299</v>
       </c>
       <c r="BE26" t="n">
+        <v>1299</v>
+      </c>
+      <c r="BF26" t="n">
         <v>1299</v>
       </c>
     </row>
@@ -4905,7 +4986,9 @@
       <c r="B27" t="n">
         <v>199</v>
       </c>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="n">
+        <v>199</v>
+      </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
@@ -4960,6 +5043,7 @@
       <c r="BC27" t="inlineStr"/>
       <c r="BD27" t="inlineStr"/>
       <c r="BE27" t="inlineStr"/>
+      <c r="BF27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4970,7 +5054,9 @@
       <c r="B28" t="n">
         <v>213</v>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>213</v>
+      </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -5025,6 +5111,7 @@
       <c r="BC28" t="inlineStr"/>
       <c r="BD28" t="inlineStr"/>
       <c r="BE28" t="inlineStr"/>
+      <c r="BF28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -5035,7 +5122,9 @@
       <c r="B29" t="n">
         <v>251</v>
       </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="n">
+        <v>251</v>
+      </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
@@ -5090,6 +5179,7 @@
       <c r="BC29" t="inlineStr"/>
       <c r="BD29" t="inlineStr"/>
       <c r="BE29" t="inlineStr"/>
+      <c r="BF29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -5100,7 +5190,9 @@
       <c r="B30" t="n">
         <v>231</v>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="n">
+        <v>231</v>
+      </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -5155,6 +5247,139 @@
       <c r="BC30" t="inlineStr"/>
       <c r="BD30" t="inlineStr"/>
       <c r="BE30" t="inlineStr"/>
+      <c r="BF30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Adult Diaper Pants Style | Large (L) Size 10 Counts | Waist 30"-50" (76-127cm)| Upto 12 hr Absorption Protection | Unisex with Wetness Indicator | Odour Control &amp; Goodness of Aloe Vera</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>299</v>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr"/>
+      <c r="AI31" t="inlineStr"/>
+      <c r="AJ31" t="inlineStr"/>
+      <c r="AK31" t="inlineStr"/>
+      <c r="AL31" t="inlineStr"/>
+      <c r="AM31" t="inlineStr"/>
+      <c r="AN31" t="inlineStr"/>
+      <c r="AO31" t="inlineStr"/>
+      <c r="AP31" t="inlineStr"/>
+      <c r="AQ31" t="inlineStr"/>
+      <c r="AR31" t="inlineStr"/>
+      <c r="AS31" t="inlineStr"/>
+      <c r="AT31" t="inlineStr"/>
+      <c r="AU31" t="inlineStr"/>
+      <c r="AV31" t="inlineStr"/>
+      <c r="AW31" t="inlineStr"/>
+      <c r="AX31" t="inlineStr"/>
+      <c r="AY31" t="inlineStr"/>
+      <c r="AZ31" t="inlineStr"/>
+      <c r="BA31" t="inlineStr"/>
+      <c r="BB31" t="inlineStr"/>
+      <c r="BC31" t="inlineStr"/>
+      <c r="BD31" t="inlineStr"/>
+      <c r="BE31" t="inlineStr"/>
+      <c r="BF31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Jr. Sr. Adult Diaper Pants Style | Extra Large (XL) Size 30 Counts | Waist 34"-59" (86-150cm)| Upto 12 hr Absorption Protection | Unisex with Wetness Indicator | Odour Control &amp; Goodness of Aloe Vera</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>251</v>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr"/>
+      <c r="AI32" t="inlineStr"/>
+      <c r="AJ32" t="inlineStr"/>
+      <c r="AK32" t="inlineStr"/>
+      <c r="AL32" t="inlineStr"/>
+      <c r="AM32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr"/>
+      <c r="AO32" t="inlineStr"/>
+      <c r="AP32" t="inlineStr"/>
+      <c r="AQ32" t="inlineStr"/>
+      <c r="AR32" t="inlineStr"/>
+      <c r="AS32" t="inlineStr"/>
+      <c r="AT32" t="inlineStr"/>
+      <c r="AU32" t="inlineStr"/>
+      <c r="AV32" t="inlineStr"/>
+      <c r="AW32" t="inlineStr"/>
+      <c r="AX32" t="inlineStr"/>
+      <c r="AY32" t="inlineStr"/>
+      <c r="AZ32" t="inlineStr"/>
+      <c r="BA32" t="inlineStr"/>
+      <c r="BB32" t="inlineStr"/>
+      <c r="BC32" t="inlineStr"/>
+      <c r="BD32" t="inlineStr"/>
+      <c r="BE32" t="inlineStr"/>
+      <c r="BF32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
IST price update 2025-12-25 09:00
</commit_message>
<xml_diff>
--- a/price_tracker_final.xlsx
+++ b/price_tracker_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF32"/>
+  <dimension ref="A1:BG32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +491,7 @@
     <col width="21" customWidth="1" min="56" max="56"/>
     <col width="21" customWidth="1" min="57" max="57"/>
     <col width="21" customWidth="1" min="58" max="58"/>
+    <col width="21" customWidth="1" min="59" max="59"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -501,285 +502,290 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>2025-12-25 14:25</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>2025-12-25 14:18</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 14:04</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 12:29</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 10:31</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 09:25</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 04:11</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 02:11</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12-25 00:27</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 22:22</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 20:12</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 19:14</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 16:16</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 14:28</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 12:31</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 10:30</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 09:22</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 04:11</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 02:11</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2025-12-24 00:29</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 22:26</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 20:17</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 19:20</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 16:20</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 14:27</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 12:32</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 10:31</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 09:25</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 04:13</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 02:12</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-23 00:28</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 22:24</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 20:14</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 19:18</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 16:18</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 14:27</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 12:32</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 10:32</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 09:32</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 04:10</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 02:10</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-22 00:24</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 22:17</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 20:09</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 19:06</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 16:12</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 14:19</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 12:27</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 10:29</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 09:28</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 04:09</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 02:07</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:52</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>2025-12-21 00:32</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:33</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 23:18</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 22:00</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>2025-12-20 13:20</t>
         </is>
@@ -896,10 +902,10 @@
       <c r="AJ2" t="n">
         <v>929</v>
       </c>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AK2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="n">
         <v>929</v>
       </c>
@@ -912,25 +918,25 @@
       <c r="AP2" t="n">
         <v>929</v>
       </c>
-      <c r="AQ2" t="inlineStr"/>
+      <c r="AQ2" t="n">
+        <v>929</v>
+      </c>
       <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="n">
         <v>929</v>
       </c>
-      <c r="AU2" t="inlineStr"/>
-      <c r="AV2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AU2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="n">
         <v>929</v>
       </c>
-      <c r="AX2" t="inlineStr"/>
-      <c r="AY2" t="n">
-        <v>929</v>
-      </c>
+      <c r="AX2" t="n">
+        <v>929</v>
+      </c>
+      <c r="AY2" t="inlineStr"/>
       <c r="AZ2" t="n">
         <v>929</v>
       </c>
@@ -950,6 +956,9 @@
         <v>929</v>
       </c>
       <c r="BF2" t="n">
+        <v>929</v>
+      </c>
+      <c r="BG2" t="n">
         <v>929</v>
       </c>
     </row>
@@ -977,20 +986,20 @@
       <c r="G3" t="n">
         <v>569</v>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>569</v>
-      </c>
+      <c r="H3" t="n">
+        <v>569</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
         <v>569</v>
       </c>
       <c r="K3" t="n">
         <v>569</v>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>569</v>
-      </c>
+      <c r="L3" t="n">
+        <v>569</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>569</v>
       </c>
@@ -1009,10 +1018,10 @@
       <c r="S3" t="n">
         <v>569</v>
       </c>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
-        <v>569</v>
-      </c>
+      <c r="T3" t="n">
+        <v>569</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
       <c r="V3" t="n">
         <v>569</v>
       </c>
@@ -1055,26 +1064,26 @@
       <c r="AI3" t="n">
         <v>569</v>
       </c>
-      <c r="AJ3" t="inlineStr"/>
+      <c r="AJ3" t="n">
+        <v>569</v>
+      </c>
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="n">
         <v>569</v>
       </c>
       <c r="AO3" t="n">
         <v>569</v>
       </c>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="n">
-        <v>569</v>
-      </c>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AP3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AS3" t="inlineStr"/>
       <c r="AT3" t="n">
         <v>569</v>
       </c>
@@ -1090,10 +1099,10 @@
       <c r="AX3" t="n">
         <v>569</v>
       </c>
-      <c r="AY3" t="inlineStr"/>
-      <c r="AZ3" t="n">
-        <v>569</v>
-      </c>
+      <c r="AY3" t="n">
+        <v>569</v>
+      </c>
+      <c r="AZ3" t="inlineStr"/>
       <c r="BA3" t="n">
         <v>569</v>
       </c>
@@ -1110,6 +1119,9 @@
         <v>569</v>
       </c>
       <c r="BF3" t="n">
+        <v>569</v>
+      </c>
+      <c r="BG3" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1140,10 +1152,10 @@
       <c r="H4" t="n">
         <v>299</v>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="n">
-        <v>299</v>
-      </c>
+      <c r="I4" t="n">
+        <v>299</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
         <v>299</v>
       </c>
@@ -1237,10 +1249,10 @@
       <c r="AO4" t="n">
         <v>299</v>
       </c>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AP4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AQ4" t="inlineStr"/>
       <c r="AR4" t="n">
         <v>299</v>
       </c>
@@ -1262,10 +1274,10 @@
       <c r="AX4" t="n">
         <v>299</v>
       </c>
-      <c r="AY4" t="inlineStr"/>
-      <c r="AZ4" t="n">
-        <v>299</v>
-      </c>
+      <c r="AY4" t="n">
+        <v>299</v>
+      </c>
+      <c r="AZ4" t="inlineStr"/>
       <c r="BA4" t="n">
         <v>299</v>
       </c>
@@ -1282,6 +1294,9 @@
         <v>299</v>
       </c>
       <c r="BF4" t="n">
+        <v>299</v>
+      </c>
+      <c r="BG4" t="n">
         <v>299</v>
       </c>
     </row>
@@ -1291,9 +1306,7 @@
           <t>Jr. Sr. Baby Tape Style Diaper | Adjustable Fit For Babies | Extra Large (XL) Size (12+ kg), 38 Count | Pack of 1 | Upto 12 hr Absorption with Advanced Leak Protection | Soft &amp; Comfy</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>569</v>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
         <v>569</v>
       </c>
@@ -1309,11 +1322,11 @@
       <c r="G5" t="n">
         <v>569</v>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>569</v>
+      </c>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="n">
-        <v>569</v>
-      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
         <v>569</v>
       </c>
@@ -1335,10 +1348,10 @@
       <c r="Q5" t="n">
         <v>569</v>
       </c>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="n">
-        <v>569</v>
-      </c>
+      <c r="R5" t="n">
+        <v>569</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
       <c r="T5" t="n">
         <v>569</v>
       </c>
@@ -1432,10 +1445,10 @@
       <c r="AX5" t="n">
         <v>569</v>
       </c>
-      <c r="AY5" t="inlineStr"/>
-      <c r="AZ5" t="n">
-        <v>569</v>
-      </c>
+      <c r="AY5" t="n">
+        <v>569</v>
+      </c>
+      <c r="AZ5" t="inlineStr"/>
       <c r="BA5" t="n">
         <v>569</v>
       </c>
@@ -1452,6 +1465,9 @@
         <v>569</v>
       </c>
       <c r="BF5" t="n">
+        <v>569</v>
+      </c>
+      <c r="BG5" t="n">
         <v>569</v>
       </c>
     </row>
@@ -1482,15 +1498,15 @@
       <c r="H6" t="n">
         <v>499</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
-        <v>499</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>499</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="n">
+        <v>499</v>
+      </c>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>499</v>
-      </c>
+      <c r="M6" t="inline